<commit_message>
adding noise to coordinates --> manually
no LinAlg error anymore
I will try to write a code to add noise
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,10 +528,10 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>95284374.10084265</v>
+        <v>95283997.94687383</v>
       </c>
       <c r="C2" t="n">
-        <v>-181127008.4037445</v>
+        <v>-181126431.7277304</v>
       </c>
       <c r="D2" t="n">
         <v>47</v>
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>67.83333333333333</v>
+        <v>67.83336164715892</v>
       </c>
       <c r="J2" t="n">
-        <v>-178.8333333333333</v>
+        <v>-178.8333050195077</v>
       </c>
       <c r="K2" t="n">
         <v>77.19385719984045</v>
@@ -642,10 +642,10 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>119550320.9126408</v>
+        <v>119550397.81551</v>
       </c>
       <c r="C3" t="n">
-        <v>-209147146.690412</v>
+        <v>-209147245.3898863</v>
       </c>
       <c r="D3" t="n">
         <v>47</v>
@@ -671,10 +671,10 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>65.7</v>
+        <v>65.69999468594703</v>
       </c>
       <c r="J3" t="n">
-        <v>-178.0666666666667</v>
+        <v>-178.0666719807197</v>
       </c>
       <c r="K3" t="n">
         <v>76.99530516431925</v>
@@ -756,10 +756,10 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>104940963.62414</v>
+        <v>104941270.6788485</v>
       </c>
       <c r="C4" t="n">
-        <v>-184375118.5381976</v>
+        <v>-184375531.6367889</v>
       </c>
       <c r="D4" t="n">
         <v>47</v>
@@ -785,10 +785,10 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>66.40000000000001</v>
+        <v>66.39997687381246</v>
       </c>
       <c r="J4" t="n">
-        <v>-174.8833333333333</v>
+        <v>-174.8833564595209</v>
       </c>
       <c r="K4" t="n">
         <v>76.56732781819994</v>
@@ -874,10 +874,10 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>95828091.14760715</v>
+        <v>95827846.36066358</v>
       </c>
       <c r="C5" t="n">
-        <v>-182845511.2563718</v>
+        <v>-182845134.7133268</v>
       </c>
       <c r="D5" t="n">
         <v>47</v>
@@ -903,10 +903,10 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>67.84999999999999</v>
+        <v>67.85001829537772</v>
       </c>
       <c r="J5" t="n">
-        <v>-179.2833333333333</v>
+        <v>-179.2833150379556</v>
       </c>
       <c r="K5" t="n">
         <v>76.29378980891718</v>
@@ -988,10 +988,10 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>95742004.36730675</v>
+        <v>95741334.71643947</v>
       </c>
       <c r="C6" t="n">
-        <v>-182871217.1779032</v>
+        <v>-182870185.5601847</v>
       </c>
       <c r="D6" t="n">
         <v>47</v>
@@ -1017,10 +1017,10 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>67.86666666666666</v>
+        <v>67.86671670282102</v>
       </c>
       <c r="J6" t="n">
-        <v>-179.35</v>
+        <v>-179.3499499638456</v>
       </c>
       <c r="K6" t="n">
         <v>76.51060424169667</v>
@@ -1102,10 +1102,10 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>110427379.7520474</v>
+        <v>110428185.9511601</v>
       </c>
       <c r="C7" t="n">
-        <v>-201248607.2898324</v>
+        <v>-201249734.0073696</v>
       </c>
       <c r="D7" t="n">
         <v>47</v>
@@ -1131,10 +1131,10 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>66.59999999999999</v>
+        <v>66.59994315430309</v>
       </c>
       <c r="J7" t="n">
-        <v>-179.05</v>
+        <v>-179.0500568456969</v>
       </c>
       <c r="K7" t="n">
         <v>76.56250000000001</v>
@@ -1212,10 +1212,10 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>95831639.73313977</v>
+        <v>95831097.14160162</v>
       </c>
       <c r="C8" t="n">
-        <v>-182597732.6966358</v>
+        <v>-182596899.4977312</v>
       </c>
       <c r="D8" t="n">
         <v>47</v>
@@ -1241,10 +1241,10 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>67.83333333333333</v>
+        <v>67.83337393385574</v>
       </c>
       <c r="J8" t="n">
-        <v>-179.1666666666667</v>
+        <v>-179.1666260661443</v>
       </c>
       <c r="K8" t="n">
         <v>75.8226463863207</v>
@@ -1326,10 +1326,10 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>105425096.2505695</v>
+        <v>105424177.0032899</v>
       </c>
       <c r="C9" t="n">
-        <v>-186072421.7714847</v>
+        <v>-186071178.5209873</v>
       </c>
       <c r="D9" t="n">
         <v>47</v>
@@ -1355,10 +1355,10 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>66.43333333333334</v>
+        <v>66.43340208612744</v>
       </c>
       <c r="J9" t="n">
-        <v>-175.35</v>
+        <v>-175.3499312472059</v>
       </c>
       <c r="K9" t="n">
         <v>75.75636942675158</v>
@@ -1444,10 +1444,10 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>93838874.55294298</v>
+        <v>93838148.12582983</v>
       </c>
       <c r="C10" t="n">
-        <v>-180546417.700183</v>
+        <v>-180545283.6552253</v>
       </c>
       <c r="D10" t="n">
         <v>47</v>
@@ -1473,10 +1473,10 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>68.05</v>
+        <v>68.05005468778411</v>
       </c>
       <c r="J10" t="n">
-        <v>-179.5</v>
+        <v>-179.4999453122159</v>
       </c>
       <c r="K10" t="n">
         <v>76.19715487878182</v>
@@ -1562,10 +1562,10 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>105481494.1250038</v>
+        <v>105481876.0653925</v>
       </c>
       <c r="C11" t="n">
-        <v>-184961424.1195456</v>
+        <v>-184961935.7090315</v>
       </c>
       <c r="D11" t="n">
         <v>47</v>
@@ -1591,10 +1591,10 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>66.34999999999999</v>
+        <v>66.34997128755195</v>
       </c>
       <c r="J11" t="n">
-        <v>-174.8666666666667</v>
+        <v>-174.8666953791148</v>
       </c>
       <c r="K11" t="n">
         <v>76.34538152610442</v>
@@ -1676,10 +1676,10 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>124230435.9675245</v>
+        <v>124228588.4715796</v>
       </c>
       <c r="C12" t="n">
-        <v>-206496617.07635</v>
+        <v>-206494470.9674475</v>
       </c>
       <c r="D12" t="n">
         <v>47</v>
@@ -1705,10 +1705,10 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>64.86666666666666</v>
+        <v>64.86679641086742</v>
       </c>
       <c r="J12" t="n">
-        <v>-175.5166666666667</v>
+        <v>-175.5165369224659</v>
       </c>
       <c r="K12" t="n">
         <v>75.82077636962379</v>
@@ -1786,10 +1786,10 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>114775616.4159573</v>
+        <v>114775970.9772273</v>
       </c>
       <c r="C13" t="n">
-        <v>-200512082.1266816</v>
+        <v>-200512542.1981468</v>
       </c>
       <c r="D13" t="n">
         <v>47</v>
@@ -1815,10 +1815,10 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>65.88333333333334</v>
+        <v>65.88330810347263</v>
       </c>
       <c r="J13" t="n">
-        <v>-176.8333333333333</v>
+        <v>-176.833358563194</v>
       </c>
       <c r="K13" t="n">
         <v>75.33756949960284</v>
@@ -1892,10 +1892,10 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>92752723.90399264</v>
+        <v>92751788.18368557</v>
       </c>
       <c r="C14" t="n">
-        <v>-177344357.2270249</v>
+        <v>-177342903.7849017</v>
       </c>
       <c r="D14" t="n">
         <v>47</v>
@@ -1921,10 +1921,10 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>68.03333333333333</v>
+        <v>68.03340471926347</v>
       </c>
       <c r="J14" t="n">
-        <v>-178.7</v>
+        <v>-178.6999286140698</v>
       </c>
       <c r="K14" t="n">
         <v>75.96394591887831</v>
@@ -2006,10 +2006,10 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>98398735.8188502</v>
+        <v>98399684.42395204</v>
       </c>
       <c r="C15" t="n">
-        <v>-168146143.3040679</v>
+        <v>-168147393.1085977</v>
       </c>
       <c r="D15" t="n">
         <v>47</v>
@@ -2035,10 +2035,10 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>66.38333333333334</v>
+        <v>66.3832569334397</v>
       </c>
       <c r="J15" t="n">
-        <v>-171.1666666666667</v>
+        <v>-171.1667430665604</v>
       </c>
       <c r="K15" t="n">
         <v>75.67865371130922</v>
@@ -2116,10 +2116,10 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>124691394.4699661</v>
+        <v>124690050.8859959</v>
       </c>
       <c r="C16" t="n">
-        <v>-205921940.8915289</v>
+        <v>-205920400.4650612</v>
       </c>
       <c r="D16" t="n">
         <v>47</v>
@@ -2145,10 +2145,10 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>64.76666666666667</v>
+        <v>64.76676128743597</v>
       </c>
       <c r="J16" t="n">
-        <v>-175.1833333333333</v>
+        <v>-175.183238712564</v>
       </c>
       <c r="K16" t="n">
         <v>75.56533920352211</v>
@@ -2230,10 +2230,10 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>117109806.3377758</v>
+        <v>117110197.7580975</v>
       </c>
       <c r="C17" t="n">
-        <v>-202418426.7369417</v>
+        <v>-202418922.8946863</v>
       </c>
       <c r="D17" t="n">
         <v>47</v>
@@ -2259,10 +2259,10 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>65.65000000000001</v>
+        <v>65.64997228439121</v>
       </c>
       <c r="J17" t="n">
-        <v>-176.6</v>
+        <v>-176.6000277156088</v>
       </c>
       <c r="K17" t="n">
         <v>75.69465342561942</v>
@@ -2340,10 +2340,10 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>121345179.7527965</v>
+        <v>121346830.2819801</v>
       </c>
       <c r="C18" t="n">
-        <v>-211274281.6220778</v>
+        <v>-211276373.4495602</v>
       </c>
       <c r="D18" t="n">
         <v>47</v>
@@ -2369,10 +2369,10 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>65.56666666666666</v>
+        <v>65.56655332885526</v>
       </c>
       <c r="J18" t="n">
-        <v>-178.1333333333333</v>
+        <v>-178.1334466711447</v>
       </c>
       <c r="K18" t="n">
         <v>75.18699511319437</v>
@@ -2454,10 +2454,10 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>125519954.0534237</v>
+        <v>125519215.899418</v>
       </c>
       <c r="C19" t="n">
-        <v>-203199110.0709001</v>
+        <v>-203198296.5584472</v>
       </c>
       <c r="D19" t="n">
         <v>47</v>
@@ -2483,10 +2483,10 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>64.48333333333333</v>
+        <v>64.48338593502929</v>
       </c>
       <c r="J19" t="n">
-        <v>-174.05</v>
+        <v>-174.0499473983041</v>
       </c>
       <c r="K19" t="n">
         <v>74.65305313243456</v>
@@ -2560,10 +2560,10 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>95366310.44663362</v>
+        <v>95364596.81383142</v>
       </c>
       <c r="C20" t="n">
-        <v>-181347041.4569888</v>
+        <v>-181344413.6594365</v>
       </c>
       <c r="D20" t="n">
         <v>47</v>
@@ -2589,10 +2589,10 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>67.83333333333333</v>
+        <v>67.83346220749966</v>
       </c>
       <c r="J20" t="n">
-        <v>-178.8833333333333</v>
+        <v>-178.883204459167</v>
       </c>
       <c r="K20" t="n">
         <v>75.32285514065472</v>
@@ -2674,10 +2674,10 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>127329419.3064801</v>
+        <v>127328664.1379309</v>
       </c>
       <c r="C21" t="n">
-        <v>-206191994.1163333</v>
+        <v>-206191166.5138207</v>
       </c>
       <c r="D21" t="n">
         <v>47</v>
@@ -2703,10 +2703,10 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>64.41666666666667</v>
+        <v>64.41671993659487</v>
       </c>
       <c r="J21" t="n">
-        <v>-174.5</v>
+        <v>-174.4999467300718</v>
       </c>
       <c r="K21" t="n">
         <v>74.74908079101658</v>
@@ -2784,10 +2784,10 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>121268232.9128181</v>
+        <v>121266763.0873286</v>
       </c>
       <c r="C22" t="n">
-        <v>-198348877.9395528</v>
+        <v>-198347203.042288</v>
       </c>
       <c r="D22" t="n">
         <v>47</v>
@@ -2813,10 +2813,10 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>64.78333333333333</v>
+        <v>64.78343969693921</v>
       </c>
       <c r="J22" t="n">
-        <v>-173.7166666666667</v>
+        <v>-173.7165603030608</v>
       </c>
       <c r="K22" t="n">
         <v>74.78364667263506</v>
@@ -2890,10 +2890,10 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>95382638.89698099</v>
+        <v>95381528.85832316</v>
       </c>
       <c r="C23" t="n">
-        <v>-182159559.3962781</v>
+        <v>-182157848.2088327</v>
       </c>
       <c r="D23" t="n">
         <v>47</v>
@@ -2919,10 +2919,10 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>67.88333333333334</v>
+        <v>67.88341649871434</v>
       </c>
       <c r="J23" t="n">
-        <v>-179.25</v>
+        <v>-179.249916834619</v>
       </c>
       <c r="K23" t="n">
         <v>75.18759379689844</v>
@@ -2996,10 +2996,10 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>95605230.35903408</v>
+        <v>95605162.06082919</v>
       </c>
       <c r="C24" t="n">
-        <v>-182502512.0045116</v>
+        <v>-182502406.8320286</v>
       </c>
       <c r="D24" t="n">
         <v>47</v>
@@ -3025,10 +3025,10 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>67.86666666666666</v>
+        <v>67.86667177744339</v>
       </c>
       <c r="J24" t="n">
-        <v>-179.2666666666667</v>
+        <v>-179.26666155589</v>
       </c>
       <c r="K24" t="n">
         <v>74.74868119836768</v>
@@ -3110,10 +3110,10 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>121302922.7578963</v>
+        <v>121302567.4736511</v>
       </c>
       <c r="C25" t="n">
-        <v>-203758953.5618101</v>
+        <v>-203758529.3476131</v>
       </c>
       <c r="D25" t="n">
         <v>47</v>
@@ -3139,10 +3139,10 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>65.11666666666666</v>
+        <v>65.11669181224212</v>
       </c>
       <c r="J25" t="n">
-        <v>-175.55</v>
+        <v>-175.5499748544246</v>
       </c>
       <c r="K25" t="n">
         <v>74.96504893149591</v>
@@ -3224,10 +3224,10 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>112736790.3333419</v>
+        <v>112736084.8396494</v>
       </c>
       <c r="C26" t="n">
-        <v>-195554905.0331039</v>
+        <v>-195553994.4118544</v>
       </c>
       <c r="D26" t="n">
         <v>47</v>
@@ -3253,10 +3253,10 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>65.88333333333334</v>
+        <v>65.88338446289151</v>
       </c>
       <c r="J26" t="n">
-        <v>-175.8166666666667</v>
+        <v>-175.8166155371085</v>
       </c>
       <c r="K26" t="n">
         <v>74.9350908727781</v>
@@ -3334,10 +3334,10 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>95250320.69290274</v>
+        <v>95250469.72453789</v>
       </c>
       <c r="C27" t="n">
-        <v>-181546521.4671764</v>
+        <v>-181546750.717905</v>
       </c>
       <c r="D27" t="n">
         <v>47</v>
@@ -3363,10 +3363,10 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>67.86666666666666</v>
+        <v>67.86665547156203</v>
       </c>
       <c r="J27" t="n">
-        <v>-179.05</v>
+        <v>-179.0500111951046</v>
       </c>
       <c r="K27" t="n">
         <v>74.68114786767636</v>
@@ -3448,10 +3448,10 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>114519697.5267772</v>
+        <v>114519157.4111848</v>
       </c>
       <c r="C28" t="n">
-        <v>-188018848.4303199</v>
+        <v>-188018214.6526375</v>
       </c>
       <c r="D28" t="n">
         <v>47</v>
@@ -3477,10 +3477,10 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>65.11666666666666</v>
+        <v>65.11670719855645</v>
       </c>
       <c r="J28" t="n">
-        <v>-172.3333333333333</v>
+        <v>-172.3332928014435</v>
       </c>
       <c r="K28" t="n">
         <v>75.07769423558896</v>
@@ -3562,10 +3562,10 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>99552949.03530049</v>
+        <v>99552368.42483975</v>
       </c>
       <c r="C29" t="n">
-        <v>-173041385.1462702</v>
+        <v>-173040603.8722652</v>
       </c>
       <c r="D29" t="n">
         <v>47</v>
@@ -3591,10 +3591,10 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>66.53333333333333</v>
+        <v>66.53337907415737</v>
       </c>
       <c r="J29" t="n">
-        <v>-172.7333333333333</v>
+        <v>-172.7332875925092</v>
       </c>
       <c r="K29" t="n">
         <v>74.91494896938163</v>
@@ -3672,10 +3672,10 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>122385847.8125908</v>
+        <v>122386908.7302104</v>
       </c>
       <c r="C30" t="n">
-        <v>-200371221.2941432</v>
+        <v>-200372427.8239095</v>
       </c>
       <c r="D30" t="n">
         <v>47</v>
@@ -3701,10 +3701,10 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>64.75</v>
+        <v>64.74992377307039</v>
       </c>
       <c r="J30" t="n">
-        <v>-174.05</v>
+        <v>-174.0500762269296</v>
       </c>
       <c r="K30" t="n">
         <v>74.1114741114741</v>
@@ -3778,10 +3778,10 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>121302922.7578963</v>
+        <v>121305639.0987237</v>
       </c>
       <c r="C31" t="n">
-        <v>-203758953.5618101</v>
+        <v>-203762196.873767</v>
       </c>
       <c r="D31" t="n">
         <v>47</v>
@@ -3807,10 +3807,10 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>65.11666666666666</v>
+        <v>65.11647441619643</v>
       </c>
       <c r="J31" t="n">
-        <v>-175.55</v>
+        <v>-175.5501922504702</v>
       </c>
       <c r="K31" t="n">
         <v>74.53639082751742</v>
@@ -3892,10 +3892,10 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>95246344.46007697</v>
+        <v>95246610.15562837</v>
       </c>
       <c r="C32" t="n">
-        <v>-181792066.2544586</v>
+        <v>-181792475.6709797</v>
       </c>
       <c r="D32" t="n">
         <v>47</v>
@@ -3921,10 +3921,10 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>67.88333333333334</v>
+        <v>67.88331339769263</v>
       </c>
       <c r="J32" t="n">
-        <v>-179.1666666666667</v>
+        <v>-179.1666866023074</v>
       </c>
       <c r="K32" t="n">
         <v>74.59588904410298</v>
@@ -4006,10 +4006,10 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>120390771.9605777</v>
+        <v>120390801.7820959</v>
       </c>
       <c r="C33" t="n">
-        <v>-211194262.1907431</v>
+        <v>-211194300.5434513</v>
       </c>
       <c r="D33" t="n">
         <v>47</v>
@@ -4035,10 +4035,10 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>65.7</v>
+        <v>65.69999795399802</v>
       </c>
       <c r="J33" t="n">
-        <v>-178.4666666666667</v>
+        <v>-178.4666687126687</v>
       </c>
       <c r="K33" t="n">
         <v>74.37810945273633</v>
@@ -4116,10 +4116,10 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>95491782.3279893</v>
+        <v>95491579.99477631</v>
       </c>
       <c r="C34" t="n">
-        <v>-182453960.0272382</v>
+        <v>-182453648.0181718</v>
       </c>
       <c r="D34" t="n">
         <v>47</v>
@@ -4145,10 +4145,10 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>67.88333333333334</v>
+        <v>67.88334847439322</v>
       </c>
       <c r="J34" t="n">
-        <v>-179.3166666666667</v>
+        <v>-179.3166515256068</v>
       </c>
       <c r="K34" t="n">
         <v>74.27406523468576</v>
@@ -4230,10 +4230,10 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>125024042.9467272</v>
+        <v>125024109.1397756</v>
       </c>
       <c r="C35" t="n">
-        <v>-202349813.6192167</v>
+        <v>-202349886.662595</v>
       </c>
       <c r="D35" t="n">
         <v>47</v>
@@ -4259,10 +4259,10 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>64.5</v>
+        <v>64.49999526918459</v>
       </c>
       <c r="J35" t="n">
-        <v>-173.9166666666667</v>
+        <v>-173.9166713974821</v>
       </c>
       <c r="K35" t="n">
         <v>74.73958333333333</v>
@@ -4340,10 +4340,10 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>124329274.9727886</v>
+        <v>124327141.534732</v>
       </c>
       <c r="C36" t="n">
-        <v>-205633805.9033265</v>
+        <v>-205631350.3833643</v>
       </c>
       <c r="D36" t="n">
         <v>47</v>
@@ -4369,10 +4369,10 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>64.8</v>
+        <v>64.80015036111361</v>
       </c>
       <c r="J36" t="n">
-        <v>-175.2</v>
+        <v>-175.1998496388864</v>
       </c>
       <c r="K36" t="n">
         <v>74.59459459459461</v>
@@ -4458,10 +4458,10 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>100516192.4317949</v>
+        <v>100517524.5837477</v>
       </c>
       <c r="C37" t="n">
-        <v>-174698241.4453496</v>
+        <v>-174700028.5846796</v>
       </c>
       <c r="D37" t="n">
         <v>47</v>
@@ -4487,10 +4487,10 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>66.48333333333333</v>
+        <v>66.48322906384377</v>
       </c>
       <c r="J37" t="n">
-        <v>-172.9666666666667</v>
+        <v>-172.9667709361563</v>
       </c>
       <c r="K37" t="n">
         <v>74.46043165467626</v>
@@ -4568,10 +4568,10 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>101868044.6608461</v>
+        <v>101868677.8207729</v>
       </c>
       <c r="C38" t="n">
-        <v>-175393655.9404441</v>
+        <v>-175394490.4031445</v>
       </c>
       <c r="D38" t="n">
         <v>47</v>
@@ -4597,10 +4597,10 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>66.3</v>
+        <v>66.29995050572477</v>
       </c>
       <c r="J38" t="n">
-        <v>-172.6</v>
+        <v>-172.6000494942752</v>
       </c>
       <c r="K38" t="n">
         <v>74.16110723887283</v>
@@ -4682,10 +4682,10 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>92876055.8900442</v>
+        <v>92875591.35906237</v>
       </c>
       <c r="C39" t="n">
-        <v>-179716070.3565532</v>
+        <v>-179715338.5746408</v>
       </c>
       <c r="D39" t="n">
         <v>47</v>
@@ -4711,10 +4711,10 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>68.16666666666667</v>
+        <v>68.16670171430422</v>
       </c>
       <c r="J39" t="n">
-        <v>-179.75</v>
+        <v>-179.7499649523625</v>
       </c>
       <c r="K39" t="n">
         <v>74.00736391680766</v>
@@ -4800,10 +4800,10 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>94842068.59978738</v>
+        <v>94841119.89169264</v>
       </c>
       <c r="C40" t="n">
-        <v>-180448186.6503598</v>
+        <v>-180446729.0647684</v>
       </c>
       <c r="D40" t="n">
         <v>47</v>
@@ -4829,10 +4829,10 @@
         </is>
       </c>
       <c r="I40" t="n">
-        <v>67.86666666666666</v>
+        <v>67.86673825049411</v>
       </c>
       <c r="J40" t="n">
-        <v>-178.8</v>
+        <v>-178.7999284161726</v>
       </c>
       <c r="K40" t="n">
         <v>74.27228168450536</v>
@@ -4918,10 +4918,10 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>121231079.5081446</v>
+        <v>121229783.9312185</v>
       </c>
       <c r="C41" t="n">
-        <v>-203590872.726265</v>
+        <v>-203589326.0603937</v>
       </c>
       <c r="D41" t="n">
         <v>47</v>
@@ -4947,10 +4947,10 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>65.11666666666666</v>
+        <v>65.11675841779834</v>
       </c>
       <c r="J41" t="n">
-        <v>-175.5166666666667</v>
+        <v>-175.516574915535</v>
       </c>
       <c r="K41" t="n">
         <v>74.36591478696742</v>
@@ -5032,10 +5032,10 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>94348792.27090809</v>
+        <v>94348518.45245603</v>
       </c>
       <c r="C42" t="n">
-        <v>-180904827.0952213</v>
+        <v>-180904401.9074258</v>
       </c>
       <c r="D42" t="n">
         <v>47</v>
@@ -5061,10 +5061,10 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>67.98333333333333</v>
+        <v>67.98335393134224</v>
       </c>
       <c r="J42" t="n">
-        <v>-179.3333333333333</v>
+        <v>-179.3333127353244</v>
       </c>
       <c r="K42" t="n">
         <v>73.97943906577501</v>
@@ -5150,10 +5150,10 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>93968936.30973481</v>
+        <v>93969253.23702408</v>
       </c>
       <c r="C43" t="n">
-        <v>-178607658.017132</v>
+        <v>-178608145.3456385</v>
       </c>
       <c r="D43" t="n">
         <v>47</v>
@@ -5179,10 +5179,10 @@
         </is>
       </c>
       <c r="I43" t="n">
-        <v>67.90000000000001</v>
+        <v>67.89997591453019</v>
       </c>
       <c r="J43" t="n">
-        <v>-178.5</v>
+        <v>-178.5000240854698</v>
       </c>
       <c r="K43" t="n">
         <v>73.53204172876302</v>
@@ -5264,10 +5264,10 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>104812331.247064</v>
+        <v>104810639.4110961</v>
       </c>
       <c r="C44" t="n">
-        <v>-184306026.7207892</v>
+        <v>-184303746.9290686</v>
       </c>
       <c r="D44" t="n">
         <v>47</v>
@@ -5293,10 +5293,10 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>66.41666666666667</v>
+        <v>66.41679410589634</v>
       </c>
       <c r="J44" t="n">
-        <v>-174.9166666666667</v>
+        <v>-174.9165392274371</v>
       </c>
       <c r="K44" t="n">
         <v>73.88305847076461</v>
@@ -5382,10 +5382,10 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>90477982.9351497</v>
+        <v>90477776.63345405</v>
       </c>
       <c r="C45" t="n">
-        <v>-173672176.64469</v>
+        <v>-173671852.9647405</v>
       </c>
       <c r="D45" t="n">
         <v>47</v>
@@ -5411,10 +5411,10 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>68.2</v>
+        <v>68.20001595428498</v>
       </c>
       <c r="J45" t="n">
-        <v>-178.4666666666667</v>
+        <v>-178.4666507123817</v>
       </c>
       <c r="K45" t="n">
         <v>73.70995109292343</v>
@@ -5500,10 +5500,10 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>95910335.53990658</v>
+        <v>95909931.02336974</v>
       </c>
       <c r="C46" t="n">
-        <v>-183067055.2003559</v>
+        <v>-183066432.8012119</v>
       </c>
       <c r="D46" t="n">
         <v>47</v>
@@ -5529,10 +5529,10 @@
         </is>
       </c>
       <c r="I46" t="n">
-        <v>67.84999999999999</v>
+        <v>67.85003020674193</v>
       </c>
       <c r="J46" t="n">
-        <v>-179.3333333333333</v>
+        <v>-179.3333031265913</v>
       </c>
       <c r="K46" t="n">
         <v>74.10938283993977</v>
@@ -5610,10 +5610,10 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>94302113.98934323</v>
+        <v>94301473.24302509</v>
       </c>
       <c r="C47" t="n">
-        <v>-181549493.4311254</v>
+        <v>-181548493.462025</v>
       </c>
       <c r="D47" t="n">
         <v>47</v>
@@ -5639,10 +5639,10 @@
         </is>
       </c>
       <c r="I47" t="n">
-        <v>68.03333333333333</v>
+        <v>68.03338138338532</v>
       </c>
       <c r="J47" t="n">
-        <v>-179.6666666666667</v>
+        <v>-179.6666186166147</v>
       </c>
       <c r="K47" t="n">
         <v>73.38717718616013</v>
@@ -5728,10 +5728,10 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>94296468.61873128</v>
+        <v>94297103.23677927</v>
       </c>
       <c r="C48" t="n">
-        <v>-179235352.260593</v>
+        <v>-179236327.3664464</v>
       </c>
       <c r="D48" t="n">
         <v>47</v>
@@ -5757,10 +5757,10 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>67.88333333333334</v>
+        <v>67.88328522004672</v>
       </c>
       <c r="J48" t="n">
-        <v>-178.5833333333333</v>
+        <v>-178.5833814466199</v>
       </c>
       <c r="K48" t="n">
         <v>73.48590845492704</v>
@@ -5842,10 +5842,10 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>123510560.9248481</v>
+        <v>123511159.385416</v>
       </c>
       <c r="C49" t="n">
-        <v>-204562004.6381881</v>
+        <v>-204562696.9623128</v>
       </c>
       <c r="D49" t="n">
         <v>47</v>
@@ -5871,10 +5871,10 @@
         </is>
       </c>
       <c r="I49" t="n">
-        <v>64.84999999999999</v>
+        <v>64.84995767676973</v>
       </c>
       <c r="J49" t="n">
-        <v>-175.1</v>
+        <v>-175.1000423232303</v>
       </c>
       <c r="K49" t="n">
         <v>73.3113838172204</v>
@@ -5956,10 +5956,10 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>95727747.05797774</v>
+        <v>95726392.43290836</v>
       </c>
       <c r="C50" t="n">
-        <v>-181806002.1952314</v>
+        <v>-181803929.9202596</v>
       </c>
       <c r="D50" t="n">
         <v>47</v>
@@ -5985,10 +5985,10 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>67.8</v>
+        <v>67.80010172042356</v>
       </c>
       <c r="J50" t="n">
-        <v>-178.8666666666667</v>
+        <v>-178.8665649462432</v>
       </c>
       <c r="K50" t="n">
         <v>73.55032548823233</v>
@@ -6066,10 +6066,10 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>105275229.8101812</v>
+        <v>105276258.5071207</v>
       </c>
       <c r="C51" t="n">
-        <v>-175037684.2022962</v>
+        <v>-175038955.4961019</v>
       </c>
       <c r="D51" t="n">
         <v>47</v>
@@ -6095,10 +6095,10 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>65.7</v>
+        <v>65.69991906688784</v>
       </c>
       <c r="J51" t="n">
-        <v>-170.9166666666667</v>
+        <v>-170.9167475997789</v>
       </c>
       <c r="K51" t="n">
         <v>73.5070140280561</v>
@@ -6180,10 +6180,10 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>111386520.4661945</v>
+        <v>111385813.1348711</v>
       </c>
       <c r="C52" t="n">
-        <v>-202326547.8398675</v>
+        <v>-202325566.3048023</v>
       </c>
       <c r="D52" t="n">
         <v>47</v>
@@ -6209,10 +6209,10 @@
         </is>
       </c>
       <c r="I52" t="n">
-        <v>66.51666666666667</v>
+        <v>66.51671638435909</v>
       </c>
       <c r="J52" t="n">
-        <v>-179.0166666666667</v>
+        <v>-179.0166169489743</v>
       </c>
       <c r="K52" t="n">
         <v>73.24197259177751</v>
@@ -6290,10 +6290,10 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>117762717.0079449</v>
+        <v>117762280.2443921</v>
       </c>
       <c r="C53" t="n">
-        <v>-206445375.607007</v>
+        <v>-206444810.4697082</v>
       </c>
       <c r="D53" t="n">
         <v>47</v>
@@ -6319,10 +6319,10 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>65.8</v>
+        <v>65.80003044384634</v>
       </c>
       <c r="J53" t="n">
-        <v>-177.8</v>
+        <v>-177.7999695561537</v>
       </c>
       <c r="K53" t="n">
         <v>73.43640196767393</v>
@@ -6404,10 +6404,10 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>90649783.85114792</v>
+        <v>90648909.40460366</v>
       </c>
       <c r="C54" t="n">
-        <v>-173642220.5342466</v>
+        <v>-173640852.4905823</v>
       </c>
       <c r="D54" t="n">
         <v>47</v>
@@ -6433,10 +6433,10 @@
         </is>
       </c>
       <c r="I54" t="n">
-        <v>68.16666666666667</v>
+        <v>68.16673432352188</v>
       </c>
       <c r="J54" t="n">
-        <v>-178.3333333333333</v>
+        <v>-178.3332656764781</v>
       </c>
       <c r="K54" t="n">
         <v>72.71280827366745</v>
@@ -6522,10 +6522,10 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>95144827.22376937</v>
+        <v>95144979.32683986</v>
       </c>
       <c r="C55" t="n">
-        <v>-181007222.8567674</v>
+        <v>-181007456.3519843</v>
       </c>
       <c r="D55" t="n">
         <v>47</v>
@@ -6551,10 +6551,10 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>67.84999999999999</v>
+        <v>67.84998854730327</v>
       </c>
       <c r="J55" t="n">
-        <v>-178.8666666666667</v>
+        <v>-178.8666781193634</v>
       </c>
       <c r="K55" t="n">
         <v>73.0004992511233</v>
@@ -6636,10 +6636,10 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>116765950.873015</v>
+        <v>116765237.1330395</v>
       </c>
       <c r="C56" t="n">
-        <v>-201590224.5266909</v>
+        <v>-201589320.5850689</v>
       </c>
       <c r="D56" t="n">
         <v>47</v>
@@ -6665,10 +6665,10 @@
         </is>
       </c>
       <c r="I56" t="n">
-        <v>65.65000000000001</v>
+        <v>65.65005069036712</v>
       </c>
       <c r="J56" t="n">
-        <v>-176.4333333333333</v>
+        <v>-176.4332826429662</v>
       </c>
       <c r="K56" t="n">
         <v>72.89318839134337</v>
@@ -6746,10 +6746,10 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>90078421.93827379</v>
+        <v>90078482.66003077</v>
       </c>
       <c r="C57" t="n">
-        <v>-175847645.16619</v>
+        <v>-175847742.4345175</v>
       </c>
       <c r="D57" t="n">
         <v>47</v>
@@ -6775,10 +6775,10 @@
         </is>
       </c>
       <c r="I57" t="n">
-        <v>68.41666666666667</v>
+        <v>68.41666202381649</v>
       </c>
       <c r="J57" t="n">
-        <v>-179.8166666666667</v>
+        <v>-179.8166713095169</v>
       </c>
       <c r="K57" t="n">
         <v>72.84959633210406</v>
@@ -6856,10 +6856,10 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>112422290.1619789</v>
+        <v>112421186.6435295</v>
       </c>
       <c r="C58" t="n">
-        <v>-203311145.2236667</v>
+        <v>-203309627.5781915</v>
       </c>
       <c r="D58" t="n">
         <v>47</v>
@@ -6885,10 +6885,10 @@
         </is>
       </c>
       <c r="I58" t="n">
-        <v>66.41666666666667</v>
+        <v>66.41674402719615</v>
       </c>
       <c r="J58" t="n">
-        <v>-178.9166666666667</v>
+        <v>-178.9165893061372</v>
       </c>
       <c r="K58" t="n">
         <v>73.28719028989869</v>
@@ -6966,10 +6966,10 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>101352905.0940265</v>
+        <v>101353956.1124853</v>
       </c>
       <c r="C59" t="n">
-        <v>-174378892.6943066</v>
+        <v>-174380278.5482855</v>
       </c>
       <c r="D59" t="n">
         <v>47</v>
@@ -6995,10 +6995,10 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>66.31666666666666</v>
+        <v>66.31658417360453</v>
       </c>
       <c r="J59" t="n">
-        <v>-172.4166666666667</v>
+        <v>-172.4167491597289</v>
       </c>
       <c r="K59" t="n">
         <v>72.71822434557579</v>
@@ -7080,10 +7080,10 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>108991650.7730794</v>
+        <v>108990125.585209</v>
       </c>
       <c r="C60" t="n">
-        <v>-198403080.6874453</v>
+        <v>-198400944.9399034</v>
       </c>
       <c r="D60" t="n">
         <v>47</v>
@@ -7109,10 +7109,10 @@
         </is>
       </c>
       <c r="I60" t="n">
-        <v>66.65000000000001</v>
+        <v>66.65010862310646</v>
       </c>
       <c r="J60" t="n">
-        <v>-178.6166666666667</v>
+        <v>-178.6165580435602</v>
       </c>
       <c r="K60" t="n">
         <v>73.47882932716485</v>
@@ -7190,10 +7190,10 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>122729244.7314957</v>
+        <v>122728632.492375</v>
       </c>
       <c r="C61" t="n">
-        <v>-218063392.4324215</v>
+        <v>-218062593.9383368</v>
       </c>
       <c r="D61" t="n">
         <v>47</v>
@@ -7219,10 +7219,10 @@
         </is>
       </c>
       <c r="I61" t="n">
-        <v>65.76666666666667</v>
+        <v>65.76670766974841</v>
       </c>
       <c r="J61" t="n">
-        <v>-179.9666666666667</v>
+        <v>-179.9666256635849</v>
       </c>
       <c r="K61" t="n">
         <v>73.22574178027264</v>
@@ -7300,10 +7300,10 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>123510560.9248481</v>
+        <v>123510164.7726939</v>
       </c>
       <c r="C62" t="n">
-        <v>-204562004.6381881</v>
+        <v>-204561546.3511443</v>
       </c>
       <c r="D62" t="n">
         <v>47</v>
@@ -7329,10 +7329,10 @@
         </is>
       </c>
       <c r="I62" t="n">
-        <v>64.84999999999999</v>
+        <v>64.85002801599575</v>
       </c>
       <c r="J62" t="n">
-        <v>-175.1</v>
+        <v>-175.0999719840042</v>
       </c>
       <c r="K62" t="n">
         <v>73.1524133787302</v>
@@ -7414,10 +7414,10 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>100299797.0652027</v>
+        <v>100300642.5028112</v>
       </c>
       <c r="C63" t="n">
-        <v>-170668336.6487279</v>
+        <v>-170669436.9423906</v>
       </c>
       <c r="D63" t="n">
         <v>47</v>
@@ -7443,10 +7443,10 @@
         </is>
       </c>
       <c r="I63" t="n">
-        <v>66.23333333333333</v>
+        <v>66.23326588624691</v>
       </c>
       <c r="J63" t="n">
-        <v>-171.3333333333333</v>
+        <v>-171.3334007804197</v>
       </c>
       <c r="K63" t="n">
         <v>73.12355947489728</v>
@@ -7528,10 +7528,10 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>110376141.6722051</v>
+        <v>110373640.5749958</v>
       </c>
       <c r="C64" t="n">
-        <v>-200847293.8202986</v>
+        <v>-200843805.4986471</v>
       </c>
       <c r="D64" t="n">
         <v>47</v>
@@ -7557,10 +7557,10 @@
         </is>
       </c>
       <c r="I64" t="n">
-        <v>66.58333333333333</v>
+        <v>66.58350997521569</v>
       </c>
       <c r="J64" t="n">
-        <v>-178.9166666666667</v>
+        <v>-178.9164900247843</v>
       </c>
       <c r="K64" t="n">
         <v>73.1961866532865</v>
@@ -7646,10 +7646,10 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>102481604.0016726</v>
+        <v>102481904.874213</v>
       </c>
       <c r="C65" t="n">
-        <v>-192204461.4167705</v>
+        <v>-192204907.2039707</v>
       </c>
       <c r="D65" t="n">
         <v>47</v>
@@ -7675,10 +7675,10 @@
         </is>
       </c>
       <c r="I65" t="n">
-        <v>67.31666666666666</v>
+        <v>67.31664487291627</v>
       </c>
       <c r="J65" t="n">
-        <v>-179.4666666666667</v>
+        <v>-179.4666884604171</v>
       </c>
       <c r="K65" t="n">
         <v>72.43742550655541</v>
@@ -7760,10 +7760,10 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>105782639.235118</v>
+        <v>105782274.34132</v>
       </c>
       <c r="C66" t="n">
-        <v>-174816153.4121206</v>
+        <v>-174815707.5859639</v>
       </c>
       <c r="D66" t="n">
         <v>47</v>
@@ -7789,10 +7789,10 @@
         </is>
       </c>
       <c r="I66" t="n">
-        <v>65.59999999999999</v>
+        <v>65.60002875733929</v>
       </c>
       <c r="J66" t="n">
-        <v>-170.6166666666667</v>
+        <v>-170.6166379093274</v>
       </c>
       <c r="K66" t="n">
         <v>73.5534686458649</v>
@@ -7874,10 +7874,10 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>111386520.4661945</v>
+        <v>111386930.7365307</v>
       </c>
       <c r="C67" t="n">
-        <v>-202326547.8398675</v>
+        <v>-202327117.153652</v>
       </c>
       <c r="D67" t="n">
         <v>47</v>
@@ -7903,10 +7903,10 @@
         </is>
       </c>
       <c r="I67" t="n">
-        <v>66.51666666666667</v>
+        <v>66.51663782919877</v>
       </c>
       <c r="J67" t="n">
-        <v>-179.0166666666667</v>
+        <v>-179.0166955041346</v>
       </c>
       <c r="K67" t="n">
         <v>72.9056150535482</v>
@@ -7988,10 +7988,10 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>99476764.10656033</v>
+        <v>99475750.87607253</v>
       </c>
       <c r="C68" t="n">
-        <v>-172152315.9636682</v>
+        <v>-172150960.8091157</v>
       </c>
       <c r="D68" t="n">
         <v>47</v>
@@ -8017,10 +8017,10 @@
         </is>
       </c>
       <c r="I68" t="n">
-        <v>66.48333333333333</v>
+        <v>66.4834134900225</v>
       </c>
       <c r="J68" t="n">
-        <v>-172.3833333333333</v>
+        <v>-172.3832531766441</v>
       </c>
       <c r="K68" t="n">
         <v>72.98326485619801</v>
@@ -8102,10 +8102,10 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>98871095.94729911</v>
+        <v>98869816.35752448</v>
       </c>
       <c r="C69" t="n">
-        <v>-165439701.8338122</v>
+        <v>-165438070.2453113</v>
       </c>
       <c r="D69" t="n">
         <v>47</v>
@@ -8131,10 +8131,10 @@
         </is>
       </c>
       <c r="I69" t="n">
-        <v>66.09999999999999</v>
+        <v>66.10010451914354</v>
       </c>
       <c r="J69" t="n">
-        <v>-169.75</v>
+        <v>-169.7498954808565</v>
       </c>
       <c r="K69" t="n">
         <v>72.75272472752725</v>
@@ -8216,10 +8216,10 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>104220170.0391953</v>
+        <v>104219668.5023493</v>
       </c>
       <c r="C70" t="n">
-        <v>-177744483.1088804</v>
+        <v>-177743836.1466576</v>
       </c>
       <c r="D70" t="n">
         <v>47</v>
@@ -8245,10 +8245,10 @@
         </is>
       </c>
       <c r="I70" t="n">
-        <v>66.06666666666666</v>
+        <v>66.06670557210387</v>
       </c>
       <c r="J70" t="n">
-        <v>-172.4833333333333</v>
+        <v>-172.4832944278961</v>
       </c>
       <c r="K70" t="n">
         <v>72.78911564625849</v>
@@ -8326,10 +8326,10 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>117053988.4432226</v>
+        <v>117054203.5502286</v>
       </c>
       <c r="C71" t="n">
-        <v>-196200139.9330243</v>
+        <v>-196200399.241827</v>
       </c>
       <c r="D71" t="n">
         <v>47</v>
@@ -8355,10 +8355,10 @@
         </is>
       </c>
       <c r="I71" t="n">
-        <v>65.26666666666667</v>
+        <v>65.26665103512377</v>
       </c>
       <c r="J71" t="n">
-        <v>-174.3833333333333</v>
+        <v>-174.3833489648762</v>
       </c>
       <c r="K71" t="n">
         <v>72.58933918945898</v>
@@ -8436,10 +8436,10 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>95366310.44663362</v>
+        <v>95365871.76747249</v>
       </c>
       <c r="C72" t="n">
-        <v>-181347041.4569888</v>
+        <v>-181346368.7595194</v>
       </c>
       <c r="D72" t="n">
         <v>47</v>
@@ -8465,10 +8465,10 @@
         </is>
       </c>
       <c r="I72" t="n">
-        <v>67.83333333333333</v>
+        <v>67.83336632419059</v>
       </c>
       <c r="J72" t="n">
-        <v>-178.8833333333333</v>
+        <v>-178.883300342476</v>
       </c>
       <c r="K72" t="n">
         <v>72.76365819491693</v>
@@ -8550,10 +8550,10 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>121302922.7578963</v>
+        <v>121303628.3113402</v>
       </c>
       <c r="C73" t="n">
-        <v>-203758953.5618101</v>
+        <v>-203759795.9989638</v>
       </c>
       <c r="D73" t="n">
         <v>47</v>
@@ -8579,10 +8579,10 @@
         </is>
       </c>
       <c r="I73" t="n">
-        <v>65.11666666666666</v>
+        <v>65.11661673055883</v>
       </c>
       <c r="J73" t="n">
-        <v>-175.55</v>
+        <v>-175.5500499361079</v>
       </c>
       <c r="K73" t="n">
         <v>72.46333433103861</v>
@@ -8664,10 +8664,10 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>108554861.9245501</v>
+        <v>108554960.1844395</v>
       </c>
       <c r="C74" t="n">
-        <v>-192823788.690152</v>
+        <v>-192823921.6748115</v>
       </c>
       <c r="D74" t="n">
         <v>47</v>
@@ -8693,10 +8693,10 @@
         </is>
       </c>
       <c r="I74" t="n">
-        <v>66.36666666666666</v>
+        <v>66.36665950224786</v>
       </c>
       <c r="J74" t="n">
-        <v>-176.6</v>
+        <v>-176.6000071644188</v>
       </c>
       <c r="K74" t="n">
         <v>72.35975244559793</v>
@@ -8774,10 +8774,10 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>94543477.72676614</v>
+        <v>94542668.27345119</v>
       </c>
       <c r="C75" t="n">
-        <v>-181175749.1510621</v>
+        <v>-181174493.6530331</v>
       </c>
       <c r="D75" t="n">
         <v>47</v>
@@ -8803,10 +8803,10 @@
         </is>
       </c>
       <c r="I75" t="n">
-        <v>67.96666666666667</v>
+        <v>67.96672750150034</v>
       </c>
       <c r="J75" t="n">
-        <v>-179.3333333333333</v>
+        <v>-179.3332724984996</v>
       </c>
       <c r="K75" t="n">
         <v>72.48275172482751</v>
@@ -8892,10 +8892,10 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>126364408.8082207</v>
+        <v>126364001.9614239</v>
       </c>
       <c r="C76" t="n">
-        <v>-208391946.3415851</v>
+        <v>-208391483.5858551</v>
       </c>
       <c r="D76" t="n">
         <v>47</v>
@@ -8921,10 +8921,10 @@
         </is>
       </c>
       <c r="I76" t="n">
-        <v>64.68333333333334</v>
+        <v>64.68336175479625</v>
       </c>
       <c r="J76" t="n">
-        <v>-175.4833333333333</v>
+        <v>-175.4833049118704</v>
       </c>
       <c r="K76" t="n">
         <v>72.52351410846506</v>
@@ -9006,10 +9006,10 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>114600309.6025832</v>
+        <v>114600057.7617754</v>
       </c>
       <c r="C77" t="n">
-        <v>-193023541.3949634</v>
+        <v>-193023232.9809702</v>
       </c>
       <c r="D77" t="n">
         <v>47</v>
@@ -9035,10 +9035,10 @@
         </is>
       </c>
       <c r="I77" t="n">
-        <v>65.43333333333334</v>
+        <v>65.43335182853889</v>
       </c>
       <c r="J77" t="n">
-        <v>-174.1333333333333</v>
+        <v>-174.1333148381277</v>
       </c>
       <c r="K77" t="n">
         <v>72.19341974077767</v>
@@ -9120,10 +9120,10 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>96182872.47031368</v>
+        <v>96182717.2374838</v>
       </c>
       <c r="C78" t="n">
-        <v>-167069444.0541844</v>
+        <v>-167069233.2421187</v>
       </c>
       <c r="D78" t="n">
         <v>47</v>
@@ -9149,10 +9149,10 @@
         </is>
       </c>
       <c r="I78" t="n">
-        <v>66.7</v>
+        <v>66.70001252623884</v>
       </c>
       <c r="J78" t="n">
-        <v>-171.8333333333333</v>
+        <v>-171.8333208070945</v>
       </c>
       <c r="K78" t="n">
         <v>72.36855282924385</v>
@@ -9234,10 +9234,10 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>90103996.45974264</v>
+        <v>90103790.92650808</v>
       </c>
       <c r="C79" t="n">
-        <v>-175918496.8794327</v>
+        <v>-175918167.6152635</v>
       </c>
       <c r="D79" t="n">
         <v>47</v>
@@ -9263,10 +9263,10 @@
         </is>
       </c>
       <c r="I79" t="n">
-        <v>68.41666666666667</v>
+        <v>68.41668237733052</v>
       </c>
       <c r="J79" t="n">
-        <v>-179.8333333333333</v>
+        <v>-179.8333176226694</v>
       </c>
       <c r="K79" t="n">
         <v>71.7088229436367</v>
@@ -9348,10 +9348,10 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>112422290.1619789</v>
+        <v>112423939.6619415</v>
       </c>
       <c r="C80" t="n">
-        <v>-203311145.2236667</v>
+        <v>-203313413.7283501</v>
       </c>
       <c r="D80" t="n">
         <v>47</v>
@@ -9377,10 +9377,10 @@
         </is>
       </c>
       <c r="I80" t="n">
-        <v>66.41666666666667</v>
+        <v>66.41655103159917</v>
       </c>
       <c r="J80" t="n">
-        <v>-178.9166666666667</v>
+        <v>-178.9167823017342</v>
       </c>
       <c r="K80" t="n">
         <v>72.24620945878098</v>
@@ -9458,10 +9458,10 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>110880692.5942751</v>
+        <v>110880978.5168227</v>
       </c>
       <c r="C81" t="n">
-        <v>-201586831.3702166</v>
+        <v>-201587229.1416554</v>
       </c>
       <c r="D81" t="n">
         <v>47</v>
@@ -9487,10 +9487,10 @@
         </is>
       </c>
       <c r="I81" t="n">
-        <v>66.55</v>
+        <v>66.54997985485556</v>
       </c>
       <c r="J81" t="n">
-        <v>-178.9666666666667</v>
+        <v>-178.9666868118111</v>
       </c>
       <c r="K81" t="n">
         <v>71.84097492757967</v>
@@ -9572,10 +9572,10 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>111720704.4516372</v>
+        <v>111720135.9280964</v>
       </c>
       <c r="C82" t="n">
-        <v>-202901214.7686998</v>
+        <v>-202900426.6929799</v>
       </c>
       <c r="D82" t="n">
         <v>47</v>
@@ -9601,10 +9601,10 @@
         </is>
       </c>
       <c r="I82" t="n">
-        <v>66.5</v>
+        <v>66.50003988393064</v>
       </c>
       <c r="J82" t="n">
-        <v>-179.0833333333333</v>
+        <v>-179.0832934494026</v>
       </c>
       <c r="K82" t="n">
         <v>72.01242111589704</v>
@@ -9686,10 +9686,10 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>112375952.3542469</v>
+        <v>112374935.9972873</v>
       </c>
       <c r="C83" t="n">
-        <v>-185558503.7297454</v>
+        <v>-185557290.790704</v>
       </c>
       <c r="D83" t="n">
         <v>47</v>
@@ -9715,10 +9715,10 @@
         </is>
       </c>
       <c r="I83" t="n">
-        <v>65.28333333333333</v>
+        <v>65.28341023740553</v>
       </c>
       <c r="J83" t="n">
-        <v>-172.2</v>
+        <v>-172.1999230959278</v>
       </c>
       <c r="K83" t="n">
         <v>72.24399557833382</v>
@@ -9796,10 +9796,10 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>103128391.90762</v>
+        <v>103127393.1932825</v>
       </c>
       <c r="C84" t="n">
-        <v>-172089975.3335668</v>
+        <v>-172088725.1295874</v>
       </c>
       <c r="D84" t="n">
         <v>47</v>
@@ -9825,10 +9825,10 @@
         </is>
       </c>
       <c r="I84" t="n">
-        <v>65.84999999999999</v>
+        <v>65.85007944968972</v>
       </c>
       <c r="J84" t="n">
-        <v>-170.6333333333333</v>
+        <v>-170.6332538836436</v>
       </c>
       <c r="K84" t="n">
         <v>71.55249775650614</v>
@@ -9906,10 +9906,10 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>122710851.0832534</v>
+        <v>122710867.0445147</v>
       </c>
       <c r="C85" t="n">
-        <v>-203257306.8410021</v>
+        <v>-203257325.3563437</v>
       </c>
       <c r="D85" t="n">
         <v>47</v>
@@ -9935,10 +9935,10 @@
         </is>
       </c>
       <c r="I85" t="n">
-        <v>64.88333333333334</v>
+        <v>64.8833321995574</v>
       </c>
       <c r="J85" t="n">
-        <v>-174.9166666666667</v>
+        <v>-174.9166678004426</v>
       </c>
       <c r="K85" t="n">
         <v>71.23002084781098</v>
@@ -10016,10 +10016,10 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>111990802.0731752</v>
+        <v>111990549.4419555</v>
       </c>
       <c r="C86" t="n">
-        <v>-203312556.6516881</v>
+        <v>-203312206.8927979</v>
       </c>
       <c r="D86" t="n">
         <v>47</v>
@@ -10045,10 +10045,10 @@
         </is>
       </c>
       <c r="I86" t="n">
-        <v>66.48333333333333</v>
+        <v>66.48335103265381</v>
       </c>
       <c r="J86" t="n">
-        <v>-179.1166666666667</v>
+        <v>-179.1166489673462</v>
       </c>
       <c r="K86" t="n">
         <v>71.66983111821725</v>
@@ -10130,10 +10130,10 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>98872498.37953989</v>
+        <v>98871311.63442823</v>
       </c>
       <c r="C87" t="n">
-        <v>-168606397.5936514</v>
+        <v>-168604841.0895316</v>
       </c>
       <c r="D87" t="n">
         <v>47</v>
@@ -10159,10 +10159,10 @@
         </is>
       </c>
       <c r="I87" t="n">
-        <v>66.33333333333333</v>
+        <v>66.33342876510508</v>
       </c>
       <c r="J87" t="n">
-        <v>-171.1333333333333</v>
+        <v>-171.1332379015615</v>
       </c>
       <c r="K87" t="n">
         <v>71.77613135762914</v>
@@ -10244,10 +10244,10 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>107111219.4867288</v>
+        <v>107111056.3425351</v>
       </c>
       <c r="C88" t="n">
-        <v>-195472580.201184</v>
+        <v>-195472349.8516857</v>
       </c>
       <c r="D88" t="n">
         <v>47</v>
@@ -10273,10 +10273,10 @@
         </is>
       </c>
       <c r="I88" t="n">
-        <v>66.76666666666667</v>
+        <v>66.76667840048799</v>
       </c>
       <c r="J88" t="n">
-        <v>-178.3666666666667</v>
+        <v>-178.3666549328454</v>
       </c>
       <c r="K88" t="n">
         <v>71.57558197622139</v>
@@ -10354,10 +10354,10 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>90347820.69530219</v>
+        <v>90347365.26830955</v>
       </c>
       <c r="C89" t="n">
-        <v>-176338851.1894838</v>
+        <v>-176338122.2630417</v>
       </c>
       <c r="D89" t="n">
         <v>47</v>
@@ -10383,10 +10383,10 @@
         </is>
       </c>
       <c r="I89" t="n">
-        <v>68.40000000000001</v>
+        <v>68.40003475744538</v>
       </c>
       <c r="J89" t="n">
-        <v>-179.8666666666667</v>
+        <v>-179.8666319092213</v>
       </c>
       <c r="K89" t="n">
         <v>71.23779150886985</v>
@@ -10464,10 +10464,10 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>102529146.2410535</v>
+        <v>102530379.9016063</v>
       </c>
       <c r="C90" t="n">
-        <v>-191800516.1325061</v>
+        <v>-191802337.6301251</v>
       </c>
       <c r="D90" t="n">
         <v>47</v>
@@ -10493,10 +10493,10 @@
         </is>
       </c>
       <c r="I90" t="n">
-        <v>67.28333333333333</v>
+        <v>67.2832438056665</v>
       </c>
       <c r="J90" t="n">
-        <v>-179.2666666666667</v>
+        <v>-179.2667561943335</v>
       </c>
       <c r="K90" t="n">
         <v>71.19337457593295</v>
@@ -10578,10 +10578,10 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>90103996.45974264</v>
+        <v>90103925.83790122</v>
       </c>
       <c r="C91" t="n">
-        <v>-175918496.8794327</v>
+        <v>-175918383.7433024</v>
       </c>
       <c r="D91" t="n">
         <v>47</v>
@@ -10607,10 +10607,10 @@
         </is>
       </c>
       <c r="I91" t="n">
-        <v>68.41666666666667</v>
+        <v>68.41667206489616</v>
       </c>
       <c r="J91" t="n">
-        <v>-179.8333333333333</v>
+        <v>-179.8333279351038</v>
       </c>
       <c r="K91" t="n">
         <v>70.98543786155993</v>
@@ -10696,10 +10696,10 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>99292045.85393476</v>
+        <v>99291195.39419353</v>
       </c>
       <c r="C92" t="n">
-        <v>-180337952.3938077</v>
+        <v>-180336735.1781213</v>
       </c>
       <c r="D92" t="n">
         <v>47</v>
@@ -10725,10 +10725,10 @@
         </is>
       </c>
       <c r="I92" t="n">
-        <v>67.08333333333333</v>
+        <v>67.08339802509568</v>
       </c>
       <c r="J92" t="n">
-        <v>-176.0833333333333</v>
+        <v>-176.083268641571</v>
       </c>
       <c r="K92" t="n">
         <v>71.29676060575669</v>
@@ -10810,10 +10810,10 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>89515881.81893797</v>
+        <v>89515138.18118136</v>
       </c>
       <c r="C93" t="n">
-        <v>-174796885.38356</v>
+        <v>-174795692.2836212</v>
       </c>
       <c r="D93" t="n">
         <v>47</v>
@@ -10839,10 +10839,10 @@
         </is>
       </c>
       <c r="I93" t="n">
-        <v>68.45</v>
+        <v>68.4500570897184</v>
       </c>
       <c r="J93" t="n">
-        <v>-179.7</v>
+        <v>-179.6999429102816</v>
       </c>
       <c r="K93" t="n">
         <v>70.91689115035416</v>
@@ -10920,10 +10920,10 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>90103996.45974264</v>
+        <v>90104599.81563872</v>
       </c>
       <c r="C94" t="n">
-        <v>-175918496.8794327</v>
+        <v>-175919463.4535802</v>
       </c>
       <c r="D94" t="n">
         <v>47</v>
@@ -10949,10 +10949,10 @@
         </is>
       </c>
       <c r="I94" t="n">
-        <v>68.41666666666667</v>
+        <v>68.41662054712215</v>
       </c>
       <c r="J94" t="n">
-        <v>-179.8333333333333</v>
+        <v>-179.8333794528778</v>
       </c>
       <c r="K94" t="n">
         <v>70.77812095247586</v>
@@ -11030,10 +11030,10 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>89566723.90536708</v>
+        <v>89566559.09773922</v>
       </c>
       <c r="C95" t="n">
-        <v>-174937869.9467148</v>
+        <v>-174937605.485363</v>
       </c>
       <c r="D95" t="n">
         <v>47</v>
@@ -11059,10 +11059,10 @@
         </is>
       </c>
       <c r="I95" t="n">
-        <v>68.45</v>
+        <v>68.45001264493334</v>
       </c>
       <c r="J95" t="n">
-        <v>-179.7333333333333</v>
+        <v>-179.7333206884</v>
       </c>
       <c r="K95" t="n">
         <v>70.72489779639045</v>
@@ -11140,10 +11140,10 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>105284087.2029519</v>
+        <v>105283032.7366307</v>
       </c>
       <c r="C96" t="n">
-        <v>-180789466.1385245</v>
+        <v>-180788096.2565957</v>
       </c>
       <c r="D96" t="n">
         <v>47</v>
@@ -11169,10 +11169,10 @@
         </is>
       </c>
       <c r="I96" t="n">
-        <v>66.09999999999999</v>
+        <v>66.10008077205472</v>
       </c>
       <c r="J96" t="n">
-        <v>-173.25</v>
+        <v>-173.2499192279453</v>
       </c>
       <c r="K96" t="n">
         <v>71.15616218386189</v>
@@ -11250,10 +11250,10 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>92664753.25568184</v>
+        <v>92664415.74031872</v>
       </c>
       <c r="C97" t="n">
-        <v>-179137645.1744695</v>
+        <v>-179137113.8263955</v>
       </c>
       <c r="D97" t="n">
         <v>47</v>
@@ -11279,10 +11279,10 @@
         </is>
       </c>
       <c r="I97" t="n">
-        <v>68.16666666666667</v>
+        <v>68.16669219156609</v>
       </c>
       <c r="J97" t="n">
-        <v>-179.6166666666667</v>
+        <v>-179.6166411417673</v>
       </c>
       <c r="K97" t="n">
         <v>70.79876037188845</v>
@@ -11368,10 +11368,10 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>105995749.0037229</v>
+        <v>105995905.4567777</v>
       </c>
       <c r="C98" t="n">
-        <v>-186983286.9084893</v>
+        <v>-186983498.0103559</v>
       </c>
       <c r="D98" t="n">
         <v>47</v>
@@ -11397,10 +11397,10 @@
         </is>
       </c>
       <c r="I98" t="n">
-        <v>66.40000000000001</v>
+        <v>66.39998833668601</v>
       </c>
       <c r="J98" t="n">
-        <v>-175.45</v>
+        <v>-175.450011663314</v>
       </c>
       <c r="K98" t="n">
         <v>70.71514182980424</v>
@@ -11482,10 +11482,10 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>111850064.579375</v>
+        <v>111850004.2022698</v>
       </c>
       <c r="C99" t="n">
-        <v>-203229137.2118905</v>
+        <v>-203229053.4905242</v>
       </c>
       <c r="D99" t="n">
         <v>47</v>
@@ -11511,10 +11511,10 @@
         </is>
       </c>
       <c r="I99" t="n">
-        <v>66.5</v>
+        <v>66.50000423063585</v>
       </c>
       <c r="J99" t="n">
-        <v>-179.15</v>
+        <v>-179.1499957693642</v>
       </c>
       <c r="K99" t="n">
         <v>70.59469167830773</v>
@@ -11596,10 +11596,10 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>108681298.5286668</v>
+        <v>108682215.0231036</v>
       </c>
       <c r="C100" t="n">
-        <v>-198148236.6325628</v>
+        <v>-198149523.846813</v>
       </c>
       <c r="D100" t="n">
         <v>47</v>
@@ -11625,10 +11625,10 @@
         </is>
       </c>
       <c r="I100" t="n">
-        <v>66.68333333333334</v>
+        <v>66.6832680201298</v>
       </c>
       <c r="J100" t="n">
-        <v>-178.6666666666667</v>
+        <v>-178.6667319798702</v>
       </c>
       <c r="K100" t="n">
         <v>70.73999999999998</v>
@@ -11706,10 +11706,10 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>123264265.9088128</v>
+        <v>123263194.7934499</v>
       </c>
       <c r="C101" t="n">
-        <v>-200774758.6199253</v>
+        <v>-200773555.3995813</v>
       </c>
       <c r="D101" t="n">
         <v>47</v>
@@ -11735,10 +11735,10 @@
         </is>
       </c>
       <c r="I101" t="n">
-        <v>64.65000000000001</v>
+        <v>64.65007690462897</v>
       </c>
       <c r="J101" t="n">
-        <v>-173.9166666666667</v>
+        <v>-173.9165897620377</v>
       </c>
       <c r="K101" t="n">
         <v>70.87592703948687</v>
@@ -11820,10 +11820,10 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>95284374.10084265</v>
+        <v>95284001.11153802</v>
       </c>
       <c r="C102" t="n">
-        <v>-181127008.4037445</v>
+        <v>-181126436.5794339</v>
       </c>
       <c r="D102" t="n">
         <v>47</v>
@@ -11849,10 +11849,10 @@
         </is>
       </c>
       <c r="I102" t="n">
-        <v>67.83333333333333</v>
+        <v>67.83336140894836</v>
       </c>
       <c r="J102" t="n">
-        <v>-178.8333333333333</v>
+        <v>-178.8333052577183</v>
       </c>
       <c r="K102" t="n">
         <v>70.27161476470002</v>
@@ -11934,10 +11934,10 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>103204631.5691882</v>
+        <v>103206311.7080425</v>
       </c>
       <c r="C103" t="n">
-        <v>-192250415.9355209</v>
+        <v>-192252878.875446</v>
       </c>
       <c r="D103" t="n">
         <v>47</v>
@@ -11963,10 +11963,10 @@
         </is>
       </c>
       <c r="I103" t="n">
-        <v>67.2</v>
+        <v>67.19987818182531</v>
       </c>
       <c r="J103" t="n">
-        <v>-179.0833333333333</v>
+        <v>-179.083455151508</v>
       </c>
       <c r="K103" t="n">
         <v>70.59823929571829</v>
@@ -12052,10 +12052,10 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>106043485.1668052</v>
+        <v>106044442.6357666</v>
       </c>
       <c r="C104" t="n">
-        <v>-192487223.5078029</v>
+        <v>-192488568.9412396</v>
       </c>
       <c r="D104" t="n">
         <v>47</v>
@@ -12081,10 +12081,10 @@
         </is>
       </c>
       <c r="I104" t="n">
-        <v>66.75</v>
+        <v>66.74993034355941</v>
       </c>
       <c r="J104" t="n">
-        <v>-177.6833333333333</v>
+        <v>-177.6834029897739</v>
       </c>
       <c r="K104" t="n">
         <v>70.8463005722317</v>
@@ -12166,10 +12166,10 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>97109254.17282365</v>
+        <v>97110995.55015253</v>
       </c>
       <c r="C105" t="n">
-        <v>-181414175.192572</v>
+        <v>-181416775.6881125</v>
       </c>
       <c r="D105" t="n">
         <v>47</v>
@@ -12195,10 +12195,10 @@
         </is>
       </c>
       <c r="I105" t="n">
-        <v>67.53333333333333</v>
+        <v>67.53320201763403</v>
       </c>
       <c r="J105" t="n">
-        <v>-177.8333333333333</v>
+        <v>-177.8334646490326</v>
       </c>
       <c r="K105" t="n">
         <v>70.29989040549964</v>
@@ -12280,10 +12280,10 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>131244616.2271291</v>
+        <v>131242611.0262185</v>
       </c>
       <c r="C106" t="n">
-        <v>-226694032.8228069</v>
+        <v>-226691592.6217423</v>
       </c>
       <c r="D106" t="n">
         <v>47</v>
@@ -12309,10 +12309,10 @@
         </is>
       </c>
       <c r="I106" t="n">
-        <v>65.08333333333333</v>
+        <v>65.08346460721658</v>
       </c>
       <c r="J106" t="n">
-        <v>-179.8333333333333</v>
+        <v>-179.83320205945</v>
       </c>
       <c r="K106" t="n">
         <v>70.11631374888159</v>
@@ -12394,10 +12394,10 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>117128874.3009306</v>
+        <v>117129515.137243</v>
       </c>
       <c r="C107" t="n">
-        <v>-199529013.1732362</v>
+        <v>-199529806.5510803</v>
       </c>
       <c r="D107" t="n">
         <v>47</v>
@@ -12423,10 +12423,10 @@
         </is>
       </c>
       <c r="I107" t="n">
-        <v>65.46666666666667</v>
+        <v>65.46662074064554</v>
       </c>
       <c r="J107" t="n">
-        <v>-175.55</v>
+        <v>-175.5500459260211</v>
       </c>
       <c r="K107" t="n">
         <v>70.5480827143144</v>
@@ -12508,10 +12508,10 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>94927905.58056711</v>
+        <v>94929093.34019737</v>
       </c>
       <c r="C108" t="n">
-        <v>-181959714.6332012</v>
+        <v>-181961555.8396538</v>
       </c>
       <c r="D108" t="n">
         <v>47</v>
@@ -12537,10 +12537,10 @@
         </is>
       </c>
       <c r="I108" t="n">
-        <v>67.95</v>
+        <v>67.94991100094209</v>
       </c>
       <c r="J108" t="n">
-        <v>-179.45</v>
+        <v>-179.4500889990579</v>
       </c>
       <c r="K108" t="n">
         <v>69.97702068138675</v>
@@ -12622,10 +12622,10 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>108290844.4657277</v>
+        <v>108291038.0034577</v>
       </c>
       <c r="C109" t="n">
-        <v>-179956991.4277062</v>
+        <v>-179957228.0258081</v>
       </c>
       <c r="D109" t="n">
         <v>47</v>
@@ -12651,10 +12651,10 @@
         </is>
       </c>
       <c r="I109" t="n">
-        <v>65.55</v>
+        <v>65.54998505796823</v>
       </c>
       <c r="J109" t="n">
-        <v>-171.6333333333333</v>
+        <v>-171.6333482753651</v>
       </c>
       <c r="K109" t="n">
         <v>70.32238626092196</v>
@@ -12736,10 +12736,10 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>88935099.59304748</v>
+        <v>88934289.42342946</v>
       </c>
       <c r="C110" t="n">
-        <v>-170948659.5389487</v>
+        <v>-170947381.6615569</v>
       </c>
       <c r="D110" t="n">
         <v>47</v>
@@ -12765,10 +12765,10 @@
         </is>
       </c>
       <c r="I110" t="n">
-        <v>68.3</v>
+        <v>68.30006331731207</v>
       </c>
       <c r="J110" t="n">
-        <v>-178.2</v>
+        <v>-178.1999366826879</v>
       </c>
       <c r="K110" t="n">
         <v>69.7549312612074</v>
@@ -12854,10 +12854,10 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>103971849.2538242</v>
+        <v>103973242.3097483</v>
       </c>
       <c r="C111" t="n">
-        <v>-177148130.6374139</v>
+        <v>-177149926.3409938</v>
       </c>
       <c r="D111" t="n">
         <v>47</v>
@@ -12883,10 +12883,10 @@
         </is>
       </c>
       <c r="I111" t="n">
-        <v>66.06666666666666</v>
+        <v>66.06655834058715</v>
       </c>
       <c r="J111" t="n">
-        <v>-172.35</v>
+        <v>-172.3501083260795</v>
       </c>
       <c r="K111" t="n">
         <v>69.81847197287053</v>
@@ -12964,10 +12964,10 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>112619027.8978438</v>
+        <v>112619363.6736304</v>
       </c>
       <c r="C112" t="n">
-        <v>-204630160.0728068</v>
+        <v>-204630624.7919917</v>
       </c>
       <c r="D112" t="n">
         <v>47</v>
@@ -12993,10 +12993,10 @@
         </is>
       </c>
       <c r="I112" t="n">
-        <v>66.46666666666667</v>
+        <v>66.46664325015371</v>
       </c>
       <c r="J112" t="n">
-        <v>-179.3333333333333</v>
+        <v>-179.3333567498462</v>
       </c>
       <c r="K112" t="n">
         <v>69.63272618692147</v>
@@ -13074,10 +13074,10 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>90460392.6231131</v>
+        <v>90461016.56727831</v>
       </c>
       <c r="C113" t="n">
-        <v>-173375664.0443612</v>
+        <v>-173376641.2661828</v>
       </c>
       <c r="D113" t="n">
         <v>47</v>
@@ -13103,10 +13103,10 @@
         </is>
       </c>
       <c r="I113" t="n">
-        <v>68.18333333333334</v>
+        <v>68.18328501231335</v>
       </c>
       <c r="J113" t="n">
-        <v>-178.3333333333333</v>
+        <v>-178.3333816543533</v>
       </c>
       <c r="K113" t="n">
         <v>69.46762018275724</v>
@@ -13192,10 +13192,10 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>90322822.99425556</v>
+        <v>90323452.64385182</v>
       </c>
       <c r="C114" t="n">
-        <v>-173249626.158198</v>
+        <v>-173250613.5704355</v>
       </c>
       <c r="D114" t="n">
         <v>47</v>
@@ -13221,10 +13221,10 @@
         </is>
       </c>
       <c r="I114" t="n">
-        <v>68.2</v>
+        <v>68.1999512195265</v>
       </c>
       <c r="J114" t="n">
-        <v>-178.3666666666667</v>
+        <v>-178.3667154471402</v>
       </c>
       <c r="K114" t="n">
         <v>69.40848436566421</v>
@@ -13310,10 +13310,10 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>127185395.2545457</v>
+        <v>127185600.9567544</v>
       </c>
       <c r="C115" t="n">
-        <v>-222549368.7669788</v>
+        <v>-222549627.4635976</v>
       </c>
       <c r="D115" t="n">
         <v>47</v>
@@ -13339,10 +13339,10 @@
         </is>
       </c>
       <c r="I115" t="n">
-        <v>65.40000000000001</v>
+        <v>65.39998638549125</v>
       </c>
       <c r="J115" t="n">
-        <v>-179.85</v>
+        <v>-179.8500136145088</v>
       </c>
       <c r="K115" t="n">
         <v>69.9488105992171</v>
@@ -13416,10 +13416,10 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>104322746.363537</v>
+        <v>104323840.462929</v>
       </c>
       <c r="C116" t="n">
-        <v>-179674902.4374239</v>
+        <v>-179676334.3504549</v>
       </c>
       <c r="D116" t="n">
         <v>47</v>
@@ -13445,10 +13445,10 @@
         </is>
       </c>
       <c r="I116" t="n">
-        <v>66.18333333333334</v>
+        <v>66.18324920806168</v>
       </c>
       <c r="J116" t="n">
-        <v>-173.2333333333333</v>
+        <v>-173.2334174586049</v>
       </c>
       <c r="K116" t="n">
         <v>69.41258601775206</v>
@@ -13526,10 +13526,10 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>104883914.7120557</v>
+        <v>104885273.8681174</v>
       </c>
       <c r="C117" t="n">
-        <v>-183985993.9971741</v>
+        <v>-183987818.6619841</v>
       </c>
       <c r="D117" t="n">
         <v>47</v>
@@ -13555,10 +13555,10 @@
         </is>
       </c>
       <c r="I117" t="n">
-        <v>66.38333333333334</v>
+        <v>66.38323079425454</v>
       </c>
       <c r="J117" t="n">
-        <v>-174.75</v>
+        <v>-174.7501025390788</v>
       </c>
       <c r="K117" t="n">
         <v>69.68847039967945</v>
@@ -13644,10 +13644,10 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>120625228.7227587</v>
+        <v>120626242.0701926</v>
       </c>
       <c r="C118" t="n">
-        <v>-201105858.6705678</v>
+        <v>-201107055.5776693</v>
       </c>
       <c r="D118" t="n">
         <v>47</v>
@@ -13673,10 +13673,10 @@
         </is>
       </c>
       <c r="I118" t="n">
-        <v>65.05</v>
+        <v>65.04992755189618</v>
       </c>
       <c r="J118" t="n">
-        <v>-174.8666666666667</v>
+        <v>-174.8667391147705</v>
       </c>
       <c r="K118" t="n">
         <v>69.19544819325213</v>
@@ -13754,10 +13754,10 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>106252700.4338813</v>
+        <v>106254081.1004089</v>
       </c>
       <c r="C119" t="n">
-        <v>-191198951.3299352</v>
+        <v>-191200866.8442713</v>
       </c>
       <c r="D119" t="n">
         <v>47</v>
@@ -13783,10 +13783,10 @@
         </is>
       </c>
       <c r="I119" t="n">
-        <v>66.63333333333334</v>
+        <v>66.63323228473124</v>
       </c>
       <c r="J119" t="n">
-        <v>-177.05</v>
+        <v>-177.0501010486021</v>
       </c>
       <c r="K119" t="n">
         <v>69.24767709061842</v>
@@ -13860,10 +13860,10 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>93419264.31423302</v>
+        <v>93418420.93201588</v>
       </c>
       <c r="C120" t="n">
-        <v>-177884624.4752734</v>
+        <v>-177883323.0553674</v>
       </c>
       <c r="D120" t="n">
         <v>47</v>
@@ -13889,10 +13889,10 @@
         </is>
       </c>
       <c r="I120" t="n">
-        <v>67.95</v>
+        <v>67.95006425270499</v>
       </c>
       <c r="J120" t="n">
-        <v>-178.5166666666667</v>
+        <v>-178.5166024139617</v>
       </c>
       <c r="K120" t="n">
         <v>69.16475401656521</v>
@@ -13970,10 +13970,10 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>90103996.45974264</v>
+        <v>90102621.94079775</v>
       </c>
       <c r="C121" t="n">
-        <v>-175918496.8794327</v>
+        <v>-175916294.8946933</v>
       </c>
       <c r="D121" t="n">
         <v>47</v>
@@ -13999,10 +13999,10 @@
         </is>
       </c>
       <c r="I121" t="n">
-        <v>68.41666666666667</v>
+        <v>68.4167717332719</v>
       </c>
       <c r="J121" t="n">
-        <v>-179.8333333333333</v>
+        <v>-179.833228266728</v>
       </c>
       <c r="K121" t="n">
         <v>69.07894736842105</v>
@@ -14084,10 +14084,10 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>89438875.47264081</v>
+        <v>89439994.28489967</v>
       </c>
       <c r="C122" t="n">
-        <v>-171830953.8393525</v>
+        <v>-171832715.3857557</v>
       </c>
       <c r="D122" t="n">
         <v>47</v>
@@ -14113,10 +14113,10 @@
         </is>
       </c>
       <c r="I122" t="n">
-        <v>68.26666666666667</v>
+        <v>68.26657952686253</v>
       </c>
       <c r="J122" t="n">
-        <v>-178.2833333333333</v>
+        <v>-178.2834204731374</v>
       </c>
       <c r="K122" t="n">
         <v>69.26536731634184</v>
@@ -14202,10 +14202,10 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>90056280.89464915</v>
+        <v>90056071.40156201</v>
       </c>
       <c r="C123" t="n">
-        <v>-172771877.2222292</v>
+        <v>-172771548.4129456</v>
       </c>
       <c r="D123" t="n">
         <v>47</v>
@@ -14231,10 +14231,10 @@
         </is>
       </c>
       <c r="I123" t="n">
-        <v>68.21666666666667</v>
+        <v>68.21668292665927</v>
       </c>
       <c r="J123" t="n">
-        <v>-178.3166666666667</v>
+        <v>-178.3166504066741</v>
       </c>
       <c r="K123" t="n">
         <v>69.16391968834283</v>
@@ -14320,10 +14320,10 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>112340498.6061008</v>
+        <v>112339625.2761361</v>
       </c>
       <c r="C124" t="n">
-        <v>-191250127.3640674</v>
+        <v>-191249031.5810917</v>
       </c>
       <c r="D124" t="n">
         <v>47</v>
@@ -14349,10 +14349,10 @@
         </is>
       </c>
       <c r="I124" t="n">
-        <v>65.66666666666667</v>
+        <v>65.66673111396588</v>
       </c>
       <c r="J124" t="n">
-        <v>-174.35</v>
+        <v>-174.3499355527008</v>
       </c>
       <c r="K124" t="n">
         <v>69.03406253121565</v>
@@ -14426,10 +14426,10 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>91637457.91925877</v>
+        <v>91638675.91084142</v>
       </c>
       <c r="C125" t="n">
-        <v>-174578910.7106527</v>
+        <v>-174580799.3188672</v>
       </c>
       <c r="D125" t="n">
         <v>47</v>
@@ -14455,10 +14455,10 @@
         </is>
       </c>
       <c r="I125" t="n">
-        <v>68.05</v>
+        <v>68.04990602153245</v>
       </c>
       <c r="J125" t="n">
-        <v>-178.1166666666667</v>
+        <v>-178.1167606451342</v>
       </c>
       <c r="K125" t="n">
         <v>68.38863500894098</v>
@@ -14536,10 +14536,10 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>104043059.8112647</v>
+        <v>104042168.0730878</v>
       </c>
       <c r="C126" t="n">
-        <v>-182407022.5705877</v>
+        <v>-182405823.5215728</v>
       </c>
       <c r="D126" t="n">
         <v>47</v>
@@ -14565,10 +14565,10 @@
         </is>
       </c>
       <c r="I126" t="n">
-        <v>66.41666666666667</v>
+        <v>66.41673434655264</v>
       </c>
       <c r="J126" t="n">
-        <v>-174.5</v>
+        <v>-174.499932320114</v>
       </c>
       <c r="K126" t="n">
         <v>69.03135048231512</v>
@@ -14650,10 +14650,10 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>98433737.48922175</v>
+        <v>98433685.40547928</v>
       </c>
       <c r="C127" t="n">
-        <v>-164848683.7189589</v>
+        <v>-164848617.1248325</v>
       </c>
       <c r="D127" t="n">
         <v>47</v>
@@ -14679,10 +14679,10 @@
         </is>
       </c>
       <c r="I127" t="n">
-        <v>66.13333333333334</v>
+        <v>66.13333759743972</v>
       </c>
       <c r="J127" t="n">
-        <v>-169.7</v>
+        <v>-169.6999957358936</v>
       </c>
       <c r="K127" t="n">
         <v>68.49137501246383</v>
@@ -14768,10 +14768,10 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>90103996.45974264</v>
+        <v>90105029.24682693</v>
       </c>
       <c r="C128" t="n">
-        <v>-175918496.8794327</v>
+        <v>-175920151.3993</v>
       </c>
       <c r="D128" t="n">
         <v>47</v>
@@ -14797,10 +14797,10 @@
         </is>
       </c>
       <c r="I128" t="n">
-        <v>68.41666666666667</v>
+        <v>68.41658772219928</v>
       </c>
       <c r="J128" t="n">
-        <v>-179.8333333333333</v>
+        <v>-179.8334122778007</v>
       </c>
       <c r="K128" t="n">
         <v>68.63627274545091</v>
@@ -14878,10 +14878,10 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>105295142.5592089</v>
+        <v>105297571.7318893</v>
       </c>
       <c r="C129" t="n">
-        <v>-186001124.266245</v>
+        <v>-186004414.8481569</v>
       </c>
       <c r="D129" t="n">
         <v>47</v>
@@ -14907,10 +14907,10 @@
         </is>
       </c>
       <c r="I129" t="n">
-        <v>66.45</v>
+        <v>66.44981829372792</v>
       </c>
       <c r="J129" t="n">
-        <v>-175.3833333333333</v>
+        <v>-175.3835150396054</v>
       </c>
       <c r="K129" t="n">
         <v>68.87550200803211</v>
@@ -14992,10 +14992,10 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>91507304.90359768</v>
+        <v>91506452.89152119</v>
       </c>
       <c r="C130" t="n">
-        <v>-168657511.852959</v>
+        <v>-168656243.1493973</v>
       </c>
       <c r="D130" t="n">
         <v>47</v>
@@ -15021,10 +15021,10 @@
         </is>
       </c>
       <c r="I130" t="n">
-        <v>67.66666666666667</v>
+        <v>67.66673433990181</v>
       </c>
       <c r="J130" t="n">
-        <v>-175.3333333333333</v>
+        <v>-175.3332656600982</v>
       </c>
       <c r="K130" t="n">
         <v>68.60955056179776</v>
@@ -15106,10 +15106,10 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>100244311.317205</v>
+        <v>100244127.4586507</v>
       </c>
       <c r="C131" t="n">
-        <v>-181532192.037241</v>
+        <v>-181531930.5944287</v>
       </c>
       <c r="D131" t="n">
         <v>47</v>
@@ -15135,10 +15135,10 @@
         </is>
       </c>
       <c r="I131" t="n">
-        <v>67</v>
+        <v>67.00001392915915</v>
       </c>
       <c r="J131" t="n">
-        <v>-176.0833333333333</v>
+        <v>-176.0833194041741</v>
       </c>
       <c r="K131" t="n">
         <v>68.39523475823404</v>
@@ -15220,10 +15220,10 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>90931829.25551559</v>
+        <v>90930277.77780448</v>
       </c>
       <c r="C132" t="n">
-        <v>-173662932.8158309</v>
+        <v>-173660515.8562022</v>
       </c>
       <c r="D132" t="n">
         <v>47</v>
@@ -15249,10 +15249,10 @@
         </is>
       </c>
       <c r="I132" t="n">
-        <v>68.11666666666666</v>
+        <v>68.11678675721816</v>
       </c>
       <c r="J132" t="n">
-        <v>-178.15</v>
+        <v>-178.1498799094485</v>
       </c>
       <c r="K132" t="n">
         <v>67.96174536760311</v>
@@ -15334,10 +15334,10 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>89886095.87301485</v>
+        <v>89886613.54807913</v>
       </c>
       <c r="C133" t="n">
-        <v>-175569246.7581899</v>
+        <v>-175570076.8970628</v>
       </c>
       <c r="D133" t="n">
         <v>47</v>
@@ -15363,10 +15363,10 @@
         </is>
       </c>
       <c r="I133" t="n">
-        <v>68.43333333333334</v>
+        <v>68.43329371234678</v>
       </c>
       <c r="J133" t="n">
-        <v>-179.8166666666667</v>
+        <v>-179.8167062876532</v>
       </c>
       <c r="K133" t="n">
         <v>67.66347687400319</v>
@@ -15444,10 +15444,10 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>102208251.7804037</v>
+        <v>102207984.6576595</v>
       </c>
       <c r="C134" t="n">
-        <v>-187580400.5637736</v>
+        <v>-187580015.7520474</v>
       </c>
       <c r="D134" t="n">
         <v>47</v>
@@ -15473,10 +15473,10 @@
         </is>
       </c>
       <c r="I134" t="n">
-        <v>67.06666666666666</v>
+        <v>67.06668641223058</v>
       </c>
       <c r="J134" t="n">
-        <v>-177.6333333333333</v>
+        <v>-177.6333135877694</v>
       </c>
       <c r="K134" t="n">
         <v>67.53905861279729</v>
@@ -15562,10 +15562,10 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>105296593.0105529</v>
+        <v>105297903.1240131</v>
       </c>
       <c r="C135" t="n">
-        <v>-174150971.1252465</v>
+        <v>-174152576.490499</v>
       </c>
       <c r="D135" t="n">
         <v>47</v>
@@ -15591,10 +15591,10 @@
         </is>
       </c>
       <c r="I135" t="n">
-        <v>65.63333333333334</v>
+        <v>65.63322982578258</v>
       </c>
       <c r="J135" t="n">
-        <v>-170.55</v>
+        <v>-170.5501035075508</v>
       </c>
       <c r="K135" t="n">
         <v>67.92585170340682</v>
@@ -15676,10 +15676,10 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>94630828.93782759</v>
+        <v>94630448.58195198</v>
       </c>
       <c r="C136" t="n">
-        <v>-179374031.6436072</v>
+        <v>-179373449.67</v>
       </c>
       <c r="D136" t="n">
         <v>47</v>
@@ -15705,10 +15705,10 @@
         </is>
       </c>
       <c r="I136" t="n">
-        <v>67.83333333333333</v>
+        <v>67.83336216811897</v>
       </c>
       <c r="J136" t="n">
-        <v>-178.4333333333333</v>
+        <v>-178.4333044985477</v>
       </c>
       <c r="K136" t="n">
         <v>67.46134663341647</v>
@@ -15790,10 +15790,10 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>103647846.1349454</v>
+        <v>103648394.1056142</v>
       </c>
       <c r="C137" t="n">
-        <v>-182662819.6936542</v>
+        <v>-182663562.9066028</v>
       </c>
       <c r="D137" t="n">
         <v>47</v>
@@ -15819,10 +15819,10 @@
         </is>
       </c>
       <c r="I137" t="n">
-        <v>66.5</v>
+        <v>66.49995848417912</v>
       </c>
       <c r="J137" t="n">
-        <v>-174.8</v>
+        <v>-174.8000415158209</v>
       </c>
       <c r="K137" t="n">
         <v>67.4074074074074</v>
@@ -15904,10 +15904,10 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>98267514.86073907</v>
+        <v>98266681.69730829</v>
       </c>
       <c r="C138" t="n">
-        <v>-180678614.399678</v>
+        <v>-180677399.1216154</v>
       </c>
       <c r="D138" t="n">
         <v>47</v>
@@ -15933,10 +15933,10 @@
         </is>
       </c>
       <c r="I138" t="n">
-        <v>67.28333333333333</v>
+        <v>67.28339650198974</v>
       </c>
       <c r="J138" t="n">
-        <v>-176.8166666666667</v>
+        <v>-176.8166034980103</v>
       </c>
       <c r="K138" t="n">
         <v>67.05577172503243</v>
@@ -16014,10 +16014,10 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>119294747.7463775</v>
+        <v>119294187.3056267</v>
       </c>
       <c r="C139" t="n">
-        <v>-214137032.3292559</v>
+        <v>-214136283.2011814</v>
       </c>
       <c r="D139" t="n">
         <v>47</v>
@@ -16043,10 +16043,10 @@
         </is>
       </c>
       <c r="I139" t="n">
-        <v>66.03333333333333</v>
+        <v>66.03337128277319</v>
       </c>
       <c r="J139" t="n">
-        <v>-179.95</v>
+        <v>-179.9499620505601</v>
       </c>
       <c r="K139" t="n">
         <v>66.98084829038403</v>
@@ -16128,10 +16128,10 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>108799342.8716356</v>
+        <v>108799312.6881271</v>
       </c>
       <c r="C140" t="n">
-        <v>-196582679.2592897</v>
+        <v>-196582637.4172918</v>
       </c>
       <c r="D140" t="n">
         <v>47</v>
@@ -16157,10 +16157,10 @@
         </is>
       </c>
       <c r="I140" t="n">
-        <v>66.56666666666666</v>
+        <v>66.56666883258055</v>
       </c>
       <c r="J140" t="n">
-        <v>-177.9833333333333</v>
+        <v>-177.9833311674194</v>
       </c>
       <c r="K140" t="n">
         <v>66.63673550833083</v>
@@ -16238,10 +16238,10 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>90649783.85114792</v>
+        <v>90651463.50287198</v>
       </c>
       <c r="C141" t="n">
-        <v>-173642220.5342466</v>
+        <v>-173644848.279627</v>
       </c>
       <c r="D141" t="n">
         <v>47</v>
@@ -16267,10 +16267,10 @@
         </is>
       </c>
       <c r="I141" t="n">
-        <v>68.16666666666667</v>
+        <v>68.1665367111958</v>
       </c>
       <c r="J141" t="n">
-        <v>-178.3333333333333</v>
+        <v>-178.3334632888042</v>
       </c>
       <c r="K141" t="n">
         <v>66.73001900570171</v>
@@ -16356,10 +16356,10 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>109559818.9381728</v>
+        <v>109559762.8263735</v>
       </c>
       <c r="C142" t="n">
-        <v>-185388426.5181114</v>
+        <v>-185388356.1909328</v>
       </c>
       <c r="D142" t="n">
         <v>47</v>
@@ -16385,10 +16385,10 @@
         </is>
       </c>
       <c r="I142" t="n">
-        <v>65.71666666666667</v>
+        <v>65.71667090057571</v>
       </c>
       <c r="J142" t="n">
-        <v>-173.2333333333333</v>
+        <v>-173.2333290994243</v>
       </c>
       <c r="K142" t="n">
         <v>66.67000100030009</v>
@@ -16466,10 +16466,10 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>103634873.023112</v>
+        <v>103634673.1074151</v>
       </c>
       <c r="C143" t="n">
-        <v>-181891736.5182458</v>
+        <v>-181891466.9635093</v>
       </c>
       <c r="D143" t="n">
         <v>47</v>
@@ -16495,10 +16495,10 @@
         </is>
       </c>
       <c r="I143" t="n">
-        <v>66.45</v>
+        <v>66.45001519971581</v>
       </c>
       <c r="J143" t="n">
-        <v>-174.4833333333333</v>
+        <v>-174.4833181336175</v>
       </c>
       <c r="K143" t="n">
         <v>66.78722121760097</v>
@@ -16584,10 +16584,10 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>93414531.88644587</v>
+        <v>93414692.50158627</v>
       </c>
       <c r="C144" t="n">
-        <v>-163614092.342849</v>
+        <v>-163614314.8440734</v>
       </c>
       <c r="D144" t="n">
         <v>47</v>
@@ -16613,10 +16613,10 @@
         </is>
       </c>
       <c r="I144" t="n">
-        <v>66.95</v>
+        <v>66.94998687113755</v>
       </c>
       <c r="J144" t="n">
-        <v>-171.7666666666667</v>
+        <v>-171.7666797955291</v>
       </c>
       <c r="K144" t="n">
         <v>66.4894150697301</v>
@@ -16698,10 +16698,10 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>119402144.3029108</v>
+        <v>119403173.9746964</v>
       </c>
       <c r="C145" t="n">
-        <v>-193068783.1791871</v>
+        <v>-193069939.7414641</v>
       </c>
       <c r="D145" t="n">
         <v>47</v>
@@ -16727,10 +16727,10 @@
         </is>
       </c>
       <c r="I145" t="n">
-        <v>64.71666666666667</v>
+        <v>64.71659064187352</v>
       </c>
       <c r="J145" t="n">
-        <v>-172.5</v>
+        <v>-172.5000760247931</v>
       </c>
       <c r="K145" t="n">
         <v>65.58376649340263</v>
@@ -16808,10 +16808,10 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>91237707.20005527</v>
+        <v>91237591.3195311</v>
       </c>
       <c r="C146" t="n">
-        <v>-174741473.3009983</v>
+        <v>-174741292.29525</v>
       </c>
       <c r="D146" t="n">
         <v>47</v>
@@ -16837,10 +16837,10 @@
         </is>
       </c>
       <c r="I146" t="n">
-        <v>68.13333333333334</v>
+        <v>68.13334226087335</v>
       </c>
       <c r="J146" t="n">
-        <v>-178.4666666666667</v>
+        <v>-178.4666577391267</v>
       </c>
       <c r="K146" t="n">
         <v>65.76413959085438</v>
@@ -16926,10 +16926,10 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>107560858.2974484</v>
+        <v>107559905.6503057</v>
       </c>
       <c r="C147" t="n">
-        <v>-196356017.1712792</v>
+        <v>-196354673.0070667</v>
       </c>
       <c r="D147" t="n">
         <v>47</v>
@@ -16955,10 +16955,10 @@
         </is>
       </c>
       <c r="I147" t="n">
-        <v>66.75</v>
+        <v>66.7500683016478</v>
       </c>
       <c r="J147" t="n">
-        <v>-178.5</v>
+        <v>-178.4999316983522</v>
       </c>
       <c r="K147" t="n">
         <v>65.23947027780544</v>
@@ -17036,10 +17036,10 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>125910981.5746388</v>
+        <v>125912277.5563406</v>
       </c>
       <c r="C148" t="n">
-        <v>-202192984.9374151</v>
+        <v>-202194389.5591151</v>
       </c>
       <c r="D148" t="n">
         <v>47</v>
@@ -17065,10 +17065,10 @@
         </is>
       </c>
       <c r="I148" t="n">
-        <v>64.36666666666666</v>
+        <v>64.36657390169819</v>
       </c>
       <c r="J148" t="n">
-        <v>-173.6166666666667</v>
+        <v>-173.6167594316352</v>
       </c>
       <c r="K148" t="n">
         <v>65.53417518540789</v>
@@ -17150,10 +17150,10 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>107664801.1138998</v>
+        <v>107665495.2339031</v>
       </c>
       <c r="C149" t="n">
-        <v>-194505614.1276624</v>
+        <v>-194506578.9795287</v>
       </c>
       <c r="D149" t="n">
         <v>47</v>
@@ -17179,10 +17179,10 @@
         </is>
       </c>
       <c r="I149" t="n">
-        <v>66.61666666666666</v>
+        <v>66.61661649160766</v>
       </c>
       <c r="J149" t="n">
-        <v>-177.7</v>
+        <v>-177.700050175059</v>
       </c>
       <c r="K149" t="n">
         <v>65.22738630684657</v>
@@ -17260,10 +17260,10 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>96675750.00955042</v>
+        <v>96673180.40597731</v>
       </c>
       <c r="C150" t="n">
-        <v>-182295869.3714011</v>
+        <v>-182291982.2595517</v>
       </c>
       <c r="D150" t="n">
         <v>47</v>
@@ -17289,10 +17289,10 @@
         </is>
       </c>
       <c r="I150" t="n">
-        <v>67.66666666666667</v>
+        <v>67.66685949910348</v>
       </c>
       <c r="J150" t="n">
-        <v>-178.5</v>
+        <v>-178.4998071675632</v>
       </c>
       <c r="K150" t="n">
         <v>65.2369526094781</v>
@@ -17370,10 +17370,10 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>105034908.8301694</v>
+        <v>105035929.1928367</v>
       </c>
       <c r="C151" t="n">
-        <v>-185856805.7194933</v>
+        <v>-185858192.3171963</v>
       </c>
       <c r="D151" t="n">
         <v>47</v>
@@ -17399,10 +17399,10 @@
         </is>
       </c>
       <c r="I151" t="n">
-        <v>66.48333333333333</v>
+        <v>66.48325698771632</v>
       </c>
       <c r="J151" t="n">
-        <v>-175.45</v>
+        <v>-175.450076345617</v>
       </c>
       <c r="K151" t="n">
         <v>65.14576677316293</v>
@@ -17484,10 +17484,10 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>129709770.814583</v>
+        <v>129710198.4596708</v>
       </c>
       <c r="C152" t="n">
-        <v>-224507859.3043121</v>
+        <v>-224508383.7818565</v>
       </c>
       <c r="D152" t="n">
         <v>47</v>
@@ -17513,10 +17513,10 @@
         </is>
       </c>
       <c r="I152" t="n">
-        <v>65.16666666666667</v>
+        <v>65.16663848931606</v>
       </c>
       <c r="J152" t="n">
-        <v>-179.6333333333333</v>
+        <v>-179.6333615106839</v>
       </c>
       <c r="K152" t="n">
         <v>65.30161597912276</v>
@@ -17590,10 +17590,10 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>110113416.0791342</v>
+        <v>110114046.0511149</v>
       </c>
       <c r="C153" t="n">
-        <v>-198836178.6264879</v>
+        <v>-198837048.2266916</v>
       </c>
       <c r="D153" t="n">
         <v>47</v>
@@ -17619,10 +17619,10 @@
         </is>
       </c>
       <c r="I153" t="n">
-        <v>66.5</v>
+        <v>66.49995514339913</v>
       </c>
       <c r="J153" t="n">
-        <v>-178.25</v>
+        <v>-178.2500448566009</v>
       </c>
       <c r="K153" t="n">
         <v>65.25798032523589</v>
@@ -17704,10 +17704,10 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>95344254.52384453</v>
+        <v>95345677.07905038</v>
       </c>
       <c r="C154" t="n">
-        <v>-180778271.406379</v>
+        <v>-180780445.0931121</v>
       </c>
       <c r="D154" t="n">
         <v>47</v>
@@ -17733,10 +17733,10 @@
         </is>
       </c>
       <c r="I154" t="n">
-        <v>67.8</v>
+        <v>67.7998927347974</v>
       </c>
       <c r="J154" t="n">
-        <v>-178.6333333333333</v>
+        <v>-178.6334405985359</v>
       </c>
       <c r="K154" t="n">
         <v>64.6935516071072</v>
@@ -17814,10 +17814,10 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>119326691.2342879</v>
+        <v>119325984.7731324</v>
       </c>
       <c r="C155" t="n">
-        <v>-200736715.1884735</v>
+        <v>-200735864.3579961</v>
       </c>
       <c r="D155" t="n">
         <v>47</v>
@@ -17843,10 +17843,10 @@
         </is>
       </c>
       <c r="I155" t="n">
-        <v>65.21666666666667</v>
+        <v>65.21671717554545</v>
       </c>
       <c r="J155" t="n">
-        <v>-175.1833333333333</v>
+        <v>-175.1832828244545</v>
       </c>
       <c r="K155" t="n">
         <v>64.60079840319362</v>
@@ -17928,10 +17928,10 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>93427617.83138026</v>
+        <v>93428580.87039356</v>
       </c>
       <c r="C156" t="n">
-        <v>-177404317.869261</v>
+        <v>-177405798.8254772</v>
       </c>
       <c r="D156" t="n">
         <v>47</v>
@@ -17957,10 +17957,10 @@
         </is>
       </c>
       <c r="I156" t="n">
-        <v>67.91666666666667</v>
+        <v>67.91659312823128</v>
       </c>
       <c r="J156" t="n">
-        <v>-178.2833333333333</v>
+        <v>-178.2834068717687</v>
       </c>
       <c r="K156" t="n">
         <v>64.42518429966128</v>
@@ -18038,10 +18038,10 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>114373560.9518803</v>
+        <v>114373753.1311606</v>
       </c>
       <c r="C157" t="n">
-        <v>-190704983.4679076</v>
+        <v>-190705215.0722503</v>
       </c>
       <c r="D157" t="n">
         <v>47</v>
@@ -18067,10 +18067,10 @@
         </is>
       </c>
       <c r="I157" t="n">
-        <v>65.31666666666666</v>
+        <v>65.31665241504226</v>
       </c>
       <c r="J157" t="n">
-        <v>-173.3666666666667</v>
+        <v>-173.3666809182911</v>
       </c>
       <c r="K157" t="n">
         <v>64.75541299117882</v>
@@ -18148,10 +18148,10 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>104586603.4806901</v>
+        <v>104586924.6323144</v>
       </c>
       <c r="C158" t="n">
-        <v>-174358647.206953</v>
+        <v>-174359046.694427</v>
       </c>
       <c r="D158" t="n">
         <v>47</v>
@@ -18177,10 +18177,10 @@
         </is>
       </c>
       <c r="I158" t="n">
-        <v>65.76666666666667</v>
+        <v>65.76664134229371</v>
       </c>
       <c r="J158" t="n">
-        <v>-170.9333333333333</v>
+        <v>-170.9333586577063</v>
       </c>
       <c r="K158" t="n">
         <v>64.6216973578863</v>
@@ -18262,10 +18262,10 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>91749659.50187095</v>
+        <v>91749763.98484507</v>
       </c>
       <c r="C159" t="n">
-        <v>-175631056.0094321</v>
+        <v>-175631218.9138206</v>
       </c>
       <c r="D159" t="n">
         <v>47</v>
@@ -18291,10 +18291,10 @@
         </is>
       </c>
       <c r="I159" t="n">
-        <v>68.09999999999999</v>
+        <v>68.09999197765791</v>
       </c>
       <c r="J159" t="n">
-        <v>-178.55</v>
+        <v>-178.5500080223421</v>
       </c>
       <c r="K159" t="n">
         <v>64.23774681768066</v>
@@ -18376,10 +18376,10 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>125835486.3192114</v>
+        <v>125836086.652237</v>
       </c>
       <c r="C160" t="n">
-        <v>-202024034.3492684</v>
+        <v>-202024684.8876894</v>
       </c>
       <c r="D160" t="n">
         <v>47</v>
@@ -18405,10 +18405,10 @@
         </is>
       </c>
       <c r="I160" t="n">
-        <v>64.36666666666666</v>
+        <v>64.36662366929453</v>
       </c>
       <c r="J160" t="n">
-        <v>-173.5833333333333</v>
+        <v>-173.5833763307054</v>
       </c>
       <c r="K160" t="n">
         <v>64.43661971830984</v>
@@ -18490,10 +18490,10 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>116302677.9913912</v>
+        <v>116302363.5055453</v>
       </c>
       <c r="C161" t="n">
-        <v>-190096722.4190246</v>
+        <v>-190096358.4436287</v>
       </c>
       <c r="D161" t="n">
         <v>47</v>
@@ -18519,10 +18519,10 @@
         </is>
       </c>
       <c r="I161" t="n">
-        <v>64.98333333333333</v>
+        <v>64.98335676951956</v>
       </c>
       <c r="J161" t="n">
-        <v>-172.4666666666667</v>
+        <v>-172.4666432304805</v>
       </c>
       <c r="K161" t="n">
         <v>64.06453552460167</v>
@@ -18604,10 +18604,10 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>107311988.5897881</v>
+        <v>107310720.9184249</v>
       </c>
       <c r="C162" t="n">
-        <v>-195720365.1089697</v>
+        <v>-195718577.6450581</v>
       </c>
       <c r="D162" t="n">
         <v>47</v>
@@ -18633,10 +18633,10 @@
         </is>
       </c>
       <c r="I162" t="n">
-        <v>66.75</v>
+        <v>66.7500911044866</v>
       </c>
       <c r="J162" t="n">
-        <v>-178.3666666666667</v>
+        <v>-178.3665755621801</v>
       </c>
       <c r="K162" t="n">
         <v>63.88194097048524</v>
@@ -18718,10 +18718,10 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>114563909.9541486</v>
+        <v>114563223.8634599</v>
       </c>
       <c r="C163" t="n">
-        <v>-192169352.3438501</v>
+        <v>-192168517.7273502</v>
       </c>
       <c r="D163" t="n">
         <v>47</v>
@@ -18747,10 +18747,10 @@
         </is>
       </c>
       <c r="I163" t="n">
-        <v>65.38333333333334</v>
+        <v>65.3833839032541</v>
       </c>
       <c r="J163" t="n">
-        <v>-173.8333333333333</v>
+        <v>-173.8332827634125</v>
       </c>
       <c r="K163" t="n">
         <v>63.91670004004805</v>
@@ -18828,10 +18828,10 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>95011643.57201217</v>
+        <v>95010238.99019727</v>
       </c>
       <c r="C164" t="n">
-        <v>-180395028.5643392</v>
+        <v>-180392876.9759969</v>
       </c>
       <c r="D164" t="n">
         <v>47</v>
@@ -18857,10 +18857,10 @@
         </is>
       </c>
       <c r="I164" t="n">
-        <v>67.83333333333333</v>
+        <v>67.83343937331193</v>
       </c>
       <c r="J164" t="n">
-        <v>-178.6666666666667</v>
+        <v>-178.6665606266881</v>
       </c>
       <c r="K164" t="n">
         <v>64.24114331723028</v>
@@ -18938,10 +18938,10 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>116834069.2012096</v>
+        <v>116834089.474993</v>
       </c>
       <c r="C165" t="n">
-        <v>-190551558.9028648</v>
+        <v>-190551582.2354816</v>
       </c>
       <c r="D165" t="n">
         <v>47</v>
@@ -18967,10 +18967,10 @@
         </is>
       </c>
       <c r="I165" t="n">
-        <v>64.93333333333334</v>
+        <v>64.93333182453715</v>
       </c>
       <c r="J165" t="n">
-        <v>-172.45</v>
+        <v>-172.4500015087962</v>
       </c>
       <c r="K165" t="n">
         <v>63.33931061964534</v>
@@ -19052,10 +19052,10 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>123868003.4497282</v>
+        <v>123867543.5620008</v>
       </c>
       <c r="C166" t="n">
-        <v>-203491349.3494467</v>
+        <v>-203490825.668832</v>
       </c>
       <c r="D166" t="n">
         <v>47</v>
@@ -19081,10 +19081,10 @@
         </is>
       </c>
       <c r="I166" t="n">
-        <v>64.73333333333333</v>
+        <v>64.73336601050909</v>
       </c>
       <c r="J166" t="n">
-        <v>-174.6333333333333</v>
+        <v>-174.6333006561576</v>
       </c>
       <c r="K166" t="n">
         <v>62.97952693301529</v>
@@ -19162,10 +19162,10 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>94929941.49687661</v>
+        <v>94930724.12062098</v>
       </c>
       <c r="C167" t="n">
-        <v>-180175873.1514853</v>
+        <v>-180177071.7016331</v>
       </c>
       <c r="D167" t="n">
         <v>47</v>
@@ -19191,10 +19191,10 @@
         </is>
       </c>
       <c r="I167" t="n">
-        <v>67.83333333333333</v>
+        <v>67.83327419627541</v>
       </c>
       <c r="J167" t="n">
-        <v>-178.6166666666667</v>
+        <v>-178.6167258037246</v>
       </c>
       <c r="K167" t="n">
         <v>63.20199501246881</v>
@@ -19276,10 +19276,10 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>109023228.3389354</v>
+        <v>109023935.8231804</v>
       </c>
       <c r="C168" t="n">
-        <v>-190378776.8569978</v>
+        <v>-190379709.2240946</v>
       </c>
       <c r="D168" t="n">
         <v>47</v>
@@ -19305,10 +19305,10 @@
         </is>
       </c>
       <c r="I168" t="n">
-        <v>66.13333333333334</v>
+        <v>66.13328115770848</v>
       </c>
       <c r="J168" t="n">
-        <v>-175.4166666666667</v>
+        <v>-175.4167188422916</v>
       </c>
       <c r="K168" t="n">
         <v>62.96036126442549</v>
@@ -19382,10 +19382,10 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>122611944.6073932</v>
+        <v>122611482.311808</v>
       </c>
       <c r="C169" t="n">
-        <v>-195357698.1838692</v>
+        <v>-195357198.7251206</v>
       </c>
       <c r="D169" t="n">
         <v>47</v>
@@ -19411,10 +19411,10 @@
         </is>
       </c>
       <c r="I169" t="n">
-        <v>64.40000000000001</v>
+        <v>64.40003391967613</v>
       </c>
       <c r="J169" t="n">
-        <v>-172.3166666666667</v>
+        <v>-172.3166327469906</v>
       </c>
       <c r="K169" t="n">
         <v>61.63147982951729</v>
@@ -19496,10 +19496,10 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>112013880.8583967</v>
+        <v>112012002.4043519</v>
       </c>
       <c r="C170" t="n">
-        <v>-187949669.3206637</v>
+        <v>-187947364.5359129</v>
       </c>
       <c r="D170" t="n">
         <v>47</v>
@@ -19525,10 +19525,10 @@
         </is>
       </c>
       <c r="I170" t="n">
-        <v>65.5</v>
+        <v>65.50014057935047</v>
       </c>
       <c r="J170" t="n">
-        <v>-173.2333333333333</v>
+        <v>-173.2331927539828</v>
       </c>
       <c r="K170" t="n">
         <v>61.96491228070173</v>
@@ -19606,10 +19606,10 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>115463714.8997631</v>
+        <v>115464219.5656805</v>
       </c>
       <c r="C171" t="n">
-        <v>-189435652.1500535</v>
+        <v>-189436241.734163</v>
       </c>
       <c r="D171" t="n">
         <v>47</v>
@@ -19635,10 +19635,10 @@
         </is>
       </c>
       <c r="I171" t="n">
-        <v>65.06666666666666</v>
+        <v>65.0666289865151</v>
       </c>
       <c r="J171" t="n">
-        <v>-172.5166666666667</v>
+        <v>-172.5167043468183</v>
       </c>
       <c r="K171" t="n">
         <v>61.35640413683373</v>
@@ -19716,10 +19716,10 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>123165112.2984624</v>
+        <v>123165732.0728984</v>
       </c>
       <c r="C172" t="n">
-        <v>-204035708.748305</v>
+        <v>-204036426.8111035</v>
       </c>
       <c r="D172" t="n">
         <v>47</v>
@@ -19745,10 +19745,10 @@
         </is>
       </c>
       <c r="I172" t="n">
-        <v>64.86666666666666</v>
+        <v>64.86662275926916</v>
       </c>
       <c r="J172" t="n">
-        <v>-175.0333333333333</v>
+        <v>-175.0333772407308</v>
       </c>
       <c r="K172" t="n">
         <v>60.88697567324057</v>
@@ -19830,10 +19830,10 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>126036306.6992295</v>
+        <v>126036634.0646268</v>
       </c>
       <c r="C173" t="n">
-        <v>-201935878.6672168</v>
+        <v>-201936231.7772607</v>
       </c>
       <c r="D173" t="n">
         <v>47</v>
@@ -19859,10 +19859,10 @@
         </is>
       </c>
       <c r="I173" t="n">
-        <v>64.33333333333333</v>
+        <v>64.33330987357901</v>
       </c>
       <c r="J173" t="n">
-        <v>-173.5</v>
+        <v>-173.5000234597543</v>
       </c>
       <c r="K173" t="n">
         <v>59.95813397129186</v>
@@ -19944,10 +19944,10 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>103962442.9232851</v>
+        <v>103962297.5280395</v>
       </c>
       <c r="C174" t="n">
-        <v>-184188619.6538791</v>
+        <v>-184188421.1273362</v>
       </c>
       <c r="D174" t="n">
         <v>47</v>
@@ -19973,10 +19973,10 @@
         </is>
       </c>
       <c r="I174" t="n">
-        <v>66.55</v>
+        <v>66.55001094406209</v>
       </c>
       <c r="J174" t="n">
-        <v>-175.2833333333333</v>
+        <v>-175.2833223892712</v>
       </c>
       <c r="K174" t="n">
         <v>58.0490724117295</v>
@@ -20058,10 +20058,10 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>123167282.702717</v>
+        <v>123167497.8179095</v>
       </c>
       <c r="C175" t="n">
-        <v>-196594906.1205665</v>
+        <v>-196595138.8558727</v>
       </c>
       <c r="D175" t="n">
         <v>47</v>
@@ -20087,10 +20087,10 @@
         </is>
       </c>
       <c r="I175" t="n">
-        <v>64.40000000000001</v>
+        <v>64.39998428865744</v>
       </c>
       <c r="J175" t="n">
-        <v>-172.5666666666667</v>
+        <v>-172.5666823780093</v>
       </c>
       <c r="K175" t="n">
         <v>57.96623713914693</v>
@@ -20168,10 +20168,10 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>125010710.1779163</v>
+        <v>125007944.8906292</v>
       </c>
       <c r="C176" t="n">
-        <v>-206929784.8167274</v>
+        <v>-206926604.33199</v>
       </c>
       <c r="D176" t="n">
         <v>47</v>
@@ -20197,10 +20197,10 @@
         </is>
       </c>
       <c r="I176" t="n">
-        <v>64.78333333333333</v>
+        <v>64.78352735916813</v>
       </c>
       <c r="J176" t="n">
-        <v>-175.4166666666667</v>
+        <v>-175.4164726408319</v>
       </c>
       <c r="K176" t="n">
         <v>56.76590660161306</v>
@@ -20274,10 +20274,10 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>104729464.4104264</v>
+        <v>104730402.1973267</v>
       </c>
       <c r="C177" t="n">
-        <v>-183605281.7788929</v>
+        <v>-183606540.2147338</v>
       </c>
       <c r="D177" t="n">
         <v>47</v>
@@ -20303,10 +20303,10 @@
         </is>
       </c>
       <c r="I177" t="n">
-        <v>66.38333333333334</v>
+        <v>66.38326247672906</v>
       </c>
       <c r="J177" t="n">
-        <v>-174.6666666666667</v>
+        <v>-174.666737523271</v>
       </c>
       <c r="K177" t="n">
         <v>55.99558853017847</v>
@@ -20384,10 +20384,10 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>108429877.3972789</v>
+        <v>108429037.3583531</v>
       </c>
       <c r="C178" t="n">
-        <v>-197507406.5182095</v>
+        <v>-197506227.4677483</v>
       </c>
       <c r="D178" t="n">
         <v>47</v>
@@ -20413,10 +20413,10 @@
         </is>
       </c>
       <c r="I178" t="n">
-        <v>66.68333333333334</v>
+        <v>66.68339334081354</v>
       </c>
       <c r="J178" t="n">
-        <v>-178.5333333333333</v>
+        <v>-178.5332733258531</v>
       </c>
       <c r="K178" t="n">
         <v>53.94579513750498</v>
@@ -20498,10 +20498,10 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>107512874.7280466</v>
+        <v>107512582.6285103</v>
       </c>
       <c r="C179" t="n">
-        <v>-195967860.4381379</v>
+        <v>-195967449.1250856</v>
       </c>
       <c r="D179" t="n">
         <v>47</v>
@@ -20527,10 +20527,10 @@
         </is>
       </c>
       <c r="I179" t="n">
-        <v>66.73333333333333</v>
+        <v>66.73335430959045</v>
       </c>
       <c r="J179" t="n">
-        <v>-178.3666666666667</v>
+        <v>-178.3666456904096</v>
       </c>
       <c r="K179" t="n">
         <v>53.40088282504012</v>
@@ -20612,10 +20612,10 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>119546848.2491341</v>
+        <v>119548694.4906461</v>
       </c>
       <c r="C180" t="n">
-        <v>-208861574.6260518</v>
+        <v>-208863939.1255731</v>
       </c>
       <c r="D180" t="n">
         <v>47</v>
@@ -20641,10 +20641,10 @@
         </is>
       </c>
       <c r="I180" t="n">
-        <v>65.68333333333334</v>
+        <v>65.68320561056693</v>
       </c>
       <c r="J180" t="n">
-        <v>-177.9666666666667</v>
+        <v>-177.9667943894331</v>
       </c>
       <c r="K180" t="n">
         <v>52.50074872716382</v>

</xml_diff>

<commit_message>
adding noise: code implemented in notebook preprocessing
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,10 +528,10 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>95283997.94687383</v>
+        <v>95282423.42394386</v>
       </c>
       <c r="C2" t="n">
-        <v>-181126431.7277304</v>
+        <v>-181124017.8387472</v>
       </c>
       <c r="D2" t="n">
         <v>47</v>
@@ -557,10 +557,10 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>67.83336164715892</v>
+        <v>67.83348016512761</v>
       </c>
       <c r="J2" t="n">
-        <v>-178.8333050195077</v>
+        <v>-178.833186501539</v>
       </c>
       <c r="K2" t="n">
         <v>77.19385719984045</v>
@@ -642,10 +642,10 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>119550397.81551</v>
+        <v>119552764.2797502</v>
       </c>
       <c r="C3" t="n">
-        <v>-209147245.3898863</v>
+        <v>-209150282.5585824</v>
       </c>
       <c r="D3" t="n">
         <v>47</v>
@@ -671,10 +671,10 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>65.69999468594703</v>
+        <v>65.69983116205766</v>
       </c>
       <c r="J3" t="n">
-        <v>-178.0666719807197</v>
+        <v>-178.0668355046091</v>
       </c>
       <c r="K3" t="n">
         <v>76.99530516431925</v>
@@ -756,10 +756,10 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>104941270.6788485</v>
+        <v>104941148.9373436</v>
       </c>
       <c r="C4" t="n">
-        <v>-184375531.6367889</v>
+        <v>-184375367.8509409</v>
       </c>
       <c r="D4" t="n">
         <v>47</v>
@@ -785,10 +785,10 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>66.39997687381246</v>
+        <v>66.39998604291354</v>
       </c>
       <c r="J4" t="n">
-        <v>-174.8833564595209</v>
+        <v>-174.8833472904198</v>
       </c>
       <c r="K4" t="n">
         <v>76.56732781819994</v>
@@ -874,10 +874,10 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>95827846.36066358</v>
+        <v>95828445.73439915</v>
       </c>
       <c r="C5" t="n">
-        <v>-182845134.7133268</v>
+        <v>-182846056.6980341</v>
       </c>
       <c r="D5" t="n">
         <v>47</v>
@@ -903,10 +903,10 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>67.85001829537772</v>
+        <v>67.84997349822386</v>
       </c>
       <c r="J5" t="n">
-        <v>-179.2833150379556</v>
+        <v>-179.2833598351095</v>
       </c>
       <c r="K5" t="n">
         <v>76.29378980891718</v>
@@ -988,10 +988,10 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>95741334.71643947</v>
+        <v>95741241.542317</v>
       </c>
       <c r="C6" t="n">
-        <v>-182870185.5601847</v>
+        <v>-182870042.0223253</v>
       </c>
       <c r="D6" t="n">
         <v>47</v>
@@ -1017,10 +1017,10 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>67.86671670282102</v>
+        <v>67.86672366478381</v>
       </c>
       <c r="J6" t="n">
-        <v>-179.3499499638456</v>
+        <v>-179.3499430018828</v>
       </c>
       <c r="K6" t="n">
         <v>76.51060424169667</v>
@@ -1102,10 +1102,10 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>110428185.9511601</v>
+        <v>110429225.6288865</v>
       </c>
       <c r="C7" t="n">
-        <v>-201249734.0073696</v>
+        <v>-201251187.019623</v>
       </c>
       <c r="D7" t="n">
         <v>47</v>
@@ -1131,10 +1131,10 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>66.59994315430309</v>
+        <v>66.59986984615693</v>
       </c>
       <c r="J7" t="n">
-        <v>-179.0500568456969</v>
+        <v>-179.050130153843</v>
       </c>
       <c r="K7" t="n">
         <v>76.56250000000001</v>
@@ -1212,10 +1212,10 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>95831097.14160162</v>
+        <v>95831264.53457274</v>
       </c>
       <c r="C8" t="n">
-        <v>-182596899.4977312</v>
+        <v>-182597156.5451731</v>
       </c>
       <c r="D8" t="n">
         <v>47</v>
@@ -1241,10 +1241,10 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>67.83337393385574</v>
+        <v>67.83336140832134</v>
       </c>
       <c r="J8" t="n">
-        <v>-179.1666260661443</v>
+        <v>-179.1666385916787</v>
       </c>
       <c r="K8" t="n">
         <v>75.8226463863207</v>
@@ -1326,10 +1326,10 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>105424177.0032899</v>
+        <v>105424615.0091471</v>
       </c>
       <c r="C9" t="n">
-        <v>-186071178.5209873</v>
+        <v>-186071770.9097808</v>
       </c>
       <c r="D9" t="n">
         <v>47</v>
@@ -1355,10 +1355,10 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>66.43340208612744</v>
+        <v>66.43336932654165</v>
       </c>
       <c r="J9" t="n">
-        <v>-175.3499312472059</v>
+        <v>-175.3499640067917</v>
       </c>
       <c r="K9" t="n">
         <v>75.75636942675158</v>
@@ -1444,10 +1444,10 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>93838148.12582983</v>
+        <v>93838358.02530071</v>
       </c>
       <c r="C10" t="n">
-        <v>-180545283.6552253</v>
+        <v>-180545611.33535</v>
       </c>
       <c r="D10" t="n">
         <v>47</v>
@@ -1473,10 +1473,10 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>68.05005468778411</v>
+        <v>68.0500388858499</v>
       </c>
       <c r="J10" t="n">
-        <v>-179.4999453122159</v>
+        <v>-179.4999611141501</v>
       </c>
       <c r="K10" t="n">
         <v>76.19715487878182</v>
@@ -1562,10 +1562,10 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>105481876.0653925</v>
+        <v>105480970.7099347</v>
       </c>
       <c r="C11" t="n">
-        <v>-184961935.7090315</v>
+        <v>-184960723.030066</v>
       </c>
       <c r="D11" t="n">
         <v>47</v>
@@ -1591,10 +1591,10 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>66.34997128755195</v>
+        <v>66.35003934791879</v>
       </c>
       <c r="J11" t="n">
-        <v>-174.8666953791148</v>
+        <v>-174.866627318748</v>
       </c>
       <c r="K11" t="n">
         <v>76.34538152610442</v>
@@ -1676,10 +1676,10 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>124228588.4715796</v>
+        <v>124229411.8829788</v>
       </c>
       <c r="C12" t="n">
-        <v>-206494470.9674475</v>
+        <v>-206495427.4714684</v>
       </c>
       <c r="D12" t="n">
         <v>47</v>
@@ -1705,10 +1705,10 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>64.86679641086742</v>
+        <v>64.86673858500359</v>
       </c>
       <c r="J12" t="n">
-        <v>-175.5165369224659</v>
+        <v>-175.5165947483297</v>
       </c>
       <c r="K12" t="n">
         <v>75.82077636962379</v>
@@ -1786,10 +1786,10 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>114775970.9772273</v>
+        <v>114776304.1833821</v>
       </c>
       <c r="C13" t="n">
-        <v>-200512542.1981468</v>
+        <v>-200512974.5587198</v>
       </c>
       <c r="D13" t="n">
         <v>47</v>
@@ -1815,10 +1815,10 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>65.88330810347263</v>
+        <v>65.88328439323223</v>
       </c>
       <c r="J13" t="n">
-        <v>-176.833358563194</v>
+        <v>-176.8333822734344</v>
       </c>
       <c r="K13" t="n">
         <v>75.33756949960284</v>
@@ -1892,10 +1892,10 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>92751788.18368557</v>
+        <v>92751328.5513556</v>
       </c>
       <c r="C14" t="n">
-        <v>-177342903.7849017</v>
+        <v>-177342189.8416194</v>
       </c>
       <c r="D14" t="n">
         <v>47</v>
@@ -1921,10 +1921,10 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>68.03340471926347</v>
+        <v>68.03343978466725</v>
       </c>
       <c r="J14" t="n">
-        <v>-178.6999286140698</v>
+        <v>-178.699893548666</v>
       </c>
       <c r="K14" t="n">
         <v>75.96394591887831</v>
@@ -2006,10 +2006,10 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>98399684.42395204</v>
+        <v>98397391.14028972</v>
       </c>
       <c r="C15" t="n">
-        <v>-168147393.1085977</v>
+        <v>-168144371.6522151</v>
       </c>
       <c r="D15" t="n">
         <v>47</v>
@@ -2035,10 +2035,10 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>66.3832569334397</v>
+        <v>66.38344163328402</v>
       </c>
       <c r="J15" t="n">
-        <v>-171.1667430665604</v>
+        <v>-171.1665583667161</v>
       </c>
       <c r="K15" t="n">
         <v>75.67865371130922</v>
@@ -2116,10 +2116,10 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>124690050.8859959</v>
+        <v>124689994.5163658</v>
       </c>
       <c r="C16" t="n">
-        <v>-205920400.4650612</v>
+        <v>-205920335.8366216</v>
       </c>
       <c r="D16" t="n">
         <v>47</v>
@@ -2145,10 +2145,10 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>64.76676128743597</v>
+        <v>64.76676525722948</v>
       </c>
       <c r="J16" t="n">
-        <v>-175.183238712564</v>
+        <v>-175.1832347427705</v>
       </c>
       <c r="K16" t="n">
         <v>75.56533920352211</v>
@@ -2230,10 +2230,10 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>117110197.7580975</v>
+        <v>117110889.8931256</v>
       </c>
       <c r="C17" t="n">
-        <v>-202418922.8946863</v>
+        <v>-202419800.2301919</v>
       </c>
       <c r="D17" t="n">
         <v>47</v>
@@ -2259,10 +2259,10 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>65.64997228439121</v>
+        <v>65.64992327594379</v>
       </c>
       <c r="J17" t="n">
-        <v>-176.6000277156088</v>
+        <v>-176.6000767240562</v>
       </c>
       <c r="K17" t="n">
         <v>75.69465342561942</v>
@@ -2340,10 +2340,10 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>121346830.2819801</v>
+        <v>121345514.7420146</v>
       </c>
       <c r="C18" t="n">
-        <v>-211276373.4495602</v>
+        <v>-211274706.1783964</v>
       </c>
       <c r="D18" t="n">
         <v>47</v>
@@ -2369,10 +2369,10 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>65.56655332885526</v>
+        <v>65.5666436637167</v>
       </c>
       <c r="J18" t="n">
-        <v>-178.1334466711447</v>
+        <v>-178.1333563362832</v>
       </c>
       <c r="K18" t="n">
         <v>75.18699511319437</v>
@@ -2454,10 +2454,10 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>125519215.899418</v>
+        <v>125518658.9725189</v>
       </c>
       <c r="C19" t="n">
-        <v>-203198296.5584472</v>
+        <v>-203197682.7713831</v>
       </c>
       <c r="D19" t="n">
         <v>47</v>
@@ -2483,10 +2483,10 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>64.48338593502929</v>
+        <v>64.4834256223632</v>
       </c>
       <c r="J19" t="n">
-        <v>-174.0499473983041</v>
+        <v>-174.0499077109702</v>
       </c>
       <c r="K19" t="n">
         <v>74.65305313243456</v>
@@ -2560,10 +2560,10 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>95364596.81383142</v>
+        <v>95364025.13515216</v>
       </c>
       <c r="C20" t="n">
-        <v>-181344413.6594365</v>
+        <v>-181343537.004773</v>
       </c>
       <c r="D20" t="n">
         <v>47</v>
@@ -2589,10 +2589,10 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>67.83346220749966</v>
+        <v>67.83350520099918</v>
       </c>
       <c r="J20" t="n">
-        <v>-178.883204459167</v>
+        <v>-178.8831614656675</v>
       </c>
       <c r="K20" t="n">
         <v>75.32285514065472</v>
@@ -2674,10 +2674,10 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>127328664.1379309</v>
+        <v>127327723.273805</v>
       </c>
       <c r="C21" t="n">
-        <v>-206191166.5138207</v>
+        <v>-206190135.3970429</v>
       </c>
       <c r="D21" t="n">
         <v>47</v>
@@ -2703,10 +2703,10 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>64.41671993659487</v>
+        <v>64.41678630576148</v>
       </c>
       <c r="J21" t="n">
-        <v>-174.4999467300718</v>
+        <v>-174.4998803609052</v>
       </c>
       <c r="K21" t="n">
         <v>74.74908079101658</v>
@@ -2784,10 +2784,10 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>121266763.0873286</v>
+        <v>121267982.8839387</v>
       </c>
       <c r="C22" t="n">
-        <v>-198347203.042288</v>
+        <v>-198348593.0277166</v>
       </c>
       <c r="D22" t="n">
         <v>47</v>
@@ -2813,10 +2813,10 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>64.78343969693921</v>
+        <v>64.78335142657936</v>
       </c>
       <c r="J22" t="n">
-        <v>-173.7165603030608</v>
+        <v>-173.7166485734207</v>
       </c>
       <c r="K22" t="n">
         <v>74.78364667263506</v>
@@ -2890,10 +2890,10 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>95381528.85832316</v>
+        <v>95380300.6148705</v>
       </c>
       <c r="C23" t="n">
-        <v>-182157848.2088327</v>
+        <v>-182155954.7913481</v>
       </c>
       <c r="D23" t="n">
         <v>47</v>
@@ -2919,10 +2919,10 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>67.88341649871434</v>
+        <v>67.88350852072125</v>
       </c>
       <c r="J23" t="n">
-        <v>-179.249916834619</v>
+        <v>-179.2498248126121</v>
       </c>
       <c r="K23" t="n">
         <v>75.18759379689844</v>
@@ -2996,10 +2996,10 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>95605162.06082919</v>
+        <v>95605805.78367405</v>
       </c>
       <c r="C24" t="n">
-        <v>-182502406.8320286</v>
+        <v>-182503398.1001907</v>
       </c>
       <c r="D24" t="n">
         <v>47</v>
@@ -3025,10 +3025,10 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>67.86667177744339</v>
+        <v>67.86662360753036</v>
       </c>
       <c r="J24" t="n">
-        <v>-179.26666155589</v>
+        <v>-179.2667097258031</v>
       </c>
       <c r="K24" t="n">
         <v>74.74868119836768</v>
@@ -3110,10 +3110,10 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>121302567.4736511</v>
+        <v>121303364.1280309</v>
       </c>
       <c r="C25" t="n">
-        <v>-203758529.3476131</v>
+        <v>-203759480.5622177</v>
       </c>
       <c r="D25" t="n">
         <v>47</v>
@@ -3139,10 +3139,10 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>65.11669181224212</v>
+        <v>65.11663542832794</v>
       </c>
       <c r="J25" t="n">
-        <v>-175.5499748544246</v>
+        <v>-175.5500312383388</v>
       </c>
       <c r="K25" t="n">
         <v>74.96504893149591</v>
@@ -3224,10 +3224,10 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>112736084.8396494</v>
+        <v>112735035.5398172</v>
       </c>
       <c r="C26" t="n">
-        <v>-195553994.4118544</v>
+        <v>-195552640.0126746</v>
       </c>
       <c r="D26" t="n">
         <v>47</v>
@@ -3253,10 +3253,10 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>65.88338446289151</v>
+        <v>65.88346050954543</v>
       </c>
       <c r="J26" t="n">
-        <v>-175.8166155371085</v>
+        <v>-175.8165394904546</v>
       </c>
       <c r="K26" t="n">
         <v>74.9350908727781</v>
@@ -3334,10 +3334,10 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>95250469.72453789</v>
+        <v>95250007.58868599</v>
       </c>
       <c r="C27" t="n">
-        <v>-181546750.717905</v>
+        <v>-181546039.8281603</v>
       </c>
       <c r="D27" t="n">
         <v>47</v>
@@ -3363,10 +3363,10 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>67.86665547156203</v>
+        <v>67.86669018676611</v>
       </c>
       <c r="J27" t="n">
-        <v>-179.0500111951046</v>
+        <v>-179.0499764799005</v>
       </c>
       <c r="K27" t="n">
         <v>74.68114786767636</v>
@@ -3448,10 +3448,10 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>114519157.4111848</v>
+        <v>114518586.2557847</v>
       </c>
       <c r="C28" t="n">
-        <v>-188018214.6526375</v>
+        <v>-188017544.4496489</v>
       </c>
       <c r="D28" t="n">
         <v>47</v>
@@ -3477,10 +3477,10 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>65.11670719855645</v>
+        <v>65.11675005986048</v>
       </c>
       <c r="J28" t="n">
-        <v>-172.3332928014435</v>
+        <v>-172.3332499401395</v>
       </c>
       <c r="K28" t="n">
         <v>75.07769423558896</v>
@@ -3562,10 +3562,10 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>99552368.42483975</v>
+        <v>99552257.76107493</v>
       </c>
       <c r="C29" t="n">
-        <v>-173040603.8722652</v>
+        <v>-173040454.961911</v>
       </c>
       <c r="D29" t="n">
         <v>47</v>
@@ -3591,10 +3591,10 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>66.53337907415737</v>
+        <v>66.53338779232693</v>
       </c>
       <c r="J29" t="n">
-        <v>-172.7332875925092</v>
+        <v>-172.7332788743396</v>
       </c>
       <c r="K29" t="n">
         <v>74.91494896938163</v>
@@ -3672,10 +3672,10 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>122386908.7302104</v>
+        <v>122387987.0239019</v>
       </c>
       <c r="C30" t="n">
-        <v>-200372427.8239095</v>
+        <v>-200373654.1043369</v>
       </c>
       <c r="D30" t="n">
         <v>47</v>
@@ -3701,10 +3701,10 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>64.74992377307039</v>
+        <v>64.74984629796785</v>
       </c>
       <c r="J30" t="n">
-        <v>-174.0500762269296</v>
+        <v>-174.0501537020322</v>
       </c>
       <c r="K30" t="n">
         <v>74.1114741114741</v>
@@ -3778,10 +3778,10 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>121305639.0987237</v>
+        <v>121305548.1740049</v>
       </c>
       <c r="C31" t="n">
-        <v>-203762196.873767</v>
+        <v>-203762088.3106418</v>
       </c>
       <c r="D31" t="n">
         <v>47</v>
@@ -3807,10 +3807,10 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>65.11647441619643</v>
+        <v>65.11648085141046</v>
       </c>
       <c r="J31" t="n">
-        <v>-175.5501922504702</v>
+        <v>-175.5501858152562</v>
       </c>
       <c r="K31" t="n">
         <v>74.53639082751742</v>
@@ -3892,10 +3892,10 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>95246610.15562837</v>
+        <v>95247441.91766733</v>
       </c>
       <c r="C32" t="n">
-        <v>-181792475.6709797</v>
+        <v>-181793757.3492677</v>
       </c>
       <c r="D32" t="n">
         <v>47</v>
@@ -3921,10 +3921,10 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>67.88331339769263</v>
+        <v>67.88325098919744</v>
       </c>
       <c r="J32" t="n">
-        <v>-179.1666866023074</v>
+        <v>-179.1667490108026</v>
       </c>
       <c r="K32" t="n">
         <v>74.59588904410298</v>
@@ -4006,10 +4006,10 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>120390801.7820959</v>
+        <v>120389586.4569375</v>
       </c>
       <c r="C33" t="n">
-        <v>-211194300.5434513</v>
+        <v>-211192737.5384258</v>
       </c>
       <c r="D33" t="n">
         <v>47</v>
@@ -4035,10 +4035,10 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>65.69999795399802</v>
+        <v>65.70008133551484</v>
       </c>
       <c r="J33" t="n">
-        <v>-178.4666687126687</v>
+        <v>-178.4665853311519</v>
       </c>
       <c r="K33" t="n">
         <v>74.37810945273633</v>
@@ -4116,10 +4116,10 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>95491579.99477631</v>
+        <v>95492687.50073972</v>
       </c>
       <c r="C34" t="n">
-        <v>-182453648.0181718</v>
+        <v>-182455355.850242</v>
       </c>
       <c r="D34" t="n">
         <v>47</v>
@@ -4145,10 +4145,10 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>67.88334847439322</v>
+        <v>67.88326559737777</v>
       </c>
       <c r="J34" t="n">
-        <v>-179.3166515256068</v>
+        <v>-179.3167344026222</v>
       </c>
       <c r="K34" t="n">
         <v>74.27406523468576</v>
@@ -4230,10 +4230,10 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>125024109.1397756</v>
+        <v>125025500.7311581</v>
       </c>
       <c r="C35" t="n">
-        <v>-202349886.662595</v>
+        <v>-202351422.2608036</v>
       </c>
       <c r="D35" t="n">
         <v>47</v>
@@ -4259,10 +4259,10 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>64.49999526918459</v>
+        <v>64.4998958124353</v>
       </c>
       <c r="J35" t="n">
-        <v>-173.9166713974821</v>
+        <v>-173.9167708542314</v>
       </c>
       <c r="K35" t="n">
         <v>74.73958333333333</v>
@@ -4340,10 +4340,10 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>124327141.534732</v>
+        <v>124325830.1572926</v>
       </c>
       <c r="C36" t="n">
-        <v>-205631350.3833643</v>
+        <v>-205629841.009484</v>
       </c>
       <c r="D36" t="n">
         <v>47</v>
@@ -4369,10 +4369,10 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>64.80015036111361</v>
+        <v>64.80024278534684</v>
       </c>
       <c r="J36" t="n">
-        <v>-175.1998496388864</v>
+        <v>-175.1997572146532</v>
       </c>
       <c r="K36" t="n">
         <v>74.59459459459461</v>
@@ -4458,10 +4458,10 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>100517524.5837477</v>
+        <v>100517604.8722086</v>
       </c>
       <c r="C37" t="n">
-        <v>-174700028.5846796</v>
+        <v>-174700136.2946388</v>
       </c>
       <c r="D37" t="n">
         <v>47</v>
@@ -4487,10 +4487,10 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>66.48322906384377</v>
+        <v>66.48322277956974</v>
       </c>
       <c r="J37" t="n">
-        <v>-172.9667709361563</v>
+        <v>-172.9667772204303</v>
       </c>
       <c r="K37" t="n">
         <v>74.46043165467626</v>
@@ -4568,10 +4568,10 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>101868677.8207729</v>
+        <v>101868946.7203449</v>
       </c>
       <c r="C38" t="n">
-        <v>-175394490.4031445</v>
+        <v>-175394844.7938784</v>
       </c>
       <c r="D38" t="n">
         <v>47</v>
@@ -4597,10 +4597,10 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>66.29995050572477</v>
+        <v>66.299929485821</v>
       </c>
       <c r="J38" t="n">
-        <v>-172.6000494942752</v>
+        <v>-172.600070514179</v>
       </c>
       <c r="K38" t="n">
         <v>74.16110723887283</v>
@@ -4682,10 +4682,10 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>92875591.35906237</v>
+        <v>92874531.14906563</v>
       </c>
       <c r="C39" t="n">
-        <v>-179715338.5746408</v>
+        <v>-179713668.4056195</v>
       </c>
       <c r="D39" t="n">
         <v>47</v>
@@ -4711,10 +4711,10 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>68.16670171430422</v>
+        <v>68.16678170469702</v>
       </c>
       <c r="J39" t="n">
-        <v>-179.7499649523625</v>
+        <v>-179.7498849619697</v>
       </c>
       <c r="K39" t="n">
         <v>74.00736391680766</v>
@@ -4800,10 +4800,10 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>94841119.89169264</v>
+        <v>94840572.3892775</v>
       </c>
       <c r="C40" t="n">
-        <v>-180446729.0647684</v>
+        <v>-180445887.8844967</v>
       </c>
       <c r="D40" t="n">
         <v>47</v>
@@ -4829,10 +4829,10 @@
         </is>
       </c>
       <c r="I40" t="n">
-        <v>67.86673825049411</v>
+        <v>67.86677956191454</v>
       </c>
       <c r="J40" t="n">
-        <v>-178.7999284161726</v>
+        <v>-178.7998871047522</v>
       </c>
       <c r="K40" t="n">
         <v>74.27228168450536</v>
@@ -4918,10 +4918,10 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>121229783.9312185</v>
+        <v>121229719.0507312</v>
       </c>
       <c r="C41" t="n">
-        <v>-203589326.0603937</v>
+        <v>-203589248.6053825</v>
       </c>
       <c r="D41" t="n">
         <v>47</v>
@@ -4947,10 +4947,10 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>65.11675841779834</v>
+        <v>65.11676301256466</v>
       </c>
       <c r="J41" t="n">
-        <v>-175.516574915535</v>
+        <v>-175.5165703207687</v>
       </c>
       <c r="K41" t="n">
         <v>74.36591478696742</v>
@@ -5032,10 +5032,10 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>94348518.45245603</v>
+        <v>94348291.96360223</v>
       </c>
       <c r="C42" t="n">
-        <v>-180904401.9074258</v>
+        <v>-180904050.2130439</v>
       </c>
       <c r="D42" t="n">
         <v>47</v>
@@ -5061,10 +5061,10 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>67.98335393134224</v>
+        <v>67.98337096900292</v>
       </c>
       <c r="J42" t="n">
-        <v>-179.3333127353244</v>
+        <v>-179.3332956976637</v>
       </c>
       <c r="K42" t="n">
         <v>73.97943906577501</v>
@@ -5150,10 +5150,10 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>93969253.23702408</v>
+        <v>93970184.60001004</v>
       </c>
       <c r="C43" t="n">
-        <v>-178608145.3456385</v>
+        <v>-178609577.4670362</v>
       </c>
       <c r="D43" t="n">
         <v>47</v>
@@ -5179,10 +5179,10 @@
         </is>
       </c>
       <c r="I43" t="n">
-        <v>67.89997591453019</v>
+        <v>67.89990513413876</v>
       </c>
       <c r="J43" t="n">
-        <v>-178.5000240854698</v>
+        <v>-178.5000948658612</v>
       </c>
       <c r="K43" t="n">
         <v>73.53204172876302</v>
@@ -5264,10 +5264,10 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>104810639.4110961</v>
+        <v>104810660.9949679</v>
       </c>
       <c r="C44" t="n">
-        <v>-184303746.9290686</v>
+        <v>-184303776.0140289</v>
       </c>
       <c r="D44" t="n">
         <v>47</v>
@@ -5293,10 +5293,10 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>66.41679410589634</v>
+        <v>66.41679248006338</v>
       </c>
       <c r="J44" t="n">
-        <v>-174.9165392274371</v>
+        <v>-174.9165408532701</v>
       </c>
       <c r="K44" t="n">
         <v>73.88305847076461</v>
@@ -5382,10 +5382,10 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>90477776.63345405</v>
+        <v>90476856.36681883</v>
       </c>
       <c r="C45" t="n">
-        <v>-173671852.9647405</v>
+        <v>-173670409.0955782</v>
       </c>
       <c r="D45" t="n">
         <v>47</v>
@@ -5411,10 +5411,10 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>68.20001595428498</v>
+        <v>68.20008712308544</v>
       </c>
       <c r="J45" t="n">
-        <v>-178.4666507123817</v>
+        <v>-178.4665795435812</v>
       </c>
       <c r="K45" t="n">
         <v>73.70995109292343</v>
@@ -5500,10 +5500,10 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>95909931.02336974</v>
+        <v>95910579.3488552</v>
       </c>
       <c r="C46" t="n">
-        <v>-183066432.8012119</v>
+        <v>-183067430.3302456</v>
       </c>
       <c r="D46" t="n">
         <v>47</v>
@@ -5529,10 +5529,10 @@
         </is>
       </c>
       <c r="I46" t="n">
-        <v>67.85003020674193</v>
+        <v>67.84998179391836</v>
       </c>
       <c r="J46" t="n">
-        <v>-179.3333031265913</v>
+        <v>-179.3333515394148</v>
       </c>
       <c r="K46" t="n">
         <v>74.10938283993977</v>
@@ -5610,10 +5610,10 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>94301473.24302509</v>
+        <v>94300459.77152336</v>
       </c>
       <c r="C47" t="n">
-        <v>-181548493.462025</v>
+        <v>-181546911.7999673</v>
       </c>
       <c r="D47" t="n">
         <v>47</v>
@@ -5639,10 +5639,10 @@
         </is>
       </c>
       <c r="I47" t="n">
-        <v>68.03338138338532</v>
+        <v>68.0334573847293</v>
       </c>
       <c r="J47" t="n">
-        <v>-179.6666186166147</v>
+        <v>-179.6665426152707</v>
       </c>
       <c r="K47" t="n">
         <v>73.38717718616013</v>
@@ -5728,10 +5728,10 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>94297103.23677927</v>
+        <v>94297707.20916051</v>
       </c>
       <c r="C48" t="n">
-        <v>-179236327.3664464</v>
+        <v>-179237255.3816975</v>
       </c>
       <c r="D48" t="n">
         <v>47</v>
@@ -5757,10 +5757,10 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>67.88328522004672</v>
+        <v>67.88323943030409</v>
       </c>
       <c r="J48" t="n">
-        <v>-178.5833814466199</v>
+        <v>-178.5834272363626</v>
       </c>
       <c r="K48" t="n">
         <v>73.48590845492704</v>
@@ -5842,10 +5842,10 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>123511159.385416</v>
+        <v>123510846.9439162</v>
       </c>
       <c r="C49" t="n">
-        <v>-204562696.9623128</v>
+        <v>-204562335.5173564</v>
       </c>
       <c r="D49" t="n">
         <v>47</v>
@@ -5871,10 +5871,10 @@
         </is>
       </c>
       <c r="I49" t="n">
-        <v>64.84995767676973</v>
+        <v>64.84997977267291</v>
       </c>
       <c r="J49" t="n">
-        <v>-175.1000423232303</v>
+        <v>-175.1000202273271</v>
       </c>
       <c r="K49" t="n">
         <v>73.3113838172204</v>
@@ -5956,10 +5956,10 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>95726392.43290836</v>
+        <v>95725352.49476045</v>
       </c>
       <c r="C50" t="n">
-        <v>-181803929.9202596</v>
+        <v>-181802339.0369653</v>
       </c>
       <c r="D50" t="n">
         <v>47</v>
@@ -5985,10 +5985,10 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>67.80010172042356</v>
+        <v>67.80017981113411</v>
       </c>
       <c r="J50" t="n">
-        <v>-178.8665649462432</v>
+        <v>-178.8664868555326</v>
       </c>
       <c r="K50" t="n">
         <v>73.55032548823233</v>
@@ -6066,10 +6066,10 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>105276258.5071207</v>
+        <v>105275316.8308108</v>
       </c>
       <c r="C51" t="n">
-        <v>-175038955.4961019</v>
+        <v>-175037791.7453042</v>
       </c>
       <c r="D51" t="n">
         <v>47</v>
@@ -6095,10 +6095,10 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>65.69991906688784</v>
+        <v>65.69999315360536</v>
       </c>
       <c r="J51" t="n">
-        <v>-170.9167475997789</v>
+        <v>-170.9166735130614</v>
       </c>
       <c r="K51" t="n">
         <v>73.5070140280561</v>
@@ -6180,10 +6180,10 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>111385813.1348711</v>
+        <v>111385953.0881969</v>
       </c>
       <c r="C52" t="n">
-        <v>-202325566.3048023</v>
+        <v>-202325760.512677</v>
       </c>
       <c r="D52" t="n">
         <v>47</v>
@@ -6209,10 +6209,10 @@
         </is>
       </c>
       <c r="I52" t="n">
-        <v>66.51671638435909</v>
+        <v>66.51670654715149</v>
       </c>
       <c r="J52" t="n">
-        <v>-179.0166169489743</v>
+        <v>-179.0166267861819</v>
       </c>
       <c r="K52" t="n">
         <v>73.24197259177751</v>
@@ -6290,10 +6290,10 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>117762280.2443921</v>
+        <v>117762322.5122562</v>
       </c>
       <c r="C53" t="n">
-        <v>-206444810.4697082</v>
+        <v>-206444865.1610297</v>
       </c>
       <c r="D53" t="n">
         <v>47</v>
@@ -6319,10 +6319,10 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>65.80003044384634</v>
+        <v>65.80002749763581</v>
       </c>
       <c r="J53" t="n">
-        <v>-177.7999695561537</v>
+        <v>-177.7999725023642</v>
       </c>
       <c r="K53" t="n">
         <v>73.43640196767393</v>
@@ -6404,10 +6404,10 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>90648909.40460366</v>
+        <v>90649208.32910211</v>
       </c>
       <c r="C54" t="n">
-        <v>-173640852.4905823</v>
+        <v>-173641320.1490476</v>
       </c>
       <c r="D54" t="n">
         <v>47</v>
@@ -6433,10 +6433,10 @@
         </is>
       </c>
       <c r="I54" t="n">
-        <v>68.16673432352188</v>
+        <v>68.16671119537828</v>
       </c>
       <c r="J54" t="n">
-        <v>-178.3332656764781</v>
+        <v>-178.3332888046217</v>
       </c>
       <c r="K54" t="n">
         <v>72.71280827366745</v>
@@ -6522,10 +6522,10 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>95144979.32683986</v>
+        <v>95144377.64945558</v>
       </c>
       <c r="C55" t="n">
-        <v>-181007456.3519843</v>
+        <v>-181006532.7089282</v>
       </c>
       <c r="D55" t="n">
         <v>47</v>
@@ -6551,10 +6551,10 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>67.84998854730327</v>
+        <v>67.85003385103735</v>
       </c>
       <c r="J55" t="n">
-        <v>-178.8666781193634</v>
+        <v>-178.8666328156293</v>
       </c>
       <c r="K55" t="n">
         <v>73.0004992511233</v>
@@ -6636,10 +6636,10 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>116765237.1330395</v>
+        <v>116766921.1118291</v>
       </c>
       <c r="C56" t="n">
-        <v>-201589320.5850689</v>
+        <v>-201591453.3137347</v>
       </c>
       <c r="D56" t="n">
         <v>47</v>
@@ -6665,10 +6665,10 @@
         </is>
       </c>
       <c r="I56" t="n">
-        <v>65.65005069036712</v>
+        <v>65.64993109311825</v>
       </c>
       <c r="J56" t="n">
-        <v>-176.4332826429662</v>
+        <v>-176.4334022402151</v>
       </c>
       <c r="K56" t="n">
         <v>72.89318839134337</v>
@@ -6746,10 +6746,10 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>90078482.66003077</v>
+        <v>90078456.88577609</v>
       </c>
       <c r="C57" t="n">
-        <v>-175847742.4345175</v>
+        <v>-175847701.1475296</v>
       </c>
       <c r="D57" t="n">
         <v>47</v>
@@ -6775,10 +6775,10 @@
         </is>
       </c>
       <c r="I57" t="n">
-        <v>68.41666202381649</v>
+        <v>68.41666399454323</v>
       </c>
       <c r="J57" t="n">
-        <v>-179.8166713095169</v>
+        <v>-179.8166693387901</v>
       </c>
       <c r="K57" t="n">
         <v>72.84959633210406</v>
@@ -6856,10 +6856,10 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>112421186.6435295</v>
+        <v>112420323.0307304</v>
       </c>
       <c r="C58" t="n">
-        <v>-203309627.5781915</v>
+        <v>-203308439.8632879</v>
       </c>
       <c r="D58" t="n">
         <v>47</v>
@@ -6885,10 +6885,10 @@
         </is>
       </c>
       <c r="I58" t="n">
-        <v>66.41674402719615</v>
+        <v>66.41680456975236</v>
       </c>
       <c r="J58" t="n">
-        <v>-178.9165893061372</v>
+        <v>-178.916528763581</v>
       </c>
       <c r="K58" t="n">
         <v>73.28719028989869</v>
@@ -6966,10 +6966,10 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>101353956.1124853</v>
+        <v>101355383.3196585</v>
       </c>
       <c r="C59" t="n">
-        <v>-174380278.5482855</v>
+        <v>-174382160.4228776</v>
       </c>
       <c r="D59" t="n">
         <v>47</v>
@@ -6995,10 +6995,10 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>66.31658417360453</v>
+        <v>66.31647215465077</v>
       </c>
       <c r="J59" t="n">
-        <v>-172.4167491597289</v>
+        <v>-172.4168611786827</v>
       </c>
       <c r="K59" t="n">
         <v>72.71822434557579</v>
@@ -7080,10 +7080,10 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>108990125.585209</v>
+        <v>108991586.5147202</v>
       </c>
       <c r="C60" t="n">
-        <v>-198400944.9399034</v>
+        <v>-198402990.7056906</v>
       </c>
       <c r="D60" t="n">
         <v>47</v>
@@ -7109,10 +7109,10 @@
         </is>
       </c>
       <c r="I60" t="n">
-        <v>66.65010862310646</v>
+        <v>66.65000457643262</v>
       </c>
       <c r="J60" t="n">
-        <v>-178.6165580435602</v>
+        <v>-178.616662090234</v>
       </c>
       <c r="K60" t="n">
         <v>73.47882932716485</v>
@@ -7190,10 +7190,10 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>122728632.492375</v>
+        <v>122728333.8382406</v>
       </c>
       <c r="C61" t="n">
-        <v>-218062593.9383368</v>
+        <v>-218062204.4267837</v>
       </c>
       <c r="D61" t="n">
         <v>47</v>
@@ -7219,10 +7219,10 @@
         </is>
       </c>
       <c r="I61" t="n">
-        <v>65.76670766974841</v>
+        <v>65.76672767134704</v>
       </c>
       <c r="J61" t="n">
-        <v>-179.9666256635849</v>
+        <v>-179.9666056619863</v>
       </c>
       <c r="K61" t="n">
         <v>73.22574178027264</v>
@@ -7300,10 +7300,10 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>123510164.7726939</v>
+        <v>123509537.614461</v>
       </c>
       <c r="C62" t="n">
-        <v>-204561546.3511443</v>
+        <v>-204560820.8228306</v>
       </c>
       <c r="D62" t="n">
         <v>47</v>
@@ -7329,10 +7329,10 @@
         </is>
       </c>
       <c r="I62" t="n">
-        <v>64.85002801599575</v>
+        <v>64.85007236888998</v>
       </c>
       <c r="J62" t="n">
-        <v>-175.0999719840042</v>
+        <v>-175.09992763111</v>
       </c>
       <c r="K62" t="n">
         <v>73.1524133787302</v>
@@ -7414,10 +7414,10 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>100300642.5028112</v>
+        <v>100299148.9200183</v>
       </c>
       <c r="C63" t="n">
-        <v>-170669436.9423906</v>
+        <v>-170667493.1168369</v>
       </c>
       <c r="D63" t="n">
         <v>47</v>
@@ -7443,10 +7443,10 @@
         </is>
       </c>
       <c r="I63" t="n">
-        <v>66.23326588624691</v>
+        <v>66.23338504106674</v>
       </c>
       <c r="J63" t="n">
-        <v>-171.3334007804197</v>
+        <v>-171.3332816255999</v>
       </c>
       <c r="K63" t="n">
         <v>73.12355947489728</v>
@@ -7528,10 +7528,10 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>110373640.5749958</v>
+        <v>110374195.7526035</v>
       </c>
       <c r="C64" t="n">
-        <v>-200843805.4986471</v>
+        <v>-200844579.8181961</v>
       </c>
       <c r="D64" t="n">
         <v>47</v>
@@ -7557,10 +7557,10 @@
         </is>
       </c>
       <c r="I64" t="n">
-        <v>66.58350997521569</v>
+        <v>66.58347076520759</v>
       </c>
       <c r="J64" t="n">
-        <v>-178.9164900247843</v>
+        <v>-178.9165292347924</v>
       </c>
       <c r="K64" t="n">
         <v>73.1961866532865</v>
@@ -7646,10 +7646,10 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>102481904.874213</v>
+        <v>102482765.1258514</v>
       </c>
       <c r="C65" t="n">
-        <v>-192204907.2039707</v>
+        <v>-192206181.790361</v>
       </c>
       <c r="D65" t="n">
         <v>47</v>
@@ -7675,10 +7675,10 @@
         </is>
       </c>
       <c r="I65" t="n">
-        <v>67.31664487291627</v>
+        <v>67.31658256063095</v>
       </c>
       <c r="J65" t="n">
-        <v>-179.4666884604171</v>
+        <v>-179.4667507727024</v>
       </c>
       <c r="K65" t="n">
         <v>72.43742550655541</v>
@@ -7760,10 +7760,10 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>105782274.34132</v>
+        <v>105781919.9968431</v>
       </c>
       <c r="C66" t="n">
-        <v>-174815707.5859639</v>
+        <v>-174815274.6477909</v>
       </c>
       <c r="D66" t="n">
         <v>47</v>
@@ -7789,10 +7789,10 @@
         </is>
       </c>
       <c r="I66" t="n">
-        <v>65.60002875733929</v>
+        <v>65.60005668332937</v>
       </c>
       <c r="J66" t="n">
-        <v>-170.6166379093274</v>
+        <v>-170.6166099833373</v>
       </c>
       <c r="K66" t="n">
         <v>73.5534686458649</v>
@@ -7874,10 +7874,10 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>111386930.7365307</v>
+        <v>111386948.7224587</v>
       </c>
       <c r="C67" t="n">
-        <v>-202327117.153652</v>
+        <v>-202327142.1118898</v>
       </c>
       <c r="D67" t="n">
         <v>47</v>
@@ -7903,10 +7903,10 @@
         </is>
       </c>
       <c r="I67" t="n">
-        <v>66.51663782919877</v>
+        <v>66.5166365649881</v>
       </c>
       <c r="J67" t="n">
-        <v>-179.0166955041346</v>
+        <v>-179.0166967683453</v>
       </c>
       <c r="K67" t="n">
         <v>72.9056150535482</v>
@@ -7988,10 +7988,10 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>99475750.87607253</v>
+        <v>99476173.42223467</v>
       </c>
       <c r="C68" t="n">
-        <v>-172150960.8091157</v>
+        <v>-172151525.9484709</v>
       </c>
       <c r="D68" t="n">
         <v>47</v>
@@ -8017,10 +8017,10 @@
         </is>
       </c>
       <c r="I68" t="n">
-        <v>66.4834134900225</v>
+        <v>66.48338006233624</v>
       </c>
       <c r="J68" t="n">
-        <v>-172.3832531766441</v>
+        <v>-172.3832866043304</v>
       </c>
       <c r="K68" t="n">
         <v>72.98326485619801</v>
@@ -8102,10 +8102,10 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>98869816.35752448</v>
+        <v>98869799.25116791</v>
       </c>
       <c r="C69" t="n">
-        <v>-165438070.2453113</v>
+        <v>-165438048.4331167</v>
       </c>
       <c r="D69" t="n">
         <v>47</v>
@@ -8131,10 +8131,10 @@
         </is>
       </c>
       <c r="I69" t="n">
-        <v>66.10010451914354</v>
+        <v>66.10010591642528</v>
       </c>
       <c r="J69" t="n">
-        <v>-169.7498954808565</v>
+        <v>-169.7498940835748</v>
       </c>
       <c r="K69" t="n">
         <v>72.75272472752725</v>
@@ -8216,10 +8216,10 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>104219668.5023493</v>
+        <v>104221392.1295946</v>
       </c>
       <c r="C70" t="n">
-        <v>-177743836.1466576</v>
+        <v>-177746059.5469749</v>
       </c>
       <c r="D70" t="n">
         <v>47</v>
@@ -8245,10 +8245,10 @@
         </is>
       </c>
       <c r="I70" t="n">
-        <v>66.06670557210387</v>
+        <v>66.0665718665087</v>
       </c>
       <c r="J70" t="n">
-        <v>-172.4832944278961</v>
+        <v>-172.4834281334913</v>
       </c>
       <c r="K70" t="n">
         <v>72.78911564625849</v>
@@ -8326,10 +8326,10 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>117054203.5502286</v>
+        <v>117053928.7929806</v>
       </c>
       <c r="C71" t="n">
-        <v>-196200399.241827</v>
+        <v>-196200068.0253333</v>
       </c>
       <c r="D71" t="n">
         <v>47</v>
@@ -8355,10 +8355,10 @@
         </is>
       </c>
       <c r="I71" t="n">
-        <v>65.26665103512377</v>
+        <v>65.26667100137352</v>
       </c>
       <c r="J71" t="n">
-        <v>-174.3833489648762</v>
+        <v>-174.3833289986264</v>
       </c>
       <c r="K71" t="n">
         <v>72.58933918945898</v>
@@ -8436,10 +8436,10 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>95365871.76747249</v>
+        <v>95365514.89714105</v>
       </c>
       <c r="C72" t="n">
-        <v>-181346368.7595194</v>
+        <v>-181345821.511656</v>
       </c>
       <c r="D72" t="n">
         <v>47</v>
@@ -8465,10 +8465,10 @@
         </is>
       </c>
       <c r="I72" t="n">
-        <v>67.83336632419059</v>
+        <v>67.83339316267457</v>
       </c>
       <c r="J72" t="n">
-        <v>-178.883300342476</v>
+        <v>-178.883273503992</v>
       </c>
       <c r="K72" t="n">
         <v>72.76365819491693</v>
@@ -8550,10 +8550,10 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>121303628.3113402</v>
+        <v>121303952.3934693</v>
       </c>
       <c r="C73" t="n">
-        <v>-203759795.9989638</v>
+        <v>-203760182.954509</v>
       </c>
       <c r="D73" t="n">
         <v>47</v>
@@ -8579,10 +8579,10 @@
         </is>
       </c>
       <c r="I73" t="n">
-        <v>65.11661673055883</v>
+        <v>65.11659379343152</v>
       </c>
       <c r="J73" t="n">
-        <v>-175.5500499361079</v>
+        <v>-175.5500728732352</v>
       </c>
       <c r="K73" t="n">
         <v>72.46333433103861</v>
@@ -8664,10 +8664,10 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>108554960.1844395</v>
+        <v>108553564.6148994</v>
       </c>
       <c r="C74" t="n">
-        <v>-192823921.6748115</v>
+        <v>-192822032.907654</v>
       </c>
       <c r="D74" t="n">
         <v>47</v>
@@ -8693,10 +8693,10 @@
         </is>
       </c>
       <c r="I74" t="n">
-        <v>66.36665950224786</v>
+        <v>66.36676125764126</v>
       </c>
       <c r="J74" t="n">
-        <v>-176.6000071644188</v>
+        <v>-176.5999054090254</v>
       </c>
       <c r="K74" t="n">
         <v>72.35975244559793</v>
@@ -8774,10 +8774,10 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>94542668.27345119</v>
+        <v>94543489.69320977</v>
       </c>
       <c r="C75" t="n">
-        <v>-181174493.6530331</v>
+        <v>-181175767.7115108</v>
       </c>
       <c r="D75" t="n">
         <v>47</v>
@@ -8803,10 +8803,10 @@
         </is>
       </c>
       <c r="I75" t="n">
-        <v>67.96672750150034</v>
+        <v>67.96666576732515</v>
       </c>
       <c r="J75" t="n">
-        <v>-179.3332724984996</v>
+        <v>-179.3333342326748</v>
       </c>
       <c r="K75" t="n">
         <v>72.48275172482751</v>
@@ -8892,10 +8892,10 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>126364001.9614239</v>
+        <v>126364914.1193085</v>
       </c>
       <c r="C76" t="n">
-        <v>-208391483.5858551</v>
+        <v>-208392521.0905573</v>
       </c>
       <c r="D76" t="n">
         <v>47</v>
@@ -8921,10 +8921,10 @@
         </is>
       </c>
       <c r="I76" t="n">
-        <v>64.68336175479625</v>
+        <v>64.68329803341744</v>
       </c>
       <c r="J76" t="n">
-        <v>-175.4833049118704</v>
+        <v>-175.4833686332492</v>
       </c>
       <c r="K76" t="n">
         <v>72.52351410846506</v>
@@ -9006,10 +9006,10 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>114600057.7617754</v>
+        <v>114600012.8629923</v>
       </c>
       <c r="C77" t="n">
-        <v>-193023232.9809702</v>
+        <v>-193023177.9961263</v>
       </c>
       <c r="D77" t="n">
         <v>47</v>
@@ -9035,10 +9035,10 @@
         </is>
       </c>
       <c r="I77" t="n">
-        <v>65.43335182853889</v>
+        <v>65.43335512591045</v>
       </c>
       <c r="J77" t="n">
-        <v>-174.1333148381277</v>
+        <v>-174.1333115407561</v>
       </c>
       <c r="K77" t="n">
         <v>72.19341974077767</v>
@@ -9120,10 +9120,10 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>96182717.2374838</v>
+        <v>96183315.66373654</v>
       </c>
       <c r="C78" t="n">
-        <v>-167069233.2421187</v>
+        <v>-167070045.9265256</v>
       </c>
       <c r="D78" t="n">
         <v>47</v>
@@ -9149,10 +9149,10 @@
         </is>
       </c>
       <c r="I78" t="n">
-        <v>66.70001252623884</v>
+        <v>66.69996423734543</v>
       </c>
       <c r="J78" t="n">
-        <v>-171.8333208070945</v>
+        <v>-171.8333690959879</v>
       </c>
       <c r="K78" t="n">
         <v>72.36855282924385</v>
@@ -9234,10 +9234,10 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>90103790.92650808</v>
+        <v>90102554.08998811</v>
       </c>
       <c r="C79" t="n">
-        <v>-175918167.6152635</v>
+        <v>-175916186.1970724</v>
       </c>
       <c r="D79" t="n">
         <v>47</v>
@@ -9263,10 +9263,10 @@
         </is>
       </c>
       <c r="I79" t="n">
-        <v>68.41668237733052</v>
+        <v>68.41677691972966</v>
       </c>
       <c r="J79" t="n">
-        <v>-179.8333176226694</v>
+        <v>-179.8332230802703</v>
       </c>
       <c r="K79" t="n">
         <v>71.7088229436367</v>
@@ -9348,10 +9348,10 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>112423939.6619415</v>
+        <v>112423974.4583378</v>
       </c>
       <c r="C80" t="n">
-        <v>-203313413.7283501</v>
+        <v>-203313461.5824972</v>
       </c>
       <c r="D80" t="n">
         <v>47</v>
@@ -9377,10 +9377,10 @@
         </is>
       </c>
       <c r="I80" t="n">
-        <v>66.41655103159917</v>
+        <v>66.41654859227266</v>
       </c>
       <c r="J80" t="n">
-        <v>-178.9167823017342</v>
+        <v>-178.9167847410607</v>
       </c>
       <c r="K80" t="n">
         <v>72.24620945878098</v>
@@ -9458,10 +9458,10 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>110880978.5168227</v>
+        <v>110882036.2597607</v>
       </c>
       <c r="C81" t="n">
-        <v>-201587229.1416554</v>
+        <v>-201588700.6533288</v>
       </c>
       <c r="D81" t="n">
         <v>47</v>
@@ -9487,10 +9487,10 @@
         </is>
       </c>
       <c r="I81" t="n">
-        <v>66.54997985485556</v>
+        <v>66.5499053300544</v>
       </c>
       <c r="J81" t="n">
-        <v>-178.9666868118111</v>
+        <v>-178.9667613366123</v>
       </c>
       <c r="K81" t="n">
         <v>71.84097492757967</v>
@@ -9572,10 +9572,10 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>111720135.9280964</v>
+        <v>111720467.1438562</v>
       </c>
       <c r="C82" t="n">
-        <v>-202900426.6929799</v>
+        <v>-202900885.8178033</v>
       </c>
       <c r="D82" t="n">
         <v>47</v>
@@ -9601,10 +9601,10 @@
         </is>
       </c>
       <c r="I82" t="n">
-        <v>66.50003988393064</v>
+        <v>66.50001664796537</v>
       </c>
       <c r="J82" t="n">
-        <v>-179.0832934494026</v>
+        <v>-179.0833166853679</v>
       </c>
       <c r="K82" t="n">
         <v>72.01242111589704</v>
@@ -9686,10 +9686,10 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>112374935.9972873</v>
+        <v>112373855.7463913</v>
       </c>
       <c r="C83" t="n">
-        <v>-185557290.790704</v>
+        <v>-185556001.5893668</v>
       </c>
       <c r="D83" t="n">
         <v>47</v>
@@ -9715,10 +9715,10 @@
         </is>
       </c>
       <c r="I83" t="n">
-        <v>65.28341023740553</v>
+        <v>65.28349197645129</v>
       </c>
       <c r="J83" t="n">
-        <v>-172.1999230959278</v>
+        <v>-172.199841356882</v>
       </c>
       <c r="K83" t="n">
         <v>72.24399557833382</v>
@@ -9796,10 +9796,10 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>103127393.1932825</v>
+        <v>103127200.0445412</v>
       </c>
       <c r="C84" t="n">
-        <v>-172088725.1295874</v>
+        <v>-172088483.342384</v>
       </c>
       <c r="D84" t="n">
         <v>47</v>
@@ -9825,10 +9825,10 @@
         </is>
       </c>
       <c r="I84" t="n">
-        <v>65.85007944968972</v>
+        <v>65.85009481509421</v>
       </c>
       <c r="J84" t="n">
-        <v>-170.6332538836436</v>
+        <v>-170.6332385182391</v>
       </c>
       <c r="K84" t="n">
         <v>71.55249775650614</v>
@@ -9906,10 +9906,10 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>122710867.0445147</v>
+        <v>122708990.1519759</v>
       </c>
       <c r="C85" t="n">
-        <v>-203257325.3563437</v>
+        <v>-203255148.1129821</v>
       </c>
       <c r="D85" t="n">
         <v>47</v>
@@ -9935,10 +9935,10 @@
         </is>
       </c>
       <c r="I85" t="n">
-        <v>64.8833321995574</v>
+        <v>64.88346552127494</v>
       </c>
       <c r="J85" t="n">
-        <v>-174.9166678004426</v>
+        <v>-174.9165344787251</v>
       </c>
       <c r="K85" t="n">
         <v>71.23002084781098</v>
@@ -10016,10 +10016,10 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>111990549.4419555</v>
+        <v>111990891.5363045</v>
       </c>
       <c r="C86" t="n">
-        <v>-203312206.8927979</v>
+        <v>-203312680.5100742</v>
       </c>
       <c r="D86" t="n">
         <v>47</v>
@@ -10045,10 +10045,10 @@
         </is>
       </c>
       <c r="I86" t="n">
-        <v>66.48335103265381</v>
+        <v>66.48332706555925</v>
       </c>
       <c r="J86" t="n">
-        <v>-179.1166489673462</v>
+        <v>-179.1166729344408</v>
       </c>
       <c r="K86" t="n">
         <v>71.66983111821725</v>
@@ -10130,10 +10130,10 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>98871311.63442823</v>
+        <v>98870863.49995132</v>
       </c>
       <c r="C87" t="n">
-        <v>-168604841.0895316</v>
+        <v>-168604253.3247996</v>
       </c>
       <c r="D87" t="n">
         <v>47</v>
@@ -10159,10 +10159,10 @@
         </is>
       </c>
       <c r="I87" t="n">
-        <v>66.33342876510508</v>
+        <v>66.33346480185764</v>
       </c>
       <c r="J87" t="n">
-        <v>-171.1332379015615</v>
+        <v>-171.1332018648089</v>
       </c>
       <c r="K87" t="n">
         <v>71.77613135762914</v>
@@ -10244,10 +10244,10 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>107111056.3425351</v>
+        <v>107111037.3784975</v>
       </c>
       <c r="C88" t="n">
-        <v>-195472349.8516857</v>
+        <v>-195472323.0756261</v>
       </c>
       <c r="D88" t="n">
         <v>47</v>
@@ -10273,10 +10273,10 @@
         </is>
       </c>
       <c r="I88" t="n">
-        <v>66.76667840048799</v>
+        <v>66.76667976443922</v>
       </c>
       <c r="J88" t="n">
-        <v>-178.3666549328454</v>
+        <v>-178.3666535688942</v>
       </c>
       <c r="K88" t="n">
         <v>71.57558197622139</v>
@@ -10354,10 +10354,10 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>90347365.26830955</v>
+        <v>90346546.34698622</v>
       </c>
       <c r="C89" t="n">
-        <v>-176338122.2630417</v>
+        <v>-176336811.5477049</v>
       </c>
       <c r="D89" t="n">
         <v>47</v>
@@ -10383,10 +10383,10 @@
         </is>
       </c>
       <c r="I89" t="n">
-        <v>68.40003475744538</v>
+        <v>68.40009725641835</v>
       </c>
       <c r="J89" t="n">
-        <v>-179.8666319092213</v>
+        <v>-179.8665694102483</v>
       </c>
       <c r="K89" t="n">
         <v>71.23779150886985</v>
@@ -10464,10 +10464,10 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>102530379.9016063</v>
+        <v>102529579.9533198</v>
       </c>
       <c r="C90" t="n">
-        <v>-191802337.6301251</v>
+        <v>-191801156.5092006</v>
       </c>
       <c r="D90" t="n">
         <v>47</v>
@@ -10493,10 +10493,10 @@
         </is>
       </c>
       <c r="I90" t="n">
-        <v>67.2832438056665</v>
+        <v>67.2833018584483</v>
       </c>
       <c r="J90" t="n">
-        <v>-179.2667561943335</v>
+        <v>-179.2666981415517</v>
       </c>
       <c r="K90" t="n">
         <v>71.19337457593295</v>
@@ -10578,10 +10578,10 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>90103925.83790122</v>
+        <v>90104528.73577157</v>
       </c>
       <c r="C91" t="n">
-        <v>-175918383.7433024</v>
+        <v>-175919349.5840066</v>
       </c>
       <c r="D91" t="n">
         <v>47</v>
@@ -10607,10 +10607,10 @@
         </is>
       </c>
       <c r="I91" t="n">
-        <v>68.41667206489616</v>
+        <v>68.41662598034323</v>
       </c>
       <c r="J91" t="n">
-        <v>-179.8333279351038</v>
+        <v>-179.8333740196567</v>
       </c>
       <c r="K91" t="n">
         <v>70.98543786155993</v>
@@ -10696,10 +10696,10 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>99291195.39419353</v>
+        <v>99291993.9236518</v>
       </c>
       <c r="C92" t="n">
-        <v>-180336735.1781213</v>
+        <v>-180337878.069048</v>
       </c>
       <c r="D92" t="n">
         <v>47</v>
@@ -10725,10 +10725,10 @@
         </is>
       </c>
       <c r="I92" t="n">
-        <v>67.08339802509568</v>
+        <v>67.08333728349645</v>
       </c>
       <c r="J92" t="n">
-        <v>-176.083268641571</v>
+        <v>-176.0833293831702</v>
       </c>
       <c r="K92" t="n">
         <v>71.29676060575669</v>
@@ -10810,10 +10810,10 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>89515138.18118136</v>
+        <v>89515739.4878577</v>
       </c>
       <c r="C93" t="n">
-        <v>-174795692.2836212</v>
+        <v>-174796657.0264485</v>
       </c>
       <c r="D93" t="n">
         <v>47</v>
@@ -10839,10 +10839,10 @@
         </is>
       </c>
       <c r="I93" t="n">
-        <v>68.4500570897184</v>
+        <v>68.45001092686159</v>
       </c>
       <c r="J93" t="n">
-        <v>-179.6999429102816</v>
+        <v>-179.6999890731384</v>
       </c>
       <c r="K93" t="n">
         <v>70.91689115035416</v>
@@ -10920,10 +10920,10 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>90104599.81563872</v>
+        <v>90103705.07885629</v>
       </c>
       <c r="C94" t="n">
-        <v>-175919463.4535802</v>
+        <v>-175918030.0872642</v>
       </c>
       <c r="D94" t="n">
         <v>47</v>
@@ -10949,10 +10949,10 @@
         </is>
       </c>
       <c r="I94" t="n">
-        <v>68.41662054712215</v>
+        <v>68.41668893940675</v>
       </c>
       <c r="J94" t="n">
-        <v>-179.8333794528778</v>
+        <v>-179.8333110605932</v>
       </c>
       <c r="K94" t="n">
         <v>70.77812095247586</v>
@@ -11030,10 +11030,10 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>89566559.09773922</v>
+        <v>89565870.73928922</v>
       </c>
       <c r="C95" t="n">
-        <v>-174937605.485363</v>
+        <v>-174936500.8971657</v>
       </c>
       <c r="D95" t="n">
         <v>47</v>
@@ -11059,10 +11059,10 @@
         </is>
       </c>
       <c r="I95" t="n">
-        <v>68.45001264493334</v>
+        <v>68.45006545965302</v>
       </c>
       <c r="J95" t="n">
-        <v>-179.7333206884</v>
+        <v>-179.7332678736803</v>
       </c>
       <c r="K95" t="n">
         <v>70.72489779639045</v>
@@ -11140,10 +11140,10 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>105283032.7366307</v>
+        <v>105283796.2110587</v>
       </c>
       <c r="C96" t="n">
-        <v>-180788096.2565957</v>
+        <v>-180789088.1050727</v>
       </c>
       <c r="D96" t="n">
         <v>47</v>
@@ -11169,10 +11169,10 @@
         </is>
       </c>
       <c r="I96" t="n">
-        <v>66.10008077205472</v>
+        <v>66.10002228992205</v>
       </c>
       <c r="J96" t="n">
-        <v>-173.2499192279453</v>
+        <v>-173.249977710078</v>
       </c>
       <c r="K96" t="n">
         <v>71.15616218386189</v>
@@ -11250,10 +11250,10 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>92664415.74031872</v>
+        <v>92663656.04225837</v>
       </c>
       <c r="C97" t="n">
-        <v>-179137113.8263955</v>
+        <v>-179135917.8359909</v>
       </c>
       <c r="D97" t="n">
         <v>47</v>
@@ -11279,10 +11279,10 @@
         </is>
       </c>
       <c r="I97" t="n">
-        <v>68.16669219156609</v>
+        <v>68.16674964458576</v>
       </c>
       <c r="J97" t="n">
-        <v>-179.6166411417673</v>
+        <v>-179.6165836887476</v>
       </c>
       <c r="K97" t="n">
         <v>70.79876037188845</v>
@@ -11368,10 +11368,10 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>105995905.4567777</v>
+        <v>105995838.9598717</v>
       </c>
       <c r="C98" t="n">
-        <v>-186983498.0103559</v>
+        <v>-186983408.2862068</v>
       </c>
       <c r="D98" t="n">
         <v>47</v>
@@ -11397,10 +11397,10 @@
         </is>
       </c>
       <c r="I98" t="n">
-        <v>66.39998833668601</v>
+        <v>66.39999329391829</v>
       </c>
       <c r="J98" t="n">
-        <v>-175.450011663314</v>
+        <v>-175.4500067060817</v>
       </c>
       <c r="K98" t="n">
         <v>70.71514182980424</v>
@@ -11482,10 +11482,10 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>111850004.2022698</v>
+        <v>111852843.7911268</v>
       </c>
       <c r="C99" t="n">
-        <v>-203229053.4905242</v>
+        <v>-203232990.950353</v>
       </c>
       <c r="D99" t="n">
         <v>47</v>
@@ -11511,10 +11511,10 @@
         </is>
       </c>
       <c r="I99" t="n">
-        <v>66.50000423063585</v>
+        <v>66.4998052612837</v>
       </c>
       <c r="J99" t="n">
-        <v>-179.1499957693642</v>
+        <v>-179.1501947387164</v>
       </c>
       <c r="K99" t="n">
         <v>70.59469167830773</v>
@@ -11596,10 +11596,10 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>108682215.0231036</v>
+        <v>108682011.9880013</v>
       </c>
       <c r="C100" t="n">
-        <v>-198149523.846813</v>
+        <v>-198149238.6850535</v>
       </c>
       <c r="D100" t="n">
         <v>47</v>
@@ -11625,10 +11625,10 @@
         </is>
       </c>
       <c r="I100" t="n">
-        <v>66.6832680201298</v>
+        <v>66.6832824892318</v>
       </c>
       <c r="J100" t="n">
-        <v>-178.6667319798702</v>
+        <v>-178.6667175107682</v>
       </c>
       <c r="K100" t="n">
         <v>70.73999999999998</v>
@@ -11706,10 +11706,10 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>123263194.7934499</v>
+        <v>123262330.9647697</v>
       </c>
       <c r="C101" t="n">
-        <v>-200773555.3995813</v>
+        <v>-200772585.0239061</v>
       </c>
       <c r="D101" t="n">
         <v>47</v>
@@ -11735,10 +11735,10 @@
         </is>
       </c>
       <c r="I101" t="n">
-        <v>64.65007690462897</v>
+        <v>64.65013892656799</v>
       </c>
       <c r="J101" t="n">
-        <v>-173.9165897620377</v>
+        <v>-173.9165277400987</v>
       </c>
       <c r="K101" t="n">
         <v>70.87592703948687</v>
@@ -11820,10 +11820,10 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>95284001.11153802</v>
+        <v>95285337.07413501</v>
       </c>
       <c r="C102" t="n">
-        <v>-181126436.5794339</v>
+        <v>-181128484.7188572</v>
       </c>
       <c r="D102" t="n">
         <v>47</v>
@@ -11849,10 +11849,10 @@
         </is>
       </c>
       <c r="I102" t="n">
-        <v>67.83336140894836</v>
+        <v>67.83326084876389</v>
       </c>
       <c r="J102" t="n">
-        <v>-178.8333052577183</v>
+        <v>-178.8334058179028</v>
       </c>
       <c r="K102" t="n">
         <v>70.27161476470002</v>
@@ -11934,10 +11934,10 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>103206311.7080425</v>
+        <v>103205198.4397278</v>
       </c>
       <c r="C103" t="n">
-        <v>-192252878.875446</v>
+        <v>-192251246.9216498</v>
       </c>
       <c r="D103" t="n">
         <v>47</v>
@@ -11963,10 +11963,10 @@
         </is>
       </c>
       <c r="I103" t="n">
-        <v>67.19987818182531</v>
+        <v>67.19995889903838</v>
       </c>
       <c r="J103" t="n">
-        <v>-179.083455151508</v>
+        <v>-179.0833744342949</v>
       </c>
       <c r="K103" t="n">
         <v>70.59823929571829</v>
@@ -12052,10 +12052,10 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>106044442.6357666</v>
+        <v>106043189.6412067</v>
       </c>
       <c r="C104" t="n">
-        <v>-192488568.9412396</v>
+        <v>-192486808.2343917</v>
       </c>
       <c r="D104" t="n">
         <v>47</v>
@@ -12081,10 +12081,10 @@
         </is>
       </c>
       <c r="I104" t="n">
-        <v>66.74993034355941</v>
+        <v>66.75002149972727</v>
       </c>
       <c r="J104" t="n">
-        <v>-177.6834029897739</v>
+        <v>-177.683311833606</v>
       </c>
       <c r="K104" t="n">
         <v>70.8463005722317</v>
@@ -12166,10 +12166,10 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>97110995.55015253</v>
+        <v>97110372.26147208</v>
       </c>
       <c r="C105" t="n">
-        <v>-181416775.6881125</v>
+        <v>-181415844.8991398</v>
       </c>
       <c r="D105" t="n">
         <v>47</v>
@@ -12195,10 +12195,10 @@
         </is>
       </c>
       <c r="I105" t="n">
-        <v>67.53320201763403</v>
+        <v>67.5332490191344</v>
       </c>
       <c r="J105" t="n">
-        <v>-177.8334646490326</v>
+        <v>-177.8334176475322</v>
       </c>
       <c r="K105" t="n">
         <v>70.29989040549964</v>
@@ -12280,10 +12280,10 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>131242611.0262185</v>
+        <v>131241033.4827757</v>
       </c>
       <c r="C106" t="n">
-        <v>-226691592.6217423</v>
+        <v>-226689672.8295892</v>
       </c>
       <c r="D106" t="n">
         <v>47</v>
@@ -12309,10 +12309,10 @@
         </is>
       </c>
       <c r="I106" t="n">
-        <v>65.08346460721658</v>
+        <v>65.08356788440834</v>
       </c>
       <c r="J106" t="n">
-        <v>-179.83320205945</v>
+        <v>-179.8330987822582</v>
       </c>
       <c r="K106" t="n">
         <v>70.11631374888159</v>
@@ -12394,10 +12394,10 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>117129515.137243</v>
+        <v>117129631.2220052</v>
       </c>
       <c r="C107" t="n">
-        <v>-199529806.5510803</v>
+        <v>-199529950.2677192</v>
       </c>
       <c r="D107" t="n">
         <v>47</v>
@@ -12423,10 +12423,10 @@
         </is>
       </c>
       <c r="I107" t="n">
-        <v>65.46662074064554</v>
+        <v>65.46661242135529</v>
       </c>
       <c r="J107" t="n">
-        <v>-175.5500459260211</v>
+        <v>-175.5500542453113</v>
       </c>
       <c r="K107" t="n">
         <v>70.5480827143144</v>
@@ -12508,10 +12508,10 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>94929093.34019737</v>
+        <v>94928926.66890271</v>
       </c>
       <c r="C108" t="n">
-        <v>-181961555.8396538</v>
+        <v>-181961297.4746547</v>
       </c>
       <c r="D108" t="n">
         <v>47</v>
@@ -12537,10 +12537,10 @@
         </is>
       </c>
       <c r="I108" t="n">
-        <v>67.94991100094209</v>
+        <v>67.94992348961935</v>
       </c>
       <c r="J108" t="n">
-        <v>-179.4500889990579</v>
+        <v>-179.4500765103807</v>
       </c>
       <c r="K108" t="n">
         <v>69.97702068138675</v>
@@ -12622,10 +12622,10 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>108291038.0034577</v>
+        <v>108290145.0312245</v>
       </c>
       <c r="C109" t="n">
-        <v>-179957228.0258081</v>
+        <v>-179956136.3726603</v>
       </c>
       <c r="D109" t="n">
         <v>47</v>
@@ -12651,10 +12651,10 @@
         </is>
       </c>
       <c r="I109" t="n">
-        <v>65.54998505796823</v>
+        <v>65.55005399976875</v>
       </c>
       <c r="J109" t="n">
-        <v>-171.6333482753651</v>
+        <v>-171.6332793335646</v>
       </c>
       <c r="K109" t="n">
         <v>70.32238626092196</v>
@@ -12736,10 +12736,10 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>88934289.42342946</v>
+        <v>88934308.95905775</v>
       </c>
       <c r="C110" t="n">
-        <v>-170947381.6615569</v>
+        <v>-170947412.4750854</v>
       </c>
       <c r="D110" t="n">
         <v>47</v>
@@ -12765,10 +12765,10 @@
         </is>
       </c>
       <c r="I110" t="n">
-        <v>68.30006331731207</v>
+        <v>68.30006179053748</v>
       </c>
       <c r="J110" t="n">
-        <v>-178.1999366826879</v>
+        <v>-178.1999382094625</v>
       </c>
       <c r="K110" t="n">
         <v>69.7549312612074</v>
@@ -12854,10 +12854,10 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>103973242.3097483</v>
+        <v>103972565.9586297</v>
       </c>
       <c r="C111" t="n">
-        <v>-177149926.3409938</v>
+        <v>-177149054.5000275</v>
       </c>
       <c r="D111" t="n">
         <v>47</v>
@@ -12883,10 +12883,10 @@
         </is>
       </c>
       <c r="I111" t="n">
-        <v>66.06655834058715</v>
+        <v>66.06661093455867</v>
       </c>
       <c r="J111" t="n">
-        <v>-172.3501083260795</v>
+        <v>-172.350055732108</v>
       </c>
       <c r="K111" t="n">
         <v>69.81847197287053</v>
@@ -12964,10 +12964,10 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>112619363.6736304</v>
+        <v>112619817.770193</v>
       </c>
       <c r="C112" t="n">
-        <v>-204630624.7919917</v>
+        <v>-204631253.2676903</v>
       </c>
       <c r="D112" t="n">
         <v>47</v>
@@ -12993,10 +12993,10 @@
         </is>
       </c>
       <c r="I112" t="n">
-        <v>66.46664325015371</v>
+        <v>66.4666115821768</v>
       </c>
       <c r="J112" t="n">
-        <v>-179.3333567498462</v>
+        <v>-179.3333884178231</v>
       </c>
       <c r="K112" t="n">
         <v>69.63272618692147</v>
@@ -13074,10 +13074,10 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>90461016.56727831</v>
+        <v>90460510.7681088</v>
       </c>
       <c r="C113" t="n">
-        <v>-173376641.2661828</v>
+        <v>-173375849.083366</v>
       </c>
       <c r="D113" t="n">
         <v>47</v>
@@ -13103,10 +13103,10 @@
         </is>
       </c>
       <c r="I113" t="n">
-        <v>68.18328501231335</v>
+        <v>68.18332418364429</v>
       </c>
       <c r="J113" t="n">
-        <v>-178.3333816543533</v>
+        <v>-178.3333424830224</v>
       </c>
       <c r="K113" t="n">
         <v>69.46762018275724</v>
@@ -13192,10 +13192,10 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>90323452.64385182</v>
+        <v>90322966.28199582</v>
       </c>
       <c r="C114" t="n">
-        <v>-173250613.5704355</v>
+        <v>-173249850.8613234</v>
       </c>
       <c r="D114" t="n">
         <v>47</v>
@@ -13221,10 +13221,10 @@
         </is>
       </c>
       <c r="I114" t="n">
-        <v>68.1999512195265</v>
+        <v>68.19998889913731</v>
       </c>
       <c r="J114" t="n">
-        <v>-178.3667154471402</v>
+        <v>-178.3666777675294</v>
       </c>
       <c r="K114" t="n">
         <v>69.40848436566421</v>
@@ -13310,10 +13310,10 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>127185600.9567544</v>
+        <v>127185375.7843002</v>
       </c>
       <c r="C115" t="n">
-        <v>-222549627.4635976</v>
+        <v>-222549344.2806582</v>
       </c>
       <c r="D115" t="n">
         <v>47</v>
@@ -13339,10 +13339,10 @@
         </is>
       </c>
       <c r="I115" t="n">
-        <v>65.39998638549125</v>
+        <v>65.40000128864895</v>
       </c>
       <c r="J115" t="n">
-        <v>-179.8500136145088</v>
+        <v>-179.8499987113511</v>
       </c>
       <c r="K115" t="n">
         <v>69.9488105992171</v>
@@ -13416,10 +13416,10 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>104323840.462929</v>
+        <v>104324543.1966155</v>
       </c>
       <c r="C116" t="n">
-        <v>-179676334.3504549</v>
+        <v>-179677254.0545461</v>
       </c>
       <c r="D116" t="n">
         <v>47</v>
@@ -13445,10 +13445,10 @@
         </is>
       </c>
       <c r="I116" t="n">
-        <v>66.18324920806168</v>
+        <v>66.18319517511321</v>
       </c>
       <c r="J116" t="n">
-        <v>-173.2334174586049</v>
+        <v>-173.2334714915534</v>
       </c>
       <c r="K116" t="n">
         <v>69.41258601775206</v>
@@ -13526,10 +13526,10 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>104885273.8681174</v>
+        <v>104886990.260056</v>
       </c>
       <c r="C117" t="n">
-        <v>-183987818.6619841</v>
+        <v>-183990122.8937142</v>
       </c>
       <c r="D117" t="n">
         <v>47</v>
@@ -13555,10 +13555,10 @@
         </is>
       </c>
       <c r="I117" t="n">
-        <v>66.38323079425454</v>
+        <v>66.38310130508553</v>
       </c>
       <c r="J117" t="n">
-        <v>-174.7501025390788</v>
+        <v>-174.7502320282478</v>
       </c>
       <c r="K117" t="n">
         <v>69.68847039967945</v>
@@ -13644,10 +13644,10 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>120626242.0701926</v>
+        <v>120626767.3054073</v>
       </c>
       <c r="C118" t="n">
-        <v>-201107055.5776693</v>
+        <v>-201107675.9514737</v>
       </c>
       <c r="D118" t="n">
         <v>47</v>
@@ -13673,10 +13673,10 @@
         </is>
       </c>
       <c r="I118" t="n">
-        <v>65.04992755189618</v>
+        <v>65.04989000091901</v>
       </c>
       <c r="J118" t="n">
-        <v>-174.8667391147705</v>
+        <v>-174.8667766657477</v>
       </c>
       <c r="K118" t="n">
         <v>69.19544819325213</v>
@@ -13754,10 +13754,10 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>106254081.1004089</v>
+        <v>106253987.7411452</v>
       </c>
       <c r="C119" t="n">
-        <v>-191200866.8442713</v>
+        <v>-191200737.3196173</v>
       </c>
       <c r="D119" t="n">
         <v>47</v>
@@ -13783,10 +13783,10 @@
         </is>
       </c>
       <c r="I119" t="n">
-        <v>66.63323228473124</v>
+        <v>66.63323911751434</v>
       </c>
       <c r="J119" t="n">
-        <v>-177.0501010486021</v>
+        <v>-177.050094215819</v>
       </c>
       <c r="K119" t="n">
         <v>69.24767709061842</v>
@@ -13860,10 +13860,10 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>93418420.93201588</v>
+        <v>93418613.15065667</v>
       </c>
       <c r="C120" t="n">
-        <v>-177883323.0553674</v>
+        <v>-177883619.6676927</v>
       </c>
       <c r="D120" t="n">
         <v>47</v>
@@ -13889,10 +13889,10 @@
         </is>
       </c>
       <c r="I120" t="n">
-        <v>67.95006425270499</v>
+        <v>67.95004960858539</v>
       </c>
       <c r="J120" t="n">
-        <v>-178.5166024139617</v>
+        <v>-178.5166170580813</v>
       </c>
       <c r="K120" t="n">
         <v>69.16475401656521</v>
@@ -13970,10 +13970,10 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>90102621.94079775</v>
+        <v>90103152.92810416</v>
       </c>
       <c r="C121" t="n">
-        <v>-175916294.8946933</v>
+        <v>-175917145.5400779</v>
       </c>
       <c r="D121" t="n">
         <v>47</v>
@@ -13999,10 +13999,10 @@
         </is>
       </c>
       <c r="I121" t="n">
-        <v>68.4167717332719</v>
+        <v>68.41673114512862</v>
       </c>
       <c r="J121" t="n">
-        <v>-179.833228266728</v>
+        <v>-179.8332688548713</v>
       </c>
       <c r="K121" t="n">
         <v>69.07894736842105</v>
@@ -14084,10 +14084,10 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>89439994.28489967</v>
+        <v>89440695.01134434</v>
       </c>
       <c r="C122" t="n">
-        <v>-171832715.3857557</v>
+        <v>-171833818.660059</v>
       </c>
       <c r="D122" t="n">
         <v>47</v>
@@ -14113,10 +14113,10 @@
         </is>
       </c>
       <c r="I122" t="n">
-        <v>68.26657952686253</v>
+        <v>68.26652495038006</v>
       </c>
       <c r="J122" t="n">
-        <v>-178.2834204731374</v>
+        <v>-178.2834750496199</v>
       </c>
       <c r="K122" t="n">
         <v>69.26536731634184</v>
@@ -14202,10 +14202,10 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>90056071.40156201</v>
+        <v>90056417.80823579</v>
       </c>
       <c r="C123" t="n">
-        <v>-172771548.4129456</v>
+        <v>-172772092.1143855</v>
       </c>
       <c r="D123" t="n">
         <v>47</v>
@@ -14231,10 +14231,10 @@
         </is>
       </c>
       <c r="I123" t="n">
-        <v>68.21668292665927</v>
+        <v>68.21665604000741</v>
       </c>
       <c r="J123" t="n">
-        <v>-178.3166504066741</v>
+        <v>-178.316677293326</v>
       </c>
       <c r="K123" t="n">
         <v>69.16391968834283</v>
@@ -14320,10 +14320,10 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>112339625.2761361</v>
+        <v>112341383.2848444</v>
       </c>
       <c r="C124" t="n">
-        <v>-191249031.5810917</v>
+        <v>-191251237.3799561</v>
       </c>
       <c r="D124" t="n">
         <v>47</v>
@@ -14349,10 +14349,10 @@
         </is>
       </c>
       <c r="I124" t="n">
-        <v>65.66673111396588</v>
+        <v>65.6666013821248</v>
       </c>
       <c r="J124" t="n">
-        <v>-174.3499355527008</v>
+        <v>-174.3500652845419</v>
       </c>
       <c r="K124" t="n">
         <v>69.03406253121565</v>
@@ -14426,10 +14426,10 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>91638675.91084142</v>
+        <v>91638603.847031</v>
       </c>
       <c r="C125" t="n">
-        <v>-174580799.3188672</v>
+        <v>-174580687.5775971</v>
       </c>
       <c r="D125" t="n">
         <v>47</v>
@@ -14455,10 +14455,10 @@
         </is>
       </c>
       <c r="I125" t="n">
-        <v>68.04990602153245</v>
+        <v>68.04991158185356</v>
       </c>
       <c r="J125" t="n">
-        <v>-178.1167606451342</v>
+        <v>-178.1167550848131</v>
       </c>
       <c r="K125" t="n">
         <v>68.38863500894098</v>
@@ -14536,10 +14536,10 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>104042168.0730878</v>
+        <v>104041565.2928592</v>
       </c>
       <c r="C126" t="n">
-        <v>-182405823.5215728</v>
+        <v>-182405013.0074969</v>
       </c>
       <c r="D126" t="n">
         <v>47</v>
@@ -14565,10 +14565,10 @@
         </is>
       </c>
       <c r="I126" t="n">
-        <v>66.41673434655264</v>
+        <v>66.41678009567661</v>
       </c>
       <c r="J126" t="n">
-        <v>-174.499932320114</v>
+        <v>-174.49988657099</v>
       </c>
       <c r="K126" t="n">
         <v>69.03135048231512</v>
@@ -14650,10 +14650,10 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>98433685.40547928</v>
+        <v>98434944.37232505</v>
       </c>
       <c r="C127" t="n">
-        <v>-164848617.1248325</v>
+        <v>-164850226.8295321</v>
       </c>
       <c r="D127" t="n">
         <v>47</v>
@@ -14679,10 +14679,10 @@
         </is>
       </c>
       <c r="I127" t="n">
-        <v>66.13333759743972</v>
+        <v>66.13323452587909</v>
       </c>
       <c r="J127" t="n">
-        <v>-169.6999957358936</v>
+        <v>-169.7000988074542</v>
       </c>
       <c r="K127" t="n">
         <v>68.49137501246383</v>
@@ -14768,10 +14768,10 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>90105029.24682693</v>
+        <v>90102346.77343935</v>
       </c>
       <c r="C128" t="n">
-        <v>-175920151.3993</v>
+        <v>-175915854.0738463</v>
       </c>
       <c r="D128" t="n">
         <v>47</v>
@@ -14797,10 +14797,10 @@
         </is>
       </c>
       <c r="I128" t="n">
-        <v>68.41658772219928</v>
+        <v>68.41679276684177</v>
       </c>
       <c r="J128" t="n">
-        <v>-179.8334122778007</v>
+        <v>-179.8332072331582</v>
       </c>
       <c r="K128" t="n">
         <v>68.63627274545091</v>
@@ -14878,10 +14878,10 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>105297571.7318893</v>
+        <v>105297578.2185064</v>
       </c>
       <c r="C129" t="n">
-        <v>-186004414.8481569</v>
+        <v>-186004423.6349301</v>
       </c>
       <c r="D129" t="n">
         <v>47</v>
@@ -14907,10 +14907,10 @@
         </is>
       </c>
       <c r="I129" t="n">
-        <v>66.44981829372792</v>
+        <v>66.44981780852062</v>
       </c>
       <c r="J129" t="n">
-        <v>-175.3835150396054</v>
+        <v>-175.3835155248127</v>
       </c>
       <c r="K129" t="n">
         <v>68.87550200803211</v>
@@ -14992,10 +14992,10 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>91506452.89152119</v>
+        <v>91506333.97392675</v>
       </c>
       <c r="C130" t="n">
-        <v>-168656243.1493973</v>
+        <v>-168656066.0726092</v>
       </c>
       <c r="D130" t="n">
         <v>47</v>
@@ -15021,10 +15021,10 @@
         </is>
       </c>
       <c r="I130" t="n">
-        <v>67.66673433990181</v>
+        <v>67.66674378526137</v>
       </c>
       <c r="J130" t="n">
-        <v>-175.3332656600982</v>
+        <v>-175.3332562147386</v>
       </c>
       <c r="K130" t="n">
         <v>68.60955056179776</v>
@@ -15106,10 +15106,10 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>100244127.4586507</v>
+        <v>100244385.6920507</v>
       </c>
       <c r="C131" t="n">
-        <v>-181531930.5944287</v>
+        <v>-181532297.7965564</v>
       </c>
       <c r="D131" t="n">
         <v>47</v>
@@ -15135,10 +15135,10 @@
         </is>
       </c>
       <c r="I131" t="n">
-        <v>67.00001392915915</v>
+        <v>66.99999436535114</v>
       </c>
       <c r="J131" t="n">
-        <v>-176.0833194041741</v>
+        <v>-176.0833389679821</v>
       </c>
       <c r="K131" t="n">
         <v>68.39523475823404</v>
@@ -15220,10 +15220,10 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>90930277.77780448</v>
+        <v>90930063.13631396</v>
       </c>
       <c r="C132" t="n">
-        <v>-173660515.8562022</v>
+        <v>-173660181.4769069</v>
       </c>
       <c r="D132" t="n">
         <v>47</v>
@@ -15249,10 +15249,10 @@
         </is>
       </c>
       <c r="I132" t="n">
-        <v>68.11678675721816</v>
+        <v>68.11680337140869</v>
       </c>
       <c r="J132" t="n">
-        <v>-178.1498799094485</v>
+        <v>-178.149863295258</v>
       </c>
       <c r="K132" t="n">
         <v>67.96174536760311</v>
@@ -15334,10 +15334,10 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>89886613.54807913</v>
+        <v>89889286.84587127</v>
       </c>
       <c r="C133" t="n">
-        <v>-175570076.8970628</v>
+        <v>-175574363.7411091</v>
       </c>
       <c r="D133" t="n">
         <v>47</v>
@@ -15363,10 +15363,10 @@
         </is>
       </c>
       <c r="I133" t="n">
-        <v>68.43329371234678</v>
+        <v>68.43308910967613</v>
       </c>
       <c r="J133" t="n">
-        <v>-179.8167062876532</v>
+        <v>-179.8169108903238</v>
       </c>
       <c r="K133" t="n">
         <v>67.66347687400319</v>
@@ -15444,10 +15444,10 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>102207984.6576595</v>
+        <v>102209313.6826625</v>
       </c>
       <c r="C134" t="n">
-        <v>-187580015.7520474</v>
+        <v>-187581930.313654</v>
       </c>
       <c r="D134" t="n">
         <v>47</v>
@@ -15473,10 +15473,10 @@
         </is>
       </c>
       <c r="I134" t="n">
-        <v>67.06668641223058</v>
+        <v>67.06658817170199</v>
       </c>
       <c r="J134" t="n">
-        <v>-177.6333135877694</v>
+        <v>-177.633411828298</v>
       </c>
       <c r="K134" t="n">
         <v>67.53905861279729</v>
@@ -15562,10 +15562,10 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>105297903.1240131</v>
+        <v>105299421.9336895</v>
       </c>
       <c r="C135" t="n">
-        <v>-174152576.490499</v>
+        <v>-174154437.565182</v>
       </c>
       <c r="D135" t="n">
         <v>47</v>
@@ -15591,10 +15591,10 @@
         </is>
       </c>
       <c r="I135" t="n">
-        <v>65.63322982578258</v>
+        <v>65.63310983062003</v>
       </c>
       <c r="J135" t="n">
-        <v>-170.5501035075508</v>
+        <v>-170.5502235027134</v>
       </c>
       <c r="K135" t="n">
         <v>67.92585170340682</v>
@@ -15676,10 +15676,10 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>94630448.58195198</v>
+        <v>94630554.37158425</v>
       </c>
       <c r="C136" t="n">
-        <v>-179373449.67</v>
+        <v>-179373611.5363451</v>
       </c>
       <c r="D136" t="n">
         <v>47</v>
@@ -15705,10 +15705,10 @@
         </is>
       </c>
       <c r="I136" t="n">
-        <v>67.83336216811897</v>
+        <v>67.83335414819905</v>
       </c>
       <c r="J136" t="n">
-        <v>-178.4333044985477</v>
+        <v>-178.4333125184676</v>
       </c>
       <c r="K136" t="n">
         <v>67.46134663341647</v>
@@ -15790,10 +15790,10 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>103648394.1056142</v>
+        <v>103648004.1509348</v>
       </c>
       <c r="C137" t="n">
-        <v>-182663562.9066028</v>
+        <v>-182663034.0110876</v>
       </c>
       <c r="D137" t="n">
         <v>47</v>
@@ -15819,10 +15819,10 @@
         </is>
       </c>
       <c r="I137" t="n">
-        <v>66.49995848417912</v>
+        <v>66.49998802824688</v>
       </c>
       <c r="J137" t="n">
-        <v>-174.8000415158209</v>
+        <v>-174.8000119717532</v>
       </c>
       <c r="K137" t="n">
         <v>67.4074074074074</v>
@@ -15904,10 +15904,10 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>98266681.69730829</v>
+        <v>98265994.57547078</v>
       </c>
       <c r="C138" t="n">
-        <v>-180677399.1216154</v>
+        <v>-180676396.8603028</v>
       </c>
       <c r="D138" t="n">
         <v>47</v>
@@ -15933,10 +15933,10 @@
         </is>
       </c>
       <c r="I138" t="n">
-        <v>67.28339650198974</v>
+        <v>67.283448598292</v>
       </c>
       <c r="J138" t="n">
-        <v>-176.8166034980103</v>
+        <v>-176.816551401708</v>
       </c>
       <c r="K138" t="n">
         <v>67.05577172503243</v>
@@ -16014,10 +16014,10 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>119294187.3056267</v>
+        <v>119293100.639567</v>
       </c>
       <c r="C139" t="n">
-        <v>-214136283.2011814</v>
+        <v>-214134830.6730939</v>
       </c>
       <c r="D139" t="n">
         <v>47</v>
@@ -16043,10 +16043,10 @@
         </is>
       </c>
       <c r="I139" t="n">
-        <v>66.03337128277319</v>
+        <v>66.03344486504511</v>
       </c>
       <c r="J139" t="n">
-        <v>-179.9499620505601</v>
+        <v>-179.9498884682882</v>
       </c>
       <c r="K139" t="n">
         <v>66.98084829038403</v>
@@ -16128,10 +16128,10 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>108799312.6881271</v>
+        <v>108800112.9038873</v>
       </c>
       <c r="C140" t="n">
-        <v>-196582637.4172918</v>
+        <v>-196583746.7168819</v>
       </c>
       <c r="D140" t="n">
         <v>47</v>
@@ -16157,10 +16157,10 @@
         </is>
       </c>
       <c r="I140" t="n">
-        <v>66.56666883258055</v>
+        <v>66.56661141064704</v>
       </c>
       <c r="J140" t="n">
-        <v>-177.9833311674194</v>
+        <v>-177.9833885893529</v>
       </c>
       <c r="K140" t="n">
         <v>66.63673550833083</v>
@@ -16238,10 +16238,10 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>90651463.50287198</v>
+        <v>90651901.65778245</v>
       </c>
       <c r="C141" t="n">
-        <v>-173644848.279627</v>
+        <v>-173645533.7513208</v>
       </c>
       <c r="D141" t="n">
         <v>47</v>
@@ -16267,10 +16267,10 @@
         </is>
       </c>
       <c r="I141" t="n">
-        <v>68.1665367111958</v>
+        <v>68.16650281114532</v>
       </c>
       <c r="J141" t="n">
-        <v>-178.3334632888042</v>
+        <v>-178.3334971888547</v>
       </c>
       <c r="K141" t="n">
         <v>66.73001900570171</v>
@@ -16356,10 +16356,10 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>109559762.8263735</v>
+        <v>109559722.9289189</v>
       </c>
       <c r="C142" t="n">
-        <v>-185388356.1909328</v>
+        <v>-185388306.1858294</v>
       </c>
       <c r="D142" t="n">
         <v>47</v>
@@ -16385,10 +16385,10 @@
         </is>
       </c>
       <c r="I142" t="n">
-        <v>65.71667090057571</v>
+        <v>65.71667391103395</v>
       </c>
       <c r="J142" t="n">
-        <v>-173.2333290994243</v>
+        <v>-173.2333260889661</v>
       </c>
       <c r="K142" t="n">
         <v>66.67000100030009</v>
@@ -16466,10 +16466,10 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>103634673.1074151</v>
+        <v>103634729.2958177</v>
       </c>
       <c r="C143" t="n">
-        <v>-181891466.9635093</v>
+        <v>-181891542.7247275</v>
       </c>
       <c r="D143" t="n">
         <v>47</v>
@@ -16495,10 +16495,10 @@
         </is>
       </c>
       <c r="I143" t="n">
-        <v>66.45001519971581</v>
+        <v>66.45001092767487</v>
       </c>
       <c r="J143" t="n">
-        <v>-174.4833181336175</v>
+        <v>-174.4833224056584</v>
       </c>
       <c r="K143" t="n">
         <v>66.78722121760097</v>
@@ -16584,10 +16584,10 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>93414692.50158627</v>
+        <v>93414706.53621852</v>
       </c>
       <c r="C144" t="n">
-        <v>-163614314.8440734</v>
+        <v>-163614334.2863328</v>
       </c>
       <c r="D144" t="n">
         <v>47</v>
@@ -16613,10 +16613,10 @@
         </is>
       </c>
       <c r="I144" t="n">
-        <v>66.94998687113755</v>
+        <v>66.94998572393146</v>
       </c>
       <c r="J144" t="n">
-        <v>-171.7666797955291</v>
+        <v>-171.7666809427352</v>
       </c>
       <c r="K144" t="n">
         <v>66.4894150697301</v>
@@ -16698,10 +16698,10 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>119403173.9746964</v>
+        <v>119403884.9223573</v>
       </c>
       <c r="C145" t="n">
-        <v>-193069939.7414641</v>
+        <v>-193070738.2963331</v>
       </c>
       <c r="D145" t="n">
         <v>47</v>
@@ -16727,10 +16727,10 @@
         </is>
       </c>
       <c r="I145" t="n">
-        <v>64.71659064187352</v>
+        <v>64.71653814992759</v>
       </c>
       <c r="J145" t="n">
-        <v>-172.5000760247931</v>
+        <v>-172.500128516739</v>
       </c>
       <c r="K145" t="n">
         <v>65.58376649340263</v>
@@ -16808,10 +16808,10 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>91237591.3195311</v>
+        <v>91236690.37009616</v>
       </c>
       <c r="C146" t="n">
-        <v>-174741292.29525</v>
+        <v>-174739885.005937</v>
       </c>
       <c r="D146" t="n">
         <v>47</v>
@@ -16837,10 +16837,10 @@
         </is>
       </c>
       <c r="I146" t="n">
-        <v>68.13334226087335</v>
+        <v>68.1334116710327</v>
       </c>
       <c r="J146" t="n">
-        <v>-178.4666577391267</v>
+        <v>-178.4665883289674</v>
       </c>
       <c r="K146" t="n">
         <v>65.76413959085438</v>
@@ -16926,10 +16926,10 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>107559905.6503057</v>
+        <v>107560206.4702901</v>
       </c>
       <c r="C147" t="n">
-        <v>-196354673.0070667</v>
+        <v>-196355097.4582179</v>
       </c>
       <c r="D147" t="n">
         <v>47</v>
@@ -16955,10 +16955,10 @@
         </is>
       </c>
       <c r="I147" t="n">
-        <v>66.7500683016478</v>
+        <v>66.750046733818</v>
       </c>
       <c r="J147" t="n">
-        <v>-178.4999316983522</v>
+        <v>-178.499953266182</v>
       </c>
       <c r="K147" t="n">
         <v>65.23947027780544</v>
@@ -17036,10 +17036,10 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>125912277.5563406</v>
+        <v>125912398.5125425</v>
       </c>
       <c r="C148" t="n">
-        <v>-202194389.5591151</v>
+        <v>-202194520.6540882</v>
       </c>
       <c r="D148" t="n">
         <v>47</v>
@@ -17065,10 +17065,10 @@
         </is>
       </c>
       <c r="I148" t="n">
-        <v>64.36657390169819</v>
+        <v>64.36656524380487</v>
       </c>
       <c r="J148" t="n">
-        <v>-173.6167594316352</v>
+        <v>-173.6167680895285</v>
       </c>
       <c r="K148" t="n">
         <v>65.53417518540789</v>
@@ -17150,10 +17150,10 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>107665495.2339031</v>
+        <v>107664834.9478427</v>
       </c>
       <c r="C149" t="n">
-        <v>-194506578.9795287</v>
+        <v>-194505661.1581519</v>
       </c>
       <c r="D149" t="n">
         <v>47</v>
@@ -17179,10 +17179,10 @@
         </is>
       </c>
       <c r="I149" t="n">
-        <v>66.61661649160766</v>
+        <v>66.61666422094743</v>
       </c>
       <c r="J149" t="n">
-        <v>-177.700050175059</v>
+        <v>-177.7000024457192</v>
       </c>
       <c r="K149" t="n">
         <v>65.22738630684657</v>
@@ -17260,10 +17260,10 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>96673180.40597731</v>
+        <v>96672242.48385458</v>
       </c>
       <c r="C150" t="n">
-        <v>-182291982.2595517</v>
+        <v>-182290563.4259088</v>
       </c>
       <c r="D150" t="n">
         <v>47</v>
@@ -17289,10 +17289,10 @@
         </is>
       </c>
       <c r="I150" t="n">
-        <v>67.66685949910348</v>
+        <v>67.66692988486324</v>
       </c>
       <c r="J150" t="n">
-        <v>-178.4998071675632</v>
+        <v>-178.4997367818034</v>
       </c>
       <c r="K150" t="n">
         <v>65.2369526094781</v>
@@ -17370,10 +17370,10 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>105035929.1928367</v>
+        <v>105035861.4768484</v>
       </c>
       <c r="C151" t="n">
-        <v>-185858192.3171963</v>
+        <v>-185858100.2964173</v>
       </c>
       <c r="D151" t="n">
         <v>47</v>
@@ -17399,10 +17399,10 @@
         </is>
       </c>
       <c r="I151" t="n">
-        <v>66.48325698771632</v>
+        <v>66.48326205435347</v>
       </c>
       <c r="J151" t="n">
-        <v>-175.450076345617</v>
+        <v>-175.4500712789798</v>
       </c>
       <c r="K151" t="n">
         <v>65.14576677316293</v>
@@ -17484,10 +17484,10 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>129710198.4596708</v>
+        <v>129709496.8307995</v>
       </c>
       <c r="C152" t="n">
-        <v>-224508383.7818565</v>
+        <v>-224507523.2811059</v>
       </c>
       <c r="D152" t="n">
         <v>47</v>
@@ -17513,10 +17513,10 @@
         </is>
       </c>
       <c r="I152" t="n">
-        <v>65.16663848931606</v>
+        <v>65.16668471936212</v>
       </c>
       <c r="J152" t="n">
-        <v>-179.6333615106839</v>
+        <v>-179.6333152806378</v>
       </c>
       <c r="K152" t="n">
         <v>65.30161597912276</v>
@@ -17590,10 +17590,10 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>110114046.0511149</v>
+        <v>110112505.5368656</v>
       </c>
       <c r="C153" t="n">
-        <v>-198837048.2266916</v>
+        <v>-198834921.7274409</v>
       </c>
       <c r="D153" t="n">
         <v>47</v>
@@ -17619,10 +17619,10 @@
         </is>
       </c>
       <c r="I153" t="n">
-        <v>66.49995514339913</v>
+        <v>66.50006483458324</v>
       </c>
       <c r="J153" t="n">
-        <v>-178.2500448566009</v>
+        <v>-178.2499351654168</v>
       </c>
       <c r="K153" t="n">
         <v>65.25798032523589</v>
@@ -17704,10 +17704,10 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>95345677.07905038</v>
+        <v>95345408.76258494</v>
       </c>
       <c r="C154" t="n">
-        <v>-180780445.0931121</v>
+        <v>-180780035.102492</v>
       </c>
       <c r="D154" t="n">
         <v>47</v>
@@ -17733,10 +17733,10 @@
         </is>
       </c>
       <c r="I154" t="n">
-        <v>67.7998927347974</v>
+        <v>67.79991296665177</v>
       </c>
       <c r="J154" t="n">
-        <v>-178.6334405985359</v>
+        <v>-178.6334203666815</v>
       </c>
       <c r="K154" t="n">
         <v>64.6935516071072</v>
@@ -17814,10 +17814,10 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>119325984.7731324</v>
+        <v>119327644.5647107</v>
       </c>
       <c r="C155" t="n">
-        <v>-200735864.3579961</v>
+        <v>-200737863.3305627</v>
       </c>
       <c r="D155" t="n">
         <v>47</v>
@@ -17843,10 +17843,10 @@
         </is>
       </c>
       <c r="I155" t="n">
-        <v>65.21671717554545</v>
+        <v>65.21659850793179</v>
       </c>
       <c r="J155" t="n">
-        <v>-175.1832828244545</v>
+        <v>-175.1834014920682</v>
       </c>
       <c r="K155" t="n">
         <v>64.60079840319362</v>
@@ -17928,10 +17928,10 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>93428580.87039356</v>
+        <v>93428592.75277303</v>
       </c>
       <c r="C156" t="n">
-        <v>-177405798.8254772</v>
+        <v>-177405817.098093</v>
       </c>
       <c r="D156" t="n">
         <v>47</v>
@@ -17957,10 +17957,10 @@
         </is>
       </c>
       <c r="I156" t="n">
-        <v>67.91659312823128</v>
+        <v>67.91659222088568</v>
       </c>
       <c r="J156" t="n">
-        <v>-178.2834068717687</v>
+        <v>-178.2834077791143</v>
       </c>
       <c r="K156" t="n">
         <v>64.42518429966128</v>
@@ -18038,10 +18038,10 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>114373753.1311606</v>
+        <v>114371692.2541738</v>
       </c>
       <c r="C157" t="n">
-        <v>-190705215.0722503</v>
+        <v>-190702731.3950348</v>
       </c>
       <c r="D157" t="n">
         <v>47</v>
@@ -18067,10 +18067,10 @@
         </is>
       </c>
       <c r="I157" t="n">
-        <v>65.31665241504226</v>
+        <v>65.31680524605893</v>
       </c>
       <c r="J157" t="n">
-        <v>-173.3666809182911</v>
+        <v>-173.3665280872744</v>
       </c>
       <c r="K157" t="n">
         <v>64.75541299117882</v>
@@ -18148,10 +18148,10 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>104586924.6323144</v>
+        <v>104586949.9232588</v>
       </c>
       <c r="C158" t="n">
-        <v>-174359046.694427</v>
+        <v>-174359078.1543424</v>
       </c>
       <c r="D158" t="n">
         <v>47</v>
@@ -18177,10 +18177,10 @@
         </is>
       </c>
       <c r="I158" t="n">
-        <v>65.76664134229371</v>
+        <v>65.76663934798087</v>
       </c>
       <c r="J158" t="n">
-        <v>-170.9333586577063</v>
+        <v>-170.9333606520191</v>
       </c>
       <c r="K158" t="n">
         <v>64.6216973578863</v>
@@ -18262,10 +18262,10 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>91749763.98484507</v>
+        <v>91749754.6950718</v>
       </c>
       <c r="C159" t="n">
-        <v>-175631218.9138206</v>
+        <v>-175631204.4296953</v>
       </c>
       <c r="D159" t="n">
         <v>47</v>
@@ -18291,10 +18291,10 @@
         </is>
       </c>
       <c r="I159" t="n">
-        <v>68.09999197765791</v>
+        <v>68.09999269093889</v>
       </c>
       <c r="J159" t="n">
-        <v>-178.5500080223421</v>
+        <v>-178.5500073090611</v>
       </c>
       <c r="K159" t="n">
         <v>64.23774681768066</v>
@@ -18376,10 +18376,10 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>125836086.652237</v>
+        <v>125835557.693632</v>
       </c>
       <c r="C160" t="n">
-        <v>-202024684.8876894</v>
+        <v>-202024111.6928512</v>
       </c>
       <c r="D160" t="n">
         <v>47</v>
@@ -18405,10 +18405,10 @@
         </is>
       </c>
       <c r="I160" t="n">
-        <v>64.36662366929453</v>
+        <v>64.36666155464526</v>
       </c>
       <c r="J160" t="n">
-        <v>-173.5833763307054</v>
+        <v>-173.5833384453547</v>
       </c>
       <c r="K160" t="n">
         <v>64.43661971830984</v>
@@ -18490,10 +18490,10 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>116302363.5055453</v>
+        <v>116300547.405243</v>
       </c>
       <c r="C161" t="n">
-        <v>-190096358.4436287</v>
+        <v>-190094256.5324488</v>
       </c>
       <c r="D161" t="n">
         <v>47</v>
@@ -18519,10 +18519,10 @@
         </is>
       </c>
       <c r="I161" t="n">
-        <v>64.98335676951956</v>
+        <v>64.9834921099181</v>
       </c>
       <c r="J161" t="n">
-        <v>-172.4666432304805</v>
+        <v>-172.466507890082</v>
       </c>
       <c r="K161" t="n">
         <v>64.06453552460167</v>
@@ -18604,10 +18604,10 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>107310720.9184249</v>
+        <v>107311224.3497591</v>
       </c>
       <c r="C162" t="n">
-        <v>-195718577.6450581</v>
+        <v>-195719287.5035029</v>
       </c>
       <c r="D162" t="n">
         <v>47</v>
@@ -18633,10 +18633,10 @@
         </is>
       </c>
       <c r="I162" t="n">
-        <v>66.7500911044866</v>
+        <v>66.75005492402578</v>
       </c>
       <c r="J162" t="n">
-        <v>-178.3665755621801</v>
+        <v>-178.3666117426409</v>
       </c>
       <c r="K162" t="n">
         <v>63.88194097048524</v>
@@ -18718,10 +18718,10 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>114563223.8634599</v>
+        <v>114562592.945937</v>
       </c>
       <c r="C163" t="n">
-        <v>-192168517.7273502</v>
+        <v>-192167750.2243736</v>
       </c>
       <c r="D163" t="n">
         <v>47</v>
@@ -18747,10 +18747,10 @@
         </is>
       </c>
       <c r="I163" t="n">
-        <v>65.3833839032541</v>
+        <v>65.38343040663055</v>
       </c>
       <c r="J163" t="n">
-        <v>-173.8332827634125</v>
+        <v>-173.8332362600361</v>
       </c>
       <c r="K163" t="n">
         <v>63.91670004004805</v>
@@ -18828,10 +18828,10 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>95010238.99019727</v>
+        <v>95010133.05762434</v>
       </c>
       <c r="C164" t="n">
-        <v>-180392876.9759969</v>
+        <v>-180392714.7041181</v>
       </c>
       <c r="D164" t="n">
         <v>47</v>
@@ -18857,10 +18857,10 @@
         </is>
       </c>
       <c r="I164" t="n">
-        <v>67.83343937331193</v>
+        <v>67.83344737080554</v>
       </c>
       <c r="J164" t="n">
-        <v>-178.6665606266881</v>
+        <v>-178.6665526291945</v>
       </c>
       <c r="K164" t="n">
         <v>64.24114331723028</v>
@@ -18938,10 +18938,10 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>116834089.474993</v>
+        <v>116833037.3592419</v>
       </c>
       <c r="C165" t="n">
-        <v>-190551582.2354816</v>
+        <v>-190550371.3754974</v>
       </c>
       <c r="D165" t="n">
         <v>47</v>
@@ -18967,10 +18967,10 @@
         </is>
       </c>
       <c r="I165" t="n">
-        <v>64.93333182453715</v>
+        <v>64.93341012424806</v>
       </c>
       <c r="J165" t="n">
-        <v>-172.4500015087962</v>
+        <v>-172.4499232090853</v>
       </c>
       <c r="K165" t="n">
         <v>63.33931061964534</v>
@@ -19052,10 +19052,10 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>123867543.5620008</v>
+        <v>123867952.8791168</v>
       </c>
       <c r="C166" t="n">
-        <v>-203490825.668832</v>
+        <v>-203491291.7640728</v>
       </c>
       <c r="D166" t="n">
         <v>47</v>
@@ -19081,10 +19081,10 @@
         </is>
       </c>
       <c r="I166" t="n">
-        <v>64.73336601050909</v>
+        <v>64.73333692660938</v>
       </c>
       <c r="J166" t="n">
-        <v>-174.6333006561576</v>
+        <v>-174.6333297400573</v>
       </c>
       <c r="K166" t="n">
         <v>62.97952693301529</v>
@@ -19162,10 +19162,10 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>94930724.12062098</v>
+        <v>94930873.93600039</v>
       </c>
       <c r="C167" t="n">
-        <v>-180177071.7016331</v>
+        <v>-180177301.1360669</v>
       </c>
       <c r="D167" t="n">
         <v>47</v>
@@ -19191,10 +19191,10 @@
         </is>
       </c>
       <c r="I167" t="n">
-        <v>67.83327419627541</v>
+        <v>67.83326287586983</v>
       </c>
       <c r="J167" t="n">
-        <v>-178.6167258037246</v>
+        <v>-178.6167371241302</v>
       </c>
       <c r="K167" t="n">
         <v>63.20199501246881</v>
@@ -19276,10 +19276,10 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>109023935.8231804</v>
+        <v>109024145.1125965</v>
       </c>
       <c r="C168" t="n">
-        <v>-190379709.2240946</v>
+        <v>-190379985.0380221</v>
       </c>
       <c r="D168" t="n">
         <v>47</v>
@@ -19305,10 +19305,10 @@
         </is>
       </c>
       <c r="I168" t="n">
-        <v>66.13328115770848</v>
+        <v>66.13326572304113</v>
       </c>
       <c r="J168" t="n">
-        <v>-175.4167188422916</v>
+        <v>-175.4167342769589</v>
       </c>
       <c r="K168" t="n">
         <v>62.96036126442549</v>
@@ -19382,10 +19382,10 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>122611482.311808</v>
+        <v>122610651.9789469</v>
       </c>
       <c r="C169" t="n">
-        <v>-195357198.7251206</v>
+        <v>-195356301.638187</v>
       </c>
       <c r="D169" t="n">
         <v>47</v>
@@ -19411,10 +19411,10 @@
         </is>
       </c>
       <c r="I169" t="n">
-        <v>64.40003391967613</v>
+        <v>64.40009484321996</v>
       </c>
       <c r="J169" t="n">
-        <v>-172.3166327469906</v>
+        <v>-172.3165718234468</v>
       </c>
       <c r="K169" t="n">
         <v>61.63147982951729</v>
@@ -19496,10 +19496,10 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>112012002.4043519</v>
+        <v>112012066.3744351</v>
       </c>
       <c r="C170" t="n">
-        <v>-187947364.5359129</v>
+        <v>-187947443.025041</v>
       </c>
       <c r="D170" t="n">
         <v>47</v>
@@ -19525,10 +19525,10 @@
         </is>
       </c>
       <c r="I170" t="n">
-        <v>65.50014057935047</v>
+        <v>65.50013579195277</v>
       </c>
       <c r="J170" t="n">
-        <v>-173.2331927539828</v>
+        <v>-173.2331975413805</v>
       </c>
       <c r="K170" t="n">
         <v>61.96491228070173</v>
@@ -19606,10 +19606,10 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>115464219.5656805</v>
+        <v>115464965.0687606</v>
       </c>
       <c r="C171" t="n">
-        <v>-189436241.734163</v>
+        <v>-189437112.6759949</v>
       </c>
       <c r="D171" t="n">
         <v>47</v>
@@ -19635,10 +19635,10 @@
         </is>
       </c>
       <c r="I171" t="n">
-        <v>65.0666289865151</v>
+        <v>65.0665733247407</v>
       </c>
       <c r="J171" t="n">
-        <v>-172.5167043468183</v>
+        <v>-172.5167600085927</v>
       </c>
       <c r="K171" t="n">
         <v>61.35640413683373</v>
@@ -19716,10 +19716,10 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>123165732.0728984</v>
+        <v>123165218.7500279</v>
       </c>
       <c r="C172" t="n">
-        <v>-204036426.8111035</v>
+        <v>-204035832.0819772</v>
       </c>
       <c r="D172" t="n">
         <v>47</v>
@@ -19745,10 +19745,10 @@
         </is>
       </c>
       <c r="I172" t="n">
-        <v>64.86662275926916</v>
+        <v>64.86665912518826</v>
       </c>
       <c r="J172" t="n">
-        <v>-175.0333772407308</v>
+        <v>-175.0333408748117</v>
       </c>
       <c r="K172" t="n">
         <v>60.88697567324057</v>
@@ -19830,10 +19830,10 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>126036634.0646268</v>
+        <v>126035442.3380523</v>
       </c>
       <c r="C173" t="n">
-        <v>-201936231.7772607</v>
+        <v>-201934946.3262615</v>
       </c>
       <c r="D173" t="n">
         <v>47</v>
@@ -19859,10 +19859,10 @@
         </is>
       </c>
       <c r="I173" t="n">
-        <v>64.33330987357901</v>
+        <v>64.33339527556001</v>
       </c>
       <c r="J173" t="n">
-        <v>-173.5000234597543</v>
+        <v>-173.4999380577733</v>
       </c>
       <c r="K173" t="n">
         <v>59.95813397129186</v>
@@ -19944,10 +19944,10 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>103962297.5280395</v>
+        <v>103963286.9951731</v>
       </c>
       <c r="C174" t="n">
-        <v>-184188421.1273362</v>
+        <v>-184189772.1687449</v>
       </c>
       <c r="D174" t="n">
         <v>47</v>
@@ -19973,10 +19973,10 @@
         </is>
       </c>
       <c r="I174" t="n">
-        <v>66.55001094406209</v>
+        <v>66.54993646591743</v>
       </c>
       <c r="J174" t="n">
-        <v>-175.2833223892712</v>
+        <v>-175.2833968674159</v>
       </c>
       <c r="K174" t="n">
         <v>58.0490724117295</v>
@@ -20058,10 +20058,10 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>123167497.8179095</v>
+        <v>123167917.7093716</v>
       </c>
       <c r="C175" t="n">
-        <v>-196595138.8558727</v>
+        <v>-196595593.1394584</v>
       </c>
       <c r="D175" t="n">
         <v>47</v>
@@ -20087,10 +20087,10 @@
         </is>
       </c>
       <c r="I175" t="n">
-        <v>64.39998428865744</v>
+        <v>64.39995362112884</v>
       </c>
       <c r="J175" t="n">
-        <v>-172.5666823780093</v>
+        <v>-172.5667130455379</v>
       </c>
       <c r="K175" t="n">
         <v>57.96623713914693</v>
@@ -20168,10 +20168,10 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>125007944.8906292</v>
+        <v>125009597.6335431</v>
       </c>
       <c r="C176" t="n">
-        <v>-206926604.33199</v>
+        <v>-206928505.2360481</v>
       </c>
       <c r="D176" t="n">
         <v>47</v>
@@ -20197,10 +20197,10 @@
         </is>
       </c>
       <c r="I176" t="n">
-        <v>64.78352735916813</v>
+        <v>64.78341139456178</v>
       </c>
       <c r="J176" t="n">
-        <v>-175.4164726408319</v>
+        <v>-175.4165886054382</v>
       </c>
       <c r="K176" t="n">
         <v>56.76590660161306</v>
@@ -20274,10 +20274,10 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>104730402.1973267</v>
+        <v>104729571.0001448</v>
       </c>
       <c r="C177" t="n">
-        <v>-183606540.2147338</v>
+        <v>-183605424.8142278</v>
       </c>
       <c r="D177" t="n">
         <v>47</v>
@@ -20303,10 +20303,10 @@
         </is>
       </c>
       <c r="I177" t="n">
-        <v>66.38326247672906</v>
+        <v>66.38332527969118</v>
       </c>
       <c r="J177" t="n">
-        <v>-174.666737523271</v>
+        <v>-174.6666747203089</v>
       </c>
       <c r="K177" t="n">
         <v>55.99558853017847</v>
@@ -20384,10 +20384,10 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>108429037.3583531</v>
+        <v>108428450.8804912</v>
       </c>
       <c r="C178" t="n">
-        <v>-197506227.4677483</v>
+        <v>-197505404.3038669</v>
       </c>
       <c r="D178" t="n">
         <v>47</v>
@@ -20413,10 +20413,10 @@
         </is>
       </c>
       <c r="I178" t="n">
-        <v>66.68339334081354</v>
+        <v>66.68343523550654</v>
       </c>
       <c r="J178" t="n">
-        <v>-178.5332733258531</v>
+        <v>-178.5332314311601</v>
       </c>
       <c r="K178" t="n">
         <v>53.94579513750498</v>
@@ -20498,10 +20498,10 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>107512582.6285103</v>
+        <v>107513991.4400155</v>
       </c>
       <c r="C179" t="n">
-        <v>-195967449.1250856</v>
+        <v>-195969432.9036126</v>
       </c>
       <c r="D179" t="n">
         <v>47</v>
@@ -20527,10 +20527,10 @@
         </is>
       </c>
       <c r="I179" t="n">
-        <v>66.73335430959045</v>
+        <v>66.73325314025344</v>
       </c>
       <c r="J179" t="n">
-        <v>-178.3666456904096</v>
+        <v>-178.3667468597466</v>
       </c>
       <c r="K179" t="n">
         <v>53.40088282504012</v>
@@ -20612,10 +20612,10 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>119548694.4906461</v>
+        <v>119549321.5548093</v>
       </c>
       <c r="C180" t="n">
-        <v>-208863939.1255731</v>
+        <v>-208864742.2065115</v>
       </c>
       <c r="D180" t="n">
         <v>47</v>
@@ -20641,10 +20641,10 @@
         </is>
       </c>
       <c r="I180" t="n">
-        <v>65.68320561056693</v>
+        <v>65.68316223055288</v>
       </c>
       <c r="J180" t="n">
-        <v>-177.9667943894331</v>
+        <v>-177.9668377694471</v>
       </c>
       <c r="K180" t="n">
         <v>52.50074872716382</v>

</xml_diff>

<commit_message>
optimizing variogram parameters for area 2
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,13 +528,13 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>95282423.42394386</v>
+        <v>141348099.896921</v>
       </c>
       <c r="C2" t="n">
-        <v>-181124017.8387472</v>
+        <v>-312922610.203993</v>
       </c>
       <c r="D2" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -642,13 +642,13 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>119552764.2797502</v>
+        <v>178703408.6955554</v>
       </c>
       <c r="C3" t="n">
-        <v>-209150282.5585824</v>
+        <v>-362295201.6112791</v>
       </c>
       <c r="D3" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -756,13 +756,13 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>104941148.9373436</v>
+        <v>157319701.6040834</v>
       </c>
       <c r="C4" t="n">
-        <v>-184375367.8509409</v>
+        <v>-322206528.3678634</v>
       </c>
       <c r="D4" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -874,13 +874,13 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>95828445.73439915</v>
+        <v>142056384.3197211</v>
       </c>
       <c r="C5" t="n">
-        <v>-182846056.6980341</v>
+        <v>-315497640.8960232</v>
       </c>
       <c r="D5" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -988,13 +988,13 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>95741241.542317</v>
+        <v>141904992.4841089</v>
       </c>
       <c r="C6" t="n">
-        <v>-182870042.0223253</v>
+        <v>-315481395.9970667</v>
       </c>
       <c r="D6" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1102,13 +1102,13 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>110429225.6288865</v>
+        <v>164413949.5216025</v>
       </c>
       <c r="C7" t="n">
-        <v>-201251187.019623</v>
+        <v>-347491935.8960524</v>
       </c>
       <c r="D7" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1212,13 +1212,13 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>95831264.53457274</v>
+        <v>142093030.5559932</v>
       </c>
       <c r="C8" t="n">
-        <v>-182597156.5451731</v>
+        <v>-315170365.2597262</v>
       </c>
       <c r="D8" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1326,13 +1326,13 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>105424615.0091471</v>
+        <v>157915916.6761881</v>
       </c>
       <c r="C9" t="n">
-        <v>-186071770.9097808</v>
+        <v>-324720174.3036515</v>
       </c>
       <c r="D9" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1444,13 +1444,13 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>93838358.02530071</v>
+        <v>138963431.6057103</v>
       </c>
       <c r="C10" t="n">
-        <v>-180545611.33535</v>
+        <v>-311358900.6426019</v>
       </c>
       <c r="D10" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1562,13 +1562,13 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>105480970.7099347</v>
+        <v>158155895.589951</v>
       </c>
       <c r="C11" t="n">
-        <v>-184960723.030066</v>
+        <v>-323250782.3943694</v>
       </c>
       <c r="D11" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1676,13 +1676,13 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>124229411.8829788</v>
+        <v>186807109.2753962</v>
       </c>
       <c r="C12" t="n">
-        <v>-206495427.4714684</v>
+        <v>-360587711.855448</v>
       </c>
       <c r="D12" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1786,13 +1786,13 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>114776304.1833821</v>
+        <v>171799814.8913856</v>
       </c>
       <c r="C13" t="n">
-        <v>-200512974.5587198</v>
+        <v>-348508131.1287501</v>
       </c>
       <c r="D13" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1892,13 +1892,13 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>92751328.5513556</v>
+        <v>137522281.9252852</v>
       </c>
       <c r="C14" t="n">
-        <v>-177342189.8416194</v>
+        <v>-306526338.6425698</v>
       </c>
       <c r="D14" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2006,13 +2006,13 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>98397391.14028972</v>
+        <v>148379064.2916293</v>
       </c>
       <c r="C15" t="n">
-        <v>-168144371.6522151</v>
+        <v>-297192877.2481689</v>
       </c>
       <c r="D15" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2116,13 +2116,13 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>124689994.5163658</v>
+        <v>187641498.9218537</v>
       </c>
       <c r="C16" t="n">
-        <v>-205920335.8366216</v>
+        <v>-359974207.1259955</v>
       </c>
       <c r="D16" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2230,13 +2230,13 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>117110889.8931256</v>
+        <v>175465203.9267208</v>
       </c>
       <c r="C17" t="n">
-        <v>-202419800.2301919</v>
+        <v>-352113034.5898279</v>
       </c>
       <c r="D17" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2340,13 +2340,13 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>121345514.7420146</v>
+        <v>181427741.6017235</v>
       </c>
       <c r="C18" t="n">
-        <v>-211274706.1783964</v>
+        <v>-365943608.0528963</v>
       </c>
       <c r="D18" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2454,13 +2454,13 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>125518658.9725189</v>
+        <v>189349594.7699511</v>
       </c>
       <c r="C19" t="n">
-        <v>-203197682.7713831</v>
+        <v>-356528717.3753525</v>
       </c>
       <c r="D19" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2560,13 +2560,13 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>95364025.13515216</v>
+        <v>141458787.0723889</v>
       </c>
       <c r="C20" t="n">
-        <v>-181343537.004773</v>
+        <v>-313257500.772146</v>
       </c>
       <c r="D20" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2674,13 +2674,13 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>127327723.273805</v>
+        <v>191972331.1404673</v>
       </c>
       <c r="C21" t="n">
-        <v>-206190135.3970429</v>
+        <v>-361328626.4466391</v>
       </c>
       <c r="D21" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2784,13 +2784,13 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>121267982.8839387</v>
+        <v>182904035.3541456</v>
       </c>
       <c r="C22" t="n">
-        <v>-198348593.0277166</v>
+        <v>-348238819.2016164</v>
       </c>
       <c r="D22" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -2890,13 +2890,13 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>95380300.6148705</v>
+        <v>141382299.2509747</v>
       </c>
       <c r="C23" t="n">
-        <v>-182155954.7913481</v>
+        <v>-314339671.5201009</v>
       </c>
       <c r="D23" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -2996,13 +2996,13 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>95605805.78367405</v>
+        <v>141721499.0632483</v>
       </c>
       <c r="C24" t="n">
-        <v>-182503398.1001907</v>
+        <v>-314922671.6170502</v>
       </c>
       <c r="D24" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3110,13 +3110,13 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>121303364.1280309</v>
+        <v>182286786.5278214</v>
       </c>
       <c r="C25" t="n">
-        <v>-203759480.5622177</v>
+        <v>-355682675.3674026</v>
       </c>
       <c r="D25" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -3224,13 +3224,13 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>112735035.5398172</v>
+        <v>169006163.3432604</v>
       </c>
       <c r="C26" t="n">
-        <v>-195552640.0126746</v>
+        <v>-340885700.9276638</v>
       </c>
       <c r="D26" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -3334,13 +3334,13 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>95250007.58868599</v>
+        <v>141238730.7640204</v>
       </c>
       <c r="C27" t="n">
-        <v>-181546039.8281603</v>
+        <v>-313462381.3896099</v>
       </c>
       <c r="D27" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -3448,13 +3448,13 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>114518586.2557847</v>
+        <v>172961831.9667335</v>
       </c>
       <c r="C28" t="n">
-        <v>-188017544.4496489</v>
+        <v>-331368761.8243606</v>
       </c>
       <c r="D28" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -3562,13 +3562,13 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>99552257.76107493</v>
+        <v>149682088.5391768</v>
       </c>
       <c r="C29" t="n">
-        <v>-173040454.961911</v>
+        <v>-304353800.1510978</v>
       </c>
       <c r="D29" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -3672,13 +3672,13 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>122387987.0239019</v>
+        <v>184511210.0317812</v>
       </c>
       <c r="C30" t="n">
-        <v>-200373654.1043369</v>
+        <v>-351457881.0413339</v>
       </c>
       <c r="D30" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -3778,13 +3778,13 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>121305548.1740049</v>
+        <v>182290094.6041036</v>
       </c>
       <c r="C31" t="n">
-        <v>-203762088.3106418</v>
+        <v>-355687121.3447877</v>
       </c>
       <c r="D31" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -3892,13 +3892,13 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>95247441.91766733</v>
+        <v>141202604.9046527</v>
       </c>
       <c r="C32" t="n">
-        <v>-181793757.3492677</v>
+        <v>-313788147.2910262</v>
       </c>
       <c r="D32" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -4006,13 +4006,13 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>120389586.4569375</v>
+        <v>179846307.3456305</v>
       </c>
       <c r="C33" t="n">
-        <v>-211192737.5384258</v>
+        <v>-365423631.8033922</v>
       </c>
       <c r="D33" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -4116,13 +4116,13 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>95492687.50073972</v>
+        <v>141535203.7030983</v>
       </c>
       <c r="C34" t="n">
-        <v>-182455355.850242</v>
+        <v>-314796955.9100499</v>
       </c>
       <c r="D34" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -4230,13 +4230,13 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>125025500.7311581</v>
+        <v>188638009.6649984</v>
       </c>
       <c r="C35" t="n">
-        <v>-202351422.2608036</v>
+        <v>-355177105.0007602</v>
       </c>
       <c r="D35" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -4340,13 +4340,13 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>124325830.1572926</v>
+        <v>187073764.5966155</v>
       </c>
       <c r="C36" t="n">
-        <v>-205629841.009484</v>
+        <v>-359435188.227848</v>
       </c>
       <c r="D36" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -4458,13 +4458,13 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>100517604.8722086</v>
+        <v>151100699.8415523</v>
       </c>
       <c r="C37" t="n">
-        <v>-174700136.2946388</v>
+        <v>-307056524.2853937</v>
       </c>
       <c r="D37" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -4568,13 +4568,13 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>101868946.7203449</v>
+        <v>153302545.1236823</v>
       </c>
       <c r="C38" t="n">
-        <v>-175394844.7938784</v>
+        <v>-308638682.613012</v>
       </c>
       <c r="D38" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -4682,13 +4682,13 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>92874531.14906563</v>
+        <v>137427790.8201395</v>
       </c>
       <c r="C39" t="n">
-        <v>-179713668.4056195</v>
+        <v>-309720944.1721357</v>
       </c>
       <c r="D39" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -4800,13 +4800,13 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>94840572.3892775</v>
+        <v>140683036.6809032</v>
       </c>
       <c r="C40" t="n">
-        <v>-180445887.8844967</v>
+        <v>-311783616.8171786</v>
       </c>
       <c r="D40" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -4918,13 +4918,13 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>121229719.0507312</v>
+        <v>182185480.8546159</v>
       </c>
       <c r="C41" t="n">
-        <v>-203589248.6053825</v>
+        <v>-355420101.1418816</v>
       </c>
       <c r="D41" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -5032,13 +5032,13 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>94348291.96360223</v>
+        <v>139785958.6206442</v>
       </c>
       <c r="C42" t="n">
-        <v>-180904050.2130439</v>
+        <v>-312116013.6802651</v>
       </c>
       <c r="D42" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -5150,13 +5150,13 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>93970184.60001004</v>
+        <v>139436924.7472599</v>
       </c>
       <c r="C43" t="n">
-        <v>-178609577.4670362</v>
+        <v>-308877426.2758054</v>
       </c>
       <c r="D43" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -5264,13 +5264,13 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>104810660.9949679</v>
+        <v>157108380.5028565</v>
       </c>
       <c r="C44" t="n">
-        <v>-184303776.0140289</v>
+        <v>-322048073.0520066</v>
       </c>
       <c r="D44" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -5382,13 +5382,13 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>90476856.36681883</v>
+        <v>134113871.8673896</v>
       </c>
       <c r="C45" t="n">
-        <v>-173670409.0955782</v>
+        <v>-300402910.3628743</v>
       </c>
       <c r="D45" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -5500,13 +5500,13 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>95910579.3488552</v>
+        <v>142167772.0194329</v>
       </c>
       <c r="C46" t="n">
-        <v>-183067430.3302456</v>
+        <v>-315835162.0295094</v>
       </c>
       <c r="D46" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -5610,13 +5610,13 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>94300459.77152336</v>
+        <v>139622332.8264687</v>
       </c>
       <c r="C47" t="n">
-        <v>-181546911.7999673</v>
+        <v>-312937151.0000179</v>
       </c>
       <c r="D47" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -5728,13 +5728,13 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>94297707.20916051</v>
+        <v>139914049.4457763</v>
       </c>
       <c r="C48" t="n">
-        <v>-179237255.3816975</v>
+        <v>-309887552.3178197</v>
       </c>
       <c r="D48" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -5842,13 +5842,13 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>123510846.9439162</v>
+        <v>185854151.742791</v>
       </c>
       <c r="C49" t="n">
-        <v>-204562335.5173564</v>
+        <v>-357653567.1813228</v>
       </c>
       <c r="D49" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -5956,13 +5956,13 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>95725352.49476045</v>
+        <v>142014766.7871837</v>
       </c>
       <c r="C50" t="n">
-        <v>-181802339.0369653</v>
+        <v>-314061916.8233049</v>
       </c>
       <c r="D50" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -6066,13 +6066,13 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>105275316.8308108</v>
+        <v>159120642.1015579</v>
       </c>
       <c r="C51" t="n">
-        <v>-175037791.7453042</v>
+        <v>-309707474.7853568</v>
       </c>
       <c r="D51" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -6180,13 +6180,13 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>111385953.0881969</v>
+        <v>165886800.0556829</v>
       </c>
       <c r="C52" t="n">
-        <v>-202325760.512677</v>
+        <v>-349389803.8062887</v>
       </c>
       <c r="D52" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -6290,13 +6290,13 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>117762322.5122562</v>
+        <v>176051257.9623712</v>
       </c>
       <c r="C53" t="n">
-        <v>-206444865.1610297</v>
+        <v>-357852654.1054109</v>
       </c>
       <c r="D53" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -6404,13 +6404,13 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>90649208.32910211</v>
+        <v>134412228.8925521</v>
       </c>
       <c r="C54" t="n">
-        <v>-173641320.1490476</v>
+        <v>-300462479.4236699</v>
       </c>
       <c r="D54" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -6522,13 +6522,13 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>95144377.64945558</v>
+        <v>141128205.7539958</v>
       </c>
       <c r="C55" t="n">
-        <v>-181006532.7089282</v>
+        <v>-312691525.8584673</v>
       </c>
       <c r="D55" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -6636,13 +6636,13 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>116766921.1118291</v>
+        <v>174994308.3881196</v>
       </c>
       <c r="C56" t="n">
-        <v>-201591453.3137347</v>
+        <v>-350840163.793776</v>
       </c>
       <c r="D56" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -6746,13 +6746,13 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>90078456.88577609</v>
+        <v>133152710.8121899</v>
       </c>
       <c r="C57" t="n">
-        <v>-175847701.1475296</v>
+        <v>-303038671.2823944</v>
       </c>
       <c r="D57" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -6856,13 +6856,13 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>112420323.0307304</v>
+        <v>167500273.6470561</v>
       </c>
       <c r="C58" t="n">
-        <v>-203308439.8632879</v>
+        <v>-351198028.2771947</v>
       </c>
       <c r="D58" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -6966,13 +6966,13 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>101355383.3196585</v>
+        <v>152566433.763808</v>
       </c>
       <c r="C59" t="n">
-        <v>-174382160.4228776</v>
+        <v>-307027879.2079807</v>
       </c>
       <c r="D59" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -7080,13 +7080,13 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>108991586.5147202</v>
+        <v>162353705.6233473</v>
       </c>
       <c r="C60" t="n">
-        <v>-198402990.7056906</v>
+        <v>-342984243.4647176</v>
       </c>
       <c r="D60" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -7190,13 +7190,13 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>122728333.8382406</v>
+        <v>182900000.1607319</v>
       </c>
       <c r="C61" t="n">
-        <v>-218062204.4267837</v>
+        <v>-375730773.3307462</v>
       </c>
       <c r="D61" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -7300,13 +7300,13 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>123509537.614461</v>
+        <v>185852166.9742152</v>
       </c>
       <c r="C62" t="n">
-        <v>-204560820.8228306</v>
+        <v>-357650979.020691</v>
       </c>
       <c r="D62" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -7414,13 +7414,13 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>100299148.9200183</v>
+        <v>151272705.8182151</v>
       </c>
       <c r="C63" t="n">
-        <v>-170667493.1168369</v>
+        <v>-301506965.1118869</v>
       </c>
       <c r="D63" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -7528,13 +7528,13 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>110374195.7526035</v>
+        <v>164372378.2907965</v>
       </c>
       <c r="C64" t="n">
-        <v>-200844579.8181961</v>
+        <v>-346920916.0419698</v>
       </c>
       <c r="D64" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -7646,13 +7646,13 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>102482765.1258514</v>
+        <v>152153190.0924732</v>
       </c>
       <c r="C65" t="n">
-        <v>-192206181.790361</v>
+        <v>-331452261.5825568</v>
       </c>
       <c r="D65" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -7760,13 +7760,13 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>105781919.9968431</v>
+        <v>160006688.2880322</v>
       </c>
       <c r="C66" t="n">
-        <v>-174815274.6477909</v>
+        <v>-309625249.6685805</v>
       </c>
       <c r="D66" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -7874,13 +7874,13 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>111386948.7224587</v>
+        <v>165888299.3243921</v>
       </c>
       <c r="C67" t="n">
-        <v>-202327142.1118898</v>
+        <v>-349392130.2866428</v>
       </c>
       <c r="D67" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -7988,13 +7988,13 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>99476173.42223467</v>
+        <v>149672339.1384026</v>
       </c>
       <c r="C68" t="n">
-        <v>-172151525.9484709</v>
+        <v>-303119257.454601</v>
       </c>
       <c r="D68" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -8102,13 +8102,13 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>98869799.25116791</v>
+        <v>149554551.1177341</v>
       </c>
       <c r="C69" t="n">
-        <v>-165438048.4331167</v>
+        <v>-293750538.5389981</v>
       </c>
       <c r="D69" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -8216,13 +8216,13 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>104221392.1295946</v>
+        <v>156976021.7356825</v>
       </c>
       <c r="C70" t="n">
-        <v>-177746059.5469749</v>
+        <v>-312915203.848655</v>
       </c>
       <c r="D70" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -8326,13 +8326,13 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>117053928.7929806</v>
+        <v>176153960.2739238</v>
       </c>
       <c r="C71" t="n">
-        <v>-196200068.0253333</v>
+        <v>-343614386.3589055</v>
       </c>
       <c r="D71" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -8436,13 +8436,13 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>95365514.89714105</v>
+        <v>141461029.2286593</v>
       </c>
       <c r="C72" t="n">
-        <v>-181345821.511656</v>
+        <v>-313261337.4333048</v>
       </c>
       <c r="D72" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -8550,13 +8550,13 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>121303952.3934693</v>
+        <v>182287677.5470982</v>
       </c>
       <c r="C73" t="n">
-        <v>-203760182.954509</v>
+        <v>-355683872.88319</v>
       </c>
       <c r="D73" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -8664,13 +8664,13 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>108553564.6148994</v>
+        <v>162324654.8337574</v>
       </c>
       <c r="C74" t="n">
-        <v>-192822032.907654</v>
+        <v>-335285133.9150388</v>
       </c>
       <c r="D74" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -8774,13 +8774,13 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>94543489.69320977</v>
+        <v>140083517.112945</v>
       </c>
       <c r="C75" t="n">
-        <v>-181175767.7115108</v>
+        <v>-312582969.6641316</v>
       </c>
       <c r="D75" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -8892,13 +8892,13 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>126364914.1193085</v>
+        <v>190110920.7044386</v>
       </c>
       <c r="C76" t="n">
-        <v>-208392521.0905573</v>
+        <v>-364012734.1181236</v>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -9006,13 +9006,13 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>114600012.8629923</v>
+        <v>172455005.3259168</v>
       </c>
       <c r="C77" t="n">
-        <v>-193023177.9961263</v>
+        <v>-338253843.2190355</v>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -9120,13 +9120,13 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>96183315.66373654</v>
+        <v>144749138.565618</v>
       </c>
       <c r="C78" t="n">
-        <v>-167070045.9265256</v>
+        <v>-294665484.1164553</v>
       </c>
       <c r="D78" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -9234,13 +9234,13 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>90102554.08998811</v>
+        <v>133185091.1502571</v>
       </c>
       <c r="C79" t="n">
-        <v>-175916186.1970724</v>
+        <v>-303142564.6646604</v>
       </c>
       <c r="D79" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -9348,13 +9348,13 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>112423974.4583378</v>
+        <v>167505773.2050066</v>
       </c>
       <c r="C80" t="n">
-        <v>-203313461.5824972</v>
+        <v>-351206488.4550836</v>
       </c>
       <c r="D80" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -9458,13 +9458,13 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>110882036.2597607</v>
+        <v>165132573.56512</v>
       </c>
       <c r="C81" t="n">
-        <v>-201588700.6533288</v>
+        <v>-348161339.9216876</v>
       </c>
       <c r="D81" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -9572,13 +9572,13 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>111720467.1438562</v>
+        <v>166376619.799163</v>
       </c>
       <c r="C82" t="n">
-        <v>-202900885.8178033</v>
+        <v>-350320043.4346986</v>
       </c>
       <c r="D82" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -9686,13 +9686,13 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>112373855.7463913</v>
+        <v>169686995.5234621</v>
       </c>
       <c r="C83" t="n">
-        <v>-185556001.5893668</v>
+        <v>-327114559.5798709</v>
       </c>
       <c r="D83" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -9796,13 +9796,13 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>103127200.0445412</v>
+        <v>155881092.0373029</v>
       </c>
       <c r="C84" t="n">
-        <v>-172088483.342384</v>
+        <v>-304734885.7252286</v>
       </c>
       <c r="D84" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -9906,13 +9906,13 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>122708990.1519759</v>
+        <v>184685398.9962063</v>
       </c>
       <c r="C85" t="n">
-        <v>-203255148.1129821</v>
+        <v>-355546272.1909546</v>
       </c>
       <c r="D85" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -10016,13 +10016,13 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>111990891.5363045</v>
+        <v>166779154.6414888</v>
       </c>
       <c r="C86" t="n">
-        <v>-203312680.5100742</v>
+        <v>-351000639.1919017</v>
       </c>
       <c r="D86" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -10130,13 +10130,13 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>98870863.49995132</v>
+        <v>149122844.3289035</v>
       </c>
       <c r="C87" t="n">
-        <v>-168604253.3247996</v>
+        <v>-298040444.5277905</v>
       </c>
       <c r="D87" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -10244,13 +10244,13 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>107111037.3784975</v>
+        <v>159556139.6523196</v>
       </c>
       <c r="C88" t="n">
-        <v>-195472323.0756261</v>
+        <v>-338145521.0098385</v>
       </c>
       <c r="D88" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -10354,13 +10354,13 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>90346546.34698622</v>
+        <v>133547828.5310905</v>
       </c>
       <c r="C89" t="n">
-        <v>-176336811.5477049</v>
+        <v>-303836046.3182639</v>
       </c>
       <c r="D89" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -10464,13 +10464,13 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>102529579.9533198</v>
+        <v>152283664.1886912</v>
       </c>
       <c r="C90" t="n">
-        <v>-191801156.5092006</v>
+        <v>-330938589.2846747</v>
       </c>
       <c r="D90" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -10578,13 +10578,13 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>90104528.73577157</v>
+        <v>133188057.8410134</v>
       </c>
       <c r="C91" t="n">
-        <v>-175919349.5840066</v>
+        <v>-303147861.3758538</v>
       </c>
       <c r="D91" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -10696,13 +10696,13 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>99291993.9236518</v>
+        <v>148270735.1169394</v>
       </c>
       <c r="C92" t="n">
-        <v>-180337878.069048</v>
+        <v>-314006239.1560445</v>
       </c>
       <c r="D92" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -10810,13 +10810,13 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>89515739.4878577</v>
+        <v>132326280.4560874</v>
       </c>
       <c r="C93" t="n">
-        <v>-174796657.0264485</v>
+        <v>-301332364.7394353</v>
       </c>
       <c r="D93" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -10920,13 +10920,13 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>90103705.07885629</v>
+        <v>133186820.3860261</v>
       </c>
       <c r="C94" t="n">
-        <v>-175918030.0872642</v>
+        <v>-303145652.0372005</v>
       </c>
       <c r="D94" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -11030,13 +11030,13 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>89565870.73928922</v>
+        <v>132393994.8824257</v>
       </c>
       <c r="C95" t="n">
-        <v>-174936500.8971657</v>
+        <v>-301545098.7286289</v>
       </c>
       <c r="D95" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -11140,13 +11140,13 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>105283796.2110587</v>
+        <v>158370105.7030456</v>
       </c>
       <c r="C96" t="n">
-        <v>-180789088.1050727</v>
+        <v>-317524795.5387079</v>
       </c>
       <c r="D96" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -11250,13 +11250,13 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>92663656.04225837</v>
+        <v>137142253.7138787</v>
       </c>
       <c r="C97" t="n">
-        <v>-179135917.8359909</v>
+        <v>-308841030.0071481</v>
       </c>
       <c r="D97" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -11368,13 +11368,13 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>105995838.9598717</v>
+        <v>158762612.8352239</v>
       </c>
       <c r="C98" t="n">
-        <v>-186983408.2862068</v>
+        <v>-326218674.1676497</v>
       </c>
       <c r="D98" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -11482,13 +11482,13 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>111852843.7911268</v>
+        <v>166557395.5412509</v>
       </c>
       <c r="C99" t="n">
-        <v>-203232990.950353</v>
+        <v>-350828214.6929647</v>
       </c>
       <c r="D99" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -11596,13 +11596,13 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>108682011.9880013</v>
+        <v>161864592.474834</v>
       </c>
       <c r="C100" t="n">
-        <v>-198149238.6850535</v>
+        <v>-342494323.4409122</v>
       </c>
       <c r="D100" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -11706,13 +11706,13 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>123262330.9647697</v>
+        <v>185912412.2909386</v>
       </c>
       <c r="C101" t="n">
-        <v>-200772585.0239061</v>
+        <v>-352339609.3305225</v>
       </c>
       <c r="D101" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -11820,13 +11820,13 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>95285337.07413501</v>
+        <v>141352485.3882477</v>
       </c>
       <c r="C102" t="n">
-        <v>-181128484.7188572</v>
+        <v>-312930112.7904053</v>
       </c>
       <c r="D102" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -11934,13 +11934,13 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>103205198.4397278</v>
+        <v>153369349.7000767</v>
       </c>
       <c r="C103" t="n">
-        <v>-192251246.9216498</v>
+        <v>-331885890.8858885</v>
       </c>
       <c r="D103" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -12052,13 +12052,13 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>106043189.6412067</v>
+        <v>158134275.1538757</v>
       </c>
       <c r="C104" t="n">
-        <v>-192486808.2343917</v>
+        <v>-333627310.9737434</v>
       </c>
       <c r="D104" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -12166,13 +12166,13 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>97110372.26147208</v>
+        <v>144420944.0583858</v>
       </c>
       <c r="C105" t="n">
-        <v>-181415844.8991398</v>
+        <v>-314299043.6368001</v>
       </c>
       <c r="D105" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -12280,13 +12280,13 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>131241033.4827757</v>
+        <v>195960828.5914616</v>
       </c>
       <c r="C106" t="n">
-        <v>-226689672.8295892</v>
+        <v>-390970843.5513169</v>
       </c>
       <c r="D106" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -12394,13 +12394,13 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>117129631.2220052</v>
+        <v>175859555.1756639</v>
       </c>
       <c r="C107" t="n">
-        <v>-199529950.2677192</v>
+        <v>-348190757.0122535</v>
       </c>
       <c r="D107" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -12508,13 +12508,13 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>94928926.66890271</v>
+        <v>140639105.5325498</v>
       </c>
       <c r="C108" t="n">
-        <v>-181961297.4746547</v>
+        <v>-313833282.4795468</v>
       </c>
       <c r="D108" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -12622,13 +12622,13 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>108290145.0312245</v>
+        <v>163555015.9934095</v>
       </c>
       <c r="C109" t="n">
-        <v>-179956136.3726603</v>
+        <v>-317730700.4146501</v>
       </c>
       <c r="D109" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -12736,13 +12736,13 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>88934308.95905775</v>
+        <v>131829548.5578723</v>
       </c>
       <c r="C110" t="n">
-        <v>-170947412.4750854</v>
+        <v>-295935671.3722316</v>
       </c>
       <c r="D110" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -12854,13 +12854,13 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>103972565.9586297</v>
+        <v>156634251.2094057</v>
       </c>
       <c r="C111" t="n">
-        <v>-177149054.5000275</v>
+        <v>-311991914.7384276</v>
       </c>
       <c r="D111" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -12964,13 +12964,13 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>112619817.770193</v>
+        <v>167670165.5312662</v>
       </c>
       <c r="C112" t="n">
-        <v>-204631253.2676903</v>
+        <v>-353066820.298147</v>
       </c>
       <c r="D112" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -13074,13 +13074,13 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>90460510.7681088</v>
+        <v>134124177.6926021</v>
       </c>
       <c r="C113" t="n">
-        <v>-173375849.083366</v>
+        <v>-300005557.9198745</v>
       </c>
       <c r="D113" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -13192,13 +13192,13 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>90322966.28199582</v>
+        <v>133905416.5137617</v>
       </c>
       <c r="C114" t="n">
-        <v>-173249850.8613234</v>
+        <v>-299761365.7542637</v>
       </c>
       <c r="D114" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -13310,13 +13310,13 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>127185375.7843002</v>
+        <v>189752920.4501799</v>
       </c>
       <c r="C115" t="n">
-        <v>-222549344.2806582</v>
+        <v>-383696858.5584973</v>
       </c>
       <c r="D115" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -13416,13 +13416,13 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>104324543.1966155</v>
+        <v>156894333.2309652</v>
       </c>
       <c r="C116" t="n">
-        <v>-179677254.0545461</v>
+        <v>-315577009.9073716</v>
       </c>
       <c r="D116" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -13526,13 +13526,13 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>104886990.260056</v>
+        <v>157278467.8209096</v>
       </c>
       <c r="C117" t="n">
-        <v>-183990122.8937142</v>
+        <v>-321661930.9312663</v>
       </c>
       <c r="D117" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -13644,13 +13644,13 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>120626767.3054073</v>
+        <v>181492026.8387491</v>
       </c>
       <c r="C118" t="n">
-        <v>-201107675.9514737</v>
+        <v>-351779561.8086059</v>
       </c>
       <c r="D118" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -13754,13 +13754,13 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>106253987.7411452</v>
+        <v>158654562.4475776</v>
       </c>
       <c r="C119" t="n">
-        <v>-191200737.3196173</v>
+        <v>-332007778.8960634</v>
       </c>
       <c r="D119" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -13860,13 +13860,13 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>93418613.15065667</v>
+        <v>138590394.9895089</v>
       </c>
       <c r="C120" t="n">
-        <v>-177883619.6676927</v>
+        <v>-307612979.354601</v>
       </c>
       <c r="D120" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -13970,13 +13970,13 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>90103152.92810416</v>
+        <v>133185990.8395032</v>
       </c>
       <c r="C121" t="n">
-        <v>-175917145.5400779</v>
+        <v>-303144170.9692506</v>
       </c>
       <c r="D121" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -14084,13 +14084,13 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>89440695.01134434</v>
+        <v>132580669.0374985</v>
       </c>
       <c r="C122" t="n">
-        <v>-171833818.660059</v>
+        <v>-297392959.7766616</v>
       </c>
       <c r="D122" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -14202,13 +14202,13 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>90056417.80823579</v>
+        <v>133511768.317774</v>
       </c>
       <c r="C123" t="n">
-        <v>-172772092.1143855</v>
+        <v>-298980260.4610214</v>
       </c>
       <c r="D123" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -14320,13 +14320,13 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>112341383.2848444</v>
+        <v>168895924.6174865</v>
       </c>
       <c r="C124" t="n">
-        <v>-191251237.3799561</v>
+        <v>-334874479.5921599</v>
       </c>
       <c r="D124" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -14426,13 +14426,13 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>91638603.847031</v>
+        <v>135980696.7712135</v>
       </c>
       <c r="C125" t="n">
-        <v>-174580687.5775971</v>
+        <v>-302259460.6362427</v>
       </c>
       <c r="D125" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -14536,13 +14536,13 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>104041565.2928592</v>
+        <v>156055763.8399591</v>
       </c>
       <c r="C126" t="n">
-        <v>-182405013.0074969</v>
+        <v>-319124905.5774159</v>
       </c>
       <c r="D126" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -14650,13 +14650,13 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>98434944.37232505</v>
+        <v>148894692.201322</v>
       </c>
       <c r="C127" t="n">
-        <v>-164850226.8295321</v>
+        <v>-292750297.2836502</v>
       </c>
       <c r="D127" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -14768,13 +14768,13 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>90102346.77343935</v>
+        <v>133184779.6796461</v>
       </c>
       <c r="C128" t="n">
-        <v>-175915854.0738463</v>
+        <v>-303142008.564218</v>
       </c>
       <c r="D128" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -14878,13 +14878,13 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>105297578.2185064</v>
+        <v>157709961.4847255</v>
       </c>
       <c r="C129" t="n">
-        <v>-186004423.6349301</v>
+        <v>-324568981.0597339</v>
       </c>
       <c r="D129" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -14992,13 +14992,13 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>91506333.97392675</v>
+        <v>136535760.4980252</v>
       </c>
       <c r="C130" t="n">
-        <v>-168656066.0726092</v>
+        <v>-294347993.0635681</v>
       </c>
       <c r="D130" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -15106,13 +15106,13 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>100244385.6920507</v>
+        <v>149732268.4740105</v>
       </c>
       <c r="C131" t="n">
-        <v>-181532297.7965564</v>
+        <v>-316086388.4335951</v>
       </c>
       <c r="D131" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -15220,13 +15220,13 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>90930063.13631396</v>
+        <v>134889794.6426065</v>
       </c>
       <c r="C132" t="n">
-        <v>-173660181.4769069</v>
+        <v>-300646322.6606014</v>
       </c>
       <c r="D132" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -15334,13 +15334,13 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>89889286.84587127</v>
+        <v>132864678.2326166</v>
       </c>
       <c r="C133" t="n">
-        <v>-175574363.7411091</v>
+        <v>-302570221.9648896</v>
       </c>
       <c r="D133" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -15444,13 +15444,13 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>102209313.6826625</v>
+        <v>152280106.6002271</v>
       </c>
       <c r="C134" t="n">
-        <v>-187581930.313654</v>
+        <v>-325158468.1114321</v>
       </c>
       <c r="D134" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -15562,13 +15562,13 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>105299421.9336895</v>
+        <v>159279825.8139072</v>
       </c>
       <c r="C135" t="n">
-        <v>-174154437.565182</v>
+        <v>-308512725.8769764</v>
       </c>
       <c r="D135" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -15676,13 +15676,13 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>94630554.37158425</v>
+        <v>140463547.6134146</v>
       </c>
       <c r="C136" t="n">
-        <v>-179373611.5363451</v>
+        <v>-310251056.9035797</v>
       </c>
       <c r="D136" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -15790,13 +15790,13 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>103648004.1509348</v>
+        <v>155355626.9989494</v>
       </c>
       <c r="C137" t="n">
-        <v>-182663034.0110876</v>
+        <v>-319283793.2341586</v>
       </c>
       <c r="D137" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -15904,13 +15904,13 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>98265994.57547078</v>
+        <v>146482371.0578764</v>
       </c>
       <c r="C138" t="n">
-        <v>-180676396.8603028</v>
+        <v>-313926944.2323142</v>
       </c>
       <c r="D138" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -16014,13 +16014,13 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>119293100.639567</v>
+        <v>177658724.1819302</v>
       </c>
       <c r="C139" t="n">
-        <v>-214134830.6730939</v>
+        <v>-368915994.1828201</v>
       </c>
       <c r="D139" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -16128,13 +16128,13 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>108800112.9038873</v>
+        <v>162261097.3869281</v>
       </c>
       <c r="C140" t="n">
-        <v>-196583746.7168819</v>
+        <v>-340454572.3690091</v>
       </c>
       <c r="D140" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -16238,13 +16238,13 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>90651901.65778245</v>
+        <v>134416284.8910971</v>
       </c>
       <c r="C141" t="n">
-        <v>-173645533.7513208</v>
+        <v>-300469559.7393534</v>
       </c>
       <c r="D141" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -16356,13 +16356,13 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>109559722.9289189</v>
+        <v>164979926.9176007</v>
       </c>
       <c r="C142" t="n">
-        <v>-185388306.1858294</v>
+        <v>-325686176.3676955</v>
       </c>
       <c r="D142" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -16466,13 +16466,13 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>103634729.2958177</v>
+        <v>155434422.7048624</v>
       </c>
       <c r="C143" t="n">
-        <v>-181891542.7247275</v>
+        <v>-318239233.6028578</v>
       </c>
       <c r="D143" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -16584,13 +16584,13 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>93414706.53621852</v>
+        <v>140488008.7864806</v>
       </c>
       <c r="C144" t="n">
-        <v>-163614334.2863328</v>
+        <v>-288631722.7400994</v>
       </c>
       <c r="D144" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -16698,13 +16698,13 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>119403884.9223573</v>
+        <v>180469151.9710608</v>
       </c>
       <c r="C145" t="n">
-        <v>-193070738.2963331</v>
+        <v>-340246412.4500048</v>
       </c>
       <c r="D145" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -16808,13 +16808,13 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>91236690.37009616</v>
+        <v>135273482.2421477</v>
       </c>
       <c r="C146" t="n">
-        <v>-174739885.005937</v>
+        <v>-302242974.9294235</v>
       </c>
       <c r="D146" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -16926,13 +16926,13 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>107560206.4702901</v>
+        <v>160201540.2584676</v>
       </c>
       <c r="C147" t="n">
-        <v>-196355097.4582179</v>
+        <v>-339546457.0315033</v>
       </c>
       <c r="D147" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -17036,13 +17036,13 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>125912398.5125425</v>
+        <v>190124677.2012815</v>
       </c>
       <c r="C148" t="n">
-        <v>-202194520.6540882</v>
+        <v>-355283189.0850319</v>
       </c>
       <c r="D148" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -17150,13 +17150,13 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>107664834.9478427</v>
+        <v>160612346.5819714</v>
       </c>
       <c r="C149" t="n">
-        <v>-194505661.1581519</v>
+        <v>-337121517.7568866</v>
       </c>
       <c r="D149" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -17260,13 +17260,13 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>96672242.48385458</v>
+        <v>143562825.7276157</v>
       </c>
       <c r="C150" t="n">
-        <v>-182290563.4259088</v>
+        <v>-315222775.6070763</v>
       </c>
       <c r="D150" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -17370,13 +17370,13 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>105035861.4768484</v>
+        <v>157286568.1629081</v>
       </c>
       <c r="C151" t="n">
-        <v>-185858100.2964173</v>
+        <v>-324247018.6740065</v>
       </c>
       <c r="D151" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -17484,13 +17484,13 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>129709496.8307995</v>
+        <v>193692536.7711925</v>
       </c>
       <c r="C152" t="n">
-        <v>-224507523.2811059</v>
+        <v>-387386853.8541706</v>
       </c>
       <c r="D152" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -17590,13 +17590,13 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>110112505.5368656</v>
+        <v>164184943.0664755</v>
       </c>
       <c r="C153" t="n">
-        <v>-198834921.7274409</v>
+        <v>-344101784.2502127</v>
       </c>
       <c r="D153" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -17704,13 +17704,13 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>95345408.76258494</v>
+        <v>141499581.2481183</v>
       </c>
       <c r="C154" t="n">
-        <v>-180780035.102492</v>
+        <v>-312502448.8642993</v>
       </c>
       <c r="D154" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -17814,13 +17814,13 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>119327644.5647107</v>
+        <v>179374978.14723</v>
       </c>
       <c r="C155" t="n">
-        <v>-200737863.3305627</v>
+        <v>-350749944.9179873</v>
       </c>
       <c r="D155" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -17928,13 +17928,13 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>93428592.75277303</v>
+        <v>138669240.9957263</v>
       </c>
       <c r="C156" t="n">
-        <v>-177405817.098093</v>
+        <v>-306987520.5271319</v>
       </c>
       <c r="D156" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -18038,13 +18038,13 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>114371692.2541738</v>
+        <v>172370145.7890951</v>
       </c>
       <c r="C157" t="n">
-        <v>-190702731.3950348</v>
+        <v>-334988174.8863518</v>
       </c>
       <c r="D157" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -18148,13 +18148,13 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>104586949.9232588</v>
+        <v>158047362.4552254</v>
       </c>
       <c r="C158" t="n">
-        <v>-174359078.1543424</v>
+        <v>-308478310.5134187</v>
       </c>
       <c r="D158" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -18262,13 +18262,13 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>91749754.6950718</v>
+        <v>136034211.1299297</v>
       </c>
       <c r="C159" t="n">
-        <v>-175631204.4296953</v>
+        <v>-303707503.5453642</v>
       </c>
       <c r="D159" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -18376,13 +18376,13 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>125835557.693632</v>
+        <v>190018661.6349129</v>
       </c>
       <c r="C160" t="n">
-        <v>-202024111.6928512</v>
+        <v>-355019272.5760236</v>
       </c>
       <c r="D160" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -18490,13 +18490,13 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>116300547.405243</v>
+        <v>175674117.4082528</v>
       </c>
       <c r="C161" t="n">
-        <v>-190094256.5324488</v>
+        <v>-334936743.4465915</v>
       </c>
       <c r="D161" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -18604,13 +18604,13 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>107311224.3497591</v>
+        <v>159862336.8049855</v>
       </c>
       <c r="C162" t="n">
-        <v>-195719287.5035029</v>
+        <v>-338574060.1625065</v>
       </c>
       <c r="D162" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -18718,13 +18718,13 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>114562592.945937</v>
+        <v>172501839.5428112</v>
       </c>
       <c r="C163" t="n">
-        <v>-192167750.2243736</v>
+        <v>-337070218.076261</v>
       </c>
       <c r="D163" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -18828,13 +18828,13 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>95010133.05762434</v>
+        <v>140978618.3775643</v>
       </c>
       <c r="C164" t="n">
-        <v>-180392714.7041181</v>
+        <v>-311806607.7948179</v>
       </c>
       <c r="D164" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -18938,13 +18938,13 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>116833037.3592419</v>
+        <v>176504865.0907648</v>
       </c>
       <c r="C165" t="n">
-        <v>-190550371.3754974</v>
+        <v>-335774920.3028822</v>
       </c>
       <c r="D165" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -19052,13 +19052,13 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>123867952.8791168</v>
+        <v>186579111.1927735</v>
       </c>
       <c r="C166" t="n">
-        <v>-203491291.7640728</v>
+        <v>-356316923.1990488</v>
       </c>
       <c r="D166" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -19162,13 +19162,13 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>94930873.93600039</v>
+        <v>140871400.795211</v>
       </c>
       <c r="C167" t="n">
-        <v>-180177301.1360669</v>
+        <v>-311478364.8432201</v>
       </c>
       <c r="D167" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -19276,13 +19276,13 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>109024145.1125965</v>
+        <v>163430863.372584</v>
       </c>
       <c r="C168" t="n">
-        <v>-190379985.0380221</v>
+        <v>-332212175.4115949</v>
       </c>
       <c r="D168" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -19382,13 +19382,13 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>122610651.9789469</v>
+        <v>185508470.2791307</v>
       </c>
       <c r="C169" t="n">
-        <v>-195356301.638187</v>
+        <v>-344604991.2797332</v>
       </c>
       <c r="D169" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -19496,13 +19496,13 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>112012066.3744351</v>
+        <v>168769481.6174906</v>
       </c>
       <c r="C170" t="n">
-        <v>-187947443.025041</v>
+        <v>-330232150.1497709</v>
       </c>
       <c r="D170" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -19606,13 +19606,13 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>115464965.0687606</v>
+        <v>174362090.1054911</v>
       </c>
       <c r="C171" t="n">
-        <v>-189437112.6759949</v>
+        <v>-333699826.9162512</v>
       </c>
       <c r="D171" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -19716,13 +19716,13 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>123165218.7500279</v>
+        <v>185345857.7778867</v>
       </c>
       <c r="C172" t="n">
-        <v>-204035832.0819772</v>
+        <v>-356796154.4118779</v>
       </c>
       <c r="D172" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -19830,13 +19830,13 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>126035442.3380523</v>
+        <v>190360136.8154513</v>
       </c>
       <c r="C173" t="n">
-        <v>-201934946.3262615</v>
+        <v>-354967632.5779494</v>
       </c>
       <c r="D173" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -19944,13 +19944,13 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>103963286.9951731</v>
+        <v>155689613.3434788</v>
       </c>
       <c r="C174" t="n">
-        <v>-184189772.1687449</v>
+        <v>-321488368.2586542</v>
       </c>
       <c r="D174" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -20058,13 +20058,13 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>123167917.7093716</v>
+        <v>186277094.8049808</v>
       </c>
       <c r="C175" t="n">
-        <v>-196595593.1394584</v>
+        <v>-346526615.0679132</v>
       </c>
       <c r="D175" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -20168,13 +20168,13 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>125009597.6335431</v>
+        <v>188046861.7576432</v>
       </c>
       <c r="C176" t="n">
-        <v>-206928505.2360481</v>
+        <v>-361483242.0999983</v>
       </c>
       <c r="D176" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -20274,13 +20274,13 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>104729571.0001448</v>
+        <v>157062556.0037677</v>
       </c>
       <c r="C177" t="n">
-        <v>-183605424.8142278</v>
+        <v>-321069006.3031799</v>
       </c>
       <c r="D177" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -20384,13 +20384,13 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>108428450.8804912</v>
+        <v>161518848.3261522</v>
       </c>
       <c r="C178" t="n">
-        <v>-197505404.3038669</v>
+        <v>-341509384.2953113</v>
       </c>
       <c r="D178" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -20498,13 +20498,13 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>107513991.4400155</v>
+        <v>160172432.4412201</v>
       </c>
       <c r="C179" t="n">
-        <v>-195969432.9036126</v>
+        <v>-339007995.8900697</v>
       </c>
       <c r="D179" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -20612,13 +20612,13 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>119549321.5548093</v>
+        <v>178732917.1826238</v>
       </c>
       <c r="C180" t="n">
-        <v>-208864742.2065115</v>
+        <v>-361906707.6826982</v>
       </c>
       <c r="D180" t="n">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
optimizing variogram parameters for area 3
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>141348099.896921</v>
+        <v>155186282.5163826</v>
       </c>
       <c r="C2" t="n">
-        <v>-312922610.203993</v>
+        <v>-355284140.737343</v>
       </c>
       <c r="D2" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>178703408.6955554</v>
+        <v>196544314.2725931</v>
       </c>
       <c r="C3" t="n">
-        <v>-362295201.6112791</v>
+        <v>-411636476.3766083</v>
       </c>
       <c r="D3" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>157319701.6040834</v>
+        <v>173130360.6929421</v>
       </c>
       <c r="C4" t="n">
-        <v>-322206528.3678634</v>
+        <v>-366720078.5053295</v>
       </c>
       <c r="D4" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>142056384.3197211</v>
+        <v>155939419.7333016</v>
       </c>
       <c r="C5" t="n">
-        <v>-315497640.8960232</v>
+        <v>-358115531.9229566</v>
       </c>
       <c r="D5" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>141904992.4841089</v>
+        <v>155767778.4642669</v>
       </c>
       <c r="C6" t="n">
-        <v>-315481395.9970667</v>
+        <v>-358083241.6631406</v>
       </c>
       <c r="D6" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>164413949.5216025</v>
+        <v>180665283.8416124</v>
       </c>
       <c r="C7" t="n">
-        <v>-347491935.8960524</v>
+        <v>-394532657.9500122</v>
       </c>
       <c r="D7" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>142093030.5559932</v>
+        <v>155987577.3472792</v>
       </c>
       <c r="C8" t="n">
-        <v>-315170365.2597262</v>
+        <v>-357768108.1902798</v>
       </c>
       <c r="D8" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>157915916.6761881</v>
+        <v>173755454.4975769</v>
       </c>
       <c r="C9" t="n">
-        <v>-324720174.3036515</v>
+        <v>-369476857.1464744</v>
       </c>
       <c r="D9" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>138963431.6057103</v>
+        <v>152508113.2399762</v>
       </c>
       <c r="C10" t="n">
-        <v>-311358900.6426019</v>
+        <v>-353371208.2346841</v>
       </c>
       <c r="D10" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>158155895.589951</v>
+        <v>174057455.4525982</v>
       </c>
       <c r="C11" t="n">
-        <v>-323250782.3943694</v>
+        <v>-367915076.6274578</v>
       </c>
       <c r="D11" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>186807109.2753962</v>
+        <v>205731289.6267988</v>
       </c>
       <c r="C12" t="n">
-        <v>-360587711.855448</v>
+        <v>-410386550.8987644</v>
       </c>
       <c r="D12" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>171799814.8913856</v>
+        <v>189006844.5387366</v>
       </c>
       <c r="C13" t="n">
-        <v>-348508131.1287501</v>
+        <v>-396237483.7314262</v>
       </c>
       <c r="D13" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>137522281.9252852</v>
+        <v>150967007.5884917</v>
       </c>
       <c r="C14" t="n">
-        <v>-306526338.6425698</v>
+        <v>-348045753.5317158</v>
       </c>
       <c r="D14" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>148379064.2916293</v>
+        <v>163499715.651751</v>
       </c>
       <c r="C15" t="n">
-        <v>-297192877.2481689</v>
+        <v>-339018591.0933486</v>
       </c>
       <c r="D15" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>187641498.9218537</v>
+        <v>206684949.9050232</v>
       </c>
       <c r="C16" t="n">
-        <v>-359974207.1259955</v>
+        <v>-409780567.1759447</v>
       </c>
       <c r="D16" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>175465203.9267208</v>
+        <v>193082177.3012131</v>
       </c>
       <c r="C17" t="n">
-        <v>-352113034.5898279</v>
+        <v>-400409682.3877724</v>
       </c>
       <c r="D17" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>181427741.6017235</v>
+        <v>199552338.6221488</v>
       </c>
       <c r="C18" t="n">
-        <v>-365943608.0528963</v>
+        <v>-415778194.4573804</v>
       </c>
       <c r="D18" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>189349594.7699511</v>
+        <v>208679123.9730402</v>
       </c>
       <c r="C19" t="n">
-        <v>-356528717.3753525</v>
+        <v>-406167113.4694846</v>
       </c>
       <c r="D19" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>141458787.0723889</v>
+        <v>155305325.9332242</v>
       </c>
       <c r="C20" t="n">
-        <v>-313257500.772146</v>
+        <v>-355654206.5168758</v>
       </c>
       <c r="D20" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>191972331.1404673</v>
+        <v>211544535.3069784</v>
       </c>
       <c r="C21" t="n">
-        <v>-361328626.4466391</v>
+        <v>-411533388.5074365</v>
       </c>
       <c r="D21" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>182904035.3541456</v>
+        <v>201565592.8729976</v>
       </c>
       <c r="C22" t="n">
-        <v>-348238819.2016164</v>
+        <v>-396766276.2385935</v>
       </c>
       <c r="D22" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>141382299.2509747</v>
+        <v>155196801.0224651</v>
       </c>
       <c r="C23" t="n">
-        <v>-314339671.5201009</v>
+        <v>-356807367.5218722</v>
       </c>
       <c r="D23" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>141721499.0632483</v>
+        <v>155570487.5770514</v>
       </c>
       <c r="C24" t="n">
-        <v>-314922671.6170502</v>
+        <v>-357465986.4543495</v>
       </c>
       <c r="D24" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>182286786.5278214</v>
+        <v>200722434.247045</v>
       </c>
       <c r="C25" t="n">
-        <v>-355682675.3674026</v>
+        <v>-404768673.6249115</v>
       </c>
       <c r="D25" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>169006163.3432604</v>
+        <v>185996213.297362</v>
       </c>
       <c r="C26" t="n">
-        <v>-340885700.9276638</v>
+        <v>-387800921.8206634</v>
       </c>
       <c r="D26" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>141238730.7640204</v>
+        <v>155051228.0084344</v>
       </c>
       <c r="C27" t="n">
-        <v>-313462381.3896099</v>
+        <v>-355852353.1976787</v>
       </c>
       <c r="D27" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>172961831.9667335</v>
+        <v>190663678.7888838</v>
       </c>
       <c r="C28" t="n">
-        <v>-331368761.8243606</v>
+        <v>-377827853.5778434</v>
       </c>
       <c r="D28" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>149682088.5391768</v>
+        <v>164829680.2202438</v>
       </c>
       <c r="C29" t="n">
-        <v>-304353800.1510978</v>
+        <v>-346844092.1084408</v>
       </c>
       <c r="D29" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>184511210.0317812</v>
+        <v>203317294.4936355</v>
       </c>
       <c r="C30" t="n">
-        <v>-351457881.0413339</v>
+        <v>-400357657.6337687</v>
       </c>
       <c r="D30" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>182290094.6041036</v>
+        <v>200726084.2348005</v>
       </c>
       <c r="C31" t="n">
-        <v>-355687121.3447877</v>
+        <v>-404773712.7128288</v>
       </c>
       <c r="D31" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>141202604.9046527</v>
+        <v>155003677.0435953</v>
       </c>
       <c r="C32" t="n">
-        <v>-313788147.2910262</v>
+        <v>-356198184.1442469</v>
       </c>
       <c r="D32" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>179846307.3456305</v>
+        <v>197775388.6890371</v>
       </c>
       <c r="C33" t="n">
-        <v>-365423631.8033922</v>
+        <v>-415096549.5071747</v>
       </c>
       <c r="D33" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>141535203.7030983</v>
+        <v>155361373.2639571</v>
       </c>
       <c r="C34" t="n">
-        <v>-314796955.9100499</v>
+        <v>-357312835.8907093</v>
       </c>
       <c r="D34" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>188638009.6649984</v>
+        <v>207902554.2738627</v>
       </c>
       <c r="C35" t="n">
-        <v>-355177105.0007602</v>
+        <v>-404657525.0644075</v>
       </c>
       <c r="D35" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>187073764.5966155</v>
+        <v>206054635.0396705</v>
       </c>
       <c r="C36" t="n">
-        <v>-359435188.227848</v>
+        <v>-409159008.4394572</v>
       </c>
       <c r="D36" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>151100699.8415523</v>
+        <v>166384437.3759427</v>
       </c>
       <c r="C37" t="n">
-        <v>-307056524.2853937</v>
+        <v>-349876582.6575621</v>
       </c>
       <c r="D37" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>153302545.1236823</v>
+        <v>168851319.6347371</v>
       </c>
       <c r="C38" t="n">
-        <v>-308638682.613012</v>
+        <v>-351767591.9995821</v>
       </c>
       <c r="D38" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>137427790.8201395</v>
+        <v>150795742.9964098</v>
       </c>
       <c r="C39" t="n">
-        <v>-309720944.1721357</v>
+        <v>-351461103.3519568</v>
       </c>
       <c r="D39" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>140683036.6809032</v>
+        <v>154453493.7807354</v>
       </c>
       <c r="C40" t="n">
-        <v>-311783616.8171786</v>
+        <v>-353997140.5139248</v>
       </c>
       <c r="D40" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>182185480.8546159</v>
+        <v>200613129.3372485</v>
       </c>
       <c r="C41" t="n">
-        <v>-355420101.1418816</v>
+        <v>-404477807.3599414</v>
       </c>
       <c r="D41" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>139785958.6206442</v>
+        <v>153427588.5896657</v>
       </c>
       <c r="C42" t="n">
-        <v>-312116013.6802651</v>
+        <v>-354264931.2292031</v>
       </c>
       <c r="D42" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>139436924.7472599</v>
+        <v>153095851.8690318</v>
       </c>
       <c r="C43" t="n">
-        <v>-308877426.2758054</v>
+        <v>-350757250.7678999</v>
       </c>
       <c r="D43" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>157108380.5028565</v>
+        <v>172893903.4587503</v>
       </c>
       <c r="C44" t="n">
-        <v>-322048073.0520066</v>
+        <v>-366531568.0279778</v>
       </c>
       <c r="D44" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>134113871.8673896</v>
+        <v>147215120.8201736</v>
       </c>
       <c r="C45" t="n">
-        <v>-300402910.3628743</v>
+        <v>-341137333.3318655</v>
       </c>
       <c r="D45" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>142167772.0194329</v>
+        <v>156059212.2187155</v>
       </c>
       <c r="C46" t="n">
-        <v>-315835162.0295094</v>
+        <v>-358488457.7172877</v>
       </c>
       <c r="D46" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>139622332.8264687</v>
+        <v>153225320.3627685</v>
       </c>
       <c r="C47" t="n">
-        <v>-312937151.0000179</v>
+        <v>-355129047.8733214</v>
       </c>
       <c r="D47" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>139914049.4457763</v>
+        <v>153617755.9656588</v>
       </c>
       <c r="C48" t="n">
-        <v>-309887552.3178197</v>
+        <v>-351887747.4773654</v>
       </c>
       <c r="D48" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>185854151.742791</v>
+        <v>204712543.8454991</v>
       </c>
       <c r="C49" t="n">
-        <v>-357653567.1813228</v>
+        <v>-407149119.8925413</v>
       </c>
       <c r="D49" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>142014766.7871837</v>
+        <v>155920833.5419316</v>
       </c>
       <c r="C50" t="n">
-        <v>-314061916.8233049</v>
+        <v>-356571491.1156015</v>
       </c>
       <c r="D50" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>159120642.1015579</v>
+        <v>175430197.5408969</v>
       </c>
       <c r="C51" t="n">
-        <v>-309707474.7853568</v>
+        <v>-353391190.5228757</v>
       </c>
       <c r="D51" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>165886800.0556829</v>
+        <v>182296023.1598229</v>
       </c>
       <c r="C52" t="n">
-        <v>-349389803.8062887</v>
+        <v>-396699916.2584975</v>
       </c>
       <c r="D52" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>176051257.9623712</v>
+        <v>193632434.3363308</v>
       </c>
       <c r="C53" t="n">
-        <v>-357852654.1054109</v>
+        <v>-406642287.6299921</v>
       </c>
       <c r="D53" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>134412228.8925521</v>
+        <v>147553207.4215885</v>
       </c>
       <c r="C54" t="n">
-        <v>-300462479.4236699</v>
+        <v>-341231416.4951763</v>
       </c>
       <c r="D54" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>141128205.7539958</v>
+        <v>154941086.9860992</v>
       </c>
       <c r="C55" t="n">
-        <v>-312691525.8584673</v>
+        <v>-355014700.9734443</v>
       </c>
       <c r="D55" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>174994308.3881196</v>
+        <v>192574674.3692023</v>
       </c>
       <c r="C56" t="n">
-        <v>-350840163.793776</v>
+        <v>-399000870.056523</v>
       </c>
       <c r="D56" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>133152710.8121899</v>
+        <v>146069419.9447235</v>
       </c>
       <c r="C57" t="n">
-        <v>-303038671.2823944</v>
+        <v>-343863818.213274</v>
       </c>
       <c r="D57" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>167500273.6470561</v>
+        <v>184087436.2332685</v>
       </c>
       <c r="C58" t="n">
-        <v>-351198028.2771947</v>
+        <v>-398781818.7649365</v>
       </c>
       <c r="D58" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>152566433.763808</v>
+        <v>168049193.5427126</v>
       </c>
       <c r="C59" t="n">
-        <v>-307027879.2079807</v>
+        <v>-349970129.3104186</v>
       </c>
       <c r="D59" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>162353705.6233473</v>
+        <v>178420228.5645504</v>
       </c>
       <c r="C60" t="n">
-        <v>-342984243.4647176</v>
+        <v>-389507600.1477705</v>
       </c>
       <c r="D60" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>182900000.1607319</v>
+        <v>201027362.5022249</v>
       </c>
       <c r="C61" t="n">
-        <v>-375730773.3307462</v>
+        <v>-426438833.8456725</v>
       </c>
       <c r="D61" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>185852166.9742152</v>
+        <v>204710353.5541095</v>
       </c>
       <c r="C62" t="n">
-        <v>-357650979.020691</v>
+        <v>-407146185.1421992</v>
       </c>
       <c r="D62" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>151272705.8182151</v>
+        <v>166695692.4632627</v>
       </c>
       <c r="C63" t="n">
-        <v>-301506965.1118869</v>
+        <v>-343911712.2507417</v>
       </c>
       <c r="D63" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>164372378.2907965</v>
+        <v>180629424.1221489</v>
       </c>
       <c r="C64" t="n">
-        <v>-346920916.0419698</v>
+        <v>-393915056.3532701</v>
       </c>
       <c r="D64" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>152153190.0924732</v>
+        <v>167083811.2216147</v>
       </c>
       <c r="C65" t="n">
-        <v>-331452261.5825568</v>
+        <v>-376200657.5862347</v>
       </c>
       <c r="D65" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>160006688.2880322</v>
+        <v>176436617.1285712</v>
       </c>
       <c r="C66" t="n">
-        <v>-309625249.6685805</v>
+        <v>-353371076.6943061</v>
       </c>
       <c r="D66" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>165888299.3243921</v>
+        <v>182297675.2594912</v>
       </c>
       <c r="C67" t="n">
-        <v>-349392130.2866428</v>
+        <v>-396702546.3344389</v>
       </c>
       <c r="D67" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>149672339.1384026</v>
+        <v>164844380.8782575</v>
       </c>
       <c r="C68" t="n">
-        <v>-303119257.454601</v>
+        <v>-345513688.5489202</v>
       </c>
       <c r="D68" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>149554551.1177341</v>
+        <v>164908082.2140847</v>
       </c>
       <c r="C69" t="n">
-        <v>-293750538.5389981</v>
+        <v>-335405353.3376096</v>
       </c>
       <c r="D69" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>156976021.7356825</v>
+        <v>172931203.1371433</v>
       </c>
       <c r="C70" t="n">
-        <v>-312915203.848655</v>
+        <v>-356680798.8871456</v>
       </c>
       <c r="D70" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>176153960.2739238</v>
+        <v>194029018.9871371</v>
       </c>
       <c r="C71" t="n">
-        <v>-343614386.3589055</v>
+        <v>-391290253.1933777</v>
       </c>
       <c r="D71" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>141461029.2286593</v>
+        <v>155307796.3672507</v>
       </c>
       <c r="C72" t="n">
-        <v>-313261337.4333048</v>
+        <v>-355658541.6282188</v>
       </c>
       <c r="D72" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>182287677.5470982</v>
+        <v>200723417.3590471</v>
       </c>
       <c r="C73" t="n">
-        <v>-355683872.88319</v>
+        <v>-404770030.8939012</v>
       </c>
       <c r="D73" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>162324654.8337574</v>
+        <v>178540398.2998848</v>
       </c>
       <c r="C74" t="n">
-        <v>-335285133.9150388</v>
+        <v>-381222269.6195494</v>
       </c>
       <c r="D74" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>140083517.112945</v>
+        <v>153756347.5309934</v>
       </c>
       <c r="C75" t="n">
-        <v>-312582969.6641316</v>
+        <v>-354795176.0726953</v>
       </c>
       <c r="D75" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>190110920.7044386</v>
+        <v>209393291.6337691</v>
       </c>
       <c r="C76" t="n">
-        <v>-364012734.1181236</v>
+        <v>-414314745.135057</v>
       </c>
       <c r="D76" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>172455005.3259168</v>
+        <v>189952042.4358481</v>
       </c>
       <c r="C77" t="n">
-        <v>-338253843.2190355</v>
+        <v>-385228080.9502848</v>
       </c>
       <c r="D77" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>144749138.565618</v>
+        <v>159427739.3415537</v>
       </c>
       <c r="C78" t="n">
-        <v>-294665484.1164553</v>
+        <v>-335982549.9278293</v>
       </c>
       <c r="D78" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>133185091.1502571</v>
+        <v>146104165.8187904</v>
       </c>
       <c r="C79" t="n">
-        <v>-303142564.6646604</v>
+        <v>-343978472.1932865</v>
       </c>
       <c r="D79" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>167505773.2050066</v>
+        <v>184093496.6619012</v>
       </c>
       <c r="C80" t="n">
-        <v>-351206488.4550836</v>
+        <v>-398791383.9021803</v>
       </c>
       <c r="D80" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>165132573.56512</v>
+        <v>181466019.6913999</v>
       </c>
       <c r="C81" t="n">
-        <v>-348161339.9216876</v>
+        <v>-395314256.5035633</v>
       </c>
       <c r="D81" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>166376619.799163</v>
+        <v>182832422.7411771</v>
       </c>
       <c r="C82" t="n">
-        <v>-350320043.4346986</v>
+        <v>-397742156.952522</v>
       </c>
       <c r="D82" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>169686995.5234621</v>
+        <v>187043943.8371796</v>
       </c>
       <c r="C83" t="n">
-        <v>-327114559.5798709</v>
+        <v>-372992014.8445476</v>
       </c>
       <c r="D83" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>155881092.0373029</v>
+        <v>171859151.1753787</v>
       </c>
       <c r="C84" t="n">
-        <v>-304734885.7252286</v>
+        <v>-347768652.5221396</v>
       </c>
       <c r="D84" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>184685398.9962063</v>
+        <v>203434052.6487181</v>
       </c>
       <c r="C85" t="n">
-        <v>-355546272.1909546</v>
+        <v>-404790327.899222</v>
       </c>
       <c r="D85" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>166779154.6414888</v>
+        <v>183274862.4207279</v>
       </c>
       <c r="C86" t="n">
-        <v>-351000639.1919017</v>
+        <v>-398508414.7768783</v>
       </c>
       <c r="D86" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>149122844.3289035</v>
+        <v>164326832.2141601</v>
       </c>
       <c r="C87" t="n">
-        <v>-298040444.5277905</v>
+        <v>-339994952.0391277</v>
       </c>
       <c r="D87" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>159556139.6523196</v>
+        <v>175345729.4866427</v>
       </c>
       <c r="C88" t="n">
-        <v>-338145521.0098385</v>
+        <v>-384061060.8133995</v>
       </c>
       <c r="D88" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>133547828.5310905</v>
+        <v>146502757.7926936</v>
       </c>
       <c r="C89" t="n">
-        <v>-303836046.3182639</v>
+        <v>-344758883.299296</v>
       </c>
       <c r="D89" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>152283664.1886912</v>
+        <v>167242000.9383193</v>
       </c>
       <c r="C90" t="n">
-        <v>-330938589.2846747</v>
+        <v>-375661303.1838116</v>
       </c>
       <c r="D90" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>133188057.8410134</v>
+        <v>146107433.2747386</v>
       </c>
       <c r="C91" t="n">
-        <v>-303147861.3758538</v>
+        <v>-343984453.2498943</v>
       </c>
       <c r="D91" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>148270735.1169394</v>
+        <v>163027691.5202828</v>
       </c>
       <c r="C92" t="n">
-        <v>-314006239.1560445</v>
+        <v>-357102970.5766314</v>
       </c>
       <c r="D92" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>132326280.4560874</v>
+        <v>145163761.412155</v>
       </c>
       <c r="C93" t="n">
-        <v>-301332364.7394353</v>
+        <v>-341950282.646686</v>
       </c>
       <c r="D93" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>133186820.3860261</v>
+        <v>146106070.3657063</v>
       </c>
       <c r="C94" t="n">
-        <v>-303145652.0372005</v>
+        <v>-343981958.4603933</v>
       </c>
       <c r="D94" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>132393994.8824257</v>
+        <v>145236516.9337514</v>
       </c>
       <c r="C95" t="n">
-        <v>-301545098.7286289</v>
+        <v>-342185209.7142633</v>
       </c>
       <c r="D95" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>158370105.7030456</v>
+        <v>174417455.1786292</v>
       </c>
       <c r="C96" t="n">
-        <v>-317524795.5387079</v>
+        <v>-361763899.8096648</v>
       </c>
       <c r="D96" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>137142253.7138787</v>
+        <v>150488769.5229253</v>
       </c>
       <c r="C97" t="n">
-        <v>-308841030.0071481</v>
+        <v>-350489125.6051613</v>
       </c>
       <c r="D97" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>158762612.8352239</v>
+        <v>174685214.2444675</v>
       </c>
       <c r="C98" t="n">
-        <v>-326218674.1676497</v>
+        <v>-371161827.429689</v>
       </c>
       <c r="D98" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>166557395.5412509</v>
+        <v>183027153.3954354</v>
       </c>
       <c r="C99" t="n">
-        <v>-350828214.6929647</v>
+        <v>-398304096.20701</v>
       </c>
       <c r="D99" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>161864592.474834</v>
+        <v>177875726.8900353</v>
       </c>
       <c r="C100" t="n">
-        <v>-342494323.4409122</v>
+        <v>-388938340.3141993</v>
       </c>
       <c r="D100" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>185912412.2909386</v>
+        <v>204881926.3042796</v>
       </c>
       <c r="C101" t="n">
-        <v>-352339609.3305225</v>
+        <v>-401406145.3559777</v>
       </c>
       <c r="D101" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>141352485.3882477</v>
+        <v>155191114.5808477</v>
       </c>
       <c r="C102" t="n">
-        <v>-312930112.7904053</v>
+        <v>-355292618.2369412</v>
       </c>
       <c r="D102" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>153369349.7000767</v>
+        <v>168454782.819856</v>
       </c>
       <c r="C103" t="n">
-        <v>-331885890.8858885</v>
+        <v>-376778827.9801158</v>
       </c>
       <c r="D103" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>158134275.1538757</v>
+        <v>173823790.5060866</v>
       </c>
       <c r="C104" t="n">
-        <v>-333627310.9737434</v>
+        <v>-379078533.6399823</v>
       </c>
       <c r="D104" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>144420944.0583858</v>
+        <v>158649347.8485456</v>
       </c>
       <c r="C105" t="n">
-        <v>-314299043.6368001</v>
+        <v>-357058245.9717941</v>
       </c>
       <c r="D105" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>195960828.5914616</v>
+        <v>215477869.4761059</v>
       </c>
       <c r="C106" t="n">
-        <v>-390970843.5513169</v>
+        <v>-443840774.1791457</v>
       </c>
       <c r="D106" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>175859555.1756639</v>
+        <v>193605458.9487942</v>
       </c>
       <c r="C107" t="n">
-        <v>-348190757.0122535</v>
+        <v>-396208703.2234319</v>
       </c>
       <c r="D107" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>140639105.5325498</v>
+        <v>154362617.2944604</v>
       </c>
       <c r="C108" t="n">
-        <v>-313833282.4795468</v>
+        <v>-356190944.6612768</v>
       </c>
       <c r="D108" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>163555015.9934095</v>
+        <v>180291008.6988493</v>
       </c>
       <c r="C109" t="n">
-        <v>-317730700.4146501</v>
+        <v>-362396142.4748845</v>
       </c>
       <c r="D109" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>131829548.5578723</v>
+        <v>144707166.1204096</v>
       </c>
       <c r="C110" t="n">
-        <v>-295935671.3722316</v>
+        <v>-336115776.506285</v>
       </c>
       <c r="D110" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>156634251.2094057</v>
+        <v>172562586.5021156</v>
       </c>
       <c r="C111" t="n">
-        <v>-311991914.7384276</v>
+        <v>-355657459.2583444</v>
       </c>
       <c r="D111" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>167670165.5312662</v>
+        <v>184243193.7140671</v>
       </c>
       <c r="C112" t="n">
-        <v>-353066820.298147</v>
+        <v>-400806347.6736974</v>
       </c>
       <c r="D112" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>134124177.6926021</v>
+        <v>147234855.1512612</v>
       </c>
       <c r="C113" t="n">
-        <v>-300005557.9198745</v>
+        <v>-340712388.8009353</v>
       </c>
       <c r="D113" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>133905416.5137617</v>
+        <v>146990999.9065391</v>
       </c>
       <c r="C114" t="n">
-        <v>-299761365.7542637</v>
+        <v>-340428419.8543003</v>
       </c>
       <c r="D114" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>189752920.4501799</v>
+        <v>208612885.8890111</v>
       </c>
       <c r="C115" t="n">
-        <v>-383696858.5584973</v>
+        <v>-435544368.7334982</v>
       </c>
       <c r="D115" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>156894333.2309652</v>
+        <v>172783613.9201464</v>
       </c>
       <c r="C116" t="n">
-        <v>-315577009.9073716</v>
+        <v>-359543283.5497022</v>
       </c>
       <c r="D116" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>157278467.8209096</v>
+        <v>173094687.9409666</v>
       </c>
       <c r="C117" t="n">
-        <v>-321661930.9312663</v>
+        <v>-366130196.9417008</v>
       </c>
       <c r="D117" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>181492026.8387491</v>
+        <v>199901069.712983</v>
       </c>
       <c r="C118" t="n">
-        <v>-351779561.8086059</v>
+        <v>-400495481.0954574</v>
       </c>
       <c r="D118" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>158654562.4475776</v>
+        <v>174446068.6922322</v>
       </c>
       <c r="C119" t="n">
-        <v>-332007778.8960634</v>
+        <v>-377382254.8228981</v>
       </c>
       <c r="D119" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>138590394.9895089</v>
+        <v>152159195.7339974</v>
       </c>
       <c r="C120" t="n">
-        <v>-307612979.354601</v>
+        <v>-349317352.6426048</v>
       </c>
       <c r="D120" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>133185990.8395032</v>
+        <v>146105156.7191732</v>
       </c>
       <c r="C121" t="n">
-        <v>-303144170.9692506</v>
+        <v>-343980286.0355747</v>
       </c>
       <c r="D121" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>132580669.0374985</v>
+        <v>145532119.3097029</v>
       </c>
       <c r="C122" t="n">
-        <v>-297392959.7766616</v>
+        <v>-337754673.5134249</v>
       </c>
       <c r="D122" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>133511768.317774</v>
+        <v>146559077.26057</v>
       </c>
       <c r="C123" t="n">
-        <v>-298980260.4610214</v>
+        <v>-339551071.5546962</v>
       </c>
       <c r="D123" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>168895924.6174865</v>
+        <v>185991746.6059622</v>
       </c>
       <c r="C124" t="n">
-        <v>-334874479.5921599</v>
+        <v>-381310169.031873</v>
       </c>
       <c r="D124" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>135980696.7712135</v>
+        <v>149300435.5431648</v>
       </c>
       <c r="C125" t="n">
-        <v>-302259460.6362427</v>
+        <v>-343316069.9764515</v>
       </c>
       <c r="D125" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>156055763.8399591</v>
+        <v>171759520.7805586</v>
       </c>
       <c r="C126" t="n">
-        <v>-319124905.5774159</v>
+        <v>-363294876.5467163</v>
       </c>
       <c r="D126" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>148894692.201322</v>
+        <v>164179708.8762757</v>
       </c>
       <c r="C127" t="n">
-        <v>-292750297.2836502</v>
+        <v>-334272069.4907164</v>
       </c>
       <c r="D127" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>133184779.6796461</v>
+        <v>146103822.7710653</v>
       </c>
       <c r="C128" t="n">
-        <v>-303142008.564218</v>
+        <v>-343977844.2435759</v>
       </c>
       <c r="D128" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>157709961.4847255</v>
+        <v>173524953.7705133</v>
       </c>
       <c r="C129" t="n">
-        <v>-324568981.0597339</v>
+        <v>-369296591.3128704</v>
       </c>
       <c r="D129" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>136535760.4980252</v>
+        <v>150093582.6407307</v>
       </c>
       <c r="C130" t="n">
-        <v>-294347993.0635681</v>
+        <v>-334881638.4605334</v>
       </c>
       <c r="D130" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>149732268.4740105</v>
+        <v>164644845.9614159</v>
       </c>
       <c r="C131" t="n">
-        <v>-316086388.4335951</v>
+        <v>-359471649.7862512</v>
       </c>
       <c r="D131" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>134889794.6426065</v>
+        <v>148092572.1163859</v>
       </c>
       <c r="C132" t="n">
-        <v>-300646322.6606014</v>
+        <v>-341476733.6014692</v>
       </c>
       <c r="D132" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>132864678.2326166</v>
+        <v>145751268.7090042</v>
       </c>
       <c r="C133" t="n">
-        <v>-302570221.9648896</v>
+        <v>-343332181.0003771</v>
       </c>
       <c r="D133" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>152280106.6002271</v>
+        <v>167353296.446941</v>
       </c>
       <c r="C134" t="n">
-        <v>-325158468.1114321</v>
+        <v>-369452708.6856144</v>
       </c>
       <c r="D134" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>159279825.8139072</v>
+        <v>175635569.0176877</v>
       </c>
       <c r="C135" t="n">
-        <v>-308512725.8769764</v>
+        <v>-352113570.1714678</v>
       </c>
       <c r="D135" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>140463547.6134146</v>
+        <v>154234866.3832964</v>
       </c>
       <c r="C136" t="n">
-        <v>-310251056.9035797</v>
+        <v>-352331683.1804975</v>
       </c>
       <c r="D136" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>155355626.9989494</v>
+        <v>170961964.344333</v>
       </c>
       <c r="C137" t="n">
-        <v>-319283793.2341586</v>
+        <v>-363406251.8609104</v>
       </c>
       <c r="D137" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>146482371.0578764</v>
+        <v>160998294.1591468</v>
       </c>
       <c r="C138" t="n">
-        <v>-313926944.2323142</v>
+        <v>-356852929.6655133</v>
       </c>
       <c r="D138" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>177658724.1819302</v>
+        <v>195235366.8572239</v>
       </c>
       <c r="C139" t="n">
-        <v>-368915994.1828201</v>
+        <v>-418685689.6050323</v>
       </c>
       <c r="D139" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>162261097.3869281</v>
+        <v>178365368.1568178</v>
       </c>
       <c r="C140" t="n">
-        <v>-340454572.3690091</v>
+        <v>-386779148.4048932</v>
       </c>
       <c r="D140" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>134416284.8910971</v>
+        <v>147557676.9639913</v>
       </c>
       <c r="C141" t="n">
-        <v>-300469559.7393534</v>
+        <v>-341239417.732734</v>
       </c>
       <c r="D141" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>164979926.9176007</v>
+        <v>181742739.278066</v>
       </c>
       <c r="C142" t="n">
-        <v>-325686176.3676955</v>
+        <v>-371093105.9075913</v>
       </c>
       <c r="D142" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>155434422.7048624</v>
+        <v>171072718.0131552</v>
       </c>
       <c r="C143" t="n">
-        <v>-318239233.6028578</v>
+        <v>-362288434.8619813</v>
       </c>
       <c r="D143" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>140488008.7864806</v>
+        <v>154709747.7508927</v>
       </c>
       <c r="C144" t="n">
-        <v>-288631722.7400994</v>
+        <v>-329108008.4755627</v>
       </c>
       <c r="D144" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>180469151.9710608</v>
+        <v>198973136.2673399</v>
       </c>
       <c r="C145" t="n">
-        <v>-340246412.4500048</v>
+        <v>-387953808.8120714</v>
       </c>
       <c r="D145" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>135273482.2421477</v>
+        <v>148496643.4106728</v>
       </c>
       <c r="C146" t="n">
-        <v>-302242974.9294235</v>
+        <v>-343227336.4894173</v>
       </c>
       <c r="D146" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>160201540.2584676</v>
+        <v>176049458.4380625</v>
       </c>
       <c r="C147" t="n">
-        <v>-339546457.0315033</v>
+        <v>-385623779.9402081</v>
       </c>
       <c r="D147" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>190124677.2012815</v>
+        <v>209577588.5162029</v>
       </c>
       <c r="C148" t="n">
-        <v>-355283189.0850319</v>
+        <v>-404868845.1667185</v>
       </c>
       <c r="D148" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>160612346.5819714</v>
+        <v>176563204.0407186</v>
       </c>
       <c r="C149" t="n">
-        <v>-337121517.7568866</v>
+        <v>-383052071.8705349</v>
       </c>
       <c r="D149" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>143562825.7276157</v>
+        <v>157656053.941559</v>
       </c>
       <c r="C150" t="n">
-        <v>-315222775.6070763</v>
+        <v>-357967292.9949096</v>
       </c>
       <c r="D150" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>157286568.1629081</v>
+        <v>173051305.9311978</v>
       </c>
       <c r="C151" t="n">
-        <v>-324247018.6740065</v>
+        <v>-368913931.3081833</v>
       </c>
       <c r="D151" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>193692536.7711925</v>
+        <v>212987548.821132</v>
       </c>
       <c r="C152" t="n">
-        <v>-387386853.8541706</v>
+        <v>-439811680.9397057</v>
       </c>
       <c r="D152" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>164184943.0664755</v>
+        <v>180472693.4205935</v>
       </c>
       <c r="C153" t="n">
-        <v>-344101784.2502127</v>
+        <v>-390866973.8515606</v>
       </c>
       <c r="D153" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>141499581.2481183</v>
+        <v>155366805.7476073</v>
       </c>
       <c r="C154" t="n">
-        <v>-312502448.8642993</v>
+        <v>-354848267.3969677</v>
       </c>
       <c r="D154" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>179374978.14723</v>
+        <v>197529149.6283872</v>
       </c>
       <c r="C155" t="n">
-        <v>-350749944.9179873</v>
+        <v>-399231200.7597978</v>
       </c>
       <c r="D155" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>138669240.9957263</v>
+        <v>152261403.9513881</v>
       </c>
       <c r="C156" t="n">
-        <v>-306987520.5271319</v>
+        <v>-348654332.7064639</v>
       </c>
       <c r="D156" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>172370145.7890951</v>
+        <v>189921480.4639137</v>
       </c>
       <c r="C157" t="n">
-        <v>-334988174.8863518</v>
+        <v>-381695488.9446354</v>
       </c>
       <c r="D157" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>158047362.4552254</v>
+        <v>174238536.8289784</v>
       </c>
       <c r="C158" t="n">
-        <v>-308478310.5134187</v>
+        <v>-351980271.3902979</v>
       </c>
       <c r="D158" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>136034211.1299297</v>
+        <v>149332075.0377696</v>
       </c>
       <c r="C159" t="n">
-        <v>-303707503.5453642</v>
+        <v>-344874158.5573787</v>
       </c>
       <c r="D159" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>190018661.6349129</v>
+        <v>209463127.6167037</v>
       </c>
       <c r="C160" t="n">
-        <v>-355019272.5760236</v>
+        <v>-404576236.2368556</v>
       </c>
       <c r="D160" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>175674117.4082528</v>
+        <v>193659538.2536888</v>
       </c>
       <c r="C161" t="n">
-        <v>-334936743.4465915</v>
+        <v>-381878480.4215465</v>
       </c>
       <c r="D161" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>159862336.8049855</v>
+        <v>175684284.8110994</v>
       </c>
       <c r="C162" t="n">
-        <v>-338574060.1625065</v>
+        <v>-384548648.3668092</v>
       </c>
       <c r="D162" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>172501839.5428112</v>
+        <v>190028725.4410807</v>
       </c>
       <c r="C163" t="n">
-        <v>-337070218.076261</v>
+        <v>-383953683.3549007</v>
       </c>
       <c r="D163" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>140978618.3775643</v>
+        <v>154788871.3331739</v>
       </c>
       <c r="C164" t="n">
-        <v>-311806607.7948179</v>
+        <v>-354050828.7706164</v>
       </c>
       <c r="D164" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>176504865.0907648</v>
+        <v>194582024.5485584</v>
       </c>
       <c r="C165" t="n">
-        <v>-335774920.3028822</v>
+        <v>-382843275.13678</v>
       </c>
       <c r="D165" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>186579111.1927735</v>
+        <v>205556916.581247</v>
       </c>
       <c r="C166" t="n">
-        <v>-356316923.1990488</v>
+        <v>-405753450.7101246</v>
       </c>
       <c r="D166" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>140871400.795211</v>
+        <v>154673637.8066049</v>
       </c>
       <c r="C167" t="n">
-        <v>-311478364.8432201</v>
+        <v>-353688216.4667994</v>
       </c>
       <c r="D167" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>163430863.372584</v>
+        <v>179855582.7257683</v>
       </c>
       <c r="C168" t="n">
-        <v>-332212175.4115949</v>
+        <v>-378005023.1803816</v>
       </c>
       <c r="D168" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>185508470.2791307</v>
+        <v>204577518.467391</v>
       </c>
       <c r="C169" t="n">
-        <v>-344604991.2797332</v>
+        <v>-393006465.9111401</v>
       </c>
       <c r="D169" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>168769481.6174906</v>
+        <v>185942175.4822106</v>
       </c>
       <c r="C170" t="n">
-        <v>-330232150.1497709</v>
+        <v>-376290533.2306234</v>
       </c>
       <c r="D170" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>174362090.1054911</v>
+        <v>192200646.2860759</v>
       </c>
       <c r="C171" t="n">
-        <v>-333699826.9162512</v>
+        <v>-380448038.9242116</v>
       </c>
       <c r="D171" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>185345857.7778867</v>
+        <v>204155389.3190665</v>
       </c>
       <c r="C172" t="n">
-        <v>-356796154.4118779</v>
+        <v>-406187150.4298787</v>
       </c>
       <c r="D172" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>190360136.8154513</v>
+        <v>209849277.2294334</v>
       </c>
       <c r="C173" t="n">
-        <v>-354967632.5779494</v>
+        <v>-404542190.4131616</v>
       </c>
       <c r="D173" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>155689613.3434788</v>
+        <v>171295928.9319431</v>
       </c>
       <c r="C174" t="n">
-        <v>-321488368.2586542</v>
+        <v>-365807842.2032521</v>
       </c>
       <c r="D174" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>186277094.8049808</v>
+        <v>205407293.227101</v>
       </c>
       <c r="C175" t="n">
-        <v>-346526615.0679132</v>
+        <v>-395137526.4503912</v>
       </c>
       <c r="D175" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>188046861.7576432</v>
+        <v>207113192.5647068</v>
       </c>
       <c r="C176" t="n">
-        <v>-361483242.0999983</v>
+        <v>-411439776.1842504</v>
       </c>
       <c r="D176" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>157062556.0037677</v>
+        <v>172861881.9526828</v>
       </c>
       <c r="C177" t="n">
-        <v>-321069006.3031799</v>
+        <v>-365473495.6424588</v>
       </c>
       <c r="D177" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>161518848.3261522</v>
+        <v>177503431.6170017</v>
       </c>
       <c r="C178" t="n">
-        <v>-341509384.2953113</v>
+        <v>-387849263.6559094</v>
       </c>
       <c r="D178" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>160172432.4412201</v>
+        <v>176027139.2620924</v>
       </c>
       <c r="C179" t="n">
-        <v>-339007995.8900697</v>
+        <v>-385042346.1472824</v>
       </c>
       <c r="D179" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>178732917.1826238</v>
+        <v>196585217.1686349</v>
       </c>
       <c r="C180" t="n">
-        <v>-361906707.6826982</v>
+        <v>-411220011.7382769</v>
       </c>
       <c r="D180" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
optimizing variogram parameters for area 4
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,13 +528,13 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>155186282.5163826</v>
+        <v>241116409.9288566</v>
       </c>
       <c r="C2" t="n">
-        <v>-355284140.737343</v>
+        <v>-640516451.8613</v>
       </c>
       <c r="D2" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -642,13 +642,13 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>196544314.2725931</v>
+        <v>307840143.1691962</v>
       </c>
       <c r="C3" t="n">
-        <v>-411636476.3766083</v>
+        <v>-744780978.6235237</v>
       </c>
       <c r="D3" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -756,13 +756,13 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>173130360.6929421</v>
+        <v>271851828.2804081</v>
       </c>
       <c r="C4" t="n">
-        <v>-366720078.5053295</v>
+        <v>-668097385.7077036</v>
       </c>
       <c r="D4" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -874,13 +874,13 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>155939419.7333016</v>
+        <v>242120270.0446654</v>
       </c>
       <c r="C5" t="n">
-        <v>-358115531.9229566</v>
+        <v>-644936176.4713304</v>
       </c>
       <c r="D5" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -988,13 +988,13 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>155767778.4642669</v>
+        <v>241816006.3231841</v>
       </c>
       <c r="C6" t="n">
-        <v>-358083241.6631406</v>
+        <v>-644771741.2745878</v>
       </c>
       <c r="D6" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1102,13 +1102,13 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>180665283.8416124</v>
+        <v>281822355.0883852</v>
       </c>
       <c r="C7" t="n">
-        <v>-394532657.9500122</v>
+        <v>-711558460.5956467</v>
       </c>
       <c r="D7" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1212,13 +1212,13 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>155987577.3472792</v>
+        <v>242249524.6977128</v>
       </c>
       <c r="C8" t="n">
-        <v>-357768108.1902798</v>
+        <v>-644492121.4329234</v>
       </c>
       <c r="D8" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1326,13 +1326,13 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>173755454.4975769</v>
+        <v>272620302.1461084</v>
       </c>
       <c r="C9" t="n">
-        <v>-369476857.1464744</v>
+        <v>-672338783.942363</v>
       </c>
       <c r="D9" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1444,13 +1444,13 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>152508113.2399762</v>
+        <v>236537929.2857987</v>
       </c>
       <c r="C10" t="n">
-        <v>-353371208.2346841</v>
+        <v>-636000231.6287237</v>
       </c>
       <c r="D10" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1562,13 +1562,13 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>174057455.4525982</v>
+        <v>273356708.5186262</v>
       </c>
       <c r="C11" t="n">
-        <v>-367915076.6274578</v>
+        <v>-670332549.0772539</v>
       </c>
       <c r="D11" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1676,13 +1676,13 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>205731289.6267988</v>
+        <v>324139109.2556922</v>
       </c>
       <c r="C12" t="n">
-        <v>-410386550.8987644</v>
+        <v>-747799482.7227929</v>
       </c>
       <c r="D12" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1786,13 +1786,13 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>189006844.5387366</v>
+        <v>296404406.2602804</v>
       </c>
       <c r="C13" t="n">
-        <v>-396237483.7314262</v>
+        <v>-718866741.0923098</v>
       </c>
       <c r="D13" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1892,13 +1892,13 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>150967007.5884917</v>
+        <v>234421992.9689757</v>
       </c>
       <c r="C14" t="n">
-        <v>-348045753.5317158</v>
+        <v>-627593821.3777303</v>
       </c>
       <c r="D14" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2006,13 +2006,13 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>163499715.651751</v>
+        <v>258153912.6522675</v>
       </c>
       <c r="C15" t="n">
-        <v>-339018591.0933486</v>
+        <v>-623356145.7801745</v>
       </c>
       <c r="D15" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2116,13 +2116,13 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>206684949.9050232</v>
+        <v>325883524.4871363</v>
       </c>
       <c r="C16" t="n">
-        <v>-409780567.1759447</v>
+        <v>-747398630.4843992</v>
       </c>
       <c r="D16" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2230,13 +2230,13 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>193082177.3012131</v>
+        <v>303097785.9272359</v>
       </c>
       <c r="C17" t="n">
-        <v>-400409682.3877724</v>
+        <v>-727024925.2444966</v>
       </c>
       <c r="D17" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2340,13 +2340,13 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>199552338.6221488</v>
+        <v>312636899.8738974</v>
       </c>
       <c r="C18" t="n">
-        <v>-415778194.4573804</v>
+        <v>-752270474.6464767</v>
       </c>
       <c r="D18" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2454,13 +2454,13 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>208679123.9730402</v>
+        <v>329811766.0912105</v>
       </c>
       <c r="C19" t="n">
-        <v>-406167113.4694846</v>
+        <v>-743155717.4879633</v>
       </c>
       <c r="D19" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2560,13 +2560,13 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>155305325.9332242</v>
+        <v>241284616.1454389</v>
       </c>
       <c r="C20" t="n">
-        <v>-355654206.5168758</v>
+        <v>-641108597.9145137</v>
       </c>
       <c r="D20" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2674,13 +2674,13 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>211544535.3069784</v>
+        <v>334170860.8161556</v>
       </c>
       <c r="C21" t="n">
-        <v>-411533388.5074365</v>
+        <v>-752220211.8294635</v>
       </c>
       <c r="D21" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2784,13 +2784,13 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>201565592.8729976</v>
+        <v>318489476.4800459</v>
       </c>
       <c r="C22" t="n">
-        <v>-396766276.2385935</v>
+        <v>-726238810.2783819</v>
       </c>
       <c r="D22" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -2890,13 +2890,13 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>155196801.0224651</v>
+        <v>240947429.0625636</v>
       </c>
       <c r="C23" t="n">
-        <v>-356807367.5218722</v>
+        <v>-642618118.4559122</v>
       </c>
       <c r="D23" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -2996,13 +2996,13 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>155570487.5770514</v>
+        <v>241537608.1774869</v>
       </c>
       <c r="C24" t="n">
-        <v>-357465986.4543495</v>
+        <v>-643785192.149943</v>
       </c>
       <c r="D24" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3110,13 +3110,13 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>200722434.247045</v>
+        <v>316028303.5171236</v>
       </c>
       <c r="C25" t="n">
-        <v>-404768673.6249115</v>
+        <v>-737261747.7522157</v>
       </c>
       <c r="D25" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -3224,13 +3224,13 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>185996213.297362</v>
+        <v>292111793.1974413</v>
       </c>
       <c r="C26" t="n">
-        <v>-387800921.8206634</v>
+        <v>-705272189.3632073</v>
       </c>
       <c r="D26" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -3334,13 +3334,13 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>155051228.0084344</v>
+        <v>240803556.7309235</v>
       </c>
       <c r="C27" t="n">
-        <v>-355852353.1976787</v>
+        <v>-641203341.7830828</v>
       </c>
       <c r="D27" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -3448,13 +3448,13 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>190663678.7888838</v>
+        <v>301625905.0998349</v>
       </c>
       <c r="C28" t="n">
-        <v>-377827853.5778434</v>
+        <v>-693639299.8900316</v>
       </c>
       <c r="D28" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -3562,13 +3562,13 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>164829680.2202438</v>
+        <v>259524364.4675499</v>
       </c>
       <c r="C29" t="n">
-        <v>-346844092.1084408</v>
+        <v>-635159537.19867</v>
       </c>
       <c r="D29" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -3672,13 +3672,13 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>203317294.4936355</v>
+        <v>321125162.8406616</v>
       </c>
       <c r="C30" t="n">
-        <v>-400357657.6337687</v>
+        <v>-732246856.0965803</v>
       </c>
       <c r="D30" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -3778,13 +3778,13 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>200726084.2348005</v>
+        <v>316034106.6327591</v>
       </c>
       <c r="C31" t="n">
-        <v>-404773712.7128288</v>
+        <v>-737270796.7957494</v>
       </c>
       <c r="D31" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -3892,13 +3892,13 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>155003677.0435953</v>
+        <v>240675486.9111191</v>
       </c>
       <c r="C32" t="n">
-        <v>-356198184.1442469</v>
+        <v>-641645409.746622</v>
       </c>
       <c r="D32" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -4006,13 +4006,13 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>197775388.6890371</v>
+        <v>309591520.6783481</v>
       </c>
       <c r="C33" t="n">
-        <v>-415096549.5071747</v>
+        <v>-750338693.3007903</v>
       </c>
       <c r="D33" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -4116,13 +4116,13 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>155361373.2639571</v>
+        <v>241180851.5727562</v>
       </c>
       <c r="C34" t="n">
-        <v>-357312835.8907093</v>
+        <v>-643428200.0245736</v>
       </c>
       <c r="D34" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -4230,13 +4230,13 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>207902554.2738627</v>
+        <v>328636380.8735353</v>
       </c>
       <c r="C35" t="n">
-        <v>-404657525.0644075</v>
+        <v>-740617600.2250655</v>
       </c>
       <c r="D35" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -4340,13 +4340,13 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>206054635.0396705</v>
+        <v>324854430.5347658</v>
       </c>
       <c r="C36" t="n">
-        <v>-409159008.4394572</v>
+        <v>-746200833.3122867</v>
       </c>
       <c r="D36" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -4458,13 +4458,13 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>166384437.3759427</v>
+        <v>261924235.3221091</v>
       </c>
       <c r="C37" t="n">
-        <v>-349876582.6575621</v>
+        <v>-640369267.1781435</v>
       </c>
       <c r="D37" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -4568,13 +4568,13 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>168851319.6347371</v>
+        <v>266105340.8550061</v>
       </c>
       <c r="C38" t="n">
-        <v>-351767591.9995821</v>
+        <v>-644524175.3137047</v>
       </c>
       <c r="D38" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -4682,13 +4682,13 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>150795742.9964098</v>
+        <v>233692973.6274313</v>
       </c>
       <c r="C39" t="n">
-        <v>-351461103.3519568</v>
+        <v>-632156415.2001097</v>
       </c>
       <c r="D39" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -4800,13 +4800,13 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>154453493.7807354</v>
+        <v>239958332.6812091</v>
       </c>
       <c r="C40" t="n">
-        <v>-353997140.5139248</v>
+        <v>-638233803.9230567</v>
       </c>
       <c r="D40" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -4918,13 +4918,13 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>200613129.3372485</v>
+        <v>315871578.7534108</v>
       </c>
       <c r="C41" t="n">
-        <v>-404477807.3599414</v>
+        <v>-736791243.5112112</v>
       </c>
       <c r="D41" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -5032,13 +5032,13 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>153427588.5896657</v>
+        <v>238081039.3346827</v>
       </c>
       <c r="C42" t="n">
-        <v>-354264931.2292031</v>
+        <v>-637879350.5167651</v>
       </c>
       <c r="D42" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -5150,13 +5150,13 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>153095851.8690318</v>
+        <v>237917772.9119691</v>
       </c>
       <c r="C43" t="n">
-        <v>-350757250.7678999</v>
+        <v>-632825810.5677013</v>
       </c>
       <c r="D43" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -5264,13 +5264,13 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>172893903.4587503</v>
+        <v>271453178.3149346</v>
       </c>
       <c r="C44" t="n">
-        <v>-366531568.0279778</v>
+        <v>-667689887.1368873</v>
       </c>
       <c r="D44" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -5382,13 +5382,13 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>147215120.8201736</v>
+        <v>228517245.6278447</v>
       </c>
       <c r="C45" t="n">
-        <v>-341137333.3318655</v>
+        <v>-615422880.303871</v>
       </c>
       <c r="D45" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -5500,13 +5500,13 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>156059212.2187155</v>
+        <v>242289512.9431651</v>
       </c>
       <c r="C46" t="n">
-        <v>-358488457.7172877</v>
+        <v>-645532582.8692462</v>
       </c>
       <c r="D46" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -5610,13 +5610,13 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>153225320.3627685</v>
+        <v>237611354.9062354</v>
       </c>
       <c r="C47" t="n">
-        <v>-355129047.8733214</v>
+        <v>-638922073.3417053</v>
       </c>
       <c r="D47" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -5728,13 +5728,13 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>153617755.9656588</v>
+        <v>238716552.1387896</v>
       </c>
       <c r="C48" t="n">
-        <v>-351887747.4773654</v>
+        <v>-634747027.1713309</v>
       </c>
       <c r="D48" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -5842,13 +5842,13 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>204712543.8454991</v>
+        <v>322745359.7031357</v>
       </c>
       <c r="C49" t="n">
-        <v>-407149119.8925413</v>
+        <v>-742664354.0434316</v>
       </c>
       <c r="D49" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -5956,13 +5956,13 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>155920833.5419316</v>
+        <v>242277238.6826189</v>
       </c>
       <c r="C50" t="n">
-        <v>-356571491.1156015</v>
+        <v>-642799677.7142836</v>
       </c>
       <c r="D50" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -6066,13 +6066,13 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>175430197.5408969</v>
+        <v>277669410.9749006</v>
       </c>
       <c r="C51" t="n">
-        <v>-353391190.5228757</v>
+        <v>-650638472.9506352</v>
       </c>
       <c r="D51" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -6180,13 +6180,13 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>182296023.1598229</v>
+        <v>284453677.0661486</v>
       </c>
       <c r="C52" t="n">
-        <v>-396699916.2584975</v>
+        <v>-715576330.4317623</v>
       </c>
       <c r="D52" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -6290,13 +6290,13 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>193632434.3363308</v>
+        <v>303309631.9706399</v>
       </c>
       <c r="C53" t="n">
-        <v>-406642287.6299921</v>
+        <v>-736125207.7363403</v>
       </c>
       <c r="D53" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -6404,13 +6404,13 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>147553207.4215885</v>
+        <v>229115395.803687</v>
       </c>
       <c r="C54" t="n">
-        <v>-341231416.4951763</v>
+        <v>-615796001.4970576</v>
       </c>
       <c r="D54" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -6522,13 +6522,13 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>154941086.9860992</v>
+        <v>240709029.5342582</v>
       </c>
       <c r="C55" t="n">
-        <v>-355014700.9734443</v>
+        <v>-639974477.0186136</v>
       </c>
       <c r="D55" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -6636,13 +6636,13 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>192574674.3692023</v>
+        <v>302373980.5765743</v>
       </c>
       <c r="C56" t="n">
-        <v>-399000870.056523</v>
+        <v>-724754887.8731717</v>
       </c>
       <c r="D56" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -6746,13 +6746,13 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>146069419.9447235</v>
+        <v>226115473.4363479</v>
       </c>
       <c r="C57" t="n">
-        <v>-343863818.213274</v>
+        <v>-618321946.9817134</v>
       </c>
       <c r="D57" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -6856,13 +6856,13 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>184087436.2332685</v>
+        <v>287378257.0332168</v>
       </c>
       <c r="C58" t="n">
-        <v>-398781818.7649365</v>
+        <v>-719565294.9595512</v>
       </c>
       <c r="D58" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -6966,13 +6966,13 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>168049193.5427126</v>
+        <v>264899440.4536139</v>
       </c>
       <c r="C59" t="n">
-        <v>-349970129.3104186</v>
+        <v>-641513779.7746129</v>
       </c>
       <c r="D59" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -7080,13 +7080,13 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>178420228.5645504</v>
+        <v>278445845.2283827</v>
       </c>
       <c r="C60" t="n">
-        <v>-389507600.1477705</v>
+        <v>-703174320.3226094</v>
       </c>
       <c r="D60" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -7190,13 +7190,13 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>201027362.5022249</v>
+        <v>313956072.1801931</v>
       </c>
       <c r="C61" t="n">
-        <v>-426438833.8456725</v>
+        <v>-768109334.7570126</v>
       </c>
       <c r="D61" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -7300,13 +7300,13 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>204710353.5541095</v>
+        <v>322741874.7063678</v>
       </c>
       <c r="C62" t="n">
-        <v>-407146185.1421992</v>
+        <v>-742659074.352662</v>
       </c>
       <c r="D62" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -7414,13 +7414,13 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>166695692.4632627</v>
+        <v>263258404.8438024</v>
       </c>
       <c r="C63" t="n">
-        <v>-343911712.2507417</v>
+        <v>-632173952.7290845</v>
       </c>
       <c r="D63" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -7528,13 +7528,13 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>180629424.1221489</v>
+        <v>281833903.6966872</v>
       </c>
       <c r="C64" t="n">
-        <v>-393915056.3532701</v>
+        <v>-710675747.4114839</v>
       </c>
       <c r="D64" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -7646,13 +7646,13 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>167083811.2216147</v>
+        <v>259864791.7006577</v>
       </c>
       <c r="C65" t="n">
-        <v>-376200657.5862347</v>
+        <v>-677451073.353865</v>
       </c>
       <c r="D65" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -7760,13 +7760,13 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>176436617.1285712</v>
+        <v>279469335.2922495</v>
       </c>
       <c r="C66" t="n">
-        <v>-353371076.6943061</v>
+        <v>-651169910.9945309</v>
       </c>
       <c r="D66" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -7874,13 +7874,13 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>182297675.2594912</v>
+        <v>284456288.9917687</v>
       </c>
       <c r="C67" t="n">
-        <v>-396702546.3344389</v>
+        <v>-715581003.6488818</v>
       </c>
       <c r="D67" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -7988,13 +7988,13 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>164844380.8782575</v>
+        <v>259723469.9714658</v>
       </c>
       <c r="C68" t="n">
-        <v>-345513688.5489202</v>
+        <v>-633302860.1094917</v>
       </c>
       <c r="D68" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -8102,13 +8102,13 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>164908082.2140847</v>
+        <v>261164753.2626413</v>
       </c>
       <c r="C69" t="n">
-        <v>-335405353.3376096</v>
+        <v>-619107805.3630104</v>
       </c>
       <c r="D69" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -8216,13 +8216,13 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>172931203.1371433</v>
+        <v>272777273.7243389</v>
       </c>
       <c r="C70" t="n">
-        <v>-356680798.8871456</v>
+        <v>-653863315.1116563</v>
       </c>
       <c r="D70" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -8326,13 +8326,13 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>194029018.9871371</v>
+        <v>305892356.1042734</v>
       </c>
       <c r="C71" t="n">
-        <v>-391290253.1933777</v>
+        <v>-714595899.8409623</v>
       </c>
       <c r="D71" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -8436,13 +8436,13 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>155307796.3672507</v>
+        <v>241288520.0071773</v>
       </c>
       <c r="C72" t="n">
-        <v>-355658541.6282188</v>
+        <v>-641116285.9121094</v>
       </c>
       <c r="D72" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -8550,13 +8550,13 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>200723417.3590471</v>
+        <v>316029866.5670241</v>
       </c>
       <c r="C73" t="n">
-        <v>-404770030.8939012</v>
+        <v>-737264185.0951921</v>
       </c>
       <c r="D73" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -8664,13 +8664,13 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>178540398.2998848</v>
+        <v>279681540.434641</v>
       </c>
       <c r="C74" t="n">
-        <v>-381222269.6195494</v>
+        <v>-691676297.3159117</v>
       </c>
       <c r="D74" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -8774,13 +8774,13 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>153756347.5309934</v>
+        <v>238606731.4384664</v>
       </c>
       <c r="C75" t="n">
-        <v>-354795176.0726953</v>
+        <v>-638839898.102951</v>
       </c>
       <c r="D75" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -8892,13 +8892,13 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>209393291.6337691</v>
+        <v>330076763.9282188</v>
       </c>
       <c r="C76" t="n">
-        <v>-414314745.135057</v>
+        <v>-755208195.1460632</v>
       </c>
       <c r="D76" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -9006,13 +9006,13 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>189952042.4358481</v>
+        <v>299439780.3822055</v>
       </c>
       <c r="C77" t="n">
-        <v>-385228080.9502848</v>
+        <v>-703812662.4923407</v>
       </c>
       <c r="D77" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -9120,13 +9120,13 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>159427739.3415537</v>
+        <v>251216849.3362035</v>
       </c>
       <c r="C78" t="n">
-        <v>-335982549.9278293</v>
+        <v>-616569650.678416</v>
       </c>
       <c r="D78" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -9234,13 +9234,13 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>146104165.8187904</v>
+        <v>226164033.8365528</v>
       </c>
       <c r="C79" t="n">
-        <v>-343978472.1932865</v>
+        <v>-618504264.9674021</v>
       </c>
       <c r="D79" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -9348,13 +9348,13 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>184093496.6619012</v>
+        <v>287387840.2114912</v>
       </c>
       <c r="C80" t="n">
-        <v>-398791383.9021803</v>
+        <v>-719582297.4409394</v>
       </c>
       <c r="D80" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -9458,13 +9458,13 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>181466019.6913999</v>
+        <v>283149053.8281337</v>
       </c>
       <c r="C81" t="n">
-        <v>-395314256.5035633</v>
+        <v>-713138153.5136787</v>
       </c>
       <c r="D81" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -9572,13 +9572,13 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>182832422.7411771</v>
+        <v>285278721.9658185</v>
       </c>
       <c r="C82" t="n">
-        <v>-397742156.952522</v>
+        <v>-717356056.9629877</v>
       </c>
       <c r="D82" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -9686,13 +9686,13 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>187043943.8371796</v>
+        <v>295826005.8928929</v>
       </c>
       <c r="C83" t="n">
-        <v>-372992014.8445476</v>
+        <v>-684845866.2343649</v>
       </c>
       <c r="D83" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -9796,13 +9796,13 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>171859151.1753787</v>
+        <v>272014231.2749047</v>
       </c>
       <c r="C84" t="n">
-        <v>-347768652.5221396</v>
+        <v>-640643632.4785765</v>
       </c>
       <c r="D84" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -9906,13 +9906,13 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>203434052.6487181</v>
+        <v>320789113.3239766</v>
       </c>
       <c r="C85" t="n">
-        <v>-404790327.899222</v>
+        <v>-738656926.3217984</v>
       </c>
       <c r="D85" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -10016,13 +10016,13 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>183274862.4207279</v>
+        <v>285970464.894981</v>
       </c>
       <c r="C86" t="n">
-        <v>-398508414.7768783</v>
+        <v>-718693340.5180732</v>
       </c>
       <c r="D86" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -10130,13 +10130,13 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>164326832.2141601</v>
+        <v>259513822.2850575</v>
       </c>
       <c r="C87" t="n">
-        <v>-339994952.0391277</v>
+        <v>-625232380.7979548</v>
       </c>
       <c r="D87" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -10244,13 +10244,13 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>175345729.4866427</v>
+        <v>273641607.671856</v>
       </c>
       <c r="C88" t="n">
-        <v>-384061060.8133995</v>
+        <v>-693677903.9160447</v>
       </c>
       <c r="D88" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -10354,13 +10354,13 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>146502757.7926936</v>
+        <v>226786550.2516718</v>
       </c>
       <c r="C89" t="n">
-        <v>-344758883.299296</v>
+        <v>-619864072.960627</v>
       </c>
       <c r="D89" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -10464,13 +10464,13 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>167242000.9383193</v>
+        <v>260213516.9754689</v>
       </c>
       <c r="C90" t="n">
-        <v>-375661303.1838116</v>
+        <v>-676810304.4705592</v>
       </c>
       <c r="D90" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -10578,13 +10578,13 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>146107433.2747386</v>
+        <v>226169188.3207233</v>
       </c>
       <c r="C91" t="n">
-        <v>-343984453.2498943</v>
+        <v>-618514843.849395</v>
       </c>
       <c r="D91" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -10696,13 +10696,13 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>163027691.5202828</v>
+        <v>254974684.4502476</v>
       </c>
       <c r="C92" t="n">
-        <v>-357102970.5766314</v>
+        <v>-648327480.5640734</v>
       </c>
       <c r="D92" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -10810,13 +10810,13 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>145163761.412155</v>
+        <v>224717828.7056844</v>
       </c>
       <c r="C93" t="n">
-        <v>-341950282.646686</v>
+        <v>-615039144.3747218</v>
       </c>
       <c r="D93" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -10920,13 +10920,13 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>146106070.3657063</v>
+        <v>226167038.3015949</v>
       </c>
       <c r="C94" t="n">
-        <v>-343981958.4603933</v>
+        <v>-618510431.2372736</v>
       </c>
       <c r="D94" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -11030,13 +11030,13 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>145236516.9337514</v>
+        <v>224820170.6684155</v>
       </c>
       <c r="C95" t="n">
-        <v>-342185209.7142633</v>
+        <v>-615413964.9004151</v>
       </c>
       <c r="D95" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -11140,13 +11140,13 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>174417455.1786292</v>
+        <v>274781804.7242188</v>
       </c>
       <c r="C96" t="n">
-        <v>-361763899.8096648</v>
+        <v>-661899490.7891164</v>
       </c>
       <c r="D96" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -11250,13 +11250,13 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>150488769.5229253</v>
+        <v>233259970.1339031</v>
       </c>
       <c r="C97" t="n">
-        <v>-350489125.6051613</v>
+        <v>-630603626.1936203</v>
       </c>
       <c r="D97" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -11368,13 +11368,13 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>174685214.2444675</v>
+        <v>274067975.5643117</v>
       </c>
       <c r="C98" t="n">
-        <v>-371161827.429689</v>
+        <v>-675262354.2216074</v>
       </c>
       <c r="D98" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -11482,13 +11482,13 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>183027153.3954354</v>
+        <v>285555902.5664799</v>
       </c>
       <c r="C99" t="n">
-        <v>-398304096.20701</v>
+        <v>-718258134.6457069</v>
       </c>
       <c r="D99" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -11596,13 +11596,13 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>177875726.8900353</v>
+        <v>277547055.5154095</v>
       </c>
       <c r="C100" t="n">
-        <v>-388938340.3141993</v>
+        <v>-702044307.992703</v>
       </c>
       <c r="D100" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -11706,13 +11706,13 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>204881926.3042796</v>
+        <v>323741591.2967488</v>
       </c>
       <c r="C101" t="n">
-        <v>-401406145.3559777</v>
+        <v>-734507953.3498362</v>
       </c>
       <c r="D101" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -11820,13 +11820,13 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>155191114.5808477</v>
+        <v>241124046.2670941</v>
       </c>
       <c r="C102" t="n">
-        <v>-355292618.2369412</v>
+        <v>-640531487.5712001</v>
       </c>
       <c r="D102" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -11934,13 +11934,13 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>168454782.819856</v>
+        <v>262243332.2856171</v>
       </c>
       <c r="C103" t="n">
-        <v>-376778827.9801158</v>
+        <v>-679154550.8067428</v>
       </c>
       <c r="D103" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -12052,13 +12052,13 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>173823790.5060866</v>
+        <v>271543321.4000739</v>
       </c>
       <c r="C104" t="n">
-        <v>-379078533.6399823</v>
+        <v>-685788883.8156843</v>
       </c>
       <c r="D104" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -12166,13 +12166,13 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>158649347.8485456</v>
+        <v>247118332.88347</v>
       </c>
       <c r="C105" t="n">
-        <v>-357058245.9717941</v>
+        <v>-645348511.1651821</v>
       </c>
       <c r="D105" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -12280,13 +12280,13 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>215477869.4761059</v>
+        <v>337201433.0136378</v>
       </c>
       <c r="C106" t="n">
-        <v>-443840774.1791457</v>
+        <v>-800345615.03389</v>
       </c>
       <c r="D106" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -12394,13 +12394,13 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>193605458.9487942</v>
+        <v>304537376.5776873</v>
       </c>
       <c r="C107" t="n">
-        <v>-396208703.2234319</v>
+        <v>-721360980.5391968</v>
       </c>
       <c r="D107" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -12508,13 +12508,13 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>154362617.2944604</v>
+        <v>239524588.7008033</v>
       </c>
       <c r="C108" t="n">
-        <v>-356190944.6612768</v>
+        <v>-641184656.1507736</v>
       </c>
       <c r="D108" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -12622,13 +12622,13 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>180291008.6988493</v>
+        <v>285177471.3559144</v>
       </c>
       <c r="C109" t="n">
-        <v>-362396142.4748845</v>
+        <v>-666124678.5824778</v>
       </c>
       <c r="D109" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -12736,13 +12736,13 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>144707166.1204096</v>
+        <v>224615062.5923977</v>
       </c>
       <c r="C110" t="n">
-        <v>-336115776.506285</v>
+        <v>-606717622.250353</v>
       </c>
       <c r="D110" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -12854,13 +12854,13 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>172562586.5021156</v>
+        <v>272249754.7655263</v>
       </c>
       <c r="C111" t="n">
-        <v>-355657459.2583444</v>
+        <v>-652204163.8814831</v>
       </c>
       <c r="D111" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -12964,13 +12964,13 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>184243193.7140671</v>
+        <v>287408714.7674247</v>
       </c>
       <c r="C112" t="n">
-        <v>-400806347.6736974</v>
+        <v>-722485408.0931526</v>
       </c>
       <c r="D112" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -13074,13 +13074,13 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>147234855.1512612</v>
+        <v>228605661.3841797</v>
       </c>
       <c r="C113" t="n">
-        <v>-340712388.8009353</v>
+        <v>-614854348.7632763</v>
       </c>
       <c r="D113" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -13192,13 +13192,13 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>146990999.9065391</v>
+        <v>228201033.2161114</v>
       </c>
       <c r="C114" t="n">
-        <v>-340428419.8543003</v>
+        <v>-614288686.2252672</v>
       </c>
       <c r="D114" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -13310,13 +13310,13 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>208612885.8890111</v>
+        <v>326181861.1804546</v>
       </c>
       <c r="C115" t="n">
-        <v>-435544368.7334982</v>
+        <v>-785049507.6016762</v>
       </c>
       <c r="D115" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -13416,13 +13416,13 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>172783613.9201464</v>
+        <v>272145706.4409218</v>
       </c>
       <c r="C116" t="n">
-        <v>-359543283.5497022</v>
+        <v>-657809791.884734</v>
       </c>
       <c r="D116" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -13526,13 +13526,13 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>173094687.9409666</v>
+        <v>271862757.4238549</v>
       </c>
       <c r="C117" t="n">
-        <v>-366130196.9417008</v>
+        <v>-667248888.2380273</v>
       </c>
       <c r="D117" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -13644,13 +13644,13 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>199901069.712983</v>
+        <v>315105951.0574893</v>
       </c>
       <c r="C118" t="n">
-        <v>-400495481.0954574</v>
+        <v>-730747426.1765029</v>
       </c>
       <c r="D118" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -13754,13 +13754,13 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>174446068.6922322</v>
+        <v>272863476.7660523</v>
       </c>
       <c r="C119" t="n">
-        <v>-377382254.8228981</v>
+        <v>-683812167.8925201</v>
       </c>
       <c r="D119" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -13860,13 +13860,13 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>152159195.7339974</v>
+        <v>236410689.9844101</v>
       </c>
       <c r="C120" t="n">
-        <v>-349317352.6426048</v>
+        <v>-630186134.2139621</v>
       </c>
       <c r="D120" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -13970,13 +13970,13 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>146105156.7191732</v>
+        <v>226165597.0039313</v>
       </c>
       <c r="C121" t="n">
-        <v>-343980286.0355747</v>
+        <v>-618507473.1671422</v>
       </c>
       <c r="D121" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -14084,13 +14084,13 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>145532119.3097029</v>
+        <v>225900681.1727424</v>
       </c>
       <c r="C122" t="n">
-        <v>-337754673.5134249</v>
+        <v>-609564829.8951237</v>
       </c>
       <c r="D122" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -14202,13 +14202,13 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>146559077.26057</v>
+        <v>227530799.8906835</v>
       </c>
       <c r="C123" t="n">
-        <v>-339551071.5546962</v>
+        <v>-612773015.4131714</v>
       </c>
       <c r="D123" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -14320,13 +14320,13 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>185991746.6059622</v>
+        <v>292912636.687263</v>
       </c>
       <c r="C124" t="n">
-        <v>-381310169.031873</v>
+        <v>-696098767.0576134</v>
       </c>
       <c r="D124" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -14426,13 +14426,13 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>149300435.5431648</v>
+        <v>232006809.2622156</v>
       </c>
       <c r="C125" t="n">
-        <v>-343316069.9764515</v>
+        <v>-619910906.2042223</v>
       </c>
       <c r="D125" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -14536,13 +14536,13 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>171759520.7805586</v>
+        <v>269835674.2570578</v>
       </c>
       <c r="C126" t="n">
-        <v>-363294876.5467163</v>
+        <v>-662465103.058249</v>
       </c>
       <c r="D126" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -14650,13 +14650,13 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>164179708.8762757</v>
+        <v>260004362.5773549</v>
       </c>
       <c r="C127" t="n">
-        <v>-334272069.4907164</v>
+        <v>-617075096.1658553</v>
       </c>
       <c r="D127" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -14768,13 +14768,13 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>146103822.7710653</v>
+        <v>226163492.6711283</v>
       </c>
       <c r="C128" t="n">
-        <v>-343977844.2435759</v>
+        <v>-618503154.2930305</v>
       </c>
       <c r="D128" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -14878,13 +14878,13 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>173524953.7705133</v>
+        <v>272231389.1081073</v>
       </c>
       <c r="C129" t="n">
-        <v>-369296591.3128704</v>
+        <v>-671946254.9176275</v>
       </c>
       <c r="D129" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -14992,13 +14992,13 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>150093582.6407307</v>
+        <v>234504158.7149849</v>
       </c>
       <c r="C130" t="n">
-        <v>-334881638.4605334</v>
+        <v>-608853674.238616</v>
       </c>
       <c r="D130" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -15106,13 +15106,13 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>164644845.9614159</v>
+        <v>257577191.2416937</v>
       </c>
       <c r="C131" t="n">
-        <v>-359471649.7862512</v>
+        <v>-652668699.3305537</v>
       </c>
       <c r="D131" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -15220,13 +15220,13 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>148092572.1163859</v>
+        <v>230057768.3387714</v>
       </c>
       <c r="C132" t="n">
-        <v>-341476733.6014692</v>
+        <v>-616520724.873842</v>
       </c>
       <c r="D132" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -15334,13 +15334,13 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>145751268.7090042</v>
+        <v>225607327.2208885</v>
       </c>
       <c r="C133" t="n">
-        <v>-343332181.0003771</v>
+        <v>-617361142.6686318</v>
       </c>
       <c r="D133" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -15444,13 +15444,13 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>167353296.446941</v>
+        <v>261178897.8119061</v>
       </c>
       <c r="C134" t="n">
-        <v>-369452708.6856144</v>
+        <v>-668284335.5192387</v>
       </c>
       <c r="D134" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -15562,13 +15562,13 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>175635569.0176877</v>
+        <v>278202125.5705481</v>
       </c>
       <c r="C135" t="n">
-        <v>-352113570.1714678</v>
+        <v>-648938013.488188</v>
       </c>
       <c r="D135" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -15676,13 +15676,13 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>154234866.3832964</v>
+        <v>239771508.8132858</v>
       </c>
       <c r="C136" t="n">
-        <v>-352331683.1804975</v>
+        <v>-635790051.9050461</v>
       </c>
       <c r="D136" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -15790,13 +15790,13 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>170961964.344333</v>
+        <v>268395005.4511626</v>
       </c>
       <c r="C137" t="n">
-        <v>-363406251.8609104</v>
+        <v>-662134595.8958046</v>
       </c>
       <c r="D137" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -15904,13 +15904,13 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>160998294.1591468</v>
+        <v>251362684.6463775</v>
       </c>
       <c r="C138" t="n">
-        <v>-356852929.6655133</v>
+        <v>-646644373.9702441</v>
       </c>
       <c r="D138" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -16014,13 +16014,13 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>195235366.8572239</v>
+        <v>304686586.0029499</v>
       </c>
       <c r="C139" t="n">
-        <v>-418685689.6050323</v>
+        <v>-753959532.9839897</v>
       </c>
       <c r="D139" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -16128,13 +16128,13 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>178365368.1568178</v>
+        <v>278683013.3011628</v>
       </c>
       <c r="C140" t="n">
-        <v>-386779148.4048932</v>
+        <v>-699336737.2919977</v>
       </c>
       <c r="D140" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -16238,13 +16238,13 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>147557676.9639913</v>
+        <v>229122462.9280137</v>
       </c>
       <c r="C141" t="n">
-        <v>-341239417.732734</v>
+        <v>-615810200.1162999</v>
       </c>
       <c r="D141" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -16356,13 +16356,13 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>181742739.278066</v>
+        <v>286652264.0822604</v>
       </c>
       <c r="C142" t="n">
-        <v>-371093105.9075913</v>
+        <v>-679269130.0227554</v>
       </c>
       <c r="D142" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -16466,13 +16466,13 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>171072718.0131552</v>
+        <v>268735102.2271433</v>
       </c>
       <c r="C143" t="n">
-        <v>-362288434.8619813</v>
+        <v>-660636716.3574395</v>
       </c>
       <c r="D143" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -16584,13 +16584,13 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>154709747.7508927</v>
+        <v>243601156.586562</v>
       </c>
       <c r="C144" t="n">
-        <v>-329108008.4755627</v>
+        <v>-603939255.377998</v>
       </c>
       <c r="D144" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -16698,13 +16698,13 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>198973136.2673399</v>
+        <v>315019437.858991</v>
       </c>
       <c r="C145" t="n">
-        <v>-387953808.8120714</v>
+        <v>-712316144.3485979</v>
       </c>
       <c r="D145" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -16808,13 +16808,13 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>148496643.4106728</v>
+        <v>230568678.7818459</v>
       </c>
       <c r="C146" t="n">
-        <v>-343227336.4894173</v>
+        <v>-619213379.4449077</v>
       </c>
       <c r="D146" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -16926,13 +16926,13 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>176049458.4380625</v>
+        <v>274703017.1193153</v>
       </c>
       <c r="C147" t="n">
-        <v>-385623779.9402081</v>
+        <v>-696292944.7845743</v>
       </c>
       <c r="D147" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -17036,13 +17036,13 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>209577588.5162029</v>
+        <v>331539974.7603281</v>
       </c>
       <c r="C148" t="n">
-        <v>-404868845.1667185</v>
+        <v>-741698511.2020931</v>
       </c>
       <c r="D148" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -17150,13 +17150,13 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>176563204.0407186</v>
+        <v>275934405.7071202</v>
       </c>
       <c r="C149" t="n">
-        <v>-383052071.8705349</v>
+        <v>-693029384.238608</v>
       </c>
       <c r="D149" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -17260,13 +17260,13 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>157656053.941559</v>
+        <v>245221390.8877693</v>
       </c>
       <c r="C150" t="n">
-        <v>-357967292.9949096</v>
+        <v>-645922673.169723</v>
       </c>
       <c r="D150" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -17370,13 +17370,13 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>173051305.9311978</v>
+        <v>271433622.9273621</v>
       </c>
       <c r="C151" t="n">
-        <v>-368913931.3081833</v>
+        <v>-671121900.1209217</v>
       </c>
       <c r="D151" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -17484,13 +17484,13 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>212987548.821132</v>
+        <v>333327753.5744264</v>
       </c>
       <c r="C152" t="n">
-        <v>-439811680.9397057</v>
+        <v>-793362759.6305578</v>
       </c>
       <c r="D152" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -17590,13 +17590,13 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>180472693.4205935</v>
+        <v>281927973.9961489</v>
       </c>
       <c r="C153" t="n">
-        <v>-390866973.8515606</v>
+        <v>-706328223.660036</v>
       </c>
       <c r="D153" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -17704,13 +17704,13 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>155366805.7476073</v>
+        <v>241494785.4813281</v>
       </c>
       <c r="C154" t="n">
-        <v>-354848267.3969677</v>
+        <v>-640042740.3329711</v>
       </c>
       <c r="D154" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -17814,13 +17814,13 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>197529149.6283872</v>
+        <v>311085736.1148545</v>
       </c>
       <c r="C155" t="n">
-        <v>-399231200.7597978</v>
+        <v>-727727749.3847228</v>
       </c>
       <c r="D155" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -17928,13 +17928,13 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>152261403.9513881</v>
+        <v>236677036.0213428</v>
       </c>
       <c r="C156" t="n">
-        <v>-348654332.7064639</v>
+        <v>-629346904.2296659</v>
       </c>
       <c r="D156" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -18038,13 +18038,13 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>189921480.4639137</v>
+        <v>299827188.9903314</v>
       </c>
       <c r="C157" t="n">
-        <v>-381695488.9446354</v>
+        <v>-698771109.8942244</v>
       </c>
       <c r="D157" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -18148,13 +18148,13 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>174238536.8289784</v>
+        <v>275722938.950241</v>
       </c>
       <c r="C158" t="n">
-        <v>-351980271.3902979</v>
+        <v>-647966189.414601</v>
       </c>
       <c r="D158" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -18262,13 +18262,13 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>149332075.0377696</v>
+        <v>231870099.3434019</v>
       </c>
       <c r="C159" t="n">
-        <v>-344874158.5573787</v>
+        <v>-622072620.8410587</v>
       </c>
       <c r="D159" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -18376,13 +18376,13 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>209463127.6167037</v>
+        <v>331375399.2707284</v>
       </c>
       <c r="C160" t="n">
-        <v>-404576236.2368556</v>
+        <v>-741223418.8351234</v>
       </c>
       <c r="D160" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -18490,13 +18490,13 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>193659538.2536888</v>
+        <v>306411760.0856024</v>
       </c>
       <c r="C161" t="n">
-        <v>-381878480.4215465</v>
+        <v>-700964540.7794162</v>
       </c>
       <c r="D161" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -18604,13 +18604,13 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>175684284.8110994</v>
+        <v>274184724.1137281</v>
       </c>
       <c r="C162" t="n">
-        <v>-384548648.3668092</v>
+        <v>-694568373.8249217</v>
       </c>
       <c r="D162" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -18718,13 +18718,13 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>190028725.4410807</v>
+        <v>299734528.2315714</v>
       </c>
       <c r="C163" t="n">
-        <v>-383953683.3549007</v>
+        <v>-702042015.4739696</v>
       </c>
       <c r="D163" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -18828,13 +18828,13 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>154788871.3331739</v>
+        <v>240554629.3470742</v>
       </c>
       <c r="C164" t="n">
-        <v>-354050828.7706164</v>
+        <v>-638542346.5098919</v>
       </c>
       <c r="D164" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -18938,13 +18938,13 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>194582024.5485584</v>
+        <v>307919216.6758572</v>
       </c>
       <c r="C165" t="n">
-        <v>-382843275.13678</v>
+        <v>-702811392.4851085</v>
       </c>
       <c r="D165" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -19052,13 +19052,13 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>205556916.581247</v>
+        <v>324395347.8652229</v>
       </c>
       <c r="C166" t="n">
-        <v>-405753450.7101246</v>
+        <v>-741076423.4641184</v>
       </c>
       <c r="D166" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -19162,13 +19162,13 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>154673637.8066049</v>
+        <v>240392358.7967031</v>
       </c>
       <c r="C167" t="n">
-        <v>-353688216.4667994</v>
+        <v>-637962998.1665426</v>
       </c>
       <c r="D167" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -19276,13 +19276,13 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>179855582.7257683</v>
+        <v>282423728.746169</v>
       </c>
       <c r="C168" t="n">
-        <v>-378005023.1803816</v>
+        <v>-687942724.5554985</v>
       </c>
       <c r="D168" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -19382,13 +19382,13 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>204577518.467391</v>
+        <v>324236869.8379742</v>
       </c>
       <c r="C169" t="n">
-        <v>-393006465.9111401</v>
+        <v>-722257016.7834637</v>
       </c>
       <c r="D169" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -19496,13 +19496,13 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>185942175.4822106</v>
+        <v>293455255.8377674</v>
       </c>
       <c r="C170" t="n">
-        <v>-376290533.2306234</v>
+        <v>-688952220.5230802</v>
       </c>
       <c r="D170" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -19606,13 +19606,13 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>192200646.2860759</v>
+        <v>304014132.5989069</v>
       </c>
       <c r="C171" t="n">
-        <v>-380448038.9242116</v>
+        <v>-698175436.5643777</v>
       </c>
       <c r="D171" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -19716,13 +19716,13 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>204155389.3190665</v>
+        <v>321884934.3653171</v>
       </c>
       <c r="C172" t="n">
-        <v>-406187150.4298787</v>
+        <v>-741012669.4637401</v>
       </c>
       <c r="D172" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -19830,13 +19830,13 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>209849277.2294334</v>
+        <v>332054352.0411416</v>
       </c>
       <c r="C173" t="n">
-        <v>-404542190.4131616</v>
+        <v>-741350897.6632477</v>
       </c>
       <c r="D173" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -19944,13 +19944,13 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>171295928.9319431</v>
+        <v>268688270.2184461</v>
       </c>
       <c r="C174" t="n">
-        <v>-365807842.2032521</v>
+        <v>-665700112.87985</v>
       </c>
       <c r="D174" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -20058,13 +20058,13 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>205407293.227101</v>
+        <v>325429242.7824501</v>
       </c>
       <c r="C175" t="n">
-        <v>-395137526.4503912</v>
+        <v>-725720479.2212398</v>
       </c>
       <c r="D175" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -20168,13 +20168,13 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>207113192.5647068</v>
+        <v>326432980.3894434</v>
       </c>
       <c r="C176" t="n">
-        <v>-411439776.1842504</v>
+        <v>-749984518.1305887</v>
       </c>
       <c r="D176" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -20274,13 +20274,13 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>172861881.9526828</v>
+        <v>271529942.5186161</v>
       </c>
       <c r="C177" t="n">
-        <v>-365473495.6424588</v>
+        <v>-666187380.9058965</v>
       </c>
       <c r="D177" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -20384,13 +20384,13 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>177503431.6170017</v>
+        <v>277018094.9322309</v>
       </c>
       <c r="C178" t="n">
-        <v>-387849263.6559094</v>
+        <v>-700296723.8155724</v>
       </c>
       <c r="D178" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -20498,13 +20498,13 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>176027139.2620924</v>
+        <v>274734659.9312125</v>
       </c>
       <c r="C179" t="n">
-        <v>-385042346.1472824</v>
+        <v>-695469769.7531233</v>
       </c>
       <c r="D179" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -20612,13 +20612,13 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>196585217.1686349</v>
+        <v>307962529.6169906</v>
       </c>
       <c r="C180" t="n">
-        <v>-411220011.7382769</v>
+        <v>-744215916.061385</v>
       </c>
       <c r="D180" t="n">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
optimizing variogram parameters for area 5
still have to look at these parameters, when changing the range, slightly better values could be obtained  for some PC's
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>241116409.9288566</v>
+        <v>422823.0001388173</v>
       </c>
       <c r="C2" t="n">
-        <v>-640516451.8613</v>
+        <v>7525442.527047326</v>
       </c>
       <c r="D2" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>307840143.1691962</v>
+        <v>451013.4314993119</v>
       </c>
       <c r="C3" t="n">
-        <v>-744780978.6235237</v>
+        <v>7286868.704686873</v>
       </c>
       <c r="D3" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>271851828.2804081</v>
+        <v>594545.9850944348</v>
       </c>
       <c r="C4" t="n">
-        <v>-668097385.7077036</v>
+        <v>7366095.350358819</v>
       </c>
       <c r="D4" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>242120270.0446654</v>
+        <v>403945.0768397648</v>
       </c>
       <c r="C5" t="n">
-        <v>-644936176.4713304</v>
+        <v>7527910.87798272</v>
       </c>
       <c r="D5" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>241816006.3231841</v>
+        <v>401216.148465685</v>
       </c>
       <c r="C6" t="n">
-        <v>-644771741.2745878</v>
+        <v>7529882.125589605</v>
       </c>
       <c r="D6" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>281822355.0883852</v>
+        <v>409155.6666583589</v>
       </c>
       <c r="C7" t="n">
-        <v>-711558460.5956467</v>
+        <v>7388267.661607112</v>
       </c>
       <c r="D7" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>242249524.6977128</v>
+        <v>408788.64986577</v>
       </c>
       <c r="C8" t="n">
-        <v>-644492121.4329234</v>
+        <v>7525883.127678607</v>
       </c>
       <c r="D8" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>272620302.1461084</v>
+        <v>573609.5498119397</v>
       </c>
       <c r="C9" t="n">
-        <v>-672338783.942363</v>
+        <v>7369187.59580075</v>
       </c>
       <c r="D9" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>236537929.2857987</v>
+        <v>395739.2028744464</v>
       </c>
       <c r="C10" t="n">
-        <v>-636000231.6287237</v>
+        <v>7550553.333618967</v>
       </c>
       <c r="D10" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>273356708.5186262</v>
+        <v>595482.5194309736</v>
       </c>
       <c r="C11" t="n">
-        <v>-670332549.0772539</v>
+        <v>7360555.884229297</v>
       </c>
       <c r="D11" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>324139109.2556922</v>
+        <v>570295.7162984037</v>
       </c>
       <c r="C12" t="n">
-        <v>-747799482.7227929</v>
+        <v>7194426.892189107</v>
       </c>
       <c r="D12" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>296404406.2602804</v>
+        <v>507596.7447241906</v>
       </c>
       <c r="C13" t="n">
-        <v>-718866741.0923098</v>
+        <v>7306910.773843632</v>
       </c>
       <c r="D13" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>234421992.9689757</v>
+        <v>429046.3551782307</v>
       </c>
       <c r="C14" t="n">
-        <v>-627593821.3777303</v>
+        <v>7547568.77555988</v>
       </c>
       <c r="D14" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>258153912.6522675</v>
+        <v>760472.461105651</v>
       </c>
       <c r="C15" t="n">
-        <v>-623356145.7801745</v>
+        <v>7374813.666059652</v>
       </c>
       <c r="D15" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>325883524.4871363</v>
+        <v>586409.6389365081</v>
       </c>
       <c r="C16" t="n">
-        <v>-747398630.4843992</v>
+        <v>7183700.825286468</v>
       </c>
       <c r="D16" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>303097785.9272359</v>
+        <v>518399.5160626545</v>
       </c>
       <c r="C17" t="n">
-        <v>-727024925.2444966</v>
+        <v>7280948.900331907</v>
       </c>
       <c r="D17" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>312636899.8738974</v>
+        <v>447691.7230347765</v>
       </c>
       <c r="C18" t="n">
-        <v>-752270474.6464767</v>
+        <v>7272079.333575497</v>
       </c>
       <c r="D18" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>329811766.0912105</v>
+        <v>641757.8655294247</v>
       </c>
       <c r="C19" t="n">
-        <v>-743155717.4879633</v>
+        <v>7154179.916507507</v>
       </c>
       <c r="D19" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>241284616.1454389</v>
+        <v>420719.6780329063</v>
       </c>
       <c r="C20" t="n">
-        <v>-641108597.9145137</v>
+        <v>7525508.513714559</v>
       </c>
       <c r="D20" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>334170860.8161556</v>
+        <v>620437.5570446817</v>
       </c>
       <c r="C21" t="n">
-        <v>-752220211.8294635</v>
+        <v>7145829.711649289</v>
       </c>
       <c r="D21" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>318489476.4800459</v>
+        <v>656030.3435174299</v>
       </c>
       <c r="C22" t="n">
-        <v>-726238810.2783819</v>
+        <v>7188356.034972786</v>
       </c>
       <c r="D22" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>240947429.0625636</v>
+        <v>405491.2708980456</v>
       </c>
       <c r="C23" t="n">
-        <v>-642618118.4559122</v>
+        <v>7531595.912204068</v>
       </c>
       <c r="D23" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>241537608.1774869</v>
+        <v>404713.2604548364</v>
       </c>
       <c r="C24" t="n">
-        <v>-643785192.149943</v>
+        <v>7529740.381576492</v>
       </c>
       <c r="D24" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>316028303.5171236</v>
+        <v>568072.7130961117</v>
       </c>
       <c r="C25" t="n">
-        <v>-737261747.7522157</v>
+        <v>7222234.914685098</v>
       </c>
       <c r="D25" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>292111793.1974413</v>
+        <v>553955.6541633958</v>
       </c>
       <c r="C26" t="n">
-        <v>-705272189.3632073</v>
+        <v>7307428.943578887</v>
       </c>
       <c r="D26" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>240803556.7309235</v>
+        <v>413821.4916065777</v>
       </c>
       <c r="C27" t="n">
-        <v>-641203341.7830828</v>
+        <v>7529429.834138079</v>
       </c>
       <c r="D27" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>301625905.0998349</v>
+        <v>718950.8143728292</v>
       </c>
       <c r="C28" t="n">
-        <v>-693639299.8900316</v>
+        <v>7229561.330213139</v>
       </c>
       <c r="D28" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>259524364.4675499</v>
+        <v>689479.0599372458</v>
       </c>
       <c r="C29" t="n">
-        <v>-635159537.19867</v>
+        <v>7385840.555939897</v>
       </c>
       <c r="D29" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>321125162.8406616</v>
+        <v>640364.9592321715</v>
       </c>
       <c r="C30" t="n">
-        <v>-732246856.0965803</v>
+        <v>7183844.981620431</v>
       </c>
       <c r="D30" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>316034106.6327591</v>
+        <v>568065.8525246648</v>
       </c>
       <c r="C31" t="n">
-        <v>-737270796.7957494</v>
+        <v>7222217.524079368</v>
       </c>
       <c r="D31" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>240675486.9111191</v>
+        <v>408978.8275499512</v>
       </c>
       <c r="C32" t="n">
-        <v>-641645409.746622</v>
+        <v>7531442.590570908</v>
       </c>
       <c r="D32" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>309591520.6783481</v>
+        <v>432660.8029019876</v>
       </c>
       <c r="C33" t="n">
-        <v>-750338693.3007903</v>
+        <v>7287266.453172042</v>
       </c>
       <c r="D33" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>241180851.5727562</v>
+        <v>402680.6572135365</v>
       </c>
       <c r="C34" t="n">
-        <v>-643428200.0245736</v>
+        <v>7531672.625937978</v>
       </c>
       <c r="D34" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>328636380.8735353</v>
+        <v>648062.4098775064</v>
       </c>
       <c r="C35" t="n">
-        <v>-740617600.2250655</v>
+        <v>7156317.765654799</v>
       </c>
       <c r="D35" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>324854430.5347658</v>
+        <v>585517.9007419647</v>
       </c>
       <c r="C36" t="n">
-        <v>-746200833.3122867</v>
+        <v>7187408.106334507</v>
       </c>
       <c r="D36" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>261924235.3221091</v>
+        <v>679482.7733917895</v>
       </c>
       <c r="C37" t="n">
-        <v>-640369267.1781435</v>
+        <v>7379568.764875205</v>
       </c>
       <c r="D37" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>266105340.8550061</v>
+        <v>697218.2558684414</v>
       </c>
       <c r="C38" t="n">
-        <v>-644524175.3137047</v>
+        <v>7360280.072632506</v>
       </c>
       <c r="D38" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>233692973.6274313</v>
+        <v>385901.2558721581</v>
       </c>
       <c r="C39" t="n">
-        <v>-632156415.2001097</v>
+        <v>7564001.44550652</v>
       </c>
       <c r="D39" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>239958332.6812091</v>
+        <v>424332.5844982759</v>
       </c>
       <c r="C40" t="n">
-        <v>-638233803.9230567</v>
+        <v>7529112.568427877</v>
       </c>
       <c r="D40" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>315871578.7534108</v>
+        <v>569643.0684379223</v>
       </c>
       <c r="C41" t="n">
-        <v>-736791243.5112112</v>
+        <v>7222285.613839785</v>
       </c>
       <c r="D41" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>238081039.3346827</v>
+        <v>402406.4354549267</v>
       </c>
       <c r="C42" t="n">
-        <v>-637879350.5167651</v>
+        <v>7542852.907356113</v>
       </c>
       <c r="D42" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>237917772.9119691</v>
+        <v>437023.185092857</v>
       </c>
       <c r="C43" t="n">
-        <v>-632825810.5677013</v>
+        <v>7532468.581112547</v>
       </c>
       <c r="D43" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>271453178.3149346</v>
+        <v>593001.3245233108</v>
       </c>
       <c r="C44" t="n">
-        <v>-667689887.1368873</v>
+        <v>7367918.094725985</v>
       </c>
       <c r="D44" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>228517245.6278447</v>
+        <v>439224.5486118381</v>
       </c>
       <c r="C45" t="n">
-        <v>-615422880.303871</v>
+        <v>7565894.75324164</v>
       </c>
       <c r="D45" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>242289512.9431651</v>
+        <v>401842.916054123</v>
       </c>
       <c r="C46" t="n">
-        <v>-645532582.8692462</v>
+        <v>7527990.288472353</v>
       </c>
       <c r="D46" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>237611354.9062354</v>
+        <v>388715.6373236501</v>
       </c>
       <c r="C47" t="n">
-        <v>-638922073.3417053</v>
+        <v>7548996.648429874</v>
       </c>
       <c r="D47" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>238716552.1387896</v>
+        <v>433477.7838170429</v>
       </c>
       <c r="C48" t="n">
-        <v>-634747027.1713309</v>
+        <v>7530698.264778861</v>
       </c>
       <c r="D48" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>322745359.7031357</v>
+        <v>590088.3297374767</v>
       </c>
       <c r="C49" t="n">
-        <v>-742664354.0434316</v>
+        <v>7193087.563682824</v>
       </c>
       <c r="D49" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>242277238.6826189</v>
+        <v>421309.4212496581</v>
       </c>
       <c r="C50" t="n">
-        <v>-642799677.7142836</v>
+        <v>7521773.247238778</v>
       </c>
       <c r="D50" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>277669410.9749006</v>
+        <v>778993.4381261227</v>
       </c>
       <c r="C51" t="n">
-        <v>-650638472.9506352</v>
+        <v>7299986.83529006</v>
       </c>
       <c r="D51" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>284453677.0661486</v>
+        <v>410340.4763310733</v>
       </c>
       <c r="C52" t="n">
-        <v>-715576330.4317623</v>
+        <v>7378952.937187641</v>
       </c>
       <c r="D52" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>303309631.9706399</v>
+        <v>463408.7043260257</v>
       </c>
       <c r="C53" t="n">
-        <v>-736125207.7363403</v>
+        <v>7297853.838466587</v>
       </c>
       <c r="D53" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>229115395.803687</v>
+        <v>444667.0044273772</v>
       </c>
       <c r="C54" t="n">
-        <v>-615796001.4970576</v>
+        <v>7562048.963216691</v>
       </c>
       <c r="D54" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>240709029.5342582</v>
+        <v>421470.9503357491</v>
       </c>
       <c r="C55" t="n">
-        <v>-639974477.0186136</v>
+        <v>7527329.485975892</v>
       </c>
       <c r="D55" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>302373980.5765743</v>
+        <v>526067.6630022393</v>
       </c>
       <c r="C56" t="n">
-        <v>-724754887.8731717</v>
+        <v>7281008.696502964</v>
       </c>
       <c r="D56" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>226115473.4363479</v>
+        <v>384404.2276939754</v>
       </c>
       <c r="C57" t="n">
-        <v>-618321946.9817134</v>
+        <v>7591962.608249241</v>
       </c>
       <c r="D57" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>287378257.0332168</v>
+        <v>414448.1731552719</v>
       </c>
       <c r="C58" t="n">
-        <v>-719565294.9595512</v>
+        <v>7367681.028654348</v>
       </c>
       <c r="D58" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>264899440.4536139</v>
+        <v>705283.5520898863</v>
       </c>
       <c r="C59" t="n">
-        <v>-641513779.7746129</v>
+        <v>7362709.877786176</v>
       </c>
       <c r="D59" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>278445845.2283827</v>
+        <v>428504.0728901725</v>
       </c>
       <c r="C60" t="n">
-        <v>-703174320.3226094</v>
+        <v>7393290.601893418</v>
       </c>
       <c r="D60" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>313956072.1801931</v>
+        <v>364167.4705087786</v>
       </c>
       <c r="C61" t="n">
-        <v>-768109334.7570126</v>
+        <v>7297116.842234123</v>
       </c>
       <c r="D61" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>322741874.7063678</v>
+        <v>590092.4094163297</v>
       </c>
       <c r="C62" t="n">
-        <v>-742659074.352662</v>
+        <v>7193098.011324367</v>
       </c>
       <c r="D62" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>263258404.8438024</v>
+        <v>754559.5701349006</v>
       </c>
       <c r="C63" t="n">
-        <v>-632173952.7290845</v>
+        <v>7357457.446217685</v>
       </c>
       <c r="D63" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>281833903.6966872</v>
+        <v>415018.0448537197</v>
       </c>
       <c r="C64" t="n">
-        <v>-710675747.4114839</v>
+        <v>7386252.235449532</v>
       </c>
       <c r="D64" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>259864791.7006577</v>
+        <v>393866.9952033143</v>
       </c>
       <c r="C65" t="n">
-        <v>-677451073.353865</v>
+        <v>7468780.921490044</v>
       </c>
       <c r="D65" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>279469335.2922495</v>
+        <v>793848.6559708756</v>
       </c>
       <c r="C66" t="n">
-        <v>-651169910.9945309</v>
+        <v>7290260.126774631</v>
       </c>
       <c r="D66" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>284456288.9917687</v>
+        <v>410337.1139574873</v>
       </c>
       <c r="C67" t="n">
-        <v>-715581003.6488818</v>
+        <v>7378945.240007831</v>
       </c>
       <c r="D67" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>259723469.9714658</v>
+        <v>705411.5012919909</v>
       </c>
       <c r="C68" t="n">
-        <v>-633302860.1094917</v>
+        <v>7381384.438635441</v>
       </c>
       <c r="D68" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>261164753.2626413</v>
+        <v>827178.5078480255</v>
       </c>
       <c r="C69" t="n">
-        <v>-619107805.3630104</v>
+        <v>7350027.173207692</v>
       </c>
       <c r="D69" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>272777273.7243389</v>
+        <v>704315.0658106438</v>
       </c>
       <c r="C70" t="n">
-        <v>-653863315.1116563</v>
+        <v>7334696.005952516</v>
       </c>
       <c r="D70" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>305892356.1042734</v>
+        <v>622134.3892227954</v>
       </c>
       <c r="C71" t="n">
-        <v>-714595899.8409623</v>
+        <v>7240708.73367288</v>
       </c>
       <c r="D71" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>241288520.0071773</v>
+        <v>420714.5822642142</v>
       </c>
       <c r="C72" t="n">
-        <v>-641116285.9121094</v>
+        <v>7525496.171109289</v>
       </c>
       <c r="D72" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>316029866.5670241</v>
+        <v>568070.8652271603</v>
       </c>
       <c r="C73" t="n">
-        <v>-737264185.0951921</v>
+        <v>7222230.230568401</v>
       </c>
       <c r="D73" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>279681540.434641</v>
+        <v>517897.6597152865</v>
       </c>
       <c r="C74" t="n">
-        <v>-691676297.3159117</v>
+        <v>7360848.522584329</v>
       </c>
       <c r="D74" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>238606731.4384664</v>
+        <v>402334.5145603271</v>
       </c>
       <c r="C75" t="n">
-        <v>-638839898.102951</v>
+        <v>7540991.602727064</v>
       </c>
       <c r="D75" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>330076763.9282188</v>
+        <v>572359.5505096086</v>
       </c>
       <c r="C76" t="n">
-        <v>-755208195.1460632</v>
+        <v>7174025.31142854</v>
       </c>
       <c r="D76" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>299439780.3822055</v>
+        <v>632953.2160392514</v>
       </c>
       <c r="C77" t="n">
-        <v>-703812662.4923407</v>
+        <v>7259778.363588417</v>
       </c>
       <c r="D77" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>251216849.3362035</v>
+        <v>727838.3447125108</v>
       </c>
       <c r="C78" t="n">
-        <v>-616569650.678416</v>
+        <v>7407376.859851267</v>
       </c>
       <c r="D78" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>226164033.8365528</v>
+        <v>383725.8459431626</v>
       </c>
       <c r="C79" t="n">
-        <v>-618504264.9674021</v>
+        <v>7592006.341748471</v>
       </c>
       <c r="D79" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>287387840.2114912</v>
+        <v>414435.8746544203</v>
       </c>
       <c r="C80" t="n">
-        <v>-719582297.4409394</v>
+        <v>7367652.856344703</v>
       </c>
       <c r="D80" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>283149053.8281337</v>
+        <v>412673.4235208518</v>
       </c>
       <c r="C81" t="n">
-        <v>-713138153.5136787</v>
+        <v>7382581.441586836</v>
       </c>
       <c r="D81" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>285278721.9658185</v>
+        <v>407314.2720218997</v>
       </c>
       <c r="C82" t="n">
-        <v>-717356056.9629877</v>
+        <v>7377190.661707142</v>
       </c>
       <c r="D82" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>295826005.8928929</v>
+        <v>723787.2073493205</v>
       </c>
       <c r="C83" t="n">
-        <v>-684845866.2343649</v>
+        <v>7248572.024052578</v>
       </c>
       <c r="D83" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>272014231.2749047</v>
+        <v>790262.1937427302</v>
       </c>
       <c r="C84" t="n">
-        <v>-640643632.4785765</v>
+        <v>7317937.23898467</v>
       </c>
       <c r="D84" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>320789113.3239766</v>
+        <v>598663.1839319061</v>
       </c>
       <c r="C85" t="n">
-        <v>-738656926.3217984</v>
+        <v>7197091.63736374</v>
       </c>
       <c r="D85" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>285970464.894981</v>
+        <v>405767.7027150932</v>
       </c>
       <c r="C86" t="n">
-        <v>-718693340.5180732</v>
+        <v>7375381.027371443</v>
       </c>
       <c r="D86" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>259513822.2850575</v>
+        <v>762480.8616364233</v>
       </c>
       <c r="C87" t="n">
-        <v>-625232380.7979548</v>
+        <v>7369402.187121131</v>
       </c>
       <c r="D87" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>273641607.671856</v>
+        <v>439843.9287411383</v>
       </c>
       <c r="C88" t="n">
-        <v>-693677903.9160447</v>
+        <v>7406029.903836646</v>
       </c>
       <c r="D88" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>226786550.2516718</v>
+        <v>382271.6480455336</v>
       </c>
       <c r="C89" t="n">
-        <v>-619864072.960627</v>
+        <v>7590211.624238232</v>
       </c>
       <c r="D89" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>260213516.9754689</v>
+        <v>402335.643714165</v>
       </c>
       <c r="C90" t="n">
-        <v>-676810304.4705592</v>
+        <v>7464744.675496253</v>
       </c>
       <c r="D90" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>226169188.3207233</v>
+        <v>383718.8813232478</v>
       </c>
       <c r="C91" t="n">
-        <v>-618514843.849395</v>
+        <v>7591989.812414211</v>
       </c>
       <c r="D91" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>254974684.4502476</v>
+        <v>539831.0236638299</v>
       </c>
       <c r="C92" t="n">
-        <v>-648327480.5640734</v>
+        <v>7440963.848228727</v>
       </c>
       <c r="D92" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>224717828.7056844</v>
+        <v>389353.0613288408</v>
       </c>
       <c r="C93" t="n">
-        <v>-615039144.3747218</v>
+        <v>7595463.263758845</v>
       </c>
       <c r="D93" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>226167038.3015949</v>
+        <v>383721.7863796732</v>
       </c>
       <c r="C94" t="n">
-        <v>-618510431.2372736</v>
+        <v>7591996.707043167</v>
       </c>
       <c r="D94" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>224820170.6684155</v>
+        <v>387990.2999005239</v>
       </c>
       <c r="C95" t="n">
-        <v>-615413964.9004151</v>
+        <v>7595529.493387843</v>
       </c>
       <c r="D95" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>274781804.7242188</v>
+        <v>669452.4467849245</v>
       </c>
       <c r="C96" t="n">
-        <v>-661899490.7891164</v>
+        <v>7336131.153987038</v>
       </c>
       <c r="D96" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>233259970.1339031</v>
+        <v>391429.212175432</v>
       </c>
       <c r="C97" t="n">
-        <v>-630603626.1936203</v>
+        <v>7563757.379410667</v>
       </c>
       <c r="D97" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>274067975.5643117</v>
+        <v>569239.5613440264</v>
       </c>
       <c r="C98" t="n">
-        <v>-675262354.2216074</v>
+        <v>7365353.885484916</v>
       </c>
       <c r="D98" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>285555902.5664799</v>
+        <v>404339.0276015802</v>
       </c>
       <c r="C99" t="n">
-        <v>-718258134.6457069</v>
+        <v>7377267.93003197</v>
       </c>
       <c r="D99" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>277547055.5154095</v>
+        <v>426389.9074570178</v>
       </c>
       <c r="C100" t="n">
-        <v>-702044307.992703</v>
+        <v>7397057.334183707</v>
       </c>
       <c r="D100" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>323741591.2967488</v>
+        <v>647260.2346404803</v>
       </c>
       <c r="C101" t="n">
-        <v>-734507953.3498362</v>
+        <v>7173046.349524124</v>
       </c>
       <c r="D101" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>241124046.2670941</v>
+        <v>422813.0446212821</v>
       </c>
       <c r="C102" t="n">
-        <v>-640531487.5712001</v>
+        <v>7525418.358305623</v>
       </c>
       <c r="D102" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>262243332.2856171</v>
+        <v>409920.3594865833</v>
       </c>
       <c r="C103" t="n">
-        <v>-679154550.8067428</v>
+        <v>7455181.222219932</v>
       </c>
       <c r="D103" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>271543321.4000739</v>
+        <v>469900.8002904762</v>
       </c>
       <c r="C104" t="n">
-        <v>-685788883.8156843</v>
+        <v>7403678.552845351</v>
       </c>
       <c r="D104" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>247118332.88347</v>
+        <v>464459.3821369232</v>
       </c>
       <c r="C105" t="n">
-        <v>-645348511.1651821</v>
+        <v>7491066.084930793</v>
       </c>
       <c r="D105" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>337201433.0136378</v>
+        <v>366853.0474747586</v>
       </c>
       <c r="C106" t="n">
-        <v>-800345615.03389</v>
+        <v>7220754.392227514</v>
       </c>
       <c r="D106" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>304537376.5776873</v>
+        <v>567174.9081824664</v>
       </c>
       <c r="C107" t="n">
-        <v>-721360980.5391968</v>
+        <v>7261232.535008149</v>
       </c>
       <c r="D107" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>239524588.7008033</v>
+        <v>397376.1849744547</v>
       </c>
       <c r="C108" t="n">
-        <v>-641184656.1507736</v>
+        <v>7539315.330421793</v>
       </c>
       <c r="D108" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>285177471.3559144</v>
+        <v>747622.3765616242</v>
       </c>
       <c r="C109" t="n">
-        <v>-666124678.5824778</v>
+        <v>7280326.687097363</v>
       </c>
       <c r="D109" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>224615062.5923977</v>
+        <v>450489.7582604677</v>
       </c>
       <c r="C110" t="n">
-        <v>-606717622.250353</v>
+        <v>7576800.85477192</v>
       </c>
       <c r="D110" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>272249754.7655263</v>
+        <v>710339.3015028904</v>
       </c>
       <c r="C111" t="n">
-        <v>-652204163.8814831</v>
+        <v>7335141.778801956</v>
       </c>
       <c r="D111" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>287408714.7674247</v>
+        <v>396053.62525233</v>
       </c>
       <c r="C112" t="n">
-        <v>-722485408.0931526</v>
+        <v>7373862.411237928</v>
       </c>
       <c r="D112" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>228605661.3841797</v>
+        <v>444704.7907449754</v>
       </c>
       <c r="C113" t="n">
-        <v>-614854348.7632763</v>
+        <v>7563900.888378733</v>
       </c>
       <c r="D113" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>228201033.2161114</v>
+        <v>443363.6732012552</v>
       </c>
       <c r="C114" t="n">
-        <v>-614288686.2252672</v>
+        <v>7565788.758657504</v>
       </c>
       <c r="D114" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>326181861.1804546</v>
+        <v>367652.259629715</v>
       </c>
       <c r="C115" t="n">
-        <v>-785049507.6016762</v>
+        <v>7256028.81467634</v>
       </c>
       <c r="D115" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>272145706.4409218</v>
+        <v>669640.2285336041</v>
       </c>
       <c r="C116" t="n">
-        <v>-657809791.884734</v>
+        <v>7345433.276130389</v>
       </c>
       <c r="D116" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>271862757.4238549</v>
+        <v>600557.637797766</v>
       </c>
       <c r="C117" t="n">
-        <v>-667248888.2380273</v>
+        <v>7364421.865823336</v>
       </c>
       <c r="D117" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>315105951.0574893</v>
+        <v>600393.0921995796</v>
       </c>
       <c r="C118" t="n">
-        <v>-730747426.1765029</v>
+        <v>7215709.499915746</v>
       </c>
       <c r="D118" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>272863476.7660523</v>
+        <v>497782.9113988071</v>
       </c>
       <c r="C119" t="n">
-        <v>-683812167.8925201</v>
+        <v>7390496.471405526</v>
       </c>
       <c r="D119" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>236410689.9844101</v>
+        <v>436466.800330822</v>
       </c>
       <c r="C120" t="n">
-        <v>-630186134.2139621</v>
+        <v>7538074.706984714</v>
       </c>
       <c r="D120" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>226165597.0039313</v>
+        <v>383723.7338277422</v>
       </c>
       <c r="C121" t="n">
-        <v>-618507473.1671422</v>
+        <v>7592001.328981454</v>
       </c>
       <c r="D121" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>225900681.1727424</v>
+        <v>446965.5634673933</v>
       </c>
       <c r="C122" t="n">
-        <v>-609564829.8951237</v>
+        <v>7573131.755081054</v>
       </c>
       <c r="D122" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>227530799.8906835</v>
+        <v>445475.1194111918</v>
       </c>
       <c r="C123" t="n">
-        <v>-612773015.4131714</v>
+        <v>7567601.635024867</v>
       </c>
       <c r="D123" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>292912636.687263</v>
+        <v>621810.8103163663</v>
       </c>
       <c r="C124" t="n">
-        <v>-696098767.0576134</v>
+        <v>7285316.554902539</v>
       </c>
       <c r="D124" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>232006809.2622156</v>
+        <v>453416.9831956982</v>
       </c>
       <c r="C125" t="n">
-        <v>-619910906.2042223</v>
+        <v>7548850.096561186</v>
       </c>
       <c r="D125" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>269835674.2570578</v>
+        <v>611592.6100460046</v>
       </c>
       <c r="C126" t="n">
-        <v>-662465103.058249</v>
+        <v>7368598.606297649</v>
       </c>
       <c r="D126" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>260004362.5773549</v>
+        <v>828987.291295761</v>
       </c>
       <c r="C127" t="n">
-        <v>-617075096.1658553</v>
+        <v>7353960.948327379</v>
       </c>
       <c r="D127" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>226163492.6711283</v>
+        <v>383726.5771532588</v>
       </c>
       <c r="C128" t="n">
-        <v>-618503154.2930305</v>
+        <v>7592008.077162812</v>
       </c>
       <c r="D128" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>272231389.1081073</v>
+        <v>572065.6433788443</v>
       </c>
       <c r="C129" t="n">
-        <v>-671946254.9176275</v>
+        <v>7370981.487775771</v>
       </c>
       <c r="D129" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>234504158.7149849</v>
+        <v>570671.744298632</v>
       </c>
       <c r="C130" t="n">
-        <v>-608853674.238616</v>
+        <v>7506660.864765343</v>
       </c>
       <c r="D130" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>257577191.2416937</v>
+        <v>539967.4751042218</v>
       </c>
       <c r="C131" t="n">
-        <v>-652668699.3305537</v>
+        <v>7431673.784536626</v>
       </c>
       <c r="D131" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>230057768.3387714</v>
+        <v>452174.9311583586</v>
       </c>
       <c r="C132" t="n">
-        <v>-616520724.873842</v>
+        <v>7556332.266056828</v>
       </c>
       <c r="D132" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>225607327.2208885</v>
+        <v>384478.042694183</v>
       </c>
       <c r="C133" t="n">
-        <v>-617361142.6686318</v>
+        <v>7593792.795184806</v>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>261178897.8119061</v>
+        <v>472457.6527888828</v>
       </c>
       <c r="C134" t="n">
-        <v>-668284335.5192387</v>
+        <v>7438943.410384167</v>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>278202125.5705481</v>
+        <v>796518.4161216137</v>
       </c>
       <c r="C135" t="n">
-        <v>-648938013.488188</v>
+        <v>7294240.829803186</v>
       </c>
       <c r="D135" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>239771508.8132858</v>
+        <v>439654.4736789956</v>
       </c>
       <c r="C136" t="n">
-        <v>-635790051.9050461</v>
+        <v>7524984.020991635</v>
       </c>
       <c r="D136" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>268395005.4511626</v>
+        <v>597874.7966290781</v>
       </c>
       <c r="C137" t="n">
-        <v>-662134595.8958046</v>
+        <v>7377365.426627968</v>
       </c>
       <c r="D137" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>251362684.6463775</v>
+        <v>507905.568870945</v>
       </c>
       <c r="C138" t="n">
-        <v>-646644373.9702441</v>
+        <v>7462990.403153609</v>
       </c>
       <c r="D138" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>304686586.0029499</v>
+        <v>366329.6275398433</v>
       </c>
       <c r="C139" t="n">
-        <v>-753959532.9839897</v>
+        <v>7326783.189303711</v>
       </c>
       <c r="D139" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>278683013.3011628</v>
+        <v>456361.2898843428</v>
       </c>
       <c r="C140" t="n">
-        <v>-699336737.2919977</v>
+        <v>7383412.108057517</v>
       </c>
       <c r="D140" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>229122462.9280137</v>
+        <v>444657.8554364101</v>
       </c>
       <c r="C141" t="n">
-        <v>-615810200.1162999</v>
+        <v>7562025.921142353</v>
       </c>
       <c r="D141" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>286652264.0822604</v>
+        <v>672768.4835952614</v>
       </c>
       <c r="C142" t="n">
-        <v>-679269130.0227554</v>
+        <v>7293509.317555598</v>
       </c>
       <c r="D142" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>268735102.2271433</v>
+        <v>612182.4967714186</v>
       </c>
       <c r="C143" t="n">
-        <v>-660636716.3574395</v>
+        <v>7372330.057555402</v>
       </c>
       <c r="D143" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>243601156.586562</v>
+        <v>728433.5137220931</v>
       </c>
       <c r="C144" t="n">
-        <v>-603939255.377998</v>
+        <v>7435412.922395073</v>
       </c>
       <c r="D144" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>315019437.858991</v>
+        <v>714304.8037613939</v>
       </c>
       <c r="C145" t="n">
-        <v>-712316144.3485979</v>
+        <v>7184478.611043642</v>
       </c>
       <c r="D145" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>230568678.7818459</v>
+        <v>439047.5535942831</v>
       </c>
       <c r="C146" t="n">
-        <v>-619213379.4449077</v>
+        <v>7558462.652592706</v>
       </c>
       <c r="D146" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>274703017.1193153</v>
+        <v>433932.7497139967</v>
       </c>
       <c r="C147" t="n">
-        <v>-696292944.7845743</v>
+        <v>7404311.079104981</v>
       </c>
       <c r="D147" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>331539974.7603281</v>
+        <v>663250.528201481</v>
       </c>
       <c r="C148" t="n">
-        <v>-741698511.2020931</v>
+        <v>7142209.795338459</v>
       </c>
       <c r="D148" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>275934405.7071202</v>
+        <v>468998.8339806726</v>
       </c>
       <c r="C149" t="n">
-        <v>-693029384.238608</v>
+        <v>7388821.772371144</v>
       </c>
       <c r="D149" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>245221390.8877693</v>
+        <v>436408.8218150658</v>
       </c>
       <c r="C150" t="n">
-        <v>-645922673.169723</v>
+        <v>7506500.594720325</v>
       </c>
       <c r="D150" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>271433622.9273621</v>
+        <v>569006.5176380178</v>
       </c>
       <c r="C151" t="n">
-        <v>-671121900.1209217</v>
+        <v>7374633.408555133</v>
       </c>
       <c r="D151" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>333327753.5744264</v>
+        <v>376624.0866571964</v>
       </c>
       <c r="C152" t="n">
-        <v>-793362759.6305578</v>
+        <v>7229605.106066765</v>
       </c>
       <c r="D152" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>281927973.9961489</v>
+        <v>444385.7615036962</v>
       </c>
       <c r="C153" t="n">
-        <v>-706328223.660036</v>
+        <v>7376206.848085475</v>
       </c>
       <c r="D153" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>241494785.4813281</v>
+        <v>431132.6180002625</v>
       </c>
       <c r="C154" t="n">
-        <v>-640042740.3329711</v>
+        <v>7521465.612824399</v>
       </c>
       <c r="D154" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>311085736.1148545</v>
+        <v>584961.2195156019</v>
       </c>
       <c r="C155" t="n">
-        <v>-727727749.3847228</v>
+        <v>7233817.372569075</v>
       </c>
       <c r="D155" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>236677036.0213428</v>
+        <v>446157.5485860738</v>
       </c>
       <c r="C156" t="n">
-        <v>-629346904.2296659</v>
+        <v>7534123.93820927</v>
       </c>
       <c r="D156" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>299827188.9903314</v>
+        <v>669236.5653518254</v>
       </c>
       <c r="C157" t="n">
-        <v>-698771109.8942244</v>
+        <v>7248640.712909578</v>
       </c>
       <c r="D157" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>275722938.950241</v>
+        <v>777512.9831815676</v>
       </c>
       <c r="C158" t="n">
-        <v>-647966189.414601</v>
+        <v>7307313.468056051</v>
       </c>
       <c r="D158" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>231870099.3434019</v>
+        <v>435487.6637338779</v>
       </c>
       <c r="C159" t="n">
-        <v>-622072620.8410587</v>
+        <v>7554822.370589631</v>
       </c>
       <c r="D159" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>331375399.2707284</v>
+        <v>664861.8344592829</v>
       </c>
       <c r="C160" t="n">
-        <v>-741223418.8351234</v>
+        <v>7142306.853326681</v>
       </c>
       <c r="D160" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>306411760.0856024</v>
+        <v>713772.8159372762</v>
       </c>
       <c r="C161" t="n">
-        <v>-700964540.7794162</v>
+        <v>7214284.154764948</v>
       </c>
       <c r="D161" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>274184724.1137281</v>
+        <v>439805.1538512177</v>
       </c>
       <c r="C162" t="n">
-        <v>-694568373.8249217</v>
+        <v>7404176.992680821</v>
       </c>
       <c r="D162" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>299734528.2315714</v>
+        <v>647141.1239790823</v>
       </c>
       <c r="C163" t="n">
-        <v>-702042015.4739696</v>
+        <v>7254886.228397596</v>
       </c>
       <c r="D163" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>240554629.3470742</v>
+        <v>429836.6878292271</v>
       </c>
       <c r="C164" t="n">
-        <v>-638542346.5098919</v>
+        <v>7525240.43409429</v>
       </c>
       <c r="D164" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>307919216.6758572</v>
+        <v>714955.4111270539</v>
       </c>
       <c r="C165" t="n">
-        <v>-702811392.4851085</v>
+        <v>7208770.172444158</v>
       </c>
       <c r="D165" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>324395347.8652229</v>
+        <v>612695.2306431417</v>
       </c>
       <c r="C166" t="n">
-        <v>-741076423.4641184</v>
+        <v>7180841.293022046</v>
       </c>
       <c r="D166" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>240392358.7967031</v>
+        <v>431933.0220172554</v>
       </c>
       <c r="C167" t="n">
-        <v>-637962998.1665426</v>
+        <v>7525164.216234216</v>
       </c>
       <c r="D167" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>282423728.746169</v>
+        <v>571477.7003448418</v>
       </c>
       <c r="C168" t="n">
-        <v>-687942724.5554985</v>
+        <v>7335667.556724924</v>
       </c>
       <c r="D168" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>324236869.8379742</v>
+        <v>725637.832248533</v>
       </c>
       <c r="C169" t="n">
-        <v>-722257016.7834637</v>
+        <v>7149922.107346477</v>
       </c>
       <c r="D169" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>293455255.8377674</v>
+        <v>674219.4674038889</v>
       </c>
       <c r="C170" t="n">
-        <v>-688952220.5230802</v>
+        <v>7269409.352310479</v>
       </c>
       <c r="D170" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>304014132.5989069</v>
+        <v>710749.5401521167</v>
       </c>
       <c r="C171" t="n">
-        <v>-698175436.5643777</v>
+        <v>7223356.075473163</v>
       </c>
       <c r="D171" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>321884934.3653171</v>
+        <v>593191.4187559042</v>
       </c>
       <c r="C172" t="n">
-        <v>-741012669.4637401</v>
+        <v>7195042.290479658</v>
       </c>
       <c r="D172" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>332054352.0411416</v>
+        <v>669087.1574735446</v>
       </c>
       <c r="C173" t="n">
-        <v>-741350897.6632477</v>
+        <v>7138823.143244307</v>
       </c>
       <c r="D173" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>268688270.2184461</v>
+        <v>576221.5915295435</v>
       </c>
       <c r="C174" t="n">
-        <v>-665700112.87985</v>
+        <v>7382257.330581195</v>
       </c>
       <c r="D174" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>325429242.7824501</v>
+        <v>713603.1766074058</v>
       </c>
       <c r="C175" t="n">
-        <v>-725720479.2212398</v>
+        <v>7149041.025246967</v>
       </c>
       <c r="D175" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>326432980.3894434</v>
+        <v>575266.3307147442</v>
       </c>
       <c r="C176" t="n">
-        <v>-749984518.1305887</v>
+        <v>7185257.558376712</v>
       </c>
       <c r="D176" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>271529942.5186161</v>
+        <v>604290.0810529721</v>
       </c>
       <c r="C177" t="n">
-        <v>-666187380.9058965</v>
+        <v>7364583.701289264</v>
       </c>
       <c r="D177" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>277018094.9322309</v>
+        <v>432284.6912633065</v>
       </c>
       <c r="C178" t="n">
-        <v>-700296723.8155724</v>
+        <v>7396923.161243825</v>
       </c>
       <c r="D178" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>274734659.9312125</v>
+        <v>439758.1563198671</v>
       </c>
       <c r="C179" t="n">
-        <v>-695469769.7531233</v>
+        <v>7402304.535486695</v>
       </c>
       <c r="D179" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>307962529.6169906</v>
+        <v>455576.2169239347</v>
       </c>
       <c r="C180" t="n">
-        <v>-744215916.061385</v>
+        <v>7284936.716519298</v>
       </c>
       <c r="D180" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
preprocessing notebook for each area
created a preprocessing notebook for each area, that way the UTM fixation point doesn't have to be changed each time when interpolating a different area
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>422823.0001388173</v>
+        <v>241116409.9288566</v>
       </c>
       <c r="C2" t="n">
-        <v>7525442.527047326</v>
+        <v>-640516451.8613</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>451013.4314993119</v>
+        <v>307840143.1691962</v>
       </c>
       <c r="C3" t="n">
-        <v>7286868.704686873</v>
+        <v>-744780978.6235237</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>594545.9850944348</v>
+        <v>271851828.2804081</v>
       </c>
       <c r="C4" t="n">
-        <v>7366095.350358819</v>
+        <v>-668097385.7077036</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>403945.0768397648</v>
+        <v>242120270.0446654</v>
       </c>
       <c r="C5" t="n">
-        <v>7527910.87798272</v>
+        <v>-644936176.4713304</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>401216.148465685</v>
+        <v>241816006.3231841</v>
       </c>
       <c r="C6" t="n">
-        <v>7529882.125589605</v>
+        <v>-644771741.2745878</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>409155.6666583589</v>
+        <v>281822355.0883852</v>
       </c>
       <c r="C7" t="n">
-        <v>7388267.661607112</v>
+        <v>-711558460.5956467</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>408788.64986577</v>
+        <v>242249524.6977128</v>
       </c>
       <c r="C8" t="n">
-        <v>7525883.127678607</v>
+        <v>-644492121.4329234</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>573609.5498119397</v>
+        <v>272620302.1461084</v>
       </c>
       <c r="C9" t="n">
-        <v>7369187.59580075</v>
+        <v>-672338783.942363</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>395739.2028744464</v>
+        <v>236537929.2857987</v>
       </c>
       <c r="C10" t="n">
-        <v>7550553.333618967</v>
+        <v>-636000231.6287237</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>595482.5194309736</v>
+        <v>273356708.5186262</v>
       </c>
       <c r="C11" t="n">
-        <v>7360555.884229297</v>
+        <v>-670332549.0772539</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>570295.7162984037</v>
+        <v>324139109.2556922</v>
       </c>
       <c r="C12" t="n">
-        <v>7194426.892189107</v>
+        <v>-747799482.7227929</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>507596.7447241906</v>
+        <v>296404406.2602804</v>
       </c>
       <c r="C13" t="n">
-        <v>7306910.773843632</v>
+        <v>-718866741.0923098</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>429046.3551782307</v>
+        <v>234421992.9689757</v>
       </c>
       <c r="C14" t="n">
-        <v>7547568.77555988</v>
+        <v>-627593821.3777303</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>760472.461105651</v>
+        <v>258153912.6522675</v>
       </c>
       <c r="C15" t="n">
-        <v>7374813.666059652</v>
+        <v>-623356145.7801745</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>586409.6389365081</v>
+        <v>325883524.4871363</v>
       </c>
       <c r="C16" t="n">
-        <v>7183700.825286468</v>
+        <v>-747398630.4843992</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>518399.5160626545</v>
+        <v>303097785.9272359</v>
       </c>
       <c r="C17" t="n">
-        <v>7280948.900331907</v>
+        <v>-727024925.2444966</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>447691.7230347765</v>
+        <v>312636899.8738974</v>
       </c>
       <c r="C18" t="n">
-        <v>7272079.333575497</v>
+        <v>-752270474.6464767</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>641757.8655294247</v>
+        <v>329811766.0912105</v>
       </c>
       <c r="C19" t="n">
-        <v>7154179.916507507</v>
+        <v>-743155717.4879633</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>420719.6780329063</v>
+        <v>241284616.1454389</v>
       </c>
       <c r="C20" t="n">
-        <v>7525508.513714559</v>
+        <v>-641108597.9145137</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>620437.5570446817</v>
+        <v>334170860.8161556</v>
       </c>
       <c r="C21" t="n">
-        <v>7145829.711649289</v>
+        <v>-752220211.8294635</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>656030.3435174299</v>
+        <v>318489476.4800459</v>
       </c>
       <c r="C22" t="n">
-        <v>7188356.034972786</v>
+        <v>-726238810.2783819</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>405491.2708980456</v>
+        <v>240947429.0625636</v>
       </c>
       <c r="C23" t="n">
-        <v>7531595.912204068</v>
+        <v>-642618118.4559122</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>404713.2604548364</v>
+        <v>241537608.1774869</v>
       </c>
       <c r="C24" t="n">
-        <v>7529740.381576492</v>
+        <v>-643785192.149943</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>568072.7130961117</v>
+        <v>316028303.5171236</v>
       </c>
       <c r="C25" t="n">
-        <v>7222234.914685098</v>
+        <v>-737261747.7522157</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>553955.6541633958</v>
+        <v>292111793.1974413</v>
       </c>
       <c r="C26" t="n">
-        <v>7307428.943578887</v>
+        <v>-705272189.3632073</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>413821.4916065777</v>
+        <v>240803556.7309235</v>
       </c>
       <c r="C27" t="n">
-        <v>7529429.834138079</v>
+        <v>-641203341.7830828</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>718950.8143728292</v>
+        <v>301625905.0998349</v>
       </c>
       <c r="C28" t="n">
-        <v>7229561.330213139</v>
+        <v>-693639299.8900316</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>689479.0599372458</v>
+        <v>259524364.4675499</v>
       </c>
       <c r="C29" t="n">
-        <v>7385840.555939897</v>
+        <v>-635159537.19867</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>640364.9592321715</v>
+        <v>321125162.8406616</v>
       </c>
       <c r="C30" t="n">
-        <v>7183844.981620431</v>
+        <v>-732246856.0965803</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>568065.8525246648</v>
+        <v>316034106.6327591</v>
       </c>
       <c r="C31" t="n">
-        <v>7222217.524079368</v>
+        <v>-737270796.7957494</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>408978.8275499512</v>
+        <v>240675486.9111191</v>
       </c>
       <c r="C32" t="n">
-        <v>7531442.590570908</v>
+        <v>-641645409.746622</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>432660.8029019876</v>
+        <v>309591520.6783481</v>
       </c>
       <c r="C33" t="n">
-        <v>7287266.453172042</v>
+        <v>-750338693.3007903</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>402680.6572135365</v>
+        <v>241180851.5727562</v>
       </c>
       <c r="C34" t="n">
-        <v>7531672.625937978</v>
+        <v>-643428200.0245736</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>648062.4098775064</v>
+        <v>328636380.8735353</v>
       </c>
       <c r="C35" t="n">
-        <v>7156317.765654799</v>
+        <v>-740617600.2250655</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>585517.9007419647</v>
+        <v>324854430.5347658</v>
       </c>
       <c r="C36" t="n">
-        <v>7187408.106334507</v>
+        <v>-746200833.3122867</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>679482.7733917895</v>
+        <v>261924235.3221091</v>
       </c>
       <c r="C37" t="n">
-        <v>7379568.764875205</v>
+        <v>-640369267.1781435</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>697218.2558684414</v>
+        <v>266105340.8550061</v>
       </c>
       <c r="C38" t="n">
-        <v>7360280.072632506</v>
+        <v>-644524175.3137047</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>385901.2558721581</v>
+        <v>233692973.6274313</v>
       </c>
       <c r="C39" t="n">
-        <v>7564001.44550652</v>
+        <v>-632156415.2001097</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>424332.5844982759</v>
+        <v>239958332.6812091</v>
       </c>
       <c r="C40" t="n">
-        <v>7529112.568427877</v>
+        <v>-638233803.9230567</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>569643.0684379223</v>
+        <v>315871578.7534108</v>
       </c>
       <c r="C41" t="n">
-        <v>7222285.613839785</v>
+        <v>-736791243.5112112</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>402406.4354549267</v>
+        <v>238081039.3346827</v>
       </c>
       <c r="C42" t="n">
-        <v>7542852.907356113</v>
+        <v>-637879350.5167651</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>437023.185092857</v>
+        <v>237917772.9119691</v>
       </c>
       <c r="C43" t="n">
-        <v>7532468.581112547</v>
+        <v>-632825810.5677013</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>593001.3245233108</v>
+        <v>271453178.3149346</v>
       </c>
       <c r="C44" t="n">
-        <v>7367918.094725985</v>
+        <v>-667689887.1368873</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>439224.5486118381</v>
+        <v>228517245.6278447</v>
       </c>
       <c r="C45" t="n">
-        <v>7565894.75324164</v>
+        <v>-615422880.303871</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>401842.916054123</v>
+        <v>242289512.9431651</v>
       </c>
       <c r="C46" t="n">
-        <v>7527990.288472353</v>
+        <v>-645532582.8692462</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>388715.6373236501</v>
+        <v>237611354.9062354</v>
       </c>
       <c r="C47" t="n">
-        <v>7548996.648429874</v>
+        <v>-638922073.3417053</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>433477.7838170429</v>
+        <v>238716552.1387896</v>
       </c>
       <c r="C48" t="n">
-        <v>7530698.264778861</v>
+        <v>-634747027.1713309</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>590088.3297374767</v>
+        <v>322745359.7031357</v>
       </c>
       <c r="C49" t="n">
-        <v>7193087.563682824</v>
+        <v>-742664354.0434316</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>421309.4212496581</v>
+        <v>242277238.6826189</v>
       </c>
       <c r="C50" t="n">
-        <v>7521773.247238778</v>
+        <v>-642799677.7142836</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>778993.4381261227</v>
+        <v>277669410.9749006</v>
       </c>
       <c r="C51" t="n">
-        <v>7299986.83529006</v>
+        <v>-650638472.9506352</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>410340.4763310733</v>
+        <v>284453677.0661486</v>
       </c>
       <c r="C52" t="n">
-        <v>7378952.937187641</v>
+        <v>-715576330.4317623</v>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>463408.7043260257</v>
+        <v>303309631.9706399</v>
       </c>
       <c r="C53" t="n">
-        <v>7297853.838466587</v>
+        <v>-736125207.7363403</v>
       </c>
       <c r="D53" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>444667.0044273772</v>
+        <v>229115395.803687</v>
       </c>
       <c r="C54" t="n">
-        <v>7562048.963216691</v>
+        <v>-615796001.4970576</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>421470.9503357491</v>
+        <v>240709029.5342582</v>
       </c>
       <c r="C55" t="n">
-        <v>7527329.485975892</v>
+        <v>-639974477.0186136</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>526067.6630022393</v>
+        <v>302373980.5765743</v>
       </c>
       <c r="C56" t="n">
-        <v>7281008.696502964</v>
+        <v>-724754887.8731717</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>384404.2276939754</v>
+        <v>226115473.4363479</v>
       </c>
       <c r="C57" t="n">
-        <v>7591962.608249241</v>
+        <v>-618321946.9817134</v>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>414448.1731552719</v>
+        <v>287378257.0332168</v>
       </c>
       <c r="C58" t="n">
-        <v>7367681.028654348</v>
+        <v>-719565294.9595512</v>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>705283.5520898863</v>
+        <v>264899440.4536139</v>
       </c>
       <c r="C59" t="n">
-        <v>7362709.877786176</v>
+        <v>-641513779.7746129</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>428504.0728901725</v>
+        <v>278445845.2283827</v>
       </c>
       <c r="C60" t="n">
-        <v>7393290.601893418</v>
+        <v>-703174320.3226094</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>364167.4705087786</v>
+        <v>313956072.1801931</v>
       </c>
       <c r="C61" t="n">
-        <v>7297116.842234123</v>
+        <v>-768109334.7570126</v>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>590092.4094163297</v>
+        <v>322741874.7063678</v>
       </c>
       <c r="C62" t="n">
-        <v>7193098.011324367</v>
+        <v>-742659074.352662</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>754559.5701349006</v>
+        <v>263258404.8438024</v>
       </c>
       <c r="C63" t="n">
-        <v>7357457.446217685</v>
+        <v>-632173952.7290845</v>
       </c>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>415018.0448537197</v>
+        <v>281833903.6966872</v>
       </c>
       <c r="C64" t="n">
-        <v>7386252.235449532</v>
+        <v>-710675747.4114839</v>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>393866.9952033143</v>
+        <v>259864791.7006577</v>
       </c>
       <c r="C65" t="n">
-        <v>7468780.921490044</v>
+        <v>-677451073.353865</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>793848.6559708756</v>
+        <v>279469335.2922495</v>
       </c>
       <c r="C66" t="n">
-        <v>7290260.126774631</v>
+        <v>-651169910.9945309</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>410337.1139574873</v>
+        <v>284456288.9917687</v>
       </c>
       <c r="C67" t="n">
-        <v>7378945.240007831</v>
+        <v>-715581003.6488818</v>
       </c>
       <c r="D67" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>705411.5012919909</v>
+        <v>259723469.9714658</v>
       </c>
       <c r="C68" t="n">
-        <v>7381384.438635441</v>
+        <v>-633302860.1094917</v>
       </c>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>827178.5078480255</v>
+        <v>261164753.2626413</v>
       </c>
       <c r="C69" t="n">
-        <v>7350027.173207692</v>
+        <v>-619107805.3630104</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>704315.0658106438</v>
+        <v>272777273.7243389</v>
       </c>
       <c r="C70" t="n">
-        <v>7334696.005952516</v>
+        <v>-653863315.1116563</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>622134.3892227954</v>
+        <v>305892356.1042734</v>
       </c>
       <c r="C71" t="n">
-        <v>7240708.73367288</v>
+        <v>-714595899.8409623</v>
       </c>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>420714.5822642142</v>
+        <v>241288520.0071773</v>
       </c>
       <c r="C72" t="n">
-        <v>7525496.171109289</v>
+        <v>-641116285.9121094</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>568070.8652271603</v>
+        <v>316029866.5670241</v>
       </c>
       <c r="C73" t="n">
-        <v>7222230.230568401</v>
+        <v>-737264185.0951921</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>517897.6597152865</v>
+        <v>279681540.434641</v>
       </c>
       <c r="C74" t="n">
-        <v>7360848.522584329</v>
+        <v>-691676297.3159117</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>402334.5145603271</v>
+        <v>238606731.4384664</v>
       </c>
       <c r="C75" t="n">
-        <v>7540991.602727064</v>
+        <v>-638839898.102951</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>572359.5505096086</v>
+        <v>330076763.9282188</v>
       </c>
       <c r="C76" t="n">
-        <v>7174025.31142854</v>
+        <v>-755208195.1460632</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>632953.2160392514</v>
+        <v>299439780.3822055</v>
       </c>
       <c r="C77" t="n">
-        <v>7259778.363588417</v>
+        <v>-703812662.4923407</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>727838.3447125108</v>
+        <v>251216849.3362035</v>
       </c>
       <c r="C78" t="n">
-        <v>7407376.859851267</v>
+        <v>-616569650.678416</v>
       </c>
       <c r="D78" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>383725.8459431626</v>
+        <v>226164033.8365528</v>
       </c>
       <c r="C79" t="n">
-        <v>7592006.341748471</v>
+        <v>-618504264.9674021</v>
       </c>
       <c r="D79" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>414435.8746544203</v>
+        <v>287387840.2114912</v>
       </c>
       <c r="C80" t="n">
-        <v>7367652.856344703</v>
+        <v>-719582297.4409394</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>412673.4235208518</v>
+        <v>283149053.8281337</v>
       </c>
       <c r="C81" t="n">
-        <v>7382581.441586836</v>
+        <v>-713138153.5136787</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>407314.2720218997</v>
+        <v>285278721.9658185</v>
       </c>
       <c r="C82" t="n">
-        <v>7377190.661707142</v>
+        <v>-717356056.9629877</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>723787.2073493205</v>
+        <v>295826005.8928929</v>
       </c>
       <c r="C83" t="n">
-        <v>7248572.024052578</v>
+        <v>-684845866.2343649</v>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>790262.1937427302</v>
+        <v>272014231.2749047</v>
       </c>
       <c r="C84" t="n">
-        <v>7317937.23898467</v>
+        <v>-640643632.4785765</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>598663.1839319061</v>
+        <v>320789113.3239766</v>
       </c>
       <c r="C85" t="n">
-        <v>7197091.63736374</v>
+        <v>-738656926.3217984</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>405767.7027150932</v>
+        <v>285970464.894981</v>
       </c>
       <c r="C86" t="n">
-        <v>7375381.027371443</v>
+        <v>-718693340.5180732</v>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>762480.8616364233</v>
+        <v>259513822.2850575</v>
       </c>
       <c r="C87" t="n">
-        <v>7369402.187121131</v>
+        <v>-625232380.7979548</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>439843.9287411383</v>
+        <v>273641607.671856</v>
       </c>
       <c r="C88" t="n">
-        <v>7406029.903836646</v>
+        <v>-693677903.9160447</v>
       </c>
       <c r="D88" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>382271.6480455336</v>
+        <v>226786550.2516718</v>
       </c>
       <c r="C89" t="n">
-        <v>7590211.624238232</v>
+        <v>-619864072.960627</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>402335.643714165</v>
+        <v>260213516.9754689</v>
       </c>
       <c r="C90" t="n">
-        <v>7464744.675496253</v>
+        <v>-676810304.4705592</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>383718.8813232478</v>
+        <v>226169188.3207233</v>
       </c>
       <c r="C91" t="n">
-        <v>7591989.812414211</v>
+        <v>-618514843.849395</v>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>539831.0236638299</v>
+        <v>254974684.4502476</v>
       </c>
       <c r="C92" t="n">
-        <v>7440963.848228727</v>
+        <v>-648327480.5640734</v>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>389353.0613288408</v>
+        <v>224717828.7056844</v>
       </c>
       <c r="C93" t="n">
-        <v>7595463.263758845</v>
+        <v>-615039144.3747218</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>383721.7863796732</v>
+        <v>226167038.3015949</v>
       </c>
       <c r="C94" t="n">
-        <v>7591996.707043167</v>
+        <v>-618510431.2372736</v>
       </c>
       <c r="D94" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>387990.2999005239</v>
+        <v>224820170.6684155</v>
       </c>
       <c r="C95" t="n">
-        <v>7595529.493387843</v>
+        <v>-615413964.9004151</v>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>669452.4467849245</v>
+        <v>274781804.7242188</v>
       </c>
       <c r="C96" t="n">
-        <v>7336131.153987038</v>
+        <v>-661899490.7891164</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>391429.212175432</v>
+        <v>233259970.1339031</v>
       </c>
       <c r="C97" t="n">
-        <v>7563757.379410667</v>
+        <v>-630603626.1936203</v>
       </c>
       <c r="D97" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>569239.5613440264</v>
+        <v>274067975.5643117</v>
       </c>
       <c r="C98" t="n">
-        <v>7365353.885484916</v>
+        <v>-675262354.2216074</v>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>404339.0276015802</v>
+        <v>285555902.5664799</v>
       </c>
       <c r="C99" t="n">
-        <v>7377267.93003197</v>
+        <v>-718258134.6457069</v>
       </c>
       <c r="D99" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>426389.9074570178</v>
+        <v>277547055.5154095</v>
       </c>
       <c r="C100" t="n">
-        <v>7397057.334183707</v>
+        <v>-702044307.992703</v>
       </c>
       <c r="D100" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>647260.2346404803</v>
+        <v>323741591.2967488</v>
       </c>
       <c r="C101" t="n">
-        <v>7173046.349524124</v>
+        <v>-734507953.3498362</v>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>422813.0446212821</v>
+        <v>241124046.2670941</v>
       </c>
       <c r="C102" t="n">
-        <v>7525418.358305623</v>
+        <v>-640531487.5712001</v>
       </c>
       <c r="D102" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>409920.3594865833</v>
+        <v>262243332.2856171</v>
       </c>
       <c r="C103" t="n">
-        <v>7455181.222219932</v>
+        <v>-679154550.8067428</v>
       </c>
       <c r="D103" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>469900.8002904762</v>
+        <v>271543321.4000739</v>
       </c>
       <c r="C104" t="n">
-        <v>7403678.552845351</v>
+        <v>-685788883.8156843</v>
       </c>
       <c r="D104" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>464459.3821369232</v>
+        <v>247118332.88347</v>
       </c>
       <c r="C105" t="n">
-        <v>7491066.084930793</v>
+        <v>-645348511.1651821</v>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>366853.0474747586</v>
+        <v>337201433.0136378</v>
       </c>
       <c r="C106" t="n">
-        <v>7220754.392227514</v>
+        <v>-800345615.03389</v>
       </c>
       <c r="D106" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>567174.9081824664</v>
+        <v>304537376.5776873</v>
       </c>
       <c r="C107" t="n">
-        <v>7261232.535008149</v>
+        <v>-721360980.5391968</v>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>397376.1849744547</v>
+        <v>239524588.7008033</v>
       </c>
       <c r="C108" t="n">
-        <v>7539315.330421793</v>
+        <v>-641184656.1507736</v>
       </c>
       <c r="D108" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>747622.3765616242</v>
+        <v>285177471.3559144</v>
       </c>
       <c r="C109" t="n">
-        <v>7280326.687097363</v>
+        <v>-666124678.5824778</v>
       </c>
       <c r="D109" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>450489.7582604677</v>
+        <v>224615062.5923977</v>
       </c>
       <c r="C110" t="n">
-        <v>7576800.85477192</v>
+        <v>-606717622.250353</v>
       </c>
       <c r="D110" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>710339.3015028904</v>
+        <v>272249754.7655263</v>
       </c>
       <c r="C111" t="n">
-        <v>7335141.778801956</v>
+        <v>-652204163.8814831</v>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>396053.62525233</v>
+        <v>287408714.7674247</v>
       </c>
       <c r="C112" t="n">
-        <v>7373862.411237928</v>
+        <v>-722485408.0931526</v>
       </c>
       <c r="D112" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>444704.7907449754</v>
+        <v>228605661.3841797</v>
       </c>
       <c r="C113" t="n">
-        <v>7563900.888378733</v>
+        <v>-614854348.7632763</v>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>443363.6732012552</v>
+        <v>228201033.2161114</v>
       </c>
       <c r="C114" t="n">
-        <v>7565788.758657504</v>
+        <v>-614288686.2252672</v>
       </c>
       <c r="D114" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>367652.259629715</v>
+        <v>326181861.1804546</v>
       </c>
       <c r="C115" t="n">
-        <v>7256028.81467634</v>
+        <v>-785049507.6016762</v>
       </c>
       <c r="D115" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>669640.2285336041</v>
+        <v>272145706.4409218</v>
       </c>
       <c r="C116" t="n">
-        <v>7345433.276130389</v>
+        <v>-657809791.884734</v>
       </c>
       <c r="D116" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>600557.637797766</v>
+        <v>271862757.4238549</v>
       </c>
       <c r="C117" t="n">
-        <v>7364421.865823336</v>
+        <v>-667248888.2380273</v>
       </c>
       <c r="D117" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>600393.0921995796</v>
+        <v>315105951.0574893</v>
       </c>
       <c r="C118" t="n">
-        <v>7215709.499915746</v>
+        <v>-730747426.1765029</v>
       </c>
       <c r="D118" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>497782.9113988071</v>
+        <v>272863476.7660523</v>
       </c>
       <c r="C119" t="n">
-        <v>7390496.471405526</v>
+        <v>-683812167.8925201</v>
       </c>
       <c r="D119" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>436466.800330822</v>
+        <v>236410689.9844101</v>
       </c>
       <c r="C120" t="n">
-        <v>7538074.706984714</v>
+        <v>-630186134.2139621</v>
       </c>
       <c r="D120" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>383723.7338277422</v>
+        <v>226165597.0039313</v>
       </c>
       <c r="C121" t="n">
-        <v>7592001.328981454</v>
+        <v>-618507473.1671422</v>
       </c>
       <c r="D121" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>446965.5634673933</v>
+        <v>225900681.1727424</v>
       </c>
       <c r="C122" t="n">
-        <v>7573131.755081054</v>
+        <v>-609564829.8951237</v>
       </c>
       <c r="D122" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>445475.1194111918</v>
+        <v>227530799.8906835</v>
       </c>
       <c r="C123" t="n">
-        <v>7567601.635024867</v>
+        <v>-612773015.4131714</v>
       </c>
       <c r="D123" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>621810.8103163663</v>
+        <v>292912636.687263</v>
       </c>
       <c r="C124" t="n">
-        <v>7285316.554902539</v>
+        <v>-696098767.0576134</v>
       </c>
       <c r="D124" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>453416.9831956982</v>
+        <v>232006809.2622156</v>
       </c>
       <c r="C125" t="n">
-        <v>7548850.096561186</v>
+        <v>-619910906.2042223</v>
       </c>
       <c r="D125" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>611592.6100460046</v>
+        <v>269835674.2570578</v>
       </c>
       <c r="C126" t="n">
-        <v>7368598.606297649</v>
+        <v>-662465103.058249</v>
       </c>
       <c r="D126" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>828987.291295761</v>
+        <v>260004362.5773549</v>
       </c>
       <c r="C127" t="n">
-        <v>7353960.948327379</v>
+        <v>-617075096.1658553</v>
       </c>
       <c r="D127" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>383726.5771532588</v>
+        <v>226163492.6711283</v>
       </c>
       <c r="C128" t="n">
-        <v>7592008.077162812</v>
+        <v>-618503154.2930305</v>
       </c>
       <c r="D128" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>572065.6433788443</v>
+        <v>272231389.1081073</v>
       </c>
       <c r="C129" t="n">
-        <v>7370981.487775771</v>
+        <v>-671946254.9176275</v>
       </c>
       <c r="D129" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>570671.744298632</v>
+        <v>234504158.7149849</v>
       </c>
       <c r="C130" t="n">
-        <v>7506660.864765343</v>
+        <v>-608853674.238616</v>
       </c>
       <c r="D130" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>539967.4751042218</v>
+        <v>257577191.2416937</v>
       </c>
       <c r="C131" t="n">
-        <v>7431673.784536626</v>
+        <v>-652668699.3305537</v>
       </c>
       <c r="D131" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>452174.9311583586</v>
+        <v>230057768.3387714</v>
       </c>
       <c r="C132" t="n">
-        <v>7556332.266056828</v>
+        <v>-616520724.873842</v>
       </c>
       <c r="D132" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>384478.042694183</v>
+        <v>225607327.2208885</v>
       </c>
       <c r="C133" t="n">
-        <v>7593792.795184806</v>
+        <v>-617361142.6686318</v>
       </c>
       <c r="D133" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>472457.6527888828</v>
+        <v>261178897.8119061</v>
       </c>
       <c r="C134" t="n">
-        <v>7438943.410384167</v>
+        <v>-668284335.5192387</v>
       </c>
       <c r="D134" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>796518.4161216137</v>
+        <v>278202125.5705481</v>
       </c>
       <c r="C135" t="n">
-        <v>7294240.829803186</v>
+        <v>-648938013.488188</v>
       </c>
       <c r="D135" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>439654.4736789956</v>
+        <v>239771508.8132858</v>
       </c>
       <c r="C136" t="n">
-        <v>7524984.020991635</v>
+        <v>-635790051.9050461</v>
       </c>
       <c r="D136" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>597874.7966290781</v>
+        <v>268395005.4511626</v>
       </c>
       <c r="C137" t="n">
-        <v>7377365.426627968</v>
+        <v>-662134595.8958046</v>
       </c>
       <c r="D137" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>507905.568870945</v>
+        <v>251362684.6463775</v>
       </c>
       <c r="C138" t="n">
-        <v>7462990.403153609</v>
+        <v>-646644373.9702441</v>
       </c>
       <c r="D138" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>366329.6275398433</v>
+        <v>304686586.0029499</v>
       </c>
       <c r="C139" t="n">
-        <v>7326783.189303711</v>
+        <v>-753959532.9839897</v>
       </c>
       <c r="D139" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>456361.2898843428</v>
+        <v>278683013.3011628</v>
       </c>
       <c r="C140" t="n">
-        <v>7383412.108057517</v>
+        <v>-699336737.2919977</v>
       </c>
       <c r="D140" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>444657.8554364101</v>
+        <v>229122462.9280137</v>
       </c>
       <c r="C141" t="n">
-        <v>7562025.921142353</v>
+        <v>-615810200.1162999</v>
       </c>
       <c r="D141" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>672768.4835952614</v>
+        <v>286652264.0822604</v>
       </c>
       <c r="C142" t="n">
-        <v>7293509.317555598</v>
+        <v>-679269130.0227554</v>
       </c>
       <c r="D142" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>612182.4967714186</v>
+        <v>268735102.2271433</v>
       </c>
       <c r="C143" t="n">
-        <v>7372330.057555402</v>
+        <v>-660636716.3574395</v>
       </c>
       <c r="D143" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>728433.5137220931</v>
+        <v>243601156.586562</v>
       </c>
       <c r="C144" t="n">
-        <v>7435412.922395073</v>
+        <v>-603939255.377998</v>
       </c>
       <c r="D144" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>714304.8037613939</v>
+        <v>315019437.858991</v>
       </c>
       <c r="C145" t="n">
-        <v>7184478.611043642</v>
+        <v>-712316144.3485979</v>
       </c>
       <c r="D145" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>439047.5535942831</v>
+        <v>230568678.7818459</v>
       </c>
       <c r="C146" t="n">
-        <v>7558462.652592706</v>
+        <v>-619213379.4449077</v>
       </c>
       <c r="D146" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>433932.7497139967</v>
+        <v>274703017.1193153</v>
       </c>
       <c r="C147" t="n">
-        <v>7404311.079104981</v>
+        <v>-696292944.7845743</v>
       </c>
       <c r="D147" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>663250.528201481</v>
+        <v>331539974.7603281</v>
       </c>
       <c r="C148" t="n">
-        <v>7142209.795338459</v>
+        <v>-741698511.2020931</v>
       </c>
       <c r="D148" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>468998.8339806726</v>
+        <v>275934405.7071202</v>
       </c>
       <c r="C149" t="n">
-        <v>7388821.772371144</v>
+        <v>-693029384.238608</v>
       </c>
       <c r="D149" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>436408.8218150658</v>
+        <v>245221390.8877693</v>
       </c>
       <c r="C150" t="n">
-        <v>7506500.594720325</v>
+        <v>-645922673.169723</v>
       </c>
       <c r="D150" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>569006.5176380178</v>
+        <v>271433622.9273621</v>
       </c>
       <c r="C151" t="n">
-        <v>7374633.408555133</v>
+        <v>-671121900.1209217</v>
       </c>
       <c r="D151" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>376624.0866571964</v>
+        <v>333327753.5744264</v>
       </c>
       <c r="C152" t="n">
-        <v>7229605.106066765</v>
+        <v>-793362759.6305578</v>
       </c>
       <c r="D152" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>444385.7615036962</v>
+        <v>281927973.9961489</v>
       </c>
       <c r="C153" t="n">
-        <v>7376206.848085475</v>
+        <v>-706328223.660036</v>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>431132.6180002625</v>
+        <v>241494785.4813281</v>
       </c>
       <c r="C154" t="n">
-        <v>7521465.612824399</v>
+        <v>-640042740.3329711</v>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>584961.2195156019</v>
+        <v>311085736.1148545</v>
       </c>
       <c r="C155" t="n">
-        <v>7233817.372569075</v>
+        <v>-727727749.3847228</v>
       </c>
       <c r="D155" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>446157.5485860738</v>
+        <v>236677036.0213428</v>
       </c>
       <c r="C156" t="n">
-        <v>7534123.93820927</v>
+        <v>-629346904.2296659</v>
       </c>
       <c r="D156" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>669236.5653518254</v>
+        <v>299827188.9903314</v>
       </c>
       <c r="C157" t="n">
-        <v>7248640.712909578</v>
+        <v>-698771109.8942244</v>
       </c>
       <c r="D157" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>777512.9831815676</v>
+        <v>275722938.950241</v>
       </c>
       <c r="C158" t="n">
-        <v>7307313.468056051</v>
+        <v>-647966189.414601</v>
       </c>
       <c r="D158" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>435487.6637338779</v>
+        <v>231870099.3434019</v>
       </c>
       <c r="C159" t="n">
-        <v>7554822.370589631</v>
+        <v>-622072620.8410587</v>
       </c>
       <c r="D159" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>664861.8344592829</v>
+        <v>331375399.2707284</v>
       </c>
       <c r="C160" t="n">
-        <v>7142306.853326681</v>
+        <v>-741223418.8351234</v>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>713772.8159372762</v>
+        <v>306411760.0856024</v>
       </c>
       <c r="C161" t="n">
-        <v>7214284.154764948</v>
+        <v>-700964540.7794162</v>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>439805.1538512177</v>
+        <v>274184724.1137281</v>
       </c>
       <c r="C162" t="n">
-        <v>7404176.992680821</v>
+        <v>-694568373.8249217</v>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>647141.1239790823</v>
+        <v>299734528.2315714</v>
       </c>
       <c r="C163" t="n">
-        <v>7254886.228397596</v>
+        <v>-702042015.4739696</v>
       </c>
       <c r="D163" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>429836.6878292271</v>
+        <v>240554629.3470742</v>
       </c>
       <c r="C164" t="n">
-        <v>7525240.43409429</v>
+        <v>-638542346.5098919</v>
       </c>
       <c r="D164" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>714955.4111270539</v>
+        <v>307919216.6758572</v>
       </c>
       <c r="C165" t="n">
-        <v>7208770.172444158</v>
+        <v>-702811392.4851085</v>
       </c>
       <c r="D165" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>612695.2306431417</v>
+        <v>324395347.8652229</v>
       </c>
       <c r="C166" t="n">
-        <v>7180841.293022046</v>
+        <v>-741076423.4641184</v>
       </c>
       <c r="D166" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>431933.0220172554</v>
+        <v>240392358.7967031</v>
       </c>
       <c r="C167" t="n">
-        <v>7525164.216234216</v>
+        <v>-637962998.1665426</v>
       </c>
       <c r="D167" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>571477.7003448418</v>
+        <v>282423728.746169</v>
       </c>
       <c r="C168" t="n">
-        <v>7335667.556724924</v>
+        <v>-687942724.5554985</v>
       </c>
       <c r="D168" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>725637.832248533</v>
+        <v>324236869.8379742</v>
       </c>
       <c r="C169" t="n">
-        <v>7149922.107346477</v>
+        <v>-722257016.7834637</v>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>674219.4674038889</v>
+        <v>293455255.8377674</v>
       </c>
       <c r="C170" t="n">
-        <v>7269409.352310479</v>
+        <v>-688952220.5230802</v>
       </c>
       <c r="D170" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>710749.5401521167</v>
+        <v>304014132.5989069</v>
       </c>
       <c r="C171" t="n">
-        <v>7223356.075473163</v>
+        <v>-698175436.5643777</v>
       </c>
       <c r="D171" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>593191.4187559042</v>
+        <v>321884934.3653171</v>
       </c>
       <c r="C172" t="n">
-        <v>7195042.290479658</v>
+        <v>-741012669.4637401</v>
       </c>
       <c r="D172" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>669087.1574735446</v>
+        <v>332054352.0411416</v>
       </c>
       <c r="C173" t="n">
-        <v>7138823.143244307</v>
+        <v>-741350897.6632477</v>
       </c>
       <c r="D173" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>576221.5915295435</v>
+        <v>268688270.2184461</v>
       </c>
       <c r="C174" t="n">
-        <v>7382257.330581195</v>
+        <v>-665700112.87985</v>
       </c>
       <c r="D174" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>713603.1766074058</v>
+        <v>325429242.7824501</v>
       </c>
       <c r="C175" t="n">
-        <v>7149041.025246967</v>
+        <v>-725720479.2212398</v>
       </c>
       <c r="D175" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>575266.3307147442</v>
+        <v>326432980.3894434</v>
       </c>
       <c r="C176" t="n">
-        <v>7185257.558376712</v>
+        <v>-749984518.1305887</v>
       </c>
       <c r="D176" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>604290.0810529721</v>
+        <v>271529942.5186161</v>
       </c>
       <c r="C177" t="n">
-        <v>7364583.701289264</v>
+        <v>-666187380.9058965</v>
       </c>
       <c r="D177" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>432284.6912633065</v>
+        <v>277018094.9322309</v>
       </c>
       <c r="C178" t="n">
-        <v>7396923.161243825</v>
+        <v>-700296723.8155724</v>
       </c>
       <c r="D178" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>439758.1563198671</v>
+        <v>274734659.9312125</v>
       </c>
       <c r="C179" t="n">
-        <v>7402304.535486695</v>
+        <v>-695469769.7531233</v>
       </c>
       <c r="D179" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>455576.2169239347</v>
+        <v>307962529.6169906</v>
       </c>
       <c r="C180" t="n">
-        <v>7284936.716519298</v>
+        <v>-744215916.061385</v>
       </c>
       <c r="D180" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
cleaning notebooks+ first time interpolating
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>241116409.9288566</v>
+        <v>422823.0001388173</v>
       </c>
       <c r="C2" t="n">
-        <v>-640516451.8613</v>
+        <v>7525442.527047326</v>
       </c>
       <c r="D2" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>307840143.1691962</v>
+        <v>451013.4314993119</v>
       </c>
       <c r="C3" t="n">
-        <v>-744780978.6235237</v>
+        <v>7286868.704686873</v>
       </c>
       <c r="D3" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>271851828.2804081</v>
+        <v>594545.9850944348</v>
       </c>
       <c r="C4" t="n">
-        <v>-668097385.7077036</v>
+        <v>7366095.350358819</v>
       </c>
       <c r="D4" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>242120270.0446654</v>
+        <v>403945.0768397648</v>
       </c>
       <c r="C5" t="n">
-        <v>-644936176.4713304</v>
+        <v>7527910.87798272</v>
       </c>
       <c r="D5" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>241816006.3231841</v>
+        <v>401216.148465685</v>
       </c>
       <c r="C6" t="n">
-        <v>-644771741.2745878</v>
+        <v>7529882.125589605</v>
       </c>
       <c r="D6" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>281822355.0883852</v>
+        <v>409155.6666583589</v>
       </c>
       <c r="C7" t="n">
-        <v>-711558460.5956467</v>
+        <v>7388267.661607112</v>
       </c>
       <c r="D7" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>242249524.6977128</v>
+        <v>408788.64986577</v>
       </c>
       <c r="C8" t="n">
-        <v>-644492121.4329234</v>
+        <v>7525883.127678607</v>
       </c>
       <c r="D8" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>272620302.1461084</v>
+        <v>573609.5498119397</v>
       </c>
       <c r="C9" t="n">
-        <v>-672338783.942363</v>
+        <v>7369187.59580075</v>
       </c>
       <c r="D9" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>236537929.2857987</v>
+        <v>395739.2028744464</v>
       </c>
       <c r="C10" t="n">
-        <v>-636000231.6287237</v>
+        <v>7550553.333618967</v>
       </c>
       <c r="D10" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>273356708.5186262</v>
+        <v>595482.5194309736</v>
       </c>
       <c r="C11" t="n">
-        <v>-670332549.0772539</v>
+        <v>7360555.884229297</v>
       </c>
       <c r="D11" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>324139109.2556922</v>
+        <v>570295.7162984037</v>
       </c>
       <c r="C12" t="n">
-        <v>-747799482.7227929</v>
+        <v>7194426.892189107</v>
       </c>
       <c r="D12" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>296404406.2602804</v>
+        <v>507596.7447241906</v>
       </c>
       <c r="C13" t="n">
-        <v>-718866741.0923098</v>
+        <v>7306910.773843632</v>
       </c>
       <c r="D13" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>234421992.9689757</v>
+        <v>429046.3551782307</v>
       </c>
       <c r="C14" t="n">
-        <v>-627593821.3777303</v>
+        <v>7547568.77555988</v>
       </c>
       <c r="D14" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>258153912.6522675</v>
+        <v>760472.461105651</v>
       </c>
       <c r="C15" t="n">
-        <v>-623356145.7801745</v>
+        <v>7374813.666059652</v>
       </c>
       <c r="D15" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>325883524.4871363</v>
+        <v>586409.6389365081</v>
       </c>
       <c r="C16" t="n">
-        <v>-747398630.4843992</v>
+        <v>7183700.825286468</v>
       </c>
       <c r="D16" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>303097785.9272359</v>
+        <v>518399.5160626545</v>
       </c>
       <c r="C17" t="n">
-        <v>-727024925.2444966</v>
+        <v>7280948.900331907</v>
       </c>
       <c r="D17" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>312636899.8738974</v>
+        <v>447691.7230347765</v>
       </c>
       <c r="C18" t="n">
-        <v>-752270474.6464767</v>
+        <v>7272079.333575497</v>
       </c>
       <c r="D18" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>329811766.0912105</v>
+        <v>641757.8655294247</v>
       </c>
       <c r="C19" t="n">
-        <v>-743155717.4879633</v>
+        <v>7154179.916507507</v>
       </c>
       <c r="D19" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>241284616.1454389</v>
+        <v>420719.6780329063</v>
       </c>
       <c r="C20" t="n">
-        <v>-641108597.9145137</v>
+        <v>7525508.513714559</v>
       </c>
       <c r="D20" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>334170860.8161556</v>
+        <v>620437.5570446817</v>
       </c>
       <c r="C21" t="n">
-        <v>-752220211.8294635</v>
+        <v>7145829.711649289</v>
       </c>
       <c r="D21" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>318489476.4800459</v>
+        <v>656030.3435174299</v>
       </c>
       <c r="C22" t="n">
-        <v>-726238810.2783819</v>
+        <v>7188356.034972786</v>
       </c>
       <c r="D22" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>240947429.0625636</v>
+        <v>405491.2708980456</v>
       </c>
       <c r="C23" t="n">
-        <v>-642618118.4559122</v>
+        <v>7531595.912204068</v>
       </c>
       <c r="D23" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>241537608.1774869</v>
+        <v>404713.2604548364</v>
       </c>
       <c r="C24" t="n">
-        <v>-643785192.149943</v>
+        <v>7529740.381576492</v>
       </c>
       <c r="D24" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>316028303.5171236</v>
+        <v>568072.7130961117</v>
       </c>
       <c r="C25" t="n">
-        <v>-737261747.7522157</v>
+        <v>7222234.914685098</v>
       </c>
       <c r="D25" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>292111793.1974413</v>
+        <v>553955.6541633958</v>
       </c>
       <c r="C26" t="n">
-        <v>-705272189.3632073</v>
+        <v>7307428.943578887</v>
       </c>
       <c r="D26" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>240803556.7309235</v>
+        <v>413821.4916065777</v>
       </c>
       <c r="C27" t="n">
-        <v>-641203341.7830828</v>
+        <v>7529429.834138079</v>
       </c>
       <c r="D27" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>301625905.0998349</v>
+        <v>718950.8143728292</v>
       </c>
       <c r="C28" t="n">
-        <v>-693639299.8900316</v>
+        <v>7229561.330213139</v>
       </c>
       <c r="D28" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>259524364.4675499</v>
+        <v>689479.0599372458</v>
       </c>
       <c r="C29" t="n">
-        <v>-635159537.19867</v>
+        <v>7385840.555939897</v>
       </c>
       <c r="D29" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>321125162.8406616</v>
+        <v>640364.9592321715</v>
       </c>
       <c r="C30" t="n">
-        <v>-732246856.0965803</v>
+        <v>7183844.981620431</v>
       </c>
       <c r="D30" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>316034106.6327591</v>
+        <v>568065.8525246648</v>
       </c>
       <c r="C31" t="n">
-        <v>-737270796.7957494</v>
+        <v>7222217.524079368</v>
       </c>
       <c r="D31" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>240675486.9111191</v>
+        <v>408978.8275499512</v>
       </c>
       <c r="C32" t="n">
-        <v>-641645409.746622</v>
+        <v>7531442.590570908</v>
       </c>
       <c r="D32" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>309591520.6783481</v>
+        <v>432660.8029019876</v>
       </c>
       <c r="C33" t="n">
-        <v>-750338693.3007903</v>
+        <v>7287266.453172042</v>
       </c>
       <c r="D33" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>241180851.5727562</v>
+        <v>402680.6572135365</v>
       </c>
       <c r="C34" t="n">
-        <v>-643428200.0245736</v>
+        <v>7531672.625937978</v>
       </c>
       <c r="D34" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>328636380.8735353</v>
+        <v>648062.4098775064</v>
       </c>
       <c r="C35" t="n">
-        <v>-740617600.2250655</v>
+        <v>7156317.765654799</v>
       </c>
       <c r="D35" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>324854430.5347658</v>
+        <v>585517.9007419647</v>
       </c>
       <c r="C36" t="n">
-        <v>-746200833.3122867</v>
+        <v>7187408.106334507</v>
       </c>
       <c r="D36" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>261924235.3221091</v>
+        <v>679482.7733917895</v>
       </c>
       <c r="C37" t="n">
-        <v>-640369267.1781435</v>
+        <v>7379568.764875205</v>
       </c>
       <c r="D37" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>266105340.8550061</v>
+        <v>697218.2558684414</v>
       </c>
       <c r="C38" t="n">
-        <v>-644524175.3137047</v>
+        <v>7360280.072632506</v>
       </c>
       <c r="D38" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>233692973.6274313</v>
+        <v>385901.2558721581</v>
       </c>
       <c r="C39" t="n">
-        <v>-632156415.2001097</v>
+        <v>7564001.44550652</v>
       </c>
       <c r="D39" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>239958332.6812091</v>
+        <v>424332.5844982759</v>
       </c>
       <c r="C40" t="n">
-        <v>-638233803.9230567</v>
+        <v>7529112.568427877</v>
       </c>
       <c r="D40" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>315871578.7534108</v>
+        <v>569643.0684379223</v>
       </c>
       <c r="C41" t="n">
-        <v>-736791243.5112112</v>
+        <v>7222285.613839785</v>
       </c>
       <c r="D41" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>238081039.3346827</v>
+        <v>402406.4354549267</v>
       </c>
       <c r="C42" t="n">
-        <v>-637879350.5167651</v>
+        <v>7542852.907356113</v>
       </c>
       <c r="D42" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>237917772.9119691</v>
+        <v>437023.185092857</v>
       </c>
       <c r="C43" t="n">
-        <v>-632825810.5677013</v>
+        <v>7532468.581112547</v>
       </c>
       <c r="D43" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>271453178.3149346</v>
+        <v>593001.3245233108</v>
       </c>
       <c r="C44" t="n">
-        <v>-667689887.1368873</v>
+        <v>7367918.094725985</v>
       </c>
       <c r="D44" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>228517245.6278447</v>
+        <v>439224.5486118381</v>
       </c>
       <c r="C45" t="n">
-        <v>-615422880.303871</v>
+        <v>7565894.75324164</v>
       </c>
       <c r="D45" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>242289512.9431651</v>
+        <v>401842.916054123</v>
       </c>
       <c r="C46" t="n">
-        <v>-645532582.8692462</v>
+        <v>7527990.288472353</v>
       </c>
       <c r="D46" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>237611354.9062354</v>
+        <v>388715.6373236501</v>
       </c>
       <c r="C47" t="n">
-        <v>-638922073.3417053</v>
+        <v>7548996.648429874</v>
       </c>
       <c r="D47" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>238716552.1387896</v>
+        <v>433477.7838170429</v>
       </c>
       <c r="C48" t="n">
-        <v>-634747027.1713309</v>
+        <v>7530698.264778861</v>
       </c>
       <c r="D48" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>322745359.7031357</v>
+        <v>590088.3297374767</v>
       </c>
       <c r="C49" t="n">
-        <v>-742664354.0434316</v>
+        <v>7193087.563682824</v>
       </c>
       <c r="D49" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>242277238.6826189</v>
+        <v>421309.4212496581</v>
       </c>
       <c r="C50" t="n">
-        <v>-642799677.7142836</v>
+        <v>7521773.247238778</v>
       </c>
       <c r="D50" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>277669410.9749006</v>
+        <v>778993.4381261227</v>
       </c>
       <c r="C51" t="n">
-        <v>-650638472.9506352</v>
+        <v>7299986.83529006</v>
       </c>
       <c r="D51" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>284453677.0661486</v>
+        <v>410340.4763310733</v>
       </c>
       <c r="C52" t="n">
-        <v>-715576330.4317623</v>
+        <v>7378952.937187641</v>
       </c>
       <c r="D52" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>303309631.9706399</v>
+        <v>463408.7043260257</v>
       </c>
       <c r="C53" t="n">
-        <v>-736125207.7363403</v>
+        <v>7297853.838466587</v>
       </c>
       <c r="D53" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>229115395.803687</v>
+        <v>444667.0044273772</v>
       </c>
       <c r="C54" t="n">
-        <v>-615796001.4970576</v>
+        <v>7562048.963216691</v>
       </c>
       <c r="D54" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>240709029.5342582</v>
+        <v>421470.9503357491</v>
       </c>
       <c r="C55" t="n">
-        <v>-639974477.0186136</v>
+        <v>7527329.485975892</v>
       </c>
       <c r="D55" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>302373980.5765743</v>
+        <v>526067.6630022393</v>
       </c>
       <c r="C56" t="n">
-        <v>-724754887.8731717</v>
+        <v>7281008.696502964</v>
       </c>
       <c r="D56" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>226115473.4363479</v>
+        <v>384404.2276939754</v>
       </c>
       <c r="C57" t="n">
-        <v>-618321946.9817134</v>
+        <v>7591962.608249241</v>
       </c>
       <c r="D57" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>287378257.0332168</v>
+        <v>414448.1731552719</v>
       </c>
       <c r="C58" t="n">
-        <v>-719565294.9595512</v>
+        <v>7367681.028654348</v>
       </c>
       <c r="D58" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>264899440.4536139</v>
+        <v>705283.5520898863</v>
       </c>
       <c r="C59" t="n">
-        <v>-641513779.7746129</v>
+        <v>7362709.877786176</v>
       </c>
       <c r="D59" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>278445845.2283827</v>
+        <v>428504.0728901725</v>
       </c>
       <c r="C60" t="n">
-        <v>-703174320.3226094</v>
+        <v>7393290.601893418</v>
       </c>
       <c r="D60" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>313956072.1801931</v>
+        <v>364167.4705087786</v>
       </c>
       <c r="C61" t="n">
-        <v>-768109334.7570126</v>
+        <v>7297116.842234123</v>
       </c>
       <c r="D61" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>322741874.7063678</v>
+        <v>590092.4094163297</v>
       </c>
       <c r="C62" t="n">
-        <v>-742659074.352662</v>
+        <v>7193098.011324367</v>
       </c>
       <c r="D62" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>263258404.8438024</v>
+        <v>754559.5701349006</v>
       </c>
       <c r="C63" t="n">
-        <v>-632173952.7290845</v>
+        <v>7357457.446217685</v>
       </c>
       <c r="D63" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>281833903.6966872</v>
+        <v>415018.0448537197</v>
       </c>
       <c r="C64" t="n">
-        <v>-710675747.4114839</v>
+        <v>7386252.235449532</v>
       </c>
       <c r="D64" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>259864791.7006577</v>
+        <v>393866.9952033143</v>
       </c>
       <c r="C65" t="n">
-        <v>-677451073.353865</v>
+        <v>7468780.921490044</v>
       </c>
       <c r="D65" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>279469335.2922495</v>
+        <v>793848.6559708756</v>
       </c>
       <c r="C66" t="n">
-        <v>-651169910.9945309</v>
+        <v>7290260.126774631</v>
       </c>
       <c r="D66" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>284456288.9917687</v>
+        <v>410337.1139574873</v>
       </c>
       <c r="C67" t="n">
-        <v>-715581003.6488818</v>
+        <v>7378945.240007831</v>
       </c>
       <c r="D67" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>259723469.9714658</v>
+        <v>705411.5012919909</v>
       </c>
       <c r="C68" t="n">
-        <v>-633302860.1094917</v>
+        <v>7381384.438635441</v>
       </c>
       <c r="D68" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>261164753.2626413</v>
+        <v>827178.5078480255</v>
       </c>
       <c r="C69" t="n">
-        <v>-619107805.3630104</v>
+        <v>7350027.173207692</v>
       </c>
       <c r="D69" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>272777273.7243389</v>
+        <v>704315.0658106438</v>
       </c>
       <c r="C70" t="n">
-        <v>-653863315.1116563</v>
+        <v>7334696.005952516</v>
       </c>
       <c r="D70" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>305892356.1042734</v>
+        <v>622134.3892227954</v>
       </c>
       <c r="C71" t="n">
-        <v>-714595899.8409623</v>
+        <v>7240708.73367288</v>
       </c>
       <c r="D71" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>241288520.0071773</v>
+        <v>420714.5822642142</v>
       </c>
       <c r="C72" t="n">
-        <v>-641116285.9121094</v>
+        <v>7525496.171109289</v>
       </c>
       <c r="D72" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>316029866.5670241</v>
+        <v>568070.8652271603</v>
       </c>
       <c r="C73" t="n">
-        <v>-737264185.0951921</v>
+        <v>7222230.230568401</v>
       </c>
       <c r="D73" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>279681540.434641</v>
+        <v>517897.6597152865</v>
       </c>
       <c r="C74" t="n">
-        <v>-691676297.3159117</v>
+        <v>7360848.522584329</v>
       </c>
       <c r="D74" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>238606731.4384664</v>
+        <v>402334.5145603271</v>
       </c>
       <c r="C75" t="n">
-        <v>-638839898.102951</v>
+        <v>7540991.602727064</v>
       </c>
       <c r="D75" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>330076763.9282188</v>
+        <v>572359.5505096086</v>
       </c>
       <c r="C76" t="n">
-        <v>-755208195.1460632</v>
+        <v>7174025.31142854</v>
       </c>
       <c r="D76" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>299439780.3822055</v>
+        <v>632953.2160392514</v>
       </c>
       <c r="C77" t="n">
-        <v>-703812662.4923407</v>
+        <v>7259778.363588417</v>
       </c>
       <c r="D77" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>251216849.3362035</v>
+        <v>727838.3447125108</v>
       </c>
       <c r="C78" t="n">
-        <v>-616569650.678416</v>
+        <v>7407376.859851267</v>
       </c>
       <c r="D78" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>226164033.8365528</v>
+        <v>383725.8459431626</v>
       </c>
       <c r="C79" t="n">
-        <v>-618504264.9674021</v>
+        <v>7592006.341748471</v>
       </c>
       <c r="D79" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>287387840.2114912</v>
+        <v>414435.8746544203</v>
       </c>
       <c r="C80" t="n">
-        <v>-719582297.4409394</v>
+        <v>7367652.856344703</v>
       </c>
       <c r="D80" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>283149053.8281337</v>
+        <v>412673.4235208518</v>
       </c>
       <c r="C81" t="n">
-        <v>-713138153.5136787</v>
+        <v>7382581.441586836</v>
       </c>
       <c r="D81" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>285278721.9658185</v>
+        <v>407314.2720218997</v>
       </c>
       <c r="C82" t="n">
-        <v>-717356056.9629877</v>
+        <v>7377190.661707142</v>
       </c>
       <c r="D82" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>295826005.8928929</v>
+        <v>723787.2073493205</v>
       </c>
       <c r="C83" t="n">
-        <v>-684845866.2343649</v>
+        <v>7248572.024052578</v>
       </c>
       <c r="D83" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>272014231.2749047</v>
+        <v>790262.1937427302</v>
       </c>
       <c r="C84" t="n">
-        <v>-640643632.4785765</v>
+        <v>7317937.23898467</v>
       </c>
       <c r="D84" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>320789113.3239766</v>
+        <v>598663.1839319061</v>
       </c>
       <c r="C85" t="n">
-        <v>-738656926.3217984</v>
+        <v>7197091.63736374</v>
       </c>
       <c r="D85" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>285970464.894981</v>
+        <v>405767.7027150932</v>
       </c>
       <c r="C86" t="n">
-        <v>-718693340.5180732</v>
+        <v>7375381.027371443</v>
       </c>
       <c r="D86" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>259513822.2850575</v>
+        <v>762480.8616364233</v>
       </c>
       <c r="C87" t="n">
-        <v>-625232380.7979548</v>
+        <v>7369402.187121131</v>
       </c>
       <c r="D87" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>273641607.671856</v>
+        <v>439843.9287411383</v>
       </c>
       <c r="C88" t="n">
-        <v>-693677903.9160447</v>
+        <v>7406029.903836646</v>
       </c>
       <c r="D88" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>226786550.2516718</v>
+        <v>382271.6480455336</v>
       </c>
       <c r="C89" t="n">
-        <v>-619864072.960627</v>
+        <v>7590211.624238232</v>
       </c>
       <c r="D89" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>260213516.9754689</v>
+        <v>402335.643714165</v>
       </c>
       <c r="C90" t="n">
-        <v>-676810304.4705592</v>
+        <v>7464744.675496253</v>
       </c>
       <c r="D90" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>226169188.3207233</v>
+        <v>383718.8813232478</v>
       </c>
       <c r="C91" t="n">
-        <v>-618514843.849395</v>
+        <v>7591989.812414211</v>
       </c>
       <c r="D91" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>254974684.4502476</v>
+        <v>539831.0236638299</v>
       </c>
       <c r="C92" t="n">
-        <v>-648327480.5640734</v>
+        <v>7440963.848228727</v>
       </c>
       <c r="D92" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>224717828.7056844</v>
+        <v>389353.0613288408</v>
       </c>
       <c r="C93" t="n">
-        <v>-615039144.3747218</v>
+        <v>7595463.263758845</v>
       </c>
       <c r="D93" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>226167038.3015949</v>
+        <v>383721.7863796732</v>
       </c>
       <c r="C94" t="n">
-        <v>-618510431.2372736</v>
+        <v>7591996.707043167</v>
       </c>
       <c r="D94" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>224820170.6684155</v>
+        <v>387990.2999005239</v>
       </c>
       <c r="C95" t="n">
-        <v>-615413964.9004151</v>
+        <v>7595529.493387843</v>
       </c>
       <c r="D95" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>274781804.7242188</v>
+        <v>669452.4467849245</v>
       </c>
       <c r="C96" t="n">
-        <v>-661899490.7891164</v>
+        <v>7336131.153987038</v>
       </c>
       <c r="D96" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>233259970.1339031</v>
+        <v>391429.212175432</v>
       </c>
       <c r="C97" t="n">
-        <v>-630603626.1936203</v>
+        <v>7563757.379410667</v>
       </c>
       <c r="D97" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>274067975.5643117</v>
+        <v>569239.5613440264</v>
       </c>
       <c r="C98" t="n">
-        <v>-675262354.2216074</v>
+        <v>7365353.885484916</v>
       </c>
       <c r="D98" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>285555902.5664799</v>
+        <v>404339.0276015802</v>
       </c>
       <c r="C99" t="n">
-        <v>-718258134.6457069</v>
+        <v>7377267.93003197</v>
       </c>
       <c r="D99" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>277547055.5154095</v>
+        <v>426389.9074570178</v>
       </c>
       <c r="C100" t="n">
-        <v>-702044307.992703</v>
+        <v>7397057.334183707</v>
       </c>
       <c r="D100" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>323741591.2967488</v>
+        <v>647260.2346404803</v>
       </c>
       <c r="C101" t="n">
-        <v>-734507953.3498362</v>
+        <v>7173046.349524124</v>
       </c>
       <c r="D101" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>241124046.2670941</v>
+        <v>422813.0446212821</v>
       </c>
       <c r="C102" t="n">
-        <v>-640531487.5712001</v>
+        <v>7525418.358305623</v>
       </c>
       <c r="D102" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>262243332.2856171</v>
+        <v>409920.3594865833</v>
       </c>
       <c r="C103" t="n">
-        <v>-679154550.8067428</v>
+        <v>7455181.222219932</v>
       </c>
       <c r="D103" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>271543321.4000739</v>
+        <v>469900.8002904762</v>
       </c>
       <c r="C104" t="n">
-        <v>-685788883.8156843</v>
+        <v>7403678.552845351</v>
       </c>
       <c r="D104" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>247118332.88347</v>
+        <v>464459.3821369232</v>
       </c>
       <c r="C105" t="n">
-        <v>-645348511.1651821</v>
+        <v>7491066.084930793</v>
       </c>
       <c r="D105" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>337201433.0136378</v>
+        <v>366853.0474747586</v>
       </c>
       <c r="C106" t="n">
-        <v>-800345615.03389</v>
+        <v>7220754.392227514</v>
       </c>
       <c r="D106" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>304537376.5776873</v>
+        <v>567174.9081824664</v>
       </c>
       <c r="C107" t="n">
-        <v>-721360980.5391968</v>
+        <v>7261232.535008149</v>
       </c>
       <c r="D107" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>239524588.7008033</v>
+        <v>397376.1849744547</v>
       </c>
       <c r="C108" t="n">
-        <v>-641184656.1507736</v>
+        <v>7539315.330421793</v>
       </c>
       <c r="D108" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>285177471.3559144</v>
+        <v>747622.3765616242</v>
       </c>
       <c r="C109" t="n">
-        <v>-666124678.5824778</v>
+        <v>7280326.687097363</v>
       </c>
       <c r="D109" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>224615062.5923977</v>
+        <v>450489.7582604677</v>
       </c>
       <c r="C110" t="n">
-        <v>-606717622.250353</v>
+        <v>7576800.85477192</v>
       </c>
       <c r="D110" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>272249754.7655263</v>
+        <v>710339.3015028904</v>
       </c>
       <c r="C111" t="n">
-        <v>-652204163.8814831</v>
+        <v>7335141.778801956</v>
       </c>
       <c r="D111" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>287408714.7674247</v>
+        <v>396053.62525233</v>
       </c>
       <c r="C112" t="n">
-        <v>-722485408.0931526</v>
+        <v>7373862.411237928</v>
       </c>
       <c r="D112" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>228605661.3841797</v>
+        <v>444704.7907449754</v>
       </c>
       <c r="C113" t="n">
-        <v>-614854348.7632763</v>
+        <v>7563900.888378733</v>
       </c>
       <c r="D113" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>228201033.2161114</v>
+        <v>443363.6732012552</v>
       </c>
       <c r="C114" t="n">
-        <v>-614288686.2252672</v>
+        <v>7565788.758657504</v>
       </c>
       <c r="D114" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>326181861.1804546</v>
+        <v>367652.259629715</v>
       </c>
       <c r="C115" t="n">
-        <v>-785049507.6016762</v>
+        <v>7256028.81467634</v>
       </c>
       <c r="D115" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>272145706.4409218</v>
+        <v>669640.2285336041</v>
       </c>
       <c r="C116" t="n">
-        <v>-657809791.884734</v>
+        <v>7345433.276130389</v>
       </c>
       <c r="D116" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>271862757.4238549</v>
+        <v>600557.637797766</v>
       </c>
       <c r="C117" t="n">
-        <v>-667248888.2380273</v>
+        <v>7364421.865823336</v>
       </c>
       <c r="D117" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>315105951.0574893</v>
+        <v>600393.0921995796</v>
       </c>
       <c r="C118" t="n">
-        <v>-730747426.1765029</v>
+        <v>7215709.499915746</v>
       </c>
       <c r="D118" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>272863476.7660523</v>
+        <v>497782.9113988071</v>
       </c>
       <c r="C119" t="n">
-        <v>-683812167.8925201</v>
+        <v>7390496.471405526</v>
       </c>
       <c r="D119" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>236410689.9844101</v>
+        <v>436466.800330822</v>
       </c>
       <c r="C120" t="n">
-        <v>-630186134.2139621</v>
+        <v>7538074.706984714</v>
       </c>
       <c r="D120" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>226165597.0039313</v>
+        <v>383723.7338277422</v>
       </c>
       <c r="C121" t="n">
-        <v>-618507473.1671422</v>
+        <v>7592001.328981454</v>
       </c>
       <c r="D121" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>225900681.1727424</v>
+        <v>446965.5634673933</v>
       </c>
       <c r="C122" t="n">
-        <v>-609564829.8951237</v>
+        <v>7573131.755081054</v>
       </c>
       <c r="D122" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>227530799.8906835</v>
+        <v>445475.1194111918</v>
       </c>
       <c r="C123" t="n">
-        <v>-612773015.4131714</v>
+        <v>7567601.635024867</v>
       </c>
       <c r="D123" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>292912636.687263</v>
+        <v>621810.8103163663</v>
       </c>
       <c r="C124" t="n">
-        <v>-696098767.0576134</v>
+        <v>7285316.554902539</v>
       </c>
       <c r="D124" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>232006809.2622156</v>
+        <v>453416.9831956982</v>
       </c>
       <c r="C125" t="n">
-        <v>-619910906.2042223</v>
+        <v>7548850.096561186</v>
       </c>
       <c r="D125" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>269835674.2570578</v>
+        <v>611592.6100460046</v>
       </c>
       <c r="C126" t="n">
-        <v>-662465103.058249</v>
+        <v>7368598.606297649</v>
       </c>
       <c r="D126" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>260004362.5773549</v>
+        <v>828987.291295761</v>
       </c>
       <c r="C127" t="n">
-        <v>-617075096.1658553</v>
+        <v>7353960.948327379</v>
       </c>
       <c r="D127" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>226163492.6711283</v>
+        <v>383726.5771532588</v>
       </c>
       <c r="C128" t="n">
-        <v>-618503154.2930305</v>
+        <v>7592008.077162812</v>
       </c>
       <c r="D128" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>272231389.1081073</v>
+        <v>572065.6433788443</v>
       </c>
       <c r="C129" t="n">
-        <v>-671946254.9176275</v>
+        <v>7370981.487775771</v>
       </c>
       <c r="D129" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>234504158.7149849</v>
+        <v>570671.744298632</v>
       </c>
       <c r="C130" t="n">
-        <v>-608853674.238616</v>
+        <v>7506660.864765343</v>
       </c>
       <c r="D130" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>257577191.2416937</v>
+        <v>539967.4751042218</v>
       </c>
       <c r="C131" t="n">
-        <v>-652668699.3305537</v>
+        <v>7431673.784536626</v>
       </c>
       <c r="D131" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>230057768.3387714</v>
+        <v>452174.9311583586</v>
       </c>
       <c r="C132" t="n">
-        <v>-616520724.873842</v>
+        <v>7556332.266056828</v>
       </c>
       <c r="D132" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>225607327.2208885</v>
+        <v>384478.042694183</v>
       </c>
       <c r="C133" t="n">
-        <v>-617361142.6686318</v>
+        <v>7593792.795184806</v>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>261178897.8119061</v>
+        <v>472457.6527888828</v>
       </c>
       <c r="C134" t="n">
-        <v>-668284335.5192387</v>
+        <v>7438943.410384167</v>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>278202125.5705481</v>
+        <v>796518.4161216137</v>
       </c>
       <c r="C135" t="n">
-        <v>-648938013.488188</v>
+        <v>7294240.829803186</v>
       </c>
       <c r="D135" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>239771508.8132858</v>
+        <v>439654.4736789956</v>
       </c>
       <c r="C136" t="n">
-        <v>-635790051.9050461</v>
+        <v>7524984.020991635</v>
       </c>
       <c r="D136" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>268395005.4511626</v>
+        <v>597874.7966290781</v>
       </c>
       <c r="C137" t="n">
-        <v>-662134595.8958046</v>
+        <v>7377365.426627968</v>
       </c>
       <c r="D137" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>251362684.6463775</v>
+        <v>507905.568870945</v>
       </c>
       <c r="C138" t="n">
-        <v>-646644373.9702441</v>
+        <v>7462990.403153609</v>
       </c>
       <c r="D138" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>304686586.0029499</v>
+        <v>366329.6275398433</v>
       </c>
       <c r="C139" t="n">
-        <v>-753959532.9839897</v>
+        <v>7326783.189303711</v>
       </c>
       <c r="D139" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>278683013.3011628</v>
+        <v>456361.2898843428</v>
       </c>
       <c r="C140" t="n">
-        <v>-699336737.2919977</v>
+        <v>7383412.108057517</v>
       </c>
       <c r="D140" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>229122462.9280137</v>
+        <v>444657.8554364101</v>
       </c>
       <c r="C141" t="n">
-        <v>-615810200.1162999</v>
+        <v>7562025.921142353</v>
       </c>
       <c r="D141" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>286652264.0822604</v>
+        <v>672768.4835952614</v>
       </c>
       <c r="C142" t="n">
-        <v>-679269130.0227554</v>
+        <v>7293509.317555598</v>
       </c>
       <c r="D142" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>268735102.2271433</v>
+        <v>612182.4967714186</v>
       </c>
       <c r="C143" t="n">
-        <v>-660636716.3574395</v>
+        <v>7372330.057555402</v>
       </c>
       <c r="D143" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>243601156.586562</v>
+        <v>728433.5137220931</v>
       </c>
       <c r="C144" t="n">
-        <v>-603939255.377998</v>
+        <v>7435412.922395073</v>
       </c>
       <c r="D144" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>315019437.858991</v>
+        <v>714304.8037613939</v>
       </c>
       <c r="C145" t="n">
-        <v>-712316144.3485979</v>
+        <v>7184478.611043642</v>
       </c>
       <c r="D145" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>230568678.7818459</v>
+        <v>439047.5535942831</v>
       </c>
       <c r="C146" t="n">
-        <v>-619213379.4449077</v>
+        <v>7558462.652592706</v>
       </c>
       <c r="D146" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>274703017.1193153</v>
+        <v>433932.7497139967</v>
       </c>
       <c r="C147" t="n">
-        <v>-696292944.7845743</v>
+        <v>7404311.079104981</v>
       </c>
       <c r="D147" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>331539974.7603281</v>
+        <v>663250.528201481</v>
       </c>
       <c r="C148" t="n">
-        <v>-741698511.2020931</v>
+        <v>7142209.795338459</v>
       </c>
       <c r="D148" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>275934405.7071202</v>
+        <v>468998.8339806726</v>
       </c>
       <c r="C149" t="n">
-        <v>-693029384.238608</v>
+        <v>7388821.772371144</v>
       </c>
       <c r="D149" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>245221390.8877693</v>
+        <v>436408.8218150658</v>
       </c>
       <c r="C150" t="n">
-        <v>-645922673.169723</v>
+        <v>7506500.594720325</v>
       </c>
       <c r="D150" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>271433622.9273621</v>
+        <v>569006.5176380178</v>
       </c>
       <c r="C151" t="n">
-        <v>-671121900.1209217</v>
+        <v>7374633.408555133</v>
       </c>
       <c r="D151" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>333327753.5744264</v>
+        <v>376624.0866571964</v>
       </c>
       <c r="C152" t="n">
-        <v>-793362759.6305578</v>
+        <v>7229605.106066765</v>
       </c>
       <c r="D152" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>281927973.9961489</v>
+        <v>444385.7615036962</v>
       </c>
       <c r="C153" t="n">
-        <v>-706328223.660036</v>
+        <v>7376206.848085475</v>
       </c>
       <c r="D153" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>241494785.4813281</v>
+        <v>431132.6180002625</v>
       </c>
       <c r="C154" t="n">
-        <v>-640042740.3329711</v>
+        <v>7521465.612824399</v>
       </c>
       <c r="D154" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>311085736.1148545</v>
+        <v>584961.2195156019</v>
       </c>
       <c r="C155" t="n">
-        <v>-727727749.3847228</v>
+        <v>7233817.372569075</v>
       </c>
       <c r="D155" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>236677036.0213428</v>
+        <v>446157.5485860738</v>
       </c>
       <c r="C156" t="n">
-        <v>-629346904.2296659</v>
+        <v>7534123.93820927</v>
       </c>
       <c r="D156" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>299827188.9903314</v>
+        <v>669236.5653518254</v>
       </c>
       <c r="C157" t="n">
-        <v>-698771109.8942244</v>
+        <v>7248640.712909578</v>
       </c>
       <c r="D157" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>275722938.950241</v>
+        <v>777512.9831815676</v>
       </c>
       <c r="C158" t="n">
-        <v>-647966189.414601</v>
+        <v>7307313.468056051</v>
       </c>
       <c r="D158" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>231870099.3434019</v>
+        <v>435487.6637338779</v>
       </c>
       <c r="C159" t="n">
-        <v>-622072620.8410587</v>
+        <v>7554822.370589631</v>
       </c>
       <c r="D159" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>331375399.2707284</v>
+        <v>664861.8344592829</v>
       </c>
       <c r="C160" t="n">
-        <v>-741223418.8351234</v>
+        <v>7142306.853326681</v>
       </c>
       <c r="D160" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>306411760.0856024</v>
+        <v>713772.8159372762</v>
       </c>
       <c r="C161" t="n">
-        <v>-700964540.7794162</v>
+        <v>7214284.154764948</v>
       </c>
       <c r="D161" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>274184724.1137281</v>
+        <v>439805.1538512177</v>
       </c>
       <c r="C162" t="n">
-        <v>-694568373.8249217</v>
+        <v>7404176.992680821</v>
       </c>
       <c r="D162" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>299734528.2315714</v>
+        <v>647141.1239790823</v>
       </c>
       <c r="C163" t="n">
-        <v>-702042015.4739696</v>
+        <v>7254886.228397596</v>
       </c>
       <c r="D163" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>240554629.3470742</v>
+        <v>429836.6878292271</v>
       </c>
       <c r="C164" t="n">
-        <v>-638542346.5098919</v>
+        <v>7525240.43409429</v>
       </c>
       <c r="D164" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>307919216.6758572</v>
+        <v>714955.4111270539</v>
       </c>
       <c r="C165" t="n">
-        <v>-702811392.4851085</v>
+        <v>7208770.172444158</v>
       </c>
       <c r="D165" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>324395347.8652229</v>
+        <v>612695.2306431417</v>
       </c>
       <c r="C166" t="n">
-        <v>-741076423.4641184</v>
+        <v>7180841.293022046</v>
       </c>
       <c r="D166" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>240392358.7967031</v>
+        <v>431933.0220172554</v>
       </c>
       <c r="C167" t="n">
-        <v>-637962998.1665426</v>
+        <v>7525164.216234216</v>
       </c>
       <c r="D167" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>282423728.746169</v>
+        <v>571477.7003448418</v>
       </c>
       <c r="C168" t="n">
-        <v>-687942724.5554985</v>
+        <v>7335667.556724924</v>
       </c>
       <c r="D168" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>324236869.8379742</v>
+        <v>725637.832248533</v>
       </c>
       <c r="C169" t="n">
-        <v>-722257016.7834637</v>
+        <v>7149922.107346477</v>
       </c>
       <c r="D169" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>293455255.8377674</v>
+        <v>674219.4674038889</v>
       </c>
       <c r="C170" t="n">
-        <v>-688952220.5230802</v>
+        <v>7269409.352310479</v>
       </c>
       <c r="D170" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>304014132.5989069</v>
+        <v>710749.5401521167</v>
       </c>
       <c r="C171" t="n">
-        <v>-698175436.5643777</v>
+        <v>7223356.075473163</v>
       </c>
       <c r="D171" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>321884934.3653171</v>
+        <v>593191.4187559042</v>
       </c>
       <c r="C172" t="n">
-        <v>-741012669.4637401</v>
+        <v>7195042.290479658</v>
       </c>
       <c r="D172" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>332054352.0411416</v>
+        <v>669087.1574735446</v>
       </c>
       <c r="C173" t="n">
-        <v>-741350897.6632477</v>
+        <v>7138823.143244307</v>
       </c>
       <c r="D173" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>268688270.2184461</v>
+        <v>576221.5915295435</v>
       </c>
       <c r="C174" t="n">
-        <v>-665700112.87985</v>
+        <v>7382257.330581195</v>
       </c>
       <c r="D174" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>325429242.7824501</v>
+        <v>713603.1766074058</v>
       </c>
       <c r="C175" t="n">
-        <v>-725720479.2212398</v>
+        <v>7149041.025246967</v>
       </c>
       <c r="D175" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>326432980.3894434</v>
+        <v>575266.3307147442</v>
       </c>
       <c r="C176" t="n">
-        <v>-749984518.1305887</v>
+        <v>7185257.558376712</v>
       </c>
       <c r="D176" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>271529942.5186161</v>
+        <v>604290.0810529721</v>
       </c>
       <c r="C177" t="n">
-        <v>-666187380.9058965</v>
+        <v>7364583.701289264</v>
       </c>
       <c r="D177" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>277018094.9322309</v>
+        <v>432284.6912633065</v>
       </c>
       <c r="C178" t="n">
-        <v>-700296723.8155724</v>
+        <v>7396923.161243825</v>
       </c>
       <c r="D178" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>274734659.9312125</v>
+        <v>439758.1563198671</v>
       </c>
       <c r="C179" t="n">
-        <v>-695469769.7531233</v>
+        <v>7402304.535486695</v>
       </c>
       <c r="D179" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>307962529.6169906</v>
+        <v>455576.2169239347</v>
       </c>
       <c r="C180" t="n">
-        <v>-744215916.061385</v>
+        <v>7284936.716519298</v>
       </c>
       <c r="D180" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
optimal variogram parameters area1: cleaning
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>422823.0001388173</v>
+        <v>95282423.42394386</v>
       </c>
       <c r="C2" t="n">
-        <v>7525442.527047326</v>
+        <v>-181124017.8387472</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>451013.4314993119</v>
+        <v>119552764.2797502</v>
       </c>
       <c r="C3" t="n">
-        <v>7286868.704686873</v>
+        <v>-209150282.5585824</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>594545.9850944348</v>
+        <v>104941148.9373436</v>
       </c>
       <c r="C4" t="n">
-        <v>7366095.350358819</v>
+        <v>-184375367.8509409</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>403945.0768397648</v>
+        <v>95828445.73439915</v>
       </c>
       <c r="C5" t="n">
-        <v>7527910.87798272</v>
+        <v>-182846056.6980341</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>401216.148465685</v>
+        <v>95741241.542317</v>
       </c>
       <c r="C6" t="n">
-        <v>7529882.125589605</v>
+        <v>-182870042.0223253</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>409155.6666583589</v>
+        <v>110429225.6288865</v>
       </c>
       <c r="C7" t="n">
-        <v>7388267.661607112</v>
+        <v>-201251187.019623</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>408788.64986577</v>
+        <v>95831264.53457274</v>
       </c>
       <c r="C8" t="n">
-        <v>7525883.127678607</v>
+        <v>-182597156.5451731</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>573609.5498119397</v>
+        <v>105424615.0091471</v>
       </c>
       <c r="C9" t="n">
-        <v>7369187.59580075</v>
+        <v>-186071770.9097808</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>395739.2028744464</v>
+        <v>93838358.02530071</v>
       </c>
       <c r="C10" t="n">
-        <v>7550553.333618967</v>
+        <v>-180545611.33535</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>595482.5194309736</v>
+        <v>105480970.7099347</v>
       </c>
       <c r="C11" t="n">
-        <v>7360555.884229297</v>
+        <v>-184960723.030066</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>570295.7162984037</v>
+        <v>124229411.8829788</v>
       </c>
       <c r="C12" t="n">
-        <v>7194426.892189107</v>
+        <v>-206495427.4714684</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>507596.7447241906</v>
+        <v>114776304.1833821</v>
       </c>
       <c r="C13" t="n">
-        <v>7306910.773843632</v>
+        <v>-200512974.5587198</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>429046.3551782307</v>
+        <v>92751328.5513556</v>
       </c>
       <c r="C14" t="n">
-        <v>7547568.77555988</v>
+        <v>-177342189.8416194</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>760472.461105651</v>
+        <v>98397391.14028972</v>
       </c>
       <c r="C15" t="n">
-        <v>7374813.666059652</v>
+        <v>-168144371.6522151</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>586409.6389365081</v>
+        <v>124689994.5163658</v>
       </c>
       <c r="C16" t="n">
-        <v>7183700.825286468</v>
+        <v>-205920335.8366216</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>518399.5160626545</v>
+        <v>117110889.8931256</v>
       </c>
       <c r="C17" t="n">
-        <v>7280948.900331907</v>
+        <v>-202419800.2301919</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>447691.7230347765</v>
+        <v>121345514.7420146</v>
       </c>
       <c r="C18" t="n">
-        <v>7272079.333575497</v>
+        <v>-211274706.1783964</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>641757.8655294247</v>
+        <v>125518658.9725189</v>
       </c>
       <c r="C19" t="n">
-        <v>7154179.916507507</v>
+        <v>-203197682.7713831</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>420719.6780329063</v>
+        <v>95364025.13515216</v>
       </c>
       <c r="C20" t="n">
-        <v>7525508.513714559</v>
+        <v>-181343537.004773</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>620437.5570446817</v>
+        <v>127327723.273805</v>
       </c>
       <c r="C21" t="n">
-        <v>7145829.711649289</v>
+        <v>-206190135.3970429</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>656030.3435174299</v>
+        <v>121267982.8839387</v>
       </c>
       <c r="C22" t="n">
-        <v>7188356.034972786</v>
+        <v>-198348593.0277166</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>405491.2708980456</v>
+        <v>95380300.6148705</v>
       </c>
       <c r="C23" t="n">
-        <v>7531595.912204068</v>
+        <v>-182155954.7913481</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>404713.2604548364</v>
+        <v>95605805.78367405</v>
       </c>
       <c r="C24" t="n">
-        <v>7529740.381576492</v>
+        <v>-182503398.1001907</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>568072.7130961117</v>
+        <v>121303364.1280309</v>
       </c>
       <c r="C25" t="n">
-        <v>7222234.914685098</v>
+        <v>-203759480.5622177</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>553955.6541633958</v>
+        <v>112735035.5398172</v>
       </c>
       <c r="C26" t="n">
-        <v>7307428.943578887</v>
+        <v>-195552640.0126746</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>413821.4916065777</v>
+        <v>95250007.58868599</v>
       </c>
       <c r="C27" t="n">
-        <v>7529429.834138079</v>
+        <v>-181546039.8281603</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>718950.8143728292</v>
+        <v>114518586.2557847</v>
       </c>
       <c r="C28" t="n">
-        <v>7229561.330213139</v>
+        <v>-188017544.4496489</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>689479.0599372458</v>
+        <v>99552257.76107493</v>
       </c>
       <c r="C29" t="n">
-        <v>7385840.555939897</v>
+        <v>-173040454.961911</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>640364.9592321715</v>
+        <v>122387987.0239019</v>
       </c>
       <c r="C30" t="n">
-        <v>7183844.981620431</v>
+        <v>-200373654.1043369</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>568065.8525246648</v>
+        <v>121305548.1740049</v>
       </c>
       <c r="C31" t="n">
-        <v>7222217.524079368</v>
+        <v>-203762088.3106418</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>408978.8275499512</v>
+        <v>95247441.91766733</v>
       </c>
       <c r="C32" t="n">
-        <v>7531442.590570908</v>
+        <v>-181793757.3492677</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>432660.8029019876</v>
+        <v>120389586.4569375</v>
       </c>
       <c r="C33" t="n">
-        <v>7287266.453172042</v>
+        <v>-211192737.5384258</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>402680.6572135365</v>
+        <v>95492687.50073972</v>
       </c>
       <c r="C34" t="n">
-        <v>7531672.625937978</v>
+        <v>-182455355.850242</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>648062.4098775064</v>
+        <v>125025500.7311581</v>
       </c>
       <c r="C35" t="n">
-        <v>7156317.765654799</v>
+        <v>-202351422.2608036</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>585517.9007419647</v>
+        <v>124325830.1572926</v>
       </c>
       <c r="C36" t="n">
-        <v>7187408.106334507</v>
+        <v>-205629841.009484</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>679482.7733917895</v>
+        <v>100517604.8722086</v>
       </c>
       <c r="C37" t="n">
-        <v>7379568.764875205</v>
+        <v>-174700136.2946388</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>697218.2558684414</v>
+        <v>101868946.7203449</v>
       </c>
       <c r="C38" t="n">
-        <v>7360280.072632506</v>
+        <v>-175394844.7938784</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>385901.2558721581</v>
+        <v>92874531.14906563</v>
       </c>
       <c r="C39" t="n">
-        <v>7564001.44550652</v>
+        <v>-179713668.4056195</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>424332.5844982759</v>
+        <v>94840572.3892775</v>
       </c>
       <c r="C40" t="n">
-        <v>7529112.568427877</v>
+        <v>-180445887.8844967</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>569643.0684379223</v>
+        <v>121229719.0507312</v>
       </c>
       <c r="C41" t="n">
-        <v>7222285.613839785</v>
+        <v>-203589248.6053825</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>402406.4354549267</v>
+        <v>94348291.96360223</v>
       </c>
       <c r="C42" t="n">
-        <v>7542852.907356113</v>
+        <v>-180904050.2130439</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>437023.185092857</v>
+        <v>93970184.60001004</v>
       </c>
       <c r="C43" t="n">
-        <v>7532468.581112547</v>
+        <v>-178609577.4670362</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>593001.3245233108</v>
+        <v>104810660.9949679</v>
       </c>
       <c r="C44" t="n">
-        <v>7367918.094725985</v>
+        <v>-184303776.0140289</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>439224.5486118381</v>
+        <v>90476856.36681883</v>
       </c>
       <c r="C45" t="n">
-        <v>7565894.75324164</v>
+        <v>-173670409.0955782</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>401842.916054123</v>
+        <v>95910579.3488552</v>
       </c>
       <c r="C46" t="n">
-        <v>7527990.288472353</v>
+        <v>-183067430.3302456</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>388715.6373236501</v>
+        <v>94300459.77152336</v>
       </c>
       <c r="C47" t="n">
-        <v>7548996.648429874</v>
+        <v>-181546911.7999673</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>433477.7838170429</v>
+        <v>94297707.20916051</v>
       </c>
       <c r="C48" t="n">
-        <v>7530698.264778861</v>
+        <v>-179237255.3816975</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>590088.3297374767</v>
+        <v>123510846.9439162</v>
       </c>
       <c r="C49" t="n">
-        <v>7193087.563682824</v>
+        <v>-204562335.5173564</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>421309.4212496581</v>
+        <v>95725352.49476045</v>
       </c>
       <c r="C50" t="n">
-        <v>7521773.247238778</v>
+        <v>-181802339.0369653</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>778993.4381261227</v>
+        <v>105275316.8308108</v>
       </c>
       <c r="C51" t="n">
-        <v>7299986.83529006</v>
+        <v>-175037791.7453042</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>410340.4763310733</v>
+        <v>111385953.0881969</v>
       </c>
       <c r="C52" t="n">
-        <v>7378952.937187641</v>
+        <v>-202325760.512677</v>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>463408.7043260257</v>
+        <v>117762322.5122562</v>
       </c>
       <c r="C53" t="n">
-        <v>7297853.838466587</v>
+        <v>-206444865.1610297</v>
       </c>
       <c r="D53" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>444667.0044273772</v>
+        <v>90649208.32910211</v>
       </c>
       <c r="C54" t="n">
-        <v>7562048.963216691</v>
+        <v>-173641320.1490476</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>421470.9503357491</v>
+        <v>95144377.64945558</v>
       </c>
       <c r="C55" t="n">
-        <v>7527329.485975892</v>
+        <v>-181006532.7089282</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>526067.6630022393</v>
+        <v>116766921.1118291</v>
       </c>
       <c r="C56" t="n">
-        <v>7281008.696502964</v>
+        <v>-201591453.3137347</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>384404.2276939754</v>
+        <v>90078456.88577609</v>
       </c>
       <c r="C57" t="n">
-        <v>7591962.608249241</v>
+        <v>-175847701.1475296</v>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>414448.1731552719</v>
+        <v>112420323.0307304</v>
       </c>
       <c r="C58" t="n">
-        <v>7367681.028654348</v>
+        <v>-203308439.8632879</v>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>705283.5520898863</v>
+        <v>101355383.3196585</v>
       </c>
       <c r="C59" t="n">
-        <v>7362709.877786176</v>
+        <v>-174382160.4228776</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>428504.0728901725</v>
+        <v>108991586.5147202</v>
       </c>
       <c r="C60" t="n">
-        <v>7393290.601893418</v>
+        <v>-198402990.7056906</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>364167.4705087786</v>
+        <v>122728333.8382406</v>
       </c>
       <c r="C61" t="n">
-        <v>7297116.842234123</v>
+        <v>-218062204.4267837</v>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>590092.4094163297</v>
+        <v>123509537.614461</v>
       </c>
       <c r="C62" t="n">
-        <v>7193098.011324367</v>
+        <v>-204560820.8228306</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>754559.5701349006</v>
+        <v>100299148.9200183</v>
       </c>
       <c r="C63" t="n">
-        <v>7357457.446217685</v>
+        <v>-170667493.1168369</v>
       </c>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>415018.0448537197</v>
+        <v>110374195.7526035</v>
       </c>
       <c r="C64" t="n">
-        <v>7386252.235449532</v>
+        <v>-200844579.8181961</v>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>393866.9952033143</v>
+        <v>102482765.1258514</v>
       </c>
       <c r="C65" t="n">
-        <v>7468780.921490044</v>
+        <v>-192206181.790361</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>793848.6559708756</v>
+        <v>105781919.9968431</v>
       </c>
       <c r="C66" t="n">
-        <v>7290260.126774631</v>
+        <v>-174815274.6477909</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>410337.1139574873</v>
+        <v>111386948.7224587</v>
       </c>
       <c r="C67" t="n">
-        <v>7378945.240007831</v>
+        <v>-202327142.1118898</v>
       </c>
       <c r="D67" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>705411.5012919909</v>
+        <v>99476173.42223467</v>
       </c>
       <c r="C68" t="n">
-        <v>7381384.438635441</v>
+        <v>-172151525.9484709</v>
       </c>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>827178.5078480255</v>
+        <v>98869799.25116791</v>
       </c>
       <c r="C69" t="n">
-        <v>7350027.173207692</v>
+        <v>-165438048.4331167</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>704315.0658106438</v>
+        <v>104221392.1295946</v>
       </c>
       <c r="C70" t="n">
-        <v>7334696.005952516</v>
+        <v>-177746059.5469749</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>622134.3892227954</v>
+        <v>117053928.7929806</v>
       </c>
       <c r="C71" t="n">
-        <v>7240708.73367288</v>
+        <v>-196200068.0253333</v>
       </c>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>420714.5822642142</v>
+        <v>95365514.89714105</v>
       </c>
       <c r="C72" t="n">
-        <v>7525496.171109289</v>
+        <v>-181345821.511656</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>568070.8652271603</v>
+        <v>121303952.3934693</v>
       </c>
       <c r="C73" t="n">
-        <v>7222230.230568401</v>
+        <v>-203760182.954509</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>517897.6597152865</v>
+        <v>108553564.6148994</v>
       </c>
       <c r="C74" t="n">
-        <v>7360848.522584329</v>
+        <v>-192822032.907654</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>402334.5145603271</v>
+        <v>94543489.69320977</v>
       </c>
       <c r="C75" t="n">
-        <v>7540991.602727064</v>
+        <v>-181175767.7115108</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>572359.5505096086</v>
+        <v>126364914.1193085</v>
       </c>
       <c r="C76" t="n">
-        <v>7174025.31142854</v>
+        <v>-208392521.0905573</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>632953.2160392514</v>
+        <v>114600012.8629923</v>
       </c>
       <c r="C77" t="n">
-        <v>7259778.363588417</v>
+        <v>-193023177.9961263</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>727838.3447125108</v>
+        <v>96183315.66373654</v>
       </c>
       <c r="C78" t="n">
-        <v>7407376.859851267</v>
+        <v>-167070045.9265256</v>
       </c>
       <c r="D78" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>383725.8459431626</v>
+        <v>90102554.08998811</v>
       </c>
       <c r="C79" t="n">
-        <v>7592006.341748471</v>
+        <v>-175916186.1970724</v>
       </c>
       <c r="D79" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>414435.8746544203</v>
+        <v>112423974.4583378</v>
       </c>
       <c r="C80" t="n">
-        <v>7367652.856344703</v>
+        <v>-203313461.5824972</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>412673.4235208518</v>
+        <v>110882036.2597607</v>
       </c>
       <c r="C81" t="n">
-        <v>7382581.441586836</v>
+        <v>-201588700.6533288</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>407314.2720218997</v>
+        <v>111720467.1438562</v>
       </c>
       <c r="C82" t="n">
-        <v>7377190.661707142</v>
+        <v>-202900885.8178033</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>723787.2073493205</v>
+        <v>112373855.7463913</v>
       </c>
       <c r="C83" t="n">
-        <v>7248572.024052578</v>
+        <v>-185556001.5893668</v>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>790262.1937427302</v>
+        <v>103127200.0445412</v>
       </c>
       <c r="C84" t="n">
-        <v>7317937.23898467</v>
+        <v>-172088483.342384</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>598663.1839319061</v>
+        <v>122708990.1519759</v>
       </c>
       <c r="C85" t="n">
-        <v>7197091.63736374</v>
+        <v>-203255148.1129821</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>405767.7027150932</v>
+        <v>111990891.5363045</v>
       </c>
       <c r="C86" t="n">
-        <v>7375381.027371443</v>
+        <v>-203312680.5100742</v>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>762480.8616364233</v>
+        <v>98870863.49995132</v>
       </c>
       <c r="C87" t="n">
-        <v>7369402.187121131</v>
+        <v>-168604253.3247996</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>439843.9287411383</v>
+        <v>107111037.3784975</v>
       </c>
       <c r="C88" t="n">
-        <v>7406029.903836646</v>
+        <v>-195472323.0756261</v>
       </c>
       <c r="D88" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>382271.6480455336</v>
+        <v>90346546.34698622</v>
       </c>
       <c r="C89" t="n">
-        <v>7590211.624238232</v>
+        <v>-176336811.5477049</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>402335.643714165</v>
+        <v>102529579.9533198</v>
       </c>
       <c r="C90" t="n">
-        <v>7464744.675496253</v>
+        <v>-191801156.5092006</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>383718.8813232478</v>
+        <v>90104528.73577157</v>
       </c>
       <c r="C91" t="n">
-        <v>7591989.812414211</v>
+        <v>-175919349.5840066</v>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>539831.0236638299</v>
+        <v>99291993.9236518</v>
       </c>
       <c r="C92" t="n">
-        <v>7440963.848228727</v>
+        <v>-180337878.069048</v>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>389353.0613288408</v>
+        <v>89515739.4878577</v>
       </c>
       <c r="C93" t="n">
-        <v>7595463.263758845</v>
+        <v>-174796657.0264485</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>383721.7863796732</v>
+        <v>90103705.07885629</v>
       </c>
       <c r="C94" t="n">
-        <v>7591996.707043167</v>
+        <v>-175918030.0872642</v>
       </c>
       <c r="D94" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>387990.2999005239</v>
+        <v>89565870.73928922</v>
       </c>
       <c r="C95" t="n">
-        <v>7595529.493387843</v>
+        <v>-174936500.8971657</v>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>669452.4467849245</v>
+        <v>105283796.2110587</v>
       </c>
       <c r="C96" t="n">
-        <v>7336131.153987038</v>
+        <v>-180789088.1050727</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>391429.212175432</v>
+        <v>92663656.04225837</v>
       </c>
       <c r="C97" t="n">
-        <v>7563757.379410667</v>
+        <v>-179135917.8359909</v>
       </c>
       <c r="D97" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>569239.5613440264</v>
+        <v>105995838.9598717</v>
       </c>
       <c r="C98" t="n">
-        <v>7365353.885484916</v>
+        <v>-186983408.2862068</v>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>404339.0276015802</v>
+        <v>111852843.7911268</v>
       </c>
       <c r="C99" t="n">
-        <v>7377267.93003197</v>
+        <v>-203232990.950353</v>
       </c>
       <c r="D99" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>426389.9074570178</v>
+        <v>108682011.9880013</v>
       </c>
       <c r="C100" t="n">
-        <v>7397057.334183707</v>
+        <v>-198149238.6850535</v>
       </c>
       <c r="D100" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>647260.2346404803</v>
+        <v>123262330.9647697</v>
       </c>
       <c r="C101" t="n">
-        <v>7173046.349524124</v>
+        <v>-200772585.0239061</v>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>422813.0446212821</v>
+        <v>95285337.07413501</v>
       </c>
       <c r="C102" t="n">
-        <v>7525418.358305623</v>
+        <v>-181128484.7188572</v>
       </c>
       <c r="D102" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>409920.3594865833</v>
+        <v>103205198.4397278</v>
       </c>
       <c r="C103" t="n">
-        <v>7455181.222219932</v>
+        <v>-192251246.9216498</v>
       </c>
       <c r="D103" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>469900.8002904762</v>
+        <v>106043189.6412067</v>
       </c>
       <c r="C104" t="n">
-        <v>7403678.552845351</v>
+        <v>-192486808.2343917</v>
       </c>
       <c r="D104" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>464459.3821369232</v>
+        <v>97110372.26147208</v>
       </c>
       <c r="C105" t="n">
-        <v>7491066.084930793</v>
+        <v>-181415844.8991398</v>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>366853.0474747586</v>
+        <v>131241033.4827757</v>
       </c>
       <c r="C106" t="n">
-        <v>7220754.392227514</v>
+        <v>-226689672.8295892</v>
       </c>
       <c r="D106" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>567174.9081824664</v>
+        <v>117129631.2220052</v>
       </c>
       <c r="C107" t="n">
-        <v>7261232.535008149</v>
+        <v>-199529950.2677192</v>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>397376.1849744547</v>
+        <v>94928926.66890271</v>
       </c>
       <c r="C108" t="n">
-        <v>7539315.330421793</v>
+        <v>-181961297.4746547</v>
       </c>
       <c r="D108" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>747622.3765616242</v>
+        <v>108290145.0312245</v>
       </c>
       <c r="C109" t="n">
-        <v>7280326.687097363</v>
+        <v>-179956136.3726603</v>
       </c>
       <c r="D109" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>450489.7582604677</v>
+        <v>88934308.95905775</v>
       </c>
       <c r="C110" t="n">
-        <v>7576800.85477192</v>
+        <v>-170947412.4750854</v>
       </c>
       <c r="D110" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>710339.3015028904</v>
+        <v>103972565.9586297</v>
       </c>
       <c r="C111" t="n">
-        <v>7335141.778801956</v>
+        <v>-177149054.5000275</v>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>396053.62525233</v>
+        <v>112619817.770193</v>
       </c>
       <c r="C112" t="n">
-        <v>7373862.411237928</v>
+        <v>-204631253.2676903</v>
       </c>
       <c r="D112" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>444704.7907449754</v>
+        <v>90460510.7681088</v>
       </c>
       <c r="C113" t="n">
-        <v>7563900.888378733</v>
+        <v>-173375849.083366</v>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>443363.6732012552</v>
+        <v>90322966.28199582</v>
       </c>
       <c r="C114" t="n">
-        <v>7565788.758657504</v>
+        <v>-173249850.8613234</v>
       </c>
       <c r="D114" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>367652.259629715</v>
+        <v>127185375.7843002</v>
       </c>
       <c r="C115" t="n">
-        <v>7256028.81467634</v>
+        <v>-222549344.2806582</v>
       </c>
       <c r="D115" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>669640.2285336041</v>
+        <v>104324543.1966155</v>
       </c>
       <c r="C116" t="n">
-        <v>7345433.276130389</v>
+        <v>-179677254.0545461</v>
       </c>
       <c r="D116" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>600557.637797766</v>
+        <v>104886990.260056</v>
       </c>
       <c r="C117" t="n">
-        <v>7364421.865823336</v>
+        <v>-183990122.8937142</v>
       </c>
       <c r="D117" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>600393.0921995796</v>
+        <v>120626767.3054073</v>
       </c>
       <c r="C118" t="n">
-        <v>7215709.499915746</v>
+        <v>-201107675.9514737</v>
       </c>
       <c r="D118" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>497782.9113988071</v>
+        <v>106253987.7411452</v>
       </c>
       <c r="C119" t="n">
-        <v>7390496.471405526</v>
+        <v>-191200737.3196173</v>
       </c>
       <c r="D119" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>436466.800330822</v>
+        <v>93418613.15065667</v>
       </c>
       <c r="C120" t="n">
-        <v>7538074.706984714</v>
+        <v>-177883619.6676927</v>
       </c>
       <c r="D120" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>383723.7338277422</v>
+        <v>90103152.92810416</v>
       </c>
       <c r="C121" t="n">
-        <v>7592001.328981454</v>
+        <v>-175917145.5400779</v>
       </c>
       <c r="D121" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>446965.5634673933</v>
+        <v>89440695.01134434</v>
       </c>
       <c r="C122" t="n">
-        <v>7573131.755081054</v>
+        <v>-171833818.660059</v>
       </c>
       <c r="D122" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>445475.1194111918</v>
+        <v>90056417.80823579</v>
       </c>
       <c r="C123" t="n">
-        <v>7567601.635024867</v>
+        <v>-172772092.1143855</v>
       </c>
       <c r="D123" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>621810.8103163663</v>
+        <v>112341383.2848444</v>
       </c>
       <c r="C124" t="n">
-        <v>7285316.554902539</v>
+        <v>-191251237.3799561</v>
       </c>
       <c r="D124" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>453416.9831956982</v>
+        <v>91638603.847031</v>
       </c>
       <c r="C125" t="n">
-        <v>7548850.096561186</v>
+        <v>-174580687.5775971</v>
       </c>
       <c r="D125" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>611592.6100460046</v>
+        <v>104041565.2928592</v>
       </c>
       <c r="C126" t="n">
-        <v>7368598.606297649</v>
+        <v>-182405013.0074969</v>
       </c>
       <c r="D126" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>828987.291295761</v>
+        <v>98434944.37232505</v>
       </c>
       <c r="C127" t="n">
-        <v>7353960.948327379</v>
+        <v>-164850226.8295321</v>
       </c>
       <c r="D127" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>383726.5771532588</v>
+        <v>90102346.77343935</v>
       </c>
       <c r="C128" t="n">
-        <v>7592008.077162812</v>
+        <v>-175915854.0738463</v>
       </c>
       <c r="D128" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>572065.6433788443</v>
+        <v>105297578.2185064</v>
       </c>
       <c r="C129" t="n">
-        <v>7370981.487775771</v>
+        <v>-186004423.6349301</v>
       </c>
       <c r="D129" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>570671.744298632</v>
+        <v>91506333.97392675</v>
       </c>
       <c r="C130" t="n">
-        <v>7506660.864765343</v>
+        <v>-168656066.0726092</v>
       </c>
       <c r="D130" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>539967.4751042218</v>
+        <v>100244385.6920507</v>
       </c>
       <c r="C131" t="n">
-        <v>7431673.784536626</v>
+        <v>-181532297.7965564</v>
       </c>
       <c r="D131" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>452174.9311583586</v>
+        <v>90930063.13631396</v>
       </c>
       <c r="C132" t="n">
-        <v>7556332.266056828</v>
+        <v>-173660181.4769069</v>
       </c>
       <c r="D132" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>384478.042694183</v>
+        <v>89889286.84587127</v>
       </c>
       <c r="C133" t="n">
-        <v>7593792.795184806</v>
+        <v>-175574363.7411091</v>
       </c>
       <c r="D133" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>472457.6527888828</v>
+        <v>102209313.6826625</v>
       </c>
       <c r="C134" t="n">
-        <v>7438943.410384167</v>
+        <v>-187581930.313654</v>
       </c>
       <c r="D134" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>796518.4161216137</v>
+        <v>105299421.9336895</v>
       </c>
       <c r="C135" t="n">
-        <v>7294240.829803186</v>
+        <v>-174154437.565182</v>
       </c>
       <c r="D135" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>439654.4736789956</v>
+        <v>94630554.37158425</v>
       </c>
       <c r="C136" t="n">
-        <v>7524984.020991635</v>
+        <v>-179373611.5363451</v>
       </c>
       <c r="D136" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>597874.7966290781</v>
+        <v>103648004.1509348</v>
       </c>
       <c r="C137" t="n">
-        <v>7377365.426627968</v>
+        <v>-182663034.0110876</v>
       </c>
       <c r="D137" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>507905.568870945</v>
+        <v>98265994.57547078</v>
       </c>
       <c r="C138" t="n">
-        <v>7462990.403153609</v>
+        <v>-180676396.8603028</v>
       </c>
       <c r="D138" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>366329.6275398433</v>
+        <v>119293100.639567</v>
       </c>
       <c r="C139" t="n">
-        <v>7326783.189303711</v>
+        <v>-214134830.6730939</v>
       </c>
       <c r="D139" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>456361.2898843428</v>
+        <v>108800112.9038873</v>
       </c>
       <c r="C140" t="n">
-        <v>7383412.108057517</v>
+        <v>-196583746.7168819</v>
       </c>
       <c r="D140" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>444657.8554364101</v>
+        <v>90651901.65778245</v>
       </c>
       <c r="C141" t="n">
-        <v>7562025.921142353</v>
+        <v>-173645533.7513208</v>
       </c>
       <c r="D141" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>672768.4835952614</v>
+        <v>109559722.9289189</v>
       </c>
       <c r="C142" t="n">
-        <v>7293509.317555598</v>
+        <v>-185388306.1858294</v>
       </c>
       <c r="D142" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>612182.4967714186</v>
+        <v>103634729.2958177</v>
       </c>
       <c r="C143" t="n">
-        <v>7372330.057555402</v>
+        <v>-181891542.7247275</v>
       </c>
       <c r="D143" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>728433.5137220931</v>
+        <v>93414706.53621852</v>
       </c>
       <c r="C144" t="n">
-        <v>7435412.922395073</v>
+        <v>-163614334.2863328</v>
       </c>
       <c r="D144" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>714304.8037613939</v>
+        <v>119403884.9223573</v>
       </c>
       <c r="C145" t="n">
-        <v>7184478.611043642</v>
+        <v>-193070738.2963331</v>
       </c>
       <c r="D145" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>439047.5535942831</v>
+        <v>91236690.37009616</v>
       </c>
       <c r="C146" t="n">
-        <v>7558462.652592706</v>
+        <v>-174739885.005937</v>
       </c>
       <c r="D146" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>433932.7497139967</v>
+        <v>107560206.4702901</v>
       </c>
       <c r="C147" t="n">
-        <v>7404311.079104981</v>
+        <v>-196355097.4582179</v>
       </c>
       <c r="D147" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>663250.528201481</v>
+        <v>125912398.5125425</v>
       </c>
       <c r="C148" t="n">
-        <v>7142209.795338459</v>
+        <v>-202194520.6540882</v>
       </c>
       <c r="D148" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>468998.8339806726</v>
+        <v>107664834.9478427</v>
       </c>
       <c r="C149" t="n">
-        <v>7388821.772371144</v>
+        <v>-194505661.1581519</v>
       </c>
       <c r="D149" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>436408.8218150658</v>
+        <v>96672242.48385458</v>
       </c>
       <c r="C150" t="n">
-        <v>7506500.594720325</v>
+        <v>-182290563.4259088</v>
       </c>
       <c r="D150" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>569006.5176380178</v>
+        <v>105035861.4768484</v>
       </c>
       <c r="C151" t="n">
-        <v>7374633.408555133</v>
+        <v>-185858100.2964173</v>
       </c>
       <c r="D151" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>376624.0866571964</v>
+        <v>129709496.8307995</v>
       </c>
       <c r="C152" t="n">
-        <v>7229605.106066765</v>
+        <v>-224507523.2811059</v>
       </c>
       <c r="D152" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>444385.7615036962</v>
+        <v>110112505.5368656</v>
       </c>
       <c r="C153" t="n">
-        <v>7376206.848085475</v>
+        <v>-198834921.7274409</v>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>431132.6180002625</v>
+        <v>95345408.76258494</v>
       </c>
       <c r="C154" t="n">
-        <v>7521465.612824399</v>
+        <v>-180780035.102492</v>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>584961.2195156019</v>
+        <v>119327644.5647107</v>
       </c>
       <c r="C155" t="n">
-        <v>7233817.372569075</v>
+        <v>-200737863.3305627</v>
       </c>
       <c r="D155" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>446157.5485860738</v>
+        <v>93428592.75277303</v>
       </c>
       <c r="C156" t="n">
-        <v>7534123.93820927</v>
+        <v>-177405817.098093</v>
       </c>
       <c r="D156" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>669236.5653518254</v>
+        <v>114371692.2541738</v>
       </c>
       <c r="C157" t="n">
-        <v>7248640.712909578</v>
+        <v>-190702731.3950348</v>
       </c>
       <c r="D157" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>777512.9831815676</v>
+        <v>104586949.9232588</v>
       </c>
       <c r="C158" t="n">
-        <v>7307313.468056051</v>
+        <v>-174359078.1543424</v>
       </c>
       <c r="D158" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>435487.6637338779</v>
+        <v>91749754.6950718</v>
       </c>
       <c r="C159" t="n">
-        <v>7554822.370589631</v>
+        <v>-175631204.4296953</v>
       </c>
       <c r="D159" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>664861.8344592829</v>
+        <v>125835557.693632</v>
       </c>
       <c r="C160" t="n">
-        <v>7142306.853326681</v>
+        <v>-202024111.6928512</v>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>713772.8159372762</v>
+        <v>116300547.405243</v>
       </c>
       <c r="C161" t="n">
-        <v>7214284.154764948</v>
+        <v>-190094256.5324488</v>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>439805.1538512177</v>
+        <v>107311224.3497591</v>
       </c>
       <c r="C162" t="n">
-        <v>7404176.992680821</v>
+        <v>-195719287.5035029</v>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>647141.1239790823</v>
+        <v>114562592.945937</v>
       </c>
       <c r="C163" t="n">
-        <v>7254886.228397596</v>
+        <v>-192167750.2243736</v>
       </c>
       <c r="D163" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>429836.6878292271</v>
+        <v>95010133.05762434</v>
       </c>
       <c r="C164" t="n">
-        <v>7525240.43409429</v>
+        <v>-180392714.7041181</v>
       </c>
       <c r="D164" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>714955.4111270539</v>
+        <v>116833037.3592419</v>
       </c>
       <c r="C165" t="n">
-        <v>7208770.172444158</v>
+        <v>-190550371.3754974</v>
       </c>
       <c r="D165" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>612695.2306431417</v>
+        <v>123867952.8791168</v>
       </c>
       <c r="C166" t="n">
-        <v>7180841.293022046</v>
+        <v>-203491291.7640728</v>
       </c>
       <c r="D166" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>431933.0220172554</v>
+        <v>94930873.93600039</v>
       </c>
       <c r="C167" t="n">
-        <v>7525164.216234216</v>
+        <v>-180177301.1360669</v>
       </c>
       <c r="D167" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>571477.7003448418</v>
+        <v>109024145.1125965</v>
       </c>
       <c r="C168" t="n">
-        <v>7335667.556724924</v>
+        <v>-190379985.0380221</v>
       </c>
       <c r="D168" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>725637.832248533</v>
+        <v>122610651.9789469</v>
       </c>
       <c r="C169" t="n">
-        <v>7149922.107346477</v>
+        <v>-195356301.638187</v>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>674219.4674038889</v>
+        <v>112012066.3744351</v>
       </c>
       <c r="C170" t="n">
-        <v>7269409.352310479</v>
+        <v>-187947443.025041</v>
       </c>
       <c r="D170" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>710749.5401521167</v>
+        <v>115464965.0687606</v>
       </c>
       <c r="C171" t="n">
-        <v>7223356.075473163</v>
+        <v>-189437112.6759949</v>
       </c>
       <c r="D171" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>593191.4187559042</v>
+        <v>123165218.7500279</v>
       </c>
       <c r="C172" t="n">
-        <v>7195042.290479658</v>
+        <v>-204035832.0819772</v>
       </c>
       <c r="D172" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>669087.1574735446</v>
+        <v>126035442.3380523</v>
       </c>
       <c r="C173" t="n">
-        <v>7138823.143244307</v>
+        <v>-201934946.3262615</v>
       </c>
       <c r="D173" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>576221.5915295435</v>
+        <v>103963286.9951731</v>
       </c>
       <c r="C174" t="n">
-        <v>7382257.330581195</v>
+        <v>-184189772.1687449</v>
       </c>
       <c r="D174" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>713603.1766074058</v>
+        <v>123167917.7093716</v>
       </c>
       <c r="C175" t="n">
-        <v>7149041.025246967</v>
+        <v>-196595593.1394584</v>
       </c>
       <c r="D175" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>575266.3307147442</v>
+        <v>125009597.6335431</v>
       </c>
       <c r="C176" t="n">
-        <v>7185257.558376712</v>
+        <v>-206928505.2360481</v>
       </c>
       <c r="D176" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>604290.0810529721</v>
+        <v>104729571.0001448</v>
       </c>
       <c r="C177" t="n">
-        <v>7364583.701289264</v>
+        <v>-183605424.8142278</v>
       </c>
       <c r="D177" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>432284.6912633065</v>
+        <v>108428450.8804912</v>
       </c>
       <c r="C178" t="n">
-        <v>7396923.161243825</v>
+        <v>-197505404.3038669</v>
       </c>
       <c r="D178" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>439758.1563198671</v>
+        <v>107513991.4400155</v>
       </c>
       <c r="C179" t="n">
-        <v>7402304.535486695</v>
+        <v>-195969432.9036126</v>
       </c>
       <c r="D179" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>455576.2169239347</v>
+        <v>119549321.5548093</v>
       </c>
       <c r="C180" t="n">
-        <v>7284936.716519298</v>
+        <v>-208864742.2065115</v>
       </c>
       <c r="D180" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
adjusting notebooks according to notebook area 1
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>95282423.42394386</v>
+        <v>422823.0001388173</v>
       </c>
       <c r="C2" t="n">
-        <v>-181124017.8387472</v>
+        <v>7525442.527047326</v>
       </c>
       <c r="D2" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>119552764.2797502</v>
+        <v>451013.4314993119</v>
       </c>
       <c r="C3" t="n">
-        <v>-209150282.5585824</v>
+        <v>7286868.704686873</v>
       </c>
       <c r="D3" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>104941148.9373436</v>
+        <v>594545.9850944348</v>
       </c>
       <c r="C4" t="n">
-        <v>-184375367.8509409</v>
+        <v>7366095.350358819</v>
       </c>
       <c r="D4" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>95828445.73439915</v>
+        <v>403945.0768397648</v>
       </c>
       <c r="C5" t="n">
-        <v>-182846056.6980341</v>
+        <v>7527910.87798272</v>
       </c>
       <c r="D5" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>95741241.542317</v>
+        <v>401216.148465685</v>
       </c>
       <c r="C6" t="n">
-        <v>-182870042.0223253</v>
+        <v>7529882.125589605</v>
       </c>
       <c r="D6" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>110429225.6288865</v>
+        <v>409155.6666583589</v>
       </c>
       <c r="C7" t="n">
-        <v>-201251187.019623</v>
+        <v>7388267.661607112</v>
       </c>
       <c r="D7" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>95831264.53457274</v>
+        <v>408788.64986577</v>
       </c>
       <c r="C8" t="n">
-        <v>-182597156.5451731</v>
+        <v>7525883.127678607</v>
       </c>
       <c r="D8" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>105424615.0091471</v>
+        <v>573609.5498119397</v>
       </c>
       <c r="C9" t="n">
-        <v>-186071770.9097808</v>
+        <v>7369187.59580075</v>
       </c>
       <c r="D9" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>93838358.02530071</v>
+        <v>395739.2028744464</v>
       </c>
       <c r="C10" t="n">
-        <v>-180545611.33535</v>
+        <v>7550553.333618967</v>
       </c>
       <c r="D10" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>105480970.7099347</v>
+        <v>595482.5194309736</v>
       </c>
       <c r="C11" t="n">
-        <v>-184960723.030066</v>
+        <v>7360555.884229297</v>
       </c>
       <c r="D11" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>124229411.8829788</v>
+        <v>570295.7162984037</v>
       </c>
       <c r="C12" t="n">
-        <v>-206495427.4714684</v>
+        <v>7194426.892189107</v>
       </c>
       <c r="D12" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>114776304.1833821</v>
+        <v>507596.7447241906</v>
       </c>
       <c r="C13" t="n">
-        <v>-200512974.5587198</v>
+        <v>7306910.773843632</v>
       </c>
       <c r="D13" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>92751328.5513556</v>
+        <v>429046.3551782307</v>
       </c>
       <c r="C14" t="n">
-        <v>-177342189.8416194</v>
+        <v>7547568.77555988</v>
       </c>
       <c r="D14" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>98397391.14028972</v>
+        <v>760472.461105651</v>
       </c>
       <c r="C15" t="n">
-        <v>-168144371.6522151</v>
+        <v>7374813.666059652</v>
       </c>
       <c r="D15" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>124689994.5163658</v>
+        <v>586409.6389365081</v>
       </c>
       <c r="C16" t="n">
-        <v>-205920335.8366216</v>
+        <v>7183700.825286468</v>
       </c>
       <c r="D16" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>117110889.8931256</v>
+        <v>518399.5160626545</v>
       </c>
       <c r="C17" t="n">
-        <v>-202419800.2301919</v>
+        <v>7280948.900331907</v>
       </c>
       <c r="D17" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>121345514.7420146</v>
+        <v>447691.7230347765</v>
       </c>
       <c r="C18" t="n">
-        <v>-211274706.1783964</v>
+        <v>7272079.333575497</v>
       </c>
       <c r="D18" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>125518658.9725189</v>
+        <v>641757.8655294247</v>
       </c>
       <c r="C19" t="n">
-        <v>-203197682.7713831</v>
+        <v>7154179.916507507</v>
       </c>
       <c r="D19" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>95364025.13515216</v>
+        <v>420719.6780329063</v>
       </c>
       <c r="C20" t="n">
-        <v>-181343537.004773</v>
+        <v>7525508.513714559</v>
       </c>
       <c r="D20" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>127327723.273805</v>
+        <v>620437.5570446817</v>
       </c>
       <c r="C21" t="n">
-        <v>-206190135.3970429</v>
+        <v>7145829.711649289</v>
       </c>
       <c r="D21" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>121267982.8839387</v>
+        <v>656030.3435174299</v>
       </c>
       <c r="C22" t="n">
-        <v>-198348593.0277166</v>
+        <v>7188356.034972786</v>
       </c>
       <c r="D22" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>95380300.6148705</v>
+        <v>405491.2708980456</v>
       </c>
       <c r="C23" t="n">
-        <v>-182155954.7913481</v>
+        <v>7531595.912204068</v>
       </c>
       <c r="D23" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>95605805.78367405</v>
+        <v>404713.2604548364</v>
       </c>
       <c r="C24" t="n">
-        <v>-182503398.1001907</v>
+        <v>7529740.381576492</v>
       </c>
       <c r="D24" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>121303364.1280309</v>
+        <v>568072.7130961117</v>
       </c>
       <c r="C25" t="n">
-        <v>-203759480.5622177</v>
+        <v>7222234.914685098</v>
       </c>
       <c r="D25" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>112735035.5398172</v>
+        <v>553955.6541633958</v>
       </c>
       <c r="C26" t="n">
-        <v>-195552640.0126746</v>
+        <v>7307428.943578887</v>
       </c>
       <c r="D26" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>95250007.58868599</v>
+        <v>413821.4916065777</v>
       </c>
       <c r="C27" t="n">
-        <v>-181546039.8281603</v>
+        <v>7529429.834138079</v>
       </c>
       <c r="D27" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>114518586.2557847</v>
+        <v>718950.8143728292</v>
       </c>
       <c r="C28" t="n">
-        <v>-188017544.4496489</v>
+        <v>7229561.330213139</v>
       </c>
       <c r="D28" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>99552257.76107493</v>
+        <v>689479.0599372458</v>
       </c>
       <c r="C29" t="n">
-        <v>-173040454.961911</v>
+        <v>7385840.555939897</v>
       </c>
       <c r="D29" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>122387987.0239019</v>
+        <v>640364.9592321715</v>
       </c>
       <c r="C30" t="n">
-        <v>-200373654.1043369</v>
+        <v>7183844.981620431</v>
       </c>
       <c r="D30" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>121305548.1740049</v>
+        <v>568065.8525246648</v>
       </c>
       <c r="C31" t="n">
-        <v>-203762088.3106418</v>
+        <v>7222217.524079368</v>
       </c>
       <c r="D31" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>95247441.91766733</v>
+        <v>408978.8275499512</v>
       </c>
       <c r="C32" t="n">
-        <v>-181793757.3492677</v>
+        <v>7531442.590570908</v>
       </c>
       <c r="D32" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>120389586.4569375</v>
+        <v>432660.8029019876</v>
       </c>
       <c r="C33" t="n">
-        <v>-211192737.5384258</v>
+        <v>7287266.453172042</v>
       </c>
       <c r="D33" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>95492687.50073972</v>
+        <v>402680.6572135365</v>
       </c>
       <c r="C34" t="n">
-        <v>-182455355.850242</v>
+        <v>7531672.625937978</v>
       </c>
       <c r="D34" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>125025500.7311581</v>
+        <v>648062.4098775064</v>
       </c>
       <c r="C35" t="n">
-        <v>-202351422.2608036</v>
+        <v>7156317.765654799</v>
       </c>
       <c r="D35" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>124325830.1572926</v>
+        <v>585517.9007419647</v>
       </c>
       <c r="C36" t="n">
-        <v>-205629841.009484</v>
+        <v>7187408.106334507</v>
       </c>
       <c r="D36" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>100517604.8722086</v>
+        <v>679482.7733917895</v>
       </c>
       <c r="C37" t="n">
-        <v>-174700136.2946388</v>
+        <v>7379568.764875205</v>
       </c>
       <c r="D37" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>101868946.7203449</v>
+        <v>697218.2558684414</v>
       </c>
       <c r="C38" t="n">
-        <v>-175394844.7938784</v>
+        <v>7360280.072632506</v>
       </c>
       <c r="D38" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>92874531.14906563</v>
+        <v>385901.2558721581</v>
       </c>
       <c r="C39" t="n">
-        <v>-179713668.4056195</v>
+        <v>7564001.44550652</v>
       </c>
       <c r="D39" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>94840572.3892775</v>
+        <v>424332.5844982759</v>
       </c>
       <c r="C40" t="n">
-        <v>-180445887.8844967</v>
+        <v>7529112.568427877</v>
       </c>
       <c r="D40" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>121229719.0507312</v>
+        <v>569643.0684379223</v>
       </c>
       <c r="C41" t="n">
-        <v>-203589248.6053825</v>
+        <v>7222285.613839785</v>
       </c>
       <c r="D41" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>94348291.96360223</v>
+        <v>402406.4354549267</v>
       </c>
       <c r="C42" t="n">
-        <v>-180904050.2130439</v>
+        <v>7542852.907356113</v>
       </c>
       <c r="D42" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>93970184.60001004</v>
+        <v>437023.185092857</v>
       </c>
       <c r="C43" t="n">
-        <v>-178609577.4670362</v>
+        <v>7532468.581112547</v>
       </c>
       <c r="D43" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>104810660.9949679</v>
+        <v>593001.3245233108</v>
       </c>
       <c r="C44" t="n">
-        <v>-184303776.0140289</v>
+        <v>7367918.094725985</v>
       </c>
       <c r="D44" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>90476856.36681883</v>
+        <v>439224.5486118381</v>
       </c>
       <c r="C45" t="n">
-        <v>-173670409.0955782</v>
+        <v>7565894.75324164</v>
       </c>
       <c r="D45" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>95910579.3488552</v>
+        <v>401842.916054123</v>
       </c>
       <c r="C46" t="n">
-        <v>-183067430.3302456</v>
+        <v>7527990.288472353</v>
       </c>
       <c r="D46" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>94300459.77152336</v>
+        <v>388715.6373236501</v>
       </c>
       <c r="C47" t="n">
-        <v>-181546911.7999673</v>
+        <v>7548996.648429874</v>
       </c>
       <c r="D47" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>94297707.20916051</v>
+        <v>433477.7838170429</v>
       </c>
       <c r="C48" t="n">
-        <v>-179237255.3816975</v>
+        <v>7530698.264778861</v>
       </c>
       <c r="D48" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>123510846.9439162</v>
+        <v>590088.3297374767</v>
       </c>
       <c r="C49" t="n">
-        <v>-204562335.5173564</v>
+        <v>7193087.563682824</v>
       </c>
       <c r="D49" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>95725352.49476045</v>
+        <v>421309.4212496581</v>
       </c>
       <c r="C50" t="n">
-        <v>-181802339.0369653</v>
+        <v>7521773.247238778</v>
       </c>
       <c r="D50" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>105275316.8308108</v>
+        <v>778993.4381261227</v>
       </c>
       <c r="C51" t="n">
-        <v>-175037791.7453042</v>
+        <v>7299986.83529006</v>
       </c>
       <c r="D51" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>111385953.0881969</v>
+        <v>410340.4763310733</v>
       </c>
       <c r="C52" t="n">
-        <v>-202325760.512677</v>
+        <v>7378952.937187641</v>
       </c>
       <c r="D52" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>117762322.5122562</v>
+        <v>463408.7043260257</v>
       </c>
       <c r="C53" t="n">
-        <v>-206444865.1610297</v>
+        <v>7297853.838466587</v>
       </c>
       <c r="D53" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>90649208.32910211</v>
+        <v>444667.0044273772</v>
       </c>
       <c r="C54" t="n">
-        <v>-173641320.1490476</v>
+        <v>7562048.963216691</v>
       </c>
       <c r="D54" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>95144377.64945558</v>
+        <v>421470.9503357491</v>
       </c>
       <c r="C55" t="n">
-        <v>-181006532.7089282</v>
+        <v>7527329.485975892</v>
       </c>
       <c r="D55" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>116766921.1118291</v>
+        <v>526067.6630022393</v>
       </c>
       <c r="C56" t="n">
-        <v>-201591453.3137347</v>
+        <v>7281008.696502964</v>
       </c>
       <c r="D56" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>90078456.88577609</v>
+        <v>384404.2276939754</v>
       </c>
       <c r="C57" t="n">
-        <v>-175847701.1475296</v>
+        <v>7591962.608249241</v>
       </c>
       <c r="D57" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>112420323.0307304</v>
+        <v>414448.1731552719</v>
       </c>
       <c r="C58" t="n">
-        <v>-203308439.8632879</v>
+        <v>7367681.028654348</v>
       </c>
       <c r="D58" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>101355383.3196585</v>
+        <v>705283.5520898863</v>
       </c>
       <c r="C59" t="n">
-        <v>-174382160.4228776</v>
+        <v>7362709.877786176</v>
       </c>
       <c r="D59" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>108991586.5147202</v>
+        <v>428504.0728901725</v>
       </c>
       <c r="C60" t="n">
-        <v>-198402990.7056906</v>
+        <v>7393290.601893418</v>
       </c>
       <c r="D60" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>122728333.8382406</v>
+        <v>364167.4705087786</v>
       </c>
       <c r="C61" t="n">
-        <v>-218062204.4267837</v>
+        <v>7297116.842234123</v>
       </c>
       <c r="D61" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>123509537.614461</v>
+        <v>590092.4094163297</v>
       </c>
       <c r="C62" t="n">
-        <v>-204560820.8228306</v>
+        <v>7193098.011324367</v>
       </c>
       <c r="D62" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>100299148.9200183</v>
+        <v>754559.5701349006</v>
       </c>
       <c r="C63" t="n">
-        <v>-170667493.1168369</v>
+        <v>7357457.446217685</v>
       </c>
       <c r="D63" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>110374195.7526035</v>
+        <v>415018.0448537197</v>
       </c>
       <c r="C64" t="n">
-        <v>-200844579.8181961</v>
+        <v>7386252.235449532</v>
       </c>
       <c r="D64" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>102482765.1258514</v>
+        <v>393866.9952033143</v>
       </c>
       <c r="C65" t="n">
-        <v>-192206181.790361</v>
+        <v>7468780.921490044</v>
       </c>
       <c r="D65" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>105781919.9968431</v>
+        <v>793848.6559708756</v>
       </c>
       <c r="C66" t="n">
-        <v>-174815274.6477909</v>
+        <v>7290260.126774631</v>
       </c>
       <c r="D66" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>111386948.7224587</v>
+        <v>410337.1139574873</v>
       </c>
       <c r="C67" t="n">
-        <v>-202327142.1118898</v>
+        <v>7378945.240007831</v>
       </c>
       <c r="D67" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>99476173.42223467</v>
+        <v>705411.5012919909</v>
       </c>
       <c r="C68" t="n">
-        <v>-172151525.9484709</v>
+        <v>7381384.438635441</v>
       </c>
       <c r="D68" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>98869799.25116791</v>
+        <v>827178.5078480255</v>
       </c>
       <c r="C69" t="n">
-        <v>-165438048.4331167</v>
+        <v>7350027.173207692</v>
       </c>
       <c r="D69" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>104221392.1295946</v>
+        <v>704315.0658106438</v>
       </c>
       <c r="C70" t="n">
-        <v>-177746059.5469749</v>
+        <v>7334696.005952516</v>
       </c>
       <c r="D70" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>117053928.7929806</v>
+        <v>622134.3892227954</v>
       </c>
       <c r="C71" t="n">
-        <v>-196200068.0253333</v>
+        <v>7240708.73367288</v>
       </c>
       <c r="D71" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>95365514.89714105</v>
+        <v>420714.5822642142</v>
       </c>
       <c r="C72" t="n">
-        <v>-181345821.511656</v>
+        <v>7525496.171109289</v>
       </c>
       <c r="D72" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>121303952.3934693</v>
+        <v>568070.8652271603</v>
       </c>
       <c r="C73" t="n">
-        <v>-203760182.954509</v>
+        <v>7222230.230568401</v>
       </c>
       <c r="D73" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>108553564.6148994</v>
+        <v>517897.6597152865</v>
       </c>
       <c r="C74" t="n">
-        <v>-192822032.907654</v>
+        <v>7360848.522584329</v>
       </c>
       <c r="D74" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>94543489.69320977</v>
+        <v>402334.5145603271</v>
       </c>
       <c r="C75" t="n">
-        <v>-181175767.7115108</v>
+        <v>7540991.602727064</v>
       </c>
       <c r="D75" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>126364914.1193085</v>
+        <v>572359.5505096086</v>
       </c>
       <c r="C76" t="n">
-        <v>-208392521.0905573</v>
+        <v>7174025.31142854</v>
       </c>
       <c r="D76" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>114600012.8629923</v>
+        <v>632953.2160392514</v>
       </c>
       <c r="C77" t="n">
-        <v>-193023177.9961263</v>
+        <v>7259778.363588417</v>
       </c>
       <c r="D77" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>96183315.66373654</v>
+        <v>727838.3447125108</v>
       </c>
       <c r="C78" t="n">
-        <v>-167070045.9265256</v>
+        <v>7407376.859851267</v>
       </c>
       <c r="D78" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>90102554.08998811</v>
+        <v>383725.8459431626</v>
       </c>
       <c r="C79" t="n">
-        <v>-175916186.1970724</v>
+        <v>7592006.341748471</v>
       </c>
       <c r="D79" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>112423974.4583378</v>
+        <v>414435.8746544203</v>
       </c>
       <c r="C80" t="n">
-        <v>-203313461.5824972</v>
+        <v>7367652.856344703</v>
       </c>
       <c r="D80" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>110882036.2597607</v>
+        <v>412673.4235208518</v>
       </c>
       <c r="C81" t="n">
-        <v>-201588700.6533288</v>
+        <v>7382581.441586836</v>
       </c>
       <c r="D81" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>111720467.1438562</v>
+        <v>407314.2720218997</v>
       </c>
       <c r="C82" t="n">
-        <v>-202900885.8178033</v>
+        <v>7377190.661707142</v>
       </c>
       <c r="D82" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>112373855.7463913</v>
+        <v>723787.2073493205</v>
       </c>
       <c r="C83" t="n">
-        <v>-185556001.5893668</v>
+        <v>7248572.024052578</v>
       </c>
       <c r="D83" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>103127200.0445412</v>
+        <v>790262.1937427302</v>
       </c>
       <c r="C84" t="n">
-        <v>-172088483.342384</v>
+        <v>7317937.23898467</v>
       </c>
       <c r="D84" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>122708990.1519759</v>
+        <v>598663.1839319061</v>
       </c>
       <c r="C85" t="n">
-        <v>-203255148.1129821</v>
+        <v>7197091.63736374</v>
       </c>
       <c r="D85" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>111990891.5363045</v>
+        <v>405767.7027150932</v>
       </c>
       <c r="C86" t="n">
-        <v>-203312680.5100742</v>
+        <v>7375381.027371443</v>
       </c>
       <c r="D86" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>98870863.49995132</v>
+        <v>762480.8616364233</v>
       </c>
       <c r="C87" t="n">
-        <v>-168604253.3247996</v>
+        <v>7369402.187121131</v>
       </c>
       <c r="D87" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>107111037.3784975</v>
+        <v>439843.9287411383</v>
       </c>
       <c r="C88" t="n">
-        <v>-195472323.0756261</v>
+        <v>7406029.903836646</v>
       </c>
       <c r="D88" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>90346546.34698622</v>
+        <v>382271.6480455336</v>
       </c>
       <c r="C89" t="n">
-        <v>-176336811.5477049</v>
+        <v>7590211.624238232</v>
       </c>
       <c r="D89" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>102529579.9533198</v>
+        <v>402335.643714165</v>
       </c>
       <c r="C90" t="n">
-        <v>-191801156.5092006</v>
+        <v>7464744.675496253</v>
       </c>
       <c r="D90" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>90104528.73577157</v>
+        <v>383718.8813232478</v>
       </c>
       <c r="C91" t="n">
-        <v>-175919349.5840066</v>
+        <v>7591989.812414211</v>
       </c>
       <c r="D91" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>99291993.9236518</v>
+        <v>539831.0236638299</v>
       </c>
       <c r="C92" t="n">
-        <v>-180337878.069048</v>
+        <v>7440963.848228727</v>
       </c>
       <c r="D92" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>89515739.4878577</v>
+        <v>389353.0613288408</v>
       </c>
       <c r="C93" t="n">
-        <v>-174796657.0264485</v>
+        <v>7595463.263758845</v>
       </c>
       <c r="D93" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>90103705.07885629</v>
+        <v>383721.7863796732</v>
       </c>
       <c r="C94" t="n">
-        <v>-175918030.0872642</v>
+        <v>7591996.707043167</v>
       </c>
       <c r="D94" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>89565870.73928922</v>
+        <v>387990.2999005239</v>
       </c>
       <c r="C95" t="n">
-        <v>-174936500.8971657</v>
+        <v>7595529.493387843</v>
       </c>
       <c r="D95" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>105283796.2110587</v>
+        <v>669452.4467849245</v>
       </c>
       <c r="C96" t="n">
-        <v>-180789088.1050727</v>
+        <v>7336131.153987038</v>
       </c>
       <c r="D96" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>92663656.04225837</v>
+        <v>391429.212175432</v>
       </c>
       <c r="C97" t="n">
-        <v>-179135917.8359909</v>
+        <v>7563757.379410667</v>
       </c>
       <c r="D97" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>105995838.9598717</v>
+        <v>569239.5613440264</v>
       </c>
       <c r="C98" t="n">
-        <v>-186983408.2862068</v>
+        <v>7365353.885484916</v>
       </c>
       <c r="D98" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>111852843.7911268</v>
+        <v>404339.0276015802</v>
       </c>
       <c r="C99" t="n">
-        <v>-203232990.950353</v>
+        <v>7377267.93003197</v>
       </c>
       <c r="D99" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>108682011.9880013</v>
+        <v>426389.9074570178</v>
       </c>
       <c r="C100" t="n">
-        <v>-198149238.6850535</v>
+        <v>7397057.334183707</v>
       </c>
       <c r="D100" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>123262330.9647697</v>
+        <v>647260.2346404803</v>
       </c>
       <c r="C101" t="n">
-        <v>-200772585.0239061</v>
+        <v>7173046.349524124</v>
       </c>
       <c r="D101" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>95285337.07413501</v>
+        <v>422813.0446212821</v>
       </c>
       <c r="C102" t="n">
-        <v>-181128484.7188572</v>
+        <v>7525418.358305623</v>
       </c>
       <c r="D102" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>103205198.4397278</v>
+        <v>409920.3594865833</v>
       </c>
       <c r="C103" t="n">
-        <v>-192251246.9216498</v>
+        <v>7455181.222219932</v>
       </c>
       <c r="D103" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>106043189.6412067</v>
+        <v>469900.8002904762</v>
       </c>
       <c r="C104" t="n">
-        <v>-192486808.2343917</v>
+        <v>7403678.552845351</v>
       </c>
       <c r="D104" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>97110372.26147208</v>
+        <v>464459.3821369232</v>
       </c>
       <c r="C105" t="n">
-        <v>-181415844.8991398</v>
+        <v>7491066.084930793</v>
       </c>
       <c r="D105" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>131241033.4827757</v>
+        <v>366853.0474747586</v>
       </c>
       <c r="C106" t="n">
-        <v>-226689672.8295892</v>
+        <v>7220754.392227514</v>
       </c>
       <c r="D106" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>117129631.2220052</v>
+        <v>567174.9081824664</v>
       </c>
       <c r="C107" t="n">
-        <v>-199529950.2677192</v>
+        <v>7261232.535008149</v>
       </c>
       <c r="D107" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>94928926.66890271</v>
+        <v>397376.1849744547</v>
       </c>
       <c r="C108" t="n">
-        <v>-181961297.4746547</v>
+        <v>7539315.330421793</v>
       </c>
       <c r="D108" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>108290145.0312245</v>
+        <v>747622.3765616242</v>
       </c>
       <c r="C109" t="n">
-        <v>-179956136.3726603</v>
+        <v>7280326.687097363</v>
       </c>
       <c r="D109" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>88934308.95905775</v>
+        <v>450489.7582604677</v>
       </c>
       <c r="C110" t="n">
-        <v>-170947412.4750854</v>
+        <v>7576800.85477192</v>
       </c>
       <c r="D110" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>103972565.9586297</v>
+        <v>710339.3015028904</v>
       </c>
       <c r="C111" t="n">
-        <v>-177149054.5000275</v>
+        <v>7335141.778801956</v>
       </c>
       <c r="D111" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>112619817.770193</v>
+        <v>396053.62525233</v>
       </c>
       <c r="C112" t="n">
-        <v>-204631253.2676903</v>
+        <v>7373862.411237928</v>
       </c>
       <c r="D112" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>90460510.7681088</v>
+        <v>444704.7907449754</v>
       </c>
       <c r="C113" t="n">
-        <v>-173375849.083366</v>
+        <v>7563900.888378733</v>
       </c>
       <c r="D113" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>90322966.28199582</v>
+        <v>443363.6732012552</v>
       </c>
       <c r="C114" t="n">
-        <v>-173249850.8613234</v>
+        <v>7565788.758657504</v>
       </c>
       <c r="D114" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>127185375.7843002</v>
+        <v>367652.259629715</v>
       </c>
       <c r="C115" t="n">
-        <v>-222549344.2806582</v>
+        <v>7256028.81467634</v>
       </c>
       <c r="D115" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>104324543.1966155</v>
+        <v>669640.2285336041</v>
       </c>
       <c r="C116" t="n">
-        <v>-179677254.0545461</v>
+        <v>7345433.276130389</v>
       </c>
       <c r="D116" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>104886990.260056</v>
+        <v>600557.637797766</v>
       </c>
       <c r="C117" t="n">
-        <v>-183990122.8937142</v>
+        <v>7364421.865823336</v>
       </c>
       <c r="D117" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>120626767.3054073</v>
+        <v>600393.0921995796</v>
       </c>
       <c r="C118" t="n">
-        <v>-201107675.9514737</v>
+        <v>7215709.499915746</v>
       </c>
       <c r="D118" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>106253987.7411452</v>
+        <v>497782.9113988071</v>
       </c>
       <c r="C119" t="n">
-        <v>-191200737.3196173</v>
+        <v>7390496.471405526</v>
       </c>
       <c r="D119" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>93418613.15065667</v>
+        <v>436466.800330822</v>
       </c>
       <c r="C120" t="n">
-        <v>-177883619.6676927</v>
+        <v>7538074.706984714</v>
       </c>
       <c r="D120" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>90103152.92810416</v>
+        <v>383723.7338277422</v>
       </c>
       <c r="C121" t="n">
-        <v>-175917145.5400779</v>
+        <v>7592001.328981454</v>
       </c>
       <c r="D121" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>89440695.01134434</v>
+        <v>446965.5634673933</v>
       </c>
       <c r="C122" t="n">
-        <v>-171833818.660059</v>
+        <v>7573131.755081054</v>
       </c>
       <c r="D122" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>90056417.80823579</v>
+        <v>445475.1194111918</v>
       </c>
       <c r="C123" t="n">
-        <v>-172772092.1143855</v>
+        <v>7567601.635024867</v>
       </c>
       <c r="D123" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>112341383.2848444</v>
+        <v>621810.8103163663</v>
       </c>
       <c r="C124" t="n">
-        <v>-191251237.3799561</v>
+        <v>7285316.554902539</v>
       </c>
       <c r="D124" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>91638603.847031</v>
+        <v>453416.9831956982</v>
       </c>
       <c r="C125" t="n">
-        <v>-174580687.5775971</v>
+        <v>7548850.096561186</v>
       </c>
       <c r="D125" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>104041565.2928592</v>
+        <v>611592.6100460046</v>
       </c>
       <c r="C126" t="n">
-        <v>-182405013.0074969</v>
+        <v>7368598.606297649</v>
       </c>
       <c r="D126" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>98434944.37232505</v>
+        <v>828987.291295761</v>
       </c>
       <c r="C127" t="n">
-        <v>-164850226.8295321</v>
+        <v>7353960.948327379</v>
       </c>
       <c r="D127" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>90102346.77343935</v>
+        <v>383726.5771532588</v>
       </c>
       <c r="C128" t="n">
-        <v>-175915854.0738463</v>
+        <v>7592008.077162812</v>
       </c>
       <c r="D128" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>105297578.2185064</v>
+        <v>572065.6433788443</v>
       </c>
       <c r="C129" t="n">
-        <v>-186004423.6349301</v>
+        <v>7370981.487775771</v>
       </c>
       <c r="D129" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>91506333.97392675</v>
+        <v>570671.744298632</v>
       </c>
       <c r="C130" t="n">
-        <v>-168656066.0726092</v>
+        <v>7506660.864765343</v>
       </c>
       <c r="D130" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>100244385.6920507</v>
+        <v>539967.4751042218</v>
       </c>
       <c r="C131" t="n">
-        <v>-181532297.7965564</v>
+        <v>7431673.784536626</v>
       </c>
       <c r="D131" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>90930063.13631396</v>
+        <v>452174.9311583586</v>
       </c>
       <c r="C132" t="n">
-        <v>-173660181.4769069</v>
+        <v>7556332.266056828</v>
       </c>
       <c r="D132" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>89889286.84587127</v>
+        <v>384478.042694183</v>
       </c>
       <c r="C133" t="n">
-        <v>-175574363.7411091</v>
+        <v>7593792.795184806</v>
       </c>
       <c r="D133" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>102209313.6826625</v>
+        <v>472457.6527888828</v>
       </c>
       <c r="C134" t="n">
-        <v>-187581930.313654</v>
+        <v>7438943.410384167</v>
       </c>
       <c r="D134" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>105299421.9336895</v>
+        <v>796518.4161216137</v>
       </c>
       <c r="C135" t="n">
-        <v>-174154437.565182</v>
+        <v>7294240.829803186</v>
       </c>
       <c r="D135" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>94630554.37158425</v>
+        <v>439654.4736789956</v>
       </c>
       <c r="C136" t="n">
-        <v>-179373611.5363451</v>
+        <v>7524984.020991635</v>
       </c>
       <c r="D136" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>103648004.1509348</v>
+        <v>597874.7966290781</v>
       </c>
       <c r="C137" t="n">
-        <v>-182663034.0110876</v>
+        <v>7377365.426627968</v>
       </c>
       <c r="D137" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>98265994.57547078</v>
+        <v>507905.568870945</v>
       </c>
       <c r="C138" t="n">
-        <v>-180676396.8603028</v>
+        <v>7462990.403153609</v>
       </c>
       <c r="D138" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>119293100.639567</v>
+        <v>366329.6275398433</v>
       </c>
       <c r="C139" t="n">
-        <v>-214134830.6730939</v>
+        <v>7326783.189303711</v>
       </c>
       <c r="D139" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>108800112.9038873</v>
+        <v>456361.2898843428</v>
       </c>
       <c r="C140" t="n">
-        <v>-196583746.7168819</v>
+        <v>7383412.108057517</v>
       </c>
       <c r="D140" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>90651901.65778245</v>
+        <v>444657.8554364101</v>
       </c>
       <c r="C141" t="n">
-        <v>-173645533.7513208</v>
+        <v>7562025.921142353</v>
       </c>
       <c r="D141" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>109559722.9289189</v>
+        <v>672768.4835952614</v>
       </c>
       <c r="C142" t="n">
-        <v>-185388306.1858294</v>
+        <v>7293509.317555598</v>
       </c>
       <c r="D142" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>103634729.2958177</v>
+        <v>612182.4967714186</v>
       </c>
       <c r="C143" t="n">
-        <v>-181891542.7247275</v>
+        <v>7372330.057555402</v>
       </c>
       <c r="D143" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>93414706.53621852</v>
+        <v>728433.5137220931</v>
       </c>
       <c r="C144" t="n">
-        <v>-163614334.2863328</v>
+        <v>7435412.922395073</v>
       </c>
       <c r="D144" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>119403884.9223573</v>
+        <v>714304.8037613939</v>
       </c>
       <c r="C145" t="n">
-        <v>-193070738.2963331</v>
+        <v>7184478.611043642</v>
       </c>
       <c r="D145" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>91236690.37009616</v>
+        <v>439047.5535942831</v>
       </c>
       <c r="C146" t="n">
-        <v>-174739885.005937</v>
+        <v>7558462.652592706</v>
       </c>
       <c r="D146" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>107560206.4702901</v>
+        <v>433932.7497139967</v>
       </c>
       <c r="C147" t="n">
-        <v>-196355097.4582179</v>
+        <v>7404311.079104981</v>
       </c>
       <c r="D147" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>125912398.5125425</v>
+        <v>663250.528201481</v>
       </c>
       <c r="C148" t="n">
-        <v>-202194520.6540882</v>
+        <v>7142209.795338459</v>
       </c>
       <c r="D148" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>107664834.9478427</v>
+        <v>468998.8339806726</v>
       </c>
       <c r="C149" t="n">
-        <v>-194505661.1581519</v>
+        <v>7388821.772371144</v>
       </c>
       <c r="D149" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>96672242.48385458</v>
+        <v>436408.8218150658</v>
       </c>
       <c r="C150" t="n">
-        <v>-182290563.4259088</v>
+        <v>7506500.594720325</v>
       </c>
       <c r="D150" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>105035861.4768484</v>
+        <v>569006.5176380178</v>
       </c>
       <c r="C151" t="n">
-        <v>-185858100.2964173</v>
+        <v>7374633.408555133</v>
       </c>
       <c r="D151" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>129709496.8307995</v>
+        <v>376624.0866571964</v>
       </c>
       <c r="C152" t="n">
-        <v>-224507523.2811059</v>
+        <v>7229605.106066765</v>
       </c>
       <c r="D152" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>110112505.5368656</v>
+        <v>444385.7615036962</v>
       </c>
       <c r="C153" t="n">
-        <v>-198834921.7274409</v>
+        <v>7376206.848085475</v>
       </c>
       <c r="D153" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>95345408.76258494</v>
+        <v>431132.6180002625</v>
       </c>
       <c r="C154" t="n">
-        <v>-180780035.102492</v>
+        <v>7521465.612824399</v>
       </c>
       <c r="D154" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>119327644.5647107</v>
+        <v>584961.2195156019</v>
       </c>
       <c r="C155" t="n">
-        <v>-200737863.3305627</v>
+        <v>7233817.372569075</v>
       </c>
       <c r="D155" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>93428592.75277303</v>
+        <v>446157.5485860738</v>
       </c>
       <c r="C156" t="n">
-        <v>-177405817.098093</v>
+        <v>7534123.93820927</v>
       </c>
       <c r="D156" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>114371692.2541738</v>
+        <v>669236.5653518254</v>
       </c>
       <c r="C157" t="n">
-        <v>-190702731.3950348</v>
+        <v>7248640.712909578</v>
       </c>
       <c r="D157" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>104586949.9232588</v>
+        <v>777512.9831815676</v>
       </c>
       <c r="C158" t="n">
-        <v>-174359078.1543424</v>
+        <v>7307313.468056051</v>
       </c>
       <c r="D158" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>91749754.6950718</v>
+        <v>435487.6637338779</v>
       </c>
       <c r="C159" t="n">
-        <v>-175631204.4296953</v>
+        <v>7554822.370589631</v>
       </c>
       <c r="D159" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>125835557.693632</v>
+        <v>664861.8344592829</v>
       </c>
       <c r="C160" t="n">
-        <v>-202024111.6928512</v>
+        <v>7142306.853326681</v>
       </c>
       <c r="D160" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>116300547.405243</v>
+        <v>713772.8159372762</v>
       </c>
       <c r="C161" t="n">
-        <v>-190094256.5324488</v>
+        <v>7214284.154764948</v>
       </c>
       <c r="D161" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>107311224.3497591</v>
+        <v>439805.1538512177</v>
       </c>
       <c r="C162" t="n">
-        <v>-195719287.5035029</v>
+        <v>7404176.992680821</v>
       </c>
       <c r="D162" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>114562592.945937</v>
+        <v>647141.1239790823</v>
       </c>
       <c r="C163" t="n">
-        <v>-192167750.2243736</v>
+        <v>7254886.228397596</v>
       </c>
       <c r="D163" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>95010133.05762434</v>
+        <v>429836.6878292271</v>
       </c>
       <c r="C164" t="n">
-        <v>-180392714.7041181</v>
+        <v>7525240.43409429</v>
       </c>
       <c r="D164" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>116833037.3592419</v>
+        <v>714955.4111270539</v>
       </c>
       <c r="C165" t="n">
-        <v>-190550371.3754974</v>
+        <v>7208770.172444158</v>
       </c>
       <c r="D165" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>123867952.8791168</v>
+        <v>612695.2306431417</v>
       </c>
       <c r="C166" t="n">
-        <v>-203491291.7640728</v>
+        <v>7180841.293022046</v>
       </c>
       <c r="D166" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>94930873.93600039</v>
+        <v>431933.0220172554</v>
       </c>
       <c r="C167" t="n">
-        <v>-180177301.1360669</v>
+        <v>7525164.216234216</v>
       </c>
       <c r="D167" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>109024145.1125965</v>
+        <v>571477.7003448418</v>
       </c>
       <c r="C168" t="n">
-        <v>-190379985.0380221</v>
+        <v>7335667.556724924</v>
       </c>
       <c r="D168" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>122610651.9789469</v>
+        <v>725637.832248533</v>
       </c>
       <c r="C169" t="n">
-        <v>-195356301.638187</v>
+        <v>7149922.107346477</v>
       </c>
       <c r="D169" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>112012066.3744351</v>
+        <v>674219.4674038889</v>
       </c>
       <c r="C170" t="n">
-        <v>-187947443.025041</v>
+        <v>7269409.352310479</v>
       </c>
       <c r="D170" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>115464965.0687606</v>
+        <v>710749.5401521167</v>
       </c>
       <c r="C171" t="n">
-        <v>-189437112.6759949</v>
+        <v>7223356.075473163</v>
       </c>
       <c r="D171" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>123165218.7500279</v>
+        <v>593191.4187559042</v>
       </c>
       <c r="C172" t="n">
-        <v>-204035832.0819772</v>
+        <v>7195042.290479658</v>
       </c>
       <c r="D172" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>126035442.3380523</v>
+        <v>669087.1574735446</v>
       </c>
       <c r="C173" t="n">
-        <v>-201934946.3262615</v>
+        <v>7138823.143244307</v>
       </c>
       <c r="D173" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>103963286.9951731</v>
+        <v>576221.5915295435</v>
       </c>
       <c r="C174" t="n">
-        <v>-184189772.1687449</v>
+        <v>7382257.330581195</v>
       </c>
       <c r="D174" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>123167917.7093716</v>
+        <v>713603.1766074058</v>
       </c>
       <c r="C175" t="n">
-        <v>-196595593.1394584</v>
+        <v>7149041.025246967</v>
       </c>
       <c r="D175" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>125009597.6335431</v>
+        <v>575266.3307147442</v>
       </c>
       <c r="C176" t="n">
-        <v>-206928505.2360481</v>
+        <v>7185257.558376712</v>
       </c>
       <c r="D176" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>104729571.0001448</v>
+        <v>604290.0810529721</v>
       </c>
       <c r="C177" t="n">
-        <v>-183605424.8142278</v>
+        <v>7364583.701289264</v>
       </c>
       <c r="D177" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>108428450.8804912</v>
+        <v>432284.6912633065</v>
       </c>
       <c r="C178" t="n">
-        <v>-197505404.3038669</v>
+        <v>7396923.161243825</v>
       </c>
       <c r="D178" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>107513991.4400155</v>
+        <v>439758.1563198671</v>
       </c>
       <c r="C179" t="n">
-        <v>-195969432.9036126</v>
+        <v>7402304.535486695</v>
       </c>
       <c r="D179" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>119549321.5548093</v>
+        <v>455576.2169239347</v>
       </c>
       <c r="C180" t="n">
-        <v>-208864742.2065115</v>
+        <v>7284936.716519298</v>
       </c>
       <c r="D180" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
Fixing new UTM origin
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -2006,13 +2006,13 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>760472.461105651</v>
+        <v>492554.167607569</v>
       </c>
       <c r="C15" t="n">
-        <v>7374813.666059652</v>
+        <v>7362660.522732426</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2784,13 +2784,13 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>656030.3435174299</v>
+        <v>370886.1153907846</v>
       </c>
       <c r="C22" t="n">
-        <v>7188356.034972786</v>
+        <v>7187079.827136386</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -3448,13 +3448,13 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>718950.8143728292</v>
+        <v>437406.5712702282</v>
       </c>
       <c r="C28" t="n">
-        <v>7229561.330213139</v>
+        <v>7222126.94299706</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -3562,13 +3562,13 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>689479.0599372458</v>
+        <v>422986.9243510979</v>
       </c>
       <c r="C29" t="n">
-        <v>7385840.555939897</v>
+        <v>7380433.667829104</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -4230,13 +4230,13 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>648062.4098775064</v>
+        <v>359926.7544846291</v>
       </c>
       <c r="C35" t="n">
-        <v>7156317.765654799</v>
+        <v>7155939.858273401</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -4458,13 +4458,13 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>679482.7733917895</v>
+        <v>412438.6987697054</v>
       </c>
       <c r="C37" t="n">
-        <v>7379568.764875205</v>
+        <v>7375151.327213982</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -4568,13 +4568,13 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>697218.2558684414</v>
+        <v>428238.5071148447</v>
       </c>
       <c r="C38" t="n">
-        <v>7360280.072632506</v>
+        <v>7354259.285437998</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -6066,13 +6066,13 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>778993.4381261227</v>
+        <v>503826.2769704363</v>
       </c>
       <c r="C51" t="n">
-        <v>7299986.83529006</v>
+        <v>7286473.625834247</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -6966,13 +6966,13 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>705283.5520898863</v>
+        <v>436495.8036802044</v>
       </c>
       <c r="C59" t="n">
-        <v>7362709.877786176</v>
+        <v>7355904.770488945</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -7414,13 +7414,13 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>754559.5701349006</v>
+        <v>485011.9113935289</v>
       </c>
       <c r="C63" t="n">
-        <v>7357457.446217685</v>
+        <v>7345964.095974515</v>
       </c>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -7760,13 +7760,13 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>793848.6559708756</v>
+        <v>517672.7437221066</v>
       </c>
       <c r="C66" t="n">
-        <v>7290260.126774631</v>
+        <v>7275386.24794451</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -7988,13 +7988,13 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>705411.5012919909</v>
+        <v>438412.035778083</v>
       </c>
       <c r="C68" t="n">
-        <v>7381384.438635441</v>
+        <v>7374472.407213761</v>
       </c>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -8102,13 +8102,13 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>827178.5078480255</v>
+        <v>556512.5125755423</v>
       </c>
       <c r="C69" t="n">
-        <v>7350027.173207692</v>
+        <v>7331631.883061054</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -8216,13 +8216,13 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>704315.0658106438</v>
+        <v>432852.8741623109</v>
       </c>
       <c r="C70" t="n">
-        <v>7334696.005952516</v>
+        <v>7328124.929287304</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -9120,13 +9120,13 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>727838.3447125108</v>
+        <v>463216.6637994376</v>
       </c>
       <c r="C78" t="n">
-        <v>7407376.859851267</v>
+        <v>7398179.292258396</v>
       </c>
       <c r="D78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -9686,13 +9686,13 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>723787.2073493205</v>
+        <v>444022.4882063934</v>
       </c>
       <c r="C83" t="n">
-        <v>7248572.024052578</v>
+        <v>7240582.251511294</v>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -9796,13 +9796,13 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>790262.1937427302</v>
+        <v>516743.6205052369</v>
       </c>
       <c r="C84" t="n">
-        <v>7317937.23898467</v>
+        <v>7303250.25192572</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -10130,13 +10130,13 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>762480.8616364233</v>
+        <v>494033.4719075484</v>
       </c>
       <c r="C87" t="n">
-        <v>7369402.187121131</v>
+        <v>7357086.139395674</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -11140,13 +11140,13 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>669452.4467849245</v>
+        <v>398298.9085244702</v>
       </c>
       <c r="C96" t="n">
-        <v>7336131.153987038</v>
+        <v>7332884.851021027</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -11706,13 +11706,13 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>647260.2346404803</v>
+        <v>360708.1992064052</v>
       </c>
       <c r="C101" t="n">
-        <v>7173046.349524124</v>
+        <v>7172668.952609244</v>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -12622,13 +12622,13 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>747622.3765616242</v>
+        <v>470752.5219873611</v>
       </c>
       <c r="C109" t="n">
-        <v>7280326.687097363</v>
+        <v>7269906.412785889</v>
       </c>
       <c r="D109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -12854,13 +12854,13 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>710339.3015028904</v>
+        <v>438889.2608200699</v>
       </c>
       <c r="C111" t="n">
-        <v>7335141.778801956</v>
+        <v>7327992.830638899</v>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -13416,13 +13416,13 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>669640.2285336041</v>
+        <v>399375.2583278379</v>
       </c>
       <c r="C116" t="n">
-        <v>7345433.276130389</v>
+        <v>7342124.276286863</v>
       </c>
       <c r="D116" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -14650,13 +14650,13 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>828987.291295761</v>
+        <v>558686.708602804</v>
       </c>
       <c r="C127" t="n">
-        <v>7353960.948327379</v>
+        <v>7335369.709418677</v>
       </c>
       <c r="D127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -15562,13 +15562,13 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>796518.4161216137</v>
+        <v>520706.5159229873</v>
       </c>
       <c r="C135" t="n">
-        <v>7294240.829803186</v>
+        <v>7279090.447065596</v>
       </c>
       <c r="D135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -16356,13 +16356,13 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>672768.4835952614</v>
+        <v>397530.8865128363</v>
       </c>
       <c r="C142" t="n">
-        <v>7293509.317555598</v>
+        <v>7290150.983906416</v>
       </c>
       <c r="D142" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -16584,13 +16584,13 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>728433.5137220931</v>
+        <v>466502.8775897114</v>
       </c>
       <c r="C144" t="n">
-        <v>7435412.922395073</v>
+        <v>7426010.897140203</v>
       </c>
       <c r="D144" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -16698,13 +16698,13 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>714304.8037613939</v>
+        <v>428515.3844426512</v>
       </c>
       <c r="C145" t="n">
-        <v>7184478.611043642</v>
+        <v>7177710.160828887</v>
       </c>
       <c r="D145" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -17036,13 +17036,13 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>663250.528201481</v>
+        <v>373715.0621996796</v>
       </c>
       <c r="C148" t="n">
-        <v>7142209.795338459</v>
+        <v>7140463.167019151</v>
       </c>
       <c r="D148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -18038,13 +18038,13 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>669236.5653518254</v>
+        <v>389746.2694711213</v>
       </c>
       <c r="C157" t="n">
-        <v>7248640.712909578</v>
+        <v>7245831.948977302</v>
       </c>
       <c r="D157" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -18148,13 +18148,13 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>777512.9831815676</v>
+        <v>503052.1425778663</v>
       </c>
       <c r="C158" t="n">
-        <v>7307313.468056051</v>
+        <v>7293901.021924582</v>
       </c>
       <c r="D158" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -18376,13 +18376,13 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>664861.8344592829</v>
+        <v>375328.1206457481</v>
       </c>
       <c r="C160" t="n">
-        <v>7142306.853326681</v>
+        <v>7140407.869943817</v>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -18490,13 +18490,13 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>713772.8159372762</v>
+        <v>430806.5620925381</v>
       </c>
       <c r="C161" t="n">
-        <v>7214284.154764948</v>
+        <v>7207417.315247957</v>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -18718,13 +18718,13 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>647141.1239790823</v>
+        <v>368347.2212977612</v>
       </c>
       <c r="C163" t="n">
-        <v>7254886.228397596</v>
+        <v>7254148.289168184</v>
       </c>
       <c r="D163" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -18938,13 +18938,13 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>714955.4111270539</v>
+        <v>431460.9907259208</v>
       </c>
       <c r="C165" t="n">
-        <v>7208770.172444158</v>
+        <v>7201818.906944926</v>
       </c>
       <c r="D165" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -19382,13 +19382,13 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>725637.832248533</v>
+        <v>436529.4858061953</v>
       </c>
       <c r="C169" t="n">
-        <v>7149922.107346477</v>
+        <v>7142256.750001465</v>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -19496,13 +19496,13 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>674219.4674038889</v>
+        <v>396680.0496550673</v>
       </c>
       <c r="C170" t="n">
-        <v>7269409.352310479</v>
+        <v>7266028.146615055</v>
       </c>
       <c r="D170" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -19606,13 +19606,13 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>710749.5401521167</v>
+        <v>428658.0909905289</v>
       </c>
       <c r="C171" t="n">
-        <v>7223356.075473163</v>
+        <v>7216730.436064484</v>
       </c>
       <c r="D171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -19830,13 +19830,13 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>669087.1574735446</v>
+        <v>379205.5803994216</v>
       </c>
       <c r="C173" t="n">
-        <v>7138823.143244307</v>
+        <v>7136541.931148331</v>
       </c>
       <c r="D173" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -20058,13 +20058,13 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>713603.1766074058</v>
+        <v>424471.7906746557</v>
       </c>
       <c r="C175" t="n">
-        <v>7149041.025246967</v>
+        <v>7142514.671104215</v>
       </c>
       <c r="D175" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
adjusting the critical distance
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>422823.0001388173</v>
+        <v>105508726.4694378</v>
       </c>
       <c r="C2" t="n">
-        <v>7525442.527047326</v>
+        <v>-209018146.6045218</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>451013.4314993119</v>
+        <v>132646577.4596441</v>
       </c>
       <c r="C3" t="n">
-        <v>7286868.704686873</v>
+        <v>-241504486.6946509</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>594545.9850944348</v>
+        <v>116529554.7152026</v>
       </c>
       <c r="C4" t="n">
-        <v>7366095.350358819</v>
+        <v>-213442943.3238954</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>403945.0768397648</v>
+        <v>106092782.3304012</v>
       </c>
       <c r="C5" t="n">
-        <v>7527910.87798272</v>
+        <v>-210929361.0420707</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>401216.148465685</v>
+        <v>105991829.6311245</v>
       </c>
       <c r="C6" t="n">
-        <v>7529882.125589605</v>
+        <v>-210946344.5005981</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>409155.6666583589</v>
+        <v>122395754.4997257</v>
       </c>
       <c r="C7" t="n">
-        <v>7388267.661607112</v>
+        <v>-232183773.5343286</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>408788.64986577</v>
+        <v>106102412.26284</v>
       </c>
       <c r="C8" t="n">
-        <v>7525883.127678607</v>
+        <v>-210661424.2871895</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>573609.5498119397</v>
+        <v>117040622.1587794</v>
       </c>
       <c r="C9" t="n">
-        <v>7369187.59580075</v>
+        <v>-215321766.9774082</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>395739.2028744464</v>
+        <v>103861518.1174055</v>
       </c>
       <c r="C10" t="n">
-        <v>7550553.333618967</v>
+        <v>-208247002.9008795</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>595482.5194309736</v>
+        <v>117134202.8675836</v>
       </c>
       <c r="C11" t="n">
-        <v>7360555.884229297</v>
+        <v>-214123845.5357292</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>570295.7162984037</v>
+        <v>138056256.2293121</v>
       </c>
       <c r="C12" t="n">
-        <v>7194426.892189107</v>
+        <v>-238975883.2737637</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>507596.7447241906</v>
+        <v>127395291.6096901</v>
       </c>
       <c r="C13" t="n">
-        <v>7306910.773843632</v>
+        <v>-231756331.7183017</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>429046.3551782307</v>
+        <v>102692553.5673765</v>
       </c>
       <c r="C14" t="n">
-        <v>7547568.77555988</v>
+        <v>-204683855.8293287</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>492554.167607569</v>
+        <v>109438266.882265</v>
       </c>
       <c r="C15" t="n">
-        <v>7362660.522732426</v>
+        <v>-195287931.0485279</v>
       </c>
       <c r="D15" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>586409.6389365081</v>
+        <v>138596224.7624223</v>
       </c>
       <c r="C16" t="n">
-        <v>7183700.825286468</v>
+        <v>-238383033.7740149</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>518399.5160626545</v>
+        <v>130020051.2517149</v>
       </c>
       <c r="C17" t="n">
-        <v>7280948.900331907</v>
+        <v>-234012094.1658826</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>447691.7230347765</v>
+        <v>134644140.8865899</v>
       </c>
       <c r="C18" t="n">
-        <v>7272079.333575497</v>
+        <v>-243949740.2878812</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>641757.8655294247</v>
+        <v>139608841.0539081</v>
       </c>
       <c r="C19" t="n">
-        <v>7154179.916507507</v>
+        <v>-235476230.8749945</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>420719.6780329063</v>
+        <v>105596981.9961531</v>
       </c>
       <c r="C20" t="n">
-        <v>7525508.513714559</v>
+        <v>-209263009.2431625</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>620437.5570446817</v>
+        <v>141599423.6154124</v>
       </c>
       <c r="C21" t="n">
-        <v>7145829.711649289</v>
+        <v>-238858232.1724758</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>370886.1153907846</v>
+        <v>134875384.7845174</v>
       </c>
       <c r="C22" t="n">
-        <v>7187079.827136386</v>
+        <v>-229901430.6513903</v>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>405491.2708980456</v>
+        <v>105594822.7153038</v>
       </c>
       <c r="C23" t="n">
-        <v>7531595.912204068</v>
+        <v>-210140147.9385734</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>404713.2604548364</v>
+        <v>105845394.8503075</v>
       </c>
       <c r="C24" t="n">
-        <v>7529740.381576492</v>
+        <v>-210537490.5371626</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>568072.7130961117</v>
+        <v>134781258.9465282</v>
       </c>
       <c r="C25" t="n">
-        <v>7222234.914685098</v>
+        <v>-235788498.9133089</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>553955.6541633958</v>
+        <v>125182348.8449171</v>
       </c>
       <c r="C26" t="n">
-        <v>7307428.943578887</v>
+        <v>-226212495.6601892</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>413821.4916065777</v>
+        <v>105460556.4692007</v>
       </c>
       <c r="C27" t="n">
-        <v>7529429.834138079</v>
+        <v>-209469655.8274356</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>437406.5712702282</v>
+        <v>127417554.1764413</v>
       </c>
       <c r="C28" t="n">
-        <v>7222126.94299706</v>
+        <v>-218170442.130488</v>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>422986.9243510979</v>
+        <v>110635064.8260035</v>
       </c>
       <c r="C29" t="n">
-        <v>7380433.667829104</v>
+        <v>-200693955.3049799</v>
       </c>
       <c r="D29" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>640364.9592321715</v>
+        <v>136104466.1075085</v>
       </c>
       <c r="C30" t="n">
-        <v>7183844.981620431</v>
+        <v>-232184709.8015506</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>568065.8525246648</v>
+        <v>134783690.3161738</v>
       </c>
       <c r="C31" t="n">
-        <v>7222217.524079368</v>
+        <v>-235791494.57205</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>408978.8275499512</v>
+        <v>105451235.8885704</v>
       </c>
       <c r="C32" t="n">
-        <v>7531442.590570908</v>
+        <v>-209736329.8344363</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>432660.8029019876</v>
+        <v>133553287.5962651</v>
       </c>
       <c r="C33" t="n">
-        <v>7287266.453172042</v>
+        <v>-243785214.8407176</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>402680.6572135365</v>
+        <v>105716464.7564075</v>
       </c>
       <c r="C34" t="n">
-        <v>7531672.625937978</v>
+        <v>-210474208.3568346</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>359926.7544846291</v>
+        <v>139066872.48509</v>
       </c>
       <c r="C35" t="n">
-        <v>7155939.858273401</v>
+        <v>-234520873.5788515</v>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>585517.9007419647</v>
+        <v>138187606.9388872</v>
       </c>
       <c r="C36" t="n">
-        <v>7187408.106334507</v>
+        <v>-238041235.5106107</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>412438.6987697054</v>
+        <v>111701037.9983043</v>
       </c>
       <c r="C37" t="n">
-        <v>7375151.327213982</v>
+        <v>-202577032.8259242</v>
       </c>
       <c r="D37" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>428238.5071148447</v>
+        <v>113236264.3979196</v>
       </c>
       <c r="C38" t="n">
-        <v>7354259.285437998</v>
+        <v>-203448141.3676558</v>
       </c>
       <c r="D38" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>385901.2558721581</v>
+        <v>102773319.0900762</v>
       </c>
       <c r="C39" t="n">
-        <v>7564001.44550652</v>
+        <v>-207250826.245541</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>424332.5844982759</v>
+        <v>105017672.2254655</v>
       </c>
       <c r="C40" t="n">
-        <v>7529112.568427877</v>
+        <v>-208242418.4061436</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>569643.0684379223</v>
+        <v>134701314.1507206</v>
       </c>
       <c r="C41" t="n">
-        <v>7222285.613839785</v>
+        <v>-235598052.3902366</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>402406.4354549267</v>
+        <v>104439268.9421774</v>
       </c>
       <c r="C42" t="n">
-        <v>7542852.907356113</v>
+        <v>-208685705.4748633</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>437023.185092857</v>
+        <v>104063185.0347636</v>
       </c>
       <c r="C43" t="n">
-        <v>7532468.581112547</v>
+        <v>-206174733.721487</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>593001.3245233108</v>
+        <v>116381563.0254742</v>
       </c>
       <c r="C44" t="n">
-        <v>7367918.094725985</v>
+        <v>-213354002.2535594</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>439224.5486118381</v>
+        <v>100167826.3336622</v>
       </c>
       <c r="C45" t="n">
-        <v>7565894.75324164</v>
+        <v>-200491735.4238619</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>401842.916054123</v>
+        <v>106181608.3227286</v>
       </c>
       <c r="C46" t="n">
-        <v>7527990.288472353</v>
+        <v>-211176252.3923558</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>388715.6373236501</v>
+        <v>104367728.3348256</v>
       </c>
       <c r="C47" t="n">
-        <v>7548996.648429874</v>
+        <v>-209373254.1300425</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>433477.7838170429</v>
+        <v>104424001.3408905</v>
       </c>
       <c r="C48" t="n">
-        <v>7530698.264778861</v>
+        <v>-206884594.4189475</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>590088.3297374767</v>
+        <v>137283281.5320168</v>
       </c>
       <c r="C49" t="n">
-        <v>7193087.563682824</v>
+        <v>-236821997.8006023</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>421309.4212496581</v>
+        <v>106000975.046599</v>
       </c>
       <c r="C50" t="n">
-        <v>7521773.247238778</v>
+        <v>-209794092.8900959</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>503826.2769704363</v>
+        <v>117159326.3814496</v>
       </c>
       <c r="C51" t="n">
-        <v>7286473.625834247</v>
+        <v>-203346207.1822138</v>
       </c>
       <c r="D51" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>410340.4763310733</v>
+        <v>123465584.6433238</v>
       </c>
       <c r="C52" t="n">
-        <v>7378952.937187641</v>
+        <v>-233430269.622158</v>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>463408.7043260257</v>
+        <v>130665300.368854</v>
       </c>
       <c r="C53" t="n">
-        <v>7297853.838466587</v>
+        <v>-238428189.4724956</v>
       </c>
       <c r="D53" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>444667.0044273772</v>
+        <v>100367178.8657337</v>
       </c>
       <c r="C54" t="n">
-        <v>7562048.963216691</v>
+        <v>-200478489.6620883</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>421470.9503357491</v>
+        <v>105352880.5020434</v>
       </c>
       <c r="C55" t="n">
-        <v>7527329.485975892</v>
+        <v>-208877513.5332501</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>526067.6630022393</v>
+        <v>129647122.8856552</v>
       </c>
       <c r="C56" t="n">
-        <v>7281008.696502964</v>
+        <v>-233086310.6818279</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>384404.2276939754</v>
+        <v>99652515.60497172</v>
       </c>
       <c r="C57" t="n">
-        <v>7591962.608249241</v>
+        <v>-202793563.913616</v>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>414448.1731552719</v>
+        <v>124626453.9291485</v>
       </c>
       <c r="C58" t="n">
-        <v>7367681.028654348</v>
+        <v>-234583616.9577389</v>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>436495.8036802044</v>
+        <v>112672866.8429443</v>
       </c>
       <c r="C59" t="n">
-        <v>7355904.770488945</v>
+        <v>-202306174.8753476</v>
       </c>
       <c r="D59" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>428504.0728901725</v>
+        <v>120818759.6407465</v>
       </c>
       <c r="C60" t="n">
-        <v>7393290.601893418</v>
+        <v>-228976588.5435393</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>364167.4705087786</v>
+        <v>136059248.6204675</v>
       </c>
       <c r="C61" t="n">
-        <v>7297116.842234123</v>
+        <v>-251416086.562739</v>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>590092.4094163297</v>
+        <v>137281823.6174914</v>
       </c>
       <c r="C62" t="n">
-        <v>7193098.011324367</v>
+        <v>-236820256.6947784</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>485011.9113935289</v>
+        <v>111557958.197442</v>
       </c>
       <c r="C63" t="n">
-        <v>7345964.095974515</v>
+        <v>-198188443.8184662</v>
       </c>
       <c r="D63" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>415018.0448537197</v>
+        <v>122342850.5698752</v>
       </c>
       <c r="C64" t="n">
-        <v>7386252.235449532</v>
+        <v>-231739329.838951</v>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>393866.9952033143</v>
+        <v>113504335.765346</v>
       </c>
       <c r="C65" t="n">
-        <v>7468780.921490044</v>
+        <v>-221679853.6071709</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>517672.7437221066</v>
+        <v>117746875.3597333</v>
       </c>
       <c r="C66" t="n">
-        <v>7275386.24794451</v>
+        <v>-203145161.1829448</v>
       </c>
       <c r="D66" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>410337.1139574873</v>
+        <v>123466691.2825127</v>
       </c>
       <c r="C67" t="n">
-        <v>7378945.240007831</v>
+        <v>-233431851.2426446</v>
       </c>
       <c r="D67" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>438412.035778083</v>
+        <v>110571376.8817002</v>
       </c>
       <c r="C68" t="n">
-        <v>7374472.407213761</v>
+        <v>-199724522.8641171</v>
       </c>
       <c r="D68" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>556512.5125755423</v>
+        <v>110055601.0016471</v>
       </c>
       <c r="C69" t="n">
-        <v>7331631.883061054</v>
+        <v>-192394145.9747593</v>
       </c>
       <c r="D69" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>432852.8741623109</v>
+        <v>115877033.3297141</v>
       </c>
       <c r="C70" t="n">
-        <v>7328124.929287304</v>
+        <v>-206198179.3881435</v>
       </c>
       <c r="D70" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>622134.3892227954</v>
+        <v>130111079.5130356</v>
       </c>
       <c r="C71" t="n">
-        <v>7240708.73367288</v>
+        <v>-227255961.6400539</v>
       </c>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>420714.5822642142</v>
+        <v>105598637.6146314</v>
       </c>
       <c r="C72" t="n">
-        <v>7525496.171109289</v>
+        <v>-209265622.4662407</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>568070.8652271603</v>
+        <v>134781913.8277764</v>
       </c>
       <c r="C73" t="n">
-        <v>7222230.230568401</v>
+        <v>-235789305.7885106</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>517897.6597152865</v>
+        <v>120457917.0446891</v>
       </c>
       <c r="C74" t="n">
-        <v>7360848.522584329</v>
+        <v>-222901472.9667384</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>402334.5145603271</v>
+        <v>104656956.3492973</v>
       </c>
       <c r="C75" t="n">
-        <v>7540991.602727064</v>
+        <v>-208998483.7739748</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>572359.5505096086</v>
+        <v>140447377.957341</v>
       </c>
       <c r="C76" t="n">
-        <v>7174025.31142854</v>
+        <v>-241190465.6660586</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>632953.2160392514</v>
+        <v>127382852.6466472</v>
       </c>
       <c r="C77" t="n">
-        <v>7259778.363588417</v>
+        <v>-223616842.4244619</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>463216.6637994376</v>
+        <v>106918502.4314488</v>
       </c>
       <c r="C78" t="n">
-        <v>7398179.292258396</v>
+        <v>-193926183.2665913</v>
       </c>
       <c r="D78" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>383725.8459431626</v>
+        <v>99678515.17212091</v>
       </c>
       <c r="C79" t="n">
-        <v>7592006.341748471</v>
+        <v>-202869844.3416095</v>
       </c>
       <c r="D79" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>414435.8746544203</v>
+        <v>124630512.6759802</v>
       </c>
       <c r="C80" t="n">
-        <v>7367652.856344703</v>
+        <v>-234589366.480262</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>412673.4235208518</v>
+        <v>122906404.1367475</v>
       </c>
       <c r="C81" t="n">
-        <v>7382581.441586836</v>
+        <v>-232588847.2752898</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>407314.2720218997</v>
+        <v>123834612.5745275</v>
       </c>
       <c r="C82" t="n">
-        <v>7377190.661707142</v>
+        <v>-234081588.0408616</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>444022.4882063934</v>
+        <v>125024745.8866452</v>
       </c>
       <c r="C83" t="n">
-        <v>7240582.251511294</v>
+        <v>-215332164.6101156</v>
       </c>
       <c r="D83" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>516743.6205052369</v>
+        <v>114770796.1817679</v>
       </c>
       <c r="C84" t="n">
-        <v>7303250.25192572</v>
+        <v>-199968539.1906832</v>
       </c>
       <c r="D84" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>598663.1839319061</v>
+        <v>136399735.7707716</v>
       </c>
       <c r="C85" t="n">
-        <v>7197091.63736374</v>
+        <v>-235342743.6443977</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>405767.7027150932</v>
+        <v>124134250.592144</v>
       </c>
       <c r="C86" t="n">
-        <v>7375381.027371443</v>
+        <v>-234550627.4243446</v>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>494033.4719075484</v>
+        <v>109970644.6036005</v>
       </c>
       <c r="C87" t="n">
-        <v>7357086.139395674</v>
+        <v>-195827838.7745652</v>
       </c>
       <c r="D87" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>439843.9287411383</v>
+        <v>118735399.5336341</v>
       </c>
       <c r="C88" t="n">
-        <v>7406029.903836646</v>
+        <v>-225639454.349205</v>
       </c>
       <c r="D88" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>382271.6480455336</v>
+        <v>99948772.93257391</v>
       </c>
       <c r="C89" t="n">
-        <v>7590211.624238232</v>
+        <v>-203348593.3003232</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>402335.643714165</v>
+        <v>113568385.9032365</v>
       </c>
       <c r="C90" t="n">
-        <v>7464744.675496253</v>
+        <v>-221247347.6185689</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>383718.8813232478</v>
+        <v>99680708.61797616</v>
       </c>
       <c r="C91" t="n">
-        <v>7591989.812414211</v>
+        <v>-202873459.8895674</v>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>539831.0236638299</v>
+        <v>110142394.5216578</v>
       </c>
       <c r="C92" t="n">
-        <v>7440963.848228727</v>
+        <v>-208562628.9073775</v>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>389353.0613288408</v>
+        <v>99031260.30550426</v>
       </c>
       <c r="C93" t="n">
-        <v>7595463.263758845</v>
+        <v>-201602192.2960845</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>383721.7863796732</v>
+        <v>99679793.69599606</v>
       </c>
       <c r="C94" t="n">
-        <v>7591996.707043167</v>
+        <v>-202871951.7895998</v>
       </c>
       <c r="D94" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>387990.2999005239</v>
+        <v>99085419.68022577</v>
       </c>
       <c r="C95" t="n">
-        <v>7595529.493387843</v>
+        <v>-201758063.0948648</v>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>398298.9085244702</v>
+        <v>117016909.536118</v>
       </c>
       <c r="C96" t="n">
-        <v>7332884.851021027</v>
+        <v>-209587252.9708545</v>
       </c>
       <c r="D96" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>391429.212175432</v>
+        <v>102545355.9689802</v>
       </c>
       <c r="C97" t="n">
-        <v>7563757.379410667</v>
+        <v>-206606667.7502118</v>
       </c>
       <c r="D97" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>569239.5613440264</v>
+        <v>117672836.3618993</v>
       </c>
       <c r="C98" t="n">
-        <v>7365353.885484916</v>
+        <v>-216358649.6340961</v>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>404339.0276015802</v>
+        <v>123978034.8062271</v>
       </c>
       <c r="C99" t="n">
-        <v>7377267.93003197</v>
+        <v>-234452325.5146987</v>
       </c>
       <c r="D99" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>426389.9074570178</v>
+        <v>120470081.3920262</v>
       </c>
       <c r="C100" t="n">
-        <v>7397057.334183707</v>
+        <v>-228674520.3612784</v>
       </c>
       <c r="D100" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>360708.1992064052</v>
+        <v>137093107.2131552</v>
       </c>
       <c r="C101" t="n">
-        <v>7172668.952609244</v>
+        <v>-232680201.6958987</v>
       </c>
       <c r="D101" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>422813.0446212821</v>
+        <v>105511964.562603</v>
       </c>
       <c r="C102" t="n">
-        <v>7525418.358305623</v>
+        <v>-209023256.3673792</v>
       </c>
       <c r="D102" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>409920.3594865833</v>
+        <v>114333012.3162275</v>
       </c>
       <c r="C103" t="n">
-        <v>7455181.222219932</v>
+        <v>-221797612.6148877</v>
       </c>
       <c r="D103" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>469900.8002904762</v>
+        <v>117585726.1880774</v>
       </c>
       <c r="C104" t="n">
-        <v>7403678.552845351</v>
+        <v>-222315825.1105521</v>
       </c>
       <c r="D104" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>464459.3821369232</v>
+        <v>107604625.910323</v>
       </c>
       <c r="C105" t="n">
-        <v>7491066.084930793</v>
+        <v>-209515713.5931183</v>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>366853.0474747586</v>
+        <v>145569466.401966</v>
       </c>
       <c r="C106" t="n">
-        <v>7220754.392227514</v>
+        <v>-261425231.6330547</v>
       </c>
       <c r="D106" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>567174.9081824664</v>
+        <v>130113878.5378258</v>
       </c>
       <c r="C107" t="n">
-        <v>7261232.535008149</v>
+        <v>-230877998.5930108</v>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>397376.1849744547</v>
+        <v>105080389.1113953</v>
       </c>
       <c r="C108" t="n">
-        <v>7539315.330421793</v>
+        <v>-209884292.3578205</v>
       </c>
       <c r="D108" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>470752.5219873611</v>
+        <v>120489265.4427217</v>
       </c>
       <c r="C109" t="n">
-        <v>7269906.412785889</v>
+        <v>-208929469.54725</v>
       </c>
       <c r="D109" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>450489.7582604677</v>
+        <v>98461024.83522852</v>
       </c>
       <c r="C110" t="n">
-        <v>7576800.85477192</v>
+        <v>-197396514.180316</v>
       </c>
       <c r="D110" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>438889.2608200699</v>
+        <v>115607022.0688982</v>
       </c>
       <c r="C111" t="n">
-        <v>7327992.830638899</v>
+        <v>-205529791.2928719</v>
       </c>
       <c r="D111" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>396053.62525233</v>
+        <v>124822083.9285265</v>
       </c>
       <c r="C112" t="n">
-        <v>7373862.411237928</v>
+        <v>-236031568.2958097</v>
       </c>
       <c r="D112" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>444704.7907449754</v>
+        <v>100156661.0837503</v>
       </c>
       <c r="C113" t="n">
-        <v>7563900.888378733</v>
+        <v>-200172776.0156584</v>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>443363.6732012552</v>
+        <v>100001447.5327858</v>
       </c>
       <c r="C114" t="n">
-        <v>7565788.758657504</v>
+        <v>-200022630.0171967</v>
       </c>
       <c r="D114" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>367652.259629715</v>
+        <v>141041486.155849</v>
       </c>
       <c r="C115" t="n">
-        <v>7256028.81467634</v>
+        <v>-256629137.1601039</v>
       </c>
       <c r="D115" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>399375.2583278379</v>
+        <v>115944493.4328775</v>
       </c>
       <c r="C116" t="n">
-        <v>7342124.276286863</v>
+        <v>-208300507.8710816</v>
       </c>
       <c r="D116" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>600557.637797766</v>
+        <v>116477400.184276</v>
       </c>
       <c r="C117" t="n">
-        <v>7364421.865823336</v>
+        <v>-213021100.7277543</v>
       </c>
       <c r="D117" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>600393.0921995796</v>
+        <v>134073855.6473529</v>
       </c>
       <c r="C118" t="n">
-        <v>7215709.499915746</v>
+        <v>-232856329.5791467</v>
       </c>
       <c r="D118" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>497782.9113988071</v>
+        <v>117860571.0843874</v>
       </c>
       <c r="C119" t="n">
-        <v>7390496.471405526</v>
+        <v>-220944422.1572055</v>
       </c>
       <c r="D119" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>436466.800330822</v>
+        <v>103446922.0606982</v>
       </c>
       <c r="C120" t="n">
-        <v>7538074.706984714</v>
+        <v>-205335959.0468844</v>
       </c>
       <c r="D120" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>383723.7338277422</v>
+        <v>99679180.36433366</v>
       </c>
       <c r="C121" t="n">
-        <v>7592001.328981454</v>
+        <v>-202870940.8090142</v>
       </c>
       <c r="D121" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>446965.5634673933</v>
+        <v>99021577.51894188</v>
       </c>
       <c r="C122" t="n">
-        <v>7573131.755081054</v>
+        <v>-198404658.9435754</v>
       </c>
       <c r="D122" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>445475.1194111918</v>
+        <v>99706732.31271403</v>
       </c>
       <c r="C123" t="n">
-        <v>7567601.635024867</v>
+        <v>-199480058.8985869</v>
       </c>
       <c r="D123" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>621810.8103163663</v>
+        <v>124840981.4588256</v>
       </c>
       <c r="C124" t="n">
-        <v>7285316.554902539</v>
+        <v>-221515326.7091922</v>
       </c>
       <c r="D124" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>453416.9831956982</v>
+        <v>101482637.130122</v>
       </c>
       <c r="C125" t="n">
-        <v>7548850.096561186</v>
+        <v>-201593533.2296944</v>
       </c>
       <c r="D125" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>611592.6100460046</v>
+        <v>115547775.5122885</v>
       </c>
       <c r="C126" t="n">
-        <v>7368598.606297649</v>
+        <v>-211230821.352387</v>
       </c>
       <c r="D126" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>558686.708602804</v>
+        <v>109571273.3401862</v>
       </c>
       <c r="C127" t="n">
-        <v>7335369.709418677</v>
+        <v>-191719277.4940407</v>
       </c>
       <c r="D127" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>383726.5771532588</v>
+        <v>99678284.8839162</v>
       </c>
       <c r="C128" t="n">
-        <v>7592008.077162812</v>
+        <v>-202869464.7461046</v>
       </c>
       <c r="D128" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>572065.6433788443</v>
+        <v>116896498.8276936</v>
       </c>
       <c r="C129" t="n">
-        <v>7370981.487775771</v>
+        <v>-215237703.2306432</v>
       </c>
       <c r="D129" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>570671.744298632</v>
+        <v>101486613.3077085</v>
       </c>
       <c r="C130" t="n">
-        <v>7506660.864765343</v>
+        <v>-195192346.6161174</v>
       </c>
       <c r="D130" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>539967.4751042218</v>
+        <v>111206429.3717718</v>
       </c>
       <c r="C131" t="n">
-        <v>7431673.784536626</v>
+        <v>-209942642.4337206</v>
       </c>
       <c r="D131" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>452174.9311583586</v>
+        <v>100690301.4471169</v>
       </c>
       <c r="C132" t="n">
-        <v>7556332.266056828</v>
+        <v>-200528169.7813111</v>
       </c>
       <c r="D132" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>384478.042694183</v>
+        <v>99441616.50272426</v>
       </c>
       <c r="C133" t="n">
-        <v>7593792.795184806</v>
+        <v>-202479162.9386826</v>
       </c>
       <c r="D133" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>472457.6527888828</v>
+        <v>113308239.1278594</v>
       </c>
       <c r="C134" t="n">
-        <v>7438943.410384167</v>
+        <v>-216662236.3820526</v>
       </c>
       <c r="D134" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>520706.5159229873</v>
+        <v>117210532.9378552</v>
       </c>
       <c r="C135" t="n">
-        <v>7279090.447065596</v>
+        <v>-202388640.3289137</v>
       </c>
       <c r="D135" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>439654.4736789956</v>
+        <v>104803634.4021675</v>
       </c>
       <c r="C136" t="n">
-        <v>7524984.020991635</v>
+        <v>-207065422.8186131</v>
       </c>
       <c r="D136" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>597874.7966290781</v>
+        <v>115088902.8054884</v>
       </c>
       <c r="C137" t="n">
-        <v>7377365.426627968</v>
+        <v>-211475437.8546615</v>
       </c>
       <c r="D137" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>507905.568870945</v>
+        <v>108953363.5511799</v>
       </c>
       <c r="C138" t="n">
-        <v>7462990.403153609</v>
+        <v>-208830389.1402352</v>
       </c>
       <c r="D138" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>366329.6275398433</v>
+        <v>132227328.7373793</v>
       </c>
       <c r="C139" t="n">
-        <v>7326783.189303711</v>
+        <v>-246882657.1680205</v>
       </c>
       <c r="D139" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>456361.2898843428</v>
+        <v>120645077.3307229</v>
       </c>
       <c r="C140" t="n">
-        <v>7383412.108057517</v>
+        <v>-226992646.1945517</v>
       </c>
       <c r="D140" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>444657.8554364101</v>
+        <v>100370172.5250075</v>
       </c>
       <c r="C141" t="n">
-        <v>7562025.921142353</v>
+        <v>-200483310.2279336</v>
       </c>
       <c r="D141" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>397530.8865128363</v>
+        <v>121803530.9674991</v>
       </c>
       <c r="C142" t="n">
-        <v>7290150.983906416</v>
+        <v>-214929262.2081245</v>
       </c>
       <c r="D142" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>612182.4967714186</v>
+        <v>115093850.2074087</v>
       </c>
       <c r="C143" t="n">
-        <v>7372330.057555402</v>
+        <v>-210639130.9912758</v>
       </c>
       <c r="D143" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>466502.8775897114</v>
+        <v>103822953.4520017</v>
       </c>
       <c r="C144" t="n">
-        <v>7426010.897140203</v>
+        <v>-189930731.702317</v>
       </c>
       <c r="D144" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>428515.3844426512</v>
+        <v>132877443.62134</v>
       </c>
       <c r="C145" t="n">
-        <v>7177710.160828887</v>
+        <v>-224023748.5784365</v>
       </c>
       <c r="D145" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>439047.5535942831</v>
+        <v>101015466.2542255</v>
       </c>
       <c r="C146" t="n">
-        <v>7558462.652592706</v>
+        <v>-201723206.6404476</v>
       </c>
       <c r="D146" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>433932.7497139967</v>
+        <v>119228449.4292004</v>
       </c>
       <c r="C147" t="n">
-        <v>7404311.079104981</v>
+        <v>-226634202.4660612</v>
       </c>
       <c r="D147" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>373715.0621996796</v>
+        <v>140082692.4468106</v>
       </c>
       <c r="C148" t="n">
-        <v>7140463.167019151</v>
+        <v>-234409595.1433657</v>
       </c>
       <c r="D148" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>468998.8339806726</v>
+        <v>119395384.9325225</v>
       </c>
       <c r="C149" t="n">
-        <v>7388821.772371144</v>
+        <v>-224644429.6894445</v>
       </c>
       <c r="D149" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>436408.8218150658</v>
+        <v>107077921.004971</v>
       </c>
       <c r="C150" t="n">
-        <v>7506500.594720325</v>
+        <v>-210415575.5129712</v>
       </c>
       <c r="D150" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>569006.5176380178</v>
+        <v>116599761.8003678</v>
       </c>
       <c r="C151" t="n">
-        <v>7374633.408555133</v>
+        <v>-215056264.1719109</v>
       </c>
       <c r="D151" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>376624.0866571964</v>
+        <v>143874749.0634952</v>
       </c>
       <c r="C152" t="n">
-        <v>7229605.106066765</v>
+        <v>-258943761.0773299</v>
       </c>
       <c r="D152" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>444385.7615036962</v>
+        <v>122093307.7635642</v>
       </c>
       <c r="C153" t="n">
-        <v>7376206.848085475</v>
+        <v>-229543200.8580566</v>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>431132.6180002625</v>
+        <v>105590085.9079321</v>
       </c>
       <c r="C154" t="n">
-        <v>7521465.612824399</v>
+        <v>-208653782.3603525</v>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>584961.2195156019</v>
+        <v>132597887.1665408</v>
       </c>
       <c r="C155" t="n">
-        <v>7233817.372569075</v>
+        <v>-232357831.3243726</v>
       </c>
       <c r="D155" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>446157.5485860738</v>
+        <v>103470805.8748131</v>
       </c>
       <c r="C156" t="n">
-        <v>7534123.93820927</v>
+        <v>-204822101.9525426</v>
       </c>
       <c r="D156" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>389746.2694711213</v>
+        <v>127180613.9277396</v>
       </c>
       <c r="C157" t="n">
-        <v>7245831.948977302</v>
+        <v>-221078511.4456128</v>
       </c>
       <c r="D157" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>503052.1425778663</v>
+        <v>116386930.9560903</v>
       </c>
       <c r="C158" t="n">
-        <v>7293901.021924582</v>
+        <v>-202553336.0838474</v>
       </c>
       <c r="D158" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>435487.6637338779</v>
+        <v>101583352.7685994</v>
       </c>
       <c r="C159" t="n">
-        <v>7554822.370589631</v>
+        <v>-202736787.3699743</v>
       </c>
       <c r="D159" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>375328.1206457481</v>
+        <v>139999211.642137</v>
       </c>
       <c r="C160" t="n">
-        <v>7140407.869943817</v>
+        <v>-234218738.9120067</v>
       </c>
       <c r="D160" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>430806.5620925381</v>
+        <v>129403918.6188121</v>
       </c>
       <c r="C161" t="n">
-        <v>7207417.315247957</v>
+        <v>-220561130.1128934</v>
       </c>
       <c r="D161" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>439805.1538512177</v>
+        <v>118958854.6132308</v>
       </c>
       <c r="C162" t="n">
-        <v>7404176.992680821</v>
+        <v>-225924513.2256453</v>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>368347.2212977612</v>
+        <v>127361799.8553083</v>
       </c>
       <c r="C163" t="n">
-        <v>7254148.289168184</v>
+        <v>-222684836.8283646</v>
       </c>
       <c r="D163" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>429836.6878292271</v>
+        <v>105214205.3888756</v>
       </c>
       <c r="C164" t="n">
-        <v>7525240.43409429</v>
+        <v>-208202346.972273</v>
       </c>
       <c r="D164" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>431460.9907259208</v>
+        <v>130001514.6469524</v>
       </c>
       <c r="C165" t="n">
-        <v>7201818.906944926</v>
+        <v>-221096251.1072609</v>
       </c>
       <c r="D165" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>612695.2306431417</v>
+        <v>137717459.0523186</v>
       </c>
       <c r="C166" t="n">
-        <v>7180841.293022046</v>
+        <v>-235681984.5561872</v>
       </c>
       <c r="D166" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>431933.0220172554</v>
+        <v>105128541.7492181</v>
       </c>
       <c r="C167" t="n">
-        <v>7525164.216234216</v>
+        <v>-207962133.4922707</v>
       </c>
       <c r="D167" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>571477.7003448418</v>
+        <v>121060300.4620544</v>
       </c>
       <c r="C168" t="n">
-        <v>7335667.556724924</v>
+        <v>-220297557.7979507</v>
       </c>
       <c r="D168" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>436529.4858061953</v>
+        <v>136483512.4430443</v>
       </c>
       <c r="C169" t="n">
-        <v>7142256.750001465</v>
+        <v>-226734556.8126839</v>
       </c>
       <c r="D169" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>396680.0496550673</v>
+        <v>124548501.1505335</v>
       </c>
       <c r="C170" t="n">
-        <v>7266028.146615055</v>
+        <v>-217902651.7519901</v>
       </c>
       <c r="D170" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>428658.0909905289</v>
+        <v>128464498.0296568</v>
       </c>
       <c r="C171" t="n">
-        <v>7216730.436064484</v>
+        <v>-219784764.8501419</v>
       </c>
       <c r="D171" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>593191.4187559042</v>
+        <v>136901542.6570788</v>
       </c>
       <c r="C172" t="n">
-        <v>7195042.290479658</v>
+        <v>-236224593.5605564</v>
       </c>
       <c r="D172" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>379205.5803994216</v>
+        <v>140229425.9082486</v>
       </c>
       <c r="C173" t="n">
-        <v>7136541.931148331</v>
+        <v>-234134835.1599286</v>
       </c>
       <c r="D173" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>576221.5915295435</v>
+        <v>115411245.186507</v>
       </c>
       <c r="C174" t="n">
-        <v>7382257.330581195</v>
+        <v>-213155727.6359349</v>
       </c>
       <c r="D174" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>424471.7906746557</v>
+        <v>137088898.2118142</v>
       </c>
       <c r="C175" t="n">
-        <v>7142514.671104215</v>
+        <v>-228123017.841619</v>
       </c>
       <c r="D175" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>575266.3307147442</v>
+        <v>138936348.0628513</v>
       </c>
       <c r="C176" t="n">
-        <v>7185257.558376712</v>
+        <v>-239502436.3370571</v>
       </c>
       <c r="D176" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>604290.0810529721</v>
+        <v>116306647.5220219</v>
       </c>
       <c r="C177" t="n">
-        <v>7364583.701289264</v>
+        <v>-212590809.3727053</v>
       </c>
       <c r="D177" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>432284.6912633065</v>
+        <v>120195467.8391005</v>
       </c>
       <c r="C178" t="n">
-        <v>7396923.161243825</v>
+        <v>-227955826.4722086</v>
       </c>
       <c r="D178" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>439758.1563198671</v>
+        <v>119185180.0915828</v>
       </c>
       <c r="C179" t="n">
-        <v>7402304.535486695</v>
+        <v>-226213221.2188751</v>
       </c>
       <c r="D179" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>455576.2169239347</v>
+        <v>132649677.9409595</v>
       </c>
       <c r="C180" t="n">
-        <v>7284936.716519298</v>
+        <v>-241194673.5050797</v>
       </c>
       <c r="D180" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
4/04 optimizing variogram parameters for area2
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>105508726.4694378</v>
+        <v>170061253.5450011</v>
       </c>
       <c r="C2" t="n">
-        <v>-209018146.6045218</v>
+        <v>-402048568.8690004</v>
       </c>
       <c r="D2" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>132646577.4596441</v>
+        <v>215751600.2529267</v>
       </c>
       <c r="C3" t="n">
-        <v>-241504486.6946509</v>
+        <v>-466156325.3815762</v>
       </c>
       <c r="D3" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>116529554.7152026</v>
+        <v>190157095.1846463</v>
       </c>
       <c r="C4" t="n">
-        <v>-213442943.3238954</v>
+        <v>-415950649.4723316</v>
       </c>
       <c r="D4" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>106092782.3304012</v>
+        <v>170860992.9712256</v>
       </c>
       <c r="C5" t="n">
-        <v>-210929361.0420707</v>
+        <v>-405155427.0714723</v>
       </c>
       <c r="D5" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>105991829.6311245</v>
+        <v>170667185.431315</v>
       </c>
       <c r="C6" t="n">
-        <v>-210946344.5005981</v>
+        <v>-405104104.4883425</v>
       </c>
       <c r="D6" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>122395754.4997257</v>
+        <v>198148318.8949276</v>
       </c>
       <c r="C7" t="n">
-        <v>-232183773.5343286</v>
+        <v>-446478395.0038871</v>
       </c>
       <c r="D7" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>106102412.26284</v>
+        <v>170922082.497805</v>
       </c>
       <c r="C8" t="n">
-        <v>-210661424.2871895</v>
+        <v>-404787896.7358894</v>
       </c>
       <c r="D8" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>117040622.1587794</v>
+        <v>190811154.076052</v>
       </c>
       <c r="C9" t="n">
-        <v>-215321766.9774082</v>
+        <v>-418967515.8208964</v>
       </c>
       <c r="D9" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>103861518.1174055</v>
+        <v>167063073.7771204</v>
       </c>
       <c r="C10" t="n">
-        <v>-208247002.9008795</v>
+        <v>-399736333.0616241</v>
       </c>
       <c r="D10" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>117134202.8675836</v>
+        <v>191182675.188347</v>
       </c>
       <c r="C11" t="n">
-        <v>-214123845.5357292</v>
+        <v>-417313437.041097</v>
       </c>
       <c r="D11" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>138056256.2293121</v>
+        <v>226125332.4069945</v>
       </c>
       <c r="C12" t="n">
-        <v>-238975883.2737637</v>
+        <v>-465476449.0371869</v>
       </c>
       <c r="D12" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>127395291.6096901</v>
+        <v>207534924.9715279</v>
       </c>
       <c r="C13" t="n">
-        <v>-231756331.7183017</v>
+        <v>-448996303.2290542</v>
       </c>
       <c r="D13" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>102692553.5673765</v>
+        <v>165417181.4159042</v>
       </c>
       <c r="C14" t="n">
-        <v>-204683855.8293287</v>
+        <v>-393879767.4921157</v>
       </c>
       <c r="D14" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>109438266.882265</v>
+        <v>179797278.9888872</v>
       </c>
       <c r="C15" t="n">
-        <v>-195287931.0485279</v>
+        <v>-385339572.3715404</v>
       </c>
       <c r="D15" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>138596224.7624223</v>
+        <v>227210100.4166648</v>
       </c>
       <c r="C16" t="n">
-        <v>-238383033.7740149</v>
+        <v>-464887206.9620859</v>
       </c>
       <c r="D16" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>130020051.2517149</v>
+        <v>212055122.9125671</v>
       </c>
       <c r="C17" t="n">
-        <v>-234012094.1658826</v>
+        <v>-453803865.4495928</v>
       </c>
       <c r="D17" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>134644140.8865899</v>
+        <v>219066152.3479342</v>
       </c>
       <c r="C18" t="n">
-        <v>-243949740.2878812</v>
+        <v>-470844080.385905</v>
       </c>
       <c r="D18" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>139608841.0539081</v>
+        <v>229520900.4912613</v>
       </c>
       <c r="C19" t="n">
-        <v>-235476230.8749945</v>
+        <v>-461115703.439372</v>
       </c>
       <c r="D19" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>105596981.9961531</v>
+        <v>170189121.3721983</v>
       </c>
       <c r="C20" t="n">
-        <v>-209263009.2431625</v>
+        <v>-402456658.3516716</v>
       </c>
       <c r="D20" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>141599423.6154124</v>
+        <v>232646418.6580028</v>
       </c>
       <c r="C21" t="n">
-        <v>-238858232.1724758</v>
+        <v>-467100958.0807744</v>
       </c>
       <c r="D21" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>134875384.7845174</v>
+        <v>221685799.896555</v>
       </c>
       <c r="C22" t="n">
-        <v>-229901430.6513903</v>
+        <v>-450486429.1942855</v>
       </c>
       <c r="D22" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>105594822.7153038</v>
+        <v>170044434.1339617</v>
       </c>
       <c r="C23" t="n">
-        <v>-210140147.9385734</v>
+        <v>-403681533.2859867</v>
       </c>
       <c r="D23" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>105845394.8503075</v>
+        <v>170455328.0702242</v>
       </c>
       <c r="C24" t="n">
-        <v>-210537490.5371626</v>
+        <v>-404423592.289158</v>
       </c>
       <c r="D24" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>134781258.9465282</v>
+        <v>220587369.5919776</v>
       </c>
       <c r="C25" t="n">
-        <v>-235788498.9133089</v>
+        <v>-459065039.3759356</v>
       </c>
       <c r="D25" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>125182348.8449171</v>
+        <v>204294828.1179895</v>
       </c>
       <c r="C26" t="n">
-        <v>-226212495.6601892</v>
+        <v>-439678649.7171889</v>
       </c>
       <c r="D26" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>105460556.4692007</v>
+        <v>169897527.0426158</v>
       </c>
       <c r="C27" t="n">
-        <v>-209469655.8274356</v>
+        <v>-402644194.6175289</v>
       </c>
       <c r="D27" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>127417554.1764413</v>
+        <v>209752092.0299546</v>
       </c>
       <c r="C28" t="n">
-        <v>-218170442.130488</v>
+        <v>-429279032.9395711</v>
       </c>
       <c r="D28" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>110635064.8260035</v>
+        <v>181148880.3769667</v>
       </c>
       <c r="C29" t="n">
-        <v>-200693955.3049799</v>
+        <v>-393871673.9209508</v>
       </c>
       <c r="D29" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>136104466.1075085</v>
+        <v>223592087.1595653</v>
       </c>
       <c r="C30" t="n">
-        <v>-232184709.8015506</v>
+        <v>-454483925.6360297</v>
       </c>
       <c r="D30" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>134783690.3161738</v>
+        <v>220591388.8574566</v>
       </c>
       <c r="C31" t="n">
-        <v>-235791494.57205</v>
+        <v>-459070734.1471248</v>
       </c>
       <c r="D31" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>105451235.8885704</v>
+        <v>169837139.3715255</v>
       </c>
       <c r="C32" t="n">
-        <v>-209736329.8344363</v>
+        <v>-403010049.6333153</v>
       </c>
       <c r="D32" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>133553287.5962651</v>
+        <v>217075885.120332</v>
       </c>
       <c r="C33" t="n">
-        <v>-243785214.8407176</v>
+        <v>-469975118.9094672</v>
       </c>
       <c r="D33" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>105716464.7564075</v>
+        <v>170221339.6758617</v>
       </c>
       <c r="C34" t="n">
-        <v>-210474208.3568346</v>
+        <v>-404239109.246271</v>
       </c>
       <c r="D34" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>139066872.48509</v>
+        <v>228674745.6979045</v>
       </c>
       <c r="C35" t="n">
-        <v>-234520873.5788515</v>
+        <v>-459433627.7697359</v>
       </c>
       <c r="D35" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>138187606.9388872</v>
+        <v>226511925.3198773</v>
       </c>
       <c r="C36" t="n">
-        <v>-238041235.5106107</v>
+        <v>-464173405.9727495</v>
       </c>
       <c r="D36" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>111701037.9983043</v>
+        <v>182849971.5594774</v>
       </c>
       <c r="C37" t="n">
-        <v>-202577032.8259242</v>
+        <v>-397265861.4077961</v>
       </c>
       <c r="D37" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>113236264.3979196</v>
+        <v>185605712.1449671</v>
       </c>
       <c r="C38" t="n">
-        <v>-203448141.3676558</v>
+        <v>-399507878.409721</v>
       </c>
       <c r="D38" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>102773319.0900762</v>
+        <v>165158688.1655019</v>
       </c>
       <c r="C39" t="n">
-        <v>-207250826.245541</v>
+        <v>-397520250.4713072</v>
       </c>
       <c r="D39" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>105017672.2254655</v>
+        <v>169255388.5440889</v>
       </c>
       <c r="C40" t="n">
-        <v>-208242418.4061436</v>
+        <v>-400598228.2076799</v>
       </c>
       <c r="D40" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>134701314.1507206</v>
+        <v>220469595.8216356</v>
       </c>
       <c r="C41" t="n">
-        <v>-235598052.3902366</v>
+        <v>-458743532.120712</v>
       </c>
       <c r="D41" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>104439268.9421774</v>
+        <v>168088018.066688</v>
       </c>
       <c r="C42" t="n">
-        <v>-208685705.4748633</v>
+        <v>-400784453.2981902</v>
       </c>
       <c r="D42" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>104063185.0347636</v>
+        <v>167778416.8765537</v>
       </c>
       <c r="C43" t="n">
-        <v>-206174733.721487</v>
+        <v>-396994263.684976</v>
       </c>
       <c r="D43" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>116381563.0254742</v>
+        <v>189893264.5149418</v>
       </c>
       <c r="C44" t="n">
-        <v>-213354002.2535594</v>
+        <v>-415728052.2039195</v>
       </c>
       <c r="D44" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>100167826.3336622</v>
+        <v>161294915.6318805</v>
       </c>
       <c r="C45" t="n">
-        <v>-200491735.4238619</v>
+        <v>-386106025.2255547</v>
       </c>
       <c r="D45" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>106181608.3227286</v>
+        <v>170989661.2193642</v>
       </c>
       <c r="C46" t="n">
-        <v>-211176252.3923558</v>
+        <v>-405566621.7426242</v>
       </c>
       <c r="D46" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>104367728.3348256</v>
+        <v>167842617.8236445</v>
       </c>
       <c r="C47" t="n">
-        <v>-209373254.1300425</v>
+        <v>-401689953.4288404</v>
       </c>
       <c r="D47" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>104424001.3408905</v>
+        <v>168348387.5857986</v>
       </c>
       <c r="C48" t="n">
-        <v>-206884594.4189475</v>
+        <v>-398256561.2255399</v>
       </c>
       <c r="D48" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>137283281.5320168</v>
+        <v>225037801.297646</v>
       </c>
       <c r="C49" t="n">
-        <v>-236821997.8006023</v>
+        <v>-461912078.2331657</v>
       </c>
       <c r="D49" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>106000975.046599</v>
+        <v>170869051.6025432</v>
       </c>
       <c r="C50" t="n">
-        <v>-209794092.8900959</v>
+        <v>-403499299.370443</v>
       </c>
       <c r="D50" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>117159326.3814496</v>
+        <v>193017470.4955127</v>
       </c>
       <c r="C51" t="n">
-        <v>-203346207.1822138</v>
+        <v>-401785101.312815</v>
       </c>
       <c r="D51" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>123465584.6433238</v>
+        <v>199949949.5776266</v>
       </c>
       <c r="C52" t="n">
-        <v>-233430269.622158</v>
+        <v>-448945059.420067</v>
       </c>
       <c r="D52" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>130665300.368854</v>
+        <v>212560183.8336233</v>
       </c>
       <c r="C53" t="n">
-        <v>-238428189.4724956</v>
+        <v>-460556023.6364397</v>
       </c>
       <c r="D53" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>100367178.8657337</v>
+        <v>161676484.2880752</v>
       </c>
       <c r="C54" t="n">
-        <v>-200478489.6620883</v>
+        <v>-386240761.038307</v>
       </c>
       <c r="D54" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>105352880.5020434</v>
+        <v>169788566.1146641</v>
       </c>
       <c r="C55" t="n">
-        <v>-208877513.5332501</v>
+        <v>-401736005.8829324</v>
       </c>
       <c r="D55" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>129647122.8856552</v>
+        <v>211508905.0259657</v>
       </c>
       <c r="C56" t="n">
-        <v>-233086310.6818279</v>
+        <v>-452247932.9809692</v>
       </c>
       <c r="D56" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>99652515.60497172</v>
+        <v>159944451.6321533</v>
       </c>
       <c r="C57" t="n">
-        <v>-202793563.913616</v>
+        <v>-388908680.488093</v>
       </c>
       <c r="D57" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>124626453.9291485</v>
+        <v>201934275.4551795</v>
       </c>
       <c r="C58" t="n">
-        <v>-234583616.9577389</v>
+        <v>-451332610.6898304</v>
       </c>
       <c r="D58" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>112672866.8429443</v>
+        <v>184732978.0088556</v>
       </c>
       <c r="C59" t="n">
-        <v>-202306174.8753476</v>
+        <v>-397506742.2204202</v>
       </c>
       <c r="D59" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>120818759.6407465</v>
+        <v>195705534.4388087</v>
       </c>
       <c r="C60" t="n">
-        <v>-228976588.5435393</v>
+        <v>-440888996.2268443</v>
       </c>
       <c r="D60" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>136059248.6204675</v>
+        <v>220534136.2407041</v>
       </c>
       <c r="C61" t="n">
-        <v>-251416086.562739</v>
+        <v>-482430540.6605094</v>
       </c>
       <c r="D61" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>137281823.6174914</v>
+        <v>225035389.0068487</v>
       </c>
       <c r="C62" t="n">
-        <v>-236820256.6947784</v>
+        <v>-461908760.2337005</v>
       </c>
       <c r="D62" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>111557958.197442</v>
+        <v>183320051.9313003</v>
       </c>
       <c r="C63" t="n">
-        <v>-198188443.8184662</v>
+        <v>-390873338.4612513</v>
       </c>
       <c r="D63" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>122342850.5698752</v>
+        <v>198119290.4729356</v>
       </c>
       <c r="C64" t="n">
-        <v>-231739329.838951</v>
+        <v>-445812024.3581349</v>
       </c>
       <c r="D64" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>113504335.765346</v>
+        <v>183136998.266023</v>
       </c>
       <c r="C65" t="n">
-        <v>-221679853.6071709</v>
+        <v>-425597138.2776437</v>
       </c>
       <c r="D65" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>117746875.3597333</v>
+        <v>194155942.949601</v>
       </c>
       <c r="C66" t="n">
-        <v>-203145161.1829448</v>
+        <v>-401840817.6504443</v>
       </c>
       <c r="D66" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>123466691.2825127</v>
+        <v>199951766.5902286</v>
       </c>
       <c r="C67" t="n">
-        <v>-233431851.2426446</v>
+        <v>-448948024.5963792</v>
       </c>
       <c r="D67" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>110571376.8817002</v>
+        <v>181191745.9251307</v>
       </c>
       <c r="C68" t="n">
-        <v>-199724522.8641171</v>
+        <v>-392441938.8805223</v>
       </c>
       <c r="D68" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>110055601.0016471</v>
+        <v>181465006.6044621</v>
       </c>
       <c r="C69" t="n">
-        <v>-192394145.9747593</v>
+        <v>-381565732.0586818</v>
       </c>
       <c r="D69" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>115877033.3297141</v>
+        <v>190126419.3274445</v>
       </c>
       <c r="C70" t="n">
-        <v>-206198179.3881435</v>
+        <v>-405131540.1544722</v>
       </c>
       <c r="D70" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>130111079.5130356</v>
+        <v>213293560.7974027</v>
       </c>
       <c r="C71" t="n">
-        <v>-227255961.6400539</v>
+        <v>-444046630.9603429</v>
       </c>
       <c r="D71" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>105598637.6146314</v>
+        <v>170191838.1157665</v>
       </c>
       <c r="C72" t="n">
-        <v>-209265622.4662407</v>
+        <v>-402461543.5417274</v>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>134781913.8277764</v>
+        <v>220588452.1677152</v>
       </c>
       <c r="C73" t="n">
-        <v>-235789305.7885106</v>
+        <v>-459066573.2519769</v>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>120457917.0446891</v>
+        <v>195997045.5293688</v>
       </c>
       <c r="C74" t="n">
-        <v>-222901472.9667384</v>
+        <v>-431996651.364231</v>
       </c>
       <c r="D74" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>104656956.3492973</v>
+        <v>168450500.9432539</v>
       </c>
       <c r="C75" t="n">
-        <v>-208998483.7739748</v>
+        <v>-401384793.0106061</v>
       </c>
       <c r="D75" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>140447377.957341</v>
+        <v>230175350.2550632</v>
       </c>
       <c r="C76" t="n">
-        <v>-241190465.6660586</v>
+        <v>-469965199.3425449</v>
       </c>
       <c r="D76" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>127382852.6466472</v>
+        <v>208808591.8167622</v>
       </c>
       <c r="C77" t="n">
-        <v>-223616842.4244619</v>
+        <v>-437210044.3358359</v>
       </c>
       <c r="D77" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>106918502.4314488</v>
+        <v>175243179.3873374</v>
       </c>
       <c r="C78" t="n">
-        <v>-193926183.2665913</v>
+        <v>-381724269.4209624</v>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>99678515.17212091</v>
+        <v>159981689.5436021</v>
       </c>
       <c r="C79" t="n">
-        <v>-202869844.3416095</v>
+        <v>-389034951.2546384</v>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>124630512.6759802</v>
+        <v>201940941.1117887</v>
       </c>
       <c r="C80" t="n">
-        <v>-234589366.480262</v>
+        <v>-451343395.5166952</v>
       </c>
       <c r="D80" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>122906404.1367475</v>
+        <v>199038252.9463307</v>
       </c>
       <c r="C81" t="n">
-        <v>-232588847.2752898</v>
+        <v>-447386185.6953286</v>
       </c>
       <c r="D81" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>123834612.5745275</v>
+        <v>200536386.0293367</v>
       </c>
       <c r="C82" t="n">
-        <v>-234081588.0408616</v>
+        <v>-450110034.1736351</v>
       </c>
       <c r="D82" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>125024745.8866452</v>
+        <v>205759380.4885022</v>
       </c>
       <c r="C83" t="n">
-        <v>-215332164.6101156</v>
+        <v>-423798822.2369605</v>
       </c>
       <c r="D83" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>114770796.1817679</v>
+        <v>189088595.2522518</v>
       </c>
       <c r="C84" t="n">
-        <v>-199968539.1906832</v>
+        <v>-395445249.0775359</v>
       </c>
       <c r="D84" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>136399735.7707716</v>
+        <v>223641556.3890886</v>
       </c>
       <c r="C85" t="n">
-        <v>-235342743.6443977</v>
+        <v>-459278078.5597609</v>
       </c>
       <c r="D85" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>124134250.592144</v>
+        <v>201021809.2568428</v>
       </c>
       <c r="C86" t="n">
-        <v>-234550627.4243446</v>
+        <v>-450970544.5014009</v>
       </c>
       <c r="D86" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>109970644.6036005</v>
+        <v>180714862.6879153</v>
       </c>
       <c r="C87" t="n">
-        <v>-195827838.7745652</v>
+        <v>-386459896.4466831</v>
       </c>
       <c r="D87" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>118735399.5336341</v>
+        <v>192332759.4216259</v>
       </c>
       <c r="C88" t="n">
-        <v>-225639454.349205</v>
+        <v>-434773788.9701531</v>
       </c>
       <c r="D88" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>99948772.93257391</v>
+        <v>160418897.5706784</v>
       </c>
       <c r="C89" t="n">
-        <v>-203348593.3003232</v>
+        <v>-389911002.6655887</v>
       </c>
       <c r="D89" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>113568385.9032365</v>
+        <v>183326049.5143205</v>
       </c>
       <c r="C90" t="n">
-        <v>-221247347.6185689</v>
+        <v>-425033345.1795313</v>
       </c>
       <c r="D90" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>99680708.61797616</v>
+        <v>159985281.4310923</v>
       </c>
       <c r="C91" t="n">
-        <v>-202873459.8895674</v>
+        <v>-389041687.233989</v>
       </c>
       <c r="D91" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>110142394.5216578</v>
+        <v>178908355.1332637</v>
       </c>
       <c r="C92" t="n">
-        <v>-208562628.9073775</v>
+        <v>-404735969.3286093</v>
       </c>
       <c r="D92" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>99031260.30550426</v>
+        <v>158953626.7530148</v>
       </c>
       <c r="C93" t="n">
-        <v>-201602192.2960845</v>
+        <v>-386767804.1345814</v>
       </c>
       <c r="D93" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>99679793.69599606</v>
+        <v>159983783.1963968</v>
       </c>
       <c r="C94" t="n">
-        <v>-202871951.7895998</v>
+        <v>-389038877.5547693</v>
       </c>
       <c r="D94" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>99085419.68022577</v>
+        <v>159031701.4770814</v>
       </c>
       <c r="C95" t="n">
-        <v>-201758063.0948648</v>
+        <v>-387026708.7799101</v>
       </c>
       <c r="D95" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>117016909.536118</v>
+        <v>191708627.3984575</v>
       </c>
       <c r="C96" t="n">
-        <v>-209587252.9708545</v>
+        <v>-410724560.5956822</v>
       </c>
       <c r="D96" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>102545355.9689802</v>
+        <v>164829082.7846155</v>
       </c>
       <c r="C97" t="n">
-        <v>-206606667.7502118</v>
+        <v>-396448779.1607118</v>
       </c>
       <c r="D97" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>117672836.3618993</v>
+        <v>191830326.5457348</v>
       </c>
       <c r="C98" t="n">
-        <v>-216358649.6340961</v>
+        <v>-420857416.8751051</v>
       </c>
       <c r="D98" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>123978034.8062271</v>
+        <v>200745874.1465958</v>
       </c>
       <c r="C99" t="n">
-        <v>-234452325.5146987</v>
+        <v>-450730133.2302119</v>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>120470081.3920262</v>
+        <v>195100893.162625</v>
       </c>
       <c r="C100" t="n">
-        <v>-228674520.3612784</v>
+        <v>-440230697.0622374</v>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>137093107.2131552</v>
+        <v>225334535.0004603</v>
       </c>
       <c r="C101" t="n">
-        <v>-232680201.6958987</v>
+        <v>-455721416.1328683</v>
       </c>
       <c r="D101" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>105511964.562603</v>
+        <v>170066567.4634582</v>
       </c>
       <c r="C102" t="n">
-        <v>-209023256.3673792</v>
+        <v>-402058122.279879</v>
       </c>
       <c r="D102" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>114333012.3162275</v>
+        <v>184677066.2989198</v>
       </c>
       <c r="C103" t="n">
-        <v>-221797612.6148877</v>
+        <v>-426343195.7846923</v>
       </c>
       <c r="D103" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>117585726.1880774</v>
+        <v>190705854.829486</v>
       </c>
       <c r="C104" t="n">
-        <v>-222315825.1105521</v>
+        <v>-429290698.053645</v>
       </c>
       <c r="D104" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>107604625.910323</v>
+        <v>173950496.5190559</v>
       </c>
       <c r="C105" t="n">
-        <v>-209515713.5931183</v>
+        <v>-404282480.4928117</v>
       </c>
       <c r="D105" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>145569466.401966</v>
+        <v>236488082.5247939</v>
       </c>
       <c r="C106" t="n">
-        <v>-261425231.6330547</v>
+        <v>-502234364.1522337</v>
       </c>
       <c r="D106" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>130113878.5378258</v>
+        <v>212723687.7217174</v>
       </c>
       <c r="C107" t="n">
-        <v>-230877998.5930108</v>
+        <v>-449317799.2371773</v>
       </c>
       <c r="D107" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>105080389.1113953</v>
+        <v>169111069.225488</v>
       </c>
       <c r="C108" t="n">
-        <v>-209884292.3578205</v>
+        <v>-402939472.3102995</v>
       </c>
       <c r="D108" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>120489265.4427217</v>
+        <v>198336644.9666787</v>
       </c>
       <c r="C109" t="n">
-        <v>-208929469.54725</v>
+        <v>-411866837.4992051</v>
       </c>
       <c r="D109" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>98461024.83522852</v>
+        <v>158546247.0333468</v>
       </c>
       <c r="C110" t="n">
-        <v>-197396514.180316</v>
+        <v>-380475198.7775751</v>
       </c>
       <c r="D110" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>115607022.0688982</v>
+        <v>189729394.5335976</v>
       </c>
       <c r="C111" t="n">
-        <v>-205529791.2928719</v>
+        <v>-403999810.6284639</v>
       </c>
       <c r="D111" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>124822083.9285265</v>
+        <v>202072665.5388272</v>
       </c>
       <c r="C112" t="n">
-        <v>-236031568.2958097</v>
+        <v>-453520694.1747884</v>
       </c>
       <c r="D112" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>100156661.0837503</v>
+        <v>161325373.0124752</v>
       </c>
       <c r="C113" t="n">
-        <v>-200172776.0156584</v>
+        <v>-385652928.7783066</v>
       </c>
       <c r="D113" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>100001447.5327858</v>
+        <v>161054255.9680095</v>
       </c>
       <c r="C114" t="n">
-        <v>-200022630.0171967</v>
+        <v>-385324290.4075406</v>
       </c>
       <c r="D114" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>141041486.155849</v>
+        <v>228912456.7268519</v>
       </c>
       <c r="C115" t="n">
-        <v>-256629137.1601039</v>
+        <v>-492802897.0585838</v>
       </c>
       <c r="D115" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>115944493.4328775</v>
+        <v>189903671.6324413</v>
       </c>
       <c r="C116" t="n">
-        <v>-208300507.8710816</v>
+        <v>-408201000.6104372</v>
       </c>
       <c r="D116" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>116477400.184276</v>
+        <v>190128098.1234068</v>
       </c>
       <c r="C117" t="n">
-        <v>-213021100.7277543</v>
+        <v>-415313302.3688121</v>
       </c>
       <c r="D117" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>134073855.6473529</v>
+        <v>219741114.3635682</v>
       </c>
       <c r="C118" t="n">
-        <v>-232856329.5791467</v>
+        <v>-454396973.9048197</v>
       </c>
       <c r="D118" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>117860571.0843874</v>
+        <v>191441505.7863299</v>
       </c>
       <c r="C119" t="n">
-        <v>-220944422.1572055</v>
+        <v>-427522610.3461448</v>
       </c>
       <c r="D119" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>103446922.0606982</v>
+        <v>166744254.6523182</v>
       </c>
       <c r="C120" t="n">
-        <v>-205335959.0468844</v>
+        <v>-395359670.511667</v>
       </c>
       <c r="D120" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>99679180.36433366</v>
+        <v>159982778.8322647</v>
       </c>
       <c r="C121" t="n">
-        <v>-202870940.8090142</v>
+        <v>-389036994.0382276</v>
       </c>
       <c r="D121" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>99021577.51894188</v>
+        <v>159450693.4018503</v>
       </c>
       <c r="C122" t="n">
-        <v>-198404658.9435754</v>
+        <v>-382313786.5138384</v>
       </c>
       <c r="D122" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>99706732.31271403</v>
+        <v>160581153.2411571</v>
       </c>
       <c r="C123" t="n">
-        <v>-199480058.8985869</v>
+        <v>-384341226.8542533</v>
       </c>
       <c r="D123" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>124840981.4588256</v>
+        <v>204412644.2140465</v>
       </c>
       <c r="C124" t="n">
-        <v>-221515326.7091922</v>
+        <v>-432688320.1416128</v>
       </c>
       <c r="D124" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>101482637.130122</v>
+        <v>163617850.8680348</v>
       </c>
       <c r="C125" t="n">
-        <v>-201593533.2296944</v>
+        <v>-388648087.9597438</v>
       </c>
       <c r="D125" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>115547775.5122885</v>
+        <v>188672409.5696528</v>
       </c>
       <c r="C126" t="n">
-        <v>-211230821.352387</v>
+        <v>-412151951.1620351</v>
       </c>
       <c r="D126" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>109571273.3401862</v>
+        <v>180662603.712813</v>
       </c>
       <c r="C127" t="n">
-        <v>-191719277.4940407</v>
+        <v>-380285375.9184469</v>
       </c>
       <c r="D127" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>99678284.8839162</v>
+        <v>159981312.4340496</v>
       </c>
       <c r="C128" t="n">
-        <v>-202869464.7461046</v>
+        <v>-389034244.04576</v>
       </c>
       <c r="D128" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>116896498.8276936</v>
+        <v>190553921.2513739</v>
       </c>
       <c r="C129" t="n">
-        <v>-215237703.2306432</v>
+        <v>-418754253.6420302</v>
       </c>
       <c r="D129" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>101486613.3077085</v>
+        <v>164680010.3926166</v>
       </c>
       <c r="C130" t="n">
-        <v>-195192346.6161174</v>
+        <v>-379685424.6714844</v>
       </c>
       <c r="D130" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>111206429.3717718</v>
+        <v>180693895.2109168</v>
       </c>
       <c r="C131" t="n">
-        <v>-209942642.4337206</v>
+        <v>-407424798.7042264</v>
       </c>
       <c r="D131" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>100690301.4471169</v>
+        <v>162283396.6694638</v>
       </c>
       <c r="C132" t="n">
-        <v>-200528169.7813111</v>
+        <v>-386557522.8375871</v>
       </c>
       <c r="D132" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>99441616.50272426</v>
+        <v>159593752.1135564</v>
       </c>
       <c r="C133" t="n">
-        <v>-202479162.9386826</v>
+        <v>-388307085.0363675</v>
       </c>
       <c r="D133" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>113308239.1278594</v>
+        <v>183568970.4222474</v>
       </c>
       <c r="C134" t="n">
-        <v>-216662236.3820526</v>
+        <v>-418382782.426956</v>
       </c>
       <c r="D134" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>117210532.9378552</v>
+        <v>193274830.4161268</v>
       </c>
       <c r="C135" t="n">
-        <v>-202388640.3289137</v>
+        <v>-400423351.3916775</v>
       </c>
       <c r="D135" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>104803634.4021675</v>
+        <v>169039221.4966475</v>
       </c>
       <c r="C136" t="n">
-        <v>-207065422.8186131</v>
+        <v>-398792434.4795803</v>
       </c>
       <c r="D136" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>115088902.8054884</v>
+        <v>187767923.9888766</v>
       </c>
       <c r="C137" t="n">
-        <v>-211475437.8546615</v>
+        <v>-412204218.9547121</v>
       </c>
       <c r="D137" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>108953363.5511799</v>
+        <v>176614885.9983608</v>
       </c>
       <c r="C138" t="n">
-        <v>-208830389.1402352</v>
+        <v>-404281953.2558571</v>
       </c>
       <c r="D138" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>132227328.7373793</v>
+        <v>214146793.1152762</v>
       </c>
       <c r="C139" t="n">
-        <v>-246882657.1680205</v>
+        <v>-473637174.7999482</v>
       </c>
       <c r="D139" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>120645077.3307229</v>
+        <v>195694588.3217317</v>
       </c>
       <c r="C140" t="n">
-        <v>-226992646.1945517</v>
+        <v>-437953639.0172651</v>
       </c>
       <c r="D140" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>100370172.5250075</v>
+        <v>161681400.0862358</v>
       </c>
       <c r="C141" t="n">
-        <v>-200483310.2279336</v>
+        <v>-386249778.728037</v>
       </c>
       <c r="D141" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>121803530.9674991</v>
+        <v>199808924.882672</v>
       </c>
       <c r="C142" t="n">
-        <v>-214929262.2081245</v>
+        <v>-421352675.5362641</v>
       </c>
       <c r="D142" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>115093850.2074087</v>
+        <v>187914817.4255285</v>
       </c>
       <c r="C143" t="n">
-        <v>-210639130.9912758</v>
+        <v>-411011705.6538569</v>
       </c>
       <c r="D143" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>103822953.4520017</v>
+        <v>170030570.7160479</v>
       </c>
       <c r="C144" t="n">
-        <v>-189930731.702317</v>
+        <v>-373916385.7070824</v>
       </c>
       <c r="D144" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>132877443.62134</v>
+        <v>218929775.7707652</v>
       </c>
       <c r="C145" t="n">
-        <v>-224023748.5784365</v>
+        <v>-440791059.8359208</v>
       </c>
       <c r="D145" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>101015466.2542255</v>
+        <v>162708234.4723862</v>
       </c>
       <c r="C146" t="n">
-        <v>-201723206.6404476</v>
+        <v>-388472907.154898</v>
       </c>
       <c r="D146" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>119228449.4292004</v>
+        <v>193098927.3384862</v>
       </c>
       <c r="C147" t="n">
-        <v>-226634202.4660612</v>
+        <v>-436513085.7480596</v>
       </c>
       <c r="D147" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>140082692.4468106</v>
+        <v>230555666.8963441</v>
       </c>
       <c r="C148" t="n">
-        <v>-234409595.1433657</v>
+        <v>-459769917.9560463</v>
       </c>
       <c r="D148" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>119395384.9325225</v>
+        <v>193727869.7420573</v>
       </c>
       <c r="C149" t="n">
-        <v>-224644429.6894445</v>
+        <v>-433795557.1452767</v>
       </c>
       <c r="D149" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>107077921.004971</v>
+        <v>172808170.7906583</v>
       </c>
       <c r="C150" t="n">
-        <v>-210415575.5129712</v>
+        <v>-405162410.6592178</v>
       </c>
       <c r="D150" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>116599761.8003678</v>
+        <v>190025554.5393861</v>
       </c>
       <c r="C151" t="n">
-        <v>-215056264.1719109</v>
+        <v>-418302784.1040679</v>
       </c>
       <c r="D151" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>143874749.0634952</v>
+        <v>233758818.4293233</v>
       </c>
       <c r="C152" t="n">
-        <v>-258943761.0773299</v>
+        <v>-497716248.5745634</v>
       </c>
       <c r="D152" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>122093307.7635642</v>
+        <v>197999048.2211913</v>
       </c>
       <c r="C153" t="n">
-        <v>-229543200.8580566</v>
+        <v>-442524433.6819119</v>
       </c>
       <c r="D153" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>105590085.9079321</v>
+        <v>170274010.9602531</v>
       </c>
       <c r="C154" t="n">
-        <v>-208653782.3603525</v>
+        <v>-401599067.683601</v>
       </c>
       <c r="D154" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>132597887.1665408</v>
+        <v>217091423.600224</v>
       </c>
       <c r="C155" t="n">
-        <v>-232357831.3243726</v>
+        <v>-452864053.2432491</v>
       </c>
       <c r="D155" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>103470805.8748131</v>
+        <v>166872681.8275874</v>
       </c>
       <c r="C156" t="n">
-        <v>-204822101.9525426</v>
+        <v>-394659380.2129357</v>
       </c>
       <c r="D156" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>127180613.9277396</v>
+        <v>208841063.2337069</v>
       </c>
       <c r="C157" t="n">
-        <v>-221078511.4456128</v>
+        <v>-433398500.873895</v>
       </c>
       <c r="D157" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>116386930.9560903</v>
+        <v>191697416.7709543</v>
       </c>
       <c r="C158" t="n">
-        <v>-202553336.0838474</v>
+        <v>-400171482.9756765</v>
       </c>
       <c r="D158" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>101583352.7685994</v>
+        <v>163624090.056206</v>
       </c>
       <c r="C159" t="n">
-        <v>-202736787.3699743</v>
+        <v>-390320148.7865415</v>
       </c>
       <c r="D159" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>139999211.642137</v>
+        <v>230432261.7004661</v>
       </c>
       <c r="C160" t="n">
-        <v>-234218738.9120067</v>
+        <v>-459446216.7997958</v>
       </c>
       <c r="D160" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>129403918.6188121</v>
+        <v>213054465.7445063</v>
       </c>
       <c r="C161" t="n">
-        <v>-220561130.1128934</v>
+        <v>-433863851.7112849</v>
       </c>
       <c r="D161" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>118958854.6132308</v>
+        <v>192706308.6065789</v>
       </c>
       <c r="C162" t="n">
-        <v>-225924513.2256453</v>
+        <v>-435326852.917184</v>
       </c>
       <c r="D162" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>127361799.8553083</v>
+        <v>208919250.3967201</v>
       </c>
       <c r="C163" t="n">
-        <v>-222684836.8283646</v>
+        <v>-435841706.9338781</v>
       </c>
       <c r="D163" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>105214205.3888756</v>
+        <v>169634345.0394309</v>
       </c>
       <c r="C164" t="n">
-        <v>-208202346.972273</v>
+        <v>-400688439.0056636</v>
       </c>
       <c r="D164" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>130001514.6469524</v>
+        <v>214076451.9032896</v>
       </c>
       <c r="C165" t="n">
-        <v>-221096251.1072609</v>
+        <v>-434970040.9152226</v>
       </c>
       <c r="D165" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>137717459.0523186</v>
+        <v>226014241.3440962</v>
       </c>
       <c r="C166" t="n">
-        <v>-235681984.5561872</v>
+        <v>-460462448.9135036</v>
       </c>
       <c r="D166" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>105128541.7492181</v>
+        <v>169510653.6271445</v>
       </c>
       <c r="C167" t="n">
-        <v>-207962133.4922707</v>
+        <v>-400288688.0457355</v>
       </c>
       <c r="D167" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>121060300.4620544</v>
+        <v>197544351.2653601</v>
       </c>
       <c r="C168" t="n">
-        <v>-220297557.7979507</v>
+        <v>-428644976.7766817</v>
       </c>
       <c r="D168" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>136483512.4430443</v>
+        <v>225147600.0272056</v>
       </c>
       <c r="C169" t="n">
-        <v>-226734556.8126839</v>
+        <v>-446621699.3602381</v>
       </c>
       <c r="D169" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>124548501.1505335</v>
+        <v>204452339.7224762</v>
       </c>
       <c r="C170" t="n">
-        <v>-217902651.7519901</v>
+        <v>-427274707.5131188</v>
       </c>
       <c r="D170" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>128464498.0296568</v>
+        <v>211436154.0418527</v>
       </c>
       <c r="C171" t="n">
-        <v>-219784764.8501419</v>
+        <v>-432216727.6757636</v>
       </c>
       <c r="D171" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>136901542.6570788</v>
+        <v>224428130.6488923</v>
       </c>
       <c r="C172" t="n">
-        <v>-236224593.5605564</v>
+        <v>-460835459.0009965</v>
       </c>
       <c r="D172" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>140229425.9082486</v>
+        <v>230867323.3203529</v>
       </c>
       <c r="C173" t="n">
-        <v>-234134835.1599286</v>
+        <v>-459433945.2831934</v>
       </c>
       <c r="D173" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>115411245.186507</v>
+        <v>188099519.5105205</v>
       </c>
       <c r="C174" t="n">
-        <v>-213155727.6359349</v>
+        <v>-414814430.0133743</v>
       </c>
       <c r="D174" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>137088898.2118142</v>
+        <v>226042122.9440573</v>
       </c>
       <c r="C175" t="n">
-        <v>-228123017.841619</v>
+        <v>-448979737.9827173</v>
       </c>
       <c r="D175" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>138936348.0628513</v>
+        <v>227661733.7457307</v>
       </c>
       <c r="C176" t="n">
-        <v>-239502436.3370571</v>
+        <v>-466707593.4775785</v>
       </c>
       <c r="D176" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>116306647.5220219</v>
+        <v>189877414.6763963</v>
       </c>
       <c r="C177" t="n">
-        <v>-212590809.3727053</v>
+        <v>-414587537.4387551</v>
       </c>
       <c r="D177" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>120195467.8391005</v>
+        <v>194700531.8312197</v>
       </c>
       <c r="C178" t="n">
-        <v>-227955826.4722086</v>
+        <v>-439028991.2625205</v>
       </c>
       <c r="D178" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>119185180.0915828</v>
+        <v>193084589.4705866</v>
       </c>
       <c r="C179" t="n">
-        <v>-226213221.2188751</v>
+        <v>-435886815.5279012</v>
       </c>
       <c r="D179" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>132649677.9409595</v>
+        <v>215805372.3812869</v>
       </c>
       <c r="C180" t="n">
-        <v>-241194673.5050797</v>
+        <v>-465711154.7927014</v>
       </c>
       <c r="D180" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
4/04 optimizing variogram parameters for area4
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,13 +528,13 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>170061253.5450011</v>
+        <v>241116409.9288566</v>
       </c>
       <c r="C2" t="n">
-        <v>-402048568.8690004</v>
+        <v>-640516451.8613</v>
       </c>
       <c r="D2" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -642,13 +642,13 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>215751600.2529267</v>
+        <v>307840143.1691962</v>
       </c>
       <c r="C3" t="n">
-        <v>-466156325.3815762</v>
+        <v>-744780978.6235237</v>
       </c>
       <c r="D3" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -756,13 +756,13 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>190157095.1846463</v>
+        <v>271851828.2804081</v>
       </c>
       <c r="C4" t="n">
-        <v>-415950649.4723316</v>
+        <v>-668097385.7077036</v>
       </c>
       <c r="D4" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -874,13 +874,13 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>170860992.9712256</v>
+        <v>242120270.0446654</v>
       </c>
       <c r="C5" t="n">
-        <v>-405155427.0714723</v>
+        <v>-644936176.4713304</v>
       </c>
       <c r="D5" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -988,13 +988,13 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>170667185.431315</v>
+        <v>241816006.3231841</v>
       </c>
       <c r="C6" t="n">
-        <v>-405104104.4883425</v>
+        <v>-644771741.2745878</v>
       </c>
       <c r="D6" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1102,13 +1102,13 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>198148318.8949276</v>
+        <v>281822355.0883852</v>
       </c>
       <c r="C7" t="n">
-        <v>-446478395.0038871</v>
+        <v>-711558460.5956467</v>
       </c>
       <c r="D7" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1212,13 +1212,13 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>170922082.497805</v>
+        <v>242249524.6977128</v>
       </c>
       <c r="C8" t="n">
-        <v>-404787896.7358894</v>
+        <v>-644492121.4329234</v>
       </c>
       <c r="D8" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1326,13 +1326,13 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>190811154.076052</v>
+        <v>272620302.1461084</v>
       </c>
       <c r="C9" t="n">
-        <v>-418967515.8208964</v>
+        <v>-672338783.942363</v>
       </c>
       <c r="D9" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1444,13 +1444,13 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>167063073.7771204</v>
+        <v>236537929.2857987</v>
       </c>
       <c r="C10" t="n">
-        <v>-399736333.0616241</v>
+        <v>-636000231.6287237</v>
       </c>
       <c r="D10" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1562,13 +1562,13 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>191182675.188347</v>
+        <v>273356708.5186262</v>
       </c>
       <c r="C11" t="n">
-        <v>-417313437.041097</v>
+        <v>-670332549.0772539</v>
       </c>
       <c r="D11" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1676,13 +1676,13 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>226125332.4069945</v>
+        <v>324139109.2556922</v>
       </c>
       <c r="C12" t="n">
-        <v>-465476449.0371869</v>
+        <v>-747799482.7227929</v>
       </c>
       <c r="D12" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1786,13 +1786,13 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>207534924.9715279</v>
+        <v>296404406.2602804</v>
       </c>
       <c r="C13" t="n">
-        <v>-448996303.2290542</v>
+        <v>-718866741.0923098</v>
       </c>
       <c r="D13" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1892,13 +1892,13 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>165417181.4159042</v>
+        <v>234421992.9689757</v>
       </c>
       <c r="C14" t="n">
-        <v>-393879767.4921157</v>
+        <v>-627593821.3777303</v>
       </c>
       <c r="D14" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2006,13 +2006,13 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>179797278.9888872</v>
+        <v>258153912.6522675</v>
       </c>
       <c r="C15" t="n">
-        <v>-385339572.3715404</v>
+        <v>-623356145.7801745</v>
       </c>
       <c r="D15" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2116,13 +2116,13 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>227210100.4166648</v>
+        <v>325883524.4871363</v>
       </c>
       <c r="C16" t="n">
-        <v>-464887206.9620859</v>
+        <v>-747398630.4843992</v>
       </c>
       <c r="D16" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2230,13 +2230,13 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>212055122.9125671</v>
+        <v>303097785.9272359</v>
       </c>
       <c r="C17" t="n">
-        <v>-453803865.4495928</v>
+        <v>-727024925.2444966</v>
       </c>
       <c r="D17" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2340,13 +2340,13 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>219066152.3479342</v>
+        <v>312636899.8738974</v>
       </c>
       <c r="C18" t="n">
-        <v>-470844080.385905</v>
+        <v>-752270474.6464767</v>
       </c>
       <c r="D18" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2454,13 +2454,13 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>229520900.4912613</v>
+        <v>329811766.0912105</v>
       </c>
       <c r="C19" t="n">
-        <v>-461115703.439372</v>
+        <v>-743155717.4879633</v>
       </c>
       <c r="D19" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2560,13 +2560,13 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>170189121.3721983</v>
+        <v>241284616.1454389</v>
       </c>
       <c r="C20" t="n">
-        <v>-402456658.3516716</v>
+        <v>-641108597.9145137</v>
       </c>
       <c r="D20" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2674,13 +2674,13 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>232646418.6580028</v>
+        <v>334170860.8161556</v>
       </c>
       <c r="C21" t="n">
-        <v>-467100958.0807744</v>
+        <v>-752220211.8294635</v>
       </c>
       <c r="D21" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2784,13 +2784,13 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>221685799.896555</v>
+        <v>318489476.4800459</v>
       </c>
       <c r="C22" t="n">
-        <v>-450486429.1942855</v>
+        <v>-726238810.2783819</v>
       </c>
       <c r="D22" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -2890,13 +2890,13 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>170044434.1339617</v>
+        <v>240947429.0625636</v>
       </c>
       <c r="C23" t="n">
-        <v>-403681533.2859867</v>
+        <v>-642618118.4559122</v>
       </c>
       <c r="D23" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -2996,13 +2996,13 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>170455328.0702242</v>
+        <v>241537608.1774869</v>
       </c>
       <c r="C24" t="n">
-        <v>-404423592.289158</v>
+        <v>-643785192.149943</v>
       </c>
       <c r="D24" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3110,13 +3110,13 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>220587369.5919776</v>
+        <v>316028303.5171236</v>
       </c>
       <c r="C25" t="n">
-        <v>-459065039.3759356</v>
+        <v>-737261747.7522157</v>
       </c>
       <c r="D25" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -3224,13 +3224,13 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>204294828.1179895</v>
+        <v>292111793.1974413</v>
       </c>
       <c r="C26" t="n">
-        <v>-439678649.7171889</v>
+        <v>-705272189.3632073</v>
       </c>
       <c r="D26" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -3334,13 +3334,13 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>169897527.0426158</v>
+        <v>240803556.7309235</v>
       </c>
       <c r="C27" t="n">
-        <v>-402644194.6175289</v>
+        <v>-641203341.7830828</v>
       </c>
       <c r="D27" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -3448,13 +3448,13 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>209752092.0299546</v>
+        <v>301625905.0998349</v>
       </c>
       <c r="C28" t="n">
-        <v>-429279032.9395711</v>
+        <v>-693639299.8900316</v>
       </c>
       <c r="D28" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -3562,13 +3562,13 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>181148880.3769667</v>
+        <v>259524364.4675499</v>
       </c>
       <c r="C29" t="n">
-        <v>-393871673.9209508</v>
+        <v>-635159537.19867</v>
       </c>
       <c r="D29" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -3672,13 +3672,13 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>223592087.1595653</v>
+        <v>321125162.8406616</v>
       </c>
       <c r="C30" t="n">
-        <v>-454483925.6360297</v>
+        <v>-732246856.0965803</v>
       </c>
       <c r="D30" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -3778,13 +3778,13 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>220591388.8574566</v>
+        <v>316034106.6327591</v>
       </c>
       <c r="C31" t="n">
-        <v>-459070734.1471248</v>
+        <v>-737270796.7957494</v>
       </c>
       <c r="D31" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -3892,13 +3892,13 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>169837139.3715255</v>
+        <v>240675486.9111191</v>
       </c>
       <c r="C32" t="n">
-        <v>-403010049.6333153</v>
+        <v>-641645409.746622</v>
       </c>
       <c r="D32" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -4006,13 +4006,13 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>217075885.120332</v>
+        <v>309591520.6783481</v>
       </c>
       <c r="C33" t="n">
-        <v>-469975118.9094672</v>
+        <v>-750338693.3007903</v>
       </c>
       <c r="D33" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -4116,13 +4116,13 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>170221339.6758617</v>
+        <v>241180851.5727562</v>
       </c>
       <c r="C34" t="n">
-        <v>-404239109.246271</v>
+        <v>-643428200.0245736</v>
       </c>
       <c r="D34" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -4230,13 +4230,13 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>228674745.6979045</v>
+        <v>328636380.8735353</v>
       </c>
       <c r="C35" t="n">
-        <v>-459433627.7697359</v>
+        <v>-740617600.2250655</v>
       </c>
       <c r="D35" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -4340,13 +4340,13 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>226511925.3198773</v>
+        <v>324854430.5347658</v>
       </c>
       <c r="C36" t="n">
-        <v>-464173405.9727495</v>
+        <v>-746200833.3122867</v>
       </c>
       <c r="D36" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -4458,13 +4458,13 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>182849971.5594774</v>
+        <v>261924235.3221091</v>
       </c>
       <c r="C37" t="n">
-        <v>-397265861.4077961</v>
+        <v>-640369267.1781435</v>
       </c>
       <c r="D37" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -4568,13 +4568,13 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>185605712.1449671</v>
+        <v>266105340.8550061</v>
       </c>
       <c r="C38" t="n">
-        <v>-399507878.409721</v>
+        <v>-644524175.3137047</v>
       </c>
       <c r="D38" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -4682,13 +4682,13 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>165158688.1655019</v>
+        <v>233692973.6274313</v>
       </c>
       <c r="C39" t="n">
-        <v>-397520250.4713072</v>
+        <v>-632156415.2001097</v>
       </c>
       <c r="D39" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -4800,13 +4800,13 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>169255388.5440889</v>
+        <v>239958332.6812091</v>
       </c>
       <c r="C40" t="n">
-        <v>-400598228.2076799</v>
+        <v>-638233803.9230567</v>
       </c>
       <c r="D40" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -4918,13 +4918,13 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>220469595.8216356</v>
+        <v>315871578.7534108</v>
       </c>
       <c r="C41" t="n">
-        <v>-458743532.120712</v>
+        <v>-736791243.5112112</v>
       </c>
       <c r="D41" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -5032,13 +5032,13 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>168088018.066688</v>
+        <v>238081039.3346827</v>
       </c>
       <c r="C42" t="n">
-        <v>-400784453.2981902</v>
+        <v>-637879350.5167651</v>
       </c>
       <c r="D42" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -5150,13 +5150,13 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>167778416.8765537</v>
+        <v>237917772.9119691</v>
       </c>
       <c r="C43" t="n">
-        <v>-396994263.684976</v>
+        <v>-632825810.5677013</v>
       </c>
       <c r="D43" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -5264,13 +5264,13 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>189893264.5149418</v>
+        <v>271453178.3149346</v>
       </c>
       <c r="C44" t="n">
-        <v>-415728052.2039195</v>
+        <v>-667689887.1368873</v>
       </c>
       <c r="D44" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -5382,13 +5382,13 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>161294915.6318805</v>
+        <v>228517245.6278447</v>
       </c>
       <c r="C45" t="n">
-        <v>-386106025.2255547</v>
+        <v>-615422880.303871</v>
       </c>
       <c r="D45" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -5500,13 +5500,13 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>170989661.2193642</v>
+        <v>242289512.9431651</v>
       </c>
       <c r="C46" t="n">
-        <v>-405566621.7426242</v>
+        <v>-645532582.8692462</v>
       </c>
       <c r="D46" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -5610,13 +5610,13 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>167842617.8236445</v>
+        <v>237611354.9062354</v>
       </c>
       <c r="C47" t="n">
-        <v>-401689953.4288404</v>
+        <v>-638922073.3417053</v>
       </c>
       <c r="D47" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -5728,13 +5728,13 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>168348387.5857986</v>
+        <v>238716552.1387896</v>
       </c>
       <c r="C48" t="n">
-        <v>-398256561.2255399</v>
+        <v>-634747027.1713309</v>
       </c>
       <c r="D48" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -5842,13 +5842,13 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>225037801.297646</v>
+        <v>322745359.7031357</v>
       </c>
       <c r="C49" t="n">
-        <v>-461912078.2331657</v>
+        <v>-742664354.0434316</v>
       </c>
       <c r="D49" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -5956,13 +5956,13 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>170869051.6025432</v>
+        <v>242277238.6826189</v>
       </c>
       <c r="C50" t="n">
-        <v>-403499299.370443</v>
+        <v>-642799677.7142836</v>
       </c>
       <c r="D50" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -6066,13 +6066,13 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>193017470.4955127</v>
+        <v>277669410.9749006</v>
       </c>
       <c r="C51" t="n">
-        <v>-401785101.312815</v>
+        <v>-650638472.9506352</v>
       </c>
       <c r="D51" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -6180,13 +6180,13 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>199949949.5776266</v>
+        <v>284453677.0661486</v>
       </c>
       <c r="C52" t="n">
-        <v>-448945059.420067</v>
+        <v>-715576330.4317623</v>
       </c>
       <c r="D52" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -6290,13 +6290,13 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>212560183.8336233</v>
+        <v>303309631.9706399</v>
       </c>
       <c r="C53" t="n">
-        <v>-460556023.6364397</v>
+        <v>-736125207.7363403</v>
       </c>
       <c r="D53" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -6404,13 +6404,13 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>161676484.2880752</v>
+        <v>229115395.803687</v>
       </c>
       <c r="C54" t="n">
-        <v>-386240761.038307</v>
+        <v>-615796001.4970576</v>
       </c>
       <c r="D54" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -6522,13 +6522,13 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>169788566.1146641</v>
+        <v>240709029.5342582</v>
       </c>
       <c r="C55" t="n">
-        <v>-401736005.8829324</v>
+        <v>-639974477.0186136</v>
       </c>
       <c r="D55" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -6636,13 +6636,13 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>211508905.0259657</v>
+        <v>302373980.5765743</v>
       </c>
       <c r="C56" t="n">
-        <v>-452247932.9809692</v>
+        <v>-724754887.8731717</v>
       </c>
       <c r="D56" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -6746,13 +6746,13 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>159944451.6321533</v>
+        <v>226115473.4363479</v>
       </c>
       <c r="C57" t="n">
-        <v>-388908680.488093</v>
+        <v>-618321946.9817134</v>
       </c>
       <c r="D57" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -6856,13 +6856,13 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>201934275.4551795</v>
+        <v>287378257.0332168</v>
       </c>
       <c r="C58" t="n">
-        <v>-451332610.6898304</v>
+        <v>-719565294.9595512</v>
       </c>
       <c r="D58" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -6966,13 +6966,13 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>184732978.0088556</v>
+        <v>264899440.4536139</v>
       </c>
       <c r="C59" t="n">
-        <v>-397506742.2204202</v>
+        <v>-641513779.7746129</v>
       </c>
       <c r="D59" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -7080,13 +7080,13 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>195705534.4388087</v>
+        <v>278445845.2283827</v>
       </c>
       <c r="C60" t="n">
-        <v>-440888996.2268443</v>
+        <v>-703174320.3226094</v>
       </c>
       <c r="D60" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -7190,13 +7190,13 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>220534136.2407041</v>
+        <v>313956072.1801931</v>
       </c>
       <c r="C61" t="n">
-        <v>-482430540.6605094</v>
+        <v>-768109334.7570126</v>
       </c>
       <c r="D61" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -7300,13 +7300,13 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>225035389.0068487</v>
+        <v>322741874.7063678</v>
       </c>
       <c r="C62" t="n">
-        <v>-461908760.2337005</v>
+        <v>-742659074.352662</v>
       </c>
       <c r="D62" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -7414,13 +7414,13 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>183320051.9313003</v>
+        <v>263258404.8438024</v>
       </c>
       <c r="C63" t="n">
-        <v>-390873338.4612513</v>
+        <v>-632173952.7290845</v>
       </c>
       <c r="D63" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -7528,13 +7528,13 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>198119290.4729356</v>
+        <v>281833903.6966872</v>
       </c>
       <c r="C64" t="n">
-        <v>-445812024.3581349</v>
+        <v>-710675747.4114839</v>
       </c>
       <c r="D64" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -7646,13 +7646,13 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>183136998.266023</v>
+        <v>259864791.7006577</v>
       </c>
       <c r="C65" t="n">
-        <v>-425597138.2776437</v>
+        <v>-677451073.353865</v>
       </c>
       <c r="D65" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -7760,13 +7760,13 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>194155942.949601</v>
+        <v>279469335.2922495</v>
       </c>
       <c r="C66" t="n">
-        <v>-401840817.6504443</v>
+        <v>-651169910.9945309</v>
       </c>
       <c r="D66" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -7874,13 +7874,13 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>199951766.5902286</v>
+        <v>284456288.9917687</v>
       </c>
       <c r="C67" t="n">
-        <v>-448948024.5963792</v>
+        <v>-715581003.6488818</v>
       </c>
       <c r="D67" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -7988,13 +7988,13 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>181191745.9251307</v>
+        <v>259723469.9714658</v>
       </c>
       <c r="C68" t="n">
-        <v>-392441938.8805223</v>
+        <v>-633302860.1094917</v>
       </c>
       <c r="D68" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -8102,13 +8102,13 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>181465006.6044621</v>
+        <v>261164753.2626413</v>
       </c>
       <c r="C69" t="n">
-        <v>-381565732.0586818</v>
+        <v>-619107805.3630104</v>
       </c>
       <c r="D69" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -8216,13 +8216,13 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>190126419.3274445</v>
+        <v>272777273.7243389</v>
       </c>
       <c r="C70" t="n">
-        <v>-405131540.1544722</v>
+        <v>-653863315.1116563</v>
       </c>
       <c r="D70" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -8326,13 +8326,13 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>213293560.7974027</v>
+        <v>305892356.1042734</v>
       </c>
       <c r="C71" t="n">
-        <v>-444046630.9603429</v>
+        <v>-714595899.8409623</v>
       </c>
       <c r="D71" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -8436,13 +8436,13 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>170191838.1157665</v>
+        <v>241288520.0071773</v>
       </c>
       <c r="C72" t="n">
-        <v>-402461543.5417274</v>
+        <v>-641116285.9121094</v>
       </c>
       <c r="D72" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -8550,13 +8550,13 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>220588452.1677152</v>
+        <v>316029866.5670241</v>
       </c>
       <c r="C73" t="n">
-        <v>-459066573.2519769</v>
+        <v>-737264185.0951921</v>
       </c>
       <c r="D73" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -8664,13 +8664,13 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>195997045.5293688</v>
+        <v>279681540.434641</v>
       </c>
       <c r="C74" t="n">
-        <v>-431996651.364231</v>
+        <v>-691676297.3159117</v>
       </c>
       <c r="D74" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -8774,13 +8774,13 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>168450500.9432539</v>
+        <v>238606731.4384664</v>
       </c>
       <c r="C75" t="n">
-        <v>-401384793.0106061</v>
+        <v>-638839898.102951</v>
       </c>
       <c r="D75" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -8892,13 +8892,13 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>230175350.2550632</v>
+        <v>330076763.9282188</v>
       </c>
       <c r="C76" t="n">
-        <v>-469965199.3425449</v>
+        <v>-755208195.1460632</v>
       </c>
       <c r="D76" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -9006,13 +9006,13 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>208808591.8167622</v>
+        <v>299439780.3822055</v>
       </c>
       <c r="C77" t="n">
-        <v>-437210044.3358359</v>
+        <v>-703812662.4923407</v>
       </c>
       <c r="D77" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -9120,13 +9120,13 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>175243179.3873374</v>
+        <v>251216849.3362035</v>
       </c>
       <c r="C78" t="n">
-        <v>-381724269.4209624</v>
+        <v>-616569650.678416</v>
       </c>
       <c r="D78" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -9234,13 +9234,13 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>159981689.5436021</v>
+        <v>226164033.8365528</v>
       </c>
       <c r="C79" t="n">
-        <v>-389034951.2546384</v>
+        <v>-618504264.9674021</v>
       </c>
       <c r="D79" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -9348,13 +9348,13 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>201940941.1117887</v>
+        <v>287387840.2114912</v>
       </c>
       <c r="C80" t="n">
-        <v>-451343395.5166952</v>
+        <v>-719582297.4409394</v>
       </c>
       <c r="D80" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -9458,13 +9458,13 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>199038252.9463307</v>
+        <v>283149053.8281337</v>
       </c>
       <c r="C81" t="n">
-        <v>-447386185.6953286</v>
+        <v>-713138153.5136787</v>
       </c>
       <c r="D81" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -9572,13 +9572,13 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>200536386.0293367</v>
+        <v>285278721.9658185</v>
       </c>
       <c r="C82" t="n">
-        <v>-450110034.1736351</v>
+        <v>-717356056.9629877</v>
       </c>
       <c r="D82" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -9686,13 +9686,13 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>205759380.4885022</v>
+        <v>295826005.8928929</v>
       </c>
       <c r="C83" t="n">
-        <v>-423798822.2369605</v>
+        <v>-684845866.2343649</v>
       </c>
       <c r="D83" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -9796,13 +9796,13 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>189088595.2522518</v>
+        <v>272014231.2749047</v>
       </c>
       <c r="C84" t="n">
-        <v>-395445249.0775359</v>
+        <v>-640643632.4785765</v>
       </c>
       <c r="D84" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -9906,13 +9906,13 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>223641556.3890886</v>
+        <v>320789113.3239766</v>
       </c>
       <c r="C85" t="n">
-        <v>-459278078.5597609</v>
+        <v>-738656926.3217984</v>
       </c>
       <c r="D85" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -10016,13 +10016,13 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>201021809.2568428</v>
+        <v>285970464.894981</v>
       </c>
       <c r="C86" t="n">
-        <v>-450970544.5014009</v>
+        <v>-718693340.5180732</v>
       </c>
       <c r="D86" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -10130,13 +10130,13 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>180714862.6879153</v>
+        <v>259513822.2850575</v>
       </c>
       <c r="C87" t="n">
-        <v>-386459896.4466831</v>
+        <v>-625232380.7979548</v>
       </c>
       <c r="D87" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -10244,13 +10244,13 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>192332759.4216259</v>
+        <v>273641607.671856</v>
       </c>
       <c r="C88" t="n">
-        <v>-434773788.9701531</v>
+        <v>-693677903.9160447</v>
       </c>
       <c r="D88" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -10354,13 +10354,13 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>160418897.5706784</v>
+        <v>226786550.2516718</v>
       </c>
       <c r="C89" t="n">
-        <v>-389911002.6655887</v>
+        <v>-619864072.960627</v>
       </c>
       <c r="D89" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -10464,13 +10464,13 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>183326049.5143205</v>
+        <v>260213516.9754689</v>
       </c>
       <c r="C90" t="n">
-        <v>-425033345.1795313</v>
+        <v>-676810304.4705592</v>
       </c>
       <c r="D90" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -10578,13 +10578,13 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>159985281.4310923</v>
+        <v>226169188.3207233</v>
       </c>
       <c r="C91" t="n">
-        <v>-389041687.233989</v>
+        <v>-618514843.849395</v>
       </c>
       <c r="D91" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -10696,13 +10696,13 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>178908355.1332637</v>
+        <v>254974684.4502476</v>
       </c>
       <c r="C92" t="n">
-        <v>-404735969.3286093</v>
+        <v>-648327480.5640734</v>
       </c>
       <c r="D92" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -10810,13 +10810,13 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>158953626.7530148</v>
+        <v>224717828.7056844</v>
       </c>
       <c r="C93" t="n">
-        <v>-386767804.1345814</v>
+        <v>-615039144.3747218</v>
       </c>
       <c r="D93" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -10920,13 +10920,13 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>159983783.1963968</v>
+        <v>226167038.3015949</v>
       </c>
       <c r="C94" t="n">
-        <v>-389038877.5547693</v>
+        <v>-618510431.2372736</v>
       </c>
       <c r="D94" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -11030,13 +11030,13 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>159031701.4770814</v>
+        <v>224820170.6684155</v>
       </c>
       <c r="C95" t="n">
-        <v>-387026708.7799101</v>
+        <v>-615413964.9004151</v>
       </c>
       <c r="D95" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -11140,13 +11140,13 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>191708627.3984575</v>
+        <v>274781804.7242188</v>
       </c>
       <c r="C96" t="n">
-        <v>-410724560.5956822</v>
+        <v>-661899490.7891164</v>
       </c>
       <c r="D96" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -11250,13 +11250,13 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>164829082.7846155</v>
+        <v>233259970.1339031</v>
       </c>
       <c r="C97" t="n">
-        <v>-396448779.1607118</v>
+        <v>-630603626.1936203</v>
       </c>
       <c r="D97" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -11368,13 +11368,13 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>191830326.5457348</v>
+        <v>274067975.5643117</v>
       </c>
       <c r="C98" t="n">
-        <v>-420857416.8751051</v>
+        <v>-675262354.2216074</v>
       </c>
       <c r="D98" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -11482,13 +11482,13 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>200745874.1465958</v>
+        <v>285555902.5664799</v>
       </c>
       <c r="C99" t="n">
-        <v>-450730133.2302119</v>
+        <v>-718258134.6457069</v>
       </c>
       <c r="D99" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -11596,13 +11596,13 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>195100893.162625</v>
+        <v>277547055.5154095</v>
       </c>
       <c r="C100" t="n">
-        <v>-440230697.0622374</v>
+        <v>-702044307.992703</v>
       </c>
       <c r="D100" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -11706,13 +11706,13 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>225334535.0004603</v>
+        <v>323741591.2967488</v>
       </c>
       <c r="C101" t="n">
-        <v>-455721416.1328683</v>
+        <v>-734507953.3498362</v>
       </c>
       <c r="D101" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -11820,13 +11820,13 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>170066567.4634582</v>
+        <v>241124046.2670941</v>
       </c>
       <c r="C102" t="n">
-        <v>-402058122.279879</v>
+        <v>-640531487.5712001</v>
       </c>
       <c r="D102" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -11934,13 +11934,13 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>184677066.2989198</v>
+        <v>262243332.2856171</v>
       </c>
       <c r="C103" t="n">
-        <v>-426343195.7846923</v>
+        <v>-679154550.8067428</v>
       </c>
       <c r="D103" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -12052,13 +12052,13 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>190705854.829486</v>
+        <v>271543321.4000739</v>
       </c>
       <c r="C104" t="n">
-        <v>-429290698.053645</v>
+        <v>-685788883.8156843</v>
       </c>
       <c r="D104" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -12166,13 +12166,13 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>173950496.5190559</v>
+        <v>247118332.88347</v>
       </c>
       <c r="C105" t="n">
-        <v>-404282480.4928117</v>
+        <v>-645348511.1651821</v>
       </c>
       <c r="D105" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -12280,13 +12280,13 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>236488082.5247939</v>
+        <v>337201433.0136378</v>
       </c>
       <c r="C106" t="n">
-        <v>-502234364.1522337</v>
+        <v>-800345615.03389</v>
       </c>
       <c r="D106" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -12394,13 +12394,13 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>212723687.7217174</v>
+        <v>304537376.5776873</v>
       </c>
       <c r="C107" t="n">
-        <v>-449317799.2371773</v>
+        <v>-721360980.5391968</v>
       </c>
       <c r="D107" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -12508,13 +12508,13 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>169111069.225488</v>
+        <v>239524588.7008033</v>
       </c>
       <c r="C108" t="n">
-        <v>-402939472.3102995</v>
+        <v>-641184656.1507736</v>
       </c>
       <c r="D108" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -12622,13 +12622,13 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>198336644.9666787</v>
+        <v>285177471.3559144</v>
       </c>
       <c r="C109" t="n">
-        <v>-411866837.4992051</v>
+        <v>-666124678.5824778</v>
       </c>
       <c r="D109" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -12736,13 +12736,13 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>158546247.0333468</v>
+        <v>224615062.5923977</v>
       </c>
       <c r="C110" t="n">
-        <v>-380475198.7775751</v>
+        <v>-606717622.250353</v>
       </c>
       <c r="D110" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -12854,13 +12854,13 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>189729394.5335976</v>
+        <v>272249754.7655263</v>
       </c>
       <c r="C111" t="n">
-        <v>-403999810.6284639</v>
+        <v>-652204163.8814831</v>
       </c>
       <c r="D111" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -12964,13 +12964,13 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>202072665.5388272</v>
+        <v>287408714.7674247</v>
       </c>
       <c r="C112" t="n">
-        <v>-453520694.1747884</v>
+        <v>-722485408.0931526</v>
       </c>
       <c r="D112" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -13074,13 +13074,13 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>161325373.0124752</v>
+        <v>228605661.3841797</v>
       </c>
       <c r="C113" t="n">
-        <v>-385652928.7783066</v>
+        <v>-614854348.7632763</v>
       </c>
       <c r="D113" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -13192,13 +13192,13 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>161054255.9680095</v>
+        <v>228201033.2161114</v>
       </c>
       <c r="C114" t="n">
-        <v>-385324290.4075406</v>
+        <v>-614288686.2252672</v>
       </c>
       <c r="D114" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -13310,13 +13310,13 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>228912456.7268519</v>
+        <v>326181861.1804546</v>
       </c>
       <c r="C115" t="n">
-        <v>-492802897.0585838</v>
+        <v>-785049507.6016762</v>
       </c>
       <c r="D115" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -13416,13 +13416,13 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>189903671.6324413</v>
+        <v>272145706.4409218</v>
       </c>
       <c r="C116" t="n">
-        <v>-408201000.6104372</v>
+        <v>-657809791.884734</v>
       </c>
       <c r="D116" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -13526,13 +13526,13 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>190128098.1234068</v>
+        <v>271862757.4238549</v>
       </c>
       <c r="C117" t="n">
-        <v>-415313302.3688121</v>
+        <v>-667248888.2380273</v>
       </c>
       <c r="D117" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -13644,13 +13644,13 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>219741114.3635682</v>
+        <v>315105951.0574893</v>
       </c>
       <c r="C118" t="n">
-        <v>-454396973.9048197</v>
+        <v>-730747426.1765029</v>
       </c>
       <c r="D118" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -13754,13 +13754,13 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>191441505.7863299</v>
+        <v>272863476.7660523</v>
       </c>
       <c r="C119" t="n">
-        <v>-427522610.3461448</v>
+        <v>-683812167.8925201</v>
       </c>
       <c r="D119" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -13860,13 +13860,13 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>166744254.6523182</v>
+        <v>236410689.9844101</v>
       </c>
       <c r="C120" t="n">
-        <v>-395359670.511667</v>
+        <v>-630186134.2139621</v>
       </c>
       <c r="D120" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -13970,13 +13970,13 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>159982778.8322647</v>
+        <v>226165597.0039313</v>
       </c>
       <c r="C121" t="n">
-        <v>-389036994.0382276</v>
+        <v>-618507473.1671422</v>
       </c>
       <c r="D121" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -14084,13 +14084,13 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>159450693.4018503</v>
+        <v>225900681.1727424</v>
       </c>
       <c r="C122" t="n">
-        <v>-382313786.5138384</v>
+        <v>-609564829.8951237</v>
       </c>
       <c r="D122" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -14202,13 +14202,13 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>160581153.2411571</v>
+        <v>227530799.8906835</v>
       </c>
       <c r="C123" t="n">
-        <v>-384341226.8542533</v>
+        <v>-612773015.4131714</v>
       </c>
       <c r="D123" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -14320,13 +14320,13 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>204412644.2140465</v>
+        <v>292912636.687263</v>
       </c>
       <c r="C124" t="n">
-        <v>-432688320.1416128</v>
+        <v>-696098767.0576134</v>
       </c>
       <c r="D124" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -14426,13 +14426,13 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>163617850.8680348</v>
+        <v>232006809.2622156</v>
       </c>
       <c r="C125" t="n">
-        <v>-388648087.9597438</v>
+        <v>-619910906.2042223</v>
       </c>
       <c r="D125" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -14536,13 +14536,13 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>188672409.5696528</v>
+        <v>269835674.2570578</v>
       </c>
       <c r="C126" t="n">
-        <v>-412151951.1620351</v>
+        <v>-662465103.058249</v>
       </c>
       <c r="D126" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -14650,13 +14650,13 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>180662603.712813</v>
+        <v>260004362.5773549</v>
       </c>
       <c r="C127" t="n">
-        <v>-380285375.9184469</v>
+        <v>-617075096.1658553</v>
       </c>
       <c r="D127" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -14768,13 +14768,13 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>159981312.4340496</v>
+        <v>226163492.6711283</v>
       </c>
       <c r="C128" t="n">
-        <v>-389034244.04576</v>
+        <v>-618503154.2930305</v>
       </c>
       <c r="D128" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -14878,13 +14878,13 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>190553921.2513739</v>
+        <v>272231389.1081073</v>
       </c>
       <c r="C129" t="n">
-        <v>-418754253.6420302</v>
+        <v>-671946254.9176275</v>
       </c>
       <c r="D129" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -14992,13 +14992,13 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>164680010.3926166</v>
+        <v>234504158.7149849</v>
       </c>
       <c r="C130" t="n">
-        <v>-379685424.6714844</v>
+        <v>-608853674.238616</v>
       </c>
       <c r="D130" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -15106,13 +15106,13 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>180693895.2109168</v>
+        <v>257577191.2416937</v>
       </c>
       <c r="C131" t="n">
-        <v>-407424798.7042264</v>
+        <v>-652668699.3305537</v>
       </c>
       <c r="D131" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -15220,13 +15220,13 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>162283396.6694638</v>
+        <v>230057768.3387714</v>
       </c>
       <c r="C132" t="n">
-        <v>-386557522.8375871</v>
+        <v>-616520724.873842</v>
       </c>
       <c r="D132" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -15334,13 +15334,13 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>159593752.1135564</v>
+        <v>225607327.2208885</v>
       </c>
       <c r="C133" t="n">
-        <v>-388307085.0363675</v>
+        <v>-617361142.6686318</v>
       </c>
       <c r="D133" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -15444,13 +15444,13 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>183568970.4222474</v>
+        <v>261178897.8119061</v>
       </c>
       <c r="C134" t="n">
-        <v>-418382782.426956</v>
+        <v>-668284335.5192387</v>
       </c>
       <c r="D134" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -15562,13 +15562,13 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>193274830.4161268</v>
+        <v>278202125.5705481</v>
       </c>
       <c r="C135" t="n">
-        <v>-400423351.3916775</v>
+        <v>-648938013.488188</v>
       </c>
       <c r="D135" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -15676,13 +15676,13 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>169039221.4966475</v>
+        <v>239771508.8132858</v>
       </c>
       <c r="C136" t="n">
-        <v>-398792434.4795803</v>
+        <v>-635790051.9050461</v>
       </c>
       <c r="D136" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -15790,13 +15790,13 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>187767923.9888766</v>
+        <v>268395005.4511626</v>
       </c>
       <c r="C137" t="n">
-        <v>-412204218.9547121</v>
+        <v>-662134595.8958046</v>
       </c>
       <c r="D137" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -15904,13 +15904,13 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>176614885.9983608</v>
+        <v>251362684.6463775</v>
       </c>
       <c r="C138" t="n">
-        <v>-404281953.2558571</v>
+        <v>-646644373.9702441</v>
       </c>
       <c r="D138" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -16014,13 +16014,13 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>214146793.1152762</v>
+        <v>304686586.0029499</v>
       </c>
       <c r="C139" t="n">
-        <v>-473637174.7999482</v>
+        <v>-753959532.9839897</v>
       </c>
       <c r="D139" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -16128,13 +16128,13 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>195694588.3217317</v>
+        <v>278683013.3011628</v>
       </c>
       <c r="C140" t="n">
-        <v>-437953639.0172651</v>
+        <v>-699336737.2919977</v>
       </c>
       <c r="D140" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -16238,13 +16238,13 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>161681400.0862358</v>
+        <v>229122462.9280137</v>
       </c>
       <c r="C141" t="n">
-        <v>-386249778.728037</v>
+        <v>-615810200.1162999</v>
       </c>
       <c r="D141" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -16356,13 +16356,13 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>199808924.882672</v>
+        <v>286652264.0822604</v>
       </c>
       <c r="C142" t="n">
-        <v>-421352675.5362641</v>
+        <v>-679269130.0227554</v>
       </c>
       <c r="D142" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -16466,13 +16466,13 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>187914817.4255285</v>
+        <v>268735102.2271433</v>
       </c>
       <c r="C143" t="n">
-        <v>-411011705.6538569</v>
+        <v>-660636716.3574395</v>
       </c>
       <c r="D143" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -16584,13 +16584,13 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>170030570.7160479</v>
+        <v>243601156.586562</v>
       </c>
       <c r="C144" t="n">
-        <v>-373916385.7070824</v>
+        <v>-603939255.377998</v>
       </c>
       <c r="D144" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -16698,13 +16698,13 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>218929775.7707652</v>
+        <v>315019437.858991</v>
       </c>
       <c r="C145" t="n">
-        <v>-440791059.8359208</v>
+        <v>-712316144.3485979</v>
       </c>
       <c r="D145" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -16808,13 +16808,13 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>162708234.4723862</v>
+        <v>230568678.7818459</v>
       </c>
       <c r="C146" t="n">
-        <v>-388472907.154898</v>
+        <v>-619213379.4449077</v>
       </c>
       <c r="D146" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -16926,13 +16926,13 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>193098927.3384862</v>
+        <v>274703017.1193153</v>
       </c>
       <c r="C147" t="n">
-        <v>-436513085.7480596</v>
+        <v>-696292944.7845743</v>
       </c>
       <c r="D147" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -17036,13 +17036,13 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>230555666.8963441</v>
+        <v>331539974.7603281</v>
       </c>
       <c r="C148" t="n">
-        <v>-459769917.9560463</v>
+        <v>-741698511.2020931</v>
       </c>
       <c r="D148" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -17150,13 +17150,13 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>193727869.7420573</v>
+        <v>275934405.7071202</v>
       </c>
       <c r="C149" t="n">
-        <v>-433795557.1452767</v>
+        <v>-693029384.238608</v>
       </c>
       <c r="D149" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -17260,13 +17260,13 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>172808170.7906583</v>
+        <v>245221390.8877693</v>
       </c>
       <c r="C150" t="n">
-        <v>-405162410.6592178</v>
+        <v>-645922673.169723</v>
       </c>
       <c r="D150" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -17370,13 +17370,13 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>190025554.5393861</v>
+        <v>271433622.9273621</v>
       </c>
       <c r="C151" t="n">
-        <v>-418302784.1040679</v>
+        <v>-671121900.1209217</v>
       </c>
       <c r="D151" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -17484,13 +17484,13 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>233758818.4293233</v>
+        <v>333327753.5744264</v>
       </c>
       <c r="C152" t="n">
-        <v>-497716248.5745634</v>
+        <v>-793362759.6305578</v>
       </c>
       <c r="D152" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -17590,13 +17590,13 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>197999048.2211913</v>
+        <v>281927973.9961489</v>
       </c>
       <c r="C153" t="n">
-        <v>-442524433.6819119</v>
+        <v>-706328223.660036</v>
       </c>
       <c r="D153" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -17704,13 +17704,13 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>170274010.9602531</v>
+        <v>241494785.4813281</v>
       </c>
       <c r="C154" t="n">
-        <v>-401599067.683601</v>
+        <v>-640042740.3329711</v>
       </c>
       <c r="D154" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -17814,13 +17814,13 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>217091423.600224</v>
+        <v>311085736.1148545</v>
       </c>
       <c r="C155" t="n">
-        <v>-452864053.2432491</v>
+        <v>-727727749.3847228</v>
       </c>
       <c r="D155" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -17928,13 +17928,13 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>166872681.8275874</v>
+        <v>236677036.0213428</v>
       </c>
       <c r="C156" t="n">
-        <v>-394659380.2129357</v>
+        <v>-629346904.2296659</v>
       </c>
       <c r="D156" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -18038,13 +18038,13 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>208841063.2337069</v>
+        <v>299827188.9903314</v>
       </c>
       <c r="C157" t="n">
-        <v>-433398500.873895</v>
+        <v>-698771109.8942244</v>
       </c>
       <c r="D157" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -18148,13 +18148,13 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>191697416.7709543</v>
+        <v>275722938.950241</v>
       </c>
       <c r="C158" t="n">
-        <v>-400171482.9756765</v>
+        <v>-647966189.414601</v>
       </c>
       <c r="D158" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -18262,13 +18262,13 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>163624090.056206</v>
+        <v>231870099.3434019</v>
       </c>
       <c r="C159" t="n">
-        <v>-390320148.7865415</v>
+        <v>-622072620.8410587</v>
       </c>
       <c r="D159" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -18376,13 +18376,13 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>230432261.7004661</v>
+        <v>331375399.2707284</v>
       </c>
       <c r="C160" t="n">
-        <v>-459446216.7997958</v>
+        <v>-741223418.8351234</v>
       </c>
       <c r="D160" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -18490,13 +18490,13 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>213054465.7445063</v>
+        <v>306411760.0856024</v>
       </c>
       <c r="C161" t="n">
-        <v>-433863851.7112849</v>
+        <v>-700964540.7794162</v>
       </c>
       <c r="D161" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -18604,13 +18604,13 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>192706308.6065789</v>
+        <v>274184724.1137281</v>
       </c>
       <c r="C162" t="n">
-        <v>-435326852.917184</v>
+        <v>-694568373.8249217</v>
       </c>
       <c r="D162" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -18718,13 +18718,13 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>208919250.3967201</v>
+        <v>299734528.2315714</v>
       </c>
       <c r="C163" t="n">
-        <v>-435841706.9338781</v>
+        <v>-702042015.4739696</v>
       </c>
       <c r="D163" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -18828,13 +18828,13 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>169634345.0394309</v>
+        <v>240554629.3470742</v>
       </c>
       <c r="C164" t="n">
-        <v>-400688439.0056636</v>
+        <v>-638542346.5098919</v>
       </c>
       <c r="D164" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -18938,13 +18938,13 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>214076451.9032896</v>
+        <v>307919216.6758572</v>
       </c>
       <c r="C165" t="n">
-        <v>-434970040.9152226</v>
+        <v>-702811392.4851085</v>
       </c>
       <c r="D165" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -19052,13 +19052,13 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>226014241.3440962</v>
+        <v>324395347.8652229</v>
       </c>
       <c r="C166" t="n">
-        <v>-460462448.9135036</v>
+        <v>-741076423.4641184</v>
       </c>
       <c r="D166" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -19162,13 +19162,13 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>169510653.6271445</v>
+        <v>240392358.7967031</v>
       </c>
       <c r="C167" t="n">
-        <v>-400288688.0457355</v>
+        <v>-637962998.1665426</v>
       </c>
       <c r="D167" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -19276,13 +19276,13 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>197544351.2653601</v>
+        <v>282423728.746169</v>
       </c>
       <c r="C168" t="n">
-        <v>-428644976.7766817</v>
+        <v>-687942724.5554985</v>
       </c>
       <c r="D168" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -19382,13 +19382,13 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>225147600.0272056</v>
+        <v>324236869.8379742</v>
       </c>
       <c r="C169" t="n">
-        <v>-446621699.3602381</v>
+        <v>-722257016.7834637</v>
       </c>
       <c r="D169" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -19496,13 +19496,13 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>204452339.7224762</v>
+        <v>293455255.8377674</v>
       </c>
       <c r="C170" t="n">
-        <v>-427274707.5131188</v>
+        <v>-688952220.5230802</v>
       </c>
       <c r="D170" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -19606,13 +19606,13 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>211436154.0418527</v>
+        <v>304014132.5989069</v>
       </c>
       <c r="C171" t="n">
-        <v>-432216727.6757636</v>
+        <v>-698175436.5643777</v>
       </c>
       <c r="D171" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -19716,13 +19716,13 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>224428130.6488923</v>
+        <v>321884934.3653171</v>
       </c>
       <c r="C172" t="n">
-        <v>-460835459.0009965</v>
+        <v>-741012669.4637401</v>
       </c>
       <c r="D172" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -19830,13 +19830,13 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>230867323.3203529</v>
+        <v>332054352.0411416</v>
       </c>
       <c r="C173" t="n">
-        <v>-459433945.2831934</v>
+        <v>-741350897.6632477</v>
       </c>
       <c r="D173" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -19944,13 +19944,13 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>188099519.5105205</v>
+        <v>268688270.2184461</v>
       </c>
       <c r="C174" t="n">
-        <v>-414814430.0133743</v>
+        <v>-665700112.87985</v>
       </c>
       <c r="D174" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -20058,13 +20058,13 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>226042122.9440573</v>
+        <v>325429242.7824501</v>
       </c>
       <c r="C175" t="n">
-        <v>-448979737.9827173</v>
+        <v>-725720479.2212398</v>
       </c>
       <c r="D175" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -20168,13 +20168,13 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>227661733.7457307</v>
+        <v>326432980.3894434</v>
       </c>
       <c r="C176" t="n">
-        <v>-466707593.4775785</v>
+        <v>-749984518.1305887</v>
       </c>
       <c r="D176" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -20274,13 +20274,13 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>189877414.6763963</v>
+        <v>271529942.5186161</v>
       </c>
       <c r="C177" t="n">
-        <v>-414587537.4387551</v>
+        <v>-666187380.9058965</v>
       </c>
       <c r="D177" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -20384,13 +20384,13 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>194700531.8312197</v>
+        <v>277018094.9322309</v>
       </c>
       <c r="C178" t="n">
-        <v>-439028991.2625205</v>
+        <v>-700296723.8155724</v>
       </c>
       <c r="D178" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -20498,13 +20498,13 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>193084589.4705866</v>
+        <v>274734659.9312125</v>
       </c>
       <c r="C179" t="n">
-        <v>-435886815.5279012</v>
+        <v>-695469769.7531233</v>
       </c>
       <c r="D179" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -20612,13 +20612,13 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>215805372.3812869</v>
+        <v>307962529.6169906</v>
       </c>
       <c r="C180" t="n">
-        <v>-465711154.7927014</v>
+        <v>-744215916.061385</v>
       </c>
       <c r="D180" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
increasing the grid size
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>241116409.9288566</v>
+        <v>105508726.4694378</v>
       </c>
       <c r="C2" t="n">
-        <v>-640516451.8613</v>
+        <v>-209018146.6045218</v>
       </c>
       <c r="D2" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>307840143.1691962</v>
+        <v>132646577.4596441</v>
       </c>
       <c r="C3" t="n">
-        <v>-744780978.6235237</v>
+        <v>-241504486.6946509</v>
       </c>
       <c r="D3" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>271851828.2804081</v>
+        <v>116529554.7152026</v>
       </c>
       <c r="C4" t="n">
-        <v>-668097385.7077036</v>
+        <v>-213442943.3238954</v>
       </c>
       <c r="D4" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>242120270.0446654</v>
+        <v>106092782.3304012</v>
       </c>
       <c r="C5" t="n">
-        <v>-644936176.4713304</v>
+        <v>-210929361.0420707</v>
       </c>
       <c r="D5" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>241816006.3231841</v>
+        <v>105991829.6311245</v>
       </c>
       <c r="C6" t="n">
-        <v>-644771741.2745878</v>
+        <v>-210946344.5005981</v>
       </c>
       <c r="D6" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>281822355.0883852</v>
+        <v>122395754.4997257</v>
       </c>
       <c r="C7" t="n">
-        <v>-711558460.5956467</v>
+        <v>-232183773.5343286</v>
       </c>
       <c r="D7" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>242249524.6977128</v>
+        <v>106102412.26284</v>
       </c>
       <c r="C8" t="n">
-        <v>-644492121.4329234</v>
+        <v>-210661424.2871895</v>
       </c>
       <c r="D8" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>272620302.1461084</v>
+        <v>117040622.1587794</v>
       </c>
       <c r="C9" t="n">
-        <v>-672338783.942363</v>
+        <v>-215321766.9774082</v>
       </c>
       <c r="D9" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>236537929.2857987</v>
+        <v>103861518.1174055</v>
       </c>
       <c r="C10" t="n">
-        <v>-636000231.6287237</v>
+        <v>-208247002.9008795</v>
       </c>
       <c r="D10" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>273356708.5186262</v>
+        <v>117134202.8675836</v>
       </c>
       <c r="C11" t="n">
-        <v>-670332549.0772539</v>
+        <v>-214123845.5357292</v>
       </c>
       <c r="D11" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>324139109.2556922</v>
+        <v>138056256.2293121</v>
       </c>
       <c r="C12" t="n">
-        <v>-747799482.7227929</v>
+        <v>-238975883.2737637</v>
       </c>
       <c r="D12" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>296404406.2602804</v>
+        <v>127395291.6096901</v>
       </c>
       <c r="C13" t="n">
-        <v>-718866741.0923098</v>
+        <v>-231756331.7183017</v>
       </c>
       <c r="D13" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>234421992.9689757</v>
+        <v>102692553.5673765</v>
       </c>
       <c r="C14" t="n">
-        <v>-627593821.3777303</v>
+        <v>-204683855.8293287</v>
       </c>
       <c r="D14" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>258153912.6522675</v>
+        <v>109438266.882265</v>
       </c>
       <c r="C15" t="n">
-        <v>-623356145.7801745</v>
+        <v>-195287931.0485279</v>
       </c>
       <c r="D15" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>325883524.4871363</v>
+        <v>138596224.7624223</v>
       </c>
       <c r="C16" t="n">
-        <v>-747398630.4843992</v>
+        <v>-238383033.7740149</v>
       </c>
       <c r="D16" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>303097785.9272359</v>
+        <v>130020051.2517149</v>
       </c>
       <c r="C17" t="n">
-        <v>-727024925.2444966</v>
+        <v>-234012094.1658826</v>
       </c>
       <c r="D17" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>312636899.8738974</v>
+        <v>134644140.8865899</v>
       </c>
       <c r="C18" t="n">
-        <v>-752270474.6464767</v>
+        <v>-243949740.2878812</v>
       </c>
       <c r="D18" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>329811766.0912105</v>
+        <v>139608841.0539081</v>
       </c>
       <c r="C19" t="n">
-        <v>-743155717.4879633</v>
+        <v>-235476230.8749945</v>
       </c>
       <c r="D19" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>241284616.1454389</v>
+        <v>105596981.9961531</v>
       </c>
       <c r="C20" t="n">
-        <v>-641108597.9145137</v>
+        <v>-209263009.2431625</v>
       </c>
       <c r="D20" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>334170860.8161556</v>
+        <v>141599423.6154124</v>
       </c>
       <c r="C21" t="n">
-        <v>-752220211.8294635</v>
+        <v>-238858232.1724758</v>
       </c>
       <c r="D21" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>318489476.4800459</v>
+        <v>134875384.7845174</v>
       </c>
       <c r="C22" t="n">
-        <v>-726238810.2783819</v>
+        <v>-229901430.6513903</v>
       </c>
       <c r="D22" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>240947429.0625636</v>
+        <v>105594822.7153038</v>
       </c>
       <c r="C23" t="n">
-        <v>-642618118.4559122</v>
+        <v>-210140147.9385734</v>
       </c>
       <c r="D23" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>241537608.1774869</v>
+        <v>105845394.8503075</v>
       </c>
       <c r="C24" t="n">
-        <v>-643785192.149943</v>
+        <v>-210537490.5371626</v>
       </c>
       <c r="D24" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>316028303.5171236</v>
+        <v>134781258.9465282</v>
       </c>
       <c r="C25" t="n">
-        <v>-737261747.7522157</v>
+        <v>-235788498.9133089</v>
       </c>
       <c r="D25" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>292111793.1974413</v>
+        <v>125182348.8449171</v>
       </c>
       <c r="C26" t="n">
-        <v>-705272189.3632073</v>
+        <v>-226212495.6601892</v>
       </c>
       <c r="D26" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>240803556.7309235</v>
+        <v>105460556.4692007</v>
       </c>
       <c r="C27" t="n">
-        <v>-641203341.7830828</v>
+        <v>-209469655.8274356</v>
       </c>
       <c r="D27" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>301625905.0998349</v>
+        <v>127417554.1764413</v>
       </c>
       <c r="C28" t="n">
-        <v>-693639299.8900316</v>
+        <v>-218170442.130488</v>
       </c>
       <c r="D28" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>259524364.4675499</v>
+        <v>110635064.8260035</v>
       </c>
       <c r="C29" t="n">
-        <v>-635159537.19867</v>
+        <v>-200693955.3049799</v>
       </c>
       <c r="D29" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>321125162.8406616</v>
+        <v>136104466.1075085</v>
       </c>
       <c r="C30" t="n">
-        <v>-732246856.0965803</v>
+        <v>-232184709.8015506</v>
       </c>
       <c r="D30" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>316034106.6327591</v>
+        <v>134783690.3161738</v>
       </c>
       <c r="C31" t="n">
-        <v>-737270796.7957494</v>
+        <v>-235791494.57205</v>
       </c>
       <c r="D31" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>240675486.9111191</v>
+        <v>105451235.8885704</v>
       </c>
       <c r="C32" t="n">
-        <v>-641645409.746622</v>
+        <v>-209736329.8344363</v>
       </c>
       <c r="D32" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>309591520.6783481</v>
+        <v>133553287.5962651</v>
       </c>
       <c r="C33" t="n">
-        <v>-750338693.3007903</v>
+        <v>-243785214.8407176</v>
       </c>
       <c r="D33" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>241180851.5727562</v>
+        <v>105716464.7564075</v>
       </c>
       <c r="C34" t="n">
-        <v>-643428200.0245736</v>
+        <v>-210474208.3568346</v>
       </c>
       <c r="D34" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>328636380.8735353</v>
+        <v>139066872.48509</v>
       </c>
       <c r="C35" t="n">
-        <v>-740617600.2250655</v>
+        <v>-234520873.5788515</v>
       </c>
       <c r="D35" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>324854430.5347658</v>
+        <v>138187606.9388872</v>
       </c>
       <c r="C36" t="n">
-        <v>-746200833.3122867</v>
+        <v>-238041235.5106107</v>
       </c>
       <c r="D36" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>261924235.3221091</v>
+        <v>111701037.9983043</v>
       </c>
       <c r="C37" t="n">
-        <v>-640369267.1781435</v>
+        <v>-202577032.8259242</v>
       </c>
       <c r="D37" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>266105340.8550061</v>
+        <v>113236264.3979196</v>
       </c>
       <c r="C38" t="n">
-        <v>-644524175.3137047</v>
+        <v>-203448141.3676558</v>
       </c>
       <c r="D38" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>233692973.6274313</v>
+        <v>102773319.0900762</v>
       </c>
       <c r="C39" t="n">
-        <v>-632156415.2001097</v>
+        <v>-207250826.245541</v>
       </c>
       <c r="D39" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>239958332.6812091</v>
+        <v>105017672.2254655</v>
       </c>
       <c r="C40" t="n">
-        <v>-638233803.9230567</v>
+        <v>-208242418.4061436</v>
       </c>
       <c r="D40" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>315871578.7534108</v>
+        <v>134701314.1507206</v>
       </c>
       <c r="C41" t="n">
-        <v>-736791243.5112112</v>
+        <v>-235598052.3902366</v>
       </c>
       <c r="D41" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>238081039.3346827</v>
+        <v>104439268.9421774</v>
       </c>
       <c r="C42" t="n">
-        <v>-637879350.5167651</v>
+        <v>-208685705.4748633</v>
       </c>
       <c r="D42" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>237917772.9119691</v>
+        <v>104063185.0347636</v>
       </c>
       <c r="C43" t="n">
-        <v>-632825810.5677013</v>
+        <v>-206174733.721487</v>
       </c>
       <c r="D43" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>271453178.3149346</v>
+        <v>116381563.0254742</v>
       </c>
       <c r="C44" t="n">
-        <v>-667689887.1368873</v>
+        <v>-213354002.2535594</v>
       </c>
       <c r="D44" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>228517245.6278447</v>
+        <v>100167826.3336622</v>
       </c>
       <c r="C45" t="n">
-        <v>-615422880.303871</v>
+        <v>-200491735.4238619</v>
       </c>
       <c r="D45" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>242289512.9431651</v>
+        <v>106181608.3227286</v>
       </c>
       <c r="C46" t="n">
-        <v>-645532582.8692462</v>
+        <v>-211176252.3923558</v>
       </c>
       <c r="D46" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>237611354.9062354</v>
+        <v>104367728.3348256</v>
       </c>
       <c r="C47" t="n">
-        <v>-638922073.3417053</v>
+        <v>-209373254.1300425</v>
       </c>
       <c r="D47" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>238716552.1387896</v>
+        <v>104424001.3408905</v>
       </c>
       <c r="C48" t="n">
-        <v>-634747027.1713309</v>
+        <v>-206884594.4189475</v>
       </c>
       <c r="D48" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>322745359.7031357</v>
+        <v>137283281.5320168</v>
       </c>
       <c r="C49" t="n">
-        <v>-742664354.0434316</v>
+        <v>-236821997.8006023</v>
       </c>
       <c r="D49" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>242277238.6826189</v>
+        <v>106000975.046599</v>
       </c>
       <c r="C50" t="n">
-        <v>-642799677.7142836</v>
+        <v>-209794092.8900959</v>
       </c>
       <c r="D50" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>277669410.9749006</v>
+        <v>117159326.3814496</v>
       </c>
       <c r="C51" t="n">
-        <v>-650638472.9506352</v>
+        <v>-203346207.1822138</v>
       </c>
       <c r="D51" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>284453677.0661486</v>
+        <v>123465584.6433238</v>
       </c>
       <c r="C52" t="n">
-        <v>-715576330.4317623</v>
+        <v>-233430269.622158</v>
       </c>
       <c r="D52" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>303309631.9706399</v>
+        <v>130665300.368854</v>
       </c>
       <c r="C53" t="n">
-        <v>-736125207.7363403</v>
+        <v>-238428189.4724956</v>
       </c>
       <c r="D53" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>229115395.803687</v>
+        <v>100367178.8657337</v>
       </c>
       <c r="C54" t="n">
-        <v>-615796001.4970576</v>
+        <v>-200478489.6620883</v>
       </c>
       <c r="D54" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>240709029.5342582</v>
+        <v>105352880.5020434</v>
       </c>
       <c r="C55" t="n">
-        <v>-639974477.0186136</v>
+        <v>-208877513.5332501</v>
       </c>
       <c r="D55" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>302373980.5765743</v>
+        <v>129647122.8856552</v>
       </c>
       <c r="C56" t="n">
-        <v>-724754887.8731717</v>
+        <v>-233086310.6818279</v>
       </c>
       <c r="D56" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>226115473.4363479</v>
+        <v>99652515.60497172</v>
       </c>
       <c r="C57" t="n">
-        <v>-618321946.9817134</v>
+        <v>-202793563.913616</v>
       </c>
       <c r="D57" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>287378257.0332168</v>
+        <v>124626453.9291485</v>
       </c>
       <c r="C58" t="n">
-        <v>-719565294.9595512</v>
+        <v>-234583616.9577389</v>
       </c>
       <c r="D58" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>264899440.4536139</v>
+        <v>112672866.8429443</v>
       </c>
       <c r="C59" t="n">
-        <v>-641513779.7746129</v>
+        <v>-202306174.8753476</v>
       </c>
       <c r="D59" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>278445845.2283827</v>
+        <v>120818759.6407465</v>
       </c>
       <c r="C60" t="n">
-        <v>-703174320.3226094</v>
+        <v>-228976588.5435393</v>
       </c>
       <c r="D60" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>313956072.1801931</v>
+        <v>136059248.6204675</v>
       </c>
       <c r="C61" t="n">
-        <v>-768109334.7570126</v>
+        <v>-251416086.562739</v>
       </c>
       <c r="D61" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>322741874.7063678</v>
+        <v>137281823.6174914</v>
       </c>
       <c r="C62" t="n">
-        <v>-742659074.352662</v>
+        <v>-236820256.6947784</v>
       </c>
       <c r="D62" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>263258404.8438024</v>
+        <v>111557958.197442</v>
       </c>
       <c r="C63" t="n">
-        <v>-632173952.7290845</v>
+        <v>-198188443.8184662</v>
       </c>
       <c r="D63" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>281833903.6966872</v>
+        <v>122342850.5698752</v>
       </c>
       <c r="C64" t="n">
-        <v>-710675747.4114839</v>
+        <v>-231739329.838951</v>
       </c>
       <c r="D64" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>259864791.7006577</v>
+        <v>113504335.765346</v>
       </c>
       <c r="C65" t="n">
-        <v>-677451073.353865</v>
+        <v>-221679853.6071709</v>
       </c>
       <c r="D65" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>279469335.2922495</v>
+        <v>117746875.3597333</v>
       </c>
       <c r="C66" t="n">
-        <v>-651169910.9945309</v>
+        <v>-203145161.1829448</v>
       </c>
       <c r="D66" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>284456288.9917687</v>
+        <v>123466691.2825127</v>
       </c>
       <c r="C67" t="n">
-        <v>-715581003.6488818</v>
+        <v>-233431851.2426446</v>
       </c>
       <c r="D67" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>259723469.9714658</v>
+        <v>110571376.8817002</v>
       </c>
       <c r="C68" t="n">
-        <v>-633302860.1094917</v>
+        <v>-199724522.8641171</v>
       </c>
       <c r="D68" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>261164753.2626413</v>
+        <v>110055601.0016471</v>
       </c>
       <c r="C69" t="n">
-        <v>-619107805.3630104</v>
+        <v>-192394145.9747593</v>
       </c>
       <c r="D69" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>272777273.7243389</v>
+        <v>115877033.3297141</v>
       </c>
       <c r="C70" t="n">
-        <v>-653863315.1116563</v>
+        <v>-206198179.3881435</v>
       </c>
       <c r="D70" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>305892356.1042734</v>
+        <v>130111079.5130356</v>
       </c>
       <c r="C71" t="n">
-        <v>-714595899.8409623</v>
+        <v>-227255961.6400539</v>
       </c>
       <c r="D71" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>241288520.0071773</v>
+        <v>105598637.6146314</v>
       </c>
       <c r="C72" t="n">
-        <v>-641116285.9121094</v>
+        <v>-209265622.4662407</v>
       </c>
       <c r="D72" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>316029866.5670241</v>
+        <v>134781913.8277764</v>
       </c>
       <c r="C73" t="n">
-        <v>-737264185.0951921</v>
+        <v>-235789305.7885106</v>
       </c>
       <c r="D73" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>279681540.434641</v>
+        <v>120457917.0446891</v>
       </c>
       <c r="C74" t="n">
-        <v>-691676297.3159117</v>
+        <v>-222901472.9667384</v>
       </c>
       <c r="D74" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>238606731.4384664</v>
+        <v>104656956.3492973</v>
       </c>
       <c r="C75" t="n">
-        <v>-638839898.102951</v>
+        <v>-208998483.7739748</v>
       </c>
       <c r="D75" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>330076763.9282188</v>
+        <v>140447377.957341</v>
       </c>
       <c r="C76" t="n">
-        <v>-755208195.1460632</v>
+        <v>-241190465.6660586</v>
       </c>
       <c r="D76" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>299439780.3822055</v>
+        <v>127382852.6466472</v>
       </c>
       <c r="C77" t="n">
-        <v>-703812662.4923407</v>
+        <v>-223616842.4244619</v>
       </c>
       <c r="D77" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>251216849.3362035</v>
+        <v>106918502.4314488</v>
       </c>
       <c r="C78" t="n">
-        <v>-616569650.678416</v>
+        <v>-193926183.2665913</v>
       </c>
       <c r="D78" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>226164033.8365528</v>
+        <v>99678515.17212091</v>
       </c>
       <c r="C79" t="n">
-        <v>-618504264.9674021</v>
+        <v>-202869844.3416095</v>
       </c>
       <c r="D79" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>287387840.2114912</v>
+        <v>124630512.6759802</v>
       </c>
       <c r="C80" t="n">
-        <v>-719582297.4409394</v>
+        <v>-234589366.480262</v>
       </c>
       <c r="D80" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>283149053.8281337</v>
+        <v>122906404.1367475</v>
       </c>
       <c r="C81" t="n">
-        <v>-713138153.5136787</v>
+        <v>-232588847.2752898</v>
       </c>
       <c r="D81" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>285278721.9658185</v>
+        <v>123834612.5745275</v>
       </c>
       <c r="C82" t="n">
-        <v>-717356056.9629877</v>
+        <v>-234081588.0408616</v>
       </c>
       <c r="D82" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>295826005.8928929</v>
+        <v>125024745.8866452</v>
       </c>
       <c r="C83" t="n">
-        <v>-684845866.2343649</v>
+        <v>-215332164.6101156</v>
       </c>
       <c r="D83" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>272014231.2749047</v>
+        <v>114770796.1817679</v>
       </c>
       <c r="C84" t="n">
-        <v>-640643632.4785765</v>
+        <v>-199968539.1906832</v>
       </c>
       <c r="D84" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>320789113.3239766</v>
+        <v>136399735.7707716</v>
       </c>
       <c r="C85" t="n">
-        <v>-738656926.3217984</v>
+        <v>-235342743.6443977</v>
       </c>
       <c r="D85" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>285970464.894981</v>
+        <v>124134250.592144</v>
       </c>
       <c r="C86" t="n">
-        <v>-718693340.5180732</v>
+        <v>-234550627.4243446</v>
       </c>
       <c r="D86" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>259513822.2850575</v>
+        <v>109970644.6036005</v>
       </c>
       <c r="C87" t="n">
-        <v>-625232380.7979548</v>
+        <v>-195827838.7745652</v>
       </c>
       <c r="D87" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>273641607.671856</v>
+        <v>118735399.5336341</v>
       </c>
       <c r="C88" t="n">
-        <v>-693677903.9160447</v>
+        <v>-225639454.349205</v>
       </c>
       <c r="D88" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>226786550.2516718</v>
+        <v>99948772.93257391</v>
       </c>
       <c r="C89" t="n">
-        <v>-619864072.960627</v>
+        <v>-203348593.3003232</v>
       </c>
       <c r="D89" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>260213516.9754689</v>
+        <v>113568385.9032365</v>
       </c>
       <c r="C90" t="n">
-        <v>-676810304.4705592</v>
+        <v>-221247347.6185689</v>
       </c>
       <c r="D90" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>226169188.3207233</v>
+        <v>99680708.61797616</v>
       </c>
       <c r="C91" t="n">
-        <v>-618514843.849395</v>
+        <v>-202873459.8895674</v>
       </c>
       <c r="D91" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>254974684.4502476</v>
+        <v>110142394.5216578</v>
       </c>
       <c r="C92" t="n">
-        <v>-648327480.5640734</v>
+        <v>-208562628.9073775</v>
       </c>
       <c r="D92" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>224717828.7056844</v>
+        <v>99031260.30550426</v>
       </c>
       <c r="C93" t="n">
-        <v>-615039144.3747218</v>
+        <v>-201602192.2960845</v>
       </c>
       <c r="D93" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>226167038.3015949</v>
+        <v>99679793.69599606</v>
       </c>
       <c r="C94" t="n">
-        <v>-618510431.2372736</v>
+        <v>-202871951.7895998</v>
       </c>
       <c r="D94" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>224820170.6684155</v>
+        <v>99085419.68022577</v>
       </c>
       <c r="C95" t="n">
-        <v>-615413964.9004151</v>
+        <v>-201758063.0948648</v>
       </c>
       <c r="D95" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>274781804.7242188</v>
+        <v>117016909.536118</v>
       </c>
       <c r="C96" t="n">
-        <v>-661899490.7891164</v>
+        <v>-209587252.9708545</v>
       </c>
       <c r="D96" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>233259970.1339031</v>
+        <v>102545355.9689802</v>
       </c>
       <c r="C97" t="n">
-        <v>-630603626.1936203</v>
+        <v>-206606667.7502118</v>
       </c>
       <c r="D97" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>274067975.5643117</v>
+        <v>117672836.3618993</v>
       </c>
       <c r="C98" t="n">
-        <v>-675262354.2216074</v>
+        <v>-216358649.6340961</v>
       </c>
       <c r="D98" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>285555902.5664799</v>
+        <v>123978034.8062271</v>
       </c>
       <c r="C99" t="n">
-        <v>-718258134.6457069</v>
+        <v>-234452325.5146987</v>
       </c>
       <c r="D99" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>277547055.5154095</v>
+        <v>120470081.3920262</v>
       </c>
       <c r="C100" t="n">
-        <v>-702044307.992703</v>
+        <v>-228674520.3612784</v>
       </c>
       <c r="D100" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>323741591.2967488</v>
+        <v>137093107.2131552</v>
       </c>
       <c r="C101" t="n">
-        <v>-734507953.3498362</v>
+        <v>-232680201.6958987</v>
       </c>
       <c r="D101" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>241124046.2670941</v>
+        <v>105511964.562603</v>
       </c>
       <c r="C102" t="n">
-        <v>-640531487.5712001</v>
+        <v>-209023256.3673792</v>
       </c>
       <c r="D102" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>262243332.2856171</v>
+        <v>114333012.3162275</v>
       </c>
       <c r="C103" t="n">
-        <v>-679154550.8067428</v>
+        <v>-221797612.6148877</v>
       </c>
       <c r="D103" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>271543321.4000739</v>
+        <v>117585726.1880774</v>
       </c>
       <c r="C104" t="n">
-        <v>-685788883.8156843</v>
+        <v>-222315825.1105521</v>
       </c>
       <c r="D104" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>247118332.88347</v>
+        <v>107604625.910323</v>
       </c>
       <c r="C105" t="n">
-        <v>-645348511.1651821</v>
+        <v>-209515713.5931183</v>
       </c>
       <c r="D105" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>337201433.0136378</v>
+        <v>145569466.401966</v>
       </c>
       <c r="C106" t="n">
-        <v>-800345615.03389</v>
+        <v>-261425231.6330547</v>
       </c>
       <c r="D106" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>304537376.5776873</v>
+        <v>130113878.5378258</v>
       </c>
       <c r="C107" t="n">
-        <v>-721360980.5391968</v>
+        <v>-230877998.5930108</v>
       </c>
       <c r="D107" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>239524588.7008033</v>
+        <v>105080389.1113953</v>
       </c>
       <c r="C108" t="n">
-        <v>-641184656.1507736</v>
+        <v>-209884292.3578205</v>
       </c>
       <c r="D108" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>285177471.3559144</v>
+        <v>120489265.4427217</v>
       </c>
       <c r="C109" t="n">
-        <v>-666124678.5824778</v>
+        <v>-208929469.54725</v>
       </c>
       <c r="D109" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>224615062.5923977</v>
+        <v>98461024.83522852</v>
       </c>
       <c r="C110" t="n">
-        <v>-606717622.250353</v>
+        <v>-197396514.180316</v>
       </c>
       <c r="D110" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>272249754.7655263</v>
+        <v>115607022.0688982</v>
       </c>
       <c r="C111" t="n">
-        <v>-652204163.8814831</v>
+        <v>-205529791.2928719</v>
       </c>
       <c r="D111" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>287408714.7674247</v>
+        <v>124822083.9285265</v>
       </c>
       <c r="C112" t="n">
-        <v>-722485408.0931526</v>
+        <v>-236031568.2958097</v>
       </c>
       <c r="D112" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>228605661.3841797</v>
+        <v>100156661.0837503</v>
       </c>
       <c r="C113" t="n">
-        <v>-614854348.7632763</v>
+        <v>-200172776.0156584</v>
       </c>
       <c r="D113" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>228201033.2161114</v>
+        <v>100001447.5327858</v>
       </c>
       <c r="C114" t="n">
-        <v>-614288686.2252672</v>
+        <v>-200022630.0171967</v>
       </c>
       <c r="D114" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>326181861.1804546</v>
+        <v>141041486.155849</v>
       </c>
       <c r="C115" t="n">
-        <v>-785049507.6016762</v>
+        <v>-256629137.1601039</v>
       </c>
       <c r="D115" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>272145706.4409218</v>
+        <v>115944493.4328775</v>
       </c>
       <c r="C116" t="n">
-        <v>-657809791.884734</v>
+        <v>-208300507.8710816</v>
       </c>
       <c r="D116" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>271862757.4238549</v>
+        <v>116477400.184276</v>
       </c>
       <c r="C117" t="n">
-        <v>-667248888.2380273</v>
+        <v>-213021100.7277543</v>
       </c>
       <c r="D117" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>315105951.0574893</v>
+        <v>134073855.6473529</v>
       </c>
       <c r="C118" t="n">
-        <v>-730747426.1765029</v>
+        <v>-232856329.5791467</v>
       </c>
       <c r="D118" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>272863476.7660523</v>
+        <v>117860571.0843874</v>
       </c>
       <c r="C119" t="n">
-        <v>-683812167.8925201</v>
+        <v>-220944422.1572055</v>
       </c>
       <c r="D119" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>236410689.9844101</v>
+        <v>103446922.0606982</v>
       </c>
       <c r="C120" t="n">
-        <v>-630186134.2139621</v>
+        <v>-205335959.0468844</v>
       </c>
       <c r="D120" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>226165597.0039313</v>
+        <v>99679180.36433366</v>
       </c>
       <c r="C121" t="n">
-        <v>-618507473.1671422</v>
+        <v>-202870940.8090142</v>
       </c>
       <c r="D121" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>225900681.1727424</v>
+        <v>99021577.51894188</v>
       </c>
       <c r="C122" t="n">
-        <v>-609564829.8951237</v>
+        <v>-198404658.9435754</v>
       </c>
       <c r="D122" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>227530799.8906835</v>
+        <v>99706732.31271403</v>
       </c>
       <c r="C123" t="n">
-        <v>-612773015.4131714</v>
+        <v>-199480058.8985869</v>
       </c>
       <c r="D123" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>292912636.687263</v>
+        <v>124840981.4588256</v>
       </c>
       <c r="C124" t="n">
-        <v>-696098767.0576134</v>
+        <v>-221515326.7091922</v>
       </c>
       <c r="D124" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>232006809.2622156</v>
+        <v>101482637.130122</v>
       </c>
       <c r="C125" t="n">
-        <v>-619910906.2042223</v>
+        <v>-201593533.2296944</v>
       </c>
       <c r="D125" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>269835674.2570578</v>
+        <v>115547775.5122885</v>
       </c>
       <c r="C126" t="n">
-        <v>-662465103.058249</v>
+        <v>-211230821.352387</v>
       </c>
       <c r="D126" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>260004362.5773549</v>
+        <v>109571273.3401862</v>
       </c>
       <c r="C127" t="n">
-        <v>-617075096.1658553</v>
+        <v>-191719277.4940407</v>
       </c>
       <c r="D127" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>226163492.6711283</v>
+        <v>99678284.8839162</v>
       </c>
       <c r="C128" t="n">
-        <v>-618503154.2930305</v>
+        <v>-202869464.7461046</v>
       </c>
       <c r="D128" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>272231389.1081073</v>
+        <v>116896498.8276936</v>
       </c>
       <c r="C129" t="n">
-        <v>-671946254.9176275</v>
+        <v>-215237703.2306432</v>
       </c>
       <c r="D129" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>234504158.7149849</v>
+        <v>101486613.3077085</v>
       </c>
       <c r="C130" t="n">
-        <v>-608853674.238616</v>
+        <v>-195192346.6161174</v>
       </c>
       <c r="D130" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>257577191.2416937</v>
+        <v>111206429.3717718</v>
       </c>
       <c r="C131" t="n">
-        <v>-652668699.3305537</v>
+        <v>-209942642.4337206</v>
       </c>
       <c r="D131" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>230057768.3387714</v>
+        <v>100690301.4471169</v>
       </c>
       <c r="C132" t="n">
-        <v>-616520724.873842</v>
+        <v>-200528169.7813111</v>
       </c>
       <c r="D132" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>225607327.2208885</v>
+        <v>99441616.50272426</v>
       </c>
       <c r="C133" t="n">
-        <v>-617361142.6686318</v>
+        <v>-202479162.9386826</v>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>261178897.8119061</v>
+        <v>113308239.1278594</v>
       </c>
       <c r="C134" t="n">
-        <v>-668284335.5192387</v>
+        <v>-216662236.3820526</v>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>278202125.5705481</v>
+        <v>117210532.9378552</v>
       </c>
       <c r="C135" t="n">
-        <v>-648938013.488188</v>
+        <v>-202388640.3289137</v>
       </c>
       <c r="D135" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>239771508.8132858</v>
+        <v>104803634.4021675</v>
       </c>
       <c r="C136" t="n">
-        <v>-635790051.9050461</v>
+        <v>-207065422.8186131</v>
       </c>
       <c r="D136" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>268395005.4511626</v>
+        <v>115088902.8054884</v>
       </c>
       <c r="C137" t="n">
-        <v>-662134595.8958046</v>
+        <v>-211475437.8546615</v>
       </c>
       <c r="D137" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>251362684.6463775</v>
+        <v>108953363.5511799</v>
       </c>
       <c r="C138" t="n">
-        <v>-646644373.9702441</v>
+        <v>-208830389.1402352</v>
       </c>
       <c r="D138" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>304686586.0029499</v>
+        <v>132227328.7373793</v>
       </c>
       <c r="C139" t="n">
-        <v>-753959532.9839897</v>
+        <v>-246882657.1680205</v>
       </c>
       <c r="D139" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>278683013.3011628</v>
+        <v>120645077.3307229</v>
       </c>
       <c r="C140" t="n">
-        <v>-699336737.2919977</v>
+        <v>-226992646.1945517</v>
       </c>
       <c r="D140" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>229122462.9280137</v>
+        <v>100370172.5250075</v>
       </c>
       <c r="C141" t="n">
-        <v>-615810200.1162999</v>
+        <v>-200483310.2279336</v>
       </c>
       <c r="D141" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>286652264.0822604</v>
+        <v>121803530.9674991</v>
       </c>
       <c r="C142" t="n">
-        <v>-679269130.0227554</v>
+        <v>-214929262.2081245</v>
       </c>
       <c r="D142" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>268735102.2271433</v>
+        <v>115093850.2074087</v>
       </c>
       <c r="C143" t="n">
-        <v>-660636716.3574395</v>
+        <v>-210639130.9912758</v>
       </c>
       <c r="D143" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>243601156.586562</v>
+        <v>103822953.4520017</v>
       </c>
       <c r="C144" t="n">
-        <v>-603939255.377998</v>
+        <v>-189930731.702317</v>
       </c>
       <c r="D144" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>315019437.858991</v>
+        <v>132877443.62134</v>
       </c>
       <c r="C145" t="n">
-        <v>-712316144.3485979</v>
+        <v>-224023748.5784365</v>
       </c>
       <c r="D145" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>230568678.7818459</v>
+        <v>101015466.2542255</v>
       </c>
       <c r="C146" t="n">
-        <v>-619213379.4449077</v>
+        <v>-201723206.6404476</v>
       </c>
       <c r="D146" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>274703017.1193153</v>
+        <v>119228449.4292004</v>
       </c>
       <c r="C147" t="n">
-        <v>-696292944.7845743</v>
+        <v>-226634202.4660612</v>
       </c>
       <c r="D147" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>331539974.7603281</v>
+        <v>140082692.4468106</v>
       </c>
       <c r="C148" t="n">
-        <v>-741698511.2020931</v>
+        <v>-234409595.1433657</v>
       </c>
       <c r="D148" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>275934405.7071202</v>
+        <v>119395384.9325225</v>
       </c>
       <c r="C149" t="n">
-        <v>-693029384.238608</v>
+        <v>-224644429.6894445</v>
       </c>
       <c r="D149" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>245221390.8877693</v>
+        <v>107077921.004971</v>
       </c>
       <c r="C150" t="n">
-        <v>-645922673.169723</v>
+        <v>-210415575.5129712</v>
       </c>
       <c r="D150" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>271433622.9273621</v>
+        <v>116599761.8003678</v>
       </c>
       <c r="C151" t="n">
-        <v>-671121900.1209217</v>
+        <v>-215056264.1719109</v>
       </c>
       <c r="D151" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>333327753.5744264</v>
+        <v>143874749.0634952</v>
       </c>
       <c r="C152" t="n">
-        <v>-793362759.6305578</v>
+        <v>-258943761.0773299</v>
       </c>
       <c r="D152" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>281927973.9961489</v>
+        <v>122093307.7635642</v>
       </c>
       <c r="C153" t="n">
-        <v>-706328223.660036</v>
+        <v>-229543200.8580566</v>
       </c>
       <c r="D153" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>241494785.4813281</v>
+        <v>105590085.9079321</v>
       </c>
       <c r="C154" t="n">
-        <v>-640042740.3329711</v>
+        <v>-208653782.3603525</v>
       </c>
       <c r="D154" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>311085736.1148545</v>
+        <v>132597887.1665408</v>
       </c>
       <c r="C155" t="n">
-        <v>-727727749.3847228</v>
+        <v>-232357831.3243726</v>
       </c>
       <c r="D155" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>236677036.0213428</v>
+        <v>103470805.8748131</v>
       </c>
       <c r="C156" t="n">
-        <v>-629346904.2296659</v>
+        <v>-204822101.9525426</v>
       </c>
       <c r="D156" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>299827188.9903314</v>
+        <v>127180613.9277396</v>
       </c>
       <c r="C157" t="n">
-        <v>-698771109.8942244</v>
+        <v>-221078511.4456128</v>
       </c>
       <c r="D157" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>275722938.950241</v>
+        <v>116386930.9560903</v>
       </c>
       <c r="C158" t="n">
-        <v>-647966189.414601</v>
+        <v>-202553336.0838474</v>
       </c>
       <c r="D158" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>231870099.3434019</v>
+        <v>101583352.7685994</v>
       </c>
       <c r="C159" t="n">
-        <v>-622072620.8410587</v>
+        <v>-202736787.3699743</v>
       </c>
       <c r="D159" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>331375399.2707284</v>
+        <v>139999211.642137</v>
       </c>
       <c r="C160" t="n">
-        <v>-741223418.8351234</v>
+        <v>-234218738.9120067</v>
       </c>
       <c r="D160" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>306411760.0856024</v>
+        <v>129403918.6188121</v>
       </c>
       <c r="C161" t="n">
-        <v>-700964540.7794162</v>
+        <v>-220561130.1128934</v>
       </c>
       <c r="D161" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>274184724.1137281</v>
+        <v>118958854.6132308</v>
       </c>
       <c r="C162" t="n">
-        <v>-694568373.8249217</v>
+        <v>-225924513.2256453</v>
       </c>
       <c r="D162" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>299734528.2315714</v>
+        <v>127361799.8553083</v>
       </c>
       <c r="C163" t="n">
-        <v>-702042015.4739696</v>
+        <v>-222684836.8283646</v>
       </c>
       <c r="D163" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>240554629.3470742</v>
+        <v>105214205.3888756</v>
       </c>
       <c r="C164" t="n">
-        <v>-638542346.5098919</v>
+        <v>-208202346.972273</v>
       </c>
       <c r="D164" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>307919216.6758572</v>
+        <v>130001514.6469524</v>
       </c>
       <c r="C165" t="n">
-        <v>-702811392.4851085</v>
+        <v>-221096251.1072609</v>
       </c>
       <c r="D165" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>324395347.8652229</v>
+        <v>137717459.0523186</v>
       </c>
       <c r="C166" t="n">
-        <v>-741076423.4641184</v>
+        <v>-235681984.5561872</v>
       </c>
       <c r="D166" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>240392358.7967031</v>
+        <v>105128541.7492181</v>
       </c>
       <c r="C167" t="n">
-        <v>-637962998.1665426</v>
+        <v>-207962133.4922707</v>
       </c>
       <c r="D167" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>282423728.746169</v>
+        <v>121060300.4620544</v>
       </c>
       <c r="C168" t="n">
-        <v>-687942724.5554985</v>
+        <v>-220297557.7979507</v>
       </c>
       <c r="D168" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>324236869.8379742</v>
+        <v>136483512.4430443</v>
       </c>
       <c r="C169" t="n">
-        <v>-722257016.7834637</v>
+        <v>-226734556.8126839</v>
       </c>
       <c r="D169" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>293455255.8377674</v>
+        <v>124548501.1505335</v>
       </c>
       <c r="C170" t="n">
-        <v>-688952220.5230802</v>
+        <v>-217902651.7519901</v>
       </c>
       <c r="D170" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>304014132.5989069</v>
+        <v>128464498.0296568</v>
       </c>
       <c r="C171" t="n">
-        <v>-698175436.5643777</v>
+        <v>-219784764.8501419</v>
       </c>
       <c r="D171" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>321884934.3653171</v>
+        <v>136901542.6570788</v>
       </c>
       <c r="C172" t="n">
-        <v>-741012669.4637401</v>
+        <v>-236224593.5605564</v>
       </c>
       <c r="D172" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>332054352.0411416</v>
+        <v>140229425.9082486</v>
       </c>
       <c r="C173" t="n">
-        <v>-741350897.6632477</v>
+        <v>-234134835.1599286</v>
       </c>
       <c r="D173" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>268688270.2184461</v>
+        <v>115411245.186507</v>
       </c>
       <c r="C174" t="n">
-        <v>-665700112.87985</v>
+        <v>-213155727.6359349</v>
       </c>
       <c r="D174" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>325429242.7824501</v>
+        <v>137088898.2118142</v>
       </c>
       <c r="C175" t="n">
-        <v>-725720479.2212398</v>
+        <v>-228123017.841619</v>
       </c>
       <c r="D175" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>326432980.3894434</v>
+        <v>138936348.0628513</v>
       </c>
       <c r="C176" t="n">
-        <v>-749984518.1305887</v>
+        <v>-239502436.3370571</v>
       </c>
       <c r="D176" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>271529942.5186161</v>
+        <v>116306647.5220219</v>
       </c>
       <c r="C177" t="n">
-        <v>-666187380.9058965</v>
+        <v>-212590809.3727053</v>
       </c>
       <c r="D177" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>277018094.9322309</v>
+        <v>120195467.8391005</v>
       </c>
       <c r="C178" t="n">
-        <v>-700296723.8155724</v>
+        <v>-227955826.4722086</v>
       </c>
       <c r="D178" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>274734659.9312125</v>
+        <v>119185180.0915828</v>
       </c>
       <c r="C179" t="n">
-        <v>-695469769.7531233</v>
+        <v>-226213221.2188751</v>
       </c>
       <c r="D179" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>307962529.6169906</v>
+        <v>132649677.9409595</v>
       </c>
       <c r="C180" t="n">
-        <v>-744215916.061385</v>
+        <v>-241194673.5050797</v>
       </c>
       <c r="D180" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
implementing CIPW on given data of Al-Mishwat
tried to run CIPWFULL with the data already given
eventually it worked
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>241116409.9288566</v>
+        <v>105508726.4694378</v>
       </c>
       <c r="C2" t="n">
-        <v>-640516451.8613</v>
+        <v>-209018146.6045218</v>
       </c>
       <c r="D2" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>307840143.1691962</v>
+        <v>132646577.4596441</v>
       </c>
       <c r="C3" t="n">
-        <v>-744780978.6235237</v>
+        <v>-241504486.6946509</v>
       </c>
       <c r="D3" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>271851828.2804081</v>
+        <v>116529554.7152026</v>
       </c>
       <c r="C4" t="n">
-        <v>-668097385.7077036</v>
+        <v>-213442943.3238954</v>
       </c>
       <c r="D4" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>242120270.0446654</v>
+        <v>106092782.3304012</v>
       </c>
       <c r="C5" t="n">
-        <v>-644936176.4713304</v>
+        <v>-210929361.0420707</v>
       </c>
       <c r="D5" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>241816006.3231841</v>
+        <v>105991829.6311245</v>
       </c>
       <c r="C6" t="n">
-        <v>-644771741.2745878</v>
+        <v>-210946344.5005981</v>
       </c>
       <c r="D6" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>281822355.0883852</v>
+        <v>122395754.4997257</v>
       </c>
       <c r="C7" t="n">
-        <v>-711558460.5956467</v>
+        <v>-232183773.5343286</v>
       </c>
       <c r="D7" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>242249524.6977128</v>
+        <v>106102412.26284</v>
       </c>
       <c r="C8" t="n">
-        <v>-644492121.4329234</v>
+        <v>-210661424.2871895</v>
       </c>
       <c r="D8" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>272620302.1461084</v>
+        <v>117040622.1587794</v>
       </c>
       <c r="C9" t="n">
-        <v>-672338783.942363</v>
+        <v>-215321766.9774082</v>
       </c>
       <c r="D9" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>236537929.2857987</v>
+        <v>103861518.1174055</v>
       </c>
       <c r="C10" t="n">
-        <v>-636000231.6287237</v>
+        <v>-208247002.9008795</v>
       </c>
       <c r="D10" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>273356708.5186262</v>
+        <v>117134202.8675836</v>
       </c>
       <c r="C11" t="n">
-        <v>-670332549.0772539</v>
+        <v>-214123845.5357292</v>
       </c>
       <c r="D11" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>324139109.2556922</v>
+        <v>138056256.2293121</v>
       </c>
       <c r="C12" t="n">
-        <v>-747799482.7227929</v>
+        <v>-238975883.2737637</v>
       </c>
       <c r="D12" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>296404406.2602804</v>
+        <v>127395291.6096901</v>
       </c>
       <c r="C13" t="n">
-        <v>-718866741.0923098</v>
+        <v>-231756331.7183017</v>
       </c>
       <c r="D13" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>234421992.9689757</v>
+        <v>102692553.5673765</v>
       </c>
       <c r="C14" t="n">
-        <v>-627593821.3777303</v>
+        <v>-204683855.8293287</v>
       </c>
       <c r="D14" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>258153912.6522675</v>
+        <v>109438266.882265</v>
       </c>
       <c r="C15" t="n">
-        <v>-623356145.7801745</v>
+        <v>-195287931.0485279</v>
       </c>
       <c r="D15" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>325883524.4871363</v>
+        <v>138596224.7624223</v>
       </c>
       <c r="C16" t="n">
-        <v>-747398630.4843992</v>
+        <v>-238383033.7740149</v>
       </c>
       <c r="D16" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>303097785.9272359</v>
+        <v>130020051.2517149</v>
       </c>
       <c r="C17" t="n">
-        <v>-727024925.2444966</v>
+        <v>-234012094.1658826</v>
       </c>
       <c r="D17" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>312636899.8738974</v>
+        <v>134644140.8865899</v>
       </c>
       <c r="C18" t="n">
-        <v>-752270474.6464767</v>
+        <v>-243949740.2878812</v>
       </c>
       <c r="D18" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>329811766.0912105</v>
+        <v>139608841.0539081</v>
       </c>
       <c r="C19" t="n">
-        <v>-743155717.4879633</v>
+        <v>-235476230.8749945</v>
       </c>
       <c r="D19" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>241284616.1454389</v>
+        <v>105596981.9961531</v>
       </c>
       <c r="C20" t="n">
-        <v>-641108597.9145137</v>
+        <v>-209263009.2431625</v>
       </c>
       <c r="D20" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>334170860.8161556</v>
+        <v>141599423.6154124</v>
       </c>
       <c r="C21" t="n">
-        <v>-752220211.8294635</v>
+        <v>-238858232.1724758</v>
       </c>
       <c r="D21" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>318489476.4800459</v>
+        <v>134875384.7845174</v>
       </c>
       <c r="C22" t="n">
-        <v>-726238810.2783819</v>
+        <v>-229901430.6513903</v>
       </c>
       <c r="D22" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>240947429.0625636</v>
+        <v>105594822.7153038</v>
       </c>
       <c r="C23" t="n">
-        <v>-642618118.4559122</v>
+        <v>-210140147.9385734</v>
       </c>
       <c r="D23" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>241537608.1774869</v>
+        <v>105845394.8503075</v>
       </c>
       <c r="C24" t="n">
-        <v>-643785192.149943</v>
+        <v>-210537490.5371626</v>
       </c>
       <c r="D24" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>316028303.5171236</v>
+        <v>134781258.9465282</v>
       </c>
       <c r="C25" t="n">
-        <v>-737261747.7522157</v>
+        <v>-235788498.9133089</v>
       </c>
       <c r="D25" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>292111793.1974413</v>
+        <v>125182348.8449171</v>
       </c>
       <c r="C26" t="n">
-        <v>-705272189.3632073</v>
+        <v>-226212495.6601892</v>
       </c>
       <c r="D26" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>240803556.7309235</v>
+        <v>105460556.4692007</v>
       </c>
       <c r="C27" t="n">
-        <v>-641203341.7830828</v>
+        <v>-209469655.8274356</v>
       </c>
       <c r="D27" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>301625905.0998349</v>
+        <v>127417554.1764413</v>
       </c>
       <c r="C28" t="n">
-        <v>-693639299.8900316</v>
+        <v>-218170442.130488</v>
       </c>
       <c r="D28" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>259524364.4675499</v>
+        <v>110635064.8260035</v>
       </c>
       <c r="C29" t="n">
-        <v>-635159537.19867</v>
+        <v>-200693955.3049799</v>
       </c>
       <c r="D29" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>321125162.8406616</v>
+        <v>136104466.1075085</v>
       </c>
       <c r="C30" t="n">
-        <v>-732246856.0965803</v>
+        <v>-232184709.8015506</v>
       </c>
       <c r="D30" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>316034106.6327591</v>
+        <v>134783690.3161738</v>
       </c>
       <c r="C31" t="n">
-        <v>-737270796.7957494</v>
+        <v>-235791494.57205</v>
       </c>
       <c r="D31" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>240675486.9111191</v>
+        <v>105451235.8885704</v>
       </c>
       <c r="C32" t="n">
-        <v>-641645409.746622</v>
+        <v>-209736329.8344363</v>
       </c>
       <c r="D32" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>309591520.6783481</v>
+        <v>133553287.5962651</v>
       </c>
       <c r="C33" t="n">
-        <v>-750338693.3007903</v>
+        <v>-243785214.8407176</v>
       </c>
       <c r="D33" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>241180851.5727562</v>
+        <v>105716464.7564075</v>
       </c>
       <c r="C34" t="n">
-        <v>-643428200.0245736</v>
+        <v>-210474208.3568346</v>
       </c>
       <c r="D34" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>328636380.8735353</v>
+        <v>139066872.48509</v>
       </c>
       <c r="C35" t="n">
-        <v>-740617600.2250655</v>
+        <v>-234520873.5788515</v>
       </c>
       <c r="D35" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>324854430.5347658</v>
+        <v>138187606.9388872</v>
       </c>
       <c r="C36" t="n">
-        <v>-746200833.3122867</v>
+        <v>-238041235.5106107</v>
       </c>
       <c r="D36" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>261924235.3221091</v>
+        <v>111701037.9983043</v>
       </c>
       <c r="C37" t="n">
-        <v>-640369267.1781435</v>
+        <v>-202577032.8259242</v>
       </c>
       <c r="D37" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>266105340.8550061</v>
+        <v>113236264.3979196</v>
       </c>
       <c r="C38" t="n">
-        <v>-644524175.3137047</v>
+        <v>-203448141.3676558</v>
       </c>
       <c r="D38" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>233692973.6274313</v>
+        <v>102773319.0900762</v>
       </c>
       <c r="C39" t="n">
-        <v>-632156415.2001097</v>
+        <v>-207250826.245541</v>
       </c>
       <c r="D39" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>239958332.6812091</v>
+        <v>105017672.2254655</v>
       </c>
       <c r="C40" t="n">
-        <v>-638233803.9230567</v>
+        <v>-208242418.4061436</v>
       </c>
       <c r="D40" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>315871578.7534108</v>
+        <v>134701314.1507206</v>
       </c>
       <c r="C41" t="n">
-        <v>-736791243.5112112</v>
+        <v>-235598052.3902366</v>
       </c>
       <c r="D41" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>238081039.3346827</v>
+        <v>104439268.9421774</v>
       </c>
       <c r="C42" t="n">
-        <v>-637879350.5167651</v>
+        <v>-208685705.4748633</v>
       </c>
       <c r="D42" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>237917772.9119691</v>
+        <v>104063185.0347636</v>
       </c>
       <c r="C43" t="n">
-        <v>-632825810.5677013</v>
+        <v>-206174733.721487</v>
       </c>
       <c r="D43" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>271453178.3149346</v>
+        <v>116381563.0254742</v>
       </c>
       <c r="C44" t="n">
-        <v>-667689887.1368873</v>
+        <v>-213354002.2535594</v>
       </c>
       <c r="D44" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>228517245.6278447</v>
+        <v>100167826.3336622</v>
       </c>
       <c r="C45" t="n">
-        <v>-615422880.303871</v>
+        <v>-200491735.4238619</v>
       </c>
       <c r="D45" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>242289512.9431651</v>
+        <v>106181608.3227286</v>
       </c>
       <c r="C46" t="n">
-        <v>-645532582.8692462</v>
+        <v>-211176252.3923558</v>
       </c>
       <c r="D46" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>237611354.9062354</v>
+        <v>104367728.3348256</v>
       </c>
       <c r="C47" t="n">
-        <v>-638922073.3417053</v>
+        <v>-209373254.1300425</v>
       </c>
       <c r="D47" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>238716552.1387896</v>
+        <v>104424001.3408905</v>
       </c>
       <c r="C48" t="n">
-        <v>-634747027.1713309</v>
+        <v>-206884594.4189475</v>
       </c>
       <c r="D48" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>322745359.7031357</v>
+        <v>137283281.5320168</v>
       </c>
       <c r="C49" t="n">
-        <v>-742664354.0434316</v>
+        <v>-236821997.8006023</v>
       </c>
       <c r="D49" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>242277238.6826189</v>
+        <v>106000975.046599</v>
       </c>
       <c r="C50" t="n">
-        <v>-642799677.7142836</v>
+        <v>-209794092.8900959</v>
       </c>
       <c r="D50" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>277669410.9749006</v>
+        <v>117159326.3814496</v>
       </c>
       <c r="C51" t="n">
-        <v>-650638472.9506352</v>
+        <v>-203346207.1822138</v>
       </c>
       <c r="D51" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>284453677.0661486</v>
+        <v>123465584.6433238</v>
       </c>
       <c r="C52" t="n">
-        <v>-715576330.4317623</v>
+        <v>-233430269.622158</v>
       </c>
       <c r="D52" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>303309631.9706399</v>
+        <v>130665300.368854</v>
       </c>
       <c r="C53" t="n">
-        <v>-736125207.7363403</v>
+        <v>-238428189.4724956</v>
       </c>
       <c r="D53" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>229115395.803687</v>
+        <v>100367178.8657337</v>
       </c>
       <c r="C54" t="n">
-        <v>-615796001.4970576</v>
+        <v>-200478489.6620883</v>
       </c>
       <c r="D54" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>240709029.5342582</v>
+        <v>105352880.5020434</v>
       </c>
       <c r="C55" t="n">
-        <v>-639974477.0186136</v>
+        <v>-208877513.5332501</v>
       </c>
       <c r="D55" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>302373980.5765743</v>
+        <v>129647122.8856552</v>
       </c>
       <c r="C56" t="n">
-        <v>-724754887.8731717</v>
+        <v>-233086310.6818279</v>
       </c>
       <c r="D56" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>226115473.4363479</v>
+        <v>99652515.60497172</v>
       </c>
       <c r="C57" t="n">
-        <v>-618321946.9817134</v>
+        <v>-202793563.913616</v>
       </c>
       <c r="D57" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>287378257.0332168</v>
+        <v>124626453.9291485</v>
       </c>
       <c r="C58" t="n">
-        <v>-719565294.9595512</v>
+        <v>-234583616.9577389</v>
       </c>
       <c r="D58" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>264899440.4536139</v>
+        <v>112672866.8429443</v>
       </c>
       <c r="C59" t="n">
-        <v>-641513779.7746129</v>
+        <v>-202306174.8753476</v>
       </c>
       <c r="D59" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>278445845.2283827</v>
+        <v>120818759.6407465</v>
       </c>
       <c r="C60" t="n">
-        <v>-703174320.3226094</v>
+        <v>-228976588.5435393</v>
       </c>
       <c r="D60" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>313956072.1801931</v>
+        <v>136059248.6204675</v>
       </c>
       <c r="C61" t="n">
-        <v>-768109334.7570126</v>
+        <v>-251416086.562739</v>
       </c>
       <c r="D61" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>322741874.7063678</v>
+        <v>137281823.6174914</v>
       </c>
       <c r="C62" t="n">
-        <v>-742659074.352662</v>
+        <v>-236820256.6947784</v>
       </c>
       <c r="D62" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>263258404.8438024</v>
+        <v>111557958.197442</v>
       </c>
       <c r="C63" t="n">
-        <v>-632173952.7290845</v>
+        <v>-198188443.8184662</v>
       </c>
       <c r="D63" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>281833903.6966872</v>
+        <v>122342850.5698752</v>
       </c>
       <c r="C64" t="n">
-        <v>-710675747.4114839</v>
+        <v>-231739329.838951</v>
       </c>
       <c r="D64" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>259864791.7006577</v>
+        <v>113504335.765346</v>
       </c>
       <c r="C65" t="n">
-        <v>-677451073.353865</v>
+        <v>-221679853.6071709</v>
       </c>
       <c r="D65" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>279469335.2922495</v>
+        <v>117746875.3597333</v>
       </c>
       <c r="C66" t="n">
-        <v>-651169910.9945309</v>
+        <v>-203145161.1829448</v>
       </c>
       <c r="D66" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>284456288.9917687</v>
+        <v>123466691.2825127</v>
       </c>
       <c r="C67" t="n">
-        <v>-715581003.6488818</v>
+        <v>-233431851.2426446</v>
       </c>
       <c r="D67" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>259723469.9714658</v>
+        <v>110571376.8817002</v>
       </c>
       <c r="C68" t="n">
-        <v>-633302860.1094917</v>
+        <v>-199724522.8641171</v>
       </c>
       <c r="D68" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>261164753.2626413</v>
+        <v>110055601.0016471</v>
       </c>
       <c r="C69" t="n">
-        <v>-619107805.3630104</v>
+        <v>-192394145.9747593</v>
       </c>
       <c r="D69" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>272777273.7243389</v>
+        <v>115877033.3297141</v>
       </c>
       <c r="C70" t="n">
-        <v>-653863315.1116563</v>
+        <v>-206198179.3881435</v>
       </c>
       <c r="D70" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>305892356.1042734</v>
+        <v>130111079.5130356</v>
       </c>
       <c r="C71" t="n">
-        <v>-714595899.8409623</v>
+        <v>-227255961.6400539</v>
       </c>
       <c r="D71" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>241288520.0071773</v>
+        <v>105598637.6146314</v>
       </c>
       <c r="C72" t="n">
-        <v>-641116285.9121094</v>
+        <v>-209265622.4662407</v>
       </c>
       <c r="D72" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>316029866.5670241</v>
+        <v>134781913.8277764</v>
       </c>
       <c r="C73" t="n">
-        <v>-737264185.0951921</v>
+        <v>-235789305.7885106</v>
       </c>
       <c r="D73" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>279681540.434641</v>
+        <v>120457917.0446891</v>
       </c>
       <c r="C74" t="n">
-        <v>-691676297.3159117</v>
+        <v>-222901472.9667384</v>
       </c>
       <c r="D74" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>238606731.4384664</v>
+        <v>104656956.3492973</v>
       </c>
       <c r="C75" t="n">
-        <v>-638839898.102951</v>
+        <v>-208998483.7739748</v>
       </c>
       <c r="D75" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>330076763.9282188</v>
+        <v>140447377.957341</v>
       </c>
       <c r="C76" t="n">
-        <v>-755208195.1460632</v>
+        <v>-241190465.6660586</v>
       </c>
       <c r="D76" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>299439780.3822055</v>
+        <v>127382852.6466472</v>
       </c>
       <c r="C77" t="n">
-        <v>-703812662.4923407</v>
+        <v>-223616842.4244619</v>
       </c>
       <c r="D77" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>251216849.3362035</v>
+        <v>106918502.4314488</v>
       </c>
       <c r="C78" t="n">
-        <v>-616569650.678416</v>
+        <v>-193926183.2665913</v>
       </c>
       <c r="D78" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>226164033.8365528</v>
+        <v>99678515.17212091</v>
       </c>
       <c r="C79" t="n">
-        <v>-618504264.9674021</v>
+        <v>-202869844.3416095</v>
       </c>
       <c r="D79" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>287387840.2114912</v>
+        <v>124630512.6759802</v>
       </c>
       <c r="C80" t="n">
-        <v>-719582297.4409394</v>
+        <v>-234589366.480262</v>
       </c>
       <c r="D80" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>283149053.8281337</v>
+        <v>122906404.1367475</v>
       </c>
       <c r="C81" t="n">
-        <v>-713138153.5136787</v>
+        <v>-232588847.2752898</v>
       </c>
       <c r="D81" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>285278721.9658185</v>
+        <v>123834612.5745275</v>
       </c>
       <c r="C82" t="n">
-        <v>-717356056.9629877</v>
+        <v>-234081588.0408616</v>
       </c>
       <c r="D82" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>295826005.8928929</v>
+        <v>125024745.8866452</v>
       </c>
       <c r="C83" t="n">
-        <v>-684845866.2343649</v>
+        <v>-215332164.6101156</v>
       </c>
       <c r="D83" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>272014231.2749047</v>
+        <v>114770796.1817679</v>
       </c>
       <c r="C84" t="n">
-        <v>-640643632.4785765</v>
+        <v>-199968539.1906832</v>
       </c>
       <c r="D84" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>320789113.3239766</v>
+        <v>136399735.7707716</v>
       </c>
       <c r="C85" t="n">
-        <v>-738656926.3217984</v>
+        <v>-235342743.6443977</v>
       </c>
       <c r="D85" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>285970464.894981</v>
+        <v>124134250.592144</v>
       </c>
       <c r="C86" t="n">
-        <v>-718693340.5180732</v>
+        <v>-234550627.4243446</v>
       </c>
       <c r="D86" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>259513822.2850575</v>
+        <v>109970644.6036005</v>
       </c>
       <c r="C87" t="n">
-        <v>-625232380.7979548</v>
+        <v>-195827838.7745652</v>
       </c>
       <c r="D87" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>273641607.671856</v>
+        <v>118735399.5336341</v>
       </c>
       <c r="C88" t="n">
-        <v>-693677903.9160447</v>
+        <v>-225639454.349205</v>
       </c>
       <c r="D88" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>226786550.2516718</v>
+        <v>99948772.93257391</v>
       </c>
       <c r="C89" t="n">
-        <v>-619864072.960627</v>
+        <v>-203348593.3003232</v>
       </c>
       <c r="D89" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>260213516.9754689</v>
+        <v>113568385.9032365</v>
       </c>
       <c r="C90" t="n">
-        <v>-676810304.4705592</v>
+        <v>-221247347.6185689</v>
       </c>
       <c r="D90" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>226169188.3207233</v>
+        <v>99680708.61797616</v>
       </c>
       <c r="C91" t="n">
-        <v>-618514843.849395</v>
+        <v>-202873459.8895674</v>
       </c>
       <c r="D91" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>254974684.4502476</v>
+        <v>110142394.5216578</v>
       </c>
       <c r="C92" t="n">
-        <v>-648327480.5640734</v>
+        <v>-208562628.9073775</v>
       </c>
       <c r="D92" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>224717828.7056844</v>
+        <v>99031260.30550426</v>
       </c>
       <c r="C93" t="n">
-        <v>-615039144.3747218</v>
+        <v>-201602192.2960845</v>
       </c>
       <c r="D93" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>226167038.3015949</v>
+        <v>99679793.69599606</v>
       </c>
       <c r="C94" t="n">
-        <v>-618510431.2372736</v>
+        <v>-202871951.7895998</v>
       </c>
       <c r="D94" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>224820170.6684155</v>
+        <v>99085419.68022577</v>
       </c>
       <c r="C95" t="n">
-        <v>-615413964.9004151</v>
+        <v>-201758063.0948648</v>
       </c>
       <c r="D95" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>274781804.7242188</v>
+        <v>117016909.536118</v>
       </c>
       <c r="C96" t="n">
-        <v>-661899490.7891164</v>
+        <v>-209587252.9708545</v>
       </c>
       <c r="D96" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>233259970.1339031</v>
+        <v>102545355.9689802</v>
       </c>
       <c r="C97" t="n">
-        <v>-630603626.1936203</v>
+        <v>-206606667.7502118</v>
       </c>
       <c r="D97" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>274067975.5643117</v>
+        <v>117672836.3618993</v>
       </c>
       <c r="C98" t="n">
-        <v>-675262354.2216074</v>
+        <v>-216358649.6340961</v>
       </c>
       <c r="D98" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>285555902.5664799</v>
+        <v>123978034.8062271</v>
       </c>
       <c r="C99" t="n">
-        <v>-718258134.6457069</v>
+        <v>-234452325.5146987</v>
       </c>
       <c r="D99" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>277547055.5154095</v>
+        <v>120470081.3920262</v>
       </c>
       <c r="C100" t="n">
-        <v>-702044307.992703</v>
+        <v>-228674520.3612784</v>
       </c>
       <c r="D100" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>323741591.2967488</v>
+        <v>137093107.2131552</v>
       </c>
       <c r="C101" t="n">
-        <v>-734507953.3498362</v>
+        <v>-232680201.6958987</v>
       </c>
       <c r="D101" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>241124046.2670941</v>
+        <v>105511964.562603</v>
       </c>
       <c r="C102" t="n">
-        <v>-640531487.5712001</v>
+        <v>-209023256.3673792</v>
       </c>
       <c r="D102" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>262243332.2856171</v>
+        <v>114333012.3162275</v>
       </c>
       <c r="C103" t="n">
-        <v>-679154550.8067428</v>
+        <v>-221797612.6148877</v>
       </c>
       <c r="D103" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>271543321.4000739</v>
+        <v>117585726.1880774</v>
       </c>
       <c r="C104" t="n">
-        <v>-685788883.8156843</v>
+        <v>-222315825.1105521</v>
       </c>
       <c r="D104" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>247118332.88347</v>
+        <v>107604625.910323</v>
       </c>
       <c r="C105" t="n">
-        <v>-645348511.1651821</v>
+        <v>-209515713.5931183</v>
       </c>
       <c r="D105" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>337201433.0136378</v>
+        <v>145569466.401966</v>
       </c>
       <c r="C106" t="n">
-        <v>-800345615.03389</v>
+        <v>-261425231.6330547</v>
       </c>
       <c r="D106" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>304537376.5776873</v>
+        <v>130113878.5378258</v>
       </c>
       <c r="C107" t="n">
-        <v>-721360980.5391968</v>
+        <v>-230877998.5930108</v>
       </c>
       <c r="D107" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>239524588.7008033</v>
+        <v>105080389.1113953</v>
       </c>
       <c r="C108" t="n">
-        <v>-641184656.1507736</v>
+        <v>-209884292.3578205</v>
       </c>
       <c r="D108" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>285177471.3559144</v>
+        <v>120489265.4427217</v>
       </c>
       <c r="C109" t="n">
-        <v>-666124678.5824778</v>
+        <v>-208929469.54725</v>
       </c>
       <c r="D109" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>224615062.5923977</v>
+        <v>98461024.83522852</v>
       </c>
       <c r="C110" t="n">
-        <v>-606717622.250353</v>
+        <v>-197396514.180316</v>
       </c>
       <c r="D110" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>272249754.7655263</v>
+        <v>115607022.0688982</v>
       </c>
       <c r="C111" t="n">
-        <v>-652204163.8814831</v>
+        <v>-205529791.2928719</v>
       </c>
       <c r="D111" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>287408714.7674247</v>
+        <v>124822083.9285265</v>
       </c>
       <c r="C112" t="n">
-        <v>-722485408.0931526</v>
+        <v>-236031568.2958097</v>
       </c>
       <c r="D112" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>228605661.3841797</v>
+        <v>100156661.0837503</v>
       </c>
       <c r="C113" t="n">
-        <v>-614854348.7632763</v>
+        <v>-200172776.0156584</v>
       </c>
       <c r="D113" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>228201033.2161114</v>
+        <v>100001447.5327858</v>
       </c>
       <c r="C114" t="n">
-        <v>-614288686.2252672</v>
+        <v>-200022630.0171967</v>
       </c>
       <c r="D114" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>326181861.1804546</v>
+        <v>141041486.155849</v>
       </c>
       <c r="C115" t="n">
-        <v>-785049507.6016762</v>
+        <v>-256629137.1601039</v>
       </c>
       <c r="D115" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>272145706.4409218</v>
+        <v>115944493.4328775</v>
       </c>
       <c r="C116" t="n">
-        <v>-657809791.884734</v>
+        <v>-208300507.8710816</v>
       </c>
       <c r="D116" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>271862757.4238549</v>
+        <v>116477400.184276</v>
       </c>
       <c r="C117" t="n">
-        <v>-667248888.2380273</v>
+        <v>-213021100.7277543</v>
       </c>
       <c r="D117" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>315105951.0574893</v>
+        <v>134073855.6473529</v>
       </c>
       <c r="C118" t="n">
-        <v>-730747426.1765029</v>
+        <v>-232856329.5791467</v>
       </c>
       <c r="D118" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>272863476.7660523</v>
+        <v>117860571.0843874</v>
       </c>
       <c r="C119" t="n">
-        <v>-683812167.8925201</v>
+        <v>-220944422.1572055</v>
       </c>
       <c r="D119" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>236410689.9844101</v>
+        <v>103446922.0606982</v>
       </c>
       <c r="C120" t="n">
-        <v>-630186134.2139621</v>
+        <v>-205335959.0468844</v>
       </c>
       <c r="D120" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>226165597.0039313</v>
+        <v>99679180.36433366</v>
       </c>
       <c r="C121" t="n">
-        <v>-618507473.1671422</v>
+        <v>-202870940.8090142</v>
       </c>
       <c r="D121" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>225900681.1727424</v>
+        <v>99021577.51894188</v>
       </c>
       <c r="C122" t="n">
-        <v>-609564829.8951237</v>
+        <v>-198404658.9435754</v>
       </c>
       <c r="D122" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>227530799.8906835</v>
+        <v>99706732.31271403</v>
       </c>
       <c r="C123" t="n">
-        <v>-612773015.4131714</v>
+        <v>-199480058.8985869</v>
       </c>
       <c r="D123" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>292912636.687263</v>
+        <v>124840981.4588256</v>
       </c>
       <c r="C124" t="n">
-        <v>-696098767.0576134</v>
+        <v>-221515326.7091922</v>
       </c>
       <c r="D124" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>232006809.2622156</v>
+        <v>101482637.130122</v>
       </c>
       <c r="C125" t="n">
-        <v>-619910906.2042223</v>
+        <v>-201593533.2296944</v>
       </c>
       <c r="D125" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>269835674.2570578</v>
+        <v>115547775.5122885</v>
       </c>
       <c r="C126" t="n">
-        <v>-662465103.058249</v>
+        <v>-211230821.352387</v>
       </c>
       <c r="D126" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>260004362.5773549</v>
+        <v>109571273.3401862</v>
       </c>
       <c r="C127" t="n">
-        <v>-617075096.1658553</v>
+        <v>-191719277.4940407</v>
       </c>
       <c r="D127" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>226163492.6711283</v>
+        <v>99678284.8839162</v>
       </c>
       <c r="C128" t="n">
-        <v>-618503154.2930305</v>
+        <v>-202869464.7461046</v>
       </c>
       <c r="D128" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>272231389.1081073</v>
+        <v>116896498.8276936</v>
       </c>
       <c r="C129" t="n">
-        <v>-671946254.9176275</v>
+        <v>-215237703.2306432</v>
       </c>
       <c r="D129" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>234504158.7149849</v>
+        <v>101486613.3077085</v>
       </c>
       <c r="C130" t="n">
-        <v>-608853674.238616</v>
+        <v>-195192346.6161174</v>
       </c>
       <c r="D130" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>257577191.2416937</v>
+        <v>111206429.3717718</v>
       </c>
       <c r="C131" t="n">
-        <v>-652668699.3305537</v>
+        <v>-209942642.4337206</v>
       </c>
       <c r="D131" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>230057768.3387714</v>
+        <v>100690301.4471169</v>
       </c>
       <c r="C132" t="n">
-        <v>-616520724.873842</v>
+        <v>-200528169.7813111</v>
       </c>
       <c r="D132" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>225607327.2208885</v>
+        <v>99441616.50272426</v>
       </c>
       <c r="C133" t="n">
-        <v>-617361142.6686318</v>
+        <v>-202479162.9386826</v>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>261178897.8119061</v>
+        <v>113308239.1278594</v>
       </c>
       <c r="C134" t="n">
-        <v>-668284335.5192387</v>
+        <v>-216662236.3820526</v>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>278202125.5705481</v>
+        <v>117210532.9378552</v>
       </c>
       <c r="C135" t="n">
-        <v>-648938013.488188</v>
+        <v>-202388640.3289137</v>
       </c>
       <c r="D135" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>239771508.8132858</v>
+        <v>104803634.4021675</v>
       </c>
       <c r="C136" t="n">
-        <v>-635790051.9050461</v>
+        <v>-207065422.8186131</v>
       </c>
       <c r="D136" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>268395005.4511626</v>
+        <v>115088902.8054884</v>
       </c>
       <c r="C137" t="n">
-        <v>-662134595.8958046</v>
+        <v>-211475437.8546615</v>
       </c>
       <c r="D137" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>251362684.6463775</v>
+        <v>108953363.5511799</v>
       </c>
       <c r="C138" t="n">
-        <v>-646644373.9702441</v>
+        <v>-208830389.1402352</v>
       </c>
       <c r="D138" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>304686586.0029499</v>
+        <v>132227328.7373793</v>
       </c>
       <c r="C139" t="n">
-        <v>-753959532.9839897</v>
+        <v>-246882657.1680205</v>
       </c>
       <c r="D139" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>278683013.3011628</v>
+        <v>120645077.3307229</v>
       </c>
       <c r="C140" t="n">
-        <v>-699336737.2919977</v>
+        <v>-226992646.1945517</v>
       </c>
       <c r="D140" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>229122462.9280137</v>
+        <v>100370172.5250075</v>
       </c>
       <c r="C141" t="n">
-        <v>-615810200.1162999</v>
+        <v>-200483310.2279336</v>
       </c>
       <c r="D141" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>286652264.0822604</v>
+        <v>121803530.9674991</v>
       </c>
       <c r="C142" t="n">
-        <v>-679269130.0227554</v>
+        <v>-214929262.2081245</v>
       </c>
       <c r="D142" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>268735102.2271433</v>
+        <v>115093850.2074087</v>
       </c>
       <c r="C143" t="n">
-        <v>-660636716.3574395</v>
+        <v>-210639130.9912758</v>
       </c>
       <c r="D143" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>243601156.586562</v>
+        <v>103822953.4520017</v>
       </c>
       <c r="C144" t="n">
-        <v>-603939255.377998</v>
+        <v>-189930731.702317</v>
       </c>
       <c r="D144" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>315019437.858991</v>
+        <v>132877443.62134</v>
       </c>
       <c r="C145" t="n">
-        <v>-712316144.3485979</v>
+        <v>-224023748.5784365</v>
       </c>
       <c r="D145" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>230568678.7818459</v>
+        <v>101015466.2542255</v>
       </c>
       <c r="C146" t="n">
-        <v>-619213379.4449077</v>
+        <v>-201723206.6404476</v>
       </c>
       <c r="D146" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>274703017.1193153</v>
+        <v>119228449.4292004</v>
       </c>
       <c r="C147" t="n">
-        <v>-696292944.7845743</v>
+        <v>-226634202.4660612</v>
       </c>
       <c r="D147" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>331539974.7603281</v>
+        <v>140082692.4468106</v>
       </c>
       <c r="C148" t="n">
-        <v>-741698511.2020931</v>
+        <v>-234409595.1433657</v>
       </c>
       <c r="D148" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>275934405.7071202</v>
+        <v>119395384.9325225</v>
       </c>
       <c r="C149" t="n">
-        <v>-693029384.238608</v>
+        <v>-224644429.6894445</v>
       </c>
       <c r="D149" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>245221390.8877693</v>
+        <v>107077921.004971</v>
       </c>
       <c r="C150" t="n">
-        <v>-645922673.169723</v>
+        <v>-210415575.5129712</v>
       </c>
       <c r="D150" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>271433622.9273621</v>
+        <v>116599761.8003678</v>
       </c>
       <c r="C151" t="n">
-        <v>-671121900.1209217</v>
+        <v>-215056264.1719109</v>
       </c>
       <c r="D151" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>333327753.5744264</v>
+        <v>143874749.0634952</v>
       </c>
       <c r="C152" t="n">
-        <v>-793362759.6305578</v>
+        <v>-258943761.0773299</v>
       </c>
       <c r="D152" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>281927973.9961489</v>
+        <v>122093307.7635642</v>
       </c>
       <c r="C153" t="n">
-        <v>-706328223.660036</v>
+        <v>-229543200.8580566</v>
       </c>
       <c r="D153" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>241494785.4813281</v>
+        <v>105590085.9079321</v>
       </c>
       <c r="C154" t="n">
-        <v>-640042740.3329711</v>
+        <v>-208653782.3603525</v>
       </c>
       <c r="D154" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>311085736.1148545</v>
+        <v>132597887.1665408</v>
       </c>
       <c r="C155" t="n">
-        <v>-727727749.3847228</v>
+        <v>-232357831.3243726</v>
       </c>
       <c r="D155" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>236677036.0213428</v>
+        <v>103470805.8748131</v>
       </c>
       <c r="C156" t="n">
-        <v>-629346904.2296659</v>
+        <v>-204822101.9525426</v>
       </c>
       <c r="D156" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>299827188.9903314</v>
+        <v>127180613.9277396</v>
       </c>
       <c r="C157" t="n">
-        <v>-698771109.8942244</v>
+        <v>-221078511.4456128</v>
       </c>
       <c r="D157" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>275722938.950241</v>
+        <v>116386930.9560903</v>
       </c>
       <c r="C158" t="n">
-        <v>-647966189.414601</v>
+        <v>-202553336.0838474</v>
       </c>
       <c r="D158" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>231870099.3434019</v>
+        <v>101583352.7685994</v>
       </c>
       <c r="C159" t="n">
-        <v>-622072620.8410587</v>
+        <v>-202736787.3699743</v>
       </c>
       <c r="D159" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>331375399.2707284</v>
+        <v>139999211.642137</v>
       </c>
       <c r="C160" t="n">
-        <v>-741223418.8351234</v>
+        <v>-234218738.9120067</v>
       </c>
       <c r="D160" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>306411760.0856024</v>
+        <v>129403918.6188121</v>
       </c>
       <c r="C161" t="n">
-        <v>-700964540.7794162</v>
+        <v>-220561130.1128934</v>
       </c>
       <c r="D161" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>274184724.1137281</v>
+        <v>118958854.6132308</v>
       </c>
       <c r="C162" t="n">
-        <v>-694568373.8249217</v>
+        <v>-225924513.2256453</v>
       </c>
       <c r="D162" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>299734528.2315714</v>
+        <v>127361799.8553083</v>
       </c>
       <c r="C163" t="n">
-        <v>-702042015.4739696</v>
+        <v>-222684836.8283646</v>
       </c>
       <c r="D163" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>240554629.3470742</v>
+        <v>105214205.3888756</v>
       </c>
       <c r="C164" t="n">
-        <v>-638542346.5098919</v>
+        <v>-208202346.972273</v>
       </c>
       <c r="D164" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>307919216.6758572</v>
+        <v>130001514.6469524</v>
       </c>
       <c r="C165" t="n">
-        <v>-702811392.4851085</v>
+        <v>-221096251.1072609</v>
       </c>
       <c r="D165" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>324395347.8652229</v>
+        <v>137717459.0523186</v>
       </c>
       <c r="C166" t="n">
-        <v>-741076423.4641184</v>
+        <v>-235681984.5561872</v>
       </c>
       <c r="D166" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>240392358.7967031</v>
+        <v>105128541.7492181</v>
       </c>
       <c r="C167" t="n">
-        <v>-637962998.1665426</v>
+        <v>-207962133.4922707</v>
       </c>
       <c r="D167" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>282423728.746169</v>
+        <v>121060300.4620544</v>
       </c>
       <c r="C168" t="n">
-        <v>-687942724.5554985</v>
+        <v>-220297557.7979507</v>
       </c>
       <c r="D168" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>324236869.8379742</v>
+        <v>136483512.4430443</v>
       </c>
       <c r="C169" t="n">
-        <v>-722257016.7834637</v>
+        <v>-226734556.8126839</v>
       </c>
       <c r="D169" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>293455255.8377674</v>
+        <v>124548501.1505335</v>
       </c>
       <c r="C170" t="n">
-        <v>-688952220.5230802</v>
+        <v>-217902651.7519901</v>
       </c>
       <c r="D170" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>304014132.5989069</v>
+        <v>128464498.0296568</v>
       </c>
       <c r="C171" t="n">
-        <v>-698175436.5643777</v>
+        <v>-219784764.8501419</v>
       </c>
       <c r="D171" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>321884934.3653171</v>
+        <v>136901542.6570788</v>
       </c>
       <c r="C172" t="n">
-        <v>-741012669.4637401</v>
+        <v>-236224593.5605564</v>
       </c>
       <c r="D172" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>332054352.0411416</v>
+        <v>140229425.9082486</v>
       </c>
       <c r="C173" t="n">
-        <v>-741350897.6632477</v>
+        <v>-234134835.1599286</v>
       </c>
       <c r="D173" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>268688270.2184461</v>
+        <v>115411245.186507</v>
       </c>
       <c r="C174" t="n">
-        <v>-665700112.87985</v>
+        <v>-213155727.6359349</v>
       </c>
       <c r="D174" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>325429242.7824501</v>
+        <v>137088898.2118142</v>
       </c>
       <c r="C175" t="n">
-        <v>-725720479.2212398</v>
+        <v>-228123017.841619</v>
       </c>
       <c r="D175" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>326432980.3894434</v>
+        <v>138936348.0628513</v>
       </c>
       <c r="C176" t="n">
-        <v>-749984518.1305887</v>
+        <v>-239502436.3370571</v>
       </c>
       <c r="D176" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>271529942.5186161</v>
+        <v>116306647.5220219</v>
       </c>
       <c r="C177" t="n">
-        <v>-666187380.9058965</v>
+        <v>-212590809.3727053</v>
       </c>
       <c r="D177" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>277018094.9322309</v>
+        <v>120195467.8391005</v>
       </c>
       <c r="C178" t="n">
-        <v>-700296723.8155724</v>
+        <v>-227955826.4722086</v>
       </c>
       <c r="D178" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>274734659.9312125</v>
+        <v>119185180.0915828</v>
       </c>
       <c r="C179" t="n">
-        <v>-695469769.7531233</v>
+        <v>-226213221.2188751</v>
       </c>
       <c r="D179" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>307962529.6169906</v>
+        <v>132649677.9409595</v>
       </c>
       <c r="C180" t="n">
-        <v>-744215916.061385</v>
+        <v>-241194673.5050797</v>
       </c>
       <c r="D180" t="n">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
Biplot of with QAPF classification highlighted
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF180"/>
+  <dimension ref="A1:AG180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,11 @@
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
+          <t>QAPF</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
           <t>area</t>
         </is>
       </c>
@@ -633,7 +638,12 @@
           <t>A.I.Kyshtymov,1959</t>
         </is>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG2" t="n">
         <v>5</v>
       </c>
     </row>
@@ -747,7 +757,12 @@
           <t>E.K.Boborykin,1955</t>
         </is>
       </c>
-      <c r="AF3" t="n">
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -865,7 +880,12 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF4" t="n">
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -979,7 +999,12 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF5" t="n">
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1093,7 +1118,12 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF6" t="n">
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG6" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1203,7 +1233,12 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF7" t="n">
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1317,7 +1352,12 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF8" t="n">
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1435,7 +1475,12 @@
           <t>V.K.Sadakov,1966</t>
         </is>
       </c>
-      <c r="AF9" t="n">
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG9" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1553,7 +1598,12 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF10" t="n">
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG10" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1667,7 +1717,12 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF11" t="n">
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG11" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1777,7 +1832,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF12" t="n">
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG12" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1883,7 +1943,12 @@
           <t>I.M.Sargina,1959</t>
         </is>
       </c>
-      <c r="AF13" t="n">
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG13" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1997,7 +2062,12 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF14" t="n">
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG14" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2107,7 +2177,12 @@
           <t>I.A.Sklyar,1938</t>
         </is>
       </c>
-      <c r="AF15" t="n">
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG15" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2221,7 +2296,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF16" t="n">
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG16" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2331,7 +2411,12 @@
           <t>I.M.Sargina,1959</t>
         </is>
       </c>
-      <c r="AF17" t="n">
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG17" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2445,7 +2530,12 @@
           <t>E.K.Boborykin,1955</t>
         </is>
       </c>
-      <c r="AF18" t="n">
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG18" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2551,7 +2641,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF19" t="n">
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG19" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2665,7 +2760,12 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF20" t="n">
+      <c r="AF20" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG20" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2775,7 +2875,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF21" t="n">
+      <c r="AF21" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG21" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2881,7 +2986,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF22" t="n">
+      <c r="AF22" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG22" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2987,7 +3097,12 @@
           <t>E.G.Bordyugov,1966</t>
         </is>
       </c>
-      <c r="AF23" t="n">
+      <c r="AF23" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG23" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3101,7 +3216,12 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF24" t="n">
+      <c r="AF24" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG24" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3215,7 +3335,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF25" t="n">
+      <c r="AF25" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG25" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3325,7 +3450,12 @@
           <t>I.A.Nikitin,1959</t>
         </is>
       </c>
-      <c r="AF26" t="n">
+      <c r="AF26" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG26" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3439,7 +3569,12 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF27" t="n">
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG27" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3553,7 +3688,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF28" t="n">
+      <c r="AF28" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG28" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3663,7 +3803,12 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF29" t="n">
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG29" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3769,7 +3914,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF30" t="n">
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG30" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3883,7 +4033,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF31" t="n">
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG31" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3997,7 +4152,12 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF32" t="n">
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG32" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4107,7 +4267,12 @@
           <t>E.K.Boborykin,1955</t>
         </is>
       </c>
-      <c r="AF33" t="n">
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG33" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4221,7 +4386,12 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF34" t="n">
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG34" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4331,7 +4501,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF35" t="n">
+      <c r="AF35" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG35" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4449,7 +4624,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF36" t="n">
+      <c r="AF36" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG36" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4559,7 +4739,12 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF37" t="n">
+      <c r="AF37" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG37" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4673,7 +4858,12 @@
           <t>l.D.Gatiev,1938</t>
         </is>
       </c>
-      <c r="AF38" t="n">
+      <c r="AF38" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG38" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4791,7 +4981,12 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF39" t="n">
+      <c r="AF39" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG39" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4909,7 +5104,12 @@
           <t>P.P.Kolesnichenko,1964</t>
         </is>
       </c>
-      <c r="AF40" t="n">
+      <c r="AF40" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG40" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5023,7 +5223,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF41" t="n">
+      <c r="AF41" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5141,7 +5346,12 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF42" t="n">
+      <c r="AF42" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG42" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5255,7 +5465,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF43" t="n">
+      <c r="AF43" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG43" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5373,7 +5588,12 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF44" t="n">
+      <c r="AF44" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG44" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5491,7 +5711,12 @@
           <t>E.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF45" t="n">
+      <c r="AF45" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG45" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5601,7 +5826,12 @@
           <t>A.I.Kyshtymov,1962</t>
         </is>
       </c>
-      <c r="AF46" t="n">
+      <c r="AF46" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG46" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5719,7 +5949,12 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF47" t="n">
+      <c r="AF47" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG47" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5833,7 +6068,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF48" t="n">
+      <c r="AF48" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG48" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5947,7 +6187,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF49" t="n">
+      <c r="AF49" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG49" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6057,7 +6302,12 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF50" t="n">
+      <c r="AF50" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG50" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6171,7 +6421,12 @@
           <t>I.M.Sargina,1960</t>
         </is>
       </c>
-      <c r="AF51" t="n">
+      <c r="AF51" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG51" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6281,7 +6536,12 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF52" t="n">
+      <c r="AF52" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG52" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6395,7 +6655,12 @@
           <t>V.M.Ol'khovik,1959</t>
         </is>
       </c>
-      <c r="AF53" t="n">
+      <c r="AF53" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG53" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6513,7 +6778,12 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF54" t="n">
+      <c r="AF54" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG54" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6627,7 +6897,12 @@
           <t>Yu.A.Odinetz,1937</t>
         </is>
       </c>
-      <c r="AF55" t="n">
+      <c r="AF55" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG55" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6737,7 +7012,12 @@
           <t>I.M.Sargina,1958</t>
         </is>
       </c>
-      <c r="AF56" t="n">
+      <c r="AF56" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG56" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6847,7 +7127,12 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF57" t="n">
+      <c r="AF57" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG57" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6957,7 +7242,12 @@
           <t>V.I.Plyasunov,1976</t>
         </is>
       </c>
-      <c r="AF58" t="n">
+      <c r="AF58" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG58" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7071,7 +7361,12 @@
           <t>I.D.Gatiev,1938</t>
         </is>
       </c>
-      <c r="AF59" t="n">
+      <c r="AF59" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG59" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7181,7 +7476,12 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF60" t="n">
+      <c r="AF60" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG60" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7291,7 +7591,12 @@
           <t>E.K.Boborykin,1965</t>
         </is>
       </c>
-      <c r="AF61" t="n">
+      <c r="AF61" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG61" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7405,7 +7710,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF62" t="n">
+      <c r="AF62" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG62" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7519,7 +7829,12 @@
           <t>I.A.Sklyar,1938</t>
         </is>
       </c>
-      <c r="AF63" t="n">
+      <c r="AF63" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG63" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7637,7 +7952,12 @@
           <t>G.A.Zhukov,1954</t>
         </is>
       </c>
-      <c r="AF64" t="n">
+      <c r="AF64" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG64" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7751,7 +8071,12 @@
           <t>A.I.Kyshtymov,1962</t>
         </is>
       </c>
-      <c r="AF65" t="n">
+      <c r="AF65" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG65" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7865,7 +8190,12 @@
           <t>I.M.Sargina,1956</t>
         </is>
       </c>
-      <c r="AF66" t="n">
+      <c r="AF66" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG66" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7979,7 +8309,12 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF67" t="n">
+      <c r="AF67" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG67" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8093,7 +8428,12 @@
           <t>I.D.Gatiev,1938</t>
         </is>
       </c>
-      <c r="AF68" t="n">
+      <c r="AF68" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG68" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8207,7 +8547,12 @@
           <t>I.M.Sargina,1956</t>
         </is>
       </c>
-      <c r="AF69" t="n">
+      <c r="AF69" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG69" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8317,7 +8662,12 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF70" t="n">
+      <c r="AF70" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG70" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8427,7 +8777,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF71" t="n">
+      <c r="AF71" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG71" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8541,7 +8896,12 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF72" t="n">
+      <c r="AF72" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG72" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8655,7 +9015,12 @@
           <t>V.N.Stavitsky,1958</t>
         </is>
       </c>
-      <c r="AF73" t="n">
+      <c r="AF73" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG73" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8765,7 +9130,12 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF74" t="n">
+      <c r="AF74" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG74" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8883,7 +9253,12 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF75" t="n">
+      <c r="AF75" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG75" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8997,7 +9372,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF76" t="n">
+      <c r="AF76" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG76" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9111,7 +9491,12 @@
           <t>V.P.Azhina,1960</t>
         </is>
       </c>
-      <c r="AF77" t="n">
+      <c r="AF77" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG77" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9225,7 +9610,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF78" t="n">
+      <c r="AF78" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG78" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9339,7 +9729,12 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
-      <c r="AF79" t="n">
+      <c r="AF79" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG79" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9449,7 +9844,12 @@
           <t>V.I.Plyasunov,1976</t>
         </is>
       </c>
-      <c r="AF80" t="n">
+      <c r="AF80" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG80" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9563,7 +9963,12 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF81" t="n">
+      <c r="AF81" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG81" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9677,7 +10082,12 @@
           <t>S.V.Blagodatsky,1964</t>
         </is>
       </c>
-      <c r="AF82" t="n">
+      <c r="AF82" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG82" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9787,7 +10197,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF83" t="n">
+      <c r="AF83" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG83" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9897,7 +10312,12 @@
           <t>I.M.Sargina,1960</t>
         </is>
       </c>
-      <c r="AF84" t="n">
+      <c r="AF84" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG84" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10007,7 +10427,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF85" t="n">
+      <c r="AF85" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG85" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10121,7 +10546,12 @@
           <t>S.V.Blagodatsky,1964</t>
         </is>
       </c>
-      <c r="AF86" t="n">
+      <c r="AF86" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG86" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10235,7 +10665,12 @@
           <t>l.A.Sklyar,1938</t>
         </is>
       </c>
-      <c r="AF87" t="n">
+      <c r="AF87" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG87" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10345,7 +10780,12 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF88" t="n">
+      <c r="AF88" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG88" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10455,7 +10895,12 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF89" t="n">
+      <c r="AF89" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG89" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10569,7 +11014,12 @@
           <t>A.l.Kyshtymov,1962</t>
         </is>
       </c>
-      <c r="AF90" t="n">
+      <c r="AF90" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG90" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10687,7 +11137,12 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
-      <c r="AF91" t="n">
+      <c r="AF91" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG91" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10801,7 +11256,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF92" t="n">
+      <c r="AF92" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG92" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10911,7 +11371,12 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF93" t="n">
+      <c r="AF93" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG93" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11021,7 +11486,12 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF94" t="n">
+      <c r="AF94" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG94" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11131,7 +11601,12 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF95" t="n">
+      <c r="AF95" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG95" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11241,7 +11716,12 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF96" t="n">
+      <c r="AF96" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG96" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11359,7 +11839,12 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF97" t="n">
+      <c r="AF97" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG97" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11473,7 +11958,12 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF98" t="n">
+      <c r="AF98" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG98" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11587,7 +12077,12 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF99" t="n">
+      <c r="AF99" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG99" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11697,7 +12192,12 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF100" t="n">
+      <c r="AF100" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG100" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11811,7 +12311,12 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF101" t="n">
+      <c r="AF101" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG101" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11925,7 +12430,12 @@
           <t>Yu.A.Odinetz,1937</t>
         </is>
       </c>
-      <c r="AF102" t="n">
+      <c r="AF102" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG102" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12043,7 +12553,12 @@
           <t>A.I.Kyshtymov,1962</t>
         </is>
       </c>
-      <c r="AF103" t="n">
+      <c r="AF103" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG103" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12157,7 +12672,12 @@
           <t>G.V.Andreev,1955</t>
         </is>
       </c>
-      <c r="AF104" t="n">
+      <c r="AF104" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG104" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12271,7 +12791,12 @@
           <t>A.E.Fishkin,1967</t>
         </is>
       </c>
-      <c r="AF105" t="n">
+      <c r="AF105" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG105" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12385,7 +12910,12 @@
           <t>E.K.Boborykin,1956</t>
         </is>
       </c>
-      <c r="AF106" t="n">
+      <c r="AF106" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG106" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12499,7 +13029,12 @@
           <t>l.A.Nikitin,1959</t>
         </is>
       </c>
-      <c r="AF107" t="n">
+      <c r="AF107" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG107" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12613,7 +13148,12 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF108" t="n">
+      <c r="AF108" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG108" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12727,7 +13267,12 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF109" t="n">
+      <c r="AF109" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG109" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12845,7 +13390,12 @@
           <t>K.S.Sukhov,1962</t>
         </is>
       </c>
-      <c r="AF110" t="n">
+      <c r="AF110" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG110" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12955,7 +13505,12 @@
           <t>S.E.Sinitsky,1957</t>
         </is>
       </c>
-      <c r="AF111" t="n">
+      <c r="AF111" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG111" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13065,7 +13620,12 @@
           <t>G.I.Kremchukov,1936</t>
         </is>
       </c>
-      <c r="AF112" t="n">
+      <c r="AF112" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG112" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13183,7 +13743,12 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF113" t="n">
+      <c r="AF113" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG113" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13301,7 +13866,12 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF114" t="n">
+      <c r="AF114" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG114" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13407,7 +13977,12 @@
           <t>E.K.Boborykin,1956</t>
         </is>
       </c>
-      <c r="AF115" t="n">
+      <c r="AF115" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG115" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13517,7 +14092,12 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF116" t="n">
+      <c r="AF116" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG116" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13635,7 +14215,12 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF117" t="n">
+      <c r="AF117" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG117" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13745,7 +14330,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF118" t="n">
+      <c r="AF118" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG118" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13851,7 +14441,12 @@
           <t>G.I.Bogomolov,1967</t>
         </is>
       </c>
-      <c r="AF119" t="n">
+      <c r="AF119" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG119" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13961,7 +14556,12 @@
           <t>A.l.Kyshtymov,1959</t>
         </is>
       </c>
-      <c r="AF120" t="n">
+      <c r="AF120" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG120" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14075,7 +14675,12 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
-      <c r="AF121" t="n">
+      <c r="AF121" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG121" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14193,7 +14798,12 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF122" t="n">
+      <c r="AF122" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG122" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14311,7 +14921,12 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF123" t="n">
+      <c r="AF123" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG123" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14417,7 +15032,12 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF124" t="n">
+      <c r="AF124" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG124" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14527,7 +15147,12 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF125" t="n">
+      <c r="AF125" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG125" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14641,7 +15266,12 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF126" t="n">
+      <c r="AF126" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG126" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14759,7 +15389,12 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF127" t="n">
+      <c r="AF127" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG127" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14869,7 +15504,12 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF128" t="n">
+      <c r="AF128" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG128" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14983,7 +15623,12 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF129" t="n">
+      <c r="AF129" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG129" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15097,7 +15742,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF130" t="n">
+      <c r="AF130" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG130" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15211,7 +15861,12 @@
           <t>E.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF131" t="n">
+      <c r="AF131" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG131" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15325,7 +15980,12 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF132" t="n">
+      <c r="AF132" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG132" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15435,7 +16095,12 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF133" t="n">
+      <c r="AF133" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG133" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15553,7 +16218,12 @@
           <t>G.P.Kozlov,1964</t>
         </is>
       </c>
-      <c r="AF134" t="n">
+      <c r="AF134" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG134" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15667,7 +16337,12 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF135" t="n">
+      <c r="AF135" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG135" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15781,7 +16456,12 @@
           <t>Yu.A.Odinetz,1937</t>
         </is>
       </c>
-      <c r="AF136" t="n">
+      <c r="AF136" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG136" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15895,7 +16575,12 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF137" t="n">
+      <c r="AF137" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG137" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16005,7 +16690,12 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF138" t="n">
+      <c r="AF138" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG138" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16119,7 +16809,12 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF139" t="n">
+      <c r="AF139" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG139" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16229,7 +16924,12 @@
           <t>A.D.Sokolov,1961</t>
         </is>
       </c>
-      <c r="AF140" t="n">
+      <c r="AF140" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG140" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16347,7 +17047,12 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF141" t="n">
+      <c r="AF141" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG141" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16457,7 +17162,12 @@
           <t>G.A.Zhukov,1956</t>
         </is>
       </c>
-      <c r="AF142" t="n">
+      <c r="AF142" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG142" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16575,7 +17285,12 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF143" t="n">
+      <c r="AF143" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG143" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16689,7 +17404,12 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF144" t="n">
+      <c r="AF144" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG144" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16799,7 +17519,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF145" t="n">
+      <c r="AF145" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG145" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16917,7 +17642,12 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF146" t="n">
+      <c r="AF146" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG146" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17027,7 +17757,12 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF147" t="n">
+      <c r="AF147" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG147" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17141,7 +17876,12 @@
           <t>F.A.Golovachev,1935</t>
         </is>
       </c>
-      <c r="AF148" t="n">
+      <c r="AF148" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG148" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17251,7 +17991,12 @@
           <t>G.I.Bogomolov,1967</t>
         </is>
       </c>
-      <c r="AF149" t="n">
+      <c r="AF149" t="inlineStr">
+        <is>
+          <t>quartz monzodiorite\quartz monzogabbro</t>
+        </is>
+      </c>
+      <c r="AG149" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17361,7 +18106,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF150" t="n">
+      <c r="AF150" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG150" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17475,7 +18225,12 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF151" t="n">
+      <c r="AF151" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG151" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17581,7 +18336,12 @@
           <t>E.K.Boborykin,1955</t>
         </is>
       </c>
-      <c r="AF152" t="n">
+      <c r="AF152" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG152" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17695,7 +18455,12 @@
           <t>V.I.Plyasunov,1976</t>
         </is>
       </c>
-      <c r="AF153" t="n">
+      <c r="AF153" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG153" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17805,7 +18570,12 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF154" t="n">
+      <c r="AF154" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG154" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17919,7 +18689,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF155" t="n">
+      <c r="AF155" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG155" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18029,7 +18804,12 @@
           <t>A.A.Dontsov,1946</t>
         </is>
       </c>
-      <c r="AF156" t="n">
+      <c r="AF156" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG156" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18139,7 +18919,12 @@
           <t>E.A.Makarov,1976</t>
         </is>
       </c>
-      <c r="AF157" t="n">
+      <c r="AF157" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG157" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18253,7 +19038,12 @@
           <t>I.M.Sargina,1960</t>
         </is>
       </c>
-      <c r="AF158" t="n">
+      <c r="AF158" t="inlineStr">
+        <is>
+          <t>quartz monzodiorite\quartz monzogabbro</t>
+        </is>
+      </c>
+      <c r="AG158" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18367,7 +19157,12 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF159" t="n">
+      <c r="AF159" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG159" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18481,7 +19276,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF160" t="n">
+      <c r="AF160" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG160" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18595,7 +19395,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF161" t="n">
+      <c r="AF161" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG161" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18709,7 +19514,12 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF162" t="n">
+      <c r="AF162" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG162" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18819,7 +19629,12 @@
           <t>G.A.Zhukov,1956</t>
         </is>
       </c>
-      <c r="AF163" t="n">
+      <c r="AF163" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG163" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18929,7 +19744,12 @@
           <t>L.V.Kuz'mina,1940</t>
         </is>
       </c>
-      <c r="AF164" t="n">
+      <c r="AF164" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG164" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19043,7 +19863,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF165" t="n">
+      <c r="AF165" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG165" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19153,7 +19978,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF166" t="n">
+      <c r="AF166" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="AG166" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19267,7 +20097,12 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF167" t="n">
+      <c r="AF167" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG167" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19373,7 +20208,12 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF168" t="n">
+      <c r="AF168" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG168" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19487,7 +20327,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF169" t="n">
+      <c r="AF169" t="inlineStr">
+        <is>
+          <t>quartz monzonite</t>
+        </is>
+      </c>
+      <c r="AG169" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19597,7 +20442,12 @@
           <t>G.A.Zhukov,1956</t>
         </is>
       </c>
-      <c r="AF170" t="n">
+      <c r="AF170" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG170" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19707,7 +20557,12 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF171" t="n">
+      <c r="AF171" t="inlineStr">
+        <is>
+          <t>monzo granite</t>
+        </is>
+      </c>
+      <c r="AG171" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19821,7 +20676,12 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF172" t="n">
+      <c r="AF172" t="inlineStr">
+        <is>
+          <t>quartz monzodiorite\quartz monzogabbro</t>
+        </is>
+      </c>
+      <c r="AG172" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19935,7 +20795,12 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF173" t="n">
+      <c r="AF173" t="inlineStr">
+        <is>
+          <t>quartz monzodiorite\quartz monzogabbro</t>
+        </is>
+      </c>
+      <c r="AG173" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20049,7 +20914,12 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF174" t="n">
+      <c r="AF174" t="inlineStr">
+        <is>
+          <t>monzonite</t>
+        </is>
+      </c>
+      <c r="AG174" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20159,7 +21029,12 @@
           <t>I.A.Peresypkin,1972</t>
         </is>
       </c>
-      <c r="AF175" t="n">
+      <c r="AF175" t="inlineStr">
+        <is>
+          <t>quartz monzodiorite\quartz monzogabbro</t>
+        </is>
+      </c>
+      <c r="AG175" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20265,7 +21140,12 @@
           <t>V.I.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF176" t="n">
+      <c r="AF176" t="inlineStr">
+        <is>
+          <t>quartz monzodiorite\quartz monzogabbro</t>
+        </is>
+      </c>
+      <c r="AG176" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20375,7 +21255,12 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF177" t="n">
+      <c r="AF177" t="inlineStr">
+        <is>
+          <t>quartz monzodiorite\quartz monzogabbro</t>
+        </is>
+      </c>
+      <c r="AG177" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20489,7 +21374,12 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF178" t="n">
+      <c r="AF178" t="inlineStr">
+        <is>
+          <t>monzonite</t>
+        </is>
+      </c>
+      <c r="AG178" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20603,7 +21493,12 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF179" t="n">
+      <c r="AF179" t="inlineStr">
+        <is>
+          <t>monzodiorite monzogabbro</t>
+        </is>
+      </c>
+      <c r="AG179" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20713,7 +21608,12 @@
           <t>V.M.Ol'khovik,1959</t>
         </is>
       </c>
-      <c r="AF180" t="n">
+      <c r="AF180" t="inlineStr">
+        <is>
+          <t>monzodiorite monzogabbro</t>
+        </is>
+      </c>
+      <c r="AG180" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Biplots: column higlighting points with zero values
only 736 datapoints have no zero values in any of the columns
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG180"/>
+  <dimension ref="A1:AH180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,11 @@
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
+          <t>zero</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
           <t>area</t>
         </is>
       </c>
@@ -643,7 +648,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH2" t="n">
         <v>5</v>
       </c>
     </row>
@@ -762,7 +772,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG3" t="n">
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -885,7 +900,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG4" t="n">
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1004,7 +1024,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG5" t="n">
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1123,7 +1148,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG6" t="n">
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH6" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1238,7 +1268,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG7" t="n">
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1357,7 +1392,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG8" t="n">
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1480,7 +1520,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG9" t="n">
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH9" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1603,7 +1648,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG10" t="n">
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH10" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1722,7 +1772,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG11" t="n">
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH11" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1837,7 +1892,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG12" t="n">
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH12" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1948,7 +2008,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG13" t="n">
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH13" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2067,7 +2132,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG14" t="n">
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TiO2  P2O5 </t>
+        </is>
+      </c>
+      <c r="AH14" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2182,7 +2252,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG15" t="n">
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH15" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2301,7 +2376,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG16" t="n">
+      <c r="AG16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH16" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2416,7 +2496,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG17" t="n">
+      <c r="AG17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH17" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2535,7 +2620,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG18" t="n">
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH18" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2646,7 +2736,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG19" t="n">
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH19" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2765,7 +2860,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG20" t="n">
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH20" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2880,7 +2980,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG21" t="n">
+      <c r="AG21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH21" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2991,7 +3096,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG22" t="n">
+      <c r="AG22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH22" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3102,7 +3212,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG23" t="n">
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH23" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3221,7 +3336,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG24" t="n">
+      <c r="AG24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH24" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3340,7 +3460,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG25" t="n">
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH25" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3455,7 +3580,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG26" t="n">
+      <c r="AG26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH26" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3574,7 +3704,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG27" t="n">
+      <c r="AG27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH27" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3693,7 +3828,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG28" t="n">
+      <c r="AG28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH28" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3808,7 +3948,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG29" t="n">
+      <c r="AG29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH29" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3919,7 +4064,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG30" t="n">
+      <c r="AG30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH30" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4038,7 +4188,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG31" t="n">
+      <c r="AG31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH31" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4157,7 +4312,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG32" t="n">
+      <c r="AG32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH32" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4272,7 +4432,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG33" t="n">
+      <c r="AG33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH33" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4391,7 +4556,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG34" t="n">
+      <c r="AG34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH34" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4506,7 +4676,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG35" t="n">
+      <c r="AG35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH35" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4629,7 +4804,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG36" t="n">
+      <c r="AG36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH36" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4744,7 +4924,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG37" t="n">
+      <c r="AG37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH37" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4863,7 +5048,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG38" t="n">
+      <c r="AG38" t="inlineStr">
+        <is>
+          <t>MnO TiO2  P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH38" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4986,7 +5176,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG39" t="n">
+      <c r="AG39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH39" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5109,7 +5304,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG40" t="n">
+      <c r="AG40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH40" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5228,7 +5428,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG41" t="n">
+      <c r="AG41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5351,7 +5556,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG42" t="n">
+      <c r="AG42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH42" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5470,7 +5680,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG43" t="n">
+      <c r="AG43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH43" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5593,7 +5808,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG44" t="n">
+      <c r="AG44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH44" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5716,7 +5936,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG45" t="n">
+      <c r="AG45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH45" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5831,7 +6056,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG46" t="n">
+      <c r="AG46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH46" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5954,7 +6184,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG47" t="n">
+      <c r="AG47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH47" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6073,7 +6308,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG48" t="n">
+      <c r="AG48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH48" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6192,7 +6432,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG49" t="n">
+      <c r="AG49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH49" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6307,7 +6552,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG50" t="n">
+      <c r="AG50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH50" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6426,7 +6676,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG51" t="n">
+      <c r="AG51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH51" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6541,7 +6796,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG52" t="n">
+      <c r="AG52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH52" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6660,7 +6920,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG53" t="n">
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH53" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6783,7 +7048,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG54" t="n">
+      <c r="AG54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH54" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6902,7 +7172,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG55" t="n">
+      <c r="AG55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH55" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7017,7 +7292,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG56" t="n">
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH56" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7132,7 +7412,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG57" t="n">
+      <c r="AG57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH57" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7247,7 +7532,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG58" t="n">
+      <c r="AG58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH58" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7366,7 +7656,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG59" t="n">
+      <c r="AG59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH59" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7481,7 +7776,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG60" t="n">
+      <c r="AG60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH60" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7596,7 +7896,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG61" t="n">
+      <c r="AG61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH61" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7715,7 +8020,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG62" t="n">
+      <c r="AG62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH62" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7834,7 +8144,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG63" t="n">
+      <c r="AG63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH63" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7957,7 +8272,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG64" t="n">
+      <c r="AG64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH64" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8076,7 +8396,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG65" t="n">
+      <c r="AG65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH65" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8195,7 +8520,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG66" t="n">
+      <c r="AG66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH66" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8314,7 +8644,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG67" t="n">
+      <c r="AG67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH67" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8433,7 +8768,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG68" t="n">
+      <c r="AG68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH68" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8552,7 +8892,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG69" t="n">
+      <c r="AG69" t="inlineStr">
+        <is>
+          <t>MnO   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH69" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8667,7 +9012,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG70" t="n">
+      <c r="AG70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH70" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8782,7 +9132,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG71" t="n">
+      <c r="AG71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH71" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8901,7 +9256,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG72" t="n">
+      <c r="AG72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH72" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9020,7 +9380,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG73" t="n">
+      <c r="AG73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH73" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9135,7 +9500,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG74" t="n">
+      <c r="AG74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH74" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9258,7 +9628,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG75" t="n">
+      <c r="AG75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH75" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9377,7 +9752,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG76" t="n">
+      <c r="AG76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH76" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9496,7 +9876,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG77" t="n">
+      <c r="AG77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH77" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9615,7 +10000,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG78" t="n">
+      <c r="AG78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> TiO2  P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH78" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9734,7 +10124,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG79" t="n">
+      <c r="AG79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH79" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9849,7 +10244,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG80" t="n">
+      <c r="AG80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH80" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9968,7 +10368,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG81" t="n">
+      <c r="AG81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH81" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10087,7 +10492,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG82" t="n">
+      <c r="AG82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH82" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10202,7 +10612,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG83" t="n">
+      <c r="AG83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH83" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10317,7 +10732,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG84" t="n">
+      <c r="AG84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH84" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10432,7 +10852,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG85" t="n">
+      <c r="AG85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH85" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10551,7 +10976,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG86" t="n">
+      <c r="AG86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH86" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10670,7 +11100,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG87" t="n">
+      <c r="AG87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH87" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10785,7 +11220,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG88" t="n">
+      <c r="AG88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH88" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10900,7 +11340,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG89" t="n">
+      <c r="AG89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH89" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11019,7 +11464,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG90" t="n">
+      <c r="AG90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH90" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11142,7 +11592,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG91" t="n">
+      <c r="AG91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH91" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11261,7 +11716,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG92" t="n">
+      <c r="AG92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH92" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11376,7 +11836,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG93" t="n">
+      <c r="AG93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH93" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11491,7 +11956,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG94" t="n">
+      <c r="AG94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH94" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11606,7 +12076,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG95" t="n">
+      <c r="AG95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH95" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11721,7 +12196,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG96" t="n">
+      <c r="AG96" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH96" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11844,7 +12324,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG97" t="n">
+      <c r="AG97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH97" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11963,7 +12448,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG98" t="n">
+      <c r="AG98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH98" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12082,7 +12572,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG99" t="n">
+      <c r="AG99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH99" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12197,7 +12692,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG100" t="n">
+      <c r="AG100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH100" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12316,7 +12816,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG101" t="n">
+      <c r="AG101" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH101" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12435,7 +12940,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG102" t="n">
+      <c r="AG102" t="inlineStr">
+        <is>
+          <t>MnO    oth</t>
+        </is>
+      </c>
+      <c r="AH102" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12558,7 +13068,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG103" t="n">
+      <c r="AG103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH103" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12677,7 +13192,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG104" t="n">
+      <c r="AG104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH104" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12796,7 +13316,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG105" t="n">
+      <c r="AG105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH105" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12915,7 +13440,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG106" t="n">
+      <c r="AG106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH106" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13034,7 +13564,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG107" t="n">
+      <c r="AG107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH107" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13153,7 +13688,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG108" t="n">
+      <c r="AG108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH108" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13272,7 +13812,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG109" t="n">
+      <c r="AG109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH109" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13395,7 +13940,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG110" t="n">
+      <c r="AG110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH110" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13510,7 +14060,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG111" t="n">
+      <c r="AG111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH111" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13625,7 +14180,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG112" t="n">
+      <c r="AG112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH112" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13748,7 +14308,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG113" t="n">
+      <c r="AG113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH113" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13871,7 +14436,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG114" t="n">
+      <c r="AG114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH114" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13982,7 +14552,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG115" t="n">
+      <c r="AG115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH115" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14097,7 +14672,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG116" t="n">
+      <c r="AG116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH116" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14220,7 +14800,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG117" t="n">
+      <c r="AG117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH117" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14335,7 +14920,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG118" t="n">
+      <c r="AG118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH118" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14446,7 +15036,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG119" t="n">
+      <c r="AG119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH119" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14561,7 +15156,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG120" t="n">
+      <c r="AG120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH120" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14680,7 +15280,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG121" t="n">
+      <c r="AG121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH121" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14803,7 +15408,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG122" t="n">
+      <c r="AG122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH122" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14926,7 +15536,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG123" t="n">
+      <c r="AG123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH123" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15037,7 +15652,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG124" t="n">
+      <c r="AG124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH124" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15152,7 +15772,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG125" t="n">
+      <c r="AG125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH125" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15271,7 +15896,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG126" t="n">
+      <c r="AG126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH126" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15394,7 +16024,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG127" t="n">
+      <c r="AG127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH127" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15509,7 +16144,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG128" t="n">
+      <c r="AG128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH128" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15628,7 +16268,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG129" t="n">
+      <c r="AG129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH129" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15747,7 +16392,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG130" t="n">
+      <c r="AG130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH130" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15866,7 +16516,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG131" t="n">
+      <c r="AG131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH131" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15985,7 +16640,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG132" t="n">
+      <c r="AG132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH132" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16100,7 +16760,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG133" t="n">
+      <c r="AG133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH133" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16223,7 +16888,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG134" t="n">
+      <c r="AG134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH134" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16342,7 +17012,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG135" t="n">
+      <c r="AG135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH135" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16461,7 +17136,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG136" t="n">
+      <c r="AG136" t="inlineStr">
+        <is>
+          <t>MnO    oth</t>
+        </is>
+      </c>
+      <c r="AH136" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16580,7 +17260,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG137" t="n">
+      <c r="AG137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH137" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16695,7 +17380,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG138" t="n">
+      <c r="AG138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH138" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16814,7 +17504,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG139" t="n">
+      <c r="AG139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH139" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16929,7 +17624,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG140" t="n">
+      <c r="AG140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH140" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17052,7 +17752,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG141" t="n">
+      <c r="AG141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH141" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17167,7 +17872,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG142" t="n">
+      <c r="AG142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH142" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17290,7 +18000,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG143" t="n">
+      <c r="AG143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH143" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17409,7 +18124,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG144" t="n">
+      <c r="AG144" t="inlineStr">
+        <is>
+          <t>MnO   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH144" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17524,7 +18244,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG145" t="n">
+      <c r="AG145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH145" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17647,7 +18372,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG146" t="n">
+      <c r="AG146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH146" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17762,7 +18492,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG147" t="n">
+      <c r="AG147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH147" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17881,7 +18616,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG148" t="n">
+      <c r="AG148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH148" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17996,7 +18736,12 @@
           <t>quartz monzodiorite\quartz monzogabbro</t>
         </is>
       </c>
-      <c r="AG149" t="n">
+      <c r="AG149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH149" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18111,7 +18856,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG150" t="n">
+      <c r="AG150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH150" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18230,7 +18980,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG151" t="n">
+      <c r="AG151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH151" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18341,7 +19096,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG152" t="n">
+      <c r="AG152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH152" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18460,7 +19220,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG153" t="n">
+      <c r="AG153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH153" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18575,7 +19340,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG154" t="n">
+      <c r="AG154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH154" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18694,7 +19464,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG155" t="n">
+      <c r="AG155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH155" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18809,7 +19584,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG156" t="n">
+      <c r="AG156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH156" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18924,7 +19704,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG157" t="n">
+      <c r="AG157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH157" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19043,7 +19828,12 @@
           <t>quartz monzodiorite\quartz monzogabbro</t>
         </is>
       </c>
-      <c r="AG158" t="n">
+      <c r="AG158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH158" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19162,7 +19952,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG159" t="n">
+      <c r="AG159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH159" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19281,7 +20076,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG160" t="n">
+      <c r="AG160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH160" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19400,7 +20200,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG161" t="n">
+      <c r="AG161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH161" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19519,7 +20324,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG162" t="n">
+      <c r="AG162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH162" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19634,7 +20444,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG163" t="n">
+      <c r="AG163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH163" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19749,7 +20564,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG164" t="n">
+      <c r="AG164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH164" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19868,7 +20688,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG165" t="n">
+      <c r="AG165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH165" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19983,7 +20808,12 @@
           <t>granodiorite</t>
         </is>
       </c>
-      <c r="AG166" t="n">
+      <c r="AG166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH166" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20102,7 +20932,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG167" t="n">
+      <c r="AG167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH167" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20213,7 +21048,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG168" t="n">
+      <c r="AG168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MnO    </t>
+        </is>
+      </c>
+      <c r="AH168" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20332,7 +21172,12 @@
           <t>quartz monzonite</t>
         </is>
       </c>
-      <c r="AG169" t="n">
+      <c r="AG169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH169" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20447,7 +21292,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG170" t="n">
+      <c r="AG170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH170" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20562,7 +21412,12 @@
           <t>monzo granite</t>
         </is>
       </c>
-      <c r="AG171" t="n">
+      <c r="AG171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH171" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20681,7 +21536,12 @@
           <t>quartz monzodiorite\quartz monzogabbro</t>
         </is>
       </c>
-      <c r="AG172" t="n">
+      <c r="AG172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 </t>
+        </is>
+      </c>
+      <c r="AH172" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20800,7 +21660,12 @@
           <t>quartz monzodiorite\quartz monzogabbro</t>
         </is>
       </c>
-      <c r="AG173" t="n">
+      <c r="AG173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH173" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20919,7 +21784,12 @@
           <t>monzonite</t>
         </is>
       </c>
-      <c r="AG174" t="n">
+      <c r="AG174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    </t>
+        </is>
+      </c>
+      <c r="AH174" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21034,7 +21904,12 @@
           <t>quartz monzodiorite\quartz monzogabbro</t>
         </is>
       </c>
-      <c r="AG175" t="n">
+      <c r="AG175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH175" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21145,7 +22020,12 @@
           <t>quartz monzodiorite\quartz monzogabbro</t>
         </is>
       </c>
-      <c r="AG176" t="n">
+      <c r="AG176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH176" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21260,7 +22140,12 @@
           <t>quartz monzodiorite\quartz monzogabbro</t>
         </is>
       </c>
-      <c r="AG177" t="n">
+      <c r="AG177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH177" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21379,7 +22264,12 @@
           <t>monzonite</t>
         </is>
       </c>
-      <c r="AG178" t="n">
+      <c r="AG178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH178" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21498,7 +22388,12 @@
           <t>monzodiorite monzogabbro</t>
         </is>
       </c>
-      <c r="AG179" t="n">
+      <c r="AG179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    oth</t>
+        </is>
+      </c>
+      <c r="AH179" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21613,7 +22508,12 @@
           <t>monzodiorite monzogabbro</t>
         </is>
       </c>
-      <c r="AG180" t="n">
+      <c r="AG180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   P2O5 oth</t>
+        </is>
+      </c>
+      <c r="AH180" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finetuning PC's for interpolation
adjusted the amount of PC's used in step 1.8. amount of PC's used found in error budget excel when MSPE gain was higher as 0.01
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH180"/>
+  <dimension ref="A1:AF180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,16 +519,6 @@
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>QAPF</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>zero</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
           <t>area</t>
         </is>
       </c>
@@ -643,17 +633,7 @@
           <t>A.I.Kyshtymov,1959</t>
         </is>
       </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH2" t="n">
+      <c r="AF2" t="n">
         <v>5</v>
       </c>
     </row>
@@ -767,17 +747,7 @@
           <t>E.K.Boborykin,1955</t>
         </is>
       </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH3" t="n">
+      <c r="AF3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -895,17 +865,7 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH4" t="n">
+      <c r="AF4" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1019,17 +979,7 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH5" t="n">
+      <c r="AF5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1143,17 +1093,7 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH6" t="n">
+      <c r="AF6" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1263,17 +1203,7 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH7" t="n">
+      <c r="AF7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1387,17 +1317,7 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH8" t="n">
+      <c r="AF8" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1515,17 +1435,7 @@
           <t>V.K.Sadakov,1966</t>
         </is>
       </c>
-      <c r="AF9" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG9" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH9" t="n">
+      <c r="AF9" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1643,17 +1553,7 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF10" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG10" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH10" t="n">
+      <c r="AF10" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1767,17 +1667,7 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF11" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG11" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH11" t="n">
+      <c r="AF11" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1887,17 +1777,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF12" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG12" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH12" t="n">
+      <c r="AF12" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2003,17 +1883,7 @@
           <t>I.M.Sargina,1959</t>
         </is>
       </c>
-      <c r="AF13" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG13" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH13" t="n">
+      <c r="AF13" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2127,17 +1997,7 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF14" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG14" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH14" t="n">
+      <c r="AF14" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2247,17 +2107,7 @@
           <t>I.A.Sklyar,1938</t>
         </is>
       </c>
-      <c r="AF15" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG15" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH15" t="n">
+      <c r="AF15" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2371,17 +2221,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF16" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG16" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH16" t="n">
+      <c r="AF16" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2491,17 +2331,7 @@
           <t>I.M.Sargina,1959</t>
         </is>
       </c>
-      <c r="AF17" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG17" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH17" t="n">
+      <c r="AF17" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2615,17 +2445,7 @@
           <t>E.K.Boborykin,1955</t>
         </is>
       </c>
-      <c r="AF18" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG18" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH18" t="n">
+      <c r="AF18" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2731,17 +2551,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF19" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG19" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH19" t="n">
+      <c r="AF19" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2855,17 +2665,7 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF20" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG20" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH20" t="n">
+      <c r="AF20" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2975,17 +2775,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF21" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG21" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH21" t="n">
+      <c r="AF21" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3091,17 +2881,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF22" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG22" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH22" t="n">
+      <c r="AF22" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3207,17 +2987,7 @@
           <t>E.G.Bordyugov,1966</t>
         </is>
       </c>
-      <c r="AF23" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG23" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH23" t="n">
+      <c r="AF23" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3331,17 +3101,7 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF24" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG24" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH24" t="n">
+      <c r="AF24" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3455,17 +3215,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF25" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG25" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH25" t="n">
+      <c r="AF25" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3575,17 +3325,7 @@
           <t>I.A.Nikitin,1959</t>
         </is>
       </c>
-      <c r="AF26" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG26" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH26" t="n">
+      <c r="AF26" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3699,17 +3439,7 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF27" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG27" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH27" t="n">
+      <c r="AF27" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3823,17 +3553,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF28" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG28" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH28" t="n">
+      <c r="AF28" t="n">
         <v>5</v>
       </c>
     </row>
@@ -3943,17 +3663,7 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF29" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG29" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH29" t="n">
+      <c r="AF29" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4059,17 +3769,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF30" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG30" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH30" t="n">
+      <c r="AF30" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4183,17 +3883,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF31" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG31" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH31" t="n">
+      <c r="AF31" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4307,17 +3997,7 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF32" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG32" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH32" t="n">
+      <c r="AF32" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4427,17 +4107,7 @@
           <t>E.K.Boborykin,1955</t>
         </is>
       </c>
-      <c r="AF33" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG33" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH33" t="n">
+      <c r="AF33" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4551,17 +4221,7 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF34" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG34" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH34" t="n">
+      <c r="AF34" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4671,17 +4331,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF35" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG35" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH35" t="n">
+      <c r="AF35" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4799,17 +4449,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF36" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG36" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH36" t="n">
+      <c r="AF36" t="n">
         <v>5</v>
       </c>
     </row>
@@ -4919,17 +4559,7 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF37" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG37" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH37" t="n">
+      <c r="AF37" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5043,17 +4673,7 @@
           <t>l.D.Gatiev,1938</t>
         </is>
       </c>
-      <c r="AF38" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG38" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH38" t="n">
+      <c r="AF38" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5171,17 +4791,7 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF39" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG39" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH39" t="n">
+      <c r="AF39" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5299,17 +4909,7 @@
           <t>P.P.Kolesnichenko,1964</t>
         </is>
       </c>
-      <c r="AF40" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG40" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH40" t="n">
+      <c r="AF40" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5423,17 +5023,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF41" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG41" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH41" t="n">
+      <c r="AF41" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5551,17 +5141,7 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF42" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG42" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH42" t="n">
+      <c r="AF42" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5675,17 +5255,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF43" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG43" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH43" t="n">
+      <c r="AF43" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5803,17 +5373,7 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF44" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG44" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH44" t="n">
+      <c r="AF44" t="n">
         <v>5</v>
       </c>
     </row>
@@ -5931,17 +5491,7 @@
           <t>E.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF45" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG45" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH45" t="n">
+      <c r="AF45" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6051,17 +5601,7 @@
           <t>A.I.Kyshtymov,1962</t>
         </is>
       </c>
-      <c r="AF46" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG46" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH46" t="n">
+      <c r="AF46" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6179,17 +5719,7 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF47" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG47" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH47" t="n">
+      <c r="AF47" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6303,17 +5833,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF48" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG48" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH48" t="n">
+      <c r="AF48" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6427,17 +5947,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF49" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG49" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH49" t="n">
+      <c r="AF49" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6547,17 +6057,7 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF50" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG50" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH50" t="n">
+      <c r="AF50" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6671,17 +6171,7 @@
           <t>I.M.Sargina,1960</t>
         </is>
       </c>
-      <c r="AF51" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG51" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH51" t="n">
+      <c r="AF51" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6791,17 +6281,7 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF52" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG52" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH52" t="n">
+      <c r="AF52" t="n">
         <v>5</v>
       </c>
     </row>
@@ -6915,17 +6395,7 @@
           <t>V.M.Ol'khovik,1959</t>
         </is>
       </c>
-      <c r="AF53" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG53" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH53" t="n">
+      <c r="AF53" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7043,17 +6513,7 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF54" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG54" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH54" t="n">
+      <c r="AF54" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7167,17 +6627,7 @@
           <t>Yu.A.Odinetz,1937</t>
         </is>
       </c>
-      <c r="AF55" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG55" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH55" t="n">
+      <c r="AF55" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7287,17 +6737,7 @@
           <t>I.M.Sargina,1958</t>
         </is>
       </c>
-      <c r="AF56" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG56" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH56" t="n">
+      <c r="AF56" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7407,17 +6847,7 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF57" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG57" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH57" t="n">
+      <c r="AF57" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7527,17 +6957,7 @@
           <t>V.I.Plyasunov,1976</t>
         </is>
       </c>
-      <c r="AF58" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG58" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH58" t="n">
+      <c r="AF58" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7651,17 +7071,7 @@
           <t>I.D.Gatiev,1938</t>
         </is>
       </c>
-      <c r="AF59" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG59" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH59" t="n">
+      <c r="AF59" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7771,17 +7181,7 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF60" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG60" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH60" t="n">
+      <c r="AF60" t="n">
         <v>5</v>
       </c>
     </row>
@@ -7891,17 +7291,7 @@
           <t>E.K.Boborykin,1965</t>
         </is>
       </c>
-      <c r="AF61" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG61" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH61" t="n">
+      <c r="AF61" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8015,17 +7405,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF62" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG62" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH62" t="n">
+      <c r="AF62" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8139,17 +7519,7 @@
           <t>I.A.Sklyar,1938</t>
         </is>
       </c>
-      <c r="AF63" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG63" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH63" t="n">
+      <c r="AF63" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8267,17 +7637,7 @@
           <t>G.A.Zhukov,1954</t>
         </is>
       </c>
-      <c r="AF64" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG64" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH64" t="n">
+      <c r="AF64" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8391,17 +7751,7 @@
           <t>A.I.Kyshtymov,1962</t>
         </is>
       </c>
-      <c r="AF65" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG65" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH65" t="n">
+      <c r="AF65" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8515,17 +7865,7 @@
           <t>I.M.Sargina,1956</t>
         </is>
       </c>
-      <c r="AF66" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG66" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH66" t="n">
+      <c r="AF66" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8639,17 +7979,7 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF67" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG67" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH67" t="n">
+      <c r="AF67" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8763,17 +8093,7 @@
           <t>I.D.Gatiev,1938</t>
         </is>
       </c>
-      <c r="AF68" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG68" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH68" t="n">
+      <c r="AF68" t="n">
         <v>5</v>
       </c>
     </row>
@@ -8887,17 +8207,7 @@
           <t>I.M.Sargina,1956</t>
         </is>
       </c>
-      <c r="AF69" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG69" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH69" t="n">
+      <c r="AF69" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9007,17 +8317,7 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF70" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG70" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH70" t="n">
+      <c r="AF70" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9127,17 +8427,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF71" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG71" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH71" t="n">
+      <c r="AF71" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9251,17 +8541,7 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF72" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG72" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH72" t="n">
+      <c r="AF72" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9375,17 +8655,7 @@
           <t>V.N.Stavitsky,1958</t>
         </is>
       </c>
-      <c r="AF73" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG73" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH73" t="n">
+      <c r="AF73" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9495,17 +8765,7 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF74" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG74" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH74" t="n">
+      <c r="AF74" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9623,17 +8883,7 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF75" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG75" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH75" t="n">
+      <c r="AF75" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9747,17 +8997,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF76" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG76" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH76" t="n">
+      <c r="AF76" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9871,17 +9111,7 @@
           <t>V.P.Azhina,1960</t>
         </is>
       </c>
-      <c r="AF77" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG77" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH77" t="n">
+      <c r="AF77" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9995,17 +9225,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF78" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG78" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH78" t="n">
+      <c r="AF78" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10119,17 +9339,7 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
-      <c r="AF79" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG79" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH79" t="n">
+      <c r="AF79" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10239,17 +9449,7 @@
           <t>V.I.Plyasunov,1976</t>
         </is>
       </c>
-      <c r="AF80" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG80" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH80" t="n">
+      <c r="AF80" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10363,17 +9563,7 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF81" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG81" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH81" t="n">
+      <c r="AF81" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10487,17 +9677,7 @@
           <t>S.V.Blagodatsky,1964</t>
         </is>
       </c>
-      <c r="AF82" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG82" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH82" t="n">
+      <c r="AF82" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10607,17 +9787,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF83" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG83" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH83" t="n">
+      <c r="AF83" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10727,17 +9897,7 @@
           <t>I.M.Sargina,1960</t>
         </is>
       </c>
-      <c r="AF84" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG84" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH84" t="n">
+      <c r="AF84" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10847,17 +10007,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF85" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG85" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH85" t="n">
+      <c r="AF85" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10971,17 +10121,7 @@
           <t>S.V.Blagodatsky,1964</t>
         </is>
       </c>
-      <c r="AF86" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG86" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH86" t="n">
+      <c r="AF86" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11095,17 +10235,7 @@
           <t>l.A.Sklyar,1938</t>
         </is>
       </c>
-      <c r="AF87" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG87" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH87" t="n">
+      <c r="AF87" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11215,17 +10345,7 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF88" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG88" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH88" t="n">
+      <c r="AF88" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11335,17 +10455,7 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF89" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG89" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH89" t="n">
+      <c r="AF89" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11459,17 +10569,7 @@
           <t>A.l.Kyshtymov,1962</t>
         </is>
       </c>
-      <c r="AF90" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG90" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH90" t="n">
+      <c r="AF90" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11587,17 +10687,7 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
-      <c r="AF91" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG91" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH91" t="n">
+      <c r="AF91" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11711,17 +10801,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF92" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG92" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH92" t="n">
+      <c r="AF92" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11831,17 +10911,7 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF93" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG93" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH93" t="n">
+      <c r="AF93" t="n">
         <v>5</v>
       </c>
     </row>
@@ -11951,17 +11021,7 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF94" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG94" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH94" t="n">
+      <c r="AF94" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12071,17 +11131,7 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF95" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG95" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH95" t="n">
+      <c r="AF95" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12191,17 +11241,7 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF96" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG96" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH96" t="n">
+      <c r="AF96" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12319,17 +11359,7 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF97" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG97" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH97" t="n">
+      <c r="AF97" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12443,17 +11473,7 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF98" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG98" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH98" t="n">
+      <c r="AF98" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12567,17 +11587,7 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF99" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG99" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH99" t="n">
+      <c r="AF99" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12687,17 +11697,7 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF100" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG100" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH100" t="n">
+      <c r="AF100" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12811,17 +11811,7 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF101" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG101" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH101" t="n">
+      <c r="AF101" t="n">
         <v>5</v>
       </c>
     </row>
@@ -12935,17 +11925,7 @@
           <t>Yu.A.Odinetz,1937</t>
         </is>
       </c>
-      <c r="AF102" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG102" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH102" t="n">
+      <c r="AF102" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13063,17 +12043,7 @@
           <t>A.I.Kyshtymov,1962</t>
         </is>
       </c>
-      <c r="AF103" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG103" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH103" t="n">
+      <c r="AF103" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13187,17 +12157,7 @@
           <t>G.V.Andreev,1955</t>
         </is>
       </c>
-      <c r="AF104" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG104" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH104" t="n">
+      <c r="AF104" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13311,17 +12271,7 @@
           <t>A.E.Fishkin,1967</t>
         </is>
       </c>
-      <c r="AF105" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG105" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH105" t="n">
+      <c r="AF105" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13435,17 +12385,7 @@
           <t>E.K.Boborykin,1956</t>
         </is>
       </c>
-      <c r="AF106" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG106" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH106" t="n">
+      <c r="AF106" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13559,17 +12499,7 @@
           <t>l.A.Nikitin,1959</t>
         </is>
       </c>
-      <c r="AF107" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG107" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH107" t="n">
+      <c r="AF107" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13683,17 +12613,7 @@
           <t>E.G.Bordyugov,1964</t>
         </is>
       </c>
-      <c r="AF108" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG108" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH108" t="n">
+      <c r="AF108" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13807,17 +12727,7 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF109" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG109" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH109" t="n">
+      <c r="AF109" t="n">
         <v>5</v>
       </c>
     </row>
@@ -13935,17 +12845,7 @@
           <t>K.S.Sukhov,1962</t>
         </is>
       </c>
-      <c r="AF110" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG110" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH110" t="n">
+      <c r="AF110" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14055,17 +12955,7 @@
           <t>S.E.Sinitsky,1957</t>
         </is>
       </c>
-      <c r="AF111" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG111" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH111" t="n">
+      <c r="AF111" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14175,17 +13065,7 @@
           <t>G.I.Kremchukov,1936</t>
         </is>
       </c>
-      <c r="AF112" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG112" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH112" t="n">
+      <c r="AF112" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14303,17 +13183,7 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF113" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG113" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH113" t="n">
+      <c r="AF113" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14431,17 +13301,7 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF114" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG114" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH114" t="n">
+      <c r="AF114" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14547,17 +13407,7 @@
           <t>E.K.Boborykin,1956</t>
         </is>
       </c>
-      <c r="AF115" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG115" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH115" t="n">
+      <c r="AF115" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14667,17 +13517,7 @@
           <t>I.A.Nikitin,1957</t>
         </is>
       </c>
-      <c r="AF116" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG116" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH116" t="n">
+      <c r="AF116" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14795,17 +13635,7 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF117" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG117" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH117" t="n">
+      <c r="AF117" t="n">
         <v>5</v>
       </c>
     </row>
@@ -14915,17 +13745,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF118" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG118" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH118" t="n">
+      <c r="AF118" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15031,17 +13851,7 @@
           <t>G.I.Bogomolov,1967</t>
         </is>
       </c>
-      <c r="AF119" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG119" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH119" t="n">
+      <c r="AF119" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15151,17 +13961,7 @@
           <t>A.l.Kyshtymov,1959</t>
         </is>
       </c>
-      <c r="AF120" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG120" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH120" t="n">
+      <c r="AF120" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15275,17 +14075,7 @@
           <t>S.F.Lugov,1953</t>
         </is>
       </c>
-      <c r="AF121" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG121" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH121" t="n">
+      <c r="AF121" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15403,17 +14193,7 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF122" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG122" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH122" t="n">
+      <c r="AF122" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15531,17 +14311,7 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF123" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG123" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH123" t="n">
+      <c r="AF123" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15647,17 +14417,7 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF124" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG124" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH124" t="n">
+      <c r="AF124" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15767,17 +14527,7 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF125" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG125" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH125" t="n">
+      <c r="AF125" t="n">
         <v>5</v>
       </c>
     </row>
@@ -15891,17 +14641,7 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF126" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG126" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH126" t="n">
+      <c r="AF126" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16019,17 +14759,7 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF127" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG127" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH127" t="n">
+      <c r="AF127" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16139,17 +14869,7 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF128" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG128" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH128" t="n">
+      <c r="AF128" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16263,17 +14983,7 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF129" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG129" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH129" t="n">
+      <c r="AF129" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16387,17 +15097,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF130" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG130" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH130" t="n">
+      <c r="AF130" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16511,17 +15211,7 @@
           <t>E.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF131" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG131" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH131" t="n">
+      <c r="AF131" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16635,17 +15325,7 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF132" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG132" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH132" t="n">
+      <c r="AF132" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16755,17 +15435,7 @@
           <t>V.I.Tutubalin,1967</t>
         </is>
       </c>
-      <c r="AF133" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG133" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH133" t="n">
+      <c r="AF133" t="n">
         <v>5</v>
       </c>
     </row>
@@ -16883,17 +15553,7 @@
           <t>G.P.Kozlov,1964</t>
         </is>
       </c>
-      <c r="AF134" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG134" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH134" t="n">
+      <c r="AF134" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17007,17 +15667,7 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF135" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG135" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH135" t="n">
+      <c r="AF135" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17131,17 +15781,7 @@
           <t>Yu.A.Odinetz,1937</t>
         </is>
       </c>
-      <c r="AF136" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG136" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH136" t="n">
+      <c r="AF136" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17255,17 +15895,7 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF137" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG137" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH137" t="n">
+      <c r="AF137" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17375,17 +16005,7 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF138" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG138" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH138" t="n">
+      <c r="AF138" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17499,17 +16119,7 @@
           <t>A.M.Timofeev,1956</t>
         </is>
       </c>
-      <c r="AF139" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG139" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH139" t="n">
+      <c r="AF139" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17619,17 +16229,7 @@
           <t>A.D.Sokolov,1961</t>
         </is>
       </c>
-      <c r="AF140" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG140" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH140" t="n">
+      <c r="AF140" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17747,17 +16347,7 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF141" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG141" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH141" t="n">
+      <c r="AF141" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17867,17 +16457,7 @@
           <t>G.A.Zhukov,1956</t>
         </is>
       </c>
-      <c r="AF142" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG142" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH142" t="n">
+      <c r="AF142" t="n">
         <v>5</v>
       </c>
     </row>
@@ -17995,17 +16575,7 @@
           <t>E.A.Makarov,1975</t>
         </is>
       </c>
-      <c r="AF143" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG143" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH143" t="n">
+      <c r="AF143" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18119,17 +16689,7 @@
           <t>M.I.Rabkin,1941</t>
         </is>
       </c>
-      <c r="AF144" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG144" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH144" t="n">
+      <c r="AF144" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18239,17 +16799,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF145" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG145" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH145" t="n">
+      <c r="AF145" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18367,17 +16917,7 @@
           <t>K.S.Sukhov,1963</t>
         </is>
       </c>
-      <c r="AF146" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG146" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH146" t="n">
+      <c r="AF146" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18487,17 +17027,7 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF147" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG147" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH147" t="n">
+      <c r="AF147" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18611,17 +17141,7 @@
           <t>F.A.Golovachev,1935</t>
         </is>
       </c>
-      <c r="AF148" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG148" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH148" t="n">
+      <c r="AF148" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18731,17 +17251,7 @@
           <t>G.I.Bogomolov,1967</t>
         </is>
       </c>
-      <c r="AF149" t="inlineStr">
-        <is>
-          <t>quartz monzodiorite\quartz monzogabbro</t>
-        </is>
-      </c>
-      <c r="AG149" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH149" t="n">
+      <c r="AF149" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18851,17 +17361,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF150" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG150" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH150" t="n">
+      <c r="AF150" t="n">
         <v>5</v>
       </c>
     </row>
@@ -18975,17 +17475,7 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF151" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG151" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH151" t="n">
+      <c r="AF151" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19091,17 +17581,7 @@
           <t>E.K.Boborykin,1955</t>
         </is>
       </c>
-      <c r="AF152" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG152" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH152" t="n">
+      <c r="AF152" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19215,17 +17695,7 @@
           <t>V.I.Plyasunov,1976</t>
         </is>
       </c>
-      <c r="AF153" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG153" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH153" t="n">
+      <c r="AF153" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19335,17 +17805,7 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF154" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG154" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH154" t="n">
+      <c r="AF154" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19459,17 +17919,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF155" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG155" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH155" t="n">
+      <c r="AF155" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19579,17 +18029,7 @@
           <t>A.A.Dontsov,1946</t>
         </is>
       </c>
-      <c r="AF156" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG156" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH156" t="n">
+      <c r="AF156" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19699,17 +18139,7 @@
           <t>E.A.Makarov,1976</t>
         </is>
       </c>
-      <c r="AF157" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG157" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH157" t="n">
+      <c r="AF157" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19823,17 +18253,7 @@
           <t>I.M.Sargina,1960</t>
         </is>
       </c>
-      <c r="AF158" t="inlineStr">
-        <is>
-          <t>quartz monzodiorite\quartz monzogabbro</t>
-        </is>
-      </c>
-      <c r="AG158" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH158" t="n">
+      <c r="AF158" t="n">
         <v>5</v>
       </c>
     </row>
@@ -19947,17 +18367,7 @@
           <t>Z.G.Karaeva,1967</t>
         </is>
       </c>
-      <c r="AF159" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG159" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH159" t="n">
+      <c r="AF159" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20071,17 +18481,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF160" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG160" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH160" t="n">
+      <c r="AF160" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20195,17 +18595,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF161" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG161" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH161" t="n">
+      <c r="AF161" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20319,17 +18709,7 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF162" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG162" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH162" t="n">
+      <c r="AF162" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20439,17 +18819,7 @@
           <t>G.A.Zhukov,1956</t>
         </is>
       </c>
-      <c r="AF163" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG163" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH163" t="n">
+      <c r="AF163" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20559,17 +18929,7 @@
           <t>L.V.Kuz'mina,1940</t>
         </is>
       </c>
-      <c r="AF164" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG164" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH164" t="n">
+      <c r="AF164" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20683,17 +19043,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF165" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG165" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH165" t="n">
+      <c r="AF165" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20803,17 +19153,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF166" t="inlineStr">
-        <is>
-          <t>granodiorite</t>
-        </is>
-      </c>
-      <c r="AG166" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH166" t="n">
+      <c r="AF166" t="n">
         <v>5</v>
       </c>
     </row>
@@ -20927,17 +19267,7 @@
           <t>A.P.Milov,1964</t>
         </is>
       </c>
-      <c r="AF167" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG167" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH167" t="n">
+      <c r="AF167" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21043,17 +19373,7 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF168" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG168" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH168" t="n">
+      <c r="AF168" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21167,17 +19487,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF169" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="AG169" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH169" t="n">
+      <c r="AF169" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21287,17 +19597,7 @@
           <t>G.A.Zhukov,1956</t>
         </is>
       </c>
-      <c r="AF170" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG170" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH170" t="n">
+      <c r="AF170" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21407,17 +19707,7 @@
           <t>S.E.Sinitsky,1953</t>
         </is>
       </c>
-      <c r="AF171" t="inlineStr">
-        <is>
-          <t>monzo granite</t>
-        </is>
-      </c>
-      <c r="AG171" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH171" t="n">
+      <c r="AF171" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21531,17 +19821,7 @@
           <t>V.N.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF172" t="inlineStr">
-        <is>
-          <t>quartz monzodiorite\quartz monzogabbro</t>
-        </is>
-      </c>
-      <c r="AG172" t="inlineStr">
-        <is>
-          <t>mineral</t>
-        </is>
-      </c>
-      <c r="AH172" t="n">
+      <c r="AF172" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21655,17 +19935,7 @@
           <t>A.V.Andrianov,1939</t>
         </is>
       </c>
-      <c r="AF173" t="inlineStr">
-        <is>
-          <t>quartz monzodiorite\quartz monzogabbro</t>
-        </is>
-      </c>
-      <c r="AG173" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH173" t="n">
+      <c r="AF173" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21779,17 +20049,7 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF174" t="inlineStr">
-        <is>
-          <t>monzonite</t>
-        </is>
-      </c>
-      <c r="AG174" t="inlineStr">
-        <is>
-          <t>no_zero</t>
-        </is>
-      </c>
-      <c r="AH174" t="n">
+      <c r="AF174" t="n">
         <v>5</v>
       </c>
     </row>
@@ -21899,17 +20159,7 @@
           <t>I.A.Peresypkin,1972</t>
         </is>
       </c>
-      <c r="AF175" t="inlineStr">
-        <is>
-          <t>quartz monzodiorite\quartz monzogabbro</t>
-        </is>
-      </c>
-      <c r="AG175" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH175" t="n">
+      <c r="AF175" t="n">
         <v>5</v>
       </c>
     </row>
@@ -22015,17 +20265,7 @@
           <t>V.I.Stavitsky,1959</t>
         </is>
       </c>
-      <c r="AF176" t="inlineStr">
-        <is>
-          <t>quartz monzodiorite\quartz monzogabbro</t>
-        </is>
-      </c>
-      <c r="AG176" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH176" t="n">
+      <c r="AF176" t="n">
         <v>5</v>
       </c>
     </row>
@@ -22135,17 +20375,7 @@
           <t>S.P.Stoyalov,1961</t>
         </is>
       </c>
-      <c r="AF177" t="inlineStr">
-        <is>
-          <t>quartz monzodiorite\quartz monzogabbro</t>
-        </is>
-      </c>
-      <c r="AG177" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH177" t="n">
+      <c r="AF177" t="n">
         <v>5</v>
       </c>
     </row>
@@ -22259,17 +20489,7 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF178" t="inlineStr">
-        <is>
-          <t>monzonite</t>
-        </is>
-      </c>
-      <c r="AG178" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH178" t="n">
+      <c r="AF178" t="n">
         <v>5</v>
       </c>
     </row>
@@ -22383,17 +20603,7 @@
           <t>V.K.Sadakov,1963</t>
         </is>
       </c>
-      <c r="AF179" t="inlineStr">
-        <is>
-          <t>monzodiorite monzogabbro</t>
-        </is>
-      </c>
-      <c r="AG179" t="inlineStr">
-        <is>
-          <t>oth</t>
-        </is>
-      </c>
-      <c r="AH179" t="n">
+      <c r="AF179" t="n">
         <v>5</v>
       </c>
     </row>
@@ -22503,17 +20713,7 @@
           <t>V.M.Ol'khovik,1959</t>
         </is>
       </c>
-      <c r="AF180" t="inlineStr">
-        <is>
-          <t>monzodiorite monzogabbro</t>
-        </is>
-      </c>
-      <c r="AG180" t="inlineStr">
-        <is>
-          <t>mineraloth</t>
-        </is>
-      </c>
-      <c r="AH180" t="n">
+      <c r="AF180" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first try making a geological map with CIPWFULL
only a small amount of granites --> something wrong, will look into it tomorrow
also very large excel files
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>105508726.4694378</v>
+        <v>422823.0001388173</v>
       </c>
       <c r="C2" t="n">
-        <v>-209018146.6045218</v>
+        <v>7525442.527047326</v>
       </c>
       <c r="D2" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>132646577.4596441</v>
+        <v>451013.4314993119</v>
       </c>
       <c r="C3" t="n">
-        <v>-241504486.6946509</v>
+        <v>7286868.704686873</v>
       </c>
       <c r="D3" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>116529554.7152026</v>
+        <v>594545.9850944348</v>
       </c>
       <c r="C4" t="n">
-        <v>-213442943.3238954</v>
+        <v>7366095.350358819</v>
       </c>
       <c r="D4" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>106092782.3304012</v>
+        <v>403945.0768397648</v>
       </c>
       <c r="C5" t="n">
-        <v>-210929361.0420707</v>
+        <v>7527910.87798272</v>
       </c>
       <c r="D5" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>105991829.6311245</v>
+        <v>401216.148465685</v>
       </c>
       <c r="C6" t="n">
-        <v>-210946344.5005981</v>
+        <v>7529882.125589605</v>
       </c>
       <c r="D6" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>122395754.4997257</v>
+        <v>409155.6666583589</v>
       </c>
       <c r="C7" t="n">
-        <v>-232183773.5343286</v>
+        <v>7388267.661607112</v>
       </c>
       <c r="D7" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>106102412.26284</v>
+        <v>408788.64986577</v>
       </c>
       <c r="C8" t="n">
-        <v>-210661424.2871895</v>
+        <v>7525883.127678607</v>
       </c>
       <c r="D8" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>117040622.1587794</v>
+        <v>573609.5498119397</v>
       </c>
       <c r="C9" t="n">
-        <v>-215321766.9774082</v>
+        <v>7369187.59580075</v>
       </c>
       <c r="D9" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>103861518.1174055</v>
+        <v>395739.2028744464</v>
       </c>
       <c r="C10" t="n">
-        <v>-208247002.9008795</v>
+        <v>7550553.333618967</v>
       </c>
       <c r="D10" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>117134202.8675836</v>
+        <v>595482.5194309736</v>
       </c>
       <c r="C11" t="n">
-        <v>-214123845.5357292</v>
+        <v>7360555.884229297</v>
       </c>
       <c r="D11" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>138056256.2293121</v>
+        <v>570295.7162984037</v>
       </c>
       <c r="C12" t="n">
-        <v>-238975883.2737637</v>
+        <v>7194426.892189107</v>
       </c>
       <c r="D12" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>127395291.6096901</v>
+        <v>507596.7447241906</v>
       </c>
       <c r="C13" t="n">
-        <v>-231756331.7183017</v>
+        <v>7306910.773843632</v>
       </c>
       <c r="D13" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>102692553.5673765</v>
+        <v>429046.3551782307</v>
       </c>
       <c r="C14" t="n">
-        <v>-204683855.8293287</v>
+        <v>7547568.77555988</v>
       </c>
       <c r="D14" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>109438266.882265</v>
+        <v>760472.461105651</v>
       </c>
       <c r="C15" t="n">
-        <v>-195287931.0485279</v>
+        <v>7374813.666059652</v>
       </c>
       <c r="D15" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>138596224.7624223</v>
+        <v>586409.6389365081</v>
       </c>
       <c r="C16" t="n">
-        <v>-238383033.7740149</v>
+        <v>7183700.825286468</v>
       </c>
       <c r="D16" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>130020051.2517149</v>
+        <v>518399.5160626545</v>
       </c>
       <c r="C17" t="n">
-        <v>-234012094.1658826</v>
+        <v>7280948.900331907</v>
       </c>
       <c r="D17" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>134644140.8865899</v>
+        <v>447691.7230347765</v>
       </c>
       <c r="C18" t="n">
-        <v>-243949740.2878812</v>
+        <v>7272079.333575497</v>
       </c>
       <c r="D18" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>139608841.0539081</v>
+        <v>641757.8655294247</v>
       </c>
       <c r="C19" t="n">
-        <v>-235476230.8749945</v>
+        <v>7154179.916507507</v>
       </c>
       <c r="D19" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>105596981.9961531</v>
+        <v>420719.6780329063</v>
       </c>
       <c r="C20" t="n">
-        <v>-209263009.2431625</v>
+        <v>7525508.513714559</v>
       </c>
       <c r="D20" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>141599423.6154124</v>
+        <v>620437.5570446817</v>
       </c>
       <c r="C21" t="n">
-        <v>-238858232.1724758</v>
+        <v>7145829.711649289</v>
       </c>
       <c r="D21" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>134875384.7845174</v>
+        <v>656030.3435174299</v>
       </c>
       <c r="C22" t="n">
-        <v>-229901430.6513903</v>
+        <v>7188356.034972786</v>
       </c>
       <c r="D22" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>105594822.7153038</v>
+        <v>405491.2708980456</v>
       </c>
       <c r="C23" t="n">
-        <v>-210140147.9385734</v>
+        <v>7531595.912204068</v>
       </c>
       <c r="D23" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>105845394.8503075</v>
+        <v>404713.2604548364</v>
       </c>
       <c r="C24" t="n">
-        <v>-210537490.5371626</v>
+        <v>7529740.381576492</v>
       </c>
       <c r="D24" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>134781258.9465282</v>
+        <v>568072.7130961117</v>
       </c>
       <c r="C25" t="n">
-        <v>-235788498.9133089</v>
+        <v>7222234.914685098</v>
       </c>
       <c r="D25" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>125182348.8449171</v>
+        <v>553955.6541633958</v>
       </c>
       <c r="C26" t="n">
-        <v>-226212495.6601892</v>
+        <v>7307428.943578887</v>
       </c>
       <c r="D26" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>105460556.4692007</v>
+        <v>413821.4916065777</v>
       </c>
       <c r="C27" t="n">
-        <v>-209469655.8274356</v>
+        <v>7529429.834138079</v>
       </c>
       <c r="D27" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>127417554.1764413</v>
+        <v>718950.8143728292</v>
       </c>
       <c r="C28" t="n">
-        <v>-218170442.130488</v>
+        <v>7229561.330213139</v>
       </c>
       <c r="D28" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>110635064.8260035</v>
+        <v>689479.0599372458</v>
       </c>
       <c r="C29" t="n">
-        <v>-200693955.3049799</v>
+        <v>7385840.555939897</v>
       </c>
       <c r="D29" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>136104466.1075085</v>
+        <v>640364.9592321715</v>
       </c>
       <c r="C30" t="n">
-        <v>-232184709.8015506</v>
+        <v>7183844.981620431</v>
       </c>
       <c r="D30" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>134783690.3161738</v>
+        <v>568065.8525246648</v>
       </c>
       <c r="C31" t="n">
-        <v>-235791494.57205</v>
+        <v>7222217.524079368</v>
       </c>
       <c r="D31" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>105451235.8885704</v>
+        <v>408978.8275499512</v>
       </c>
       <c r="C32" t="n">
-        <v>-209736329.8344363</v>
+        <v>7531442.590570908</v>
       </c>
       <c r="D32" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>133553287.5962651</v>
+        <v>432660.8029019876</v>
       </c>
       <c r="C33" t="n">
-        <v>-243785214.8407176</v>
+        <v>7287266.453172042</v>
       </c>
       <c r="D33" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>105716464.7564075</v>
+        <v>402680.6572135365</v>
       </c>
       <c r="C34" t="n">
-        <v>-210474208.3568346</v>
+        <v>7531672.625937978</v>
       </c>
       <c r="D34" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>139066872.48509</v>
+        <v>648062.4098775064</v>
       </c>
       <c r="C35" t="n">
-        <v>-234520873.5788515</v>
+        <v>7156317.765654799</v>
       </c>
       <c r="D35" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>138187606.9388872</v>
+        <v>585517.9007419647</v>
       </c>
       <c r="C36" t="n">
-        <v>-238041235.5106107</v>
+        <v>7187408.106334507</v>
       </c>
       <c r="D36" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>111701037.9983043</v>
+        <v>679482.7733917895</v>
       </c>
       <c r="C37" t="n">
-        <v>-202577032.8259242</v>
+        <v>7379568.764875205</v>
       </c>
       <c r="D37" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>113236264.3979196</v>
+        <v>697218.2558684414</v>
       </c>
       <c r="C38" t="n">
-        <v>-203448141.3676558</v>
+        <v>7360280.072632506</v>
       </c>
       <c r="D38" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>102773319.0900762</v>
+        <v>385901.2558721581</v>
       </c>
       <c r="C39" t="n">
-        <v>-207250826.245541</v>
+        <v>7564001.44550652</v>
       </c>
       <c r="D39" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>105017672.2254655</v>
+        <v>424332.5844982759</v>
       </c>
       <c r="C40" t="n">
-        <v>-208242418.4061436</v>
+        <v>7529112.568427877</v>
       </c>
       <c r="D40" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>134701314.1507206</v>
+        <v>569643.0684379223</v>
       </c>
       <c r="C41" t="n">
-        <v>-235598052.3902366</v>
+        <v>7222285.613839785</v>
       </c>
       <c r="D41" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>104439268.9421774</v>
+        <v>402406.4354549267</v>
       </c>
       <c r="C42" t="n">
-        <v>-208685705.4748633</v>
+        <v>7542852.907356113</v>
       </c>
       <c r="D42" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>104063185.0347636</v>
+        <v>437023.185092857</v>
       </c>
       <c r="C43" t="n">
-        <v>-206174733.721487</v>
+        <v>7532468.581112547</v>
       </c>
       <c r="D43" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>116381563.0254742</v>
+        <v>593001.3245233108</v>
       </c>
       <c r="C44" t="n">
-        <v>-213354002.2535594</v>
+        <v>7367918.094725985</v>
       </c>
       <c r="D44" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>100167826.3336622</v>
+        <v>439224.5486118381</v>
       </c>
       <c r="C45" t="n">
-        <v>-200491735.4238619</v>
+        <v>7565894.75324164</v>
       </c>
       <c r="D45" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>106181608.3227286</v>
+        <v>401842.916054123</v>
       </c>
       <c r="C46" t="n">
-        <v>-211176252.3923558</v>
+        <v>7527990.288472353</v>
       </c>
       <c r="D46" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>104367728.3348256</v>
+        <v>388715.6373236501</v>
       </c>
       <c r="C47" t="n">
-        <v>-209373254.1300425</v>
+        <v>7548996.648429874</v>
       </c>
       <c r="D47" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>104424001.3408905</v>
+        <v>433477.7838170429</v>
       </c>
       <c r="C48" t="n">
-        <v>-206884594.4189475</v>
+        <v>7530698.264778861</v>
       </c>
       <c r="D48" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>137283281.5320168</v>
+        <v>590088.3297374767</v>
       </c>
       <c r="C49" t="n">
-        <v>-236821997.8006023</v>
+        <v>7193087.563682824</v>
       </c>
       <c r="D49" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>106000975.046599</v>
+        <v>421309.4212496581</v>
       </c>
       <c r="C50" t="n">
-        <v>-209794092.8900959</v>
+        <v>7521773.247238778</v>
       </c>
       <c r="D50" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>117159326.3814496</v>
+        <v>778993.4381261227</v>
       </c>
       <c r="C51" t="n">
-        <v>-203346207.1822138</v>
+        <v>7299986.83529006</v>
       </c>
       <c r="D51" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>123465584.6433238</v>
+        <v>410340.4763310733</v>
       </c>
       <c r="C52" t="n">
-        <v>-233430269.622158</v>
+        <v>7378952.937187641</v>
       </c>
       <c r="D52" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>130665300.368854</v>
+        <v>463408.7043260257</v>
       </c>
       <c r="C53" t="n">
-        <v>-238428189.4724956</v>
+        <v>7297853.838466587</v>
       </c>
       <c r="D53" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>100367178.8657337</v>
+        <v>444667.0044273772</v>
       </c>
       <c r="C54" t="n">
-        <v>-200478489.6620883</v>
+        <v>7562048.963216691</v>
       </c>
       <c r="D54" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>105352880.5020434</v>
+        <v>421470.9503357491</v>
       </c>
       <c r="C55" t="n">
-        <v>-208877513.5332501</v>
+        <v>7527329.485975892</v>
       </c>
       <c r="D55" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>129647122.8856552</v>
+        <v>526067.6630022393</v>
       </c>
       <c r="C56" t="n">
-        <v>-233086310.6818279</v>
+        <v>7281008.696502964</v>
       </c>
       <c r="D56" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>99652515.60497172</v>
+        <v>384404.2276939754</v>
       </c>
       <c r="C57" t="n">
-        <v>-202793563.913616</v>
+        <v>7591962.608249241</v>
       </c>
       <c r="D57" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>124626453.9291485</v>
+        <v>414448.1731552719</v>
       </c>
       <c r="C58" t="n">
-        <v>-234583616.9577389</v>
+        <v>7367681.028654348</v>
       </c>
       <c r="D58" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>112672866.8429443</v>
+        <v>705283.5520898863</v>
       </c>
       <c r="C59" t="n">
-        <v>-202306174.8753476</v>
+        <v>7362709.877786176</v>
       </c>
       <c r="D59" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>120818759.6407465</v>
+        <v>428504.0728901725</v>
       </c>
       <c r="C60" t="n">
-        <v>-228976588.5435393</v>
+        <v>7393290.601893418</v>
       </c>
       <c r="D60" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>136059248.6204675</v>
+        <v>364167.4705087786</v>
       </c>
       <c r="C61" t="n">
-        <v>-251416086.562739</v>
+        <v>7297116.842234123</v>
       </c>
       <c r="D61" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>137281823.6174914</v>
+        <v>590092.4094163297</v>
       </c>
       <c r="C62" t="n">
-        <v>-236820256.6947784</v>
+        <v>7193098.011324367</v>
       </c>
       <c r="D62" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>111557958.197442</v>
+        <v>754559.5701349006</v>
       </c>
       <c r="C63" t="n">
-        <v>-198188443.8184662</v>
+        <v>7357457.446217685</v>
       </c>
       <c r="D63" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>122342850.5698752</v>
+        <v>415018.0448537197</v>
       </c>
       <c r="C64" t="n">
-        <v>-231739329.838951</v>
+        <v>7386252.235449532</v>
       </c>
       <c r="D64" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>113504335.765346</v>
+        <v>393866.9952033143</v>
       </c>
       <c r="C65" t="n">
-        <v>-221679853.6071709</v>
+        <v>7468780.921490044</v>
       </c>
       <c r="D65" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>117746875.3597333</v>
+        <v>793848.6559708756</v>
       </c>
       <c r="C66" t="n">
-        <v>-203145161.1829448</v>
+        <v>7290260.126774631</v>
       </c>
       <c r="D66" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>123466691.2825127</v>
+        <v>410337.1139574873</v>
       </c>
       <c r="C67" t="n">
-        <v>-233431851.2426446</v>
+        <v>7378945.240007831</v>
       </c>
       <c r="D67" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>110571376.8817002</v>
+        <v>705411.5012919909</v>
       </c>
       <c r="C68" t="n">
-        <v>-199724522.8641171</v>
+        <v>7381384.438635441</v>
       </c>
       <c r="D68" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>110055601.0016471</v>
+        <v>827178.5078480255</v>
       </c>
       <c r="C69" t="n">
-        <v>-192394145.9747593</v>
+        <v>7350027.173207692</v>
       </c>
       <c r="D69" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>115877033.3297141</v>
+        <v>704315.0658106438</v>
       </c>
       <c r="C70" t="n">
-        <v>-206198179.3881435</v>
+        <v>7334696.005952516</v>
       </c>
       <c r="D70" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>130111079.5130356</v>
+        <v>622134.3892227954</v>
       </c>
       <c r="C71" t="n">
-        <v>-227255961.6400539</v>
+        <v>7240708.73367288</v>
       </c>
       <c r="D71" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>105598637.6146314</v>
+        <v>420714.5822642142</v>
       </c>
       <c r="C72" t="n">
-        <v>-209265622.4662407</v>
+        <v>7525496.171109289</v>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>134781913.8277764</v>
+        <v>568070.8652271603</v>
       </c>
       <c r="C73" t="n">
-        <v>-235789305.7885106</v>
+        <v>7222230.230568401</v>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>120457917.0446891</v>
+        <v>517897.6597152865</v>
       </c>
       <c r="C74" t="n">
-        <v>-222901472.9667384</v>
+        <v>7360848.522584329</v>
       </c>
       <c r="D74" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>104656956.3492973</v>
+        <v>402334.5145603271</v>
       </c>
       <c r="C75" t="n">
-        <v>-208998483.7739748</v>
+        <v>7540991.602727064</v>
       </c>
       <c r="D75" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>140447377.957341</v>
+        <v>572359.5505096086</v>
       </c>
       <c r="C76" t="n">
-        <v>-241190465.6660586</v>
+        <v>7174025.31142854</v>
       </c>
       <c r="D76" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>127382852.6466472</v>
+        <v>632953.2160392514</v>
       </c>
       <c r="C77" t="n">
-        <v>-223616842.4244619</v>
+        <v>7259778.363588417</v>
       </c>
       <c r="D77" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>106918502.4314488</v>
+        <v>727838.3447125108</v>
       </c>
       <c r="C78" t="n">
-        <v>-193926183.2665913</v>
+        <v>7407376.859851267</v>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>99678515.17212091</v>
+        <v>383725.8459431626</v>
       </c>
       <c r="C79" t="n">
-        <v>-202869844.3416095</v>
+        <v>7592006.341748471</v>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>124630512.6759802</v>
+        <v>414435.8746544203</v>
       </c>
       <c r="C80" t="n">
-        <v>-234589366.480262</v>
+        <v>7367652.856344703</v>
       </c>
       <c r="D80" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>122906404.1367475</v>
+        <v>412673.4235208518</v>
       </c>
       <c r="C81" t="n">
-        <v>-232588847.2752898</v>
+        <v>7382581.441586836</v>
       </c>
       <c r="D81" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>123834612.5745275</v>
+        <v>407314.2720218997</v>
       </c>
       <c r="C82" t="n">
-        <v>-234081588.0408616</v>
+        <v>7377190.661707142</v>
       </c>
       <c r="D82" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>125024745.8866452</v>
+        <v>723787.2073493205</v>
       </c>
       <c r="C83" t="n">
-        <v>-215332164.6101156</v>
+        <v>7248572.024052578</v>
       </c>
       <c r="D83" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>114770796.1817679</v>
+        <v>790262.1937427302</v>
       </c>
       <c r="C84" t="n">
-        <v>-199968539.1906832</v>
+        <v>7317937.23898467</v>
       </c>
       <c r="D84" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>136399735.7707716</v>
+        <v>598663.1839319061</v>
       </c>
       <c r="C85" t="n">
-        <v>-235342743.6443977</v>
+        <v>7197091.63736374</v>
       </c>
       <c r="D85" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>124134250.592144</v>
+        <v>405767.7027150932</v>
       </c>
       <c r="C86" t="n">
-        <v>-234550627.4243446</v>
+        <v>7375381.027371443</v>
       </c>
       <c r="D86" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>109970644.6036005</v>
+        <v>762480.8616364233</v>
       </c>
       <c r="C87" t="n">
-        <v>-195827838.7745652</v>
+        <v>7369402.187121131</v>
       </c>
       <c r="D87" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>118735399.5336341</v>
+        <v>439843.9287411383</v>
       </c>
       <c r="C88" t="n">
-        <v>-225639454.349205</v>
+        <v>7406029.903836646</v>
       </c>
       <c r="D88" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>99948772.93257391</v>
+        <v>382271.6480455336</v>
       </c>
       <c r="C89" t="n">
-        <v>-203348593.3003232</v>
+        <v>7590211.624238232</v>
       </c>
       <c r="D89" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>113568385.9032365</v>
+        <v>402335.643714165</v>
       </c>
       <c r="C90" t="n">
-        <v>-221247347.6185689</v>
+        <v>7464744.675496253</v>
       </c>
       <c r="D90" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>99680708.61797616</v>
+        <v>383718.8813232478</v>
       </c>
       <c r="C91" t="n">
-        <v>-202873459.8895674</v>
+        <v>7591989.812414211</v>
       </c>
       <c r="D91" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>110142394.5216578</v>
+        <v>539831.0236638299</v>
       </c>
       <c r="C92" t="n">
-        <v>-208562628.9073775</v>
+        <v>7440963.848228727</v>
       </c>
       <c r="D92" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>99031260.30550426</v>
+        <v>389353.0613288408</v>
       </c>
       <c r="C93" t="n">
-        <v>-201602192.2960845</v>
+        <v>7595463.263758845</v>
       </c>
       <c r="D93" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>99679793.69599606</v>
+        <v>383721.7863796732</v>
       </c>
       <c r="C94" t="n">
-        <v>-202871951.7895998</v>
+        <v>7591996.707043167</v>
       </c>
       <c r="D94" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>99085419.68022577</v>
+        <v>387990.2999005239</v>
       </c>
       <c r="C95" t="n">
-        <v>-201758063.0948648</v>
+        <v>7595529.493387843</v>
       </c>
       <c r="D95" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>117016909.536118</v>
+        <v>669452.4467849245</v>
       </c>
       <c r="C96" t="n">
-        <v>-209587252.9708545</v>
+        <v>7336131.153987038</v>
       </c>
       <c r="D96" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>102545355.9689802</v>
+        <v>391429.212175432</v>
       </c>
       <c r="C97" t="n">
-        <v>-206606667.7502118</v>
+        <v>7563757.379410667</v>
       </c>
       <c r="D97" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>117672836.3618993</v>
+        <v>569239.5613440264</v>
       </c>
       <c r="C98" t="n">
-        <v>-216358649.6340961</v>
+        <v>7365353.885484916</v>
       </c>
       <c r="D98" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>123978034.8062271</v>
+        <v>404339.0276015802</v>
       </c>
       <c r="C99" t="n">
-        <v>-234452325.5146987</v>
+        <v>7377267.93003197</v>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>120470081.3920262</v>
+        <v>426389.9074570178</v>
       </c>
       <c r="C100" t="n">
-        <v>-228674520.3612784</v>
+        <v>7397057.334183707</v>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>137093107.2131552</v>
+        <v>647260.2346404803</v>
       </c>
       <c r="C101" t="n">
-        <v>-232680201.6958987</v>
+        <v>7173046.349524124</v>
       </c>
       <c r="D101" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>105511964.562603</v>
+        <v>422813.0446212821</v>
       </c>
       <c r="C102" t="n">
-        <v>-209023256.3673792</v>
+        <v>7525418.358305623</v>
       </c>
       <c r="D102" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>114333012.3162275</v>
+        <v>409920.3594865833</v>
       </c>
       <c r="C103" t="n">
-        <v>-221797612.6148877</v>
+        <v>7455181.222219932</v>
       </c>
       <c r="D103" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>117585726.1880774</v>
+        <v>469900.8002904762</v>
       </c>
       <c r="C104" t="n">
-        <v>-222315825.1105521</v>
+        <v>7403678.552845351</v>
       </c>
       <c r="D104" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>107604625.910323</v>
+        <v>464459.3821369232</v>
       </c>
       <c r="C105" t="n">
-        <v>-209515713.5931183</v>
+        <v>7491066.084930793</v>
       </c>
       <c r="D105" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>145569466.401966</v>
+        <v>366853.0474747586</v>
       </c>
       <c r="C106" t="n">
-        <v>-261425231.6330547</v>
+        <v>7220754.392227514</v>
       </c>
       <c r="D106" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>130113878.5378258</v>
+        <v>567174.9081824664</v>
       </c>
       <c r="C107" t="n">
-        <v>-230877998.5930108</v>
+        <v>7261232.535008149</v>
       </c>
       <c r="D107" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>105080389.1113953</v>
+        <v>397376.1849744547</v>
       </c>
       <c r="C108" t="n">
-        <v>-209884292.3578205</v>
+        <v>7539315.330421793</v>
       </c>
       <c r="D108" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>120489265.4427217</v>
+        <v>747622.3765616242</v>
       </c>
       <c r="C109" t="n">
-        <v>-208929469.54725</v>
+        <v>7280326.687097363</v>
       </c>
       <c r="D109" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>98461024.83522852</v>
+        <v>450489.7582604677</v>
       </c>
       <c r="C110" t="n">
-        <v>-197396514.180316</v>
+        <v>7576800.85477192</v>
       </c>
       <c r="D110" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>115607022.0688982</v>
+        <v>710339.3015028904</v>
       </c>
       <c r="C111" t="n">
-        <v>-205529791.2928719</v>
+        <v>7335141.778801956</v>
       </c>
       <c r="D111" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>124822083.9285265</v>
+        <v>396053.62525233</v>
       </c>
       <c r="C112" t="n">
-        <v>-236031568.2958097</v>
+        <v>7373862.411237928</v>
       </c>
       <c r="D112" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>100156661.0837503</v>
+        <v>444704.7907449754</v>
       </c>
       <c r="C113" t="n">
-        <v>-200172776.0156584</v>
+        <v>7563900.888378733</v>
       </c>
       <c r="D113" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>100001447.5327858</v>
+        <v>443363.6732012552</v>
       </c>
       <c r="C114" t="n">
-        <v>-200022630.0171967</v>
+        <v>7565788.758657504</v>
       </c>
       <c r="D114" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>141041486.155849</v>
+        <v>367652.259629715</v>
       </c>
       <c r="C115" t="n">
-        <v>-256629137.1601039</v>
+        <v>7256028.81467634</v>
       </c>
       <c r="D115" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>115944493.4328775</v>
+        <v>669640.2285336041</v>
       </c>
       <c r="C116" t="n">
-        <v>-208300507.8710816</v>
+        <v>7345433.276130389</v>
       </c>
       <c r="D116" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>116477400.184276</v>
+        <v>600557.637797766</v>
       </c>
       <c r="C117" t="n">
-        <v>-213021100.7277543</v>
+        <v>7364421.865823336</v>
       </c>
       <c r="D117" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>134073855.6473529</v>
+        <v>600393.0921995796</v>
       </c>
       <c r="C118" t="n">
-        <v>-232856329.5791467</v>
+        <v>7215709.499915746</v>
       </c>
       <c r="D118" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>117860571.0843874</v>
+        <v>497782.9113988071</v>
       </c>
       <c r="C119" t="n">
-        <v>-220944422.1572055</v>
+        <v>7390496.471405526</v>
       </c>
       <c r="D119" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>103446922.0606982</v>
+        <v>436466.800330822</v>
       </c>
       <c r="C120" t="n">
-        <v>-205335959.0468844</v>
+        <v>7538074.706984714</v>
       </c>
       <c r="D120" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>99679180.36433366</v>
+        <v>383723.7338277422</v>
       </c>
       <c r="C121" t="n">
-        <v>-202870940.8090142</v>
+        <v>7592001.328981454</v>
       </c>
       <c r="D121" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>99021577.51894188</v>
+        <v>446965.5634673933</v>
       </c>
       <c r="C122" t="n">
-        <v>-198404658.9435754</v>
+        <v>7573131.755081054</v>
       </c>
       <c r="D122" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>99706732.31271403</v>
+        <v>445475.1194111918</v>
       </c>
       <c r="C123" t="n">
-        <v>-199480058.8985869</v>
+        <v>7567601.635024867</v>
       </c>
       <c r="D123" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>124840981.4588256</v>
+        <v>621810.8103163663</v>
       </c>
       <c r="C124" t="n">
-        <v>-221515326.7091922</v>
+        <v>7285316.554902539</v>
       </c>
       <c r="D124" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>101482637.130122</v>
+        <v>453416.9831956982</v>
       </c>
       <c r="C125" t="n">
-        <v>-201593533.2296944</v>
+        <v>7548850.096561186</v>
       </c>
       <c r="D125" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>115547775.5122885</v>
+        <v>611592.6100460046</v>
       </c>
       <c r="C126" t="n">
-        <v>-211230821.352387</v>
+        <v>7368598.606297649</v>
       </c>
       <c r="D126" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>109571273.3401862</v>
+        <v>828987.291295761</v>
       </c>
       <c r="C127" t="n">
-        <v>-191719277.4940407</v>
+        <v>7353960.948327379</v>
       </c>
       <c r="D127" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>99678284.8839162</v>
+        <v>383726.5771532588</v>
       </c>
       <c r="C128" t="n">
-        <v>-202869464.7461046</v>
+        <v>7592008.077162812</v>
       </c>
       <c r="D128" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>116896498.8276936</v>
+        <v>572065.6433788443</v>
       </c>
       <c r="C129" t="n">
-        <v>-215237703.2306432</v>
+        <v>7370981.487775771</v>
       </c>
       <c r="D129" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>101486613.3077085</v>
+        <v>570671.744298632</v>
       </c>
       <c r="C130" t="n">
-        <v>-195192346.6161174</v>
+        <v>7506660.864765343</v>
       </c>
       <c r="D130" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>111206429.3717718</v>
+        <v>539967.4751042218</v>
       </c>
       <c r="C131" t="n">
-        <v>-209942642.4337206</v>
+        <v>7431673.784536626</v>
       </c>
       <c r="D131" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>100690301.4471169</v>
+        <v>452174.9311583586</v>
       </c>
       <c r="C132" t="n">
-        <v>-200528169.7813111</v>
+        <v>7556332.266056828</v>
       </c>
       <c r="D132" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>99441616.50272426</v>
+        <v>384478.042694183</v>
       </c>
       <c r="C133" t="n">
-        <v>-202479162.9386826</v>
+        <v>7593792.795184806</v>
       </c>
       <c r="D133" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>113308239.1278594</v>
+        <v>472457.6527888828</v>
       </c>
       <c r="C134" t="n">
-        <v>-216662236.3820526</v>
+        <v>7438943.410384167</v>
       </c>
       <c r="D134" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>117210532.9378552</v>
+        <v>796518.4161216137</v>
       </c>
       <c r="C135" t="n">
-        <v>-202388640.3289137</v>
+        <v>7294240.829803186</v>
       </c>
       <c r="D135" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>104803634.4021675</v>
+        <v>439654.4736789956</v>
       </c>
       <c r="C136" t="n">
-        <v>-207065422.8186131</v>
+        <v>7524984.020991635</v>
       </c>
       <c r="D136" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>115088902.8054884</v>
+        <v>597874.7966290781</v>
       </c>
       <c r="C137" t="n">
-        <v>-211475437.8546615</v>
+        <v>7377365.426627968</v>
       </c>
       <c r="D137" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>108953363.5511799</v>
+        <v>507905.568870945</v>
       </c>
       <c r="C138" t="n">
-        <v>-208830389.1402352</v>
+        <v>7462990.403153609</v>
       </c>
       <c r="D138" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>132227328.7373793</v>
+        <v>366329.6275398433</v>
       </c>
       <c r="C139" t="n">
-        <v>-246882657.1680205</v>
+        <v>7326783.189303711</v>
       </c>
       <c r="D139" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>120645077.3307229</v>
+        <v>456361.2898843428</v>
       </c>
       <c r="C140" t="n">
-        <v>-226992646.1945517</v>
+        <v>7383412.108057517</v>
       </c>
       <c r="D140" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>100370172.5250075</v>
+        <v>444657.8554364101</v>
       </c>
       <c r="C141" t="n">
-        <v>-200483310.2279336</v>
+        <v>7562025.921142353</v>
       </c>
       <c r="D141" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>121803530.9674991</v>
+        <v>672768.4835952614</v>
       </c>
       <c r="C142" t="n">
-        <v>-214929262.2081245</v>
+        <v>7293509.317555598</v>
       </c>
       <c r="D142" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>115093850.2074087</v>
+        <v>612182.4967714186</v>
       </c>
       <c r="C143" t="n">
-        <v>-210639130.9912758</v>
+        <v>7372330.057555402</v>
       </c>
       <c r="D143" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>103822953.4520017</v>
+        <v>728433.5137220931</v>
       </c>
       <c r="C144" t="n">
-        <v>-189930731.702317</v>
+        <v>7435412.922395073</v>
       </c>
       <c r="D144" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>132877443.62134</v>
+        <v>714304.8037613939</v>
       </c>
       <c r="C145" t="n">
-        <v>-224023748.5784365</v>
+        <v>7184478.611043642</v>
       </c>
       <c r="D145" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>101015466.2542255</v>
+        <v>439047.5535942831</v>
       </c>
       <c r="C146" t="n">
-        <v>-201723206.6404476</v>
+        <v>7558462.652592706</v>
       </c>
       <c r="D146" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>119228449.4292004</v>
+        <v>433932.7497139967</v>
       </c>
       <c r="C147" t="n">
-        <v>-226634202.4660612</v>
+        <v>7404311.079104981</v>
       </c>
       <c r="D147" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>140082692.4468106</v>
+        <v>663250.528201481</v>
       </c>
       <c r="C148" t="n">
-        <v>-234409595.1433657</v>
+        <v>7142209.795338459</v>
       </c>
       <c r="D148" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>119395384.9325225</v>
+        <v>468998.8339806726</v>
       </c>
       <c r="C149" t="n">
-        <v>-224644429.6894445</v>
+        <v>7388821.772371144</v>
       </c>
       <c r="D149" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>107077921.004971</v>
+        <v>436408.8218150658</v>
       </c>
       <c r="C150" t="n">
-        <v>-210415575.5129712</v>
+        <v>7506500.594720325</v>
       </c>
       <c r="D150" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>116599761.8003678</v>
+        <v>569006.5176380178</v>
       </c>
       <c r="C151" t="n">
-        <v>-215056264.1719109</v>
+        <v>7374633.408555133</v>
       </c>
       <c r="D151" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>143874749.0634952</v>
+        <v>376624.0866571964</v>
       </c>
       <c r="C152" t="n">
-        <v>-258943761.0773299</v>
+        <v>7229605.106066765</v>
       </c>
       <c r="D152" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>122093307.7635642</v>
+        <v>444385.7615036962</v>
       </c>
       <c r="C153" t="n">
-        <v>-229543200.8580566</v>
+        <v>7376206.848085475</v>
       </c>
       <c r="D153" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>105590085.9079321</v>
+        <v>431132.6180002625</v>
       </c>
       <c r="C154" t="n">
-        <v>-208653782.3603525</v>
+        <v>7521465.612824399</v>
       </c>
       <c r="D154" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>132597887.1665408</v>
+        <v>584961.2195156019</v>
       </c>
       <c r="C155" t="n">
-        <v>-232357831.3243726</v>
+        <v>7233817.372569075</v>
       </c>
       <c r="D155" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>103470805.8748131</v>
+        <v>446157.5485860738</v>
       </c>
       <c r="C156" t="n">
-        <v>-204822101.9525426</v>
+        <v>7534123.93820927</v>
       </c>
       <c r="D156" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>127180613.9277396</v>
+        <v>669236.5653518254</v>
       </c>
       <c r="C157" t="n">
-        <v>-221078511.4456128</v>
+        <v>7248640.712909578</v>
       </c>
       <c r="D157" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>116386930.9560903</v>
+        <v>777512.9831815676</v>
       </c>
       <c r="C158" t="n">
-        <v>-202553336.0838474</v>
+        <v>7307313.468056051</v>
       </c>
       <c r="D158" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>101583352.7685994</v>
+        <v>435487.6637338779</v>
       </c>
       <c r="C159" t="n">
-        <v>-202736787.3699743</v>
+        <v>7554822.370589631</v>
       </c>
       <c r="D159" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>139999211.642137</v>
+        <v>664861.8344592829</v>
       </c>
       <c r="C160" t="n">
-        <v>-234218738.9120067</v>
+        <v>7142306.853326681</v>
       </c>
       <c r="D160" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>129403918.6188121</v>
+        <v>713772.8159372762</v>
       </c>
       <c r="C161" t="n">
-        <v>-220561130.1128934</v>
+        <v>7214284.154764948</v>
       </c>
       <c r="D161" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>118958854.6132308</v>
+        <v>439805.1538512177</v>
       </c>
       <c r="C162" t="n">
-        <v>-225924513.2256453</v>
+        <v>7404176.992680821</v>
       </c>
       <c r="D162" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>127361799.8553083</v>
+        <v>647141.1239790823</v>
       </c>
       <c r="C163" t="n">
-        <v>-222684836.8283646</v>
+        <v>7254886.228397596</v>
       </c>
       <c r="D163" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>105214205.3888756</v>
+        <v>429836.6878292271</v>
       </c>
       <c r="C164" t="n">
-        <v>-208202346.972273</v>
+        <v>7525240.43409429</v>
       </c>
       <c r="D164" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>130001514.6469524</v>
+        <v>714955.4111270539</v>
       </c>
       <c r="C165" t="n">
-        <v>-221096251.1072609</v>
+        <v>7208770.172444158</v>
       </c>
       <c r="D165" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>137717459.0523186</v>
+        <v>612695.2306431417</v>
       </c>
       <c r="C166" t="n">
-        <v>-235681984.5561872</v>
+        <v>7180841.293022046</v>
       </c>
       <c r="D166" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>105128541.7492181</v>
+        <v>431933.0220172554</v>
       </c>
       <c r="C167" t="n">
-        <v>-207962133.4922707</v>
+        <v>7525164.216234216</v>
       </c>
       <c r="D167" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>121060300.4620544</v>
+        <v>571477.7003448418</v>
       </c>
       <c r="C168" t="n">
-        <v>-220297557.7979507</v>
+        <v>7335667.556724924</v>
       </c>
       <c r="D168" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>136483512.4430443</v>
+        <v>725637.832248533</v>
       </c>
       <c r="C169" t="n">
-        <v>-226734556.8126839</v>
+        <v>7149922.107346477</v>
       </c>
       <c r="D169" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>124548501.1505335</v>
+        <v>674219.4674038889</v>
       </c>
       <c r="C170" t="n">
-        <v>-217902651.7519901</v>
+        <v>7269409.352310479</v>
       </c>
       <c r="D170" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>128464498.0296568</v>
+        <v>710749.5401521167</v>
       </c>
       <c r="C171" t="n">
-        <v>-219784764.8501419</v>
+        <v>7223356.075473163</v>
       </c>
       <c r="D171" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>136901542.6570788</v>
+        <v>593191.4187559042</v>
       </c>
       <c r="C172" t="n">
-        <v>-236224593.5605564</v>
+        <v>7195042.290479658</v>
       </c>
       <c r="D172" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>140229425.9082486</v>
+        <v>669087.1574735446</v>
       </c>
       <c r="C173" t="n">
-        <v>-234134835.1599286</v>
+        <v>7138823.143244307</v>
       </c>
       <c r="D173" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>115411245.186507</v>
+        <v>576221.5915295435</v>
       </c>
       <c r="C174" t="n">
-        <v>-213155727.6359349</v>
+        <v>7382257.330581195</v>
       </c>
       <c r="D174" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>137088898.2118142</v>
+        <v>713603.1766074058</v>
       </c>
       <c r="C175" t="n">
-        <v>-228123017.841619</v>
+        <v>7149041.025246967</v>
       </c>
       <c r="D175" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>138936348.0628513</v>
+        <v>575266.3307147442</v>
       </c>
       <c r="C176" t="n">
-        <v>-239502436.3370571</v>
+        <v>7185257.558376712</v>
       </c>
       <c r="D176" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>116306647.5220219</v>
+        <v>604290.0810529721</v>
       </c>
       <c r="C177" t="n">
-        <v>-212590809.3727053</v>
+        <v>7364583.701289264</v>
       </c>
       <c r="D177" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>120195467.8391005</v>
+        <v>432284.6912633065</v>
       </c>
       <c r="C178" t="n">
-        <v>-227955826.4722086</v>
+        <v>7396923.161243825</v>
       </c>
       <c r="D178" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>119185180.0915828</v>
+        <v>439758.1563198671</v>
       </c>
       <c r="C179" t="n">
-        <v>-226213221.2188751</v>
+        <v>7402304.535486695</v>
       </c>
       <c r="D179" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>132649677.9409595</v>
+        <v>455576.2169239347</v>
       </c>
       <c r="C180" t="n">
-        <v>-241194673.5050797</v>
+        <v>7284936.716519298</v>
       </c>
       <c r="D180" t="n">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
first try geological map: area2
-still same problem as previous time, couldn't fix it
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,17 +528,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>422823.0001388173</v>
+        <v>170061253.5450011</v>
       </c>
       <c r="C2" t="n">
-        <v>7525442.527047326</v>
+        <v>-402048568.8690004</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -642,17 +642,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>451013.4314993119</v>
+        <v>215751600.2529267</v>
       </c>
       <c r="C3" t="n">
-        <v>7286868.704686873</v>
+        <v>-466156325.3815762</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -756,17 +756,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>594545.9850944348</v>
+        <v>190157095.1846463</v>
       </c>
       <c r="C4" t="n">
-        <v>7366095.350358819</v>
+        <v>-415950649.4723316</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -874,17 +874,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>403945.0768397648</v>
+        <v>170860992.9712256</v>
       </c>
       <c r="C5" t="n">
-        <v>7527910.87798272</v>
+        <v>-405155427.0714723</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -988,17 +988,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>401216.148465685</v>
+        <v>170667185.431315</v>
       </c>
       <c r="C6" t="n">
-        <v>7529882.125589605</v>
+        <v>-405104104.4883425</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1102,17 +1102,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>409155.6666583589</v>
+        <v>198148318.8949276</v>
       </c>
       <c r="C7" t="n">
-        <v>7388267.661607112</v>
+        <v>-446478395.0038871</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1212,17 +1212,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>408788.64986577</v>
+        <v>170922082.497805</v>
       </c>
       <c r="C8" t="n">
-        <v>7525883.127678607</v>
+        <v>-404787896.7358894</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1326,17 +1326,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>573609.5498119397</v>
+        <v>190811154.076052</v>
       </c>
       <c r="C9" t="n">
-        <v>7369187.59580075</v>
+        <v>-418967515.8208964</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1444,17 +1444,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>395739.2028744464</v>
+        <v>167063073.7771204</v>
       </c>
       <c r="C10" t="n">
-        <v>7550553.333618967</v>
+        <v>-399736333.0616241</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1562,17 +1562,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>595482.5194309736</v>
+        <v>191182675.188347</v>
       </c>
       <c r="C11" t="n">
-        <v>7360555.884229297</v>
+        <v>-417313437.041097</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1676,17 +1676,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>570295.7162984037</v>
+        <v>226125332.4069945</v>
       </c>
       <c r="C12" t="n">
-        <v>7194426.892189107</v>
+        <v>-465476449.0371869</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1786,17 +1786,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>507596.7447241906</v>
+        <v>207534924.9715279</v>
       </c>
       <c r="C13" t="n">
-        <v>7306910.773843632</v>
+        <v>-448996303.2290542</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1892,17 +1892,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>429046.3551782307</v>
+        <v>165417181.4159042</v>
       </c>
       <c r="C14" t="n">
-        <v>7547568.77555988</v>
+        <v>-393879767.4921157</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2006,17 +2006,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>760472.461105651</v>
+        <v>179797278.9888872</v>
       </c>
       <c r="C15" t="n">
-        <v>7374813.666059652</v>
+        <v>-385339572.3715404</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2116,17 +2116,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>586409.6389365081</v>
+        <v>227210100.4166648</v>
       </c>
       <c r="C16" t="n">
-        <v>7183700.825286468</v>
+        <v>-464887206.9620859</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2230,17 +2230,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>518399.5160626545</v>
+        <v>212055122.9125671</v>
       </c>
       <c r="C17" t="n">
-        <v>7280948.900331907</v>
+        <v>-453803865.4495928</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2340,17 +2340,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>447691.7230347765</v>
+        <v>219066152.3479342</v>
       </c>
       <c r="C18" t="n">
-        <v>7272079.333575497</v>
+        <v>-470844080.385905</v>
       </c>
       <c r="D18" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2454,17 +2454,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>641757.8655294247</v>
+        <v>229520900.4912613</v>
       </c>
       <c r="C19" t="n">
-        <v>7154179.916507507</v>
+        <v>-461115703.439372</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2560,17 +2560,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>420719.6780329063</v>
+        <v>170189121.3721983</v>
       </c>
       <c r="C20" t="n">
-        <v>7525508.513714559</v>
+        <v>-402456658.3516716</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2674,17 +2674,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>620437.5570446817</v>
+        <v>232646418.6580028</v>
       </c>
       <c r="C21" t="n">
-        <v>7145829.711649289</v>
+        <v>-467100958.0807744</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2784,17 +2784,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>656030.3435174299</v>
+        <v>221685799.896555</v>
       </c>
       <c r="C22" t="n">
-        <v>7188356.034972786</v>
+        <v>-450486429.1942855</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2890,17 +2890,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>405491.2708980456</v>
+        <v>170044434.1339617</v>
       </c>
       <c r="C23" t="n">
-        <v>7531595.912204068</v>
+        <v>-403681533.2859867</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2996,17 +2996,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>404713.2604548364</v>
+        <v>170455328.0702242</v>
       </c>
       <c r="C24" t="n">
-        <v>7529740.381576492</v>
+        <v>-404423592.289158</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3110,17 +3110,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>568072.7130961117</v>
+        <v>220587369.5919776</v>
       </c>
       <c r="C25" t="n">
-        <v>7222234.914685098</v>
+        <v>-459065039.3759356</v>
       </c>
       <c r="D25" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3224,17 +3224,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>553955.6541633958</v>
+        <v>204294828.1179895</v>
       </c>
       <c r="C26" t="n">
-        <v>7307428.943578887</v>
+        <v>-439678649.7171889</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3334,17 +3334,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>413821.4916065777</v>
+        <v>169897527.0426158</v>
       </c>
       <c r="C27" t="n">
-        <v>7529429.834138079</v>
+        <v>-402644194.6175289</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3448,17 +3448,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>718950.8143728292</v>
+        <v>209752092.0299546</v>
       </c>
       <c r="C28" t="n">
-        <v>7229561.330213139</v>
+        <v>-429279032.9395711</v>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3562,17 +3562,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>689479.0599372458</v>
+        <v>181148880.3769667</v>
       </c>
       <c r="C29" t="n">
-        <v>7385840.555939897</v>
+        <v>-393871673.9209508</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3672,17 +3672,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>640364.9592321715</v>
+        <v>223592087.1595653</v>
       </c>
       <c r="C30" t="n">
-        <v>7183844.981620431</v>
+        <v>-454483925.6360297</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3778,17 +3778,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>568065.8525246648</v>
+        <v>220591388.8574566</v>
       </c>
       <c r="C31" t="n">
-        <v>7222217.524079368</v>
+        <v>-459070734.1471248</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3892,17 +3892,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>408978.8275499512</v>
+        <v>169837139.3715255</v>
       </c>
       <c r="C32" t="n">
-        <v>7531442.590570908</v>
+        <v>-403010049.6333153</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -4006,17 +4006,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>432660.8029019876</v>
+        <v>217075885.120332</v>
       </c>
       <c r="C33" t="n">
-        <v>7287266.453172042</v>
+        <v>-469975118.9094672</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4116,17 +4116,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>402680.6572135365</v>
+        <v>170221339.6758617</v>
       </c>
       <c r="C34" t="n">
-        <v>7531672.625937978</v>
+        <v>-404239109.246271</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4230,17 +4230,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>648062.4098775064</v>
+        <v>228674745.6979045</v>
       </c>
       <c r="C35" t="n">
-        <v>7156317.765654799</v>
+        <v>-459433627.7697359</v>
       </c>
       <c r="D35" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4340,17 +4340,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>585517.9007419647</v>
+        <v>226511925.3198773</v>
       </c>
       <c r="C36" t="n">
-        <v>7187408.106334507</v>
+        <v>-464173405.9727495</v>
       </c>
       <c r="D36" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4458,17 +4458,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>679482.7733917895</v>
+        <v>182849971.5594774</v>
       </c>
       <c r="C37" t="n">
-        <v>7379568.764875205</v>
+        <v>-397265861.4077961</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4568,17 +4568,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>697218.2558684414</v>
+        <v>185605712.1449671</v>
       </c>
       <c r="C38" t="n">
-        <v>7360280.072632506</v>
+        <v>-399507878.409721</v>
       </c>
       <c r="D38" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4682,17 +4682,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>385901.2558721581</v>
+        <v>165158688.1655019</v>
       </c>
       <c r="C39" t="n">
-        <v>7564001.44550652</v>
+        <v>-397520250.4713072</v>
       </c>
       <c r="D39" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4800,17 +4800,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>424332.5844982759</v>
+        <v>169255388.5440889</v>
       </c>
       <c r="C40" t="n">
-        <v>7529112.568427877</v>
+        <v>-400598228.2076799</v>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4918,17 +4918,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>569643.0684379223</v>
+        <v>220469595.8216356</v>
       </c>
       <c r="C41" t="n">
-        <v>7222285.613839785</v>
+        <v>-458743532.120712</v>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5032,17 +5032,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>402406.4354549267</v>
+        <v>168088018.066688</v>
       </c>
       <c r="C42" t="n">
-        <v>7542852.907356113</v>
+        <v>-400784453.2981902</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5150,17 +5150,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>437023.185092857</v>
+        <v>167778416.8765537</v>
       </c>
       <c r="C43" t="n">
-        <v>7532468.581112547</v>
+        <v>-396994263.684976</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5264,17 +5264,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>593001.3245233108</v>
+        <v>189893264.5149418</v>
       </c>
       <c r="C44" t="n">
-        <v>7367918.094725985</v>
+        <v>-415728052.2039195</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5382,17 +5382,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>439224.5486118381</v>
+        <v>161294915.6318805</v>
       </c>
       <c r="C45" t="n">
-        <v>7565894.75324164</v>
+        <v>-386106025.2255547</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5500,17 +5500,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>401842.916054123</v>
+        <v>170989661.2193642</v>
       </c>
       <c r="C46" t="n">
-        <v>7527990.288472353</v>
+        <v>-405566621.7426242</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5610,17 +5610,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>388715.6373236501</v>
+        <v>167842617.8236445</v>
       </c>
       <c r="C47" t="n">
-        <v>7548996.648429874</v>
+        <v>-401689953.4288404</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5728,17 +5728,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>433477.7838170429</v>
+        <v>168348387.5857986</v>
       </c>
       <c r="C48" t="n">
-        <v>7530698.264778861</v>
+        <v>-398256561.2255399</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5842,17 +5842,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>590088.3297374767</v>
+        <v>225037801.297646</v>
       </c>
       <c r="C49" t="n">
-        <v>7193087.563682824</v>
+        <v>-461912078.2331657</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5956,17 +5956,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>421309.4212496581</v>
+        <v>170869051.6025432</v>
       </c>
       <c r="C50" t="n">
-        <v>7521773.247238778</v>
+        <v>-403499299.370443</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -6066,17 +6066,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>778993.4381261227</v>
+        <v>193017470.4955127</v>
       </c>
       <c r="C51" t="n">
-        <v>7299986.83529006</v>
+        <v>-401785101.312815</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -6180,17 +6180,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>410340.4763310733</v>
+        <v>199949949.5776266</v>
       </c>
       <c r="C52" t="n">
-        <v>7378952.937187641</v>
+        <v>-448945059.420067</v>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -6290,17 +6290,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>463408.7043260257</v>
+        <v>212560183.8336233</v>
       </c>
       <c r="C53" t="n">
-        <v>7297853.838466587</v>
+        <v>-460556023.6364397</v>
       </c>
       <c r="D53" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6404,17 +6404,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>444667.0044273772</v>
+        <v>161676484.2880752</v>
       </c>
       <c r="C54" t="n">
-        <v>7562048.963216691</v>
+        <v>-386240761.038307</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6522,17 +6522,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>421470.9503357491</v>
+        <v>169788566.1146641</v>
       </c>
       <c r="C55" t="n">
-        <v>7527329.485975892</v>
+        <v>-401736005.8829324</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6636,17 +6636,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>526067.6630022393</v>
+        <v>211508905.0259657</v>
       </c>
       <c r="C56" t="n">
-        <v>7281008.696502964</v>
+        <v>-452247932.9809692</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6746,17 +6746,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>384404.2276939754</v>
+        <v>159944451.6321533</v>
       </c>
       <c r="C57" t="n">
-        <v>7591962.608249241</v>
+        <v>-388908680.488093</v>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6856,17 +6856,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>414448.1731552719</v>
+        <v>201934275.4551795</v>
       </c>
       <c r="C58" t="n">
-        <v>7367681.028654348</v>
+        <v>-451332610.6898304</v>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6966,17 +6966,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>705283.5520898863</v>
+        <v>184732978.0088556</v>
       </c>
       <c r="C59" t="n">
-        <v>7362709.877786176</v>
+        <v>-397506742.2204202</v>
       </c>
       <c r="D59" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -7080,17 +7080,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>428504.0728901725</v>
+        <v>195705534.4388087</v>
       </c>
       <c r="C60" t="n">
-        <v>7393290.601893418</v>
+        <v>-440888996.2268443</v>
       </c>
       <c r="D60" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -7190,17 +7190,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>364167.4705087786</v>
+        <v>220534136.2407041</v>
       </c>
       <c r="C61" t="n">
-        <v>7297116.842234123</v>
+        <v>-482430540.6605094</v>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7300,17 +7300,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>590092.4094163297</v>
+        <v>225035389.0068487</v>
       </c>
       <c r="C62" t="n">
-        <v>7193098.011324367</v>
+        <v>-461908760.2337005</v>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7414,17 +7414,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>754559.5701349006</v>
+        <v>183320051.9313003</v>
       </c>
       <c r="C63" t="n">
-        <v>7357457.446217685</v>
+        <v>-390873338.4612513</v>
       </c>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7528,17 +7528,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>415018.0448537197</v>
+        <v>198119290.4729356</v>
       </c>
       <c r="C64" t="n">
-        <v>7386252.235449532</v>
+        <v>-445812024.3581349</v>
       </c>
       <c r="D64" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7646,17 +7646,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>393866.9952033143</v>
+        <v>183136998.266023</v>
       </c>
       <c r="C65" t="n">
-        <v>7468780.921490044</v>
+        <v>-425597138.2776437</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7760,17 +7760,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>793848.6559708756</v>
+        <v>194155942.949601</v>
       </c>
       <c r="C66" t="n">
-        <v>7290260.126774631</v>
+        <v>-401840817.6504443</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7874,17 +7874,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>410337.1139574873</v>
+        <v>199951766.5902286</v>
       </c>
       <c r="C67" t="n">
-        <v>7378945.240007831</v>
+        <v>-448948024.5963792</v>
       </c>
       <c r="D67" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7988,17 +7988,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>705411.5012919909</v>
+        <v>181191745.9251307</v>
       </c>
       <c r="C68" t="n">
-        <v>7381384.438635441</v>
+        <v>-392441938.8805223</v>
       </c>
       <c r="D68" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -8102,17 +8102,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>827178.5078480255</v>
+        <v>181465006.6044621</v>
       </c>
       <c r="C69" t="n">
-        <v>7350027.173207692</v>
+        <v>-381565732.0586818</v>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -8216,17 +8216,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>704315.0658106438</v>
+        <v>190126419.3274445</v>
       </c>
       <c r="C70" t="n">
-        <v>7334696.005952516</v>
+        <v>-405131540.1544722</v>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>622134.3892227954</v>
+        <v>213293560.7974027</v>
       </c>
       <c r="C71" t="n">
-        <v>7240708.73367288</v>
+        <v>-444046630.9603429</v>
       </c>
       <c r="D71" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8436,17 +8436,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>420714.5822642142</v>
+        <v>170191838.1157665</v>
       </c>
       <c r="C72" t="n">
-        <v>7525496.171109289</v>
+        <v>-402461543.5417274</v>
       </c>
       <c r="D72" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8550,17 +8550,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>568070.8652271603</v>
+        <v>220588452.1677152</v>
       </c>
       <c r="C73" t="n">
-        <v>7222230.230568401</v>
+        <v>-459066573.2519769</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8664,17 +8664,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>517897.6597152865</v>
+        <v>195997045.5293688</v>
       </c>
       <c r="C74" t="n">
-        <v>7360848.522584329</v>
+        <v>-431996651.364231</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8774,17 +8774,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>402334.5145603271</v>
+        <v>168450500.9432539</v>
       </c>
       <c r="C75" t="n">
-        <v>7540991.602727064</v>
+        <v>-401384793.0106061</v>
       </c>
       <c r="D75" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8892,17 +8892,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>572359.5505096086</v>
+        <v>230175350.2550632</v>
       </c>
       <c r="C76" t="n">
-        <v>7174025.31142854</v>
+        <v>-469965199.3425449</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -9006,17 +9006,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>632953.2160392514</v>
+        <v>208808591.8167622</v>
       </c>
       <c r="C77" t="n">
-        <v>7259778.363588417</v>
+        <v>-437210044.3358359</v>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -9120,17 +9120,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>727838.3447125108</v>
+        <v>175243179.3873374</v>
       </c>
       <c r="C78" t="n">
-        <v>7407376.859851267</v>
+        <v>-381724269.4209624</v>
       </c>
       <c r="D78" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -9234,17 +9234,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>383725.8459431626</v>
+        <v>159981689.5436021</v>
       </c>
       <c r="C79" t="n">
-        <v>7592006.341748471</v>
+        <v>-389034951.2546384</v>
       </c>
       <c r="D79" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -9348,17 +9348,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>414435.8746544203</v>
+        <v>201940941.1117887</v>
       </c>
       <c r="C80" t="n">
-        <v>7367652.856344703</v>
+        <v>-451343395.5166952</v>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -9458,17 +9458,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>412673.4235208518</v>
+        <v>199038252.9463307</v>
       </c>
       <c r="C81" t="n">
-        <v>7382581.441586836</v>
+        <v>-447386185.6953286</v>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9572,17 +9572,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>407314.2720218997</v>
+        <v>200536386.0293367</v>
       </c>
       <c r="C82" t="n">
-        <v>7377190.661707142</v>
+        <v>-450110034.1736351</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9686,17 +9686,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>723787.2073493205</v>
+        <v>205759380.4885022</v>
       </c>
       <c r="C83" t="n">
-        <v>7248572.024052578</v>
+        <v>-423798822.2369605</v>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9796,17 +9796,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>790262.1937427302</v>
+        <v>189088595.2522518</v>
       </c>
       <c r="C84" t="n">
-        <v>7317937.23898467</v>
+        <v>-395445249.0775359</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9906,17 +9906,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>598663.1839319061</v>
+        <v>223641556.3890886</v>
       </c>
       <c r="C85" t="n">
-        <v>7197091.63736374</v>
+        <v>-459278078.5597609</v>
       </c>
       <c r="D85" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -10016,17 +10016,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>405767.7027150932</v>
+        <v>201021809.2568428</v>
       </c>
       <c r="C86" t="n">
-        <v>7375381.027371443</v>
+        <v>-450970544.5014009</v>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -10130,17 +10130,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>762480.8616364233</v>
+        <v>180714862.6879153</v>
       </c>
       <c r="C87" t="n">
-        <v>7369402.187121131</v>
+        <v>-386459896.4466831</v>
       </c>
       <c r="D87" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -10244,17 +10244,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>439843.9287411383</v>
+        <v>192332759.4216259</v>
       </c>
       <c r="C88" t="n">
-        <v>7406029.903836646</v>
+        <v>-434773788.9701531</v>
       </c>
       <c r="D88" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -10354,17 +10354,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>382271.6480455336</v>
+        <v>160418897.5706784</v>
       </c>
       <c r="C89" t="n">
-        <v>7590211.624238232</v>
+        <v>-389911002.6655887</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -10464,17 +10464,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>402335.643714165</v>
+        <v>183326049.5143205</v>
       </c>
       <c r="C90" t="n">
-        <v>7464744.675496253</v>
+        <v>-425033345.1795313</v>
       </c>
       <c r="D90" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10578,17 +10578,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>383718.8813232478</v>
+        <v>159985281.4310923</v>
       </c>
       <c r="C91" t="n">
-        <v>7591989.812414211</v>
+        <v>-389041687.233989</v>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10696,17 +10696,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>539831.0236638299</v>
+        <v>178908355.1332637</v>
       </c>
       <c r="C92" t="n">
-        <v>7440963.848228727</v>
+        <v>-404735969.3286093</v>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10810,17 +10810,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>389353.0613288408</v>
+        <v>158953626.7530148</v>
       </c>
       <c r="C93" t="n">
-        <v>7595463.263758845</v>
+        <v>-386767804.1345814</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10920,17 +10920,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>383721.7863796732</v>
+        <v>159983783.1963968</v>
       </c>
       <c r="C94" t="n">
-        <v>7591996.707043167</v>
+        <v>-389038877.5547693</v>
       </c>
       <c r="D94" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -11030,17 +11030,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>387990.2999005239</v>
+        <v>159031701.4770814</v>
       </c>
       <c r="C95" t="n">
-        <v>7595529.493387843</v>
+        <v>-387026708.7799101</v>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -11140,17 +11140,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>669452.4467849245</v>
+        <v>191708627.3984575</v>
       </c>
       <c r="C96" t="n">
-        <v>7336131.153987038</v>
+        <v>-410724560.5956822</v>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -11250,17 +11250,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>391429.212175432</v>
+        <v>164829082.7846155</v>
       </c>
       <c r="C97" t="n">
-        <v>7563757.379410667</v>
+        <v>-396448779.1607118</v>
       </c>
       <c r="D97" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -11368,17 +11368,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>569239.5613440264</v>
+        <v>191830326.5457348</v>
       </c>
       <c r="C98" t="n">
-        <v>7365353.885484916</v>
+        <v>-420857416.8751051</v>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -11482,17 +11482,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>404339.0276015802</v>
+        <v>200745874.1465958</v>
       </c>
       <c r="C99" t="n">
-        <v>7377267.93003197</v>
+        <v>-450730133.2302119</v>
       </c>
       <c r="D99" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11596,17 +11596,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>426389.9074570178</v>
+        <v>195100893.162625</v>
       </c>
       <c r="C100" t="n">
-        <v>7397057.334183707</v>
+        <v>-440230697.0622374</v>
       </c>
       <c r="D100" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11706,17 +11706,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>647260.2346404803</v>
+        <v>225334535.0004603</v>
       </c>
       <c r="C101" t="n">
-        <v>7173046.349524124</v>
+        <v>-455721416.1328683</v>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11820,17 +11820,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>422813.0446212821</v>
+        <v>170066567.4634582</v>
       </c>
       <c r="C102" t="n">
-        <v>7525418.358305623</v>
+        <v>-402058122.279879</v>
       </c>
       <c r="D102" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11934,17 +11934,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>409920.3594865833</v>
+        <v>184677066.2989198</v>
       </c>
       <c r="C103" t="n">
-        <v>7455181.222219932</v>
+        <v>-426343195.7846923</v>
       </c>
       <c r="D103" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -12052,17 +12052,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>469900.8002904762</v>
+        <v>190705854.829486</v>
       </c>
       <c r="C104" t="n">
-        <v>7403678.552845351</v>
+        <v>-429290698.053645</v>
       </c>
       <c r="D104" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -12166,17 +12166,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>464459.3821369232</v>
+        <v>173950496.5190559</v>
       </c>
       <c r="C105" t="n">
-        <v>7491066.084930793</v>
+        <v>-404282480.4928117</v>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -12280,17 +12280,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>366853.0474747586</v>
+        <v>236488082.5247939</v>
       </c>
       <c r="C106" t="n">
-        <v>7220754.392227514</v>
+        <v>-502234364.1522337</v>
       </c>
       <c r="D106" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -12394,17 +12394,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>567174.9081824664</v>
+        <v>212723687.7217174</v>
       </c>
       <c r="C107" t="n">
-        <v>7261232.535008149</v>
+        <v>-449317799.2371773</v>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -12508,17 +12508,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>397376.1849744547</v>
+        <v>169111069.225488</v>
       </c>
       <c r="C108" t="n">
-        <v>7539315.330421793</v>
+        <v>-402939472.3102995</v>
       </c>
       <c r="D108" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>747622.3765616242</v>
+        <v>198336644.9666787</v>
       </c>
       <c r="C109" t="n">
-        <v>7280326.687097363</v>
+        <v>-411866837.4992051</v>
       </c>
       <c r="D109" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12736,17 +12736,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>450489.7582604677</v>
+        <v>158546247.0333468</v>
       </c>
       <c r="C110" t="n">
-        <v>7576800.85477192</v>
+        <v>-380475198.7775751</v>
       </c>
       <c r="D110" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12854,17 +12854,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>710339.3015028904</v>
+        <v>189729394.5335976</v>
       </c>
       <c r="C111" t="n">
-        <v>7335141.778801956</v>
+        <v>-403999810.6284639</v>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12964,17 +12964,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>396053.62525233</v>
+        <v>202072665.5388272</v>
       </c>
       <c r="C112" t="n">
-        <v>7373862.411237928</v>
+        <v>-453520694.1747884</v>
       </c>
       <c r="D112" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -13074,17 +13074,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>444704.7907449754</v>
+        <v>161325373.0124752</v>
       </c>
       <c r="C113" t="n">
-        <v>7563900.888378733</v>
+        <v>-385652928.7783066</v>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -13192,17 +13192,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>443363.6732012552</v>
+        <v>161054255.9680095</v>
       </c>
       <c r="C114" t="n">
-        <v>7565788.758657504</v>
+        <v>-385324290.4075406</v>
       </c>
       <c r="D114" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -13310,17 +13310,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>367652.259629715</v>
+        <v>228912456.7268519</v>
       </c>
       <c r="C115" t="n">
-        <v>7256028.81467634</v>
+        <v>-492802897.0585838</v>
       </c>
       <c r="D115" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -13416,17 +13416,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>669640.2285336041</v>
+        <v>189903671.6324413</v>
       </c>
       <c r="C116" t="n">
-        <v>7345433.276130389</v>
+        <v>-408201000.6104372</v>
       </c>
       <c r="D116" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -13526,17 +13526,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>600557.637797766</v>
+        <v>190128098.1234068</v>
       </c>
       <c r="C117" t="n">
-        <v>7364421.865823336</v>
+        <v>-415313302.3688121</v>
       </c>
       <c r="D117" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -13644,17 +13644,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>600393.0921995796</v>
+        <v>219741114.3635682</v>
       </c>
       <c r="C118" t="n">
-        <v>7215709.499915746</v>
+        <v>-454396973.9048197</v>
       </c>
       <c r="D118" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13754,17 +13754,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>497782.9113988071</v>
+        <v>191441505.7863299</v>
       </c>
       <c r="C119" t="n">
-        <v>7390496.471405526</v>
+        <v>-427522610.3461448</v>
       </c>
       <c r="D119" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13860,17 +13860,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>436466.800330822</v>
+        <v>166744254.6523182</v>
       </c>
       <c r="C120" t="n">
-        <v>7538074.706984714</v>
+        <v>-395359670.511667</v>
       </c>
       <c r="D120" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13970,17 +13970,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>383723.7338277422</v>
+        <v>159982778.8322647</v>
       </c>
       <c r="C121" t="n">
-        <v>7592001.328981454</v>
+        <v>-389036994.0382276</v>
       </c>
       <c r="D121" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -14084,17 +14084,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>446965.5634673933</v>
+        <v>159450693.4018503</v>
       </c>
       <c r="C122" t="n">
-        <v>7573131.755081054</v>
+        <v>-382313786.5138384</v>
       </c>
       <c r="D122" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -14202,17 +14202,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>445475.1194111918</v>
+        <v>160581153.2411571</v>
       </c>
       <c r="C123" t="n">
-        <v>7567601.635024867</v>
+        <v>-384341226.8542533</v>
       </c>
       <c r="D123" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -14320,17 +14320,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>621810.8103163663</v>
+        <v>204412644.2140465</v>
       </c>
       <c r="C124" t="n">
-        <v>7285316.554902539</v>
+        <v>-432688320.1416128</v>
       </c>
       <c r="D124" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -14426,17 +14426,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>453416.9831956982</v>
+        <v>163617850.8680348</v>
       </c>
       <c r="C125" t="n">
-        <v>7548850.096561186</v>
+        <v>-388648087.9597438</v>
       </c>
       <c r="D125" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -14536,17 +14536,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>611592.6100460046</v>
+        <v>188672409.5696528</v>
       </c>
       <c r="C126" t="n">
-        <v>7368598.606297649</v>
+        <v>-412151951.1620351</v>
       </c>
       <c r="D126" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -14650,17 +14650,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>828987.291295761</v>
+        <v>180662603.712813</v>
       </c>
       <c r="C127" t="n">
-        <v>7353960.948327379</v>
+        <v>-380285375.9184469</v>
       </c>
       <c r="D127" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14768,17 +14768,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>383726.5771532588</v>
+        <v>159981312.4340496</v>
       </c>
       <c r="C128" t="n">
-        <v>7592008.077162812</v>
+        <v>-389034244.04576</v>
       </c>
       <c r="D128" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14878,17 +14878,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>572065.6433788443</v>
+        <v>190553921.2513739</v>
       </c>
       <c r="C129" t="n">
-        <v>7370981.487775771</v>
+        <v>-418754253.6420302</v>
       </c>
       <c r="D129" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14992,17 +14992,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>570671.744298632</v>
+        <v>164680010.3926166</v>
       </c>
       <c r="C130" t="n">
-        <v>7506660.864765343</v>
+        <v>-379685424.6714844</v>
       </c>
       <c r="D130" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -15106,17 +15106,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>539967.4751042218</v>
+        <v>180693895.2109168</v>
       </c>
       <c r="C131" t="n">
-        <v>7431673.784536626</v>
+        <v>-407424798.7042264</v>
       </c>
       <c r="D131" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -15220,17 +15220,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>452174.9311583586</v>
+        <v>162283396.6694638</v>
       </c>
       <c r="C132" t="n">
-        <v>7556332.266056828</v>
+        <v>-386557522.8375871</v>
       </c>
       <c r="D132" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -15334,17 +15334,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>384478.042694183</v>
+        <v>159593752.1135564</v>
       </c>
       <c r="C133" t="n">
-        <v>7593792.795184806</v>
+        <v>-388307085.0363675</v>
       </c>
       <c r="D133" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -15444,17 +15444,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>472457.6527888828</v>
+        <v>183568970.4222474</v>
       </c>
       <c r="C134" t="n">
-        <v>7438943.410384167</v>
+        <v>-418382782.426956</v>
       </c>
       <c r="D134" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -15562,17 +15562,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>796518.4161216137</v>
+        <v>193274830.4161268</v>
       </c>
       <c r="C135" t="n">
-        <v>7294240.829803186</v>
+        <v>-400423351.3916775</v>
       </c>
       <c r="D135" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -15676,17 +15676,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>439654.4736789956</v>
+        <v>169039221.4966475</v>
       </c>
       <c r="C136" t="n">
-        <v>7524984.020991635</v>
+        <v>-398792434.4795803</v>
       </c>
       <c r="D136" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -15790,17 +15790,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>597874.7966290781</v>
+        <v>187767923.9888766</v>
       </c>
       <c r="C137" t="n">
-        <v>7377365.426627968</v>
+        <v>-412204218.9547121</v>
       </c>
       <c r="D137" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15904,17 +15904,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>507905.568870945</v>
+        <v>176614885.9983608</v>
       </c>
       <c r="C138" t="n">
-        <v>7462990.403153609</v>
+        <v>-404281953.2558571</v>
       </c>
       <c r="D138" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -16014,17 +16014,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>366329.6275398433</v>
+        <v>214146793.1152762</v>
       </c>
       <c r="C139" t="n">
-        <v>7326783.189303711</v>
+        <v>-473637174.7999482</v>
       </c>
       <c r="D139" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -16128,17 +16128,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>456361.2898843428</v>
+        <v>195694588.3217317</v>
       </c>
       <c r="C140" t="n">
-        <v>7383412.108057517</v>
+        <v>-437953639.0172651</v>
       </c>
       <c r="D140" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -16238,17 +16238,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>444657.8554364101</v>
+        <v>161681400.0862358</v>
       </c>
       <c r="C141" t="n">
-        <v>7562025.921142353</v>
+        <v>-386249778.728037</v>
       </c>
       <c r="D141" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -16356,17 +16356,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>672768.4835952614</v>
+        <v>199808924.882672</v>
       </c>
       <c r="C142" t="n">
-        <v>7293509.317555598</v>
+        <v>-421352675.5362641</v>
       </c>
       <c r="D142" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>612182.4967714186</v>
+        <v>187914817.4255285</v>
       </c>
       <c r="C143" t="n">
-        <v>7372330.057555402</v>
+        <v>-411011705.6538569</v>
       </c>
       <c r="D143" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -16584,17 +16584,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>728433.5137220931</v>
+        <v>170030570.7160479</v>
       </c>
       <c r="C144" t="n">
-        <v>7435412.922395073</v>
+        <v>-373916385.7070824</v>
       </c>
       <c r="D144" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -16698,17 +16698,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>714304.8037613939</v>
+        <v>218929775.7707652</v>
       </c>
       <c r="C145" t="n">
-        <v>7184478.611043642</v>
+        <v>-440791059.8359208</v>
       </c>
       <c r="D145" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -16808,17 +16808,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>439047.5535942831</v>
+        <v>162708234.4723862</v>
       </c>
       <c r="C146" t="n">
-        <v>7558462.652592706</v>
+        <v>-388472907.154898</v>
       </c>
       <c r="D146" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16926,17 +16926,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>433932.7497139967</v>
+        <v>193098927.3384862</v>
       </c>
       <c r="C147" t="n">
-        <v>7404311.079104981</v>
+        <v>-436513085.7480596</v>
       </c>
       <c r="D147" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -17036,17 +17036,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>663250.528201481</v>
+        <v>230555666.8963441</v>
       </c>
       <c r="C148" t="n">
-        <v>7142209.795338459</v>
+        <v>-459769917.9560463</v>
       </c>
       <c r="D148" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -17150,17 +17150,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>468998.8339806726</v>
+        <v>193727869.7420573</v>
       </c>
       <c r="C149" t="n">
-        <v>7388821.772371144</v>
+        <v>-433795557.1452767</v>
       </c>
       <c r="D149" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -17260,17 +17260,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>436408.8218150658</v>
+        <v>172808170.7906583</v>
       </c>
       <c r="C150" t="n">
-        <v>7506500.594720325</v>
+        <v>-405162410.6592178</v>
       </c>
       <c r="D150" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -17370,17 +17370,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>569006.5176380178</v>
+        <v>190025554.5393861</v>
       </c>
       <c r="C151" t="n">
-        <v>7374633.408555133</v>
+        <v>-418302784.1040679</v>
       </c>
       <c r="D151" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -17484,17 +17484,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>376624.0866571964</v>
+        <v>233758818.4293233</v>
       </c>
       <c r="C152" t="n">
-        <v>7229605.106066765</v>
+        <v>-497716248.5745634</v>
       </c>
       <c r="D152" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -17590,17 +17590,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>444385.7615036962</v>
+        <v>197999048.2211913</v>
       </c>
       <c r="C153" t="n">
-        <v>7376206.848085475</v>
+        <v>-442524433.6819119</v>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -17704,17 +17704,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>431132.6180002625</v>
+        <v>170274010.9602531</v>
       </c>
       <c r="C154" t="n">
-        <v>7521465.612824399</v>
+        <v>-401599067.683601</v>
       </c>
       <c r="D154" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -17814,17 +17814,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>584961.2195156019</v>
+        <v>217091423.600224</v>
       </c>
       <c r="C155" t="n">
-        <v>7233817.372569075</v>
+        <v>-452864053.2432491</v>
       </c>
       <c r="D155" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17928,17 +17928,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>446157.5485860738</v>
+        <v>166872681.8275874</v>
       </c>
       <c r="C156" t="n">
-        <v>7534123.93820927</v>
+        <v>-394659380.2129357</v>
       </c>
       <c r="D156" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -18038,17 +18038,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>669236.5653518254</v>
+        <v>208841063.2337069</v>
       </c>
       <c r="C157" t="n">
-        <v>7248640.712909578</v>
+        <v>-433398500.873895</v>
       </c>
       <c r="D157" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -18148,17 +18148,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>777512.9831815676</v>
+        <v>191697416.7709543</v>
       </c>
       <c r="C158" t="n">
-        <v>7307313.468056051</v>
+        <v>-400171482.9756765</v>
       </c>
       <c r="D158" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -18262,17 +18262,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>435487.6637338779</v>
+        <v>163624090.056206</v>
       </c>
       <c r="C159" t="n">
-        <v>7554822.370589631</v>
+        <v>-390320148.7865415</v>
       </c>
       <c r="D159" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -18376,17 +18376,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>664861.8344592829</v>
+        <v>230432261.7004661</v>
       </c>
       <c r="C160" t="n">
-        <v>7142306.853326681</v>
+        <v>-459446216.7997958</v>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -18490,17 +18490,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>713772.8159372762</v>
+        <v>213054465.7445063</v>
       </c>
       <c r="C161" t="n">
-        <v>7214284.154764948</v>
+        <v>-433863851.7112849</v>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -18604,17 +18604,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>439805.1538512177</v>
+        <v>192706308.6065789</v>
       </c>
       <c r="C162" t="n">
-        <v>7404176.992680821</v>
+        <v>-435326852.917184</v>
       </c>
       <c r="D162" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -18718,17 +18718,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>647141.1239790823</v>
+        <v>208919250.3967201</v>
       </c>
       <c r="C163" t="n">
-        <v>7254886.228397596</v>
+        <v>-435841706.9338781</v>
       </c>
       <c r="D163" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -18828,17 +18828,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>429836.6878292271</v>
+        <v>169634345.0394309</v>
       </c>
       <c r="C164" t="n">
-        <v>7525240.43409429</v>
+        <v>-400688439.0056636</v>
       </c>
       <c r="D164" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -18938,17 +18938,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>714955.4111270539</v>
+        <v>214076451.9032896</v>
       </c>
       <c r="C165" t="n">
-        <v>7208770.172444158</v>
+        <v>-434970040.9152226</v>
       </c>
       <c r="D165" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -19052,17 +19052,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>612695.2306431417</v>
+        <v>226014241.3440962</v>
       </c>
       <c r="C166" t="n">
-        <v>7180841.293022046</v>
+        <v>-460462448.9135036</v>
       </c>
       <c r="D166" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -19162,17 +19162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>431933.0220172554</v>
+        <v>169510653.6271445</v>
       </c>
       <c r="C167" t="n">
-        <v>7525164.216234216</v>
+        <v>-400288688.0457355</v>
       </c>
       <c r="D167" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -19276,17 +19276,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>571477.7003448418</v>
+        <v>197544351.2653601</v>
       </c>
       <c r="C168" t="n">
-        <v>7335667.556724924</v>
+        <v>-428644976.7766817</v>
       </c>
       <c r="D168" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -19382,17 +19382,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>725637.832248533</v>
+        <v>225147600.0272056</v>
       </c>
       <c r="C169" t="n">
-        <v>7149922.107346477</v>
+        <v>-446621699.3602381</v>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -19496,17 +19496,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>674219.4674038889</v>
+        <v>204452339.7224762</v>
       </c>
       <c r="C170" t="n">
-        <v>7269409.352310479</v>
+        <v>-427274707.5131188</v>
       </c>
       <c r="D170" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -19606,17 +19606,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>710749.5401521167</v>
+        <v>211436154.0418527</v>
       </c>
       <c r="C171" t="n">
-        <v>7223356.075473163</v>
+        <v>-432216727.6757636</v>
       </c>
       <c r="D171" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -19716,17 +19716,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>593191.4187559042</v>
+        <v>224428130.6488923</v>
       </c>
       <c r="C172" t="n">
-        <v>7195042.290479658</v>
+        <v>-460835459.0009965</v>
       </c>
       <c r="D172" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -19830,17 +19830,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>669087.1574735446</v>
+        <v>230867323.3203529</v>
       </c>
       <c r="C173" t="n">
-        <v>7138823.143244307</v>
+        <v>-459433945.2831934</v>
       </c>
       <c r="D173" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -19944,17 +19944,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>576221.5915295435</v>
+        <v>188099519.5105205</v>
       </c>
       <c r="C174" t="n">
-        <v>7382257.330581195</v>
+        <v>-414814430.0133743</v>
       </c>
       <c r="D174" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -20058,17 +20058,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>713603.1766074058</v>
+        <v>226042122.9440573</v>
       </c>
       <c r="C175" t="n">
-        <v>7149041.025246967</v>
+        <v>-448979737.9827173</v>
       </c>
       <c r="D175" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -20168,17 +20168,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>575266.3307147442</v>
+        <v>227661733.7457307</v>
       </c>
       <c r="C176" t="n">
-        <v>7185257.558376712</v>
+        <v>-466707593.4775785</v>
       </c>
       <c r="D176" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -20274,17 +20274,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>604290.0810529721</v>
+        <v>189877414.6763963</v>
       </c>
       <c r="C177" t="n">
-        <v>7364583.701289264</v>
+        <v>-414587537.4387551</v>
       </c>
       <c r="D177" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -20384,17 +20384,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>432284.6912633065</v>
+        <v>194700531.8312197</v>
       </c>
       <c r="C178" t="n">
-        <v>7396923.161243825</v>
+        <v>-439028991.2625205</v>
       </c>
       <c r="D178" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -20498,17 +20498,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>439758.1563198671</v>
+        <v>193084589.4705866</v>
       </c>
       <c r="C179" t="n">
-        <v>7402304.535486695</v>
+        <v>-435886815.5279012</v>
       </c>
       <c r="D179" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -20612,17 +20612,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>455576.2169239347</v>
+        <v>215805372.3812869</v>
       </c>
       <c r="C180" t="n">
-        <v>7284936.716519298</v>
+        <v>-465711154.7927014</v>
       </c>
       <c r="D180" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>W</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
optimizing variogram parameters for area2
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -518,17 +518,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>105508726.4694378</v>
+        <v>170061253.5450011</v>
       </c>
       <c r="C2" t="n">
-        <v>-209018146.6045218</v>
+        <v>-402048568.8690004</v>
       </c>
       <c r="D2" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -626,17 +626,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>132646577.4596441</v>
+        <v>215751600.2529267</v>
       </c>
       <c r="C3" t="n">
-        <v>-241504486.6946509</v>
+        <v>-466156325.3815762</v>
       </c>
       <c r="D3" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -734,17 +734,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>116529554.7152026</v>
+        <v>190157095.1846463</v>
       </c>
       <c r="C4" t="n">
-        <v>-213442943.3238954</v>
+        <v>-415950649.4723316</v>
       </c>
       <c r="D4" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -846,17 +846,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>106092782.3304012</v>
+        <v>170860992.9712256</v>
       </c>
       <c r="C5" t="n">
-        <v>-210929361.0420707</v>
+        <v>-405155427.0714723</v>
       </c>
       <c r="D5" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -954,17 +954,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>105991829.6311245</v>
+        <v>170667185.431315</v>
       </c>
       <c r="C6" t="n">
-        <v>-210946344.5005981</v>
+        <v>-405104104.4883425</v>
       </c>
       <c r="D6" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1062,17 +1062,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>122395754.4997257</v>
+        <v>198148318.8949276</v>
       </c>
       <c r="C7" t="n">
-        <v>-232183773.5343286</v>
+        <v>-446478395.0038871</v>
       </c>
       <c r="D7" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1166,17 +1166,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>106102412.26284</v>
+        <v>170922082.497805</v>
       </c>
       <c r="C8" t="n">
-        <v>-210661424.2871895</v>
+        <v>-404787896.7358894</v>
       </c>
       <c r="D8" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1274,17 +1274,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>117040622.1587794</v>
+        <v>190811154.076052</v>
       </c>
       <c r="C9" t="n">
-        <v>-215321766.9774082</v>
+        <v>-418967515.8208964</v>
       </c>
       <c r="D9" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1386,17 +1386,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>103861518.1174055</v>
+        <v>167063073.7771204</v>
       </c>
       <c r="C10" t="n">
-        <v>-208247002.9008795</v>
+        <v>-399736333.0616241</v>
       </c>
       <c r="D10" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1498,17 +1498,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>117134202.8675836</v>
+        <v>191182675.188347</v>
       </c>
       <c r="C11" t="n">
-        <v>-214123845.5357292</v>
+        <v>-417313437.041097</v>
       </c>
       <c r="D11" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1606,17 +1606,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>138056256.2293121</v>
+        <v>226125332.4069945</v>
       </c>
       <c r="C12" t="n">
-        <v>-238975883.2737637</v>
+        <v>-465476449.0371869</v>
       </c>
       <c r="D12" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1710,17 +1710,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>127395291.6096901</v>
+        <v>207534924.9715279</v>
       </c>
       <c r="C13" t="n">
-        <v>-231756331.7183017</v>
+        <v>-448996303.2290542</v>
       </c>
       <c r="D13" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1810,17 +1810,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>102692553.5673765</v>
+        <v>165417181.4159042</v>
       </c>
       <c r="C14" t="n">
-        <v>-204683855.8293287</v>
+        <v>-393879767.4921157</v>
       </c>
       <c r="D14" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1918,17 +1918,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>109438266.882265</v>
+        <v>179797278.9888872</v>
       </c>
       <c r="C15" t="n">
-        <v>-195287931.0485279</v>
+        <v>-385339572.3715404</v>
       </c>
       <c r="D15" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2022,17 +2022,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>138596224.7624223</v>
+        <v>227210100.4166648</v>
       </c>
       <c r="C16" t="n">
-        <v>-238383033.7740149</v>
+        <v>-464887206.9620859</v>
       </c>
       <c r="D16" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2130,17 +2130,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>130020051.2517149</v>
+        <v>212055122.9125671</v>
       </c>
       <c r="C17" t="n">
-        <v>-234012094.1658826</v>
+        <v>-453803865.4495928</v>
       </c>
       <c r="D17" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2234,17 +2234,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>134644140.8865899</v>
+        <v>219066152.3479342</v>
       </c>
       <c r="C18" t="n">
-        <v>-243949740.2878812</v>
+        <v>-470844080.385905</v>
       </c>
       <c r="D18" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2342,17 +2342,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>139608841.0539081</v>
+        <v>229520900.4912613</v>
       </c>
       <c r="C19" t="n">
-        <v>-235476230.8749945</v>
+        <v>-461115703.439372</v>
       </c>
       <c r="D19" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2442,17 +2442,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>105596981.9961531</v>
+        <v>170189121.3721983</v>
       </c>
       <c r="C20" t="n">
-        <v>-209263009.2431625</v>
+        <v>-402456658.3516716</v>
       </c>
       <c r="D20" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2550,17 +2550,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>141599423.6154124</v>
+        <v>232646418.6580028</v>
       </c>
       <c r="C21" t="n">
-        <v>-238858232.1724758</v>
+        <v>-467100958.0807744</v>
       </c>
       <c r="D21" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2654,17 +2654,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>134875384.7845174</v>
+        <v>221685799.896555</v>
       </c>
       <c r="C22" t="n">
-        <v>-229901430.6513903</v>
+        <v>-450486429.1942855</v>
       </c>
       <c r="D22" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2754,17 +2754,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>105594822.7153038</v>
+        <v>170044434.1339617</v>
       </c>
       <c r="C23" t="n">
-        <v>-210140147.9385734</v>
+        <v>-403681533.2859867</v>
       </c>
       <c r="D23" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2854,17 +2854,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>105845394.8503075</v>
+        <v>170455328.0702242</v>
       </c>
       <c r="C24" t="n">
-        <v>-210537490.5371626</v>
+        <v>-404423592.289158</v>
       </c>
       <c r="D24" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2962,17 +2962,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>134781258.9465282</v>
+        <v>220587369.5919776</v>
       </c>
       <c r="C25" t="n">
-        <v>-235788498.9133089</v>
+        <v>-459065039.3759356</v>
       </c>
       <c r="D25" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3070,17 +3070,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>125182348.8449171</v>
+        <v>204294828.1179895</v>
       </c>
       <c r="C26" t="n">
-        <v>-226212495.6601892</v>
+        <v>-439678649.7171889</v>
       </c>
       <c r="D26" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3174,17 +3174,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>105460556.4692007</v>
+        <v>169897527.0426158</v>
       </c>
       <c r="C27" t="n">
-        <v>-209469655.8274356</v>
+        <v>-402644194.6175289</v>
       </c>
       <c r="D27" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3282,17 +3282,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>127417554.1764413</v>
+        <v>209752092.0299546</v>
       </c>
       <c r="C28" t="n">
-        <v>-218170442.130488</v>
+        <v>-429279032.9395711</v>
       </c>
       <c r="D28" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3390,17 +3390,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>110635064.8260035</v>
+        <v>181148880.3769667</v>
       </c>
       <c r="C29" t="n">
-        <v>-200693955.3049799</v>
+        <v>-393871673.9209508</v>
       </c>
       <c r="D29" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3494,17 +3494,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>136104466.1075085</v>
+        <v>223592087.1595653</v>
       </c>
       <c r="C30" t="n">
-        <v>-232184709.8015506</v>
+        <v>-454483925.6360297</v>
       </c>
       <c r="D30" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3594,17 +3594,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>134783690.3161738</v>
+        <v>220591388.8574566</v>
       </c>
       <c r="C31" t="n">
-        <v>-235791494.57205</v>
+        <v>-459070734.1471248</v>
       </c>
       <c r="D31" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3702,17 +3702,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>105451235.8885704</v>
+        <v>169837139.3715255</v>
       </c>
       <c r="C32" t="n">
-        <v>-209736329.8344363</v>
+        <v>-403010049.6333153</v>
       </c>
       <c r="D32" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3810,17 +3810,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>133553287.5962651</v>
+        <v>217075885.120332</v>
       </c>
       <c r="C33" t="n">
-        <v>-243785214.8407176</v>
+        <v>-469975118.9094672</v>
       </c>
       <c r="D33" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3914,17 +3914,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>105716464.7564075</v>
+        <v>170221339.6758617</v>
       </c>
       <c r="C34" t="n">
-        <v>-210474208.3568346</v>
+        <v>-404239109.246271</v>
       </c>
       <c r="D34" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4022,17 +4022,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>139066872.48509</v>
+        <v>228674745.6979045</v>
       </c>
       <c r="C35" t="n">
-        <v>-234520873.5788515</v>
+        <v>-459433627.7697359</v>
       </c>
       <c r="D35" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4126,17 +4126,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>138187606.9388872</v>
+        <v>226511925.3198773</v>
       </c>
       <c r="C36" t="n">
-        <v>-238041235.5106107</v>
+        <v>-464173405.9727495</v>
       </c>
       <c r="D36" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4238,17 +4238,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>111701037.9983043</v>
+        <v>182849971.5594774</v>
       </c>
       <c r="C37" t="n">
-        <v>-202577032.8259242</v>
+        <v>-397265861.4077961</v>
       </c>
       <c r="D37" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4342,17 +4342,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>113236264.3979196</v>
+        <v>185605712.1449671</v>
       </c>
       <c r="C38" t="n">
-        <v>-203448141.3676558</v>
+        <v>-399507878.409721</v>
       </c>
       <c r="D38" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4450,17 +4450,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>102773319.0900762</v>
+        <v>165158688.1655019</v>
       </c>
       <c r="C39" t="n">
-        <v>-207250826.245541</v>
+        <v>-397520250.4713072</v>
       </c>
       <c r="D39" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4562,17 +4562,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>105017672.2254655</v>
+        <v>169255388.5440889</v>
       </c>
       <c r="C40" t="n">
-        <v>-208242418.4061436</v>
+        <v>-400598228.2076799</v>
       </c>
       <c r="D40" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4674,17 +4674,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>134701314.1507206</v>
+        <v>220469595.8216356</v>
       </c>
       <c r="C41" t="n">
-        <v>-235598052.3902366</v>
+        <v>-458743532.120712</v>
       </c>
       <c r="D41" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4782,17 +4782,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>104439268.9421774</v>
+        <v>168088018.066688</v>
       </c>
       <c r="C42" t="n">
-        <v>-208685705.4748633</v>
+        <v>-400784453.2981902</v>
       </c>
       <c r="D42" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4894,17 +4894,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>104063185.0347636</v>
+        <v>167778416.8765537</v>
       </c>
       <c r="C43" t="n">
-        <v>-206174733.721487</v>
+        <v>-396994263.684976</v>
       </c>
       <c r="D43" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5002,17 +5002,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>116381563.0254742</v>
+        <v>189893264.5149418</v>
       </c>
       <c r="C44" t="n">
-        <v>-213354002.2535594</v>
+        <v>-415728052.2039195</v>
       </c>
       <c r="D44" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5114,17 +5114,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>100167826.3336622</v>
+        <v>161294915.6318805</v>
       </c>
       <c r="C45" t="n">
-        <v>-200491735.4238619</v>
+        <v>-386106025.2255547</v>
       </c>
       <c r="D45" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5226,17 +5226,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>106181608.3227286</v>
+        <v>170989661.2193642</v>
       </c>
       <c r="C46" t="n">
-        <v>-211176252.3923558</v>
+        <v>-405566621.7426242</v>
       </c>
       <c r="D46" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5330,17 +5330,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>104367728.3348256</v>
+        <v>167842617.8236445</v>
       </c>
       <c r="C47" t="n">
-        <v>-209373254.1300425</v>
+        <v>-401689953.4288404</v>
       </c>
       <c r="D47" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5442,17 +5442,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>104424001.3408905</v>
+        <v>168348387.5857986</v>
       </c>
       <c r="C48" t="n">
-        <v>-206884594.4189475</v>
+        <v>-398256561.2255399</v>
       </c>
       <c r="D48" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5550,17 +5550,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>137283281.5320168</v>
+        <v>225037801.297646</v>
       </c>
       <c r="C49" t="n">
-        <v>-236821997.8006023</v>
+        <v>-461912078.2331657</v>
       </c>
       <c r="D49" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5658,17 +5658,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>106000975.046599</v>
+        <v>170869051.6025432</v>
       </c>
       <c r="C50" t="n">
-        <v>-209794092.8900959</v>
+        <v>-403499299.370443</v>
       </c>
       <c r="D50" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5762,17 +5762,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>117159326.3814496</v>
+        <v>193017470.4955127</v>
       </c>
       <c r="C51" t="n">
-        <v>-203346207.1822138</v>
+        <v>-401785101.312815</v>
       </c>
       <c r="D51" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5870,17 +5870,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>123465584.6433238</v>
+        <v>199949949.5776266</v>
       </c>
       <c r="C52" t="n">
-        <v>-233430269.622158</v>
+        <v>-448945059.420067</v>
       </c>
       <c r="D52" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -5974,17 +5974,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>130665300.368854</v>
+        <v>212560183.8336233</v>
       </c>
       <c r="C53" t="n">
-        <v>-238428189.4724956</v>
+        <v>-460556023.6364397</v>
       </c>
       <c r="D53" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6082,17 +6082,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>100367178.8657337</v>
+        <v>161676484.2880752</v>
       </c>
       <c r="C54" t="n">
-        <v>-200478489.6620883</v>
+        <v>-386240761.038307</v>
       </c>
       <c r="D54" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6194,17 +6194,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>105352880.5020434</v>
+        <v>169788566.1146641</v>
       </c>
       <c r="C55" t="n">
-        <v>-208877513.5332501</v>
+        <v>-401736005.8829324</v>
       </c>
       <c r="D55" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6302,17 +6302,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>129647122.8856552</v>
+        <v>211508905.0259657</v>
       </c>
       <c r="C56" t="n">
-        <v>-233086310.6818279</v>
+        <v>-452247932.9809692</v>
       </c>
       <c r="D56" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6406,17 +6406,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>99652515.60497172</v>
+        <v>159944451.6321533</v>
       </c>
       <c r="C57" t="n">
-        <v>-202793563.913616</v>
+        <v>-388908680.488093</v>
       </c>
       <c r="D57" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6510,17 +6510,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>124626453.9291485</v>
+        <v>201934275.4551795</v>
       </c>
       <c r="C58" t="n">
-        <v>-234583616.9577389</v>
+        <v>-451332610.6898304</v>
       </c>
       <c r="D58" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6614,17 +6614,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>112672866.8429443</v>
+        <v>184732978.0088556</v>
       </c>
       <c r="C59" t="n">
-        <v>-202306174.8753476</v>
+        <v>-397506742.2204202</v>
       </c>
       <c r="D59" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -6722,17 +6722,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>120818759.6407465</v>
+        <v>195705534.4388087</v>
       </c>
       <c r="C60" t="n">
-        <v>-228976588.5435393</v>
+        <v>-440888996.2268443</v>
       </c>
       <c r="D60" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -6826,17 +6826,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>136059248.6204675</v>
+        <v>220534136.2407041</v>
       </c>
       <c r="C61" t="n">
-        <v>-251416086.562739</v>
+        <v>-482430540.6605094</v>
       </c>
       <c r="D61" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -6930,17 +6930,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>137281823.6174914</v>
+        <v>225035389.0068487</v>
       </c>
       <c r="C62" t="n">
-        <v>-236820256.6947784</v>
+        <v>-461908760.2337005</v>
       </c>
       <c r="D62" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7038,17 +7038,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>111557958.197442</v>
+        <v>183320051.9313003</v>
       </c>
       <c r="C63" t="n">
-        <v>-198188443.8184662</v>
+        <v>-390873338.4612513</v>
       </c>
       <c r="D63" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7146,17 +7146,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>122342850.5698752</v>
+        <v>198119290.4729356</v>
       </c>
       <c r="C64" t="n">
-        <v>-231739329.838951</v>
+        <v>-445812024.3581349</v>
       </c>
       <c r="D64" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7258,17 +7258,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>113504335.765346</v>
+        <v>183136998.266023</v>
       </c>
       <c r="C65" t="n">
-        <v>-221679853.6071709</v>
+        <v>-425597138.2776437</v>
       </c>
       <c r="D65" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7366,17 +7366,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>117746875.3597333</v>
+        <v>194155942.949601</v>
       </c>
       <c r="C66" t="n">
-        <v>-203145161.1829448</v>
+        <v>-401840817.6504443</v>
       </c>
       <c r="D66" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7474,17 +7474,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>123466691.2825127</v>
+        <v>199951766.5902286</v>
       </c>
       <c r="C67" t="n">
-        <v>-233431851.2426446</v>
+        <v>-448948024.5963792</v>
       </c>
       <c r="D67" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7582,17 +7582,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>110571376.8817002</v>
+        <v>181191745.9251307</v>
       </c>
       <c r="C68" t="n">
-        <v>-199724522.8641171</v>
+        <v>-392441938.8805223</v>
       </c>
       <c r="D68" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -7690,17 +7690,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>110055601.0016471</v>
+        <v>181465006.6044621</v>
       </c>
       <c r="C69" t="n">
-        <v>-192394145.9747593</v>
+        <v>-381565732.0586818</v>
       </c>
       <c r="D69" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -7798,17 +7798,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>115877033.3297141</v>
+        <v>190126419.3274445</v>
       </c>
       <c r="C70" t="n">
-        <v>-206198179.3881435</v>
+        <v>-405131540.1544722</v>
       </c>
       <c r="D70" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -7902,17 +7902,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>130111079.5130356</v>
+        <v>213293560.7974027</v>
       </c>
       <c r="C71" t="n">
-        <v>-227255961.6400539</v>
+        <v>-444046630.9603429</v>
       </c>
       <c r="D71" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8006,17 +8006,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>105598637.6146314</v>
+        <v>170191838.1157665</v>
       </c>
       <c r="C72" t="n">
-        <v>-209265622.4662407</v>
+        <v>-402461543.5417274</v>
       </c>
       <c r="D72" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8114,17 +8114,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>134781913.8277764</v>
+        <v>220588452.1677152</v>
       </c>
       <c r="C73" t="n">
-        <v>-235789305.7885106</v>
+        <v>-459066573.2519769</v>
       </c>
       <c r="D73" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8222,17 +8222,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>120457917.0446891</v>
+        <v>195997045.5293688</v>
       </c>
       <c r="C74" t="n">
-        <v>-222901472.9667384</v>
+        <v>-431996651.364231</v>
       </c>
       <c r="D74" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>104656956.3492973</v>
+        <v>168450500.9432539</v>
       </c>
       <c r="C75" t="n">
-        <v>-208998483.7739748</v>
+        <v>-401384793.0106061</v>
       </c>
       <c r="D75" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8438,17 +8438,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>140447377.957341</v>
+        <v>230175350.2550632</v>
       </c>
       <c r="C76" t="n">
-        <v>-241190465.6660586</v>
+        <v>-469965199.3425449</v>
       </c>
       <c r="D76" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -8546,17 +8546,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>127382852.6466472</v>
+        <v>208808591.8167622</v>
       </c>
       <c r="C77" t="n">
-        <v>-223616842.4244619</v>
+        <v>-437210044.3358359</v>
       </c>
       <c r="D77" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -8654,17 +8654,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>106918502.4314488</v>
+        <v>175243179.3873374</v>
       </c>
       <c r="C78" t="n">
-        <v>-193926183.2665913</v>
+        <v>-381724269.4209624</v>
       </c>
       <c r="D78" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -8762,17 +8762,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>99678515.17212091</v>
+        <v>159981689.5436021</v>
       </c>
       <c r="C79" t="n">
-        <v>-202869844.3416095</v>
+        <v>-389034951.2546384</v>
       </c>
       <c r="D79" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -8870,17 +8870,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>124630512.6759802</v>
+        <v>201940941.1117887</v>
       </c>
       <c r="C80" t="n">
-        <v>-234589366.480262</v>
+        <v>-451343395.5166952</v>
       </c>
       <c r="D80" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -8974,17 +8974,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>122906404.1367475</v>
+        <v>199038252.9463307</v>
       </c>
       <c r="C81" t="n">
-        <v>-232588847.2752898</v>
+        <v>-447386185.6953286</v>
       </c>
       <c r="D81" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9082,17 +9082,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>123834612.5745275</v>
+        <v>200536386.0293367</v>
       </c>
       <c r="C82" t="n">
-        <v>-234081588.0408616</v>
+        <v>-450110034.1736351</v>
       </c>
       <c r="D82" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9190,17 +9190,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>125024745.8866452</v>
+        <v>205759380.4885022</v>
       </c>
       <c r="C83" t="n">
-        <v>-215332164.6101156</v>
+        <v>-423798822.2369605</v>
       </c>
       <c r="D83" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9294,17 +9294,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>114770796.1817679</v>
+        <v>189088595.2522518</v>
       </c>
       <c r="C84" t="n">
-        <v>-199968539.1906832</v>
+        <v>-395445249.0775359</v>
       </c>
       <c r="D84" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9398,17 +9398,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>136399735.7707716</v>
+        <v>223641556.3890886</v>
       </c>
       <c r="C85" t="n">
-        <v>-235342743.6443977</v>
+        <v>-459278078.5597609</v>
       </c>
       <c r="D85" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -9502,17 +9502,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>124134250.592144</v>
+        <v>201021809.2568428</v>
       </c>
       <c r="C86" t="n">
-        <v>-234550627.4243446</v>
+        <v>-450970544.5014009</v>
       </c>
       <c r="D86" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -9610,17 +9610,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>109970644.6036005</v>
+        <v>180714862.6879153</v>
       </c>
       <c r="C87" t="n">
-        <v>-195827838.7745652</v>
+        <v>-386459896.4466831</v>
       </c>
       <c r="D87" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -9718,17 +9718,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>118735399.5336341</v>
+        <v>192332759.4216259</v>
       </c>
       <c r="C88" t="n">
-        <v>-225639454.349205</v>
+        <v>-434773788.9701531</v>
       </c>
       <c r="D88" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -9822,17 +9822,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>99948772.93257391</v>
+        <v>160418897.5706784</v>
       </c>
       <c r="C89" t="n">
-        <v>-203348593.3003232</v>
+        <v>-389911002.6655887</v>
       </c>
       <c r="D89" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -9926,17 +9926,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>113568385.9032365</v>
+        <v>183326049.5143205</v>
       </c>
       <c r="C90" t="n">
-        <v>-221247347.6185689</v>
+        <v>-425033345.1795313</v>
       </c>
       <c r="D90" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10034,17 +10034,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>99680708.61797616</v>
+        <v>159985281.4310923</v>
       </c>
       <c r="C91" t="n">
-        <v>-202873459.8895674</v>
+        <v>-389041687.233989</v>
       </c>
       <c r="D91" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10146,17 +10146,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>110142394.5216578</v>
+        <v>178908355.1332637</v>
       </c>
       <c r="C92" t="n">
-        <v>-208562628.9073775</v>
+        <v>-404735969.3286093</v>
       </c>
       <c r="D92" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10254,17 +10254,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>99031260.30550426</v>
+        <v>158953626.7530148</v>
       </c>
       <c r="C93" t="n">
-        <v>-201602192.2960845</v>
+        <v>-386767804.1345814</v>
       </c>
       <c r="D93" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10358,17 +10358,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>99679793.69599606</v>
+        <v>159983783.1963968</v>
       </c>
       <c r="C94" t="n">
-        <v>-202871951.7895998</v>
+        <v>-389038877.5547693</v>
       </c>
       <c r="D94" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -10462,17 +10462,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>99085419.68022577</v>
+        <v>159031701.4770814</v>
       </c>
       <c r="C95" t="n">
-        <v>-201758063.0948648</v>
+        <v>-387026708.7799101</v>
       </c>
       <c r="D95" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -10566,17 +10566,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>117016909.536118</v>
+        <v>191708627.3984575</v>
       </c>
       <c r="C96" t="n">
-        <v>-209587252.9708545</v>
+        <v>-410724560.5956822</v>
       </c>
       <c r="D96" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -10670,17 +10670,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>102545355.9689802</v>
+        <v>164829082.7846155</v>
       </c>
       <c r="C97" t="n">
-        <v>-206606667.7502118</v>
+        <v>-396448779.1607118</v>
       </c>
       <c r="D97" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -10782,17 +10782,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>117672836.3618993</v>
+        <v>191830326.5457348</v>
       </c>
       <c r="C98" t="n">
-        <v>-216358649.6340961</v>
+        <v>-420857416.8751051</v>
       </c>
       <c r="D98" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -10890,17 +10890,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>123978034.8062271</v>
+        <v>200745874.1465958</v>
       </c>
       <c r="C99" t="n">
-        <v>-234452325.5146987</v>
+        <v>-450730133.2302119</v>
       </c>
       <c r="D99" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -10998,17 +10998,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>120470081.3920262</v>
+        <v>195100893.162625</v>
       </c>
       <c r="C100" t="n">
-        <v>-228674520.3612784</v>
+        <v>-440230697.0622374</v>
       </c>
       <c r="D100" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11102,17 +11102,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>137093107.2131552</v>
+        <v>225334535.0004603</v>
       </c>
       <c r="C101" t="n">
-        <v>-232680201.6958987</v>
+        <v>-455721416.1328683</v>
       </c>
       <c r="D101" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11210,17 +11210,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>105511964.562603</v>
+        <v>170066567.4634582</v>
       </c>
       <c r="C102" t="n">
-        <v>-209023256.3673792</v>
+        <v>-402058122.279879</v>
       </c>
       <c r="D102" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11318,17 +11318,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>114333012.3162275</v>
+        <v>184677066.2989198</v>
       </c>
       <c r="C103" t="n">
-        <v>-221797612.6148877</v>
+        <v>-426343195.7846923</v>
       </c>
       <c r="D103" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -11430,17 +11430,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>117585726.1880774</v>
+        <v>190705854.829486</v>
       </c>
       <c r="C104" t="n">
-        <v>-222315825.1105521</v>
+        <v>-429290698.053645</v>
       </c>
       <c r="D104" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -11538,17 +11538,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>107604625.910323</v>
+        <v>173950496.5190559</v>
       </c>
       <c r="C105" t="n">
-        <v>-209515713.5931183</v>
+        <v>-404282480.4928117</v>
       </c>
       <c r="D105" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -11646,17 +11646,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>145569466.401966</v>
+        <v>236488082.5247939</v>
       </c>
       <c r="C106" t="n">
-        <v>-261425231.6330547</v>
+        <v>-502234364.1522337</v>
       </c>
       <c r="D106" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -11754,17 +11754,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>130113878.5378258</v>
+        <v>212723687.7217174</v>
       </c>
       <c r="C107" t="n">
-        <v>-230877998.5930108</v>
+        <v>-449317799.2371773</v>
       </c>
       <c r="D107" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -11862,17 +11862,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>105080389.1113953</v>
+        <v>169111069.225488</v>
       </c>
       <c r="C108" t="n">
-        <v>-209884292.3578205</v>
+        <v>-402939472.3102995</v>
       </c>
       <c r="D108" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -11970,17 +11970,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>120489265.4427217</v>
+        <v>198336644.9666787</v>
       </c>
       <c r="C109" t="n">
-        <v>-208929469.54725</v>
+        <v>-411866837.4992051</v>
       </c>
       <c r="D109" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12078,17 +12078,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>98461024.83522852</v>
+        <v>158546247.0333468</v>
       </c>
       <c r="C110" t="n">
-        <v>-197396514.180316</v>
+        <v>-380475198.7775751</v>
       </c>
       <c r="D110" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12190,17 +12190,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>115607022.0688982</v>
+        <v>189729394.5335976</v>
       </c>
       <c r="C111" t="n">
-        <v>-205529791.2928719</v>
+        <v>-403999810.6284639</v>
       </c>
       <c r="D111" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12294,17 +12294,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>124822083.9285265</v>
+        <v>202072665.5388272</v>
       </c>
       <c r="C112" t="n">
-        <v>-236031568.2958097</v>
+        <v>-453520694.1747884</v>
       </c>
       <c r="D112" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -12398,17 +12398,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>100156661.0837503</v>
+        <v>161325373.0124752</v>
       </c>
       <c r="C113" t="n">
-        <v>-200172776.0156584</v>
+        <v>-385652928.7783066</v>
       </c>
       <c r="D113" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -12510,17 +12510,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>100001447.5327858</v>
+        <v>161054255.9680095</v>
       </c>
       <c r="C114" t="n">
-        <v>-200022630.0171967</v>
+        <v>-385324290.4075406</v>
       </c>
       <c r="D114" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>141041486.155849</v>
+        <v>228912456.7268519</v>
       </c>
       <c r="C115" t="n">
-        <v>-256629137.1601039</v>
+        <v>-492802897.0585838</v>
       </c>
       <c r="D115" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -12722,17 +12722,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>115944493.4328775</v>
+        <v>189903671.6324413</v>
       </c>
       <c r="C116" t="n">
-        <v>-208300507.8710816</v>
+        <v>-408201000.6104372</v>
       </c>
       <c r="D116" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -12826,17 +12826,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>116477400.184276</v>
+        <v>190128098.1234068</v>
       </c>
       <c r="C117" t="n">
-        <v>-213021100.7277543</v>
+        <v>-415313302.3688121</v>
       </c>
       <c r="D117" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -12938,17 +12938,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>134073855.6473529</v>
+        <v>219741114.3635682</v>
       </c>
       <c r="C118" t="n">
-        <v>-232856329.5791467</v>
+        <v>-454396973.9048197</v>
       </c>
       <c r="D118" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13042,17 +13042,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>117860571.0843874</v>
+        <v>191441505.7863299</v>
       </c>
       <c r="C119" t="n">
-        <v>-220944422.1572055</v>
+        <v>-427522610.3461448</v>
       </c>
       <c r="D119" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13142,17 +13142,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>103446922.0606982</v>
+        <v>166744254.6523182</v>
       </c>
       <c r="C120" t="n">
-        <v>-205335959.0468844</v>
+        <v>-395359670.511667</v>
       </c>
       <c r="D120" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13246,17 +13246,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>99679180.36433366</v>
+        <v>159982778.8322647</v>
       </c>
       <c r="C121" t="n">
-        <v>-202870940.8090142</v>
+        <v>-389036994.0382276</v>
       </c>
       <c r="D121" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -13354,17 +13354,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>99021577.51894188</v>
+        <v>159450693.4018503</v>
       </c>
       <c r="C122" t="n">
-        <v>-198404658.9435754</v>
+        <v>-382313786.5138384</v>
       </c>
       <c r="D122" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -13466,17 +13466,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>99706732.31271403</v>
+        <v>160581153.2411571</v>
       </c>
       <c r="C123" t="n">
-        <v>-199480058.8985869</v>
+        <v>-384341226.8542533</v>
       </c>
       <c r="D123" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -13578,17 +13578,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>124840981.4588256</v>
+        <v>204412644.2140465</v>
       </c>
       <c r="C124" t="n">
-        <v>-221515326.7091922</v>
+        <v>-432688320.1416128</v>
       </c>
       <c r="D124" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -13678,17 +13678,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>101482637.130122</v>
+        <v>163617850.8680348</v>
       </c>
       <c r="C125" t="n">
-        <v>-201593533.2296944</v>
+        <v>-388648087.9597438</v>
       </c>
       <c r="D125" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -13782,17 +13782,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>115547775.5122885</v>
+        <v>188672409.5696528</v>
       </c>
       <c r="C126" t="n">
-        <v>-211230821.352387</v>
+        <v>-412151951.1620351</v>
       </c>
       <c r="D126" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -13890,17 +13890,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>109571273.3401862</v>
+        <v>180662603.712813</v>
       </c>
       <c r="C127" t="n">
-        <v>-191719277.4940407</v>
+        <v>-380285375.9184469</v>
       </c>
       <c r="D127" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14002,17 +14002,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>99678284.8839162</v>
+        <v>159981312.4340496</v>
       </c>
       <c r="C128" t="n">
-        <v>-202869464.7461046</v>
+        <v>-389034244.04576</v>
       </c>
       <c r="D128" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14106,17 +14106,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>116896498.8276936</v>
+        <v>190553921.2513739</v>
       </c>
       <c r="C129" t="n">
-        <v>-215237703.2306432</v>
+        <v>-418754253.6420302</v>
       </c>
       <c r="D129" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14214,17 +14214,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>101486613.3077085</v>
+        <v>164680010.3926166</v>
       </c>
       <c r="C130" t="n">
-        <v>-195192346.6161174</v>
+        <v>-379685424.6714844</v>
       </c>
       <c r="D130" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -14322,17 +14322,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>111206429.3717718</v>
+        <v>180693895.2109168</v>
       </c>
       <c r="C131" t="n">
-        <v>-209942642.4337206</v>
+        <v>-407424798.7042264</v>
       </c>
       <c r="D131" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -14430,17 +14430,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>100690301.4471169</v>
+        <v>162283396.6694638</v>
       </c>
       <c r="C132" t="n">
-        <v>-200528169.7813111</v>
+        <v>-386557522.8375871</v>
       </c>
       <c r="D132" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -14538,17 +14538,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>99441616.50272426</v>
+        <v>159593752.1135564</v>
       </c>
       <c r="C133" t="n">
-        <v>-202479162.9386826</v>
+        <v>-388307085.0363675</v>
       </c>
       <c r="D133" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -14642,17 +14642,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>113308239.1278594</v>
+        <v>183568970.4222474</v>
       </c>
       <c r="C134" t="n">
-        <v>-216662236.3820526</v>
+        <v>-418382782.426956</v>
       </c>
       <c r="D134" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -14754,17 +14754,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>117210532.9378552</v>
+        <v>193274830.4161268</v>
       </c>
       <c r="C135" t="n">
-        <v>-202388640.3289137</v>
+        <v>-400423351.3916775</v>
       </c>
       <c r="D135" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -14862,17 +14862,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>104803634.4021675</v>
+        <v>169039221.4966475</v>
       </c>
       <c r="C136" t="n">
-        <v>-207065422.8186131</v>
+        <v>-398792434.4795803</v>
       </c>
       <c r="D136" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -14970,17 +14970,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>115088902.8054884</v>
+        <v>187767923.9888766</v>
       </c>
       <c r="C137" t="n">
-        <v>-211475437.8546615</v>
+        <v>-412204218.9547121</v>
       </c>
       <c r="D137" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15078,17 +15078,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>108953363.5511799</v>
+        <v>176614885.9983608</v>
       </c>
       <c r="C138" t="n">
-        <v>-208830389.1402352</v>
+        <v>-404281953.2558571</v>
       </c>
       <c r="D138" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -15182,17 +15182,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>132227328.7373793</v>
+        <v>214146793.1152762</v>
       </c>
       <c r="C139" t="n">
-        <v>-246882657.1680205</v>
+        <v>-473637174.7999482</v>
       </c>
       <c r="D139" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -15290,17 +15290,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>120645077.3307229</v>
+        <v>195694588.3217317</v>
       </c>
       <c r="C140" t="n">
-        <v>-226992646.1945517</v>
+        <v>-437953639.0172651</v>
       </c>
       <c r="D140" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -15394,17 +15394,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>100370172.5250075</v>
+        <v>161681400.0862358</v>
       </c>
       <c r="C141" t="n">
-        <v>-200483310.2279336</v>
+        <v>-386249778.728037</v>
       </c>
       <c r="D141" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -15506,17 +15506,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>121803530.9674991</v>
+        <v>199808924.882672</v>
       </c>
       <c r="C142" t="n">
-        <v>-214929262.2081245</v>
+        <v>-421352675.5362641</v>
       </c>
       <c r="D142" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -15610,17 +15610,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>115093850.2074087</v>
+        <v>187914817.4255285</v>
       </c>
       <c r="C143" t="n">
-        <v>-210639130.9912758</v>
+        <v>-411011705.6538569</v>
       </c>
       <c r="D143" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -15722,17 +15722,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>103822953.4520017</v>
+        <v>170030570.7160479</v>
       </c>
       <c r="C144" t="n">
-        <v>-189930731.702317</v>
+        <v>-373916385.7070824</v>
       </c>
       <c r="D144" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -15830,17 +15830,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>132877443.62134</v>
+        <v>218929775.7707652</v>
       </c>
       <c r="C145" t="n">
-        <v>-224023748.5784365</v>
+        <v>-440791059.8359208</v>
       </c>
       <c r="D145" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -15934,17 +15934,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>101015466.2542255</v>
+        <v>162708234.4723862</v>
       </c>
       <c r="C146" t="n">
-        <v>-201723206.6404476</v>
+        <v>-388472907.154898</v>
       </c>
       <c r="D146" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16046,17 +16046,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>119228449.4292004</v>
+        <v>193098927.3384862</v>
       </c>
       <c r="C147" t="n">
-        <v>-226634202.4660612</v>
+        <v>-436513085.7480596</v>
       </c>
       <c r="D147" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -16150,17 +16150,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>140082692.4468106</v>
+        <v>230555666.8963441</v>
       </c>
       <c r="C148" t="n">
-        <v>-234409595.1433657</v>
+        <v>-459769917.9560463</v>
       </c>
       <c r="D148" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -16258,17 +16258,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>119395384.9325225</v>
+        <v>193727869.7420573</v>
       </c>
       <c r="C149" t="n">
-        <v>-224644429.6894445</v>
+        <v>-433795557.1452767</v>
       </c>
       <c r="D149" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -16362,17 +16362,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>107077921.004971</v>
+        <v>172808170.7906583</v>
       </c>
       <c r="C150" t="n">
-        <v>-210415575.5129712</v>
+        <v>-405162410.6592178</v>
       </c>
       <c r="D150" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>116599761.8003678</v>
+        <v>190025554.5393861</v>
       </c>
       <c r="C151" t="n">
-        <v>-215056264.1719109</v>
+        <v>-418302784.1040679</v>
       </c>
       <c r="D151" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -16574,17 +16574,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>143874749.0634952</v>
+        <v>233758818.4293233</v>
       </c>
       <c r="C152" t="n">
-        <v>-258943761.0773299</v>
+        <v>-497716248.5745634</v>
       </c>
       <c r="D152" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -16674,17 +16674,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>122093307.7635642</v>
+        <v>197999048.2211913</v>
       </c>
       <c r="C153" t="n">
-        <v>-229543200.8580566</v>
+        <v>-442524433.6819119</v>
       </c>
       <c r="D153" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -16782,17 +16782,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>105590085.9079321</v>
+        <v>170274010.9602531</v>
       </c>
       <c r="C154" t="n">
-        <v>-208653782.3603525</v>
+        <v>-401599067.683601</v>
       </c>
       <c r="D154" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -16886,17 +16886,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>132597887.1665408</v>
+        <v>217091423.600224</v>
       </c>
       <c r="C155" t="n">
-        <v>-232357831.3243726</v>
+        <v>-452864053.2432491</v>
       </c>
       <c r="D155" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -16994,17 +16994,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>103470805.8748131</v>
+        <v>166872681.8275874</v>
       </c>
       <c r="C156" t="n">
-        <v>-204822101.9525426</v>
+        <v>-394659380.2129357</v>
       </c>
       <c r="D156" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -17098,17 +17098,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>127180613.9277396</v>
+        <v>208841063.2337069</v>
       </c>
       <c r="C157" t="n">
-        <v>-221078511.4456128</v>
+        <v>-433398500.873895</v>
       </c>
       <c r="D157" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -17202,17 +17202,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>116386930.9560903</v>
+        <v>191697416.7709543</v>
       </c>
       <c r="C158" t="n">
-        <v>-202553336.0838474</v>
+        <v>-400171482.9756765</v>
       </c>
       <c r="D158" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -17310,17 +17310,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>101583352.7685994</v>
+        <v>163624090.056206</v>
       </c>
       <c r="C159" t="n">
-        <v>-202736787.3699743</v>
+        <v>-390320148.7865415</v>
       </c>
       <c r="D159" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -17418,17 +17418,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>139999211.642137</v>
+        <v>230432261.7004661</v>
       </c>
       <c r="C160" t="n">
-        <v>-234218738.9120067</v>
+        <v>-459446216.7997958</v>
       </c>
       <c r="D160" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -17526,17 +17526,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>129403918.6188121</v>
+        <v>213054465.7445063</v>
       </c>
       <c r="C161" t="n">
-        <v>-220561130.1128934</v>
+        <v>-433863851.7112849</v>
       </c>
       <c r="D161" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -17634,17 +17634,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>118958854.6132308</v>
+        <v>192706308.6065789</v>
       </c>
       <c r="C162" t="n">
-        <v>-225924513.2256453</v>
+        <v>-435326852.917184</v>
       </c>
       <c r="D162" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -17742,17 +17742,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>127361799.8553083</v>
+        <v>208919250.3967201</v>
       </c>
       <c r="C163" t="n">
-        <v>-222684836.8283646</v>
+        <v>-435841706.9338781</v>
       </c>
       <c r="D163" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -17846,17 +17846,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>105214205.3888756</v>
+        <v>169634345.0394309</v>
       </c>
       <c r="C164" t="n">
-        <v>-208202346.972273</v>
+        <v>-400688439.0056636</v>
       </c>
       <c r="D164" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -17950,17 +17950,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>130001514.6469524</v>
+        <v>214076451.9032896</v>
       </c>
       <c r="C165" t="n">
-        <v>-221096251.1072609</v>
+        <v>-434970040.9152226</v>
       </c>
       <c r="D165" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -18058,17 +18058,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>137717459.0523186</v>
+        <v>226014241.3440962</v>
       </c>
       <c r="C166" t="n">
-        <v>-235681984.5561872</v>
+        <v>-460462448.9135036</v>
       </c>
       <c r="D166" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -18162,17 +18162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>105128541.7492181</v>
+        <v>169510653.6271445</v>
       </c>
       <c r="C167" t="n">
-        <v>-207962133.4922707</v>
+        <v>-400288688.0457355</v>
       </c>
       <c r="D167" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -18270,17 +18270,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>121060300.4620544</v>
+        <v>197544351.2653601</v>
       </c>
       <c r="C168" t="n">
-        <v>-220297557.7979507</v>
+        <v>-428644976.7766817</v>
       </c>
       <c r="D168" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -18370,17 +18370,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>136483512.4430443</v>
+        <v>225147600.0272056</v>
       </c>
       <c r="C169" t="n">
-        <v>-226734556.8126839</v>
+        <v>-446621699.3602381</v>
       </c>
       <c r="D169" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -18478,17 +18478,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>124548501.1505335</v>
+        <v>204452339.7224762</v>
       </c>
       <c r="C170" t="n">
-        <v>-217902651.7519901</v>
+        <v>-427274707.5131188</v>
       </c>
       <c r="D170" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -18582,17 +18582,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>128464498.0296568</v>
+        <v>211436154.0418527</v>
       </c>
       <c r="C171" t="n">
-        <v>-219784764.8501419</v>
+        <v>-432216727.6757636</v>
       </c>
       <c r="D171" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -18686,17 +18686,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>136901542.6570788</v>
+        <v>224428130.6488923</v>
       </c>
       <c r="C172" t="n">
-        <v>-236224593.5605564</v>
+        <v>-460835459.0009965</v>
       </c>
       <c r="D172" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -18794,17 +18794,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>140229425.9082486</v>
+        <v>230867323.3203529</v>
       </c>
       <c r="C173" t="n">
-        <v>-234134835.1599286</v>
+        <v>-459433945.2831934</v>
       </c>
       <c r="D173" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -18902,17 +18902,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>115411245.186507</v>
+        <v>188099519.5105205</v>
       </c>
       <c r="C174" t="n">
-        <v>-213155727.6359349</v>
+        <v>-414814430.0133743</v>
       </c>
       <c r="D174" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -19010,17 +19010,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>137088898.2118142</v>
+        <v>226042122.9440573</v>
       </c>
       <c r="C175" t="n">
-        <v>-228123017.841619</v>
+        <v>-448979737.9827173</v>
       </c>
       <c r="D175" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -19114,17 +19114,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>138936348.0628513</v>
+        <v>227661733.7457307</v>
       </c>
       <c r="C176" t="n">
-        <v>-239502436.3370571</v>
+        <v>-466707593.4775785</v>
       </c>
       <c r="D176" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -19214,17 +19214,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>116306647.5220219</v>
+        <v>189877414.6763963</v>
       </c>
       <c r="C177" t="n">
-        <v>-212590809.3727053</v>
+        <v>-414587537.4387551</v>
       </c>
       <c r="D177" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -19318,17 +19318,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>120195467.8391005</v>
+        <v>194700531.8312197</v>
       </c>
       <c r="C178" t="n">
-        <v>-227955826.4722086</v>
+        <v>-439028991.2625205</v>
       </c>
       <c r="D178" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -19426,17 +19426,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>119185180.0915828</v>
+        <v>193084589.4705866</v>
       </c>
       <c r="C179" t="n">
-        <v>-226213221.2188751</v>
+        <v>-435886815.5279012</v>
       </c>
       <c r="D179" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -19534,17 +19534,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>132649677.9409595</v>
+        <v>215805372.3812869</v>
       </c>
       <c r="C180" t="n">
-        <v>-241194673.5050797</v>
+        <v>-465711154.7927014</v>
       </c>
       <c r="D180" t="n">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>T</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
optimizing variogram parameters area3
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -964,7 +964,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1072,7 +1072,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1284,7 +1284,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1820,7 +1820,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1928,7 +1928,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2244,7 +2244,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2764,7 +2764,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2864,7 +2864,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2972,7 +2972,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3080,7 +3080,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3184,7 +3184,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3400,7 +3400,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3504,7 +3504,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3924,7 +3924,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4032,7 +4032,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4136,7 +4136,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4248,7 +4248,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4352,7 +4352,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4460,7 +4460,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4572,7 +4572,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4684,7 +4684,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4792,7 +4792,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4904,7 +4904,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5012,7 +5012,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5124,7 +5124,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5236,7 +5236,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5340,7 +5340,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5452,7 +5452,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5560,7 +5560,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5668,7 +5668,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5772,7 +5772,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5880,7 +5880,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -5984,7 +5984,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6092,7 +6092,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6204,7 +6204,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6312,7 +6312,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6520,7 +6520,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6624,7 +6624,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -6732,7 +6732,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -6836,7 +6836,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -6940,7 +6940,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7048,7 +7048,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7156,7 +7156,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7268,7 +7268,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7376,7 +7376,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7484,7 +7484,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7592,7 +7592,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -7700,7 +7700,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -7808,7 +7808,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -7912,7 +7912,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8016,7 +8016,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8124,7 +8124,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8232,7 +8232,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8336,7 +8336,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8448,7 +8448,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -8556,7 +8556,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -8664,7 +8664,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -8772,7 +8772,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -8880,7 +8880,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -8984,7 +8984,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9092,7 +9092,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9200,7 +9200,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9304,7 +9304,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9408,7 +9408,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -9512,7 +9512,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -9620,7 +9620,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -9728,7 +9728,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -9832,7 +9832,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -9936,7 +9936,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10044,7 +10044,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10156,7 +10156,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10264,7 +10264,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10368,7 +10368,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -10472,7 +10472,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -10576,7 +10576,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -10680,7 +10680,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -10792,7 +10792,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -10900,7 +10900,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -11008,7 +11008,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11112,7 +11112,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11220,7 +11220,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11328,7 +11328,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -11440,7 +11440,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -11548,7 +11548,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -11656,7 +11656,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -11764,7 +11764,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -11872,7 +11872,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -11980,7 +11980,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12088,7 +12088,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12200,7 +12200,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12304,7 +12304,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -12408,7 +12408,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -12520,7 +12520,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -12632,7 +12632,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -12732,7 +12732,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -12836,7 +12836,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -12948,7 +12948,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13052,7 +13052,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13152,7 +13152,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13256,7 +13256,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -13364,7 +13364,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -13476,7 +13476,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -13588,7 +13588,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -13688,7 +13688,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -13792,7 +13792,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -13900,7 +13900,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14012,7 +14012,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14116,7 +14116,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14224,7 +14224,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -14332,7 +14332,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -14440,7 +14440,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -14548,7 +14548,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -14652,7 +14652,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -14764,7 +14764,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -14872,7 +14872,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -14980,7 +14980,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15088,7 +15088,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -15192,7 +15192,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -15300,7 +15300,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -15404,7 +15404,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -15516,7 +15516,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -15620,7 +15620,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -15732,7 +15732,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -15840,7 +15840,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -15944,7 +15944,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16056,7 +16056,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -16160,7 +16160,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -16268,7 +16268,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -16372,7 +16372,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -16476,7 +16476,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -16584,7 +16584,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -16684,7 +16684,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -16792,7 +16792,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -16896,7 +16896,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -17004,7 +17004,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -17108,7 +17108,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -17212,7 +17212,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -17320,7 +17320,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -17428,7 +17428,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -17536,7 +17536,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -17644,7 +17644,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -17752,7 +17752,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -17856,7 +17856,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -17960,7 +17960,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -18068,7 +18068,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -18172,7 +18172,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -18280,7 +18280,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -18380,7 +18380,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -18488,7 +18488,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -18592,7 +18592,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -18696,7 +18696,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -18804,7 +18804,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -18912,7 +18912,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -19020,7 +19020,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -19124,7 +19124,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -19224,7 +19224,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -19328,7 +19328,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -19436,7 +19436,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -19544,7 +19544,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
optimizing variogram parameters area4
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -518,13 +518,13 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>170061253.5450011</v>
+        <v>241116409.9288566</v>
       </c>
       <c r="C2" t="n">
-        <v>-402048568.8690004</v>
+        <v>-640516451.8613</v>
       </c>
       <c r="D2" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -626,13 +626,13 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>215751600.2529267</v>
+        <v>307840143.1691962</v>
       </c>
       <c r="C3" t="n">
-        <v>-466156325.3815762</v>
+        <v>-744780978.6235237</v>
       </c>
       <c r="D3" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -734,13 +734,13 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>190157095.1846463</v>
+        <v>271851828.2804081</v>
       </c>
       <c r="C4" t="n">
-        <v>-415950649.4723316</v>
+        <v>-668097385.7077036</v>
       </c>
       <c r="D4" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -846,13 +846,13 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>170860992.9712256</v>
+        <v>242120270.0446654</v>
       </c>
       <c r="C5" t="n">
-        <v>-405155427.0714723</v>
+        <v>-644936176.4713304</v>
       </c>
       <c r="D5" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -954,13 +954,13 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>170667185.431315</v>
+        <v>241816006.3231841</v>
       </c>
       <c r="C6" t="n">
-        <v>-405104104.4883425</v>
+        <v>-644771741.2745878</v>
       </c>
       <c r="D6" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1062,13 +1062,13 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>198148318.8949276</v>
+        <v>281822355.0883852</v>
       </c>
       <c r="C7" t="n">
-        <v>-446478395.0038871</v>
+        <v>-711558460.5956467</v>
       </c>
       <c r="D7" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -1166,13 +1166,13 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>170922082.497805</v>
+        <v>242249524.6977128</v>
       </c>
       <c r="C8" t="n">
-        <v>-404787896.7358894</v>
+        <v>-644492121.4329234</v>
       </c>
       <c r="D8" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1274,13 +1274,13 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>190811154.076052</v>
+        <v>272620302.1461084</v>
       </c>
       <c r="C9" t="n">
-        <v>-418967515.8208964</v>
+        <v>-672338783.942363</v>
       </c>
       <c r="D9" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1386,13 +1386,13 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>167063073.7771204</v>
+        <v>236537929.2857987</v>
       </c>
       <c r="C10" t="n">
-        <v>-399736333.0616241</v>
+        <v>-636000231.6287237</v>
       </c>
       <c r="D10" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1498,13 +1498,13 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>191182675.188347</v>
+        <v>273356708.5186262</v>
       </c>
       <c r="C11" t="n">
-        <v>-417313437.041097</v>
+        <v>-670332549.0772539</v>
       </c>
       <c r="D11" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1606,13 +1606,13 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>226125332.4069945</v>
+        <v>324139109.2556922</v>
       </c>
       <c r="C12" t="n">
-        <v>-465476449.0371869</v>
+        <v>-747799482.7227929</v>
       </c>
       <c r="D12" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1710,13 +1710,13 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>207534924.9715279</v>
+        <v>296404406.2602804</v>
       </c>
       <c r="C13" t="n">
-        <v>-448996303.2290542</v>
+        <v>-718866741.0923098</v>
       </c>
       <c r="D13" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1810,13 +1810,13 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>165417181.4159042</v>
+        <v>234421992.9689757</v>
       </c>
       <c r="C14" t="n">
-        <v>-393879767.4921157</v>
+        <v>-627593821.3777303</v>
       </c>
       <c r="D14" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1918,13 +1918,13 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>179797278.9888872</v>
+        <v>258153912.6522675</v>
       </c>
       <c r="C15" t="n">
-        <v>-385339572.3715404</v>
+        <v>-623356145.7801745</v>
       </c>
       <c r="D15" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2022,13 +2022,13 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>227210100.4166648</v>
+        <v>325883524.4871363</v>
       </c>
       <c r="C16" t="n">
-        <v>-464887206.9620859</v>
+        <v>-747398630.4843992</v>
       </c>
       <c r="D16" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -2130,13 +2130,13 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>212055122.9125671</v>
+        <v>303097785.9272359</v>
       </c>
       <c r="C17" t="n">
-        <v>-453803865.4495928</v>
+        <v>-727024925.2444966</v>
       </c>
       <c r="D17" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -2234,13 +2234,13 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>219066152.3479342</v>
+        <v>312636899.8738974</v>
       </c>
       <c r="C18" t="n">
-        <v>-470844080.385905</v>
+        <v>-752270474.6464767</v>
       </c>
       <c r="D18" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -2342,13 +2342,13 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>229520900.4912613</v>
+        <v>329811766.0912105</v>
       </c>
       <c r="C19" t="n">
-        <v>-461115703.439372</v>
+        <v>-743155717.4879633</v>
       </c>
       <c r="D19" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2442,13 +2442,13 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>170189121.3721983</v>
+        <v>241284616.1454389</v>
       </c>
       <c r="C20" t="n">
-        <v>-402456658.3516716</v>
+        <v>-641108597.9145137</v>
       </c>
       <c r="D20" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2550,13 +2550,13 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>232646418.6580028</v>
+        <v>334170860.8161556</v>
       </c>
       <c r="C21" t="n">
-        <v>-467100958.0807744</v>
+        <v>-752220211.8294635</v>
       </c>
       <c r="D21" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -2654,13 +2654,13 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>221685799.896555</v>
+        <v>318489476.4800459</v>
       </c>
       <c r="C22" t="n">
-        <v>-450486429.1942855</v>
+        <v>-726238810.2783819</v>
       </c>
       <c r="D22" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -2754,13 +2754,13 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>170044434.1339617</v>
+        <v>240947429.0625636</v>
       </c>
       <c r="C23" t="n">
-        <v>-403681533.2859867</v>
+        <v>-642618118.4559122</v>
       </c>
       <c r="D23" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -2854,13 +2854,13 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>170455328.0702242</v>
+        <v>241537608.1774869</v>
       </c>
       <c r="C24" t="n">
-        <v>-404423592.289158</v>
+        <v>-643785192.149943</v>
       </c>
       <c r="D24" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -2962,13 +2962,13 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>220587369.5919776</v>
+        <v>316028303.5171236</v>
       </c>
       <c r="C25" t="n">
-        <v>-459065039.3759356</v>
+        <v>-737261747.7522157</v>
       </c>
       <c r="D25" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -3070,13 +3070,13 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>204294828.1179895</v>
+        <v>292111793.1974413</v>
       </c>
       <c r="C26" t="n">
-        <v>-439678649.7171889</v>
+        <v>-705272189.3632073</v>
       </c>
       <c r="D26" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -3174,13 +3174,13 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>169897527.0426158</v>
+        <v>240803556.7309235</v>
       </c>
       <c r="C27" t="n">
-        <v>-402644194.6175289</v>
+        <v>-641203341.7830828</v>
       </c>
       <c r="D27" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -3282,13 +3282,13 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>209752092.0299546</v>
+        <v>301625905.0998349</v>
       </c>
       <c r="C28" t="n">
-        <v>-429279032.9395711</v>
+        <v>-693639299.8900316</v>
       </c>
       <c r="D28" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -3390,13 +3390,13 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>181148880.3769667</v>
+        <v>259524364.4675499</v>
       </c>
       <c r="C29" t="n">
-        <v>-393871673.9209508</v>
+        <v>-635159537.19867</v>
       </c>
       <c r="D29" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -3494,13 +3494,13 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>223592087.1595653</v>
+        <v>321125162.8406616</v>
       </c>
       <c r="C30" t="n">
-        <v>-454483925.6360297</v>
+        <v>-732246856.0965803</v>
       </c>
       <c r="D30" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -3594,13 +3594,13 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>220591388.8574566</v>
+        <v>316034106.6327591</v>
       </c>
       <c r="C31" t="n">
-        <v>-459070734.1471248</v>
+        <v>-737270796.7957494</v>
       </c>
       <c r="D31" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -3702,13 +3702,13 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>169837139.3715255</v>
+        <v>240675486.9111191</v>
       </c>
       <c r="C32" t="n">
-        <v>-403010049.6333153</v>
+        <v>-641645409.746622</v>
       </c>
       <c r="D32" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -3810,13 +3810,13 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>217075885.120332</v>
+        <v>309591520.6783481</v>
       </c>
       <c r="C33" t="n">
-        <v>-469975118.9094672</v>
+        <v>-750338693.3007903</v>
       </c>
       <c r="D33" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -3914,13 +3914,13 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>170221339.6758617</v>
+        <v>241180851.5727562</v>
       </c>
       <c r="C34" t="n">
-        <v>-404239109.246271</v>
+        <v>-643428200.0245736</v>
       </c>
       <c r="D34" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -4022,13 +4022,13 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>228674745.6979045</v>
+        <v>328636380.8735353</v>
       </c>
       <c r="C35" t="n">
-        <v>-459433627.7697359</v>
+        <v>-740617600.2250655</v>
       </c>
       <c r="D35" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -4126,13 +4126,13 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>226511925.3198773</v>
+        <v>324854430.5347658</v>
       </c>
       <c r="C36" t="n">
-        <v>-464173405.9727495</v>
+        <v>-746200833.3122867</v>
       </c>
       <c r="D36" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -4238,13 +4238,13 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>182849971.5594774</v>
+        <v>261924235.3221091</v>
       </c>
       <c r="C37" t="n">
-        <v>-397265861.4077961</v>
+        <v>-640369267.1781435</v>
       </c>
       <c r="D37" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -4342,13 +4342,13 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>185605712.1449671</v>
+        <v>266105340.8550061</v>
       </c>
       <c r="C38" t="n">
-        <v>-399507878.409721</v>
+        <v>-644524175.3137047</v>
       </c>
       <c r="D38" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -4450,13 +4450,13 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>165158688.1655019</v>
+        <v>233692973.6274313</v>
       </c>
       <c r="C39" t="n">
-        <v>-397520250.4713072</v>
+        <v>-632156415.2001097</v>
       </c>
       <c r="D39" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -4562,13 +4562,13 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>169255388.5440889</v>
+        <v>239958332.6812091</v>
       </c>
       <c r="C40" t="n">
-        <v>-400598228.2076799</v>
+        <v>-638233803.9230567</v>
       </c>
       <c r="D40" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -4674,13 +4674,13 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>220469595.8216356</v>
+        <v>315871578.7534108</v>
       </c>
       <c r="C41" t="n">
-        <v>-458743532.120712</v>
+        <v>-736791243.5112112</v>
       </c>
       <c r="D41" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -4782,13 +4782,13 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>168088018.066688</v>
+        <v>238081039.3346827</v>
       </c>
       <c r="C42" t="n">
-        <v>-400784453.2981902</v>
+        <v>-637879350.5167651</v>
       </c>
       <c r="D42" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -4894,13 +4894,13 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>167778416.8765537</v>
+        <v>237917772.9119691</v>
       </c>
       <c r="C43" t="n">
-        <v>-396994263.684976</v>
+        <v>-632825810.5677013</v>
       </c>
       <c r="D43" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -5002,13 +5002,13 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>189893264.5149418</v>
+        <v>271453178.3149346</v>
       </c>
       <c r="C44" t="n">
-        <v>-415728052.2039195</v>
+        <v>-667689887.1368873</v>
       </c>
       <c r="D44" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -5114,13 +5114,13 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>161294915.6318805</v>
+        <v>228517245.6278447</v>
       </c>
       <c r="C45" t="n">
-        <v>-386106025.2255547</v>
+        <v>-615422880.303871</v>
       </c>
       <c r="D45" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -5226,13 +5226,13 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>170989661.2193642</v>
+        <v>242289512.9431651</v>
       </c>
       <c r="C46" t="n">
-        <v>-405566621.7426242</v>
+        <v>-645532582.8692462</v>
       </c>
       <c r="D46" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -5330,13 +5330,13 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>167842617.8236445</v>
+        <v>237611354.9062354</v>
       </c>
       <c r="C47" t="n">
-        <v>-401689953.4288404</v>
+        <v>-638922073.3417053</v>
       </c>
       <c r="D47" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -5442,13 +5442,13 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>168348387.5857986</v>
+        <v>238716552.1387896</v>
       </c>
       <c r="C48" t="n">
-        <v>-398256561.2255399</v>
+        <v>-634747027.1713309</v>
       </c>
       <c r="D48" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -5550,13 +5550,13 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>225037801.297646</v>
+        <v>322745359.7031357</v>
       </c>
       <c r="C49" t="n">
-        <v>-461912078.2331657</v>
+        <v>-742664354.0434316</v>
       </c>
       <c r="D49" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -5658,13 +5658,13 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>170869051.6025432</v>
+        <v>242277238.6826189</v>
       </c>
       <c r="C50" t="n">
-        <v>-403499299.370443</v>
+        <v>-642799677.7142836</v>
       </c>
       <c r="D50" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -5762,13 +5762,13 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>193017470.4955127</v>
+        <v>277669410.9749006</v>
       </c>
       <c r="C51" t="n">
-        <v>-401785101.312815</v>
+        <v>-650638472.9506352</v>
       </c>
       <c r="D51" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -5870,13 +5870,13 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>199949949.5776266</v>
+        <v>284453677.0661486</v>
       </c>
       <c r="C52" t="n">
-        <v>-448945059.420067</v>
+        <v>-715576330.4317623</v>
       </c>
       <c r="D52" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -5974,13 +5974,13 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>212560183.8336233</v>
+        <v>303309631.9706399</v>
       </c>
       <c r="C53" t="n">
-        <v>-460556023.6364397</v>
+        <v>-736125207.7363403</v>
       </c>
       <c r="D53" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -6082,13 +6082,13 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>161676484.2880752</v>
+        <v>229115395.803687</v>
       </c>
       <c r="C54" t="n">
-        <v>-386240761.038307</v>
+        <v>-615796001.4970576</v>
       </c>
       <c r="D54" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -6194,13 +6194,13 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>169788566.1146641</v>
+        <v>240709029.5342582</v>
       </c>
       <c r="C55" t="n">
-        <v>-401736005.8829324</v>
+        <v>-639974477.0186136</v>
       </c>
       <c r="D55" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -6302,13 +6302,13 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>211508905.0259657</v>
+        <v>302373980.5765743</v>
       </c>
       <c r="C56" t="n">
-        <v>-452247932.9809692</v>
+        <v>-724754887.8731717</v>
       </c>
       <c r="D56" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -6406,13 +6406,13 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>159944451.6321533</v>
+        <v>226115473.4363479</v>
       </c>
       <c r="C57" t="n">
-        <v>-388908680.488093</v>
+        <v>-618321946.9817134</v>
       </c>
       <c r="D57" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -6510,13 +6510,13 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>201934275.4551795</v>
+        <v>287378257.0332168</v>
       </c>
       <c r="C58" t="n">
-        <v>-451332610.6898304</v>
+        <v>-719565294.9595512</v>
       </c>
       <c r="D58" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -6614,13 +6614,13 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>184732978.0088556</v>
+        <v>264899440.4536139</v>
       </c>
       <c r="C59" t="n">
-        <v>-397506742.2204202</v>
+        <v>-641513779.7746129</v>
       </c>
       <c r="D59" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -6722,13 +6722,13 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>195705534.4388087</v>
+        <v>278445845.2283827</v>
       </c>
       <c r="C60" t="n">
-        <v>-440888996.2268443</v>
+        <v>-703174320.3226094</v>
       </c>
       <c r="D60" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -6826,13 +6826,13 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>220534136.2407041</v>
+        <v>313956072.1801931</v>
       </c>
       <c r="C61" t="n">
-        <v>-482430540.6605094</v>
+        <v>-768109334.7570126</v>
       </c>
       <c r="D61" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -6930,13 +6930,13 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>225035389.0068487</v>
+        <v>322741874.7063678</v>
       </c>
       <c r="C62" t="n">
-        <v>-461908760.2337005</v>
+        <v>-742659074.352662</v>
       </c>
       <c r="D62" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -7038,13 +7038,13 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>183320051.9313003</v>
+        <v>263258404.8438024</v>
       </c>
       <c r="C63" t="n">
-        <v>-390873338.4612513</v>
+        <v>-632173952.7290845</v>
       </c>
       <c r="D63" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -7146,13 +7146,13 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>198119290.4729356</v>
+        <v>281833903.6966872</v>
       </c>
       <c r="C64" t="n">
-        <v>-445812024.3581349</v>
+        <v>-710675747.4114839</v>
       </c>
       <c r="D64" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -7258,13 +7258,13 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>183136998.266023</v>
+        <v>259864791.7006577</v>
       </c>
       <c r="C65" t="n">
-        <v>-425597138.2776437</v>
+        <v>-677451073.353865</v>
       </c>
       <c r="D65" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -7366,13 +7366,13 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>194155942.949601</v>
+        <v>279469335.2922495</v>
       </c>
       <c r="C66" t="n">
-        <v>-401840817.6504443</v>
+        <v>-651169910.9945309</v>
       </c>
       <c r="D66" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -7474,13 +7474,13 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>199951766.5902286</v>
+        <v>284456288.9917687</v>
       </c>
       <c r="C67" t="n">
-        <v>-448948024.5963792</v>
+        <v>-715581003.6488818</v>
       </c>
       <c r="D67" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -7582,13 +7582,13 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>181191745.9251307</v>
+        <v>259723469.9714658</v>
       </c>
       <c r="C68" t="n">
-        <v>-392441938.8805223</v>
+        <v>-633302860.1094917</v>
       </c>
       <c r="D68" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -7690,13 +7690,13 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>181465006.6044621</v>
+        <v>261164753.2626413</v>
       </c>
       <c r="C69" t="n">
-        <v>-381565732.0586818</v>
+        <v>-619107805.3630104</v>
       </c>
       <c r="D69" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -7798,13 +7798,13 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>190126419.3274445</v>
+        <v>272777273.7243389</v>
       </c>
       <c r="C70" t="n">
-        <v>-405131540.1544722</v>
+        <v>-653863315.1116563</v>
       </c>
       <c r="D70" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -7902,13 +7902,13 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>213293560.7974027</v>
+        <v>305892356.1042734</v>
       </c>
       <c r="C71" t="n">
-        <v>-444046630.9603429</v>
+        <v>-714595899.8409623</v>
       </c>
       <c r="D71" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -8006,13 +8006,13 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>170191838.1157665</v>
+        <v>241288520.0071773</v>
       </c>
       <c r="C72" t="n">
-        <v>-402461543.5417274</v>
+        <v>-641116285.9121094</v>
       </c>
       <c r="D72" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -8114,13 +8114,13 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>220588452.1677152</v>
+        <v>316029866.5670241</v>
       </c>
       <c r="C73" t="n">
-        <v>-459066573.2519769</v>
+        <v>-737264185.0951921</v>
       </c>
       <c r="D73" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -8222,13 +8222,13 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>195997045.5293688</v>
+        <v>279681540.434641</v>
       </c>
       <c r="C74" t="n">
-        <v>-431996651.364231</v>
+        <v>-691676297.3159117</v>
       </c>
       <c r="D74" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -8326,13 +8326,13 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>168450500.9432539</v>
+        <v>238606731.4384664</v>
       </c>
       <c r="C75" t="n">
-        <v>-401384793.0106061</v>
+        <v>-638839898.102951</v>
       </c>
       <c r="D75" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -8438,13 +8438,13 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>230175350.2550632</v>
+        <v>330076763.9282188</v>
       </c>
       <c r="C76" t="n">
-        <v>-469965199.3425449</v>
+        <v>-755208195.1460632</v>
       </c>
       <c r="D76" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -8546,13 +8546,13 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>208808591.8167622</v>
+        <v>299439780.3822055</v>
       </c>
       <c r="C77" t="n">
-        <v>-437210044.3358359</v>
+        <v>-703812662.4923407</v>
       </c>
       <c r="D77" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -8654,13 +8654,13 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>175243179.3873374</v>
+        <v>251216849.3362035</v>
       </c>
       <c r="C78" t="n">
-        <v>-381724269.4209624</v>
+        <v>-616569650.678416</v>
       </c>
       <c r="D78" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -8762,13 +8762,13 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>159981689.5436021</v>
+        <v>226164033.8365528</v>
       </c>
       <c r="C79" t="n">
-        <v>-389034951.2546384</v>
+        <v>-618504264.9674021</v>
       </c>
       <c r="D79" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -8870,13 +8870,13 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>201940941.1117887</v>
+        <v>287387840.2114912</v>
       </c>
       <c r="C80" t="n">
-        <v>-451343395.5166952</v>
+        <v>-719582297.4409394</v>
       </c>
       <c r="D80" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -8974,13 +8974,13 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>199038252.9463307</v>
+        <v>283149053.8281337</v>
       </c>
       <c r="C81" t="n">
-        <v>-447386185.6953286</v>
+        <v>-713138153.5136787</v>
       </c>
       <c r="D81" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -9082,13 +9082,13 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>200536386.0293367</v>
+        <v>285278721.9658185</v>
       </c>
       <c r="C82" t="n">
-        <v>-450110034.1736351</v>
+        <v>-717356056.9629877</v>
       </c>
       <c r="D82" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -9190,13 +9190,13 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>205759380.4885022</v>
+        <v>295826005.8928929</v>
       </c>
       <c r="C83" t="n">
-        <v>-423798822.2369605</v>
+        <v>-684845866.2343649</v>
       </c>
       <c r="D83" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -9294,13 +9294,13 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>189088595.2522518</v>
+        <v>272014231.2749047</v>
       </c>
       <c r="C84" t="n">
-        <v>-395445249.0775359</v>
+        <v>-640643632.4785765</v>
       </c>
       <c r="D84" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -9398,13 +9398,13 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>223641556.3890886</v>
+        <v>320789113.3239766</v>
       </c>
       <c r="C85" t="n">
-        <v>-459278078.5597609</v>
+        <v>-738656926.3217984</v>
       </c>
       <c r="D85" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -9502,13 +9502,13 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>201021809.2568428</v>
+        <v>285970464.894981</v>
       </c>
       <c r="C86" t="n">
-        <v>-450970544.5014009</v>
+        <v>-718693340.5180732</v>
       </c>
       <c r="D86" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -9610,13 +9610,13 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>180714862.6879153</v>
+        <v>259513822.2850575</v>
       </c>
       <c r="C87" t="n">
-        <v>-386459896.4466831</v>
+        <v>-625232380.7979548</v>
       </c>
       <c r="D87" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -9718,13 +9718,13 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>192332759.4216259</v>
+        <v>273641607.671856</v>
       </c>
       <c r="C88" t="n">
-        <v>-434773788.9701531</v>
+        <v>-693677903.9160447</v>
       </c>
       <c r="D88" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -9822,13 +9822,13 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>160418897.5706784</v>
+        <v>226786550.2516718</v>
       </c>
       <c r="C89" t="n">
-        <v>-389911002.6655887</v>
+        <v>-619864072.960627</v>
       </c>
       <c r="D89" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -9926,13 +9926,13 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>183326049.5143205</v>
+        <v>260213516.9754689</v>
       </c>
       <c r="C90" t="n">
-        <v>-425033345.1795313</v>
+        <v>-676810304.4705592</v>
       </c>
       <c r="D90" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -10034,13 +10034,13 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>159985281.4310923</v>
+        <v>226169188.3207233</v>
       </c>
       <c r="C91" t="n">
-        <v>-389041687.233989</v>
+        <v>-618514843.849395</v>
       </c>
       <c r="D91" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -10146,13 +10146,13 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>178908355.1332637</v>
+        <v>254974684.4502476</v>
       </c>
       <c r="C92" t="n">
-        <v>-404735969.3286093</v>
+        <v>-648327480.5640734</v>
       </c>
       <c r="D92" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -10254,13 +10254,13 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>158953626.7530148</v>
+        <v>224717828.7056844</v>
       </c>
       <c r="C93" t="n">
-        <v>-386767804.1345814</v>
+        <v>-615039144.3747218</v>
       </c>
       <c r="D93" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -10358,13 +10358,13 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>159983783.1963968</v>
+        <v>226167038.3015949</v>
       </c>
       <c r="C94" t="n">
-        <v>-389038877.5547693</v>
+        <v>-618510431.2372736</v>
       </c>
       <c r="D94" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -10462,13 +10462,13 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>159031701.4770814</v>
+        <v>224820170.6684155</v>
       </c>
       <c r="C95" t="n">
-        <v>-387026708.7799101</v>
+        <v>-615413964.9004151</v>
       </c>
       <c r="D95" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -10566,13 +10566,13 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>191708627.3984575</v>
+        <v>274781804.7242188</v>
       </c>
       <c r="C96" t="n">
-        <v>-410724560.5956822</v>
+        <v>-661899490.7891164</v>
       </c>
       <c r="D96" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -10670,13 +10670,13 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>164829082.7846155</v>
+        <v>233259970.1339031</v>
       </c>
       <c r="C97" t="n">
-        <v>-396448779.1607118</v>
+        <v>-630603626.1936203</v>
       </c>
       <c r="D97" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -10782,13 +10782,13 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>191830326.5457348</v>
+        <v>274067975.5643117</v>
       </c>
       <c r="C98" t="n">
-        <v>-420857416.8751051</v>
+        <v>-675262354.2216074</v>
       </c>
       <c r="D98" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -10890,13 +10890,13 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>200745874.1465958</v>
+        <v>285555902.5664799</v>
       </c>
       <c r="C99" t="n">
-        <v>-450730133.2302119</v>
+        <v>-718258134.6457069</v>
       </c>
       <c r="D99" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -10998,13 +10998,13 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>195100893.162625</v>
+        <v>277547055.5154095</v>
       </c>
       <c r="C100" t="n">
-        <v>-440230697.0622374</v>
+        <v>-702044307.992703</v>
       </c>
       <c r="D100" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -11102,13 +11102,13 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>225334535.0004603</v>
+        <v>323741591.2967488</v>
       </c>
       <c r="C101" t="n">
-        <v>-455721416.1328683</v>
+        <v>-734507953.3498362</v>
       </c>
       <c r="D101" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -11210,13 +11210,13 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>170066567.4634582</v>
+        <v>241124046.2670941</v>
       </c>
       <c r="C102" t="n">
-        <v>-402058122.279879</v>
+        <v>-640531487.5712001</v>
       </c>
       <c r="D102" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -11318,13 +11318,13 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>184677066.2989198</v>
+        <v>262243332.2856171</v>
       </c>
       <c r="C103" t="n">
-        <v>-426343195.7846923</v>
+        <v>-679154550.8067428</v>
       </c>
       <c r="D103" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -11430,13 +11430,13 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>190705854.829486</v>
+        <v>271543321.4000739</v>
       </c>
       <c r="C104" t="n">
-        <v>-429290698.053645</v>
+        <v>-685788883.8156843</v>
       </c>
       <c r="D104" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -11538,13 +11538,13 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>173950496.5190559</v>
+        <v>247118332.88347</v>
       </c>
       <c r="C105" t="n">
-        <v>-404282480.4928117</v>
+        <v>-645348511.1651821</v>
       </c>
       <c r="D105" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -11646,13 +11646,13 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>236488082.5247939</v>
+        <v>337201433.0136378</v>
       </c>
       <c r="C106" t="n">
-        <v>-502234364.1522337</v>
+        <v>-800345615.03389</v>
       </c>
       <c r="D106" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -11754,13 +11754,13 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>212723687.7217174</v>
+        <v>304537376.5776873</v>
       </c>
       <c r="C107" t="n">
-        <v>-449317799.2371773</v>
+        <v>-721360980.5391968</v>
       </c>
       <c r="D107" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -11862,13 +11862,13 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>169111069.225488</v>
+        <v>239524588.7008033</v>
       </c>
       <c r="C108" t="n">
-        <v>-402939472.3102995</v>
+        <v>-641184656.1507736</v>
       </c>
       <c r="D108" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -11970,13 +11970,13 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>198336644.9666787</v>
+        <v>285177471.3559144</v>
       </c>
       <c r="C109" t="n">
-        <v>-411866837.4992051</v>
+        <v>-666124678.5824778</v>
       </c>
       <c r="D109" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -12078,13 +12078,13 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>158546247.0333468</v>
+        <v>224615062.5923977</v>
       </c>
       <c r="C110" t="n">
-        <v>-380475198.7775751</v>
+        <v>-606717622.250353</v>
       </c>
       <c r="D110" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -12190,13 +12190,13 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>189729394.5335976</v>
+        <v>272249754.7655263</v>
       </c>
       <c r="C111" t="n">
-        <v>-403999810.6284639</v>
+        <v>-652204163.8814831</v>
       </c>
       <c r="D111" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -12294,13 +12294,13 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>202072665.5388272</v>
+        <v>287408714.7674247</v>
       </c>
       <c r="C112" t="n">
-        <v>-453520694.1747884</v>
+        <v>-722485408.0931526</v>
       </c>
       <c r="D112" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -12398,13 +12398,13 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>161325373.0124752</v>
+        <v>228605661.3841797</v>
       </c>
       <c r="C113" t="n">
-        <v>-385652928.7783066</v>
+        <v>-614854348.7632763</v>
       </c>
       <c r="D113" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -12510,13 +12510,13 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>161054255.9680095</v>
+        <v>228201033.2161114</v>
       </c>
       <c r="C114" t="n">
-        <v>-385324290.4075406</v>
+        <v>-614288686.2252672</v>
       </c>
       <c r="D114" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -12622,13 +12622,13 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>228912456.7268519</v>
+        <v>326181861.1804546</v>
       </c>
       <c r="C115" t="n">
-        <v>-492802897.0585838</v>
+        <v>-785049507.6016762</v>
       </c>
       <c r="D115" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -12722,13 +12722,13 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>189903671.6324413</v>
+        <v>272145706.4409218</v>
       </c>
       <c r="C116" t="n">
-        <v>-408201000.6104372</v>
+        <v>-657809791.884734</v>
       </c>
       <c r="D116" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -12826,13 +12826,13 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>190128098.1234068</v>
+        <v>271862757.4238549</v>
       </c>
       <c r="C117" t="n">
-        <v>-415313302.3688121</v>
+        <v>-667248888.2380273</v>
       </c>
       <c r="D117" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -12938,13 +12938,13 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>219741114.3635682</v>
+        <v>315105951.0574893</v>
       </c>
       <c r="C118" t="n">
-        <v>-454396973.9048197</v>
+        <v>-730747426.1765029</v>
       </c>
       <c r="D118" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -13042,13 +13042,13 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>191441505.7863299</v>
+        <v>272863476.7660523</v>
       </c>
       <c r="C119" t="n">
-        <v>-427522610.3461448</v>
+        <v>-683812167.8925201</v>
       </c>
       <c r="D119" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -13142,13 +13142,13 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>166744254.6523182</v>
+        <v>236410689.9844101</v>
       </c>
       <c r="C120" t="n">
-        <v>-395359670.511667</v>
+        <v>-630186134.2139621</v>
       </c>
       <c r="D120" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -13246,13 +13246,13 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>159982778.8322647</v>
+        <v>226165597.0039313</v>
       </c>
       <c r="C121" t="n">
-        <v>-389036994.0382276</v>
+        <v>-618507473.1671422</v>
       </c>
       <c r="D121" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -13354,13 +13354,13 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>159450693.4018503</v>
+        <v>225900681.1727424</v>
       </c>
       <c r="C122" t="n">
-        <v>-382313786.5138384</v>
+        <v>-609564829.8951237</v>
       </c>
       <c r="D122" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -13466,13 +13466,13 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>160581153.2411571</v>
+        <v>227530799.8906835</v>
       </c>
       <c r="C123" t="n">
-        <v>-384341226.8542533</v>
+        <v>-612773015.4131714</v>
       </c>
       <c r="D123" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -13578,13 +13578,13 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>204412644.2140465</v>
+        <v>292912636.687263</v>
       </c>
       <c r="C124" t="n">
-        <v>-432688320.1416128</v>
+        <v>-696098767.0576134</v>
       </c>
       <c r="D124" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -13678,13 +13678,13 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>163617850.8680348</v>
+        <v>232006809.2622156</v>
       </c>
       <c r="C125" t="n">
-        <v>-388648087.9597438</v>
+        <v>-619910906.2042223</v>
       </c>
       <c r="D125" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -13782,13 +13782,13 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>188672409.5696528</v>
+        <v>269835674.2570578</v>
       </c>
       <c r="C126" t="n">
-        <v>-412151951.1620351</v>
+        <v>-662465103.058249</v>
       </c>
       <c r="D126" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -13890,13 +13890,13 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>180662603.712813</v>
+        <v>260004362.5773549</v>
       </c>
       <c r="C127" t="n">
-        <v>-380285375.9184469</v>
+        <v>-617075096.1658553</v>
       </c>
       <c r="D127" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -14002,13 +14002,13 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>159981312.4340496</v>
+        <v>226163492.6711283</v>
       </c>
       <c r="C128" t="n">
-        <v>-389034244.04576</v>
+        <v>-618503154.2930305</v>
       </c>
       <c r="D128" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -14106,13 +14106,13 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>190553921.2513739</v>
+        <v>272231389.1081073</v>
       </c>
       <c r="C129" t="n">
-        <v>-418754253.6420302</v>
+        <v>-671946254.9176275</v>
       </c>
       <c r="D129" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -14214,13 +14214,13 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>164680010.3926166</v>
+        <v>234504158.7149849</v>
       </c>
       <c r="C130" t="n">
-        <v>-379685424.6714844</v>
+        <v>-608853674.238616</v>
       </c>
       <c r="D130" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -14322,13 +14322,13 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>180693895.2109168</v>
+        <v>257577191.2416937</v>
       </c>
       <c r="C131" t="n">
-        <v>-407424798.7042264</v>
+        <v>-652668699.3305537</v>
       </c>
       <c r="D131" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -14430,13 +14430,13 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>162283396.6694638</v>
+        <v>230057768.3387714</v>
       </c>
       <c r="C132" t="n">
-        <v>-386557522.8375871</v>
+        <v>-616520724.873842</v>
       </c>
       <c r="D132" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -14538,13 +14538,13 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>159593752.1135564</v>
+        <v>225607327.2208885</v>
       </c>
       <c r="C133" t="n">
-        <v>-388307085.0363675</v>
+        <v>-617361142.6686318</v>
       </c>
       <c r="D133" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -14642,13 +14642,13 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>183568970.4222474</v>
+        <v>261178897.8119061</v>
       </c>
       <c r="C134" t="n">
-        <v>-418382782.426956</v>
+        <v>-668284335.5192387</v>
       </c>
       <c r="D134" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -14754,13 +14754,13 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>193274830.4161268</v>
+        <v>278202125.5705481</v>
       </c>
       <c r="C135" t="n">
-        <v>-400423351.3916775</v>
+        <v>-648938013.488188</v>
       </c>
       <c r="D135" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -14862,13 +14862,13 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>169039221.4966475</v>
+        <v>239771508.8132858</v>
       </c>
       <c r="C136" t="n">
-        <v>-398792434.4795803</v>
+        <v>-635790051.9050461</v>
       </c>
       <c r="D136" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -14970,13 +14970,13 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>187767923.9888766</v>
+        <v>268395005.4511626</v>
       </c>
       <c r="C137" t="n">
-        <v>-412204218.9547121</v>
+        <v>-662134595.8958046</v>
       </c>
       <c r="D137" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -15078,13 +15078,13 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>176614885.9983608</v>
+        <v>251362684.6463775</v>
       </c>
       <c r="C138" t="n">
-        <v>-404281953.2558571</v>
+        <v>-646644373.9702441</v>
       </c>
       <c r="D138" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -15182,13 +15182,13 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>214146793.1152762</v>
+        <v>304686586.0029499</v>
       </c>
       <c r="C139" t="n">
-        <v>-473637174.7999482</v>
+        <v>-753959532.9839897</v>
       </c>
       <c r="D139" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -15290,13 +15290,13 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>195694588.3217317</v>
+        <v>278683013.3011628</v>
       </c>
       <c r="C140" t="n">
-        <v>-437953639.0172651</v>
+        <v>-699336737.2919977</v>
       </c>
       <c r="D140" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -15394,13 +15394,13 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>161681400.0862358</v>
+        <v>229122462.9280137</v>
       </c>
       <c r="C141" t="n">
-        <v>-386249778.728037</v>
+        <v>-615810200.1162999</v>
       </c>
       <c r="D141" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -15506,13 +15506,13 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>199808924.882672</v>
+        <v>286652264.0822604</v>
       </c>
       <c r="C142" t="n">
-        <v>-421352675.5362641</v>
+        <v>-679269130.0227554</v>
       </c>
       <c r="D142" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -15610,13 +15610,13 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>187914817.4255285</v>
+        <v>268735102.2271433</v>
       </c>
       <c r="C143" t="n">
-        <v>-411011705.6538569</v>
+        <v>-660636716.3574395</v>
       </c>
       <c r="D143" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -15722,13 +15722,13 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>170030570.7160479</v>
+        <v>243601156.586562</v>
       </c>
       <c r="C144" t="n">
-        <v>-373916385.7070824</v>
+        <v>-603939255.377998</v>
       </c>
       <c r="D144" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -15830,13 +15830,13 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>218929775.7707652</v>
+        <v>315019437.858991</v>
       </c>
       <c r="C145" t="n">
-        <v>-440791059.8359208</v>
+        <v>-712316144.3485979</v>
       </c>
       <c r="D145" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -15934,13 +15934,13 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>162708234.4723862</v>
+        <v>230568678.7818459</v>
       </c>
       <c r="C146" t="n">
-        <v>-388472907.154898</v>
+        <v>-619213379.4449077</v>
       </c>
       <c r="D146" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -16046,13 +16046,13 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>193098927.3384862</v>
+        <v>274703017.1193153</v>
       </c>
       <c r="C147" t="n">
-        <v>-436513085.7480596</v>
+        <v>-696292944.7845743</v>
       </c>
       <c r="D147" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -16150,13 +16150,13 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>230555666.8963441</v>
+        <v>331539974.7603281</v>
       </c>
       <c r="C148" t="n">
-        <v>-459769917.9560463</v>
+        <v>-741698511.2020931</v>
       </c>
       <c r="D148" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -16258,13 +16258,13 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>193727869.7420573</v>
+        <v>275934405.7071202</v>
       </c>
       <c r="C149" t="n">
-        <v>-433795557.1452767</v>
+        <v>-693029384.238608</v>
       </c>
       <c r="D149" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -16362,13 +16362,13 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>172808170.7906583</v>
+        <v>245221390.8877693</v>
       </c>
       <c r="C150" t="n">
-        <v>-405162410.6592178</v>
+        <v>-645922673.169723</v>
       </c>
       <c r="D150" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -16466,13 +16466,13 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>190025554.5393861</v>
+        <v>271433622.9273621</v>
       </c>
       <c r="C151" t="n">
-        <v>-418302784.1040679</v>
+        <v>-671121900.1209217</v>
       </c>
       <c r="D151" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -16574,13 +16574,13 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>233758818.4293233</v>
+        <v>333327753.5744264</v>
       </c>
       <c r="C152" t="n">
-        <v>-497716248.5745634</v>
+        <v>-793362759.6305578</v>
       </c>
       <c r="D152" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -16674,13 +16674,13 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>197999048.2211913</v>
+        <v>281927973.9961489</v>
       </c>
       <c r="C153" t="n">
-        <v>-442524433.6819119</v>
+        <v>-706328223.660036</v>
       </c>
       <c r="D153" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -16782,13 +16782,13 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>170274010.9602531</v>
+        <v>241494785.4813281</v>
       </c>
       <c r="C154" t="n">
-        <v>-401599067.683601</v>
+        <v>-640042740.3329711</v>
       </c>
       <c r="D154" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -16886,13 +16886,13 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>217091423.600224</v>
+        <v>311085736.1148545</v>
       </c>
       <c r="C155" t="n">
-        <v>-452864053.2432491</v>
+        <v>-727727749.3847228</v>
       </c>
       <c r="D155" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -16994,13 +16994,13 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>166872681.8275874</v>
+        <v>236677036.0213428</v>
       </c>
       <c r="C156" t="n">
-        <v>-394659380.2129357</v>
+        <v>-629346904.2296659</v>
       </c>
       <c r="D156" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -17098,13 +17098,13 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>208841063.2337069</v>
+        <v>299827188.9903314</v>
       </c>
       <c r="C157" t="n">
-        <v>-433398500.873895</v>
+        <v>-698771109.8942244</v>
       </c>
       <c r="D157" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -17202,13 +17202,13 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>191697416.7709543</v>
+        <v>275722938.950241</v>
       </c>
       <c r="C158" t="n">
-        <v>-400171482.9756765</v>
+        <v>-647966189.414601</v>
       </c>
       <c r="D158" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -17310,13 +17310,13 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>163624090.056206</v>
+        <v>231870099.3434019</v>
       </c>
       <c r="C159" t="n">
-        <v>-390320148.7865415</v>
+        <v>-622072620.8410587</v>
       </c>
       <c r="D159" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -17418,13 +17418,13 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>230432261.7004661</v>
+        <v>331375399.2707284</v>
       </c>
       <c r="C160" t="n">
-        <v>-459446216.7997958</v>
+        <v>-741223418.8351234</v>
       </c>
       <c r="D160" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -17526,13 +17526,13 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>213054465.7445063</v>
+        <v>306411760.0856024</v>
       </c>
       <c r="C161" t="n">
-        <v>-433863851.7112849</v>
+        <v>-700964540.7794162</v>
       </c>
       <c r="D161" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -17634,13 +17634,13 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>192706308.6065789</v>
+        <v>274184724.1137281</v>
       </c>
       <c r="C162" t="n">
-        <v>-435326852.917184</v>
+        <v>-694568373.8249217</v>
       </c>
       <c r="D162" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -17742,13 +17742,13 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>208919250.3967201</v>
+        <v>299734528.2315714</v>
       </c>
       <c r="C163" t="n">
-        <v>-435841706.9338781</v>
+        <v>-702042015.4739696</v>
       </c>
       <c r="D163" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -17846,13 +17846,13 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>169634345.0394309</v>
+        <v>240554629.3470742</v>
       </c>
       <c r="C164" t="n">
-        <v>-400688439.0056636</v>
+        <v>-638542346.5098919</v>
       </c>
       <c r="D164" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -17950,13 +17950,13 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>214076451.9032896</v>
+        <v>307919216.6758572</v>
       </c>
       <c r="C165" t="n">
-        <v>-434970040.9152226</v>
+        <v>-702811392.4851085</v>
       </c>
       <c r="D165" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -18058,13 +18058,13 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>226014241.3440962</v>
+        <v>324395347.8652229</v>
       </c>
       <c r="C166" t="n">
-        <v>-460462448.9135036</v>
+        <v>-741076423.4641184</v>
       </c>
       <c r="D166" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -18162,13 +18162,13 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>169510653.6271445</v>
+        <v>240392358.7967031</v>
       </c>
       <c r="C167" t="n">
-        <v>-400288688.0457355</v>
+        <v>-637962998.1665426</v>
       </c>
       <c r="D167" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -18270,13 +18270,13 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>197544351.2653601</v>
+        <v>282423728.746169</v>
       </c>
       <c r="C168" t="n">
-        <v>-428644976.7766817</v>
+        <v>-687942724.5554985</v>
       </c>
       <c r="D168" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -18370,13 +18370,13 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>225147600.0272056</v>
+        <v>324236869.8379742</v>
       </c>
       <c r="C169" t="n">
-        <v>-446621699.3602381</v>
+        <v>-722257016.7834637</v>
       </c>
       <c r="D169" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -18478,13 +18478,13 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>204452339.7224762</v>
+        <v>293455255.8377674</v>
       </c>
       <c r="C170" t="n">
-        <v>-427274707.5131188</v>
+        <v>-688952220.5230802</v>
       </c>
       <c r="D170" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -18582,13 +18582,13 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>211436154.0418527</v>
+        <v>304014132.5989069</v>
       </c>
       <c r="C171" t="n">
-        <v>-432216727.6757636</v>
+        <v>-698175436.5643777</v>
       </c>
       <c r="D171" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -18686,13 +18686,13 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>224428130.6488923</v>
+        <v>321884934.3653171</v>
       </c>
       <c r="C172" t="n">
-        <v>-460835459.0009965</v>
+        <v>-741012669.4637401</v>
       </c>
       <c r="D172" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -18794,13 +18794,13 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>230867323.3203529</v>
+        <v>332054352.0411416</v>
       </c>
       <c r="C173" t="n">
-        <v>-459433945.2831934</v>
+        <v>-741350897.6632477</v>
       </c>
       <c r="D173" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -18902,13 +18902,13 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>188099519.5105205</v>
+        <v>268688270.2184461</v>
       </c>
       <c r="C174" t="n">
-        <v>-414814430.0133743</v>
+        <v>-665700112.87985</v>
       </c>
       <c r="D174" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -19010,13 +19010,13 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>226042122.9440573</v>
+        <v>325429242.7824501</v>
       </c>
       <c r="C175" t="n">
-        <v>-448979737.9827173</v>
+        <v>-725720479.2212398</v>
       </c>
       <c r="D175" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -19114,13 +19114,13 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>227661733.7457307</v>
+        <v>326432980.3894434</v>
       </c>
       <c r="C176" t="n">
-        <v>-466707593.4775785</v>
+        <v>-749984518.1305887</v>
       </c>
       <c r="D176" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -19214,13 +19214,13 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>189877414.6763963</v>
+        <v>271529942.5186161</v>
       </c>
       <c r="C177" t="n">
-        <v>-414587537.4387551</v>
+        <v>-666187380.9058965</v>
       </c>
       <c r="D177" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -19318,13 +19318,13 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>194700531.8312197</v>
+        <v>277018094.9322309</v>
       </c>
       <c r="C178" t="n">
-        <v>-439028991.2625205</v>
+        <v>-700296723.8155724</v>
       </c>
       <c r="D178" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -19426,13 +19426,13 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>193084589.4705866</v>
+        <v>274734659.9312125</v>
       </c>
       <c r="C179" t="n">
-        <v>-435886815.5279012</v>
+        <v>-695469769.7531233</v>
       </c>
       <c r="D179" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -19534,13 +19534,13 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>215805372.3812869</v>
+        <v>307962529.6169906</v>
       </c>
       <c r="C180" t="n">
-        <v>-465711154.7927014</v>
+        <v>-744215916.061385</v>
       </c>
       <c r="D180" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
optimizing variogram parameters area 5
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -518,17 +518,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>241116409.9288566</v>
+        <v>422823.0001388173</v>
       </c>
       <c r="C2" t="n">
-        <v>-640516451.8613</v>
+        <v>7525442.527047326</v>
       </c>
       <c r="D2" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -626,17 +626,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>307840143.1691962</v>
+        <v>451013.4314993119</v>
       </c>
       <c r="C3" t="n">
-        <v>-744780978.6235237</v>
+        <v>7286868.704686873</v>
       </c>
       <c r="D3" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -734,17 +734,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>271851828.2804081</v>
+        <v>594545.9850944348</v>
       </c>
       <c r="C4" t="n">
-        <v>-668097385.7077036</v>
+        <v>7366095.350358819</v>
       </c>
       <c r="D4" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -846,17 +846,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>242120270.0446654</v>
+        <v>403945.0768397648</v>
       </c>
       <c r="C5" t="n">
-        <v>-644936176.4713304</v>
+        <v>7527910.87798272</v>
       </c>
       <c r="D5" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -954,17 +954,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>241816006.3231841</v>
+        <v>401216.148465685</v>
       </c>
       <c r="C6" t="n">
-        <v>-644771741.2745878</v>
+        <v>7529882.125589605</v>
       </c>
       <c r="D6" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1062,17 +1062,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>281822355.0883852</v>
+        <v>409155.6666583589</v>
       </c>
       <c r="C7" t="n">
-        <v>-711558460.5956467</v>
+        <v>7388267.661607112</v>
       </c>
       <c r="D7" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1166,17 +1166,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>242249524.6977128</v>
+        <v>408788.64986577</v>
       </c>
       <c r="C8" t="n">
-        <v>-644492121.4329234</v>
+        <v>7525883.127678607</v>
       </c>
       <c r="D8" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1274,17 +1274,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>272620302.1461084</v>
+        <v>573609.5498119397</v>
       </c>
       <c r="C9" t="n">
-        <v>-672338783.942363</v>
+        <v>7369187.59580075</v>
       </c>
       <c r="D9" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1386,17 +1386,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>236537929.2857987</v>
+        <v>395739.2028744464</v>
       </c>
       <c r="C10" t="n">
-        <v>-636000231.6287237</v>
+        <v>7550553.333618967</v>
       </c>
       <c r="D10" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1498,17 +1498,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>273356708.5186262</v>
+        <v>595482.5194309736</v>
       </c>
       <c r="C11" t="n">
-        <v>-670332549.0772539</v>
+        <v>7360555.884229297</v>
       </c>
       <c r="D11" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1606,17 +1606,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>324139109.2556922</v>
+        <v>570295.7162984037</v>
       </c>
       <c r="C12" t="n">
-        <v>-747799482.7227929</v>
+        <v>7194426.892189107</v>
       </c>
       <c r="D12" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1710,17 +1710,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>296404406.2602804</v>
+        <v>507596.7447241906</v>
       </c>
       <c r="C13" t="n">
-        <v>-718866741.0923098</v>
+        <v>7306910.773843632</v>
       </c>
       <c r="D13" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1810,17 +1810,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>234421992.9689757</v>
+        <v>429046.3551782307</v>
       </c>
       <c r="C14" t="n">
-        <v>-627593821.3777303</v>
+        <v>7547568.77555988</v>
       </c>
       <c r="D14" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1918,17 +1918,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>258153912.6522675</v>
+        <v>760472.461105651</v>
       </c>
       <c r="C15" t="n">
-        <v>-623356145.7801745</v>
+        <v>7374813.666059652</v>
       </c>
       <c r="D15" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2022,17 +2022,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>325883524.4871363</v>
+        <v>586409.6389365081</v>
       </c>
       <c r="C16" t="n">
-        <v>-747398630.4843992</v>
+        <v>7183700.825286468</v>
       </c>
       <c r="D16" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2130,17 +2130,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>303097785.9272359</v>
+        <v>518399.5160626545</v>
       </c>
       <c r="C17" t="n">
-        <v>-727024925.2444966</v>
+        <v>7280948.900331907</v>
       </c>
       <c r="D17" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2234,17 +2234,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>312636899.8738974</v>
+        <v>447691.7230347765</v>
       </c>
       <c r="C18" t="n">
-        <v>-752270474.6464767</v>
+        <v>7272079.333575497</v>
       </c>
       <c r="D18" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2342,17 +2342,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>329811766.0912105</v>
+        <v>641757.8655294247</v>
       </c>
       <c r="C19" t="n">
-        <v>-743155717.4879633</v>
+        <v>7154179.916507507</v>
       </c>
       <c r="D19" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2442,17 +2442,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>241284616.1454389</v>
+        <v>420719.6780329063</v>
       </c>
       <c r="C20" t="n">
-        <v>-641108597.9145137</v>
+        <v>7525508.513714559</v>
       </c>
       <c r="D20" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2550,17 +2550,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>334170860.8161556</v>
+        <v>620437.5570446817</v>
       </c>
       <c r="C21" t="n">
-        <v>-752220211.8294635</v>
+        <v>7145829.711649289</v>
       </c>
       <c r="D21" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2654,17 +2654,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>318489476.4800459</v>
+        <v>656030.3435174299</v>
       </c>
       <c r="C22" t="n">
-        <v>-726238810.2783819</v>
+        <v>7188356.034972786</v>
       </c>
       <c r="D22" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2754,17 +2754,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>240947429.0625636</v>
+        <v>405491.2708980456</v>
       </c>
       <c r="C23" t="n">
-        <v>-642618118.4559122</v>
+        <v>7531595.912204068</v>
       </c>
       <c r="D23" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2854,17 +2854,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>241537608.1774869</v>
+        <v>404713.2604548364</v>
       </c>
       <c r="C24" t="n">
-        <v>-643785192.149943</v>
+        <v>7529740.381576492</v>
       </c>
       <c r="D24" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2962,17 +2962,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>316028303.5171236</v>
+        <v>568072.7130961117</v>
       </c>
       <c r="C25" t="n">
-        <v>-737261747.7522157</v>
+        <v>7222234.914685098</v>
       </c>
       <c r="D25" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3070,17 +3070,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>292111793.1974413</v>
+        <v>553955.6541633958</v>
       </c>
       <c r="C26" t="n">
-        <v>-705272189.3632073</v>
+        <v>7307428.943578887</v>
       </c>
       <c r="D26" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3174,17 +3174,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>240803556.7309235</v>
+        <v>413821.4916065777</v>
       </c>
       <c r="C27" t="n">
-        <v>-641203341.7830828</v>
+        <v>7529429.834138079</v>
       </c>
       <c r="D27" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3282,17 +3282,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>301625905.0998349</v>
+        <v>718950.8143728292</v>
       </c>
       <c r="C28" t="n">
-        <v>-693639299.8900316</v>
+        <v>7229561.330213139</v>
       </c>
       <c r="D28" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3390,17 +3390,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>259524364.4675499</v>
+        <v>689479.0599372458</v>
       </c>
       <c r="C29" t="n">
-        <v>-635159537.19867</v>
+        <v>7385840.555939897</v>
       </c>
       <c r="D29" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3494,17 +3494,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>321125162.8406616</v>
+        <v>640364.9592321715</v>
       </c>
       <c r="C30" t="n">
-        <v>-732246856.0965803</v>
+        <v>7183844.981620431</v>
       </c>
       <c r="D30" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3594,17 +3594,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>316034106.6327591</v>
+        <v>568065.8525246648</v>
       </c>
       <c r="C31" t="n">
-        <v>-737270796.7957494</v>
+        <v>7222217.524079368</v>
       </c>
       <c r="D31" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3702,17 +3702,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>240675486.9111191</v>
+        <v>408978.8275499512</v>
       </c>
       <c r="C32" t="n">
-        <v>-641645409.746622</v>
+        <v>7531442.590570908</v>
       </c>
       <c r="D32" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3810,17 +3810,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>309591520.6783481</v>
+        <v>432660.8029019876</v>
       </c>
       <c r="C33" t="n">
-        <v>-750338693.3007903</v>
+        <v>7287266.453172042</v>
       </c>
       <c r="D33" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3914,17 +3914,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>241180851.5727562</v>
+        <v>402680.6572135365</v>
       </c>
       <c r="C34" t="n">
-        <v>-643428200.0245736</v>
+        <v>7531672.625937978</v>
       </c>
       <c r="D34" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4022,17 +4022,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>328636380.8735353</v>
+        <v>648062.4098775064</v>
       </c>
       <c r="C35" t="n">
-        <v>-740617600.2250655</v>
+        <v>7156317.765654799</v>
       </c>
       <c r="D35" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4126,17 +4126,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>324854430.5347658</v>
+        <v>585517.9007419647</v>
       </c>
       <c r="C36" t="n">
-        <v>-746200833.3122867</v>
+        <v>7187408.106334507</v>
       </c>
       <c r="D36" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4238,17 +4238,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>261924235.3221091</v>
+        <v>679482.7733917895</v>
       </c>
       <c r="C37" t="n">
-        <v>-640369267.1781435</v>
+        <v>7379568.764875205</v>
       </c>
       <c r="D37" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4342,17 +4342,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>266105340.8550061</v>
+        <v>697218.2558684414</v>
       </c>
       <c r="C38" t="n">
-        <v>-644524175.3137047</v>
+        <v>7360280.072632506</v>
       </c>
       <c r="D38" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4450,17 +4450,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>233692973.6274313</v>
+        <v>385901.2558721581</v>
       </c>
       <c r="C39" t="n">
-        <v>-632156415.2001097</v>
+        <v>7564001.44550652</v>
       </c>
       <c r="D39" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4562,17 +4562,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>239958332.6812091</v>
+        <v>424332.5844982759</v>
       </c>
       <c r="C40" t="n">
-        <v>-638233803.9230567</v>
+        <v>7529112.568427877</v>
       </c>
       <c r="D40" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4674,17 +4674,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>315871578.7534108</v>
+        <v>569643.0684379223</v>
       </c>
       <c r="C41" t="n">
-        <v>-736791243.5112112</v>
+        <v>7222285.613839785</v>
       </c>
       <c r="D41" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4782,17 +4782,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>238081039.3346827</v>
+        <v>402406.4354549267</v>
       </c>
       <c r="C42" t="n">
-        <v>-637879350.5167651</v>
+        <v>7542852.907356113</v>
       </c>
       <c r="D42" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4894,17 +4894,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>237917772.9119691</v>
+        <v>437023.185092857</v>
       </c>
       <c r="C43" t="n">
-        <v>-632825810.5677013</v>
+        <v>7532468.581112547</v>
       </c>
       <c r="D43" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5002,17 +5002,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>271453178.3149346</v>
+        <v>593001.3245233108</v>
       </c>
       <c r="C44" t="n">
-        <v>-667689887.1368873</v>
+        <v>7367918.094725985</v>
       </c>
       <c r="D44" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5114,17 +5114,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>228517245.6278447</v>
+        <v>439224.5486118381</v>
       </c>
       <c r="C45" t="n">
-        <v>-615422880.303871</v>
+        <v>7565894.75324164</v>
       </c>
       <c r="D45" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5226,17 +5226,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>242289512.9431651</v>
+        <v>401842.916054123</v>
       </c>
       <c r="C46" t="n">
-        <v>-645532582.8692462</v>
+        <v>7527990.288472353</v>
       </c>
       <c r="D46" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5330,17 +5330,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>237611354.9062354</v>
+        <v>388715.6373236501</v>
       </c>
       <c r="C47" t="n">
-        <v>-638922073.3417053</v>
+        <v>7548996.648429874</v>
       </c>
       <c r="D47" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5442,17 +5442,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>238716552.1387896</v>
+        <v>433477.7838170429</v>
       </c>
       <c r="C48" t="n">
-        <v>-634747027.1713309</v>
+        <v>7530698.264778861</v>
       </c>
       <c r="D48" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5550,17 +5550,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>322745359.7031357</v>
+        <v>590088.3297374767</v>
       </c>
       <c r="C49" t="n">
-        <v>-742664354.0434316</v>
+        <v>7193087.563682824</v>
       </c>
       <c r="D49" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5658,17 +5658,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>242277238.6826189</v>
+        <v>421309.4212496581</v>
       </c>
       <c r="C50" t="n">
-        <v>-642799677.7142836</v>
+        <v>7521773.247238778</v>
       </c>
       <c r="D50" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5762,17 +5762,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>277669410.9749006</v>
+        <v>778993.4381261227</v>
       </c>
       <c r="C51" t="n">
-        <v>-650638472.9506352</v>
+        <v>7299986.83529006</v>
       </c>
       <c r="D51" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5870,17 +5870,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>284453677.0661486</v>
+        <v>410340.4763310733</v>
       </c>
       <c r="C52" t="n">
-        <v>-715576330.4317623</v>
+        <v>7378952.937187641</v>
       </c>
       <c r="D52" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -5974,17 +5974,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>303309631.9706399</v>
+        <v>463408.7043260257</v>
       </c>
       <c r="C53" t="n">
-        <v>-736125207.7363403</v>
+        <v>7297853.838466587</v>
       </c>
       <c r="D53" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6082,17 +6082,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>229115395.803687</v>
+        <v>444667.0044273772</v>
       </c>
       <c r="C54" t="n">
-        <v>-615796001.4970576</v>
+        <v>7562048.963216691</v>
       </c>
       <c r="D54" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6194,17 +6194,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>240709029.5342582</v>
+        <v>421470.9503357491</v>
       </c>
       <c r="C55" t="n">
-        <v>-639974477.0186136</v>
+        <v>7527329.485975892</v>
       </c>
       <c r="D55" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6302,17 +6302,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>302373980.5765743</v>
+        <v>526067.6630022393</v>
       </c>
       <c r="C56" t="n">
-        <v>-724754887.8731717</v>
+        <v>7281008.696502964</v>
       </c>
       <c r="D56" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6406,17 +6406,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>226115473.4363479</v>
+        <v>384404.2276939754</v>
       </c>
       <c r="C57" t="n">
-        <v>-618321946.9817134</v>
+        <v>7591962.608249241</v>
       </c>
       <c r="D57" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -6510,17 +6510,17 @@
         <v>1549</v>
       </c>
       <c r="B58" t="n">
-        <v>287378257.0332168</v>
+        <v>414448.1731552719</v>
       </c>
       <c r="C58" t="n">
-        <v>-719565294.9595512</v>
+        <v>7367681.028654348</v>
       </c>
       <c r="D58" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -6614,17 +6614,17 @@
         <v>1552</v>
       </c>
       <c r="B59" t="n">
-        <v>264899440.4536139</v>
+        <v>705283.5520898863</v>
       </c>
       <c r="C59" t="n">
-        <v>-641513779.7746129</v>
+        <v>7362709.877786176</v>
       </c>
       <c r="D59" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -6722,17 +6722,17 @@
         <v>1553</v>
       </c>
       <c r="B60" t="n">
-        <v>278445845.2283827</v>
+        <v>428504.0728901725</v>
       </c>
       <c r="C60" t="n">
-        <v>-703174320.3226094</v>
+        <v>7393290.601893418</v>
       </c>
       <c r="D60" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -6826,17 +6826,17 @@
         <v>1556</v>
       </c>
       <c r="B61" t="n">
-        <v>313956072.1801931</v>
+        <v>364167.4705087786</v>
       </c>
       <c r="C61" t="n">
-        <v>-768109334.7570126</v>
+        <v>7297116.842234123</v>
       </c>
       <c r="D61" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -6930,17 +6930,17 @@
         <v>1559</v>
       </c>
       <c r="B62" t="n">
-        <v>322741874.7063678</v>
+        <v>590092.4094163297</v>
       </c>
       <c r="C62" t="n">
-        <v>-742659074.352662</v>
+        <v>7193098.011324367</v>
       </c>
       <c r="D62" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -7038,17 +7038,17 @@
         <v>1597</v>
       </c>
       <c r="B63" t="n">
-        <v>263258404.8438024</v>
+        <v>754559.5701349006</v>
       </c>
       <c r="C63" t="n">
-        <v>-632173952.7290845</v>
+        <v>7357457.446217685</v>
       </c>
       <c r="D63" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -7146,17 +7146,17 @@
         <v>1610</v>
       </c>
       <c r="B64" t="n">
-        <v>281833903.6966872</v>
+        <v>415018.0448537197</v>
       </c>
       <c r="C64" t="n">
-        <v>-710675747.4114839</v>
+        <v>7386252.235449532</v>
       </c>
       <c r="D64" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -7258,17 +7258,17 @@
         <v>1611</v>
       </c>
       <c r="B65" t="n">
-        <v>259864791.7006577</v>
+        <v>393866.9952033143</v>
       </c>
       <c r="C65" t="n">
-        <v>-677451073.353865</v>
+        <v>7468780.921490044</v>
       </c>
       <c r="D65" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -7366,17 +7366,17 @@
         <v>1636</v>
       </c>
       <c r="B66" t="n">
-        <v>279469335.2922495</v>
+        <v>793848.6559708756</v>
       </c>
       <c r="C66" t="n">
-        <v>-651169910.9945309</v>
+        <v>7290260.126774631</v>
       </c>
       <c r="D66" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -7474,17 +7474,17 @@
         <v>1637</v>
       </c>
       <c r="B67" t="n">
-        <v>284456288.9917687</v>
+        <v>410337.1139574873</v>
       </c>
       <c r="C67" t="n">
-        <v>-715581003.6488818</v>
+        <v>7378945.240007831</v>
       </c>
       <c r="D67" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -7582,17 +7582,17 @@
         <v>1643</v>
       </c>
       <c r="B68" t="n">
-        <v>259723469.9714658</v>
+        <v>705411.5012919909</v>
       </c>
       <c r="C68" t="n">
-        <v>-633302860.1094917</v>
+        <v>7381384.438635441</v>
       </c>
       <c r="D68" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -7690,17 +7690,17 @@
         <v>1668</v>
       </c>
       <c r="B69" t="n">
-        <v>261164753.2626413</v>
+        <v>827178.5078480255</v>
       </c>
       <c r="C69" t="n">
-        <v>-619107805.3630104</v>
+        <v>7350027.173207692</v>
       </c>
       <c r="D69" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -7798,17 +7798,17 @@
         <v>1671</v>
       </c>
       <c r="B70" t="n">
-        <v>272777273.7243389</v>
+        <v>704315.0658106438</v>
       </c>
       <c r="C70" t="n">
-        <v>-653863315.1116563</v>
+        <v>7334696.005952516</v>
       </c>
       <c r="D70" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -7902,17 +7902,17 @@
         <v>1683</v>
       </c>
       <c r="B71" t="n">
-        <v>305892356.1042734</v>
+        <v>622134.3892227954</v>
       </c>
       <c r="C71" t="n">
-        <v>-714595899.8409623</v>
+        <v>7240708.73367288</v>
       </c>
       <c r="D71" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -8006,17 +8006,17 @@
         <v>1684</v>
       </c>
       <c r="B72" t="n">
-        <v>241288520.0071773</v>
+        <v>420714.5822642142</v>
       </c>
       <c r="C72" t="n">
-        <v>-641116285.9121094</v>
+        <v>7525496.171109289</v>
       </c>
       <c r="D72" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -8114,17 +8114,17 @@
         <v>1724</v>
       </c>
       <c r="B73" t="n">
-        <v>316029866.5670241</v>
+        <v>568070.8652271603</v>
       </c>
       <c r="C73" t="n">
-        <v>-737264185.0951921</v>
+        <v>7222230.230568401</v>
       </c>
       <c r="D73" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -8222,17 +8222,17 @@
         <v>1786</v>
       </c>
       <c r="B74" t="n">
-        <v>279681540.434641</v>
+        <v>517897.6597152865</v>
       </c>
       <c r="C74" t="n">
-        <v>-691676297.3159117</v>
+        <v>7360848.522584329</v>
       </c>
       <c r="D74" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -8326,17 +8326,17 @@
         <v>1788</v>
       </c>
       <c r="B75" t="n">
-        <v>238606731.4384664</v>
+        <v>402334.5145603271</v>
       </c>
       <c r="C75" t="n">
-        <v>-638839898.102951</v>
+        <v>7540991.602727064</v>
       </c>
       <c r="D75" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -8438,17 +8438,17 @@
         <v>1793</v>
       </c>
       <c r="B76" t="n">
-        <v>330076763.9282188</v>
+        <v>572359.5505096086</v>
       </c>
       <c r="C76" t="n">
-        <v>-755208195.1460632</v>
+        <v>7174025.31142854</v>
       </c>
       <c r="D76" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -8546,17 +8546,17 @@
         <v>1816</v>
       </c>
       <c r="B77" t="n">
-        <v>299439780.3822055</v>
+        <v>632953.2160392514</v>
       </c>
       <c r="C77" t="n">
-        <v>-703812662.4923407</v>
+        <v>7259778.363588417</v>
       </c>
       <c r="D77" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -8654,17 +8654,17 @@
         <v>1871</v>
       </c>
       <c r="B78" t="n">
-        <v>251216849.3362035</v>
+        <v>727838.3447125108</v>
       </c>
       <c r="C78" t="n">
-        <v>-616569650.678416</v>
+        <v>7407376.859851267</v>
       </c>
       <c r="D78" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -8762,17 +8762,17 @@
         <v>1961</v>
       </c>
       <c r="B79" t="n">
-        <v>226164033.8365528</v>
+        <v>383725.8459431626</v>
       </c>
       <c r="C79" t="n">
-        <v>-618504264.9674021</v>
+        <v>7592006.341748471</v>
       </c>
       <c r="D79" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -8870,17 +8870,17 @@
         <v>1985</v>
       </c>
       <c r="B80" t="n">
-        <v>287387840.2114912</v>
+        <v>414435.8746544203</v>
       </c>
       <c r="C80" t="n">
-        <v>-719582297.4409394</v>
+        <v>7367652.856344703</v>
       </c>
       <c r="D80" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -8974,17 +8974,17 @@
         <v>1996</v>
       </c>
       <c r="B81" t="n">
-        <v>283149053.8281337</v>
+        <v>412673.4235208518</v>
       </c>
       <c r="C81" t="n">
-        <v>-713138153.5136787</v>
+        <v>7382581.441586836</v>
       </c>
       <c r="D81" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -9082,17 +9082,17 @@
         <v>2007</v>
       </c>
       <c r="B82" t="n">
-        <v>285278721.9658185</v>
+        <v>407314.2720218997</v>
       </c>
       <c r="C82" t="n">
-        <v>-717356056.9629877</v>
+        <v>7377190.661707142</v>
       </c>
       <c r="D82" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -9190,17 +9190,17 @@
         <v>2009</v>
       </c>
       <c r="B83" t="n">
-        <v>295826005.8928929</v>
+        <v>723787.2073493205</v>
       </c>
       <c r="C83" t="n">
-        <v>-684845866.2343649</v>
+        <v>7248572.024052578</v>
       </c>
       <c r="D83" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -9294,17 +9294,17 @@
         <v>2052</v>
       </c>
       <c r="B84" t="n">
-        <v>272014231.2749047</v>
+        <v>790262.1937427302</v>
       </c>
       <c r="C84" t="n">
-        <v>-640643632.4785765</v>
+        <v>7317937.23898467</v>
       </c>
       <c r="D84" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -9398,17 +9398,17 @@
         <v>2054</v>
       </c>
       <c r="B85" t="n">
-        <v>320789113.3239766</v>
+        <v>598663.1839319061</v>
       </c>
       <c r="C85" t="n">
-        <v>-738656926.3217984</v>
+        <v>7197091.63736374</v>
       </c>
       <c r="D85" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -9502,17 +9502,17 @@
         <v>2064</v>
       </c>
       <c r="B86" t="n">
-        <v>285970464.894981</v>
+        <v>405767.7027150932</v>
       </c>
       <c r="C86" t="n">
-        <v>-718693340.5180732</v>
+        <v>7375381.027371443</v>
       </c>
       <c r="D86" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -9610,17 +9610,17 @@
         <v>2075</v>
       </c>
       <c r="B87" t="n">
-        <v>259513822.2850575</v>
+        <v>762480.8616364233</v>
       </c>
       <c r="C87" t="n">
-        <v>-625232380.7979548</v>
+        <v>7369402.187121131</v>
       </c>
       <c r="D87" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -9718,17 +9718,17 @@
         <v>2084</v>
       </c>
       <c r="B88" t="n">
-        <v>273641607.671856</v>
+        <v>439843.9287411383</v>
       </c>
       <c r="C88" t="n">
-        <v>-693677903.9160447</v>
+        <v>7406029.903836646</v>
       </c>
       <c r="D88" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -9822,17 +9822,17 @@
         <v>2128</v>
       </c>
       <c r="B89" t="n">
-        <v>226786550.2516718</v>
+        <v>382271.6480455336</v>
       </c>
       <c r="C89" t="n">
-        <v>-619864072.960627</v>
+        <v>7590211.624238232</v>
       </c>
       <c r="D89" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -9926,17 +9926,17 @@
         <v>2163</v>
       </c>
       <c r="B90" t="n">
-        <v>260213516.9754689</v>
+        <v>402335.643714165</v>
       </c>
       <c r="C90" t="n">
-        <v>-676810304.4705592</v>
+        <v>7464744.675496253</v>
       </c>
       <c r="D90" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -10034,17 +10034,17 @@
         <v>2235</v>
       </c>
       <c r="B91" t="n">
-        <v>226169188.3207233</v>
+        <v>383718.8813232478</v>
       </c>
       <c r="C91" t="n">
-        <v>-618514843.849395</v>
+        <v>7591989.812414211</v>
       </c>
       <c r="D91" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -10146,17 +10146,17 @@
         <v>2261</v>
       </c>
       <c r="B92" t="n">
-        <v>254974684.4502476</v>
+        <v>539831.0236638299</v>
       </c>
       <c r="C92" t="n">
-        <v>-648327480.5640734</v>
+        <v>7440963.848228727</v>
       </c>
       <c r="D92" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -10254,17 +10254,17 @@
         <v>2267</v>
       </c>
       <c r="B93" t="n">
-        <v>224717828.7056844</v>
+        <v>389353.0613288408</v>
       </c>
       <c r="C93" t="n">
-        <v>-615039144.3747218</v>
+        <v>7595463.263758845</v>
       </c>
       <c r="D93" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -10358,17 +10358,17 @@
         <v>2283</v>
       </c>
       <c r="B94" t="n">
-        <v>226167038.3015949</v>
+        <v>383721.7863796732</v>
       </c>
       <c r="C94" t="n">
-        <v>-618510431.2372736</v>
+        <v>7591996.707043167</v>
       </c>
       <c r="D94" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -10462,17 +10462,17 @@
         <v>2320</v>
       </c>
       <c r="B95" t="n">
-        <v>224820170.6684155</v>
+        <v>387990.2999005239</v>
       </c>
       <c r="C95" t="n">
-        <v>-615413964.9004151</v>
+        <v>7595529.493387843</v>
       </c>
       <c r="D95" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -10566,17 +10566,17 @@
         <v>2330</v>
       </c>
       <c r="B96" t="n">
-        <v>274781804.7242188</v>
+        <v>669452.4467849245</v>
       </c>
       <c r="C96" t="n">
-        <v>-661899490.7891164</v>
+        <v>7336131.153987038</v>
       </c>
       <c r="D96" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -10670,17 +10670,17 @@
         <v>2357</v>
       </c>
       <c r="B97" t="n">
-        <v>233259970.1339031</v>
+        <v>391429.212175432</v>
       </c>
       <c r="C97" t="n">
-        <v>-630603626.1936203</v>
+        <v>7563757.379410667</v>
       </c>
       <c r="D97" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -10782,17 +10782,17 @@
         <v>2364</v>
       </c>
       <c r="B98" t="n">
-        <v>274067975.5643117</v>
+        <v>569239.5613440264</v>
       </c>
       <c r="C98" t="n">
-        <v>-675262354.2216074</v>
+        <v>7365353.885484916</v>
       </c>
       <c r="D98" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -10890,17 +10890,17 @@
         <v>2380</v>
       </c>
       <c r="B99" t="n">
-        <v>285555902.5664799</v>
+        <v>404339.0276015802</v>
       </c>
       <c r="C99" t="n">
-        <v>-718258134.6457069</v>
+        <v>7377267.93003197</v>
       </c>
       <c r="D99" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -10998,17 +10998,17 @@
         <v>2385</v>
       </c>
       <c r="B100" t="n">
-        <v>277547055.5154095</v>
+        <v>426389.9074570178</v>
       </c>
       <c r="C100" t="n">
-        <v>-702044307.992703</v>
+        <v>7397057.334183707</v>
       </c>
       <c r="D100" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -11102,17 +11102,17 @@
         <v>2389</v>
       </c>
       <c r="B101" t="n">
-        <v>323741591.2967488</v>
+        <v>647260.2346404803</v>
       </c>
       <c r="C101" t="n">
-        <v>-734507953.3498362</v>
+        <v>7173046.349524124</v>
       </c>
       <c r="D101" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -11210,17 +11210,17 @@
         <v>2418</v>
       </c>
       <c r="B102" t="n">
-        <v>241124046.2670941</v>
+        <v>422813.0446212821</v>
       </c>
       <c r="C102" t="n">
-        <v>-640531487.5712001</v>
+        <v>7525418.358305623</v>
       </c>
       <c r="D102" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -11318,17 +11318,17 @@
         <v>2443</v>
       </c>
       <c r="B103" t="n">
-        <v>262243332.2856171</v>
+        <v>409920.3594865833</v>
       </c>
       <c r="C103" t="n">
-        <v>-679154550.8067428</v>
+        <v>7455181.222219932</v>
       </c>
       <c r="D103" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -11430,17 +11430,17 @@
         <v>2445</v>
       </c>
       <c r="B104" t="n">
-        <v>271543321.4000739</v>
+        <v>469900.8002904762</v>
       </c>
       <c r="C104" t="n">
-        <v>-685788883.8156843</v>
+        <v>7403678.552845351</v>
       </c>
       <c r="D104" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -11538,17 +11538,17 @@
         <v>2449</v>
       </c>
       <c r="B105" t="n">
-        <v>247118332.88347</v>
+        <v>464459.3821369232</v>
       </c>
       <c r="C105" t="n">
-        <v>-645348511.1651821</v>
+        <v>7491066.084930793</v>
       </c>
       <c r="D105" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -11646,17 +11646,17 @@
         <v>2461</v>
       </c>
       <c r="B106" t="n">
-        <v>337201433.0136378</v>
+        <v>366853.0474747586</v>
       </c>
       <c r="C106" t="n">
-        <v>-800345615.03389</v>
+        <v>7220754.392227514</v>
       </c>
       <c r="D106" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -11754,17 +11754,17 @@
         <v>2528</v>
       </c>
       <c r="B107" t="n">
-        <v>304537376.5776873</v>
+        <v>567174.9081824664</v>
       </c>
       <c r="C107" t="n">
-        <v>-721360980.5391968</v>
+        <v>7261232.535008149</v>
       </c>
       <c r="D107" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -11862,17 +11862,17 @@
         <v>2609</v>
       </c>
       <c r="B108" t="n">
-        <v>239524588.7008033</v>
+        <v>397376.1849744547</v>
       </c>
       <c r="C108" t="n">
-        <v>-641184656.1507736</v>
+        <v>7539315.330421793</v>
       </c>
       <c r="D108" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -11970,17 +11970,17 @@
         <v>2614</v>
       </c>
       <c r="B109" t="n">
-        <v>285177471.3559144</v>
+        <v>747622.3765616242</v>
       </c>
       <c r="C109" t="n">
-        <v>-666124678.5824778</v>
+        <v>7280326.687097363</v>
       </c>
       <c r="D109" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -12078,17 +12078,17 @@
         <v>2617</v>
       </c>
       <c r="B110" t="n">
-        <v>224615062.5923977</v>
+        <v>450489.7582604677</v>
       </c>
       <c r="C110" t="n">
-        <v>-606717622.250353</v>
+        <v>7576800.85477192</v>
       </c>
       <c r="D110" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -12190,17 +12190,17 @@
         <v>2620</v>
       </c>
       <c r="B111" t="n">
-        <v>272249754.7655263</v>
+        <v>710339.3015028904</v>
       </c>
       <c r="C111" t="n">
-        <v>-652204163.8814831</v>
+        <v>7335141.778801956</v>
       </c>
       <c r="D111" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -12294,17 +12294,17 @@
         <v>2640</v>
       </c>
       <c r="B112" t="n">
-        <v>287408714.7674247</v>
+        <v>396053.62525233</v>
       </c>
       <c r="C112" t="n">
-        <v>-722485408.0931526</v>
+        <v>7373862.411237928</v>
       </c>
       <c r="D112" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -12398,17 +12398,17 @@
         <v>2645</v>
       </c>
       <c r="B113" t="n">
-        <v>228605661.3841797</v>
+        <v>444704.7907449754</v>
       </c>
       <c r="C113" t="n">
-        <v>-614854348.7632763</v>
+        <v>7563900.888378733</v>
       </c>
       <c r="D113" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -12510,17 +12510,17 @@
         <v>2713</v>
       </c>
       <c r="B114" t="n">
-        <v>228201033.2161114</v>
+        <v>443363.6732012552</v>
       </c>
       <c r="C114" t="n">
-        <v>-614288686.2252672</v>
+        <v>7565788.758657504</v>
       </c>
       <c r="D114" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -12622,17 +12622,17 @@
         <v>2722</v>
       </c>
       <c r="B115" t="n">
-        <v>326181861.1804546</v>
+        <v>367652.259629715</v>
       </c>
       <c r="C115" t="n">
-        <v>-785049507.6016762</v>
+        <v>7256028.81467634</v>
       </c>
       <c r="D115" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -12722,17 +12722,17 @@
         <v>2749</v>
       </c>
       <c r="B116" t="n">
-        <v>272145706.4409218</v>
+        <v>669640.2285336041</v>
       </c>
       <c r="C116" t="n">
-        <v>-657809791.884734</v>
+        <v>7345433.276130389</v>
       </c>
       <c r="D116" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -12826,17 +12826,17 @@
         <v>2763</v>
       </c>
       <c r="B117" t="n">
-        <v>271862757.4238549</v>
+        <v>600557.637797766</v>
       </c>
       <c r="C117" t="n">
-        <v>-667248888.2380273</v>
+        <v>7364421.865823336</v>
       </c>
       <c r="D117" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -12938,17 +12938,17 @@
         <v>2851</v>
       </c>
       <c r="B118" t="n">
-        <v>315105951.0574893</v>
+        <v>600393.0921995796</v>
       </c>
       <c r="C118" t="n">
-        <v>-730747426.1765029</v>
+        <v>7215709.499915746</v>
       </c>
       <c r="D118" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -13042,17 +13042,17 @@
         <v>2855</v>
       </c>
       <c r="B119" t="n">
-        <v>272863476.7660523</v>
+        <v>497782.9113988071</v>
       </c>
       <c r="C119" t="n">
-        <v>-683812167.8925201</v>
+        <v>7390496.471405526</v>
       </c>
       <c r="D119" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -13142,17 +13142,17 @@
         <v>2856</v>
       </c>
       <c r="B120" t="n">
-        <v>236410689.9844101</v>
+        <v>436466.800330822</v>
       </c>
       <c r="C120" t="n">
-        <v>-630186134.2139621</v>
+        <v>7538074.706984714</v>
       </c>
       <c r="D120" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -13246,17 +13246,17 @@
         <v>2858</v>
       </c>
       <c r="B121" t="n">
-        <v>226165597.0039313</v>
+        <v>383723.7338277422</v>
       </c>
       <c r="C121" t="n">
-        <v>-618507473.1671422</v>
+        <v>7592001.328981454</v>
       </c>
       <c r="D121" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -13354,17 +13354,17 @@
         <v>2859</v>
       </c>
       <c r="B122" t="n">
-        <v>225900681.1727424</v>
+        <v>446965.5634673933</v>
       </c>
       <c r="C122" t="n">
-        <v>-609564829.8951237</v>
+        <v>7573131.755081054</v>
       </c>
       <c r="D122" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -13466,17 +13466,17 @@
         <v>2873</v>
       </c>
       <c r="B123" t="n">
-        <v>227530799.8906835</v>
+        <v>445475.1194111918</v>
       </c>
       <c r="C123" t="n">
-        <v>-612773015.4131714</v>
+        <v>7567601.635024867</v>
       </c>
       <c r="D123" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -13578,17 +13578,17 @@
         <v>2914</v>
       </c>
       <c r="B124" t="n">
-        <v>292912636.687263</v>
+        <v>621810.8103163663</v>
       </c>
       <c r="C124" t="n">
-        <v>-696098767.0576134</v>
+        <v>7285316.554902539</v>
       </c>
       <c r="D124" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -13678,17 +13678,17 @@
         <v>2987</v>
       </c>
       <c r="B125" t="n">
-        <v>232006809.2622156</v>
+        <v>453416.9831956982</v>
       </c>
       <c r="C125" t="n">
-        <v>-619910906.2042223</v>
+        <v>7548850.096561186</v>
       </c>
       <c r="D125" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -13782,17 +13782,17 @@
         <v>3007</v>
       </c>
       <c r="B126" t="n">
-        <v>269835674.2570578</v>
+        <v>611592.6100460046</v>
       </c>
       <c r="C126" t="n">
-        <v>-662465103.058249</v>
+        <v>7368598.606297649</v>
       </c>
       <c r="D126" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -13890,17 +13890,17 @@
         <v>3010</v>
       </c>
       <c r="B127" t="n">
-        <v>260004362.5773549</v>
+        <v>828987.291295761</v>
       </c>
       <c r="C127" t="n">
-        <v>-617075096.1658553</v>
+        <v>7353960.948327379</v>
       </c>
       <c r="D127" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -14002,17 +14002,17 @@
         <v>3025</v>
       </c>
       <c r="B128" t="n">
-        <v>226163492.6711283</v>
+        <v>383726.5771532588</v>
       </c>
       <c r="C128" t="n">
-        <v>-618503154.2930305</v>
+        <v>7592008.077162812</v>
       </c>
       <c r="D128" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -14106,17 +14106,17 @@
         <v>3041</v>
       </c>
       <c r="B129" t="n">
-        <v>272231389.1081073</v>
+        <v>572065.6433788443</v>
       </c>
       <c r="C129" t="n">
-        <v>-671946254.9176275</v>
+        <v>7370981.487775771</v>
       </c>
       <c r="D129" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -14214,17 +14214,17 @@
         <v>3090</v>
       </c>
       <c r="B130" t="n">
-        <v>234504158.7149849</v>
+        <v>570671.744298632</v>
       </c>
       <c r="C130" t="n">
-        <v>-608853674.238616</v>
+        <v>7506660.864765343</v>
       </c>
       <c r="D130" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -14322,17 +14322,17 @@
         <v>3106</v>
       </c>
       <c r="B131" t="n">
-        <v>257577191.2416937</v>
+        <v>539967.4751042218</v>
       </c>
       <c r="C131" t="n">
-        <v>-652668699.3305537</v>
+        <v>7431673.784536626</v>
       </c>
       <c r="D131" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -14430,17 +14430,17 @@
         <v>3124</v>
       </c>
       <c r="B132" t="n">
-        <v>230057768.3387714</v>
+        <v>452174.9311583586</v>
       </c>
       <c r="C132" t="n">
-        <v>-616520724.873842</v>
+        <v>7556332.266056828</v>
       </c>
       <c r="D132" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -14538,17 +14538,17 @@
         <v>3201</v>
       </c>
       <c r="B133" t="n">
-        <v>225607327.2208885</v>
+        <v>384478.042694183</v>
       </c>
       <c r="C133" t="n">
-        <v>-617361142.6686318</v>
+        <v>7593792.795184806</v>
       </c>
       <c r="D133" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -14642,17 +14642,17 @@
         <v>3202</v>
       </c>
       <c r="B134" t="n">
-        <v>261178897.8119061</v>
+        <v>472457.6527888828</v>
       </c>
       <c r="C134" t="n">
-        <v>-668284335.5192387</v>
+        <v>7438943.410384167</v>
       </c>
       <c r="D134" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -14754,17 +14754,17 @@
         <v>3225</v>
       </c>
       <c r="B135" t="n">
-        <v>278202125.5705481</v>
+        <v>796518.4161216137</v>
       </c>
       <c r="C135" t="n">
-        <v>-648938013.488188</v>
+        <v>7294240.829803186</v>
       </c>
       <c r="D135" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -14862,17 +14862,17 @@
         <v>3261</v>
       </c>
       <c r="B136" t="n">
-        <v>239771508.8132858</v>
+        <v>439654.4736789956</v>
       </c>
       <c r="C136" t="n">
-        <v>-635790051.9050461</v>
+        <v>7524984.020991635</v>
       </c>
       <c r="D136" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -14970,17 +14970,17 @@
         <v>3345</v>
       </c>
       <c r="B137" t="n">
-        <v>268395005.4511626</v>
+        <v>597874.7966290781</v>
       </c>
       <c r="C137" t="n">
-        <v>-662134595.8958046</v>
+        <v>7377365.426627968</v>
       </c>
       <c r="D137" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -15078,17 +15078,17 @@
         <v>3380</v>
       </c>
       <c r="B138" t="n">
-        <v>251362684.6463775</v>
+        <v>507905.568870945</v>
       </c>
       <c r="C138" t="n">
-        <v>-646644373.9702441</v>
+        <v>7462990.403153609</v>
       </c>
       <c r="D138" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -15182,17 +15182,17 @@
         <v>3482</v>
       </c>
       <c r="B139" t="n">
-        <v>304686586.0029499</v>
+        <v>366329.6275398433</v>
       </c>
       <c r="C139" t="n">
-        <v>-753959532.9839897</v>
+        <v>7326783.189303711</v>
       </c>
       <c r="D139" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -15290,17 +15290,17 @@
         <v>3487</v>
       </c>
       <c r="B140" t="n">
-        <v>278683013.3011628</v>
+        <v>456361.2898843428</v>
       </c>
       <c r="C140" t="n">
-        <v>-699336737.2919977</v>
+        <v>7383412.108057517</v>
       </c>
       <c r="D140" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -15394,17 +15394,17 @@
         <v>3500</v>
       </c>
       <c r="B141" t="n">
-        <v>229122462.9280137</v>
+        <v>444657.8554364101</v>
       </c>
       <c r="C141" t="n">
-        <v>-615810200.1162999</v>
+        <v>7562025.921142353</v>
       </c>
       <c r="D141" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -15506,17 +15506,17 @@
         <v>3510</v>
       </c>
       <c r="B142" t="n">
-        <v>286652264.0822604</v>
+        <v>672768.4835952614</v>
       </c>
       <c r="C142" t="n">
-        <v>-679269130.0227554</v>
+        <v>7293509.317555598</v>
       </c>
       <c r="D142" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -15610,17 +15610,17 @@
         <v>3543</v>
       </c>
       <c r="B143" t="n">
-        <v>268735102.2271433</v>
+        <v>612182.4967714186</v>
       </c>
       <c r="C143" t="n">
-        <v>-660636716.3574395</v>
+        <v>7372330.057555402</v>
       </c>
       <c r="D143" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -15722,17 +15722,17 @@
         <v>3588</v>
       </c>
       <c r="B144" t="n">
-        <v>243601156.586562</v>
+        <v>728433.5137220931</v>
       </c>
       <c r="C144" t="n">
-        <v>-603939255.377998</v>
+        <v>7435412.922395073</v>
       </c>
       <c r="D144" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -15830,17 +15830,17 @@
         <v>3731</v>
       </c>
       <c r="B145" t="n">
-        <v>315019437.858991</v>
+        <v>714304.8037613939</v>
       </c>
       <c r="C145" t="n">
-        <v>-712316144.3485979</v>
+        <v>7184478.611043642</v>
       </c>
       <c r="D145" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -15934,17 +15934,17 @@
         <v>3742</v>
       </c>
       <c r="B146" t="n">
-        <v>230568678.7818459</v>
+        <v>439047.5535942831</v>
       </c>
       <c r="C146" t="n">
-        <v>-619213379.4449077</v>
+        <v>7558462.652592706</v>
       </c>
       <c r="D146" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -16046,17 +16046,17 @@
         <v>3757</v>
       </c>
       <c r="B147" t="n">
-        <v>274703017.1193153</v>
+        <v>433932.7497139967</v>
       </c>
       <c r="C147" t="n">
-        <v>-696292944.7845743</v>
+        <v>7404311.079104981</v>
       </c>
       <c r="D147" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -16150,17 +16150,17 @@
         <v>3804</v>
       </c>
       <c r="B148" t="n">
-        <v>331539974.7603281</v>
+        <v>663250.528201481</v>
       </c>
       <c r="C148" t="n">
-        <v>-741698511.2020931</v>
+        <v>7142209.795338459</v>
       </c>
       <c r="D148" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -16258,17 +16258,17 @@
         <v>3833</v>
       </c>
       <c r="B149" t="n">
-        <v>275934405.7071202</v>
+        <v>468998.8339806726</v>
       </c>
       <c r="C149" t="n">
-        <v>-693029384.238608</v>
+        <v>7388821.772371144</v>
       </c>
       <c r="D149" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -16362,17 +16362,17 @@
         <v>3836</v>
       </c>
       <c r="B150" t="n">
-        <v>245221390.8877693</v>
+        <v>436408.8218150658</v>
       </c>
       <c r="C150" t="n">
-        <v>-645922673.169723</v>
+        <v>7506500.594720325</v>
       </c>
       <c r="D150" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -16466,17 +16466,17 @@
         <v>3837</v>
       </c>
       <c r="B151" t="n">
-        <v>271433622.9273621</v>
+        <v>569006.5176380178</v>
       </c>
       <c r="C151" t="n">
-        <v>-671121900.1209217</v>
+        <v>7374633.408555133</v>
       </c>
       <c r="D151" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -16574,17 +16574,17 @@
         <v>3872</v>
       </c>
       <c r="B152" t="n">
-        <v>333327753.5744264</v>
+        <v>376624.0866571964</v>
       </c>
       <c r="C152" t="n">
-        <v>-793362759.6305578</v>
+        <v>7229605.106066765</v>
       </c>
       <c r="D152" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -16674,17 +16674,17 @@
         <v>3879</v>
       </c>
       <c r="B153" t="n">
-        <v>281927973.9961489</v>
+        <v>444385.7615036962</v>
       </c>
       <c r="C153" t="n">
-        <v>-706328223.660036</v>
+        <v>7376206.848085475</v>
       </c>
       <c r="D153" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -16782,17 +16782,17 @@
         <v>3927</v>
       </c>
       <c r="B154" t="n">
-        <v>241494785.4813281</v>
+        <v>431132.6180002625</v>
       </c>
       <c r="C154" t="n">
-        <v>-640042740.3329711</v>
+        <v>7521465.612824399</v>
       </c>
       <c r="D154" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -16886,17 +16886,17 @@
         <v>3948</v>
       </c>
       <c r="B155" t="n">
-        <v>311085736.1148545</v>
+        <v>584961.2195156019</v>
       </c>
       <c r="C155" t="n">
-        <v>-727727749.3847228</v>
+        <v>7233817.372569075</v>
       </c>
       <c r="D155" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -16994,17 +16994,17 @@
         <v>3959</v>
       </c>
       <c r="B156" t="n">
-        <v>236677036.0213428</v>
+        <v>446157.5485860738</v>
       </c>
       <c r="C156" t="n">
-        <v>-629346904.2296659</v>
+        <v>7534123.93820927</v>
       </c>
       <c r="D156" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -17098,17 +17098,17 @@
         <v>3971</v>
       </c>
       <c r="B157" t="n">
-        <v>299827188.9903314</v>
+        <v>669236.5653518254</v>
       </c>
       <c r="C157" t="n">
-        <v>-698771109.8942244</v>
+        <v>7248640.712909578</v>
       </c>
       <c r="D157" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -17202,17 +17202,17 @@
         <v>3978</v>
       </c>
       <c r="B158" t="n">
-        <v>275722938.950241</v>
+        <v>777512.9831815676</v>
       </c>
       <c r="C158" t="n">
-        <v>-647966189.414601</v>
+        <v>7307313.468056051</v>
       </c>
       <c r="D158" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -17310,17 +17310,17 @@
         <v>4044</v>
       </c>
       <c r="B159" t="n">
-        <v>231870099.3434019</v>
+        <v>435487.6637338779</v>
       </c>
       <c r="C159" t="n">
-        <v>-622072620.8410587</v>
+        <v>7554822.370589631</v>
       </c>
       <c r="D159" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -17418,17 +17418,17 @@
         <v>4050</v>
       </c>
       <c r="B160" t="n">
-        <v>331375399.2707284</v>
+        <v>664861.8344592829</v>
       </c>
       <c r="C160" t="n">
-        <v>-741223418.8351234</v>
+        <v>7142306.853326681</v>
       </c>
       <c r="D160" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -17526,17 +17526,17 @@
         <v>4065</v>
       </c>
       <c r="B161" t="n">
-        <v>306411760.0856024</v>
+        <v>713772.8159372762</v>
       </c>
       <c r="C161" t="n">
-        <v>-700964540.7794162</v>
+        <v>7214284.154764948</v>
       </c>
       <c r="D161" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -17634,17 +17634,17 @@
         <v>4072</v>
       </c>
       <c r="B162" t="n">
-        <v>274184724.1137281</v>
+        <v>439805.1538512177</v>
       </c>
       <c r="C162" t="n">
-        <v>-694568373.8249217</v>
+        <v>7404176.992680821</v>
       </c>
       <c r="D162" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -17742,17 +17742,17 @@
         <v>4073</v>
       </c>
       <c r="B163" t="n">
-        <v>299734528.2315714</v>
+        <v>647141.1239790823</v>
       </c>
       <c r="C163" t="n">
-        <v>-702042015.4739696</v>
+        <v>7254886.228397596</v>
       </c>
       <c r="D163" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -17846,17 +17846,17 @@
         <v>4076</v>
       </c>
       <c r="B164" t="n">
-        <v>240554629.3470742</v>
+        <v>429836.6878292271</v>
       </c>
       <c r="C164" t="n">
-        <v>-638542346.5098919</v>
+        <v>7525240.43409429</v>
       </c>
       <c r="D164" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -17950,17 +17950,17 @@
         <v>4105</v>
       </c>
       <c r="B165" t="n">
-        <v>307919216.6758572</v>
+        <v>714955.4111270539</v>
       </c>
       <c r="C165" t="n">
-        <v>-702811392.4851085</v>
+        <v>7208770.172444158</v>
       </c>
       <c r="D165" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -18058,17 +18058,17 @@
         <v>4135</v>
       </c>
       <c r="B166" t="n">
-        <v>324395347.8652229</v>
+        <v>612695.2306431417</v>
       </c>
       <c r="C166" t="n">
-        <v>-741076423.4641184</v>
+        <v>7180841.293022046</v>
       </c>
       <c r="D166" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -18162,17 +18162,17 @@
         <v>4139</v>
       </c>
       <c r="B167" t="n">
-        <v>240392358.7967031</v>
+        <v>431933.0220172554</v>
       </c>
       <c r="C167" t="n">
-        <v>-637962998.1665426</v>
+        <v>7525164.216234216</v>
       </c>
       <c r="D167" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -18270,17 +18270,17 @@
         <v>4225</v>
       </c>
       <c r="B168" t="n">
-        <v>282423728.746169</v>
+        <v>571477.7003448418</v>
       </c>
       <c r="C168" t="n">
-        <v>-687942724.5554985</v>
+        <v>7335667.556724924</v>
       </c>
       <c r="D168" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -18370,17 +18370,17 @@
         <v>4278</v>
       </c>
       <c r="B169" t="n">
-        <v>324236869.8379742</v>
+        <v>725637.832248533</v>
       </c>
       <c r="C169" t="n">
-        <v>-722257016.7834637</v>
+        <v>7149922.107346477</v>
       </c>
       <c r="D169" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -18478,17 +18478,17 @@
         <v>4310</v>
       </c>
       <c r="B170" t="n">
-        <v>293455255.8377674</v>
+        <v>674219.4674038889</v>
       </c>
       <c r="C170" t="n">
-        <v>-688952220.5230802</v>
+        <v>7269409.352310479</v>
       </c>
       <c r="D170" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -18582,17 +18582,17 @@
         <v>4317</v>
       </c>
       <c r="B171" t="n">
-        <v>304014132.5989069</v>
+        <v>710749.5401521167</v>
       </c>
       <c r="C171" t="n">
-        <v>-698175436.5643777</v>
+        <v>7223356.075473163</v>
       </c>
       <c r="D171" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -18686,17 +18686,17 @@
         <v>4385</v>
       </c>
       <c r="B172" t="n">
-        <v>321884934.3653171</v>
+        <v>593191.4187559042</v>
       </c>
       <c r="C172" t="n">
-        <v>-741012669.4637401</v>
+        <v>7195042.290479658</v>
       </c>
       <c r="D172" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -18794,17 +18794,17 @@
         <v>4429</v>
       </c>
       <c r="B173" t="n">
-        <v>332054352.0411416</v>
+        <v>669087.1574735446</v>
       </c>
       <c r="C173" t="n">
-        <v>-741350897.6632477</v>
+        <v>7138823.143244307</v>
       </c>
       <c r="D173" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -18902,17 +18902,17 @@
         <v>4516</v>
       </c>
       <c r="B174" t="n">
-        <v>268688270.2184461</v>
+        <v>576221.5915295435</v>
       </c>
       <c r="C174" t="n">
-        <v>-665700112.87985</v>
+        <v>7382257.330581195</v>
       </c>
       <c r="D174" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -19010,17 +19010,17 @@
         <v>4522</v>
       </c>
       <c r="B175" t="n">
-        <v>325429242.7824501</v>
+        <v>713603.1766074058</v>
       </c>
       <c r="C175" t="n">
-        <v>-725720479.2212398</v>
+        <v>7149041.025246967</v>
       </c>
       <c r="D175" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -19114,17 +19114,17 @@
         <v>4562</v>
       </c>
       <c r="B176" t="n">
-        <v>326432980.3894434</v>
+        <v>575266.3307147442</v>
       </c>
       <c r="C176" t="n">
-        <v>-749984518.1305887</v>
+        <v>7185257.558376712</v>
       </c>
       <c r="D176" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -19214,17 +19214,17 @@
         <v>4594</v>
       </c>
       <c r="B177" t="n">
-        <v>271529942.5186161</v>
+        <v>604290.0810529721</v>
       </c>
       <c r="C177" t="n">
-        <v>-666187380.9058965</v>
+        <v>7364583.701289264</v>
       </c>
       <c r="D177" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -19318,17 +19318,17 @@
         <v>4628</v>
       </c>
       <c r="B178" t="n">
-        <v>277018094.9322309</v>
+        <v>432284.6912633065</v>
       </c>
       <c r="C178" t="n">
-        <v>-700296723.8155724</v>
+        <v>7396923.161243825</v>
       </c>
       <c r="D178" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -19426,17 +19426,17 @@
         <v>4643</v>
       </c>
       <c r="B179" t="n">
-        <v>274734659.9312125</v>
+        <v>439758.1563198671</v>
       </c>
       <c r="C179" t="n">
-        <v>-695469769.7531233</v>
+        <v>7402304.535486695</v>
       </c>
       <c r="D179" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -19534,17 +19534,17 @@
         <v>4647</v>
       </c>
       <c r="B180" t="n">
-        <v>307962529.6169906</v>
+        <v>455576.2169239347</v>
       </c>
       <c r="C180" t="n">
-        <v>-744215916.061385</v>
+        <v>7284936.716519298</v>
       </c>
       <c r="D180" t="n">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>W</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">

</xml_diff>

<commit_message>
QAPF map area 1_Tr
</commit_message>
<xml_diff>
--- a/_INTERPOLATION/area5.xlsx
+++ b/_INTERPOLATION/area5.xlsx
@@ -518,17 +518,17 @@
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>170061253.5450011</v>
+        <v>105508726.4694378</v>
       </c>
       <c r="C2" t="n">
-        <v>-402048568.8690004</v>
+        <v>-209018146.6045218</v>
       </c>
       <c r="D2" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -626,17 +626,17 @@
         <v>67</v>
       </c>
       <c r="B3" t="n">
-        <v>215751600.2529267</v>
+        <v>132646577.4596441</v>
       </c>
       <c r="C3" t="n">
-        <v>-466156325.3815762</v>
+        <v>-241504486.6946509</v>
       </c>
       <c r="D3" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -734,17 +734,17 @@
         <v>111</v>
       </c>
       <c r="B4" t="n">
-        <v>190157095.1846463</v>
+        <v>116529554.7152026</v>
       </c>
       <c r="C4" t="n">
-        <v>-415950649.4723316</v>
+        <v>-213442943.3238954</v>
       </c>
       <c r="D4" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -846,17 +846,17 @@
         <v>134</v>
       </c>
       <c r="B5" t="n">
-        <v>170860992.9712256</v>
+        <v>106092782.3304012</v>
       </c>
       <c r="C5" t="n">
-        <v>-405155427.0714723</v>
+        <v>-210929361.0420707</v>
       </c>
       <c r="D5" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -954,17 +954,17 @@
         <v>181</v>
       </c>
       <c r="B6" t="n">
-        <v>170667185.431315</v>
+        <v>105991829.6311245</v>
       </c>
       <c r="C6" t="n">
-        <v>-405104104.4883425</v>
+        <v>-210946344.5005981</v>
       </c>
       <c r="D6" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1062,17 +1062,17 @@
         <v>189</v>
       </c>
       <c r="B7" t="n">
-        <v>198148318.8949276</v>
+        <v>122395754.4997257</v>
       </c>
       <c r="C7" t="n">
-        <v>-446478395.0038871</v>
+        <v>-232183773.5343286</v>
       </c>
       <c r="D7" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1166,17 +1166,17 @@
         <v>232</v>
       </c>
       <c r="B8" t="n">
-        <v>170922082.497805</v>
+        <v>106102412.26284</v>
       </c>
       <c r="C8" t="n">
-        <v>-404787896.7358894</v>
+        <v>-210661424.2871895</v>
       </c>
       <c r="D8" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1274,17 +1274,17 @@
         <v>281</v>
       </c>
       <c r="B9" t="n">
-        <v>190811154.076052</v>
+        <v>117040622.1587794</v>
       </c>
       <c r="C9" t="n">
-        <v>-418967515.8208964</v>
+        <v>-215321766.9774082</v>
       </c>
       <c r="D9" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1386,17 +1386,17 @@
         <v>302</v>
       </c>
       <c r="B10" t="n">
-        <v>167063073.7771204</v>
+        <v>103861518.1174055</v>
       </c>
       <c r="C10" t="n">
-        <v>-399736333.0616241</v>
+        <v>-208247002.9008795</v>
       </c>
       <c r="D10" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1498,17 +1498,17 @@
         <v>309</v>
       </c>
       <c r="B11" t="n">
-        <v>191182675.188347</v>
+        <v>117134202.8675836</v>
       </c>
       <c r="C11" t="n">
-        <v>-417313437.041097</v>
+        <v>-214123845.5357292</v>
       </c>
       <c r="D11" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1606,17 +1606,17 @@
         <v>336</v>
       </c>
       <c r="B12" t="n">
-        <v>226125332.4069945</v>
+        <v>138056256.2293121</v>
       </c>
       <c r="C12" t="n">
-        <v>-465476449.0371869</v>
+        <v>-238975883.2737637</v>
       </c>
       <c r="D12" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1710,17 +1710,17 @@
         <v>373</v>
       </c>
       <c r="B13" t="n">
-        <v>207534924.9715279</v>
+        <v>127395291.6096901</v>
       </c>
       <c r="C13" t="n">
-        <v>-448996303.2290542</v>
+        <v>-231756331.7183017</v>
       </c>
       <c r="D13" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1810,17 +1810,17 @@
         <v>383</v>
       </c>
       <c r="B14" t="n">
-        <v>165417181.4159042</v>
+        <v>102692553.5673765</v>
       </c>
       <c r="C14" t="n">
-        <v>-393879767.4921157</v>
+        <v>-204683855.8293287</v>
       </c>
       <c r="D14" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1918,17 +1918,17 @@
         <v>495</v>
       </c>
       <c r="B15" t="n">
-        <v>179797278.9888872</v>
+        <v>109438266.882265</v>
       </c>
       <c r="C15" t="n">
-        <v>-385339572.3715404</v>
+        <v>-195287931.0485279</v>
       </c>
       <c r="D15" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2022,17 +2022,17 @@
         <v>502</v>
       </c>
       <c r="B16" t="n">
-        <v>227210100.4166648</v>
+        <v>138596224.7624223</v>
       </c>
       <c r="C16" t="n">
-        <v>-464887206.9620859</v>
+        <v>-238383033.7740149</v>
       </c>
       <c r="D16" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2130,17 +2130,17 @@
         <v>526</v>
       </c>
       <c r="B17" t="n">
-        <v>212055122.9125671</v>
+        <v>130020051.2517149</v>
       </c>
       <c r="C17" t="n">
-        <v>-453803865.4495928</v>
+        <v>-234012094.1658826</v>
       </c>
       <c r="D17" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2234,17 +2234,17 @@
         <v>561</v>
       </c>
       <c r="B18" t="n">
-        <v>219066152.3479342</v>
+        <v>134644140.8865899</v>
       </c>
       <c r="C18" t="n">
-        <v>-470844080.385905</v>
+        <v>-243949740.2878812</v>
       </c>
       <c r="D18" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2342,17 +2342,17 @@
         <v>589</v>
       </c>
       <c r="B19" t="n">
-        <v>229520900.4912613</v>
+        <v>139608841.0539081</v>
       </c>
       <c r="C19" t="n">
-        <v>-461115703.439372</v>
+        <v>-235476230.8749945</v>
       </c>
       <c r="D19" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2442,17 +2442,17 @@
         <v>623</v>
       </c>
       <c r="B20" t="n">
-        <v>170189121.3721983</v>
+        <v>105596981.9961531</v>
       </c>
       <c r="C20" t="n">
-        <v>-402456658.3516716</v>
+        <v>-209263009.2431625</v>
       </c>
       <c r="D20" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2550,17 +2550,17 @@
         <v>629</v>
       </c>
       <c r="B21" t="n">
-        <v>232646418.6580028</v>
+        <v>141599423.6154124</v>
       </c>
       <c r="C21" t="n">
-        <v>-467100958.0807744</v>
+        <v>-238858232.1724758</v>
       </c>
       <c r="D21" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2654,17 +2654,17 @@
         <v>652</v>
       </c>
       <c r="B22" t="n">
-        <v>221685799.896555</v>
+        <v>134875384.7845174</v>
       </c>
       <c r="C22" t="n">
-        <v>-450486429.1942855</v>
+        <v>-229901430.6513903</v>
       </c>
       <c r="D22" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2754,17 +2754,17 @@
         <v>663</v>
       </c>
       <c r="B23" t="n">
-        <v>170044434.1339617</v>
+        <v>105594822.7153038</v>
       </c>
       <c r="C23" t="n">
-        <v>-403681533.2859867</v>
+        <v>-210140147.9385734</v>
       </c>
       <c r="D23" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2854,17 +2854,17 @@
         <v>685</v>
       </c>
       <c r="B24" t="n">
-        <v>170455328.0702242</v>
+        <v>105845394.8503075</v>
       </c>
       <c r="C24" t="n">
-        <v>-404423592.289158</v>
+        <v>-210537490.5371626</v>
       </c>
       <c r="D24" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2962,17 +2962,17 @@
         <v>696</v>
       </c>
       <c r="B25" t="n">
-        <v>220587369.5919776</v>
+        <v>134781258.9465282</v>
       </c>
       <c r="C25" t="n">
-        <v>-459065039.3759356</v>
+        <v>-235788498.9133089</v>
       </c>
       <c r="D25" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3070,17 +3070,17 @@
         <v>704</v>
       </c>
       <c r="B26" t="n">
-        <v>204294828.1179895</v>
+        <v>125182348.8449171</v>
       </c>
       <c r="C26" t="n">
-        <v>-439678649.7171889</v>
+        <v>-226212495.6601892</v>
       </c>
       <c r="D26" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3174,17 +3174,17 @@
         <v>751</v>
       </c>
       <c r="B27" t="n">
-        <v>169897527.0426158</v>
+        <v>105460556.4692007</v>
       </c>
       <c r="C27" t="n">
-        <v>-402644194.6175289</v>
+        <v>-209469655.8274356</v>
       </c>
       <c r="D27" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3282,17 +3282,17 @@
         <v>775</v>
       </c>
       <c r="B28" t="n">
-        <v>209752092.0299546</v>
+        <v>127417554.1764413</v>
       </c>
       <c r="C28" t="n">
-        <v>-429279032.9395711</v>
+        <v>-218170442.130488</v>
       </c>
       <c r="D28" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3390,17 +3390,17 @@
         <v>783</v>
       </c>
       <c r="B29" t="n">
-        <v>181148880.3769667</v>
+        <v>110635064.8260035</v>
       </c>
       <c r="C29" t="n">
-        <v>-393871673.9209508</v>
+        <v>-200693955.3049799</v>
       </c>
       <c r="D29" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3494,17 +3494,17 @@
         <v>791</v>
       </c>
       <c r="B30" t="n">
-        <v>223592087.1595653</v>
+        <v>136104466.1075085</v>
       </c>
       <c r="C30" t="n">
-        <v>-454483925.6360297</v>
+        <v>-232184709.8015506</v>
       </c>
       <c r="D30" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -3594,17 +3594,17 @@
         <v>827</v>
       </c>
       <c r="B31" t="n">
-        <v>220591388.8574566</v>
+        <v>134783690.3161738</v>
       </c>
       <c r="C31" t="n">
-        <v>-459070734.1471248</v>
+        <v>-235791494.57205</v>
       </c>
       <c r="D31" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3702,17 +3702,17 @@
         <v>835</v>
       </c>
       <c r="B32" t="n">
-        <v>169837139.3715255</v>
+        <v>105451235.8885704</v>
       </c>
       <c r="C32" t="n">
-        <v>-403010049.6333153</v>
+        <v>-209736329.8344363</v>
       </c>
       <c r="D32" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3810,17 +3810,17 @@
         <v>841</v>
       </c>
       <c r="B33" t="n">
-        <v>217075885.120332</v>
+        <v>133553287.5962651</v>
       </c>
       <c r="C33" t="n">
-        <v>-469975118.9094672</v>
+        <v>-243785214.8407176</v>
       </c>
       <c r="D33" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3914,17 +3914,17 @@
         <v>860</v>
       </c>
       <c r="B34" t="n">
-        <v>170221339.6758617</v>
+        <v>105716464.7564075</v>
       </c>
       <c r="C34" t="n">
-        <v>-404239109.246271</v>
+        <v>-210474208.3568346</v>
       </c>
       <c r="D34" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -4022,17 +4022,17 @@
         <v>890</v>
       </c>
       <c r="B35" t="n">
-        <v>228674745.6979045</v>
+        <v>139066872.48509</v>
       </c>
       <c r="C35" t="n">
-        <v>-459433627.7697359</v>
+        <v>-234520873.5788515</v>
       </c>
       <c r="D35" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4126,17 +4126,17 @@
         <v>930</v>
       </c>
       <c r="B36" t="n">
-        <v>226511925.3198773</v>
+        <v>138187606.9388872</v>
       </c>
       <c r="C36" t="n">
-        <v>-464173405.9727495</v>
+        <v>-238041235.5106107</v>
       </c>
       <c r="D36" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4238,17 +4238,17 @@
         <v>933</v>
       </c>
       <c r="B37" t="n">
-        <v>182849971.5594774</v>
+        <v>111701037.9983043</v>
       </c>
       <c r="C37" t="n">
-        <v>-397265861.4077961</v>
+        <v>-202577032.8259242</v>
       </c>
       <c r="D37" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4342,17 +4342,17 @@
         <v>952</v>
       </c>
       <c r="B38" t="n">
-        <v>185605712.1449671</v>
+        <v>113236264.3979196</v>
       </c>
       <c r="C38" t="n">
-        <v>-399507878.409721</v>
+        <v>-203448141.3676558</v>
       </c>
       <c r="D38" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4450,17 +4450,17 @@
         <v>995</v>
       </c>
       <c r="B39" t="n">
-        <v>165158688.1655019</v>
+        <v>102773319.0900762</v>
       </c>
       <c r="C39" t="n">
-        <v>-397520250.4713072</v>
+        <v>-207250826.245541</v>
       </c>
       <c r="D39" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4562,17 +4562,17 @@
         <v>1041</v>
       </c>
       <c r="B40" t="n">
-        <v>169255388.5440889</v>
+        <v>105017672.2254655</v>
       </c>
       <c r="C40" t="n">
-        <v>-400598228.2076799</v>
+        <v>-208242418.4061436</v>
       </c>
       <c r="D40" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4674,17 +4674,17 @@
         <v>1069</v>
       </c>
       <c r="B41" t="n">
-        <v>220469595.8216356</v>
+        <v>134701314.1507206</v>
       </c>
       <c r="C41" t="n">
-        <v>-458743532.120712</v>
+        <v>-235598052.3902366</v>
       </c>
       <c r="D41" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4782,17 +4782,17 @@
         <v>1098</v>
       </c>
       <c r="B42" t="n">
-        <v>168088018.066688</v>
+        <v>104439268.9421774</v>
       </c>
       <c r="C42" t="n">
-        <v>-400784453.2981902</v>
+        <v>-208685705.4748633</v>
       </c>
       <c r="D42" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4894,17 +4894,17 @@
         <v>1143</v>
       </c>
       <c r="B43" t="n">
-        <v>167778416.8765537</v>
+        <v>104063185.0347636</v>
       </c>
       <c r="C43" t="n">
-        <v>-396994263.684976</v>
+        <v>-206174733.721487</v>
       </c>
       <c r="D43" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -5002,17 +5002,17 @@
         <v>1177</v>
       </c>
       <c r="B44" t="n">
-        <v>189893264.5149418</v>
+        <v>116381563.0254742</v>
       </c>
       <c r="C44" t="n">
-        <v>-415728052.2039195</v>
+        <v>-213354002.2535594</v>
       </c>
       <c r="D44" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -5114,17 +5114,17 @@
         <v>1219</v>
       </c>
       <c r="B45" t="n">
-        <v>161294915.6318805</v>
+        <v>100167826.3336622</v>
       </c>
       <c r="C45" t="n">
-        <v>-386106025.2255547</v>
+        <v>-200491735.4238619</v>
       </c>
       <c r="D45" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -5226,17 +5226,17 @@
         <v>1222</v>
       </c>
       <c r="B46" t="n">
-        <v>170989661.2193642</v>
+        <v>106181608.3227286</v>
       </c>
       <c r="C46" t="n">
-        <v>-405566621.7426242</v>
+        <v>-211176252.3923558</v>
       </c>
       <c r="D46" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -5330,17 +5330,17 @@
         <v>1306</v>
       </c>
       <c r="B47" t="n">
-        <v>167842617.8236445</v>
+        <v>104367728.3348256</v>
       </c>
       <c r="C47" t="n">
-        <v>-401689953.4288404</v>
+        <v>-209373254.1300425</v>
       </c>
       <c r="D47" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -5442,17 +5442,17 @@
         <v>1345</v>
       </c>
       <c r="B48" t="n">
-        <v>168348387.5857986</v>
+        <v>104424001.3408905</v>
       </c>
       <c r="C48" t="n">
-        <v>-398256561.2255399</v>
+        <v>-206884594.4189475</v>
       </c>
       <c r="D48" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -5550,17 +5550,17 @@
         <v>1368</v>
       </c>
       <c r="B49" t="n">
-        <v>225037801.297646</v>
+        <v>137283281.5320168</v>
       </c>
       <c r="C49" t="n">
-        <v>-461912078.2331657</v>
+        <v>-236821997.8006023</v>
       </c>
       <c r="D49" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5658,17 +5658,17 @@
         <v>1389</v>
       </c>
       <c r="B50" t="n">
-        <v>170869051.6025432</v>
+        <v>106000975.046599</v>
       </c>
       <c r="C50" t="n">
-        <v>-403499299.370443</v>
+        <v>-209794092.8900959</v>
       </c>
       <c r="D50" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5762,17 +5762,17 @@
         <v>1423</v>
       </c>
       <c r="B51" t="n">
-        <v>193017470.4955127</v>
+        <v>117159326.3814496</v>
       </c>
       <c r="C51" t="n">
-        <v>-401785101.312815</v>
+        <v>-203346207.1822138</v>
       </c>
       <c r="D51" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5870,17 +5870,17 @@
         <v>1485</v>
       </c>
       <c r="B52" t="n">
-        <v>199949949.5776266</v>
+        <v>123465584.6433238</v>
       </c>
       <c r="C52" t="n">
-        <v>-448945059.420067</v>
+        <v>-233430269.622158</v>
       </c>
       <c r="D52" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -5974,17 +5974,17 @@
         <v>1509</v>
       </c>
       <c r="B53" t="n">
-        <v>212560183.8336233</v>
+        <v>130665300.368854</v>
       </c>
       <c r="C53" t="n">
-        <v>-460556023.6364397</v>
+        <v>-238428189.4724956</v>
       </c>
       <c r="D53" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -6082,17 +6082,17 @@
         <v>1523</v>
       </c>
       <c r="B54" t="n">
-        <v>161676484.2880752</v>
+        <v>100367178.8657337</v>
       </c>
       <c r="C54" t="n">
-        <v>-386240761.038307</v>
+        <v>-200478489.6620883</v>
       </c>
       <c r="D54" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -6194,17 +6194,17 @@
         <v>1524</v>
       </c>
       <c r="B55" t="n">
-        <v>169788566.1146641</v>
+        <v>105352880.5020434</v>
       </c>
       <c r="C55" t="n">
-        <v>-401736005.8829324</v>
+        <v>-208877513.5332501</v>
       </c>
       <c r="D55" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -6302,17 +6302,17 @@
         <v>1533</v>
       </c>
       <c r="B56" t="n">
-        <v>211508905.0259657</v>
+        <v>129647122.8856552</v>
       </c>
       <c r="C56" t="n">
-        <v>-452247932.9809692</v>
+        <v>-233086310.6818279</v>
       </c>
       <c r="D56" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>U</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -6406,17 +6406,17 @@
         <v>1537</v>
       </c>
       <c r="B57" t="n">
-        <v>159944451.6321533</v>
+        <v>99652515.60497172</v>
       </c>
       <c r="C57" t="n">
-        <v>-388908680.488093</v>
+        <v>-202793563.913616</v>
       </c>
       <c r="D57" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t